<commit_message>
Aggiunte relazioni tra database Aggiunto database dei tool con relativa pagina Aggiunto controllo sull'esistenza dei database, prima di caricare i dati Aggiunti riferimenti ai tool nelle pagine di dettaglio del capec
</commit_message>
<xml_diff>
--- a/apps/static/assets/dbs/ThreatCatalogComplete.xlsx
+++ b/apps/static/assets/dbs/ThreatCatalogComplete.xlsx
@@ -1,29 +1,30 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10910"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10917"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fefox/Desktop/Web2/apps/static/assets/dbs/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fefox/Desktop/Web3/apps/static/assets/dbs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A0A5B65D-3C3E-2649-9FAC-6AB54C1AD19C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{E945F12F-36D1-4A44-8A28-DA6A78194157}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16380" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Threat Components" sheetId="1" r:id="rId1"/>
     <sheet name="Threat Protocols" sheetId="3" r:id="rId2"/>
     <sheet name="#ThreatPerAsset" sheetId="4" r:id="rId3"/>
     <sheet name="Threats" sheetId="5" r:id="rId4"/>
+    <sheet name="Tools" sheetId="6" r:id="rId5"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">Threats!$A$1:$B$76</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
   <pivotCaches>
-    <pivotCache cacheId="1" r:id="rId5"/>
+    <pivotCache cacheId="1" r:id="rId6"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -45,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4026" uniqueCount="910">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4036" uniqueCount="920">
   <si>
     <t>TID</t>
   </si>
@@ -2815,6 +2816,36 @@
   </si>
   <si>
     <t>16, 55, 70, 565, 163, 164, 656, 275, 543, 544, 598, 633, 587, 459, 474, 475, 476, 477, 479, 485, 467, 59, 226, 60, 61, 102, 207</t>
+  </si>
+  <si>
+    <t>CapecID</t>
+  </si>
+  <si>
+    <t>ToolID</t>
+  </si>
+  <si>
+    <t>Command</t>
+  </si>
+  <si>
+    <t>SQLMap</t>
+  </si>
+  <si>
+    <t>python sqlmap.py -u &lt;url&gt; -f --banner --dbs --users</t>
+  </si>
+  <si>
+    <t>66, 7, 108</t>
+  </si>
+  <si>
+    <t>java -jar DirBuster-1.0-RC1.jar -H -u &lt;url&gt;</t>
+  </si>
+  <si>
+    <t>Dirbuster</t>
+  </si>
+  <si>
+    <t>87, 139, 597</t>
+  </si>
+  <si>
+    <t>Name</t>
   </si>
 </sst>
 </file>
@@ -3017,20 +3048,20 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="20">
+  <dxfs count="21">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -3040,6 +3071,9 @@
           <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
@@ -8224,38 +8258,38 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{DEFAB213-4389-184E-911C-CDCC8CABBD38}" name="Tabella1" displayName="Tabella1" ref="A1:R299" totalsRowShown="0" dataDxfId="19">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{DEFAB213-4389-184E-911C-CDCC8CABBD38}" name="Tabella1" displayName="Tabella1" ref="A1:R299" totalsRowShown="0" dataDxfId="20">
   <autoFilter ref="A1:R299" xr:uid="{DEFAB213-4389-184E-911C-CDCC8CABBD38}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:R299">
     <sortCondition ref="B1:B299"/>
   </sortState>
   <tableColumns count="18">
-    <tableColumn id="16" xr3:uid="{DE426BDB-E154-EE46-B7B3-5B538C8AEC32}" name="TID" dataDxfId="18">
+    <tableColumn id="16" xr3:uid="{DE426BDB-E154-EE46-B7B3-5B538C8AEC32}" name="TID" dataDxfId="19">
       <calculatedColumnFormula>CONCATENATE("T",ROW(A2)-1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="1" xr3:uid="{A0AE63DC-99F7-7D4F-B824-AB7765893284}" name="Asset" dataDxfId="17"/>
-    <tableColumn id="2" xr3:uid="{0FA38BFF-C67B-0C43-B1BA-F6338DBFB0C8}" name="Threat" dataDxfId="16"/>
-    <tableColumn id="3" xr3:uid="{BFC77F7C-F096-8345-97EA-317816ED869D}" name="Description" dataDxfId="15"/>
-    <tableColumn id="4" xr3:uid="{258F3B86-1461-D64A-AE3B-CEAC97B2B533}" name="STRIDE" dataDxfId="14"/>
-    <tableColumn id="6" xr3:uid="{0FD06C95-5962-AC4D-B9EF-4DBB5728E736}" name="Compromised" dataDxfId="13"/>
-    <tableColumn id="7" xr3:uid="{9E5B99AD-1F1D-B44C-ABDF-6F7E9177F3DE}" name="PreC" dataDxfId="12"/>
-    <tableColumn id="8" xr3:uid="{D4F97A81-E528-2841-B4DE-321362F90F65}" name="PreI" dataDxfId="11"/>
-    <tableColumn id="9" xr3:uid="{018427D6-D385-3447-B4A4-95003B3341F6}" name="PreA" dataDxfId="10"/>
-    <tableColumn id="10" xr3:uid="{8334AC57-4A09-5744-9484-073ECEE2E513}" name="Precondition" dataDxfId="9"/>
-    <tableColumn id="12" xr3:uid="{DDBE315D-E051-2C47-A765-EE1DB2E118EA}" name="PostC" dataDxfId="8">
+    <tableColumn id="1" xr3:uid="{A0AE63DC-99F7-7D4F-B824-AB7765893284}" name="Asset" dataDxfId="18"/>
+    <tableColumn id="2" xr3:uid="{0FA38BFF-C67B-0C43-B1BA-F6338DBFB0C8}" name="Threat" dataDxfId="17"/>
+    <tableColumn id="3" xr3:uid="{BFC77F7C-F096-8345-97EA-317816ED869D}" name="Description" dataDxfId="16"/>
+    <tableColumn id="4" xr3:uid="{258F3B86-1461-D64A-AE3B-CEAC97B2B533}" name="STRIDE" dataDxfId="15"/>
+    <tableColumn id="6" xr3:uid="{0FD06C95-5962-AC4D-B9EF-4DBB5728E736}" name="Compromised" dataDxfId="14"/>
+    <tableColumn id="7" xr3:uid="{9E5B99AD-1F1D-B44C-ABDF-6F7E9177F3DE}" name="PreC" dataDxfId="13"/>
+    <tableColumn id="8" xr3:uid="{D4F97A81-E528-2841-B4DE-321362F90F65}" name="PreI" dataDxfId="12"/>
+    <tableColumn id="9" xr3:uid="{018427D6-D385-3447-B4A4-95003B3341F6}" name="PreA" dataDxfId="11"/>
+    <tableColumn id="10" xr3:uid="{8334AC57-4A09-5744-9484-073ECEE2E513}" name="Precondition" dataDxfId="10"/>
+    <tableColumn id="12" xr3:uid="{DDBE315D-E051-2C47-A765-EE1DB2E118EA}" name="PostC" dataDxfId="9">
       <calculatedColumnFormula>MID(N2,2,1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" xr3:uid="{243C1B9B-76C9-0345-B727-4F11FD75DF6B}" name="PostI" dataDxfId="7">
+    <tableColumn id="13" xr3:uid="{243C1B9B-76C9-0345-B727-4F11FD75DF6B}" name="PostI" dataDxfId="8">
       <calculatedColumnFormula>MID(N2,4,1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="14" xr3:uid="{DD688DAA-2C9A-C247-AEC4-CBDADE9B2B2E}" name="PostA" dataDxfId="6">
+    <tableColumn id="14" xr3:uid="{DD688DAA-2C9A-C247-AEC4-CBDADE9B2B2E}" name="PostA" dataDxfId="7">
       <calculatedColumnFormula>MID(N2,6,1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="15" xr3:uid="{CEE151EC-4E5B-0C41-8586-5A2D7E483661}" name="PostCondition" dataDxfId="5"/>
-    <tableColumn id="5" xr3:uid="{62EC5D77-1F78-1645-8697-BC5450583418}" name="CapecMeta" dataDxfId="4"/>
-    <tableColumn id="11" xr3:uid="{0DCD762C-4EE7-8141-BC05-9DB756A5BEF2}" name="CapecStandard" dataDxfId="3"/>
-    <tableColumn id="17" xr3:uid="{9EF317BA-855B-6E4A-9EC7-E1FB88A1FD56}" name="CapecDetailed" dataDxfId="2"/>
-    <tableColumn id="18" xr3:uid="{9BF6197D-4CF5-4941-A460-18823EEFB2E7}" name="Commento" dataDxfId="1"/>
+    <tableColumn id="15" xr3:uid="{CEE151EC-4E5B-0C41-8586-5A2D7E483661}" name="PostCondition" dataDxfId="6"/>
+    <tableColumn id="5" xr3:uid="{62EC5D77-1F78-1645-8697-BC5450583418}" name="CapecMeta" dataDxfId="5"/>
+    <tableColumn id="11" xr3:uid="{0DCD762C-4EE7-8141-BC05-9DB756A5BEF2}" name="CapecStandard" dataDxfId="4"/>
+    <tableColumn id="17" xr3:uid="{9EF317BA-855B-6E4A-9EC7-E1FB88A1FD56}" name="CapecDetailed" dataDxfId="3"/>
+    <tableColumn id="18" xr3:uid="{9BF6197D-4CF5-4941-A460-18823EEFB2E7}" name="Commento" dataDxfId="2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -8269,6 +8303,21 @@
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{2FFFB967-AADB-F047-AE3A-FED6B1206948}" name="TID"/>
     <tableColumn id="2" xr3:uid="{16F1CDC7-F519-F249-98FB-B71333839907}" name="Description"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{5ECAFCE9-964F-A04C-B050-422AACCFD3F5}" name="Tabella4" displayName="Tabella4" ref="A1:D3" totalsRowShown="0">
+  <autoFilter ref="A1:D3" xr:uid="{5ECAFCE9-964F-A04C-B050-422AACCFD3F5}"/>
+  <tableColumns count="4">
+    <tableColumn id="1" xr3:uid="{6405AD35-9222-B34C-A112-EC4FDEAC5BE2}" name="ToolID" dataDxfId="1">
+      <calculatedColumnFormula>ROW(Tabella4[[#This Row],[Name]])-1</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="4" xr3:uid="{94F8DBBB-A826-8B4A-8C87-395122CA233A}" name="Name"/>
+    <tableColumn id="2" xr3:uid="{FB636F07-AAD2-AE48-87BB-965F92F829C2}" name="CapecID"/>
+    <tableColumn id="3" xr3:uid="{52487567-ED26-B840-ABFD-DB1BF72A83C9}" name="Command"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -8539,8 +8588,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:R299"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A25" activePane="bottomLeft" state="frozen"/>
+    <sheetView zoomScale="125" zoomScaleNormal="115" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A67" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="O294" sqref="O294"/>
     </sheetView>
   </sheetViews>
@@ -25529,7 +25578,7 @@
       </c>
     </row>
     <row r="30" spans="1:13" ht="48">
-      <c r="A30" s="27" t="s">
+      <c r="A30" s="29" t="s">
         <v>732</v>
       </c>
       <c r="B30" s="5" t="s">
@@ -25572,7 +25621,7 @@
       </c>
     </row>
     <row r="31" spans="1:13" ht="48">
-      <c r="A31" s="27"/>
+      <c r="A31" s="29"/>
       <c r="B31" s="5" t="s">
         <v>735</v>
       </c>
@@ -25613,7 +25662,7 @@
       </c>
     </row>
     <row r="32" spans="1:13" ht="32">
-      <c r="A32" s="27"/>
+      <c r="A32" s="29"/>
       <c r="B32" s="5" t="s">
         <v>737</v>
       </c>
@@ -25654,7 +25703,7 @@
       </c>
     </row>
     <row r="33" spans="1:13" ht="96">
-      <c r="A33" s="27"/>
+      <c r="A33" s="29"/>
       <c r="B33" s="5" t="s">
         <v>51</v>
       </c>
@@ -25695,7 +25744,7 @@
       </c>
     </row>
     <row r="34" spans="1:13" ht="32">
-      <c r="A34" s="27"/>
+      <c r="A34" s="29"/>
       <c r="B34" s="5" t="s">
         <v>740</v>
       </c>
@@ -25736,7 +25785,7 @@
       </c>
     </row>
     <row r="35" spans="1:13" ht="32">
-      <c r="A35" s="27"/>
+      <c r="A35" s="29"/>
       <c r="B35" s="5" t="s">
         <v>414</v>
       </c>
@@ -25777,7 +25826,7 @@
       </c>
     </row>
     <row r="36" spans="1:13" ht="80">
-      <c r="A36" s="27"/>
+      <c r="A36" s="29"/>
       <c r="B36" s="5" t="s">
         <v>743</v>
       </c>
@@ -26316,7 +26365,7 @@
       </c>
     </row>
     <row r="49" spans="1:13" ht="78" customHeight="1">
-      <c r="A49" s="27" t="s">
+      <c r="A49" s="29" t="s">
         <v>761</v>
       </c>
       <c r="B49" s="5" t="s">
@@ -26359,7 +26408,7 @@
       </c>
     </row>
     <row r="50" spans="1:13" ht="32">
-      <c r="A50" s="27"/>
+      <c r="A50" s="29"/>
       <c r="B50" s="5" t="s">
         <v>409</v>
       </c>
@@ -26400,7 +26449,7 @@
       </c>
     </row>
     <row r="51" spans="1:13" ht="16">
-      <c r="A51" s="27"/>
+      <c r="A51" s="29"/>
       <c r="B51" s="5" t="s">
         <v>414</v>
       </c>
@@ -26441,7 +26490,7 @@
       </c>
     </row>
     <row r="52" spans="1:13" ht="32">
-      <c r="A52" s="27"/>
+      <c r="A52" s="29"/>
       <c r="B52" s="5" t="s">
         <v>766</v>
       </c>
@@ -26482,7 +26531,7 @@
       </c>
     </row>
     <row r="53" spans="1:13" ht="96">
-      <c r="A53" s="27"/>
+      <c r="A53" s="29"/>
       <c r="B53" s="5" t="s">
         <v>768</v>
       </c>
@@ -26523,7 +26572,7 @@
       </c>
     </row>
     <row r="54" spans="1:13">
-      <c r="A54" s="27"/>
+      <c r="A54" s="29"/>
       <c r="B54" s="5" t="s">
         <v>770</v>
       </c>
@@ -26564,7 +26613,7 @@
       </c>
     </row>
     <row r="55" spans="1:13" ht="64">
-      <c r="A55" s="27"/>
+      <c r="A55" s="29"/>
       <c r="B55" s="5" t="s">
         <v>772</v>
       </c>
@@ -26605,7 +26654,7 @@
       </c>
     </row>
     <row r="56" spans="1:13" ht="64">
-      <c r="A56" s="27"/>
+      <c r="A56" s="29"/>
       <c r="B56" s="5" t="s">
         <v>774</v>
       </c>
@@ -26646,7 +26695,7 @@
       </c>
     </row>
     <row r="57" spans="1:13" ht="32">
-      <c r="A57" s="28" t="s">
+      <c r="A57" s="27" t="s">
         <v>776</v>
       </c>
       <c r="B57" s="6" t="s">
@@ -26688,7 +26737,7 @@
       </c>
     </row>
     <row r="58" spans="1:13" ht="80">
-      <c r="A58" s="28"/>
+      <c r="A58" s="27"/>
       <c r="B58" s="7" t="s">
         <v>779</v>
       </c>
@@ -26728,7 +26777,7 @@
       </c>
     </row>
     <row r="59" spans="1:13" ht="64" customHeight="1">
-      <c r="A59" s="28"/>
+      <c r="A59" s="27"/>
       <c r="B59" s="7" t="s">
         <v>781</v>
       </c>
@@ -26768,7 +26817,7 @@
       </c>
     </row>
     <row r="60" spans="1:13" ht="16">
-      <c r="A60" s="28"/>
+      <c r="A60" s="27"/>
       <c r="B60" s="7" t="s">
         <v>283</v>
       </c>
@@ -26808,7 +26857,7 @@
       </c>
     </row>
     <row r="61" spans="1:13" ht="32">
-      <c r="A61" s="28"/>
+      <c r="A61" s="27"/>
       <c r="B61" s="7" t="s">
         <v>785</v>
       </c>
@@ -26848,7 +26897,7 @@
       </c>
     </row>
     <row r="62" spans="1:13" ht="32">
-      <c r="A62" s="28"/>
+      <c r="A62" s="27"/>
       <c r="B62" s="7" t="s">
         <v>787</v>
       </c>
@@ -26888,7 +26937,7 @@
       </c>
     </row>
     <row r="63" spans="1:13" ht="16">
-      <c r="A63" s="28"/>
+      <c r="A63" s="27"/>
       <c r="B63" s="7" t="s">
         <v>790</v>
       </c>
@@ -26928,7 +26977,7 @@
       </c>
     </row>
     <row r="64" spans="1:13" ht="32">
-      <c r="A64" s="28"/>
+      <c r="A64" s="27"/>
       <c r="B64" s="6" t="s">
         <v>792</v>
       </c>
@@ -26968,7 +27017,7 @@
       </c>
     </row>
     <row r="65" spans="1:13" ht="16">
-      <c r="A65" s="28"/>
+      <c r="A65" s="27"/>
       <c r="B65" s="7" t="s">
         <v>81</v>
       </c>
@@ -27008,7 +27057,7 @@
       </c>
     </row>
     <row r="66" spans="1:13" ht="16">
-      <c r="A66" s="28"/>
+      <c r="A66" s="27"/>
       <c r="B66" s="7" t="s">
         <v>795</v>
       </c>
@@ -27048,7 +27097,7 @@
       </c>
     </row>
     <row r="67" spans="1:13" ht="48">
-      <c r="A67" s="28"/>
+      <c r="A67" s="27"/>
       <c r="B67" s="6" t="s">
         <v>280</v>
       </c>
@@ -27088,38 +27137,38 @@
       </c>
     </row>
     <row r="68" spans="1:13" ht="16">
-      <c r="A68" s="28"/>
-      <c r="B68" s="28" t="s">
+      <c r="A68" s="27"/>
+      <c r="B68" s="27" t="s">
         <v>357</v>
       </c>
       <c r="C68" s="6" t="s">
         <v>797</v>
       </c>
-      <c r="D68" s="28" t="s">
+      <c r="D68" s="27" t="s">
         <v>274</v>
       </c>
-      <c r="E68" s="28" t="s">
+      <c r="E68" s="27" t="s">
         <v>783</v>
       </c>
-      <c r="F68" s="28" t="s">
-        <v>22</v>
-      </c>
-      <c r="G68" s="28" t="s">
+      <c r="F68" s="27" t="s">
+        <v>22</v>
+      </c>
+      <c r="G68" s="27" t="s">
         <v>22</v>
       </c>
       <c r="H68" s="26" t="s">
         <v>22</v>
       </c>
-      <c r="I68" s="28" t="s">
+      <c r="I68" s="27" t="s">
         <v>364</v>
       </c>
-      <c r="J68" s="28" t="s">
-        <v>22</v>
-      </c>
-      <c r="K68" s="28" t="s">
-        <v>22</v>
-      </c>
-      <c r="L68" s="28" t="s">
+      <c r="J68" s="27" t="s">
+        <v>22</v>
+      </c>
+      <c r="K68" s="27" t="s">
+        <v>22</v>
+      </c>
+      <c r="L68" s="27" t="s">
         <v>23</v>
       </c>
       <c r="M68" s="26" t="str">
@@ -27128,24 +27177,24 @@
       </c>
     </row>
     <row r="69" spans="1:13" ht="16">
-      <c r="A69" s="28"/>
-      <c r="B69" s="28"/>
+      <c r="A69" s="27"/>
+      <c r="B69" s="27"/>
       <c r="C69" s="6" t="s">
         <v>798</v>
       </c>
-      <c r="D69" s="28"/>
-      <c r="E69" s="28"/>
-      <c r="F69" s="28"/>
-      <c r="G69" s="28"/>
+      <c r="D69" s="27"/>
+      <c r="E69" s="27"/>
+      <c r="F69" s="27"/>
+      <c r="G69" s="27"/>
       <c r="H69" s="26"/>
-      <c r="I69" s="28"/>
-      <c r="J69" s="28"/>
-      <c r="K69" s="28"/>
-      <c r="L69" s="28"/>
+      <c r="I69" s="27"/>
+      <c r="J69" s="27"/>
+      <c r="K69" s="27"/>
+      <c r="L69" s="27"/>
       <c r="M69" s="26"/>
     </row>
     <row r="70" spans="1:13" ht="28">
-      <c r="A70" s="29" t="s">
+      <c r="A70" s="28" t="s">
         <v>799</v>
       </c>
       <c r="B70" s="16" t="s">
@@ -27191,7 +27240,7 @@
       </c>
     </row>
     <row r="71" spans="1:13" ht="51">
-      <c r="A71" s="29"/>
+      <c r="A71" s="28"/>
       <c r="B71" s="16" t="s">
         <v>51</v>
       </c>
@@ -27235,7 +27284,7 @@
       </c>
     </row>
     <row r="72" spans="1:13" ht="28">
-      <c r="A72" s="29"/>
+      <c r="A72" s="28"/>
       <c r="B72" s="16" t="s">
         <v>684</v>
       </c>
@@ -27279,7 +27328,7 @@
       </c>
     </row>
     <row r="73" spans="1:13" ht="28">
-      <c r="A73" s="29"/>
+      <c r="A73" s="28"/>
       <c r="B73" s="16" t="s">
         <v>806</v>
       </c>
@@ -27841,6 +27890,15 @@
     </row>
   </sheetData>
   <mergeCells count="23">
+    <mergeCell ref="A2:A7"/>
+    <mergeCell ref="A8:A14"/>
+    <mergeCell ref="A25:A29"/>
+    <mergeCell ref="A15:A24"/>
+    <mergeCell ref="A49:A56"/>
+    <mergeCell ref="A44:A48"/>
+    <mergeCell ref="A41:A43"/>
+    <mergeCell ref="A30:A36"/>
+    <mergeCell ref="A37:A40"/>
     <mergeCell ref="M68:M69"/>
     <mergeCell ref="H68:H69"/>
     <mergeCell ref="A74:A85"/>
@@ -27855,15 +27913,6 @@
     <mergeCell ref="B68:B69"/>
     <mergeCell ref="D68:D69"/>
     <mergeCell ref="E68:E69"/>
-    <mergeCell ref="A2:A7"/>
-    <mergeCell ref="A8:A14"/>
-    <mergeCell ref="A25:A29"/>
-    <mergeCell ref="A15:A24"/>
-    <mergeCell ref="A49:A56"/>
-    <mergeCell ref="A44:A48"/>
-    <mergeCell ref="A41:A43"/>
-    <mergeCell ref="A30:A36"/>
-    <mergeCell ref="A37:A40"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -28088,7 +28137,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8B4B4BA5-7F5F-6549-846C-E8044419A2A5}">
   <dimension ref="A1:B76"/>
   <sheetViews>
-    <sheetView zoomScale="150" workbookViewId="0">
+    <sheetView topLeftCell="A2" zoomScale="150" workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
@@ -28703,6 +28752,72 @@
       </c>
       <c r="B76" t="s">
         <v>570</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C51FC597-29FA-1D4E-A4C8-B79027768242}">
+  <dimension ref="A1:D3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="181" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <cols>
+    <col min="3" max="3" width="11.33203125" customWidth="1"/>
+    <col min="4" max="4" width="40.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" t="s">
+        <v>911</v>
+      </c>
+      <c r="B1" t="s">
+        <v>919</v>
+      </c>
+      <c r="C1" t="s">
+        <v>910</v>
+      </c>
+      <c r="D1" t="s">
+        <v>912</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2">
+        <f>ROW(Tabella4[[#This Row],[Name]])-1</f>
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>913</v>
+      </c>
+      <c r="C2" t="s">
+        <v>915</v>
+      </c>
+      <c r="D2" t="s">
+        <v>914</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3">
+        <f>ROW(Tabella4[[#This Row],[Name]])-1</f>
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>917</v>
+      </c>
+      <c r="C3" t="s">
+        <v>918</v>
+      </c>
+      <c r="D3" t="s">
+        <v>916</v>
       </c>
     </row>
   </sheetData>
@@ -28925,6 +29040,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <lcf76f155ced4ddcb4097134ff3c332f xmlns="633f040f-4953-46e7-8610-82b0c5296ba0">
@@ -28933,15 +29057,6 @@
     <TaxCatchAll xmlns="f62ef740-d444-4f18-80a2-7590fdcab1ce" xsi:nil="true"/>
   </documentManagement>
 </p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -28964,26 +29079,26 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{83D5100D-0E56-4B30-B42D-2AEC6B837C39}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2C6CC7BA-2E2C-4B0D-8103-11A51D82E8EC}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="f62ef740-d444-4f18-80a2-7590fdcab1ce"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="633f040f-4953-46e7-8610-82b0c5296ba0"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2C6CC7BA-2E2C-4B0D-8103-11A51D82E8EC}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{83D5100D-0E56-4B30-B42D-2AEC6B837C39}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="633f040f-4953-46e7-8610-82b0c5296ba0"/>
+    <ds:schemaRef ds:uri="f62ef740-d444-4f18-80a2-7590fdcab1ce"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Aggiunto popolamento dei comandi in macm-detail
</commit_message>
<xml_diff>
--- a/apps/static/assets/dbs/ThreatCatalogComplete.xlsx
+++ b/apps/static/assets/dbs/ThreatCatalogComplete.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fefox/Desktop/Web3/apps/static/assets/dbs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E945F12F-36D1-4A44-8A28-DA6A78194157}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{A20C026C-C6A7-D041-8659-4144E80AA269}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16380" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-38400" yWindow="-3100" windowWidth="38400" windowHeight="21100" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Threat Components" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
   </definedNames>
   <calcPr calcId="191028"/>
   <pivotCaches>
-    <pivotCache cacheId="1" r:id="rId6"/>
+    <pivotCache cacheId="2" r:id="rId6"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -2830,15 +2830,9 @@
     <t>SQLMap</t>
   </si>
   <si>
-    <t>python sqlmap.py -u &lt;url&gt; -f --banner --dbs --users</t>
-  </si>
-  <si>
     <t>66, 7, 108</t>
   </si>
   <si>
-    <t>java -jar DirBuster-1.0-RC1.jar -H -u &lt;url&gt;</t>
-  </si>
-  <si>
     <t>Dirbuster</t>
   </si>
   <si>
@@ -2846,6 +2840,12 @@
   </si>
   <si>
     <t>Name</t>
+  </si>
+  <si>
+    <t>python sqlmap.py -u {url} -f --banner --dbs --users</t>
+  </si>
+  <si>
+    <t>java -jar DirBuster-1.0-RC1.jar -H -u {url}</t>
   </si>
 </sst>
 </file>
@@ -8117,7 +8117,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{48CB07D6-9F6C-094F-A3D3-916741F281CD}" name="Tabella pivot1" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valori" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{48CB07D6-9F6C-094F-A3D3-916741F281CD}" name="Tabella pivot1" cacheId="2" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valori" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A1:B25" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="14">
     <pivotField showAll="0"/>
@@ -8259,7 +8259,13 @@
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{DEFAB213-4389-184E-911C-CDCC8CABBD38}" name="Tabella1" displayName="Tabella1" ref="A1:R299" totalsRowShown="0" dataDxfId="20">
-  <autoFilter ref="A1:R299" xr:uid="{DEFAB213-4389-184E-911C-CDCC8CABBD38}"/>
+  <autoFilter ref="A1:R299" xr:uid="{DEFAB213-4389-184E-911C-CDCC8CABBD38}">
+    <filterColumn colId="1">
+      <filters>
+        <filter val="HW.IOTDevice"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:R299">
     <sortCondition ref="B1:B299"/>
   </sortState>
@@ -8589,7 +8595,7 @@
   <dimension ref="A1:R299"/>
   <sheetViews>
     <sheetView zoomScale="125" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A67" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A63" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="O294" sqref="O294"/>
     </sheetView>
   </sheetViews>
@@ -8670,7 +8676,7 @@
         <v>860</v>
       </c>
     </row>
-    <row r="2" spans="1:18" ht="48">
+    <row r="2" spans="1:18" ht="48" hidden="1">
       <c r="A2" s="20" t="str">
         <f t="shared" ref="A2:A65" si="0">CONCATENATE("T",ROW(A2)-1)</f>
         <v>T1</v>
@@ -8712,7 +8718,7 @@
       <c r="Q2" s="24"/>
       <c r="R2" s="24"/>
     </row>
-    <row r="3" spans="1:18" ht="32">
+    <row r="3" spans="1:18" ht="32" hidden="1">
       <c r="A3" s="20" t="str">
         <f t="shared" si="0"/>
         <v>T2</v>
@@ -8754,7 +8760,7 @@
       <c r="Q3" s="24"/>
       <c r="R3" s="24"/>
     </row>
-    <row r="4" spans="1:18" ht="80">
+    <row r="4" spans="1:18" ht="80" hidden="1">
       <c r="A4" s="20" t="str">
         <f t="shared" si="0"/>
         <v>T3</v>
@@ -8796,7 +8802,7 @@
       <c r="Q4" s="24"/>
       <c r="R4" s="24"/>
     </row>
-    <row r="5" spans="1:18" ht="32">
+    <row r="5" spans="1:18" ht="32" hidden="1">
       <c r="A5" s="20" t="str">
         <f t="shared" si="0"/>
         <v>T4</v>
@@ -8838,7 +8844,7 @@
       <c r="Q5" s="24"/>
       <c r="R5" s="24"/>
     </row>
-    <row r="6" spans="1:18" ht="48">
+    <row r="6" spans="1:18" ht="48" hidden="1">
       <c r="A6" s="20" t="str">
         <f t="shared" si="0"/>
         <v>T5</v>
@@ -8880,7 +8886,7 @@
       <c r="Q6" s="24"/>
       <c r="R6" s="24"/>
     </row>
-    <row r="7" spans="1:18" ht="48">
+    <row r="7" spans="1:18" ht="48" hidden="1">
       <c r="A7" s="20" t="str">
         <f t="shared" si="0"/>
         <v>T6</v>
@@ -8922,7 +8928,7 @@
       <c r="Q7" s="24"/>
       <c r="R7" s="24"/>
     </row>
-    <row r="8" spans="1:18" ht="48">
+    <row r="8" spans="1:18" ht="48" hidden="1">
       <c r="A8" s="20" t="str">
         <f t="shared" si="0"/>
         <v>T7</v>
@@ -8964,7 +8970,7 @@
       <c r="Q8" s="24"/>
       <c r="R8" s="24"/>
     </row>
-    <row r="9" spans="1:18" ht="16">
+    <row r="9" spans="1:18" ht="16" hidden="1">
       <c r="A9" s="20" t="str">
         <f t="shared" si="0"/>
         <v>T8</v>
@@ -9006,7 +9012,7 @@
       <c r="Q9" s="24"/>
       <c r="R9" s="24"/>
     </row>
-    <row r="10" spans="1:18" ht="32">
+    <row r="10" spans="1:18" ht="32" hidden="1">
       <c r="A10" s="20" t="str">
         <f t="shared" si="0"/>
         <v>T9</v>
@@ -9048,7 +9054,7 @@
       <c r="Q10" s="24"/>
       <c r="R10" s="24"/>
     </row>
-    <row r="11" spans="1:18" ht="32">
+    <row r="11" spans="1:18" ht="32" hidden="1">
       <c r="A11" s="20" t="str">
         <f t="shared" si="0"/>
         <v>T10</v>
@@ -9090,7 +9096,7 @@
       <c r="Q11" s="24"/>
       <c r="R11" s="24"/>
     </row>
-    <row r="12" spans="1:18" ht="48">
+    <row r="12" spans="1:18" ht="48" hidden="1">
       <c r="A12" s="20" t="str">
         <f t="shared" si="0"/>
         <v>T11</v>
@@ -9132,7 +9138,7 @@
       <c r="Q12" s="24"/>
       <c r="R12" s="24"/>
     </row>
-    <row r="13" spans="1:18" ht="48">
+    <row r="13" spans="1:18" ht="48" hidden="1">
       <c r="A13" s="20" t="str">
         <f t="shared" si="0"/>
         <v>T12</v>
@@ -9174,7 +9180,7 @@
       <c r="Q13" s="24"/>
       <c r="R13" s="24"/>
     </row>
-    <row r="14" spans="1:18" ht="64">
+    <row r="14" spans="1:18" ht="64" hidden="1">
       <c r="A14" s="20" t="str">
         <f t="shared" si="0"/>
         <v>T13</v>
@@ -9216,7 +9222,7 @@
       <c r="Q14" s="24"/>
       <c r="R14" s="24"/>
     </row>
-    <row r="15" spans="1:18" ht="48">
+    <row r="15" spans="1:18" ht="48" hidden="1">
       <c r="A15" s="20" t="str">
         <f t="shared" si="0"/>
         <v>T14</v>
@@ -9258,7 +9264,7 @@
       <c r="Q15" s="24"/>
       <c r="R15" s="24"/>
     </row>
-    <row r="16" spans="1:18" ht="80">
+    <row r="16" spans="1:18" ht="80" hidden="1">
       <c r="A16" s="20" t="str">
         <f t="shared" si="0"/>
         <v>T15</v>
@@ -9300,7 +9306,7 @@
       <c r="Q16" s="24"/>
       <c r="R16" s="24"/>
     </row>
-    <row r="17" spans="1:18" ht="32">
+    <row r="17" spans="1:18" ht="32" hidden="1">
       <c r="A17" s="20" t="str">
         <f t="shared" si="0"/>
         <v>T16</v>
@@ -9342,7 +9348,7 @@
       <c r="Q17" s="24"/>
       <c r="R17" s="24"/>
     </row>
-    <row r="18" spans="1:18" ht="32">
+    <row r="18" spans="1:18" ht="32" hidden="1">
       <c r="A18" s="20" t="str">
         <f t="shared" si="0"/>
         <v>T17</v>
@@ -9384,7 +9390,7 @@
       <c r="Q18" s="24"/>
       <c r="R18" s="24"/>
     </row>
-    <row r="19" spans="1:18" ht="48">
+    <row r="19" spans="1:18" ht="48" hidden="1">
       <c r="A19" s="20" t="str">
         <f t="shared" si="0"/>
         <v>T18</v>
@@ -9426,7 +9432,7 @@
       <c r="Q19" s="24"/>
       <c r="R19" s="24"/>
     </row>
-    <row r="20" spans="1:18" ht="32">
+    <row r="20" spans="1:18" ht="32" hidden="1">
       <c r="A20" s="20" t="str">
         <f t="shared" si="0"/>
         <v>T19</v>
@@ -9468,7 +9474,7 @@
       <c r="Q20" s="24"/>
       <c r="R20" s="24"/>
     </row>
-    <row r="21" spans="1:18" ht="48">
+    <row r="21" spans="1:18" ht="48" hidden="1">
       <c r="A21" s="20" t="str">
         <f t="shared" si="0"/>
         <v>T20</v>
@@ -9510,7 +9516,7 @@
       <c r="Q21" s="24"/>
       <c r="R21" s="24"/>
     </row>
-    <row r="22" spans="1:18" ht="48">
+    <row r="22" spans="1:18" ht="48" hidden="1">
       <c r="A22" s="20" t="str">
         <f t="shared" si="0"/>
         <v>T21</v>
@@ -9552,7 +9558,7 @@
       <c r="Q22" s="24"/>
       <c r="R22" s="24"/>
     </row>
-    <row r="23" spans="1:18" ht="48">
+    <row r="23" spans="1:18" ht="48" hidden="1">
       <c r="A23" s="20" t="str">
         <f t="shared" si="0"/>
         <v>T22</v>
@@ -9594,7 +9600,7 @@
       <c r="Q23" s="24"/>
       <c r="R23" s="24"/>
     </row>
-    <row r="24" spans="1:18" ht="48">
+    <row r="24" spans="1:18" ht="48" hidden="1">
       <c r="A24" s="20" t="str">
         <f t="shared" si="0"/>
         <v>T23</v>
@@ -9636,7 +9642,7 @@
       <c r="Q24" s="24"/>
       <c r="R24" s="24"/>
     </row>
-    <row r="25" spans="1:18" ht="48">
+    <row r="25" spans="1:18" ht="48" hidden="1">
       <c r="A25" s="20" t="str">
         <f t="shared" si="0"/>
         <v>T24</v>
@@ -9692,7 +9698,7 @@
       </c>
       <c r="R25" s="24"/>
     </row>
-    <row r="26" spans="1:18" ht="48">
+    <row r="26" spans="1:18" ht="48" hidden="1">
       <c r="A26" s="20" t="str">
         <f t="shared" si="0"/>
         <v>T25</v>
@@ -9742,7 +9748,7 @@
       <c r="Q26" s="24"/>
       <c r="R26" s="24"/>
     </row>
-    <row r="27" spans="1:18" ht="48">
+    <row r="27" spans="1:18" ht="48" hidden="1">
       <c r="A27" s="20" t="str">
         <f t="shared" si="0"/>
         <v>T26</v>
@@ -9792,7 +9798,7 @@
       <c r="Q27" s="24"/>
       <c r="R27" s="24"/>
     </row>
-    <row r="28" spans="1:18" ht="64">
+    <row r="28" spans="1:18" ht="64" hidden="1">
       <c r="A28" s="20" t="str">
         <f t="shared" si="0"/>
         <v>T27</v>
@@ -9842,7 +9848,7 @@
       <c r="Q28" s="24"/>
       <c r="R28" s="24"/>
     </row>
-    <row r="29" spans="1:18" ht="32">
+    <row r="29" spans="1:18" ht="32" hidden="1">
       <c r="A29" s="20" t="str">
         <f t="shared" si="0"/>
         <v>T28</v>
@@ -9892,7 +9898,7 @@
       <c r="Q29" s="24"/>
       <c r="R29" s="24"/>
     </row>
-    <row r="30" spans="1:18" ht="48">
+    <row r="30" spans="1:18" ht="48" hidden="1">
       <c r="A30" s="20" t="str">
         <f t="shared" si="0"/>
         <v>T29</v>
@@ -9942,7 +9948,7 @@
       <c r="Q30" s="24"/>
       <c r="R30" s="24"/>
     </row>
-    <row r="31" spans="1:18" ht="48">
+    <row r="31" spans="1:18" ht="48" hidden="1">
       <c r="A31" s="20" t="str">
         <f t="shared" si="0"/>
         <v>T30</v>
@@ -9992,7 +9998,7 @@
       <c r="Q31" s="24"/>
       <c r="R31" s="24"/>
     </row>
-    <row r="32" spans="1:18" ht="32">
+    <row r="32" spans="1:18" ht="32" hidden="1">
       <c r="A32" s="20" t="str">
         <f t="shared" si="0"/>
         <v>T31</v>
@@ -10042,7 +10048,7 @@
       <c r="Q32" s="24"/>
       <c r="R32" s="24"/>
     </row>
-    <row r="33" spans="1:18" ht="48">
+    <row r="33" spans="1:18" ht="48" hidden="1">
       <c r="A33" s="20" t="str">
         <f t="shared" si="0"/>
         <v>T32</v>
@@ -10092,7 +10098,7 @@
       <c r="Q33" s="24"/>
       <c r="R33" s="24"/>
     </row>
-    <row r="34" spans="1:18" ht="32">
+    <row r="34" spans="1:18" ht="32" hidden="1">
       <c r="A34" s="20" t="str">
         <f t="shared" si="0"/>
         <v>T33</v>
@@ -10142,7 +10148,7 @@
       <c r="Q34" s="24"/>
       <c r="R34" s="24"/>
     </row>
-    <row r="35" spans="1:18" ht="32">
+    <row r="35" spans="1:18" ht="32" hidden="1">
       <c r="A35" s="20" t="str">
         <f t="shared" si="0"/>
         <v>T34</v>
@@ -10192,7 +10198,7 @@
       <c r="Q35" s="24"/>
       <c r="R35" s="24"/>
     </row>
-    <row r="36" spans="1:18" ht="48">
+    <row r="36" spans="1:18" ht="48" hidden="1">
       <c r="A36" s="20" t="str">
         <f t="shared" si="0"/>
         <v>T35</v>
@@ -10242,7 +10248,7 @@
       <c r="Q36" s="24"/>
       <c r="R36" s="24"/>
     </row>
-    <row r="37" spans="1:18" ht="32">
+    <row r="37" spans="1:18" ht="32" hidden="1">
       <c r="A37" s="20" t="str">
         <f t="shared" si="0"/>
         <v>T36</v>
@@ -10292,7 +10298,7 @@
       <c r="Q37" s="24"/>
       <c r="R37" s="24"/>
     </row>
-    <row r="38" spans="1:18" ht="16">
+    <row r="38" spans="1:18" ht="16" hidden="1">
       <c r="A38" s="20" t="str">
         <f t="shared" si="0"/>
         <v>T37</v>
@@ -10342,7 +10348,7 @@
       <c r="Q38" s="24"/>
       <c r="R38" s="24"/>
     </row>
-    <row r="39" spans="1:18" ht="16">
+    <row r="39" spans="1:18" ht="16" hidden="1">
       <c r="A39" s="20" t="str">
         <f t="shared" si="0"/>
         <v>T38</v>
@@ -10392,7 +10398,7 @@
       <c r="Q39" s="24"/>
       <c r="R39" s="24"/>
     </row>
-    <row r="40" spans="1:18" ht="32">
+    <row r="40" spans="1:18" ht="32" hidden="1">
       <c r="A40" s="20" t="str">
         <f t="shared" si="0"/>
         <v>T39</v>
@@ -10442,7 +10448,7 @@
       <c r="Q40" s="24"/>
       <c r="R40" s="24"/>
     </row>
-    <row r="41" spans="1:18" ht="32">
+    <row r="41" spans="1:18" ht="32" hidden="1">
       <c r="A41" s="20" t="str">
         <f t="shared" si="0"/>
         <v>T40</v>
@@ -10492,7 +10498,7 @@
       <c r="Q41" s="24"/>
       <c r="R41" s="24"/>
     </row>
-    <row r="42" spans="1:18" ht="48">
+    <row r="42" spans="1:18" ht="48" hidden="1">
       <c r="A42" s="20" t="str">
         <f t="shared" si="0"/>
         <v>T41</v>
@@ -10542,7 +10548,7 @@
       <c r="Q42" s="24"/>
       <c r="R42" s="24"/>
     </row>
-    <row r="43" spans="1:18" ht="48">
+    <row r="43" spans="1:18" ht="48" hidden="1">
       <c r="A43" s="20" t="str">
         <f t="shared" si="0"/>
         <v>T42</v>
@@ -10592,7 +10598,7 @@
       <c r="Q43" s="24"/>
       <c r="R43" s="24"/>
     </row>
-    <row r="44" spans="1:18" ht="16">
+    <row r="44" spans="1:18" ht="16" hidden="1">
       <c r="A44" s="20" t="str">
         <f t="shared" si="0"/>
         <v>T43</v>
@@ -10642,7 +10648,7 @@
       <c r="Q44" s="24"/>
       <c r="R44" s="24"/>
     </row>
-    <row r="45" spans="1:18" ht="48">
+    <row r="45" spans="1:18" ht="48" hidden="1">
       <c r="A45" s="20" t="str">
         <f t="shared" si="0"/>
         <v>T44</v>
@@ -10692,7 +10698,7 @@
       <c r="Q45" s="24"/>
       <c r="R45" s="24"/>
     </row>
-    <row r="46" spans="1:18" ht="48">
+    <row r="46" spans="1:18" ht="48" hidden="1">
       <c r="A46" s="20" t="str">
         <f t="shared" si="0"/>
         <v>T45</v>
@@ -10742,7 +10748,7 @@
       <c r="Q46" s="24"/>
       <c r="R46" s="24"/>
     </row>
-    <row r="47" spans="1:18" ht="32">
+    <row r="47" spans="1:18" ht="32" hidden="1">
       <c r="A47" s="20" t="str">
         <f t="shared" si="0"/>
         <v>T46</v>
@@ -10792,7 +10798,7 @@
       <c r="Q47" s="24"/>
       <c r="R47" s="24"/>
     </row>
-    <row r="48" spans="1:18" ht="32">
+    <row r="48" spans="1:18" ht="32" hidden="1">
       <c r="A48" s="20" t="str">
         <f t="shared" si="0"/>
         <v>T47</v>
@@ -10842,7 +10848,7 @@
       <c r="Q48" s="24"/>
       <c r="R48" s="24"/>
     </row>
-    <row r="49" spans="1:18" ht="48">
+    <row r="49" spans="1:18" ht="48" hidden="1">
       <c r="A49" s="20" t="str">
         <f t="shared" si="0"/>
         <v>T48</v>
@@ -10892,7 +10898,7 @@
       <c r="Q49" s="24"/>
       <c r="R49" s="24"/>
     </row>
-    <row r="50" spans="1:18" ht="32">
+    <row r="50" spans="1:18" ht="32" hidden="1">
       <c r="A50" s="20" t="str">
         <f t="shared" si="0"/>
         <v>T49</v>
@@ -10942,7 +10948,7 @@
       <c r="Q50" s="24"/>
       <c r="R50" s="24"/>
     </row>
-    <row r="51" spans="1:18" ht="32">
+    <row r="51" spans="1:18" ht="32" hidden="1">
       <c r="A51" s="20" t="str">
         <f t="shared" si="0"/>
         <v>T50</v>
@@ -10992,7 +10998,7 @@
       <c r="Q51" s="24"/>
       <c r="R51" s="24"/>
     </row>
-    <row r="52" spans="1:18" ht="32">
+    <row r="52" spans="1:18" ht="32" hidden="1">
       <c r="A52" s="20" t="str">
         <f t="shared" si="0"/>
         <v>T51</v>
@@ -11042,7 +11048,7 @@
       <c r="Q52" s="24"/>
       <c r="R52" s="24"/>
     </row>
-    <row r="53" spans="1:18" ht="32">
+    <row r="53" spans="1:18" ht="32" hidden="1">
       <c r="A53" s="20" t="str">
         <f t="shared" si="0"/>
         <v>T52</v>
@@ -11092,7 +11098,7 @@
       <c r="Q53" s="24"/>
       <c r="R53" s="24"/>
     </row>
-    <row r="54" spans="1:18" ht="48">
+    <row r="54" spans="1:18" ht="48" hidden="1">
       <c r="A54" s="20" t="str">
         <f t="shared" si="0"/>
         <v>T53</v>
@@ -11142,7 +11148,7 @@
       <c r="Q54" s="24"/>
       <c r="R54" s="24"/>
     </row>
-    <row r="55" spans="1:18" ht="32">
+    <row r="55" spans="1:18" ht="32" hidden="1">
       <c r="A55" s="20" t="str">
         <f t="shared" si="0"/>
         <v>T54</v>
@@ -11192,7 +11198,7 @@
       <c r="Q55" s="24"/>
       <c r="R55" s="24"/>
     </row>
-    <row r="56" spans="1:18" ht="48">
+    <row r="56" spans="1:18" ht="48" hidden="1">
       <c r="A56" s="20" t="str">
         <f t="shared" si="0"/>
         <v>T55</v>
@@ -11242,7 +11248,7 @@
       <c r="Q56" s="24"/>
       <c r="R56" s="24"/>
     </row>
-    <row r="57" spans="1:18" ht="32">
+    <row r="57" spans="1:18" ht="32" hidden="1">
       <c r="A57" s="20" t="str">
         <f t="shared" si="0"/>
         <v>T56</v>
@@ -11292,7 +11298,7 @@
       <c r="Q57" s="24"/>
       <c r="R57" s="24"/>
     </row>
-    <row r="58" spans="1:18" ht="80">
+    <row r="58" spans="1:18" ht="80" hidden="1">
       <c r="A58" s="20" t="str">
         <f t="shared" si="0"/>
         <v>T57</v>
@@ -11342,7 +11348,7 @@
       <c r="Q58" s="24"/>
       <c r="R58" s="24"/>
     </row>
-    <row r="59" spans="1:18" ht="32">
+    <row r="59" spans="1:18" ht="32" hidden="1">
       <c r="A59" s="20" t="str">
         <f t="shared" si="0"/>
         <v>T58</v>
@@ -11392,7 +11398,7 @@
       <c r="Q59" s="24"/>
       <c r="R59" s="24"/>
     </row>
-    <row r="60" spans="1:18" ht="32">
+    <row r="60" spans="1:18" ht="32" hidden="1">
       <c r="A60" s="20" t="str">
         <f t="shared" si="0"/>
         <v>T59</v>
@@ -11991,7 +11997,7 @@
         <v>904</v>
       </c>
     </row>
-    <row r="70" spans="1:18" ht="144">
+    <row r="70" spans="1:18" ht="144" hidden="1">
       <c r="A70" s="20" t="str">
         <f t="shared" si="11"/>
         <v>T69</v>
@@ -12052,7 +12058,7 @@
       </c>
       <c r="R70" s="24"/>
     </row>
-    <row r="71" spans="1:18" ht="96">
+    <row r="71" spans="1:18" ht="96" hidden="1">
       <c r="A71" s="20" t="str">
         <f t="shared" si="11"/>
         <v>T70</v>
@@ -12113,7 +12119,7 @@
       </c>
       <c r="R71" s="24"/>
     </row>
-    <row r="72" spans="1:18" ht="32">
+    <row r="72" spans="1:18" ht="32" hidden="1">
       <c r="A72" s="20" t="str">
         <f t="shared" si="11"/>
         <v>T71</v>
@@ -12170,7 +12176,7 @@
         <v>864</v>
       </c>
     </row>
-    <row r="73" spans="1:18" ht="48">
+    <row r="73" spans="1:18" ht="48" hidden="1">
       <c r="A73" s="20" t="str">
         <f t="shared" si="11"/>
         <v>T72</v>
@@ -12231,7 +12237,7 @@
       </c>
       <c r="R73" s="24"/>
     </row>
-    <row r="74" spans="1:18" ht="48">
+    <row r="74" spans="1:18" ht="48" hidden="1">
       <c r="A74" s="20" t="str">
         <f t="shared" si="11"/>
         <v>T73</v>
@@ -12292,7 +12298,7 @@
       </c>
       <c r="R74" s="24"/>
     </row>
-    <row r="75" spans="1:18" ht="32">
+    <row r="75" spans="1:18" ht="32" hidden="1">
       <c r="A75" s="20" t="str">
         <f t="shared" si="11"/>
         <v>T74</v>
@@ -12353,7 +12359,7 @@
       </c>
       <c r="R75" s="24"/>
     </row>
-    <row r="76" spans="1:18" ht="80">
+    <row r="76" spans="1:18" ht="80" hidden="1">
       <c r="A76" s="20" t="str">
         <f t="shared" si="11"/>
         <v>T75</v>
@@ -12414,7 +12420,7 @@
       </c>
       <c r="R76" s="24"/>
     </row>
-    <row r="77" spans="1:18" ht="160">
+    <row r="77" spans="1:18" ht="160" hidden="1">
       <c r="A77" s="20" t="str">
         <f t="shared" si="11"/>
         <v>T76</v>
@@ -12475,7 +12481,7 @@
       </c>
       <c r="R77" s="24"/>
     </row>
-    <row r="78" spans="1:18" ht="128">
+    <row r="78" spans="1:18" ht="128" hidden="1">
       <c r="A78" s="20" t="str">
         <f t="shared" si="11"/>
         <v>T77</v>
@@ -12534,7 +12540,7 @@
       <c r="Q78" s="24"/>
       <c r="R78" s="24"/>
     </row>
-    <row r="79" spans="1:18" ht="80">
+    <row r="79" spans="1:18" ht="80" hidden="1">
       <c r="A79" s="20" t="str">
         <f t="shared" si="11"/>
         <v>T78</v>
@@ -12595,7 +12601,7 @@
       </c>
       <c r="R79" s="24"/>
     </row>
-    <row r="80" spans="1:18" ht="96">
+    <row r="80" spans="1:18" ht="96" hidden="1">
       <c r="A80" s="20" t="str">
         <f t="shared" si="11"/>
         <v>T79</v>
@@ -12656,7 +12662,7 @@
       </c>
       <c r="R80" s="24"/>
     </row>
-    <row r="81" spans="1:18" ht="96">
+    <row r="81" spans="1:18" ht="96" hidden="1">
       <c r="A81" s="20" t="str">
         <f t="shared" si="11"/>
         <v>T80</v>
@@ -12717,7 +12723,7 @@
       </c>
       <c r="R81" s="24"/>
     </row>
-    <row r="82" spans="1:18" ht="240">
+    <row r="82" spans="1:18" ht="240" hidden="1">
       <c r="A82" s="20" t="str">
         <f t="shared" si="11"/>
         <v>T81</v>
@@ -12778,7 +12784,7 @@
       </c>
       <c r="R82" s="24"/>
     </row>
-    <row r="83" spans="1:18" ht="32">
+    <row r="83" spans="1:18" ht="32" hidden="1">
       <c r="A83" s="20" t="str">
         <f t="shared" si="11"/>
         <v>T82</v>
@@ -12829,7 +12835,7 @@
       <c r="Q83" s="24"/>
       <c r="R83" s="24"/>
     </row>
-    <row r="84" spans="1:18" ht="16">
+    <row r="84" spans="1:18" ht="16" hidden="1">
       <c r="A84" s="20" t="str">
         <f t="shared" si="11"/>
         <v>T83</v>
@@ -12880,7 +12886,7 @@
       <c r="Q84" s="24"/>
       <c r="R84" s="24"/>
     </row>
-    <row r="85" spans="1:18" ht="16">
+    <row r="85" spans="1:18" ht="16" hidden="1">
       <c r="A85" s="20" t="str">
         <f t="shared" si="11"/>
         <v>T84</v>
@@ -12931,7 +12937,7 @@
       <c r="Q85" s="24"/>
       <c r="R85" s="24"/>
     </row>
-    <row r="86" spans="1:18" ht="96">
+    <row r="86" spans="1:18" ht="96" hidden="1">
       <c r="A86" s="20" t="str">
         <f t="shared" si="11"/>
         <v>T85</v>
@@ -12982,7 +12988,7 @@
       <c r="Q86" s="24"/>
       <c r="R86" s="24"/>
     </row>
-    <row r="87" spans="1:18" ht="64">
+    <row r="87" spans="1:18" ht="64" hidden="1">
       <c r="A87" s="20" t="str">
         <f t="shared" si="11"/>
         <v>T86</v>
@@ -13033,7 +13039,7 @@
       <c r="Q87" s="24"/>
       <c r="R87" s="24"/>
     </row>
-    <row r="88" spans="1:18" ht="32">
+    <row r="88" spans="1:18" ht="32" hidden="1">
       <c r="A88" s="20" t="str">
         <f t="shared" si="11"/>
         <v>T87</v>
@@ -13084,7 +13090,7 @@
       <c r="Q88" s="24"/>
       <c r="R88" s="24"/>
     </row>
-    <row r="89" spans="1:18" ht="16">
+    <row r="89" spans="1:18" ht="16" hidden="1">
       <c r="A89" s="20" t="str">
         <f t="shared" si="11"/>
         <v>T88</v>
@@ -13135,7 +13141,7 @@
       <c r="Q89" s="24"/>
       <c r="R89" s="24"/>
     </row>
-    <row r="90" spans="1:18" ht="32">
+    <row r="90" spans="1:18" ht="32" hidden="1">
       <c r="A90" s="20" t="str">
         <f t="shared" si="11"/>
         <v>T89</v>
@@ -13186,7 +13192,7 @@
       <c r="Q90" s="24"/>
       <c r="R90" s="24"/>
     </row>
-    <row r="91" spans="1:18" ht="48">
+    <row r="91" spans="1:18" ht="48" hidden="1">
       <c r="A91" s="20" t="str">
         <f t="shared" si="11"/>
         <v>T90</v>
@@ -13237,7 +13243,7 @@
       <c r="Q91" s="24"/>
       <c r="R91" s="24"/>
     </row>
-    <row r="92" spans="1:18" ht="96">
+    <row r="92" spans="1:18" ht="96" hidden="1">
       <c r="A92" s="20" t="str">
         <f t="shared" si="11"/>
         <v>T91</v>
@@ -13288,7 +13294,7 @@
       <c r="Q92" s="24"/>
       <c r="R92" s="24"/>
     </row>
-    <row r="93" spans="1:18" ht="64">
+    <row r="93" spans="1:18" ht="64" hidden="1">
       <c r="A93" s="20" t="str">
         <f t="shared" si="11"/>
         <v>T92</v>
@@ -13339,7 +13345,7 @@
       <c r="Q93" s="24"/>
       <c r="R93" s="24"/>
     </row>
-    <row r="94" spans="1:18" ht="48">
+    <row r="94" spans="1:18" ht="48" hidden="1">
       <c r="A94" s="20" t="str">
         <f t="shared" si="11"/>
         <v>T93</v>
@@ -13390,7 +13396,7 @@
       <c r="Q94" s="24"/>
       <c r="R94" s="24"/>
     </row>
-    <row r="95" spans="1:18" ht="32">
+    <row r="95" spans="1:18" ht="32" hidden="1">
       <c r="A95" s="20" t="str">
         <f t="shared" si="11"/>
         <v>T94</v>
@@ -13441,7 +13447,7 @@
       <c r="Q95" s="24"/>
       <c r="R95" s="24"/>
     </row>
-    <row r="96" spans="1:18" ht="32">
+    <row r="96" spans="1:18" ht="32" hidden="1">
       <c r="A96" s="20" t="str">
         <f t="shared" si="11"/>
         <v>T95</v>
@@ -13492,7 +13498,7 @@
       <c r="Q96" s="24"/>
       <c r="R96" s="24"/>
     </row>
-    <row r="97" spans="1:18" ht="32">
+    <row r="97" spans="1:18" ht="32" hidden="1">
       <c r="A97" s="20" t="str">
         <f t="shared" si="11"/>
         <v>T96</v>
@@ -13543,7 +13549,7 @@
       <c r="Q97" s="24"/>
       <c r="R97" s="24"/>
     </row>
-    <row r="98" spans="1:18" ht="64">
+    <row r="98" spans="1:18" ht="64" hidden="1">
       <c r="A98" s="20" t="str">
         <f t="shared" si="11"/>
         <v>T97</v>
@@ -13594,7 +13600,7 @@
       <c r="Q98" s="24"/>
       <c r="R98" s="24"/>
     </row>
-    <row r="99" spans="1:18" ht="48">
+    <row r="99" spans="1:18" ht="48" hidden="1">
       <c r="A99" s="20" t="str">
         <f t="shared" si="11"/>
         <v>T98</v>
@@ -13645,7 +13651,7 @@
       <c r="Q99" s="24"/>
       <c r="R99" s="24"/>
     </row>
-    <row r="100" spans="1:18" ht="32">
+    <row r="100" spans="1:18" ht="32" hidden="1">
       <c r="A100" s="20" t="str">
         <f t="shared" si="11"/>
         <v>T99</v>
@@ -13706,7 +13712,7 @@
       </c>
       <c r="R100" s="24"/>
     </row>
-    <row r="101" spans="1:18" ht="48">
+    <row r="101" spans="1:18" ht="48" hidden="1">
       <c r="A101" s="20" t="str">
         <f t="shared" si="11"/>
         <v>T100</v>
@@ -13763,7 +13769,7 @@
       <c r="Q101" s="24"/>
       <c r="R101" s="24"/>
     </row>
-    <row r="102" spans="1:18" ht="48">
+    <row r="102" spans="1:18" ht="48" hidden="1">
       <c r="A102" s="20" t="str">
         <f t="shared" si="11"/>
         <v>T101</v>
@@ -13820,7 +13826,7 @@
       <c r="Q102" s="24"/>
       <c r="R102" s="24"/>
     </row>
-    <row r="103" spans="1:18" ht="112">
+    <row r="103" spans="1:18" ht="112" hidden="1">
       <c r="A103" s="20" t="str">
         <f t="shared" si="11"/>
         <v>T102</v>
@@ -13877,7 +13883,7 @@
         <v>862</v>
       </c>
     </row>
-    <row r="104" spans="1:18" ht="64">
+    <row r="104" spans="1:18" ht="64" hidden="1">
       <c r="A104" s="20" t="str">
         <f t="shared" si="11"/>
         <v>T103</v>
@@ -13938,7 +13944,7 @@
       </c>
       <c r="R104" s="24"/>
     </row>
-    <row r="105" spans="1:18" ht="32">
+    <row r="105" spans="1:18" ht="32" hidden="1">
       <c r="A105" s="20" t="str">
         <f t="shared" si="11"/>
         <v>T104</v>
@@ -13999,7 +14005,7 @@
       </c>
       <c r="R105" s="24"/>
     </row>
-    <row r="106" spans="1:18" ht="32">
+    <row r="106" spans="1:18" ht="32" hidden="1">
       <c r="A106" s="20" t="str">
         <f t="shared" si="11"/>
         <v>T105</v>
@@ -14056,7 +14062,7 @@
       <c r="Q106" s="24"/>
       <c r="R106" s="24"/>
     </row>
-    <row r="107" spans="1:18" ht="144">
+    <row r="107" spans="1:18" ht="144" hidden="1">
       <c r="A107" s="20" t="str">
         <f t="shared" si="11"/>
         <v>T106</v>
@@ -14117,7 +14123,7 @@
         <v>861</v>
       </c>
     </row>
-    <row r="108" spans="1:18" ht="32">
+    <row r="108" spans="1:18" ht="32" hidden="1">
       <c r="A108" s="20" t="str">
         <f t="shared" si="11"/>
         <v>T107</v>
@@ -14174,7 +14180,7 @@
       <c r="Q108" s="25"/>
       <c r="R108" s="25"/>
     </row>
-    <row r="109" spans="1:18" ht="32">
+    <row r="109" spans="1:18" ht="32" hidden="1">
       <c r="A109" s="20" t="str">
         <f t="shared" si="11"/>
         <v>T108</v>
@@ -14230,7 +14236,7 @@
       <c r="Q109" s="25"/>
       <c r="R109" s="25"/>
     </row>
-    <row r="110" spans="1:18" ht="16">
+    <row r="110" spans="1:18" ht="16" hidden="1">
       <c r="A110" s="20" t="str">
         <f t="shared" si="11"/>
         <v>T109</v>
@@ -14287,7 +14293,7 @@
       <c r="Q110" s="24"/>
       <c r="R110" s="24"/>
     </row>
-    <row r="111" spans="1:18" ht="32">
+    <row r="111" spans="1:18" ht="32" hidden="1">
       <c r="A111" s="20" t="str">
         <f t="shared" si="11"/>
         <v>T110</v>
@@ -14344,7 +14350,7 @@
       <c r="Q111" s="24"/>
       <c r="R111" s="24"/>
     </row>
-    <row r="112" spans="1:18" ht="48">
+    <row r="112" spans="1:18" ht="48" hidden="1">
       <c r="A112" s="20" t="str">
         <f t="shared" si="11"/>
         <v>T111</v>
@@ -14395,7 +14401,7 @@
       <c r="Q112" s="24"/>
       <c r="R112" s="24"/>
     </row>
-    <row r="113" spans="1:18" ht="80">
+    <row r="113" spans="1:18" ht="80" hidden="1">
       <c r="A113" s="20" t="str">
         <f t="shared" si="11"/>
         <v>T112</v>
@@ -14446,7 +14452,7 @@
       <c r="Q113" s="24"/>
       <c r="R113" s="24"/>
     </row>
-    <row r="114" spans="1:18" ht="64">
+    <row r="114" spans="1:18" ht="64" hidden="1">
       <c r="A114" s="20" t="str">
         <f t="shared" si="11"/>
         <v>T113</v>
@@ -14497,7 +14503,7 @@
       <c r="Q114" s="24"/>
       <c r="R114" s="24"/>
     </row>
-    <row r="115" spans="1:18" ht="48">
+    <row r="115" spans="1:18" ht="48" hidden="1">
       <c r="A115" s="20" t="str">
         <f t="shared" si="11"/>
         <v>T114</v>
@@ -14548,7 +14554,7 @@
       <c r="Q115" s="24"/>
       <c r="R115" s="24"/>
     </row>
-    <row r="116" spans="1:18" ht="48">
+    <row r="116" spans="1:18" ht="48" hidden="1">
       <c r="A116" s="20" t="str">
         <f t="shared" si="11"/>
         <v>T115</v>
@@ -14599,7 +14605,7 @@
       <c r="Q116" s="24"/>
       <c r="R116" s="24"/>
     </row>
-    <row r="117" spans="1:18" ht="16">
+    <row r="117" spans="1:18" ht="16" hidden="1">
       <c r="A117" s="20" t="str">
         <f t="shared" si="11"/>
         <v>T116</v>
@@ -14650,7 +14656,7 @@
       <c r="Q117" s="24"/>
       <c r="R117" s="24"/>
     </row>
-    <row r="118" spans="1:18" ht="16">
+    <row r="118" spans="1:18" ht="16" hidden="1">
       <c r="A118" s="20" t="str">
         <f t="shared" si="11"/>
         <v>T117</v>
@@ -14701,7 +14707,7 @@
       <c r="Q118" s="24"/>
       <c r="R118" s="24"/>
     </row>
-    <row r="119" spans="1:18" ht="48">
+    <row r="119" spans="1:18" ht="48" hidden="1">
       <c r="A119" s="20" t="str">
         <f t="shared" si="11"/>
         <v>T118</v>
@@ -14752,7 +14758,7 @@
       <c r="Q119" s="24"/>
       <c r="R119" s="24"/>
     </row>
-    <row r="120" spans="1:18" ht="96">
+    <row r="120" spans="1:18" ht="96" hidden="1">
       <c r="A120" s="20" t="str">
         <f t="shared" si="11"/>
         <v>T119</v>
@@ -14803,7 +14809,7 @@
       <c r="Q120" s="24"/>
       <c r="R120" s="24"/>
     </row>
-    <row r="121" spans="1:18" ht="64">
+    <row r="121" spans="1:18" ht="64" hidden="1">
       <c r="A121" s="20" t="str">
         <f t="shared" si="11"/>
         <v>T120</v>
@@ -14854,7 +14860,7 @@
       <c r="Q121" s="24"/>
       <c r="R121" s="24"/>
     </row>
-    <row r="122" spans="1:18" ht="48">
+    <row r="122" spans="1:18" ht="48" hidden="1">
       <c r="A122" s="20" t="str">
         <f t="shared" si="11"/>
         <v>T121</v>
@@ -14905,7 +14911,7 @@
       <c r="Q122" s="24"/>
       <c r="R122" s="24"/>
     </row>
-    <row r="123" spans="1:18" ht="48">
+    <row r="123" spans="1:18" ht="48" hidden="1">
       <c r="A123" s="20" t="str">
         <f t="shared" si="11"/>
         <v>T122</v>
@@ -14956,7 +14962,7 @@
       <c r="Q123" s="24"/>
       <c r="R123" s="24"/>
     </row>
-    <row r="124" spans="1:18" ht="16">
+    <row r="124" spans="1:18" ht="16" hidden="1">
       <c r="A124" s="20" t="str">
         <f t="shared" si="11"/>
         <v>T123</v>
@@ -15007,7 +15013,7 @@
       <c r="Q124" s="24"/>
       <c r="R124" s="24"/>
     </row>
-    <row r="125" spans="1:18" ht="32">
+    <row r="125" spans="1:18" ht="32" hidden="1">
       <c r="A125" s="20" t="str">
         <f t="shared" si="11"/>
         <v>T124</v>
@@ -15058,7 +15064,7 @@
       <c r="Q125" s="24"/>
       <c r="R125" s="24"/>
     </row>
-    <row r="126" spans="1:18" ht="16">
+    <row r="126" spans="1:18" ht="16" hidden="1">
       <c r="A126" s="20" t="str">
         <f t="shared" si="11"/>
         <v>T125</v>
@@ -15109,7 +15115,7 @@
       <c r="Q126" s="24"/>
       <c r="R126" s="24"/>
     </row>
-    <row r="127" spans="1:18" ht="64">
+    <row r="127" spans="1:18" ht="64" hidden="1">
       <c r="A127" s="20" t="str">
         <f t="shared" si="11"/>
         <v>T126</v>
@@ -15160,7 +15166,7 @@
       <c r="Q127" s="24"/>
       <c r="R127" s="24"/>
     </row>
-    <row r="128" spans="1:18" ht="48">
+    <row r="128" spans="1:18" ht="48" hidden="1">
       <c r="A128" s="20" t="str">
         <f t="shared" si="11"/>
         <v>T127</v>
@@ -15199,7 +15205,7 @@
       <c r="Q128" s="24"/>
       <c r="R128" s="24"/>
     </row>
-    <row r="129" spans="1:18" ht="96">
+    <row r="129" spans="1:18" ht="96" hidden="1">
       <c r="A129" s="20" t="str">
         <f t="shared" si="11"/>
         <v>T128</v>
@@ -15238,7 +15244,7 @@
       <c r="Q129" s="24"/>
       <c r="R129" s="24"/>
     </row>
-    <row r="130" spans="1:18" ht="32">
+    <row r="130" spans="1:18" ht="32" hidden="1">
       <c r="A130" s="20" t="str">
         <f t="shared" ref="A130:A193" si="22">CONCATENATE("T",ROW(A130)-1)</f>
         <v>T129</v>
@@ -15289,7 +15295,7 @@
       <c r="Q130" s="24"/>
       <c r="R130" s="24"/>
     </row>
-    <row r="131" spans="1:18" ht="64">
+    <row r="131" spans="1:18" ht="64" hidden="1">
       <c r="A131" s="20" t="str">
         <f t="shared" si="22"/>
         <v>T130</v>
@@ -15340,7 +15346,7 @@
       <c r="Q131" s="24"/>
       <c r="R131" s="24"/>
     </row>
-    <row r="132" spans="1:18" ht="48">
+    <row r="132" spans="1:18" ht="48" hidden="1">
       <c r="A132" s="20" t="str">
         <f t="shared" si="22"/>
         <v>T131</v>
@@ -15391,7 +15397,7 @@
       <c r="Q132" s="24"/>
       <c r="R132" s="24"/>
     </row>
-    <row r="133" spans="1:18" ht="32">
+    <row r="133" spans="1:18" ht="32" hidden="1">
       <c r="A133" s="20" t="str">
         <f t="shared" si="22"/>
         <v>T132</v>
@@ -15442,7 +15448,7 @@
       <c r="Q133" s="24"/>
       <c r="R133" s="24"/>
     </row>
-    <row r="134" spans="1:18" ht="48">
+    <row r="134" spans="1:18" ht="48" hidden="1">
       <c r="A134" s="20" t="str">
         <f t="shared" si="22"/>
         <v>T133</v>
@@ -15493,7 +15499,7 @@
       <c r="Q134" s="24"/>
       <c r="R134" s="24"/>
     </row>
-    <row r="135" spans="1:18" ht="48">
+    <row r="135" spans="1:18" ht="48" hidden="1">
       <c r="A135" s="20" t="str">
         <f t="shared" si="22"/>
         <v>T134</v>
@@ -15544,7 +15550,7 @@
       <c r="Q135" s="24"/>
       <c r="R135" s="24"/>
     </row>
-    <row r="136" spans="1:18" ht="64">
+    <row r="136" spans="1:18" ht="64" hidden="1">
       <c r="A136" s="20" t="str">
         <f t="shared" si="22"/>
         <v>T135</v>
@@ -15595,7 +15601,7 @@
       <c r="Q136" s="24"/>
       <c r="R136" s="24"/>
     </row>
-    <row r="137" spans="1:18" ht="48">
+    <row r="137" spans="1:18" ht="48" hidden="1">
       <c r="A137" s="20" t="str">
         <f t="shared" si="22"/>
         <v>T136</v>
@@ -15656,7 +15662,7 @@
       </c>
       <c r="R137" s="25"/>
     </row>
-    <row r="138" spans="1:18" ht="96">
+    <row r="138" spans="1:18" ht="96" hidden="1">
       <c r="A138" s="20" t="str">
         <f t="shared" si="22"/>
         <v>T137</v>
@@ -15707,7 +15713,7 @@
       <c r="Q138" s="24"/>
       <c r="R138" s="24"/>
     </row>
-    <row r="139" spans="1:18" ht="80">
+    <row r="139" spans="1:18" ht="80" hidden="1">
       <c r="A139" s="20" t="str">
         <f t="shared" si="22"/>
         <v>T138</v>
@@ -15758,7 +15764,7 @@
       <c r="Q139" s="24"/>
       <c r="R139" s="24"/>
     </row>
-    <row r="140" spans="1:18" ht="96">
+    <row r="140" spans="1:18" ht="96" hidden="1">
       <c r="A140" s="20" t="str">
         <f t="shared" si="22"/>
         <v>T139</v>
@@ -15809,7 +15815,7 @@
       <c r="Q140" s="24"/>
       <c r="R140" s="24"/>
     </row>
-    <row r="141" spans="1:18" ht="48">
+    <row r="141" spans="1:18" ht="48" hidden="1">
       <c r="A141" s="20" t="str">
         <f t="shared" si="22"/>
         <v>T140</v>
@@ -15860,7 +15866,7 @@
       <c r="Q141" s="24"/>
       <c r="R141" s="24"/>
     </row>
-    <row r="142" spans="1:18" ht="80">
+    <row r="142" spans="1:18" ht="80" hidden="1">
       <c r="A142" s="20" t="str">
         <f t="shared" si="22"/>
         <v>T141</v>
@@ -15911,7 +15917,7 @@
       <c r="Q142" s="24"/>
       <c r="R142" s="24"/>
     </row>
-    <row r="143" spans="1:18" ht="48">
+    <row r="143" spans="1:18" ht="48" hidden="1">
       <c r="A143" s="20" t="str">
         <f t="shared" si="22"/>
         <v>T142</v>
@@ -15962,7 +15968,7 @@
       <c r="Q143" s="24"/>
       <c r="R143" s="24"/>
     </row>
-    <row r="144" spans="1:18" ht="32">
+    <row r="144" spans="1:18" ht="32" hidden="1">
       <c r="A144" s="20" t="str">
         <f t="shared" si="22"/>
         <v>T143</v>
@@ -16013,7 +16019,7 @@
       <c r="Q144" s="24"/>
       <c r="R144" s="24"/>
     </row>
-    <row r="145" spans="1:18" ht="32">
+    <row r="145" spans="1:18" ht="32" hidden="1">
       <c r="A145" s="20" t="str">
         <f t="shared" si="22"/>
         <v>T144</v>
@@ -16064,7 +16070,7 @@
       <c r="Q145" s="24"/>
       <c r="R145" s="24"/>
     </row>
-    <row r="146" spans="1:18" ht="80">
+    <row r="146" spans="1:18" ht="80" hidden="1">
       <c r="A146" s="20" t="str">
         <f t="shared" si="22"/>
         <v>T145</v>
@@ -16115,7 +16121,7 @@
       <c r="Q146" s="24"/>
       <c r="R146" s="24"/>
     </row>
-    <row r="147" spans="1:18" ht="64">
+    <row r="147" spans="1:18" ht="64" hidden="1">
       <c r="A147" s="20" t="str">
         <f t="shared" si="22"/>
         <v>T146</v>
@@ -16166,7 +16172,7 @@
       <c r="Q147" s="24"/>
       <c r="R147" s="24"/>
     </row>
-    <row r="148" spans="1:18" ht="64">
+    <row r="148" spans="1:18" ht="64" hidden="1">
       <c r="A148" s="20" t="str">
         <f t="shared" si="22"/>
         <v>T147</v>
@@ -16217,7 +16223,7 @@
       <c r="Q148" s="24"/>
       <c r="R148" s="24"/>
     </row>
-    <row r="149" spans="1:18" ht="32">
+    <row r="149" spans="1:18" ht="32" hidden="1">
       <c r="A149" s="20" t="str">
         <f t="shared" si="22"/>
         <v>T148</v>
@@ -16268,7 +16274,7 @@
       <c r="Q149" s="24"/>
       <c r="R149" s="24"/>
     </row>
-    <row r="150" spans="1:18" ht="64">
+    <row r="150" spans="1:18" ht="64" hidden="1">
       <c r="A150" s="20" t="str">
         <f t="shared" si="22"/>
         <v>T149</v>
@@ -16319,7 +16325,7 @@
       <c r="Q150" s="24"/>
       <c r="R150" s="24"/>
     </row>
-    <row r="151" spans="1:18" ht="112">
+    <row r="151" spans="1:18" ht="112" hidden="1">
       <c r="A151" s="20" t="str">
         <f t="shared" si="22"/>
         <v>T150</v>
@@ -16370,7 +16376,7 @@
       <c r="Q151" s="24"/>
       <c r="R151" s="24"/>
     </row>
-    <row r="152" spans="1:18" ht="64">
+    <row r="152" spans="1:18" ht="64" hidden="1">
       <c r="A152" s="20" t="str">
         <f t="shared" si="22"/>
         <v>T151</v>
@@ -16421,7 +16427,7 @@
       <c r="Q152" s="24"/>
       <c r="R152" s="24"/>
     </row>
-    <row r="153" spans="1:18" ht="96">
+    <row r="153" spans="1:18" ht="96" hidden="1">
       <c r="A153" s="20" t="str">
         <f t="shared" si="22"/>
         <v>T152</v>
@@ -16472,7 +16478,7 @@
       <c r="Q153" s="24"/>
       <c r="R153" s="24"/>
     </row>
-    <row r="154" spans="1:18" ht="160">
+    <row r="154" spans="1:18" ht="160" hidden="1">
       <c r="A154" s="20" t="str">
         <f t="shared" si="22"/>
         <v>T153</v>
@@ -16523,7 +16529,7 @@
       <c r="Q154" s="24"/>
       <c r="R154" s="24"/>
     </row>
-    <row r="155" spans="1:18" ht="96">
+    <row r="155" spans="1:18" ht="96" hidden="1">
       <c r="A155" s="20" t="str">
         <f t="shared" si="22"/>
         <v>T154</v>
@@ -16574,7 +16580,7 @@
       <c r="Q155" s="24"/>
       <c r="R155" s="24"/>
     </row>
-    <row r="156" spans="1:18" ht="80">
+    <row r="156" spans="1:18" ht="80" hidden="1">
       <c r="A156" s="20" t="str">
         <f t="shared" si="22"/>
         <v>T155</v>
@@ -16625,7 +16631,7 @@
       <c r="Q156" s="24"/>
       <c r="R156" s="24"/>
     </row>
-    <row r="157" spans="1:18" ht="96">
+    <row r="157" spans="1:18" ht="96" hidden="1">
       <c r="A157" s="20" t="str">
         <f t="shared" si="22"/>
         <v>T156</v>
@@ -16676,7 +16682,7 @@
       <c r="Q157" s="24"/>
       <c r="R157" s="24"/>
     </row>
-    <row r="158" spans="1:18" ht="48">
+    <row r="158" spans="1:18" ht="48" hidden="1">
       <c r="A158" s="20" t="str">
         <f t="shared" si="22"/>
         <v>T157</v>
@@ -16727,7 +16733,7 @@
       <c r="Q158" s="24"/>
       <c r="R158" s="24"/>
     </row>
-    <row r="159" spans="1:18" ht="32">
+    <row r="159" spans="1:18" ht="32" hidden="1">
       <c r="A159" s="20" t="str">
         <f t="shared" si="22"/>
         <v>T158</v>
@@ -16778,7 +16784,7 @@
       <c r="Q159" s="24"/>
       <c r="R159" s="24"/>
     </row>
-    <row r="160" spans="1:18" ht="80">
+    <row r="160" spans="1:18" ht="80" hidden="1">
       <c r="A160" s="20" t="str">
         <f t="shared" si="22"/>
         <v>T159</v>
@@ -16829,7 +16835,7 @@
       <c r="Q160" s="24"/>
       <c r="R160" s="24"/>
     </row>
-    <row r="161" spans="1:18" ht="80">
+    <row r="161" spans="1:18" ht="80" hidden="1">
       <c r="A161" s="20" t="str">
         <f t="shared" si="22"/>
         <v>T160</v>
@@ -16880,7 +16886,7 @@
       <c r="Q161" s="24"/>
       <c r="R161" s="24"/>
     </row>
-    <row r="162" spans="1:18" ht="64">
+    <row r="162" spans="1:18" ht="64" hidden="1">
       <c r="A162" s="20" t="str">
         <f t="shared" si="22"/>
         <v>T161</v>
@@ -16931,7 +16937,7 @@
       <c r="Q162" s="24"/>
       <c r="R162" s="24"/>
     </row>
-    <row r="163" spans="1:18" ht="64">
+    <row r="163" spans="1:18" ht="64" hidden="1">
       <c r="A163" s="20" t="str">
         <f t="shared" si="22"/>
         <v>T162</v>
@@ -16982,7 +16988,7 @@
       <c r="Q163" s="24"/>
       <c r="R163" s="24"/>
     </row>
-    <row r="164" spans="1:18" ht="48">
+    <row r="164" spans="1:18" ht="48" hidden="1">
       <c r="A164" s="20" t="str">
         <f t="shared" si="22"/>
         <v>T163</v>
@@ -17033,7 +17039,7 @@
       <c r="Q164" s="24"/>
       <c r="R164" s="24"/>
     </row>
-    <row r="165" spans="1:18" ht="32">
+    <row r="165" spans="1:18" ht="32" hidden="1">
       <c r="A165" s="20" t="str">
         <f t="shared" si="22"/>
         <v>T164</v>
@@ -17084,7 +17090,7 @@
       <c r="Q165" s="24"/>
       <c r="R165" s="24"/>
     </row>
-    <row r="166" spans="1:18" ht="32">
+    <row r="166" spans="1:18" ht="32" hidden="1">
       <c r="A166" s="20" t="str">
         <f t="shared" si="22"/>
         <v>T165</v>
@@ -17135,7 +17141,7 @@
       <c r="Q166" s="24"/>
       <c r="R166" s="24"/>
     </row>
-    <row r="167" spans="1:18" ht="32">
+    <row r="167" spans="1:18" ht="32" hidden="1">
       <c r="A167" s="20" t="str">
         <f t="shared" si="22"/>
         <v>T166</v>
@@ -17186,7 +17192,7 @@
       <c r="Q167" s="24"/>
       <c r="R167" s="24"/>
     </row>
-    <row r="168" spans="1:18" ht="32">
+    <row r="168" spans="1:18" ht="32" hidden="1">
       <c r="A168" s="20" t="str">
         <f t="shared" si="22"/>
         <v>T167</v>
@@ -17237,7 +17243,7 @@
       <c r="Q168" s="24"/>
       <c r="R168" s="24"/>
     </row>
-    <row r="169" spans="1:18" ht="64">
+    <row r="169" spans="1:18" ht="64" hidden="1">
       <c r="A169" s="20" t="str">
         <f t="shared" si="22"/>
         <v>T168</v>
@@ -17288,7 +17294,7 @@
       <c r="Q169" s="24"/>
       <c r="R169" s="24"/>
     </row>
-    <row r="170" spans="1:18" ht="48">
+    <row r="170" spans="1:18" ht="48" hidden="1">
       <c r="A170" s="20" t="str">
         <f t="shared" si="22"/>
         <v>T169</v>
@@ -17339,7 +17345,7 @@
       <c r="Q170" s="24"/>
       <c r="R170" s="24"/>
     </row>
-    <row r="171" spans="1:18" ht="32">
+    <row r="171" spans="1:18" ht="32" hidden="1">
       <c r="A171" s="20" t="str">
         <f t="shared" si="22"/>
         <v>T170</v>
@@ -17390,7 +17396,7 @@
       <c r="Q171" s="24"/>
       <c r="R171" s="24"/>
     </row>
-    <row r="172" spans="1:18" ht="32">
+    <row r="172" spans="1:18" ht="32" hidden="1">
       <c r="A172" s="20" t="str">
         <f t="shared" si="22"/>
         <v>T171</v>
@@ -17441,7 +17447,7 @@
       <c r="Q172" s="24"/>
       <c r="R172" s="24"/>
     </row>
-    <row r="173" spans="1:18" ht="16">
+    <row r="173" spans="1:18" ht="16" hidden="1">
       <c r="A173" s="20" t="str">
         <f t="shared" si="22"/>
         <v>T172</v>
@@ -17492,7 +17498,7 @@
       <c r="Q173" s="24"/>
       <c r="R173" s="24"/>
     </row>
-    <row r="174" spans="1:18" ht="16">
+    <row r="174" spans="1:18" ht="16" hidden="1">
       <c r="A174" s="20" t="str">
         <f t="shared" si="22"/>
         <v>T173</v>
@@ -17543,7 +17549,7 @@
       <c r="Q174" s="24"/>
       <c r="R174" s="24"/>
     </row>
-    <row r="175" spans="1:18" ht="64">
+    <row r="175" spans="1:18" ht="64" hidden="1">
       <c r="A175" s="20" t="str">
         <f t="shared" si="22"/>
         <v>T174</v>
@@ -17594,7 +17600,7 @@
       <c r="Q175" s="24"/>
       <c r="R175" s="24"/>
     </row>
-    <row r="176" spans="1:18" ht="64">
+    <row r="176" spans="1:18" ht="64" hidden="1">
       <c r="A176" s="20" t="str">
         <f t="shared" si="22"/>
         <v>T175</v>
@@ -17645,7 +17651,7 @@
       <c r="Q176" s="24"/>
       <c r="R176" s="24"/>
     </row>
-    <row r="177" spans="1:18" ht="80">
+    <row r="177" spans="1:18" ht="80" hidden="1">
       <c r="A177" s="20" t="str">
         <f t="shared" si="22"/>
         <v>T176</v>
@@ -17696,7 +17702,7 @@
       <c r="Q177" s="24"/>
       <c r="R177" s="24"/>
     </row>
-    <row r="178" spans="1:18" ht="48">
+    <row r="178" spans="1:18" ht="48" hidden="1">
       <c r="A178" s="20" t="str">
         <f t="shared" si="22"/>
         <v>T177</v>
@@ -17747,7 +17753,7 @@
       <c r="Q178" s="24"/>
       <c r="R178" s="24"/>
     </row>
-    <row r="179" spans="1:18" ht="32">
+    <row r="179" spans="1:18" ht="32" hidden="1">
       <c r="A179" s="20" t="str">
         <f t="shared" si="22"/>
         <v>T178</v>
@@ -17798,7 +17804,7 @@
       <c r="Q179" s="24"/>
       <c r="R179" s="24"/>
     </row>
-    <row r="180" spans="1:18" ht="32">
+    <row r="180" spans="1:18" ht="32" hidden="1">
       <c r="A180" s="20" t="str">
         <f t="shared" si="22"/>
         <v>T179</v>
@@ -17849,7 +17855,7 @@
       <c r="Q180" s="24"/>
       <c r="R180" s="24"/>
     </row>
-    <row r="181" spans="1:18" ht="80">
+    <row r="181" spans="1:18" ht="80" hidden="1">
       <c r="A181" s="20" t="str">
         <f t="shared" si="22"/>
         <v>T180</v>
@@ -17900,7 +17906,7 @@
       <c r="Q181" s="24"/>
       <c r="R181" s="24"/>
     </row>
-    <row r="182" spans="1:18" ht="64">
+    <row r="182" spans="1:18" ht="64" hidden="1">
       <c r="A182" s="20" t="str">
         <f t="shared" si="22"/>
         <v>T181</v>
@@ -17951,7 +17957,7 @@
       <c r="Q182" s="24"/>
       <c r="R182" s="24"/>
     </row>
-    <row r="183" spans="1:18" ht="64">
+    <row r="183" spans="1:18" ht="64" hidden="1">
       <c r="A183" s="20" t="str">
         <f t="shared" si="22"/>
         <v>T182</v>
@@ -18002,7 +18008,7 @@
       <c r="Q183" s="24"/>
       <c r="R183" s="24"/>
     </row>
-    <row r="184" spans="1:18" ht="144">
+    <row r="184" spans="1:18" ht="144" hidden="1">
       <c r="A184" s="20" t="str">
         <f t="shared" si="22"/>
         <v>T183</v>
@@ -18053,7 +18059,7 @@
       <c r="Q184" s="24"/>
       <c r="R184" s="24"/>
     </row>
-    <row r="185" spans="1:18" ht="96">
+    <row r="185" spans="1:18" ht="96" hidden="1">
       <c r="A185" s="20" t="str">
         <f t="shared" si="22"/>
         <v>T184</v>
@@ -18104,7 +18110,7 @@
       <c r="Q185" s="24"/>
       <c r="R185" s="24"/>
     </row>
-    <row r="186" spans="1:18" ht="48">
+    <row r="186" spans="1:18" ht="48" hidden="1">
       <c r="A186" s="20" t="str">
         <f t="shared" si="22"/>
         <v>T185</v>
@@ -18155,7 +18161,7 @@
       <c r="Q186" s="24"/>
       <c r="R186" s="24"/>
     </row>
-    <row r="187" spans="1:18" ht="16">
+    <row r="187" spans="1:18" ht="16" hidden="1">
       <c r="A187" s="20" t="str">
         <f t="shared" si="22"/>
         <v>T186</v>
@@ -18206,7 +18212,7 @@
       <c r="Q187" s="24"/>
       <c r="R187" s="24"/>
     </row>
-    <row r="188" spans="1:18" ht="144">
+    <row r="188" spans="1:18" ht="144" hidden="1">
       <c r="A188" s="20" t="str">
         <f t="shared" si="22"/>
         <v>T187</v>
@@ -18257,7 +18263,7 @@
       <c r="Q188" s="24"/>
       <c r="R188" s="24"/>
     </row>
-    <row r="189" spans="1:18" ht="128">
+    <row r="189" spans="1:18" ht="128" hidden="1">
       <c r="A189" s="20" t="str">
         <f t="shared" si="22"/>
         <v>T188</v>
@@ -18308,7 +18314,7 @@
       <c r="Q189" s="24"/>
       <c r="R189" s="24"/>
     </row>
-    <row r="190" spans="1:18" ht="128">
+    <row r="190" spans="1:18" ht="128" hidden="1">
       <c r="A190" s="20" t="str">
         <f t="shared" si="22"/>
         <v>T189</v>
@@ -18359,7 +18365,7 @@
       <c r="Q190" s="24"/>
       <c r="R190" s="24"/>
     </row>
-    <row r="191" spans="1:18" ht="96">
+    <row r="191" spans="1:18" ht="96" hidden="1">
       <c r="A191" s="20" t="str">
         <f t="shared" si="22"/>
         <v>T190</v>
@@ -18410,7 +18416,7 @@
       <c r="Q191" s="24"/>
       <c r="R191" s="24"/>
     </row>
-    <row r="192" spans="1:18" ht="80">
+    <row r="192" spans="1:18" ht="80" hidden="1">
       <c r="A192" s="20" t="str">
         <f t="shared" si="22"/>
         <v>T191</v>
@@ -18461,7 +18467,7 @@
       <c r="Q192" s="24"/>
       <c r="R192" s="24"/>
     </row>
-    <row r="193" spans="1:18" ht="80">
+    <row r="193" spans="1:18" ht="80" hidden="1">
       <c r="A193" s="20" t="str">
         <f t="shared" si="22"/>
         <v>T192</v>
@@ -18512,7 +18518,7 @@
       <c r="Q193" s="24"/>
       <c r="R193" s="24"/>
     </row>
-    <row r="194" spans="1:18" ht="48">
+    <row r="194" spans="1:18" ht="48" hidden="1">
       <c r="A194" s="20" t="str">
         <f t="shared" ref="A194:A257" si="27">CONCATENATE("T",ROW(A194)-1)</f>
         <v>T193</v>
@@ -18563,7 +18569,7 @@
       <c r="Q194" s="24"/>
       <c r="R194" s="24"/>
     </row>
-    <row r="195" spans="1:18" ht="32">
+    <row r="195" spans="1:18" ht="32" hidden="1">
       <c r="A195" s="20" t="str">
         <f t="shared" si="27"/>
         <v>T194</v>
@@ -18614,7 +18620,7 @@
       <c r="Q195" s="24"/>
       <c r="R195" s="24"/>
     </row>
-    <row r="196" spans="1:18" ht="80">
+    <row r="196" spans="1:18" ht="80" hidden="1">
       <c r="A196" s="20" t="str">
         <f t="shared" si="27"/>
         <v>T195</v>
@@ -18665,7 +18671,7 @@
       <c r="Q196" s="24"/>
       <c r="R196" s="24"/>
     </row>
-    <row r="197" spans="1:18" ht="96">
+    <row r="197" spans="1:18" ht="96" hidden="1">
       <c r="A197" s="20" t="str">
         <f t="shared" si="27"/>
         <v>T196</v>
@@ -18716,7 +18722,7 @@
       <c r="Q197" s="24"/>
       <c r="R197" s="24"/>
     </row>
-    <row r="198" spans="1:18" ht="48">
+    <row r="198" spans="1:18" ht="48" hidden="1">
       <c r="A198" s="20" t="str">
         <f t="shared" si="27"/>
         <v>T197</v>
@@ -18767,7 +18773,7 @@
       <c r="Q198" s="24"/>
       <c r="R198" s="24"/>
     </row>
-    <row r="199" spans="1:18" ht="80">
+    <row r="199" spans="1:18" ht="80" hidden="1">
       <c r="A199" s="20" t="str">
         <f t="shared" si="27"/>
         <v>T198</v>
@@ -18818,7 +18824,7 @@
       <c r="Q199" s="24"/>
       <c r="R199" s="24"/>
     </row>
-    <row r="200" spans="1:18" ht="48">
+    <row r="200" spans="1:18" ht="48" hidden="1">
       <c r="A200" s="20" t="str">
         <f t="shared" si="27"/>
         <v>T199</v>
@@ -18869,7 +18875,7 @@
       <c r="Q200" s="24"/>
       <c r="R200" s="24"/>
     </row>
-    <row r="201" spans="1:18" ht="32">
+    <row r="201" spans="1:18" ht="32" hidden="1">
       <c r="A201" s="20" t="str">
         <f t="shared" si="27"/>
         <v>T200</v>
@@ -18920,7 +18926,7 @@
       <c r="Q201" s="24"/>
       <c r="R201" s="24"/>
     </row>
-    <row r="202" spans="1:18" ht="32">
+    <row r="202" spans="1:18" ht="32" hidden="1">
       <c r="A202" s="20" t="str">
         <f t="shared" si="27"/>
         <v>T201</v>
@@ -18971,7 +18977,7 @@
       <c r="Q202" s="24"/>
       <c r="R202" s="24"/>
     </row>
-    <row r="203" spans="1:18" ht="80">
+    <row r="203" spans="1:18" ht="80" hidden="1">
       <c r="A203" s="20" t="str">
         <f t="shared" si="27"/>
         <v>T202</v>
@@ -19022,7 +19028,7 @@
       <c r="Q203" s="24"/>
       <c r="R203" s="24"/>
     </row>
-    <row r="204" spans="1:18" ht="64">
+    <row r="204" spans="1:18" ht="64" hidden="1">
       <c r="A204" s="20" t="str">
         <f t="shared" si="27"/>
         <v>T203</v>
@@ -19073,7 +19079,7 @@
       <c r="Q204" s="24"/>
       <c r="R204" s="24"/>
     </row>
-    <row r="205" spans="1:18" ht="64">
+    <row r="205" spans="1:18" ht="64" hidden="1">
       <c r="A205" s="20" t="str">
         <f t="shared" si="27"/>
         <v>T204</v>
@@ -19124,7 +19130,7 @@
       <c r="Q205" s="24"/>
       <c r="R205" s="24"/>
     </row>
-    <row r="206" spans="1:18" ht="32">
+    <row r="206" spans="1:18" ht="32" hidden="1">
       <c r="A206" s="20" t="str">
         <f t="shared" si="27"/>
         <v>T205</v>
@@ -19175,7 +19181,7 @@
       <c r="Q206" s="24"/>
       <c r="R206" s="24"/>
     </row>
-    <row r="207" spans="1:18" ht="80">
+    <row r="207" spans="1:18" ht="80" hidden="1">
       <c r="A207" s="20" t="str">
         <f t="shared" si="27"/>
         <v>T206</v>
@@ -19226,7 +19232,7 @@
       <c r="Q207" s="24"/>
       <c r="R207" s="24"/>
     </row>
-    <row r="208" spans="1:18" ht="96">
+    <row r="208" spans="1:18" ht="96" hidden="1">
       <c r="A208" s="20" t="str">
         <f t="shared" si="27"/>
         <v>T207</v>
@@ -19277,7 +19283,7 @@
       <c r="Q208" s="24"/>
       <c r="R208" s="24"/>
     </row>
-    <row r="209" spans="1:18" ht="80">
+    <row r="209" spans="1:18" ht="80" hidden="1">
       <c r="A209" s="20" t="str">
         <f t="shared" si="27"/>
         <v>T208</v>
@@ -19328,7 +19334,7 @@
       <c r="Q209" s="24"/>
       <c r="R209" s="24"/>
     </row>
-    <row r="210" spans="1:18" ht="80">
+    <row r="210" spans="1:18" ht="80" hidden="1">
       <c r="A210" s="20" t="str">
         <f t="shared" si="27"/>
         <v>T209</v>
@@ -19379,7 +19385,7 @@
       <c r="Q210" s="24"/>
       <c r="R210" s="24"/>
     </row>
-    <row r="211" spans="1:18" ht="48">
+    <row r="211" spans="1:18" ht="48" hidden="1">
       <c r="A211" s="20" t="str">
         <f t="shared" si="27"/>
         <v>T210</v>
@@ -19430,7 +19436,7 @@
       <c r="Q211" s="24"/>
       <c r="R211" s="24"/>
     </row>
-    <row r="212" spans="1:18" ht="32">
+    <row r="212" spans="1:18" ht="32" hidden="1">
       <c r="A212" s="20" t="str">
         <f t="shared" si="27"/>
         <v>T211</v>
@@ -19481,7 +19487,7 @@
       <c r="Q212" s="24"/>
       <c r="R212" s="24"/>
     </row>
-    <row r="213" spans="1:18" ht="144">
+    <row r="213" spans="1:18" ht="144" hidden="1">
       <c r="A213" s="20" t="str">
         <f t="shared" si="27"/>
         <v>T212</v>
@@ -19532,7 +19538,7 @@
       <c r="Q213" s="24"/>
       <c r="R213" s="24"/>
     </row>
-    <row r="214" spans="1:18" ht="80">
+    <row r="214" spans="1:18" ht="80" hidden="1">
       <c r="A214" s="20" t="str">
         <f t="shared" si="27"/>
         <v>T213</v>
@@ -19583,7 +19589,7 @@
       <c r="Q214" s="24"/>
       <c r="R214" s="24"/>
     </row>
-    <row r="215" spans="1:18" ht="96">
+    <row r="215" spans="1:18" ht="96" hidden="1">
       <c r="A215" s="20" t="str">
         <f t="shared" si="27"/>
         <v>T214</v>
@@ -19634,7 +19640,7 @@
       <c r="Q215" s="24"/>
       <c r="R215" s="24"/>
     </row>
-    <row r="216" spans="1:18" ht="96">
+    <row r="216" spans="1:18" ht="96" hidden="1">
       <c r="A216" s="20" t="str">
         <f t="shared" si="27"/>
         <v>T215</v>
@@ -19685,7 +19691,7 @@
       <c r="Q216" s="24"/>
       <c r="R216" s="24"/>
     </row>
-    <row r="217" spans="1:18" ht="80">
+    <row r="217" spans="1:18" ht="80" hidden="1">
       <c r="A217" s="20" t="str">
         <f t="shared" si="27"/>
         <v>T216</v>
@@ -19736,7 +19742,7 @@
       <c r="Q217" s="24"/>
       <c r="R217" s="24"/>
     </row>
-    <row r="218" spans="1:18" ht="80">
+    <row r="218" spans="1:18" ht="80" hidden="1">
       <c r="A218" s="20" t="str">
         <f t="shared" si="27"/>
         <v>T217</v>
@@ -19787,7 +19793,7 @@
       <c r="Q218" s="24"/>
       <c r="R218" s="24"/>
     </row>
-    <row r="219" spans="1:18" ht="48">
+    <row r="219" spans="1:18" ht="48" hidden="1">
       <c r="A219" s="20" t="str">
         <f t="shared" si="27"/>
         <v>T218</v>
@@ -19838,7 +19844,7 @@
       <c r="Q219" s="24"/>
       <c r="R219" s="24"/>
     </row>
-    <row r="220" spans="1:18" ht="32">
+    <row r="220" spans="1:18" ht="32" hidden="1">
       <c r="A220" s="20" t="str">
         <f t="shared" si="27"/>
         <v>T219</v>
@@ -19889,7 +19895,7 @@
       <c r="Q220" s="24"/>
       <c r="R220" s="24"/>
     </row>
-    <row r="221" spans="1:18" ht="64">
+    <row r="221" spans="1:18" ht="64" hidden="1">
       <c r="A221" s="20" t="str">
         <f t="shared" si="27"/>
         <v>T220</v>
@@ -19940,7 +19946,7 @@
       <c r="Q221" s="24"/>
       <c r="R221" s="24"/>
     </row>
-    <row r="222" spans="1:18" ht="16">
+    <row r="222" spans="1:18" ht="16" hidden="1">
       <c r="A222" s="20" t="str">
         <f t="shared" si="27"/>
         <v>T221</v>
@@ -19991,7 +19997,7 @@
       <c r="Q222" s="24"/>
       <c r="R222" s="24"/>
     </row>
-    <row r="223" spans="1:18" ht="64">
+    <row r="223" spans="1:18" ht="64" hidden="1">
       <c r="A223" s="20" t="str">
         <f t="shared" si="27"/>
         <v>T222</v>
@@ -20042,7 +20048,7 @@
       <c r="Q223" s="24"/>
       <c r="R223" s="24"/>
     </row>
-    <row r="224" spans="1:18" ht="96">
+    <row r="224" spans="1:18" ht="96" hidden="1">
       <c r="A224" s="20" t="str">
         <f t="shared" si="27"/>
         <v>T223</v>
@@ -20093,7 +20099,7 @@
       <c r="Q224" s="24"/>
       <c r="R224" s="24"/>
     </row>
-    <row r="225" spans="1:18" ht="80">
+    <row r="225" spans="1:18" ht="80" hidden="1">
       <c r="A225" s="20" t="str">
         <f t="shared" si="27"/>
         <v>T224</v>
@@ -20144,7 +20150,7 @@
       <c r="Q225" s="24"/>
       <c r="R225" s="24"/>
     </row>
-    <row r="226" spans="1:18" ht="80">
+    <row r="226" spans="1:18" ht="80" hidden="1">
       <c r="A226" s="20" t="str">
         <f t="shared" si="27"/>
         <v>T225</v>
@@ -20195,7 +20201,7 @@
       <c r="Q226" s="24"/>
       <c r="R226" s="24"/>
     </row>
-    <row r="227" spans="1:18" ht="64">
+    <row r="227" spans="1:18" ht="64" hidden="1">
       <c r="A227" s="20" t="str">
         <f t="shared" si="27"/>
         <v>T226</v>
@@ -20246,7 +20252,7 @@
       <c r="Q227" s="24"/>
       <c r="R227" s="24"/>
     </row>
-    <row r="228" spans="1:18" ht="80">
+    <row r="228" spans="1:18" ht="80" hidden="1">
       <c r="A228" s="20" t="str">
         <f t="shared" si="27"/>
         <v>T227</v>
@@ -20297,7 +20303,7 @@
       <c r="Q228" s="24"/>
       <c r="R228" s="24"/>
     </row>
-    <row r="229" spans="1:18" ht="64">
+    <row r="229" spans="1:18" ht="64" hidden="1">
       <c r="A229" s="20" t="str">
         <f t="shared" si="27"/>
         <v>T228</v>
@@ -20348,7 +20354,7 @@
       <c r="Q229" s="24"/>
       <c r="R229" s="24"/>
     </row>
-    <row r="230" spans="1:18" ht="48">
+    <row r="230" spans="1:18" ht="48" hidden="1">
       <c r="A230" s="20" t="str">
         <f t="shared" si="27"/>
         <v>T229</v>
@@ -20399,7 +20405,7 @@
       <c r="Q230" s="24"/>
       <c r="R230" s="24"/>
     </row>
-    <row r="231" spans="1:18" ht="80">
+    <row r="231" spans="1:18" ht="80" hidden="1">
       <c r="A231" s="20" t="str">
         <f t="shared" si="27"/>
         <v>T230</v>
@@ -20450,7 +20456,7 @@
       <c r="Q231" s="24"/>
       <c r="R231" s="24"/>
     </row>
-    <row r="232" spans="1:18" ht="80">
+    <row r="232" spans="1:18" ht="80" hidden="1">
       <c r="A232" s="20" t="str">
         <f t="shared" si="27"/>
         <v>T231</v>
@@ -20501,7 +20507,7 @@
       <c r="Q232" s="24"/>
       <c r="R232" s="24"/>
     </row>
-    <row r="233" spans="1:18" ht="48">
+    <row r="233" spans="1:18" ht="48" hidden="1">
       <c r="A233" s="20" t="str">
         <f t="shared" si="27"/>
         <v>T232</v>
@@ -20552,7 +20558,7 @@
       <c r="Q233" s="24"/>
       <c r="R233" s="24"/>
     </row>
-    <row r="234" spans="1:18" ht="96">
+    <row r="234" spans="1:18" ht="96" hidden="1">
       <c r="A234" s="20" t="str">
         <f t="shared" si="27"/>
         <v>T233</v>
@@ -20603,7 +20609,7 @@
       <c r="Q234" s="24"/>
       <c r="R234" s="24"/>
     </row>
-    <row r="235" spans="1:18" ht="96">
+    <row r="235" spans="1:18" ht="96" hidden="1">
       <c r="A235" s="20" t="str">
         <f t="shared" si="27"/>
         <v>T234</v>
@@ -20654,7 +20660,7 @@
       <c r="Q235" s="24"/>
       <c r="R235" s="24"/>
     </row>
-    <row r="236" spans="1:18" ht="80">
+    <row r="236" spans="1:18" ht="80" hidden="1">
       <c r="A236" s="20" t="str">
         <f t="shared" si="27"/>
         <v>T235</v>
@@ -20705,7 +20711,7 @@
       <c r="Q236" s="24"/>
       <c r="R236" s="24"/>
     </row>
-    <row r="237" spans="1:18" ht="80">
+    <row r="237" spans="1:18" ht="80" hidden="1">
       <c r="A237" s="20" t="str">
         <f t="shared" si="27"/>
         <v>T236</v>
@@ -20756,7 +20762,7 @@
       <c r="Q237" s="24"/>
       <c r="R237" s="24"/>
     </row>
-    <row r="238" spans="1:18" ht="48">
+    <row r="238" spans="1:18" ht="48" hidden="1">
       <c r="A238" s="20" t="str">
         <f t="shared" si="27"/>
         <v>T237</v>
@@ -20807,7 +20813,7 @@
       <c r="Q238" s="24"/>
       <c r="R238" s="24"/>
     </row>
-    <row r="239" spans="1:18" ht="32">
+    <row r="239" spans="1:18" ht="32" hidden="1">
       <c r="A239" s="20" t="str">
         <f t="shared" si="27"/>
         <v>T238</v>
@@ -20858,7 +20864,7 @@
       <c r="Q239" s="24"/>
       <c r="R239" s="24"/>
     </row>
-    <row r="240" spans="1:18" ht="80">
+    <row r="240" spans="1:18" ht="80" hidden="1">
       <c r="A240" s="20" t="str">
         <f t="shared" si="27"/>
         <v>T239</v>
@@ -20909,7 +20915,7 @@
       <c r="Q240" s="24"/>
       <c r="R240" s="24"/>
     </row>
-    <row r="241" spans="1:18" ht="80">
+    <row r="241" spans="1:18" ht="80" hidden="1">
       <c r="A241" s="20" t="str">
         <f t="shared" si="27"/>
         <v>T240</v>
@@ -20960,7 +20966,7 @@
       <c r="Q241" s="24"/>
       <c r="R241" s="24"/>
     </row>
-    <row r="242" spans="1:18" ht="48">
+    <row r="242" spans="1:18" ht="48" hidden="1">
       <c r="A242" s="20" t="str">
         <f t="shared" si="27"/>
         <v>T241</v>
@@ -21011,7 +21017,7 @@
       <c r="Q242" s="24"/>
       <c r="R242" s="24"/>
     </row>
-    <row r="243" spans="1:18" ht="32">
+    <row r="243" spans="1:18" ht="32" hidden="1">
       <c r="A243" s="20" t="str">
         <f t="shared" si="27"/>
         <v>T242</v>
@@ -21062,7 +21068,7 @@
       <c r="Q243" s="24"/>
       <c r="R243" s="24"/>
     </row>
-    <row r="244" spans="1:18" ht="32">
+    <row r="244" spans="1:18" ht="32" hidden="1">
       <c r="A244" s="20" t="str">
         <f t="shared" si="27"/>
         <v>T243</v>
@@ -21113,7 +21119,7 @@
       <c r="Q244" s="24"/>
       <c r="R244" s="24"/>
     </row>
-    <row r="245" spans="1:18" ht="32">
+    <row r="245" spans="1:18" ht="32" hidden="1">
       <c r="A245" s="20" t="str">
         <f t="shared" si="27"/>
         <v>T244</v>
@@ -21164,7 +21170,7 @@
       <c r="Q245" s="24"/>
       <c r="R245" s="24"/>
     </row>
-    <row r="246" spans="1:18" ht="80">
+    <row r="246" spans="1:18" ht="80" hidden="1">
       <c r="A246" s="20" t="str">
         <f t="shared" si="27"/>
         <v>T245</v>
@@ -21215,7 +21221,7 @@
       <c r="Q246" s="24"/>
       <c r="R246" s="24"/>
     </row>
-    <row r="247" spans="1:18" ht="32">
+    <row r="247" spans="1:18" ht="32" hidden="1">
       <c r="A247" s="20" t="str">
         <f t="shared" si="27"/>
         <v>T246</v>
@@ -21266,7 +21272,7 @@
       <c r="Q247" s="24"/>
       <c r="R247" s="24"/>
     </row>
-    <row r="248" spans="1:18" ht="32">
+    <row r="248" spans="1:18" ht="32" hidden="1">
       <c r="A248" s="20" t="str">
         <f t="shared" si="27"/>
         <v>T247</v>
@@ -21317,7 +21323,7 @@
       <c r="Q248" s="24"/>
       <c r="R248" s="24"/>
     </row>
-    <row r="249" spans="1:18" ht="80">
+    <row r="249" spans="1:18" ht="80" hidden="1">
       <c r="A249" s="20" t="str">
         <f t="shared" si="27"/>
         <v>T248</v>
@@ -21368,7 +21374,7 @@
       <c r="Q249" s="24"/>
       <c r="R249" s="24"/>
     </row>
-    <row r="250" spans="1:18" ht="64">
+    <row r="250" spans="1:18" ht="64" hidden="1">
       <c r="A250" s="20" t="str">
         <f t="shared" si="27"/>
         <v>T249</v>
@@ -21419,7 +21425,7 @@
       <c r="Q250" s="24"/>
       <c r="R250" s="24"/>
     </row>
-    <row r="251" spans="1:18" ht="64">
+    <row r="251" spans="1:18" ht="64" hidden="1">
       <c r="A251" s="20" t="str">
         <f t="shared" si="27"/>
         <v>T250</v>
@@ -21470,7 +21476,7 @@
       <c r="Q251" s="24"/>
       <c r="R251" s="24"/>
     </row>
-    <row r="252" spans="1:18" ht="96">
+    <row r="252" spans="1:18" ht="96" hidden="1">
       <c r="A252" s="20" t="str">
         <f t="shared" si="27"/>
         <v>T251</v>
@@ -21521,7 +21527,7 @@
       <c r="Q252" s="24"/>
       <c r="R252" s="24"/>
     </row>
-    <row r="253" spans="1:18" ht="48">
+    <row r="253" spans="1:18" ht="48" hidden="1">
       <c r="A253" s="20" t="str">
         <f t="shared" si="27"/>
         <v>T252</v>
@@ -21572,7 +21578,7 @@
       <c r="Q253" s="24"/>
       <c r="R253" s="24"/>
     </row>
-    <row r="254" spans="1:18" ht="80">
+    <row r="254" spans="1:18" ht="80" hidden="1">
       <c r="A254" s="20" t="str">
         <f t="shared" si="27"/>
         <v>T253</v>
@@ -21623,7 +21629,7 @@
       <c r="Q254" s="24"/>
       <c r="R254" s="24"/>
     </row>
-    <row r="255" spans="1:18" ht="16">
+    <row r="255" spans="1:18" ht="16" hidden="1">
       <c r="A255" s="20" t="str">
         <f t="shared" si="27"/>
         <v>T254</v>
@@ -21674,7 +21680,7 @@
       <c r="Q255" s="24"/>
       <c r="R255" s="24"/>
     </row>
-    <row r="256" spans="1:18" ht="32">
+    <row r="256" spans="1:18" ht="32" hidden="1">
       <c r="A256" s="20" t="str">
         <f t="shared" si="27"/>
         <v>T255</v>
@@ -21735,7 +21741,7 @@
       </c>
       <c r="R256" s="24"/>
     </row>
-    <row r="257" spans="1:18" ht="32">
+    <row r="257" spans="1:18" ht="32" hidden="1">
       <c r="A257" s="20" t="str">
         <f t="shared" si="27"/>
         <v>T256</v>
@@ -21796,7 +21802,7 @@
       </c>
       <c r="R257" s="24"/>
     </row>
-    <row r="258" spans="1:18" ht="32">
+    <row r="258" spans="1:18" ht="32" hidden="1">
       <c r="A258" s="20" t="str">
         <f t="shared" ref="A258:A299" si="38">CONCATENATE("T",ROW(A258)-1)</f>
         <v>T257</v>
@@ -21857,7 +21863,7 @@
       </c>
       <c r="R258" s="24"/>
     </row>
-    <row r="259" spans="1:18" ht="16">
+    <row r="259" spans="1:18" ht="16" hidden="1">
       <c r="A259" s="20" t="str">
         <f t="shared" si="38"/>
         <v>T258</v>
@@ -21918,7 +21924,7 @@
       </c>
       <c r="R259" s="24"/>
     </row>
-    <row r="260" spans="1:18" ht="240">
+    <row r="260" spans="1:18" ht="240" hidden="1">
       <c r="A260" s="20" t="str">
         <f t="shared" si="38"/>
         <v>T259</v>
@@ -21979,7 +21985,7 @@
       </c>
       <c r="R260" s="24"/>
     </row>
-    <row r="261" spans="1:18" ht="32">
+    <row r="261" spans="1:18" ht="32" hidden="1">
       <c r="A261" s="20" t="str">
         <f t="shared" si="38"/>
         <v>T260</v>
@@ -22040,7 +22046,7 @@
       </c>
       <c r="R261" s="24"/>
     </row>
-    <row r="262" spans="1:18" ht="16">
+    <row r="262" spans="1:18" ht="16" hidden="1">
       <c r="A262" s="20" t="str">
         <f t="shared" si="38"/>
         <v>T261</v>
@@ -22101,7 +22107,7 @@
       </c>
       <c r="R262" s="24"/>
     </row>
-    <row r="263" spans="1:18" ht="32">
+    <row r="263" spans="1:18" ht="32" hidden="1">
       <c r="A263" s="20" t="str">
         <f t="shared" si="38"/>
         <v>T262</v>
@@ -22158,7 +22164,7 @@
         <v>864</v>
       </c>
     </row>
-    <row r="264" spans="1:18" ht="32">
+    <row r="264" spans="1:18" ht="32" hidden="1">
       <c r="A264" s="20" t="str">
         <f t="shared" si="38"/>
         <v>T263</v>
@@ -22219,7 +22225,7 @@
       </c>
       <c r="R264" s="24"/>
     </row>
-    <row r="265" spans="1:18" ht="128">
+    <row r="265" spans="1:18" ht="128" hidden="1">
       <c r="A265" s="20" t="str">
         <f t="shared" si="38"/>
         <v>T264</v>
@@ -22280,7 +22286,7 @@
       </c>
       <c r="R265" s="24"/>
     </row>
-    <row r="266" spans="1:18" ht="64">
+    <row r="266" spans="1:18" ht="64" hidden="1">
       <c r="A266" s="20" t="str">
         <f t="shared" si="38"/>
         <v>T265</v>
@@ -22341,7 +22347,7 @@
       </c>
       <c r="R266" s="24"/>
     </row>
-    <row r="267" spans="1:18" ht="48">
+    <row r="267" spans="1:18" ht="48" hidden="1">
       <c r="A267" s="20" t="str">
         <f t="shared" si="38"/>
         <v>T266</v>
@@ -22402,7 +22408,7 @@
       </c>
       <c r="R267" s="24"/>
     </row>
-    <row r="268" spans="1:18" ht="32">
+    <row r="268" spans="1:18" ht="32" hidden="1">
       <c r="A268" s="20" t="str">
         <f t="shared" si="38"/>
         <v>T267</v>
@@ -22459,7 +22465,7 @@
         <v>864</v>
       </c>
     </row>
-    <row r="269" spans="1:18" ht="32">
+    <row r="269" spans="1:18" ht="32" hidden="1">
       <c r="A269" s="20" t="str">
         <f t="shared" si="38"/>
         <v>T268</v>
@@ -22520,7 +22526,7 @@
       </c>
       <c r="R269" s="24"/>
     </row>
-    <row r="270" spans="1:18" ht="32">
+    <row r="270" spans="1:18" ht="32" hidden="1">
       <c r="A270" s="20" t="str">
         <f t="shared" si="38"/>
         <v>T269</v>
@@ -22581,7 +22587,7 @@
       </c>
       <c r="R270" s="24"/>
     </row>
-    <row r="271" spans="1:18" ht="128">
+    <row r="271" spans="1:18" ht="128" hidden="1">
       <c r="A271" s="20" t="str">
         <f t="shared" si="38"/>
         <v>T270</v>
@@ -22642,7 +22648,7 @@
       </c>
       <c r="R271" s="24"/>
     </row>
-    <row r="272" spans="1:18" ht="32">
+    <row r="272" spans="1:18" ht="32" hidden="1">
       <c r="A272" s="20" t="str">
         <f t="shared" si="38"/>
         <v>T271</v>
@@ -22703,7 +22709,7 @@
       </c>
       <c r="R272" s="24"/>
     </row>
-    <row r="273" spans="1:18" ht="96">
+    <row r="273" spans="1:18" ht="96" hidden="1">
       <c r="A273" s="20" t="str">
         <f t="shared" si="38"/>
         <v>T272</v>
@@ -22764,7 +22770,7 @@
       </c>
       <c r="R273" s="24"/>
     </row>
-    <row r="274" spans="1:18" ht="64">
+    <row r="274" spans="1:18" ht="64" hidden="1">
       <c r="A274" s="20" t="str">
         <f t="shared" si="38"/>
         <v>T273</v>
@@ -22825,7 +22831,7 @@
       </c>
       <c r="R274" s="24"/>
     </row>
-    <row r="275" spans="1:18" ht="128">
+    <row r="275" spans="1:18" ht="128" hidden="1">
       <c r="A275" s="20" t="str">
         <f t="shared" si="38"/>
         <v>T274</v>
@@ -22886,7 +22892,7 @@
       </c>
       <c r="R275" s="24"/>
     </row>
-    <row r="276" spans="1:18" ht="96">
+    <row r="276" spans="1:18" ht="96" hidden="1">
       <c r="A276" s="20" t="str">
         <f t="shared" si="38"/>
         <v>T275</v>
@@ -22943,7 +22949,7 @@
       </c>
       <c r="R276" s="24"/>
     </row>
-    <row r="277" spans="1:18" ht="80">
+    <row r="277" spans="1:18" ht="80" hidden="1">
       <c r="A277" s="20" t="str">
         <f t="shared" si="38"/>
         <v>T276</v>
@@ -23000,7 +23006,7 @@
       </c>
       <c r="R277" s="24"/>
     </row>
-    <row r="278" spans="1:18" ht="64">
+    <row r="278" spans="1:18" ht="64" hidden="1">
       <c r="A278" s="20" t="str">
         <f t="shared" si="38"/>
         <v>T277</v>
@@ -23057,7 +23063,7 @@
       </c>
       <c r="R278" s="24"/>
     </row>
-    <row r="279" spans="1:18" ht="96">
+    <row r="279" spans="1:18" ht="96" hidden="1">
       <c r="A279" s="20" t="str">
         <f t="shared" si="38"/>
         <v>T278</v>
@@ -23118,7 +23124,7 @@
       </c>
       <c r="R279" s="24"/>
     </row>
-    <row r="280" spans="1:18" ht="32">
+    <row r="280" spans="1:18" ht="32" hidden="1">
       <c r="A280" s="20" t="str">
         <f t="shared" si="38"/>
         <v>T279</v>
@@ -23175,7 +23181,7 @@
         <v>864</v>
       </c>
     </row>
-    <row r="281" spans="1:18" ht="48">
+    <row r="281" spans="1:18" ht="48" hidden="1">
       <c r="A281" s="20" t="str">
         <f t="shared" si="38"/>
         <v>T280</v>
@@ -23236,7 +23242,7 @@
       </c>
       <c r="R281" s="24"/>
     </row>
-    <row r="282" spans="1:18" ht="48">
+    <row r="282" spans="1:18" ht="48" hidden="1">
       <c r="A282" s="20" t="str">
         <f t="shared" si="38"/>
         <v>T281</v>
@@ -23297,7 +23303,7 @@
       </c>
       <c r="R282" s="24"/>
     </row>
-    <row r="283" spans="1:18" ht="32">
+    <row r="283" spans="1:18" ht="32" hidden="1">
       <c r="A283" s="20" t="str">
         <f t="shared" si="38"/>
         <v>T282</v>
@@ -23358,7 +23364,7 @@
       </c>
       <c r="R283" s="24"/>
     </row>
-    <row r="284" spans="1:18" ht="80">
+    <row r="284" spans="1:18" ht="80" hidden="1">
       <c r="A284" s="20" t="str">
         <f t="shared" si="38"/>
         <v>T283</v>
@@ -23417,7 +23423,7 @@
       <c r="Q284" s="24"/>
       <c r="R284" s="24"/>
     </row>
-    <row r="285" spans="1:18" ht="160">
+    <row r="285" spans="1:18" ht="160" hidden="1">
       <c r="A285" s="20" t="str">
         <f t="shared" si="38"/>
         <v>T284</v>
@@ -23478,7 +23484,7 @@
       </c>
       <c r="R285" s="24"/>
     </row>
-    <row r="286" spans="1:18" ht="128">
+    <row r="286" spans="1:18" ht="128" hidden="1">
       <c r="A286" s="20" t="str">
         <f t="shared" si="38"/>
         <v>T285</v>
@@ -23539,7 +23545,7 @@
       </c>
       <c r="R286" s="24"/>
     </row>
-    <row r="287" spans="1:18" ht="48">
+    <row r="287" spans="1:18" ht="48" hidden="1">
       <c r="A287" s="20" t="str">
         <f t="shared" si="38"/>
         <v>T286</v>
@@ -23600,7 +23606,7 @@
       </c>
       <c r="R287" s="24"/>
     </row>
-    <row r="288" spans="1:18" ht="96">
+    <row r="288" spans="1:18" ht="96" hidden="1">
       <c r="A288" s="20" t="str">
         <f t="shared" si="38"/>
         <v>T287</v>
@@ -23661,7 +23667,7 @@
       </c>
       <c r="R288" s="24"/>
     </row>
-    <row r="289" spans="1:18" ht="96">
+    <row r="289" spans="1:18" ht="96" hidden="1">
       <c r="A289" s="20" t="str">
         <f t="shared" si="38"/>
         <v>T288</v>
@@ -23722,7 +23728,7 @@
       </c>
       <c r="R289" s="24"/>
     </row>
-    <row r="290" spans="1:18" ht="240">
+    <row r="290" spans="1:18" ht="240" hidden="1">
       <c r="A290" s="20" t="str">
         <f t="shared" si="38"/>
         <v>T289</v>
@@ -23783,7 +23789,7 @@
       </c>
       <c r="R290" s="24"/>
     </row>
-    <row r="291" spans="1:18" ht="96">
+    <row r="291" spans="1:18" ht="96" hidden="1">
       <c r="A291" s="20" t="str">
         <f t="shared" si="38"/>
         <v>T290</v>
@@ -23846,7 +23852,7 @@
         <v>867</v>
       </c>
     </row>
-    <row r="292" spans="1:18" ht="176">
+    <row r="292" spans="1:18" ht="176" hidden="1">
       <c r="A292" s="20" t="str">
         <f t="shared" si="38"/>
         <v>T291</v>
@@ -23907,7 +23913,7 @@
       </c>
       <c r="R292" s="24"/>
     </row>
-    <row r="293" spans="1:18" ht="380">
+    <row r="293" spans="1:18" ht="380" hidden="1">
       <c r="A293" s="20" t="str">
         <f t="shared" si="38"/>
         <v>T292</v>
@@ -23968,7 +23974,7 @@
       </c>
       <c r="R293" s="24"/>
     </row>
-    <row r="294" spans="1:18" ht="144">
+    <row r="294" spans="1:18" ht="144" hidden="1">
       <c r="A294" s="20" t="str">
         <f t="shared" si="38"/>
         <v>T293</v>
@@ -24029,7 +24035,7 @@
       </c>
       <c r="R294" s="24"/>
     </row>
-    <row r="295" spans="1:18" ht="112">
+    <row r="295" spans="1:18" ht="112" hidden="1">
       <c r="A295" s="20" t="str">
         <f t="shared" si="38"/>
         <v>T294</v>
@@ -24090,7 +24096,7 @@
       </c>
       <c r="R295" s="24"/>
     </row>
-    <row r="296" spans="1:18" ht="96">
+    <row r="296" spans="1:18" ht="96" hidden="1">
       <c r="A296" s="20" t="str">
         <f t="shared" si="38"/>
         <v>T295</v>
@@ -24151,7 +24157,7 @@
       </c>
       <c r="R296" s="24"/>
     </row>
-    <row r="297" spans="1:18" ht="32">
+    <row r="297" spans="1:18" ht="32" hidden="1">
       <c r="A297" s="20" t="str">
         <f t="shared" si="38"/>
         <v>T296</v>
@@ -24210,7 +24216,7 @@
       <c r="Q297" s="24"/>
       <c r="R297" s="24"/>
     </row>
-    <row r="298" spans="1:18" ht="32">
+    <row r="298" spans="1:18" ht="32" hidden="1">
       <c r="A298" s="20" t="str">
         <f t="shared" si="38"/>
         <v>T297</v>
@@ -24271,7 +24277,7 @@
       </c>
       <c r="R298" s="24"/>
     </row>
-    <row r="299" spans="1:18" ht="48">
+    <row r="299" spans="1:18" ht="48" hidden="1">
       <c r="A299" s="20" t="str">
         <f t="shared" si="38"/>
         <v>T298</v>
@@ -28767,7 +28773,7 @@
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="181" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -28781,7 +28787,7 @@
         <v>911</v>
       </c>
       <c r="B1" t="s">
-        <v>919</v>
+        <v>917</v>
       </c>
       <c r="C1" t="s">
         <v>910</v>
@@ -28799,10 +28805,10 @@
         <v>913</v>
       </c>
       <c r="C2" t="s">
-        <v>915</v>
+        <v>914</v>
       </c>
       <c r="D2" t="s">
-        <v>914</v>
+        <v>918</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -28811,13 +28817,13 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>917</v>
+        <v>915</v>
       </c>
       <c r="C3" t="s">
-        <v>918</v>
+        <v>916</v>
       </c>
       <c r="D3" t="s">
-        <v>916</v>
+        <v>919</v>
       </c>
     </row>
   </sheetData>
@@ -29089,16 +29095,16 @@
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{83D5100D-0E56-4B30-B42D-2AEC6B837C39}">
   <ds:schemaRefs>
+    <ds:schemaRef ds:uri="633f040f-4953-46e7-8610-82b0c5296ba0"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="f62ef740-d444-4f18-80a2-7590fdcab1ce"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="633f040f-4953-46e7-8610-82b0c5296ba0"/>
-    <ds:schemaRef ds:uri="f62ef740-d444-4f18-80a2-7590fdcab1ce"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Aggiunta descrizione nel database dei tool
</commit_message>
<xml_diff>
--- a/apps/static/assets/dbs/ThreatCatalogComplete.xlsx
+++ b/apps/static/assets/dbs/ThreatCatalogComplete.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fefox/Desktop/Web3/apps/static/assets/dbs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A20C026C-C6A7-D041-8659-4144E80AA269}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{6272BCCF-FCCC-9E46-A4C9-808ABE59E86E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-38400" yWindow="-3100" windowWidth="38400" windowHeight="21100" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -24,7 +24,7 @@
   </definedNames>
   <calcPr calcId="191028"/>
   <pivotCaches>
-    <pivotCache cacheId="2" r:id="rId6"/>
+    <pivotCache cacheId="0" r:id="rId6"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4036" uniqueCount="920">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4039" uniqueCount="922">
   <si>
     <t>TID</t>
   </si>
@@ -2846,6 +2846,12 @@
   </si>
   <si>
     <t>java -jar DirBuster-1.0-RC1.jar -H -u {url}</t>
+  </si>
+  <si>
+    <t>Nmap</t>
+  </si>
+  <si>
+    <t>nmap -v -Pn {ip}</t>
   </si>
 </sst>
 </file>
@@ -2978,7 +2984,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -3048,20 +3054,24 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="21">
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -3071,9 +3081,6 @@
           <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
@@ -8117,7 +8124,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{48CB07D6-9F6C-094F-A3D3-916741F281CD}" name="Tabella pivot1" cacheId="2" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valori" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{48CB07D6-9F6C-094F-A3D3-916741F281CD}" name="Tabella pivot1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valori" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A1:B25" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="14">
     <pivotField showAll="0"/>
@@ -8315,15 +8322,16 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{5ECAFCE9-964F-A04C-B050-422AACCFD3F5}" name="Tabella4" displayName="Tabella4" ref="A1:D3" totalsRowShown="0">
-  <autoFilter ref="A1:D3" xr:uid="{5ECAFCE9-964F-A04C-B050-422AACCFD3F5}"/>
-  <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{6405AD35-9222-B34C-A112-EC4FDEAC5BE2}" name="ToolID" dataDxfId="1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{5ECAFCE9-964F-A04C-B050-422AACCFD3F5}" name="Tabella4" displayName="Tabella4" ref="A1:E4" totalsRowShown="0">
+  <autoFilter ref="A1:E4" xr:uid="{5ECAFCE9-964F-A04C-B050-422AACCFD3F5}"/>
+  <tableColumns count="5">
+    <tableColumn id="1" xr3:uid="{6405AD35-9222-B34C-A112-EC4FDEAC5BE2}" name="ToolID" dataDxfId="0">
       <calculatedColumnFormula>ROW(Tabella4[[#This Row],[Name]])-1</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="4" xr3:uid="{94F8DBBB-A826-8B4A-8C87-395122CA233A}" name="Name"/>
     <tableColumn id="2" xr3:uid="{FB636F07-AAD2-AE48-87BB-965F92F829C2}" name="CapecID"/>
     <tableColumn id="3" xr3:uid="{52487567-ED26-B840-ABFD-DB1BF72A83C9}" name="Command"/>
+    <tableColumn id="5" xr3:uid="{0296B95F-6562-0746-B0C6-FE3564F6272C}" name="Description"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -24341,7 +24349,7 @@
   </sheetData>
   <phoneticPr fontId="11" type="noConversion"/>
   <conditionalFormatting sqref="O1:Q299">
-    <cfRule type="containsBlanks" dxfId="0" priority="1" stopIfTrue="1">
+    <cfRule type="containsBlanks" dxfId="1" priority="1" stopIfTrue="1">
       <formula>LEN(TRIM(O1))=0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -25584,7 +25592,7 @@
       </c>
     </row>
     <row r="30" spans="1:13" ht="48">
-      <c r="A30" s="29" t="s">
+      <c r="A30" s="27" t="s">
         <v>732</v>
       </c>
       <c r="B30" s="5" t="s">
@@ -25627,7 +25635,7 @@
       </c>
     </row>
     <row r="31" spans="1:13" ht="48">
-      <c r="A31" s="29"/>
+      <c r="A31" s="27"/>
       <c r="B31" s="5" t="s">
         <v>735</v>
       </c>
@@ -25668,7 +25676,7 @@
       </c>
     </row>
     <row r="32" spans="1:13" ht="32">
-      <c r="A32" s="29"/>
+      <c r="A32" s="27"/>
       <c r="B32" s="5" t="s">
         <v>737</v>
       </c>
@@ -25709,7 +25717,7 @@
       </c>
     </row>
     <row r="33" spans="1:13" ht="96">
-      <c r="A33" s="29"/>
+      <c r="A33" s="27"/>
       <c r="B33" s="5" t="s">
         <v>51</v>
       </c>
@@ -25750,7 +25758,7 @@
       </c>
     </row>
     <row r="34" spans="1:13" ht="32">
-      <c r="A34" s="29"/>
+      <c r="A34" s="27"/>
       <c r="B34" s="5" t="s">
         <v>740</v>
       </c>
@@ -25791,7 +25799,7 @@
       </c>
     </row>
     <row r="35" spans="1:13" ht="32">
-      <c r="A35" s="29"/>
+      <c r="A35" s="27"/>
       <c r="B35" s="5" t="s">
         <v>414</v>
       </c>
@@ -25832,7 +25840,7 @@
       </c>
     </row>
     <row r="36" spans="1:13" ht="80">
-      <c r="A36" s="29"/>
+      <c r="A36" s="27"/>
       <c r="B36" s="5" t="s">
         <v>743</v>
       </c>
@@ -26371,7 +26379,7 @@
       </c>
     </row>
     <row r="49" spans="1:13" ht="78" customHeight="1">
-      <c r="A49" s="29" t="s">
+      <c r="A49" s="27" t="s">
         <v>761</v>
       </c>
       <c r="B49" s="5" t="s">
@@ -26414,7 +26422,7 @@
       </c>
     </row>
     <row r="50" spans="1:13" ht="32">
-      <c r="A50" s="29"/>
+      <c r="A50" s="27"/>
       <c r="B50" s="5" t="s">
         <v>409</v>
       </c>
@@ -26455,7 +26463,7 @@
       </c>
     </row>
     <row r="51" spans="1:13" ht="16">
-      <c r="A51" s="29"/>
+      <c r="A51" s="27"/>
       <c r="B51" s="5" t="s">
         <v>414</v>
       </c>
@@ -26496,7 +26504,7 @@
       </c>
     </row>
     <row r="52" spans="1:13" ht="32">
-      <c r="A52" s="29"/>
+      <c r="A52" s="27"/>
       <c r="B52" s="5" t="s">
         <v>766</v>
       </c>
@@ -26537,7 +26545,7 @@
       </c>
     </row>
     <row r="53" spans="1:13" ht="96">
-      <c r="A53" s="29"/>
+      <c r="A53" s="27"/>
       <c r="B53" s="5" t="s">
         <v>768</v>
       </c>
@@ -26578,7 +26586,7 @@
       </c>
     </row>
     <row r="54" spans="1:13">
-      <c r="A54" s="29"/>
+      <c r="A54" s="27"/>
       <c r="B54" s="5" t="s">
         <v>770</v>
       </c>
@@ -26619,7 +26627,7 @@
       </c>
     </row>
     <row r="55" spans="1:13" ht="64">
-      <c r="A55" s="29"/>
+      <c r="A55" s="27"/>
       <c r="B55" s="5" t="s">
         <v>772</v>
       </c>
@@ -26660,7 +26668,7 @@
       </c>
     </row>
     <row r="56" spans="1:13" ht="64">
-      <c r="A56" s="29"/>
+      <c r="A56" s="27"/>
       <c r="B56" s="5" t="s">
         <v>774</v>
       </c>
@@ -26701,7 +26709,7 @@
       </c>
     </row>
     <row r="57" spans="1:13" ht="32">
-      <c r="A57" s="27" t="s">
+      <c r="A57" s="28" t="s">
         <v>776</v>
       </c>
       <c r="B57" s="6" t="s">
@@ -26743,7 +26751,7 @@
       </c>
     </row>
     <row r="58" spans="1:13" ht="80">
-      <c r="A58" s="27"/>
+      <c r="A58" s="28"/>
       <c r="B58" s="7" t="s">
         <v>779</v>
       </c>
@@ -26783,7 +26791,7 @@
       </c>
     </row>
     <row r="59" spans="1:13" ht="64" customHeight="1">
-      <c r="A59" s="27"/>
+      <c r="A59" s="28"/>
       <c r="B59" s="7" t="s">
         <v>781</v>
       </c>
@@ -26823,7 +26831,7 @@
       </c>
     </row>
     <row r="60" spans="1:13" ht="16">
-      <c r="A60" s="27"/>
+      <c r="A60" s="28"/>
       <c r="B60" s="7" t="s">
         <v>283</v>
       </c>
@@ -26863,7 +26871,7 @@
       </c>
     </row>
     <row r="61" spans="1:13" ht="32">
-      <c r="A61" s="27"/>
+      <c r="A61" s="28"/>
       <c r="B61" s="7" t="s">
         <v>785</v>
       </c>
@@ -26903,7 +26911,7 @@
       </c>
     </row>
     <row r="62" spans="1:13" ht="32">
-      <c r="A62" s="27"/>
+      <c r="A62" s="28"/>
       <c r="B62" s="7" t="s">
         <v>787</v>
       </c>
@@ -26943,7 +26951,7 @@
       </c>
     </row>
     <row r="63" spans="1:13" ht="16">
-      <c r="A63" s="27"/>
+      <c r="A63" s="28"/>
       <c r="B63" s="7" t="s">
         <v>790</v>
       </c>
@@ -26983,7 +26991,7 @@
       </c>
     </row>
     <row r="64" spans="1:13" ht="32">
-      <c r="A64" s="27"/>
+      <c r="A64" s="28"/>
       <c r="B64" s="6" t="s">
         <v>792</v>
       </c>
@@ -27023,7 +27031,7 @@
       </c>
     </row>
     <row r="65" spans="1:13" ht="16">
-      <c r="A65" s="27"/>
+      <c r="A65" s="28"/>
       <c r="B65" s="7" t="s">
         <v>81</v>
       </c>
@@ -27063,7 +27071,7 @@
       </c>
     </row>
     <row r="66" spans="1:13" ht="16">
-      <c r="A66" s="27"/>
+      <c r="A66" s="28"/>
       <c r="B66" s="7" t="s">
         <v>795</v>
       </c>
@@ -27103,7 +27111,7 @@
       </c>
     </row>
     <row r="67" spans="1:13" ht="48">
-      <c r="A67" s="27"/>
+      <c r="A67" s="28"/>
       <c r="B67" s="6" t="s">
         <v>280</v>
       </c>
@@ -27143,38 +27151,38 @@
       </c>
     </row>
     <row r="68" spans="1:13" ht="16">
-      <c r="A68" s="27"/>
-      <c r="B68" s="27" t="s">
+      <c r="A68" s="28"/>
+      <c r="B68" s="28" t="s">
         <v>357</v>
       </c>
       <c r="C68" s="6" t="s">
         <v>797</v>
       </c>
-      <c r="D68" s="27" t="s">
+      <c r="D68" s="28" t="s">
         <v>274</v>
       </c>
-      <c r="E68" s="27" t="s">
+      <c r="E68" s="28" t="s">
         <v>783</v>
       </c>
-      <c r="F68" s="27" t="s">
-        <v>22</v>
-      </c>
-      <c r="G68" s="27" t="s">
+      <c r="F68" s="28" t="s">
+        <v>22</v>
+      </c>
+      <c r="G68" s="28" t="s">
         <v>22</v>
       </c>
       <c r="H68" s="26" t="s">
         <v>22</v>
       </c>
-      <c r="I68" s="27" t="s">
+      <c r="I68" s="28" t="s">
         <v>364</v>
       </c>
-      <c r="J68" s="27" t="s">
-        <v>22</v>
-      </c>
-      <c r="K68" s="27" t="s">
-        <v>22</v>
-      </c>
-      <c r="L68" s="27" t="s">
+      <c r="J68" s="28" t="s">
+        <v>22</v>
+      </c>
+      <c r="K68" s="28" t="s">
+        <v>22</v>
+      </c>
+      <c r="L68" s="28" t="s">
         <v>23</v>
       </c>
       <c r="M68" s="26" t="str">
@@ -27183,24 +27191,24 @@
       </c>
     </row>
     <row r="69" spans="1:13" ht="16">
-      <c r="A69" s="27"/>
-      <c r="B69" s="27"/>
+      <c r="A69" s="28"/>
+      <c r="B69" s="28"/>
       <c r="C69" s="6" t="s">
         <v>798</v>
       </c>
-      <c r="D69" s="27"/>
-      <c r="E69" s="27"/>
-      <c r="F69" s="27"/>
-      <c r="G69" s="27"/>
+      <c r="D69" s="28"/>
+      <c r="E69" s="28"/>
+      <c r="F69" s="28"/>
+      <c r="G69" s="28"/>
       <c r="H69" s="26"/>
-      <c r="I69" s="27"/>
-      <c r="J69" s="27"/>
-      <c r="K69" s="27"/>
-      <c r="L69" s="27"/>
+      <c r="I69" s="28"/>
+      <c r="J69" s="28"/>
+      <c r="K69" s="28"/>
+      <c r="L69" s="28"/>
       <c r="M69" s="26"/>
     </row>
     <row r="70" spans="1:13" ht="28">
-      <c r="A70" s="28" t="s">
+      <c r="A70" s="29" t="s">
         <v>799</v>
       </c>
       <c r="B70" s="16" t="s">
@@ -27246,7 +27254,7 @@
       </c>
     </row>
     <row r="71" spans="1:13" ht="51">
-      <c r="A71" s="28"/>
+      <c r="A71" s="29"/>
       <c r="B71" s="16" t="s">
         <v>51</v>
       </c>
@@ -27290,7 +27298,7 @@
       </c>
     </row>
     <row r="72" spans="1:13" ht="28">
-      <c r="A72" s="28"/>
+      <c r="A72" s="29"/>
       <c r="B72" s="16" t="s">
         <v>684</v>
       </c>
@@ -27334,7 +27342,7 @@
       </c>
     </row>
     <row r="73" spans="1:13" ht="28">
-      <c r="A73" s="28"/>
+      <c r="A73" s="29"/>
       <c r="B73" s="16" t="s">
         <v>806</v>
       </c>
@@ -27896,15 +27904,6 @@
     </row>
   </sheetData>
   <mergeCells count="23">
-    <mergeCell ref="A2:A7"/>
-    <mergeCell ref="A8:A14"/>
-    <mergeCell ref="A25:A29"/>
-    <mergeCell ref="A15:A24"/>
-    <mergeCell ref="A49:A56"/>
-    <mergeCell ref="A44:A48"/>
-    <mergeCell ref="A41:A43"/>
-    <mergeCell ref="A30:A36"/>
-    <mergeCell ref="A37:A40"/>
     <mergeCell ref="M68:M69"/>
     <mergeCell ref="H68:H69"/>
     <mergeCell ref="A74:A85"/>
@@ -27919,6 +27918,15 @@
     <mergeCell ref="B68:B69"/>
     <mergeCell ref="D68:D69"/>
     <mergeCell ref="E68:E69"/>
+    <mergeCell ref="A2:A7"/>
+    <mergeCell ref="A8:A14"/>
+    <mergeCell ref="A25:A29"/>
+    <mergeCell ref="A15:A24"/>
+    <mergeCell ref="A49:A56"/>
+    <mergeCell ref="A44:A48"/>
+    <mergeCell ref="A41:A43"/>
+    <mergeCell ref="A30:A36"/>
+    <mergeCell ref="A37:A40"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -28770,10 +28778,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C51FC597-29FA-1D4E-A4C8-B79027768242}">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="181" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -28782,7 +28790,7 @@
     <col min="4" max="4" width="40.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:5">
       <c r="A1" t="s">
         <v>911</v>
       </c>
@@ -28795,8 +28803,11 @@
       <c r="D1" t="s">
         <v>912</v>
       </c>
-    </row>
-    <row r="2" spans="1:4">
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
       <c r="A2">
         <f>ROW(Tabella4[[#This Row],[Name]])-1</f>
         <v>1</v>
@@ -28811,7 +28822,7 @@
         <v>918</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:5">
       <c r="A3">
         <f>ROW(Tabella4[[#This Row],[Name]])-1</f>
         <v>2</v>
@@ -28824,6 +28835,18 @@
       </c>
       <c r="D3" t="s">
         <v>919</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" s="30">
+        <f>ROW(Tabella4[[#This Row],[Name]])-1</f>
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>920</v>
+      </c>
+      <c r="D4" t="s">
+        <v>921</v>
       </c>
     </row>
   </sheetData>
@@ -28835,6 +28858,26 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="633f040f-4953-46e7-8610-82b0c5296ba0">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="f62ef740-d444-4f18-80a2-7590fdcab1ce" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x0101009A9CE0B21D9C3A45B31425227616CD6F" ma:contentTypeVersion="11" ma:contentTypeDescription="Creare un nuovo documento." ma:contentTypeScope="" ma:versionID="180d662eb9e2621fe5c8d1498a11e3bf">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="633f040f-4953-46e7-8610-82b0c5296ba0" xmlns:ns3="f62ef740-d444-4f18-80a2-7590fdcab1ce" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="64519aed5f694bce5dc2f4bcf073d27d" ns2:_="" ns3:_="">
     <xsd:import namespace="633f040f-4953-46e7-8610-82b0c5296ba0"/>
@@ -29045,27 +29088,32 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{83D5100D-0E56-4B30-B42D-2AEC6B837C39}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="633f040f-4953-46e7-8610-82b0c5296ba0"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="f62ef740-d444-4f18-80a2-7590fdcab1ce"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="633f040f-4953-46e7-8610-82b0c5296ba0">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="f62ef740-d444-4f18-80a2-7590fdcab1ce" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2C6CC7BA-2E2C-4B0D-8103-11A51D82E8EC}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CA355F46-8632-4C01-B7E7-8E7DCFF50FB7}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -29082,29 +29130,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2C6CC7BA-2E2C-4B0D-8103-11A51D82E8EC}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{83D5100D-0E56-4B30-B42D-2AEC6B837C39}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="633f040f-4953-46e7-8610-82b0c5296ba0"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="f62ef740-d444-4f18-80a2-7590fdcab1ce"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Modificato font-size dei badge degli attacchi sui component_id
</commit_message>
<xml_diff>
--- a/apps/static/assets/dbs/ThreatCatalogComplete.xlsx
+++ b/apps/static/assets/dbs/ThreatCatalogComplete.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fefox/Desktop/Web3/apps/static/assets/dbs/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fefox/Desktop/Web/apps/static/assets/dbs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6272BCCF-FCCC-9E46-A4C9-808ABE59E86E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3121B275-4239-FC44-813C-35F223AF8B77}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38400" yWindow="-3100" windowWidth="38400" windowHeight="21100" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16380" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Threat Components" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
   </definedNames>
   <calcPr calcId="191028"/>
   <pivotCaches>
-    <pivotCache cacheId="0" r:id="rId6"/>
+    <pivotCache cacheId="1" r:id="rId6"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4039" uniqueCount="922">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4043" uniqueCount="924">
   <si>
     <t>TID</t>
   </si>
@@ -2852,6 +2852,12 @@
   </si>
   <si>
     <t>nmap -v -Pn {ip}</t>
+  </si>
+  <si>
+    <t>nmap -v -Pn {ip_range}</t>
+  </si>
+  <si>
+    <t>292, 300</t>
   </si>
 </sst>
 </file>
@@ -2984,7 +2990,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -3063,14 +3069,13 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="21">
+  <dxfs count="22">
     <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
+      <numFmt numFmtId="30" formatCode="@"/>
     </dxf>
     <dxf>
       <font>
@@ -3081,6 +3086,9 @@
           <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
@@ -8124,7 +8132,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{48CB07D6-9F6C-094F-A3D3-916741F281CD}" name="Tabella pivot1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valori" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{48CB07D6-9F6C-094F-A3D3-916741F281CD}" name="Tabella pivot1" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valori" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A1:B25" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="14">
     <pivotField showAll="0"/>
@@ -8265,7 +8273,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{DEFAB213-4389-184E-911C-CDCC8CABBD38}" name="Tabella1" displayName="Tabella1" ref="A1:R299" totalsRowShown="0" dataDxfId="20">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{DEFAB213-4389-184E-911C-CDCC8CABBD38}" name="Tabella1" displayName="Tabella1" ref="A1:R299" totalsRowShown="0" dataDxfId="21">
   <autoFilter ref="A1:R299" xr:uid="{DEFAB213-4389-184E-911C-CDCC8CABBD38}">
     <filterColumn colId="1">
       <filters>
@@ -8277,32 +8285,32 @@
     <sortCondition ref="B1:B299"/>
   </sortState>
   <tableColumns count="18">
-    <tableColumn id="16" xr3:uid="{DE426BDB-E154-EE46-B7B3-5B538C8AEC32}" name="TID" dataDxfId="19">
+    <tableColumn id="16" xr3:uid="{DE426BDB-E154-EE46-B7B3-5B538C8AEC32}" name="TID" dataDxfId="20">
       <calculatedColumnFormula>CONCATENATE("T",ROW(A2)-1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="1" xr3:uid="{A0AE63DC-99F7-7D4F-B824-AB7765893284}" name="Asset" dataDxfId="18"/>
-    <tableColumn id="2" xr3:uid="{0FA38BFF-C67B-0C43-B1BA-F6338DBFB0C8}" name="Threat" dataDxfId="17"/>
-    <tableColumn id="3" xr3:uid="{BFC77F7C-F096-8345-97EA-317816ED869D}" name="Description" dataDxfId="16"/>
-    <tableColumn id="4" xr3:uid="{258F3B86-1461-D64A-AE3B-CEAC97B2B533}" name="STRIDE" dataDxfId="15"/>
-    <tableColumn id="6" xr3:uid="{0FD06C95-5962-AC4D-B9EF-4DBB5728E736}" name="Compromised" dataDxfId="14"/>
-    <tableColumn id="7" xr3:uid="{9E5B99AD-1F1D-B44C-ABDF-6F7E9177F3DE}" name="PreC" dataDxfId="13"/>
-    <tableColumn id="8" xr3:uid="{D4F97A81-E528-2841-B4DE-321362F90F65}" name="PreI" dataDxfId="12"/>
-    <tableColumn id="9" xr3:uid="{018427D6-D385-3447-B4A4-95003B3341F6}" name="PreA" dataDxfId="11"/>
-    <tableColumn id="10" xr3:uid="{8334AC57-4A09-5744-9484-073ECEE2E513}" name="Precondition" dataDxfId="10"/>
-    <tableColumn id="12" xr3:uid="{DDBE315D-E051-2C47-A765-EE1DB2E118EA}" name="PostC" dataDxfId="9">
+    <tableColumn id="1" xr3:uid="{A0AE63DC-99F7-7D4F-B824-AB7765893284}" name="Asset" dataDxfId="19"/>
+    <tableColumn id="2" xr3:uid="{0FA38BFF-C67B-0C43-B1BA-F6338DBFB0C8}" name="Threat" dataDxfId="18"/>
+    <tableColumn id="3" xr3:uid="{BFC77F7C-F096-8345-97EA-317816ED869D}" name="Description" dataDxfId="17"/>
+    <tableColumn id="4" xr3:uid="{258F3B86-1461-D64A-AE3B-CEAC97B2B533}" name="STRIDE" dataDxfId="16"/>
+    <tableColumn id="6" xr3:uid="{0FD06C95-5962-AC4D-B9EF-4DBB5728E736}" name="Compromised" dataDxfId="15"/>
+    <tableColumn id="7" xr3:uid="{9E5B99AD-1F1D-B44C-ABDF-6F7E9177F3DE}" name="PreC" dataDxfId="14"/>
+    <tableColumn id="8" xr3:uid="{D4F97A81-E528-2841-B4DE-321362F90F65}" name="PreI" dataDxfId="13"/>
+    <tableColumn id="9" xr3:uid="{018427D6-D385-3447-B4A4-95003B3341F6}" name="PreA" dataDxfId="12"/>
+    <tableColumn id="10" xr3:uid="{8334AC57-4A09-5744-9484-073ECEE2E513}" name="Precondition" dataDxfId="11"/>
+    <tableColumn id="12" xr3:uid="{DDBE315D-E051-2C47-A765-EE1DB2E118EA}" name="PostC" dataDxfId="10">
       <calculatedColumnFormula>MID(N2,2,1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" xr3:uid="{243C1B9B-76C9-0345-B727-4F11FD75DF6B}" name="PostI" dataDxfId="8">
+    <tableColumn id="13" xr3:uid="{243C1B9B-76C9-0345-B727-4F11FD75DF6B}" name="PostI" dataDxfId="9">
       <calculatedColumnFormula>MID(N2,4,1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="14" xr3:uid="{DD688DAA-2C9A-C247-AEC4-CBDADE9B2B2E}" name="PostA" dataDxfId="7">
+    <tableColumn id="14" xr3:uid="{DD688DAA-2C9A-C247-AEC4-CBDADE9B2B2E}" name="PostA" dataDxfId="8">
       <calculatedColumnFormula>MID(N2,6,1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="15" xr3:uid="{CEE151EC-4E5B-0C41-8586-5A2D7E483661}" name="PostCondition" dataDxfId="6"/>
-    <tableColumn id="5" xr3:uid="{62EC5D77-1F78-1645-8697-BC5450583418}" name="CapecMeta" dataDxfId="5"/>
-    <tableColumn id="11" xr3:uid="{0DCD762C-4EE7-8141-BC05-9DB756A5BEF2}" name="CapecStandard" dataDxfId="4"/>
-    <tableColumn id="17" xr3:uid="{9EF317BA-855B-6E4A-9EC7-E1FB88A1FD56}" name="CapecDetailed" dataDxfId="3"/>
-    <tableColumn id="18" xr3:uid="{9BF6197D-4CF5-4941-A460-18823EEFB2E7}" name="Commento" dataDxfId="2"/>
+    <tableColumn id="15" xr3:uid="{CEE151EC-4E5B-0C41-8586-5A2D7E483661}" name="PostCondition" dataDxfId="7"/>
+    <tableColumn id="5" xr3:uid="{62EC5D77-1F78-1645-8697-BC5450583418}" name="CapecMeta" dataDxfId="6"/>
+    <tableColumn id="11" xr3:uid="{0DCD762C-4EE7-8141-BC05-9DB756A5BEF2}" name="CapecStandard" dataDxfId="5"/>
+    <tableColumn id="17" xr3:uid="{9EF317BA-855B-6E4A-9EC7-E1FB88A1FD56}" name="CapecDetailed" dataDxfId="4"/>
+    <tableColumn id="18" xr3:uid="{9BF6197D-4CF5-4941-A460-18823EEFB2E7}" name="Commento" dataDxfId="3"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -8322,14 +8330,14 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{5ECAFCE9-964F-A04C-B050-422AACCFD3F5}" name="Tabella4" displayName="Tabella4" ref="A1:E4" totalsRowShown="0">
-  <autoFilter ref="A1:E4" xr:uid="{5ECAFCE9-964F-A04C-B050-422AACCFD3F5}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{5ECAFCE9-964F-A04C-B050-422AACCFD3F5}" name="Tabella4" displayName="Tabella4" ref="A1:E5" totalsRowShown="0">
+  <autoFilter ref="A1:E5" xr:uid="{5ECAFCE9-964F-A04C-B050-422AACCFD3F5}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{6405AD35-9222-B34C-A112-EC4FDEAC5BE2}" name="ToolID" dataDxfId="0">
+    <tableColumn id="1" xr3:uid="{6405AD35-9222-B34C-A112-EC4FDEAC5BE2}" name="ToolID" dataDxfId="2">
       <calculatedColumnFormula>ROW(Tabella4[[#This Row],[Name]])-1</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="4" xr3:uid="{94F8DBBB-A826-8B4A-8C87-395122CA233A}" name="Name"/>
-    <tableColumn id="2" xr3:uid="{FB636F07-AAD2-AE48-87BB-965F92F829C2}" name="CapecID"/>
+    <tableColumn id="2" xr3:uid="{FB636F07-AAD2-AE48-87BB-965F92F829C2}" name="CapecID" dataDxfId="0"/>
     <tableColumn id="3" xr3:uid="{52487567-ED26-B840-ABFD-DB1BF72A83C9}" name="Command"/>
     <tableColumn id="5" xr3:uid="{0296B95F-6562-0746-B0C6-FE3564F6272C}" name="Description"/>
   </tableColumns>
@@ -28778,10 +28786,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C51FC597-29FA-1D4E-A4C8-B79027768242}">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="181" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -28815,7 +28823,7 @@
       <c r="B2" t="s">
         <v>913</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="23" t="s">
         <v>914</v>
       </c>
       <c r="D2" t="s">
@@ -28830,7 +28838,7 @@
       <c r="B3" t="s">
         <v>915</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="23" t="s">
         <v>916</v>
       </c>
       <c r="D3" t="s">
@@ -28838,15 +28846,33 @@
       </c>
     </row>
     <row r="4" spans="1:5">
-      <c r="A4" s="30">
+      <c r="A4">
         <f>ROW(Tabella4[[#This Row],[Name]])-1</f>
         <v>3</v>
       </c>
       <c r="B4" t="s">
         <v>920</v>
       </c>
+      <c r="C4" s="23" t="s">
+        <v>923</v>
+      </c>
       <c r="D4" t="s">
         <v>921</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5">
+        <f>ROW(Tabella4[[#This Row],[Name]])-1</f>
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>920</v>
+      </c>
+      <c r="C5" s="23" t="s">
+        <v>859</v>
+      </c>
+      <c r="D5" t="s">
+        <v>922</v>
       </c>
     </row>
   </sheetData>
@@ -29092,15 +29118,15 @@
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{83D5100D-0E56-4B30-B42D-2AEC6B837C39}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="633f040f-4953-46e7-8610-82b0c5296ba0"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
     <ds:schemaRef ds:uri="f62ef740-d444-4f18-80a2-7590fdcab1ce"/>
+    <ds:schemaRef ds:uri="633f040f-4953-46e7-8610-82b0c5296ba0"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Modificata implementazione di macm-detail: la threat description deve essere per ciascun attacco e non per componente, perchè i threat cambiano
</commit_message>
<xml_diff>
--- a/apps/static/assets/dbs/ThreatCatalogComplete.xlsx
+++ b/apps/static/assets/dbs/ThreatCatalogComplete.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fefox/Desktop/Web/apps/static/assets/dbs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3121B275-4239-FC44-813C-35F223AF8B77}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22227CA9-676B-E042-8250-82A4742424CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16380" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4043" uniqueCount="924">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4045" uniqueCount="926">
   <si>
     <t>TID</t>
   </si>
@@ -2858,6 +2858,12 @@
   </si>
   <si>
     <t>292, 300</t>
+  </si>
+  <si>
+    <t>QueryCypher</t>
+  </si>
+  <si>
+    <t>match (target)-[:uses]-&gt;(b {type:'Service.DB'}) return target</t>
   </si>
 </sst>
 </file>
@@ -3073,7 +3079,7 @@
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="22">
+  <dxfs count="23">
     <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
     </dxf>
@@ -3086,6 +3092,9 @@
           <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
@@ -8273,7 +8282,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{DEFAB213-4389-184E-911C-CDCC8CABBD38}" name="Tabella1" displayName="Tabella1" ref="A1:R299" totalsRowShown="0" dataDxfId="21">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{DEFAB213-4389-184E-911C-CDCC8CABBD38}" name="Tabella1" displayName="Tabella1" ref="A1:R299" totalsRowShown="0" dataDxfId="22">
   <autoFilter ref="A1:R299" xr:uid="{DEFAB213-4389-184E-911C-CDCC8CABBD38}">
     <filterColumn colId="1">
       <filters>
@@ -8285,32 +8294,32 @@
     <sortCondition ref="B1:B299"/>
   </sortState>
   <tableColumns count="18">
-    <tableColumn id="16" xr3:uid="{DE426BDB-E154-EE46-B7B3-5B538C8AEC32}" name="TID" dataDxfId="20">
+    <tableColumn id="16" xr3:uid="{DE426BDB-E154-EE46-B7B3-5B538C8AEC32}" name="TID" dataDxfId="21">
       <calculatedColumnFormula>CONCATENATE("T",ROW(A2)-1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="1" xr3:uid="{A0AE63DC-99F7-7D4F-B824-AB7765893284}" name="Asset" dataDxfId="19"/>
-    <tableColumn id="2" xr3:uid="{0FA38BFF-C67B-0C43-B1BA-F6338DBFB0C8}" name="Threat" dataDxfId="18"/>
-    <tableColumn id="3" xr3:uid="{BFC77F7C-F096-8345-97EA-317816ED869D}" name="Description" dataDxfId="17"/>
-    <tableColumn id="4" xr3:uid="{258F3B86-1461-D64A-AE3B-CEAC97B2B533}" name="STRIDE" dataDxfId="16"/>
-    <tableColumn id="6" xr3:uid="{0FD06C95-5962-AC4D-B9EF-4DBB5728E736}" name="Compromised" dataDxfId="15"/>
-    <tableColumn id="7" xr3:uid="{9E5B99AD-1F1D-B44C-ABDF-6F7E9177F3DE}" name="PreC" dataDxfId="14"/>
-    <tableColumn id="8" xr3:uid="{D4F97A81-E528-2841-B4DE-321362F90F65}" name="PreI" dataDxfId="13"/>
-    <tableColumn id="9" xr3:uid="{018427D6-D385-3447-B4A4-95003B3341F6}" name="PreA" dataDxfId="12"/>
-    <tableColumn id="10" xr3:uid="{8334AC57-4A09-5744-9484-073ECEE2E513}" name="Precondition" dataDxfId="11"/>
-    <tableColumn id="12" xr3:uid="{DDBE315D-E051-2C47-A765-EE1DB2E118EA}" name="PostC" dataDxfId="10">
+    <tableColumn id="1" xr3:uid="{A0AE63DC-99F7-7D4F-B824-AB7765893284}" name="Asset" dataDxfId="20"/>
+    <tableColumn id="2" xr3:uid="{0FA38BFF-C67B-0C43-B1BA-F6338DBFB0C8}" name="Threat" dataDxfId="19"/>
+    <tableColumn id="3" xr3:uid="{BFC77F7C-F096-8345-97EA-317816ED869D}" name="Description" dataDxfId="18"/>
+    <tableColumn id="4" xr3:uid="{258F3B86-1461-D64A-AE3B-CEAC97B2B533}" name="STRIDE" dataDxfId="17"/>
+    <tableColumn id="6" xr3:uid="{0FD06C95-5962-AC4D-B9EF-4DBB5728E736}" name="Compromised" dataDxfId="16"/>
+    <tableColumn id="7" xr3:uid="{9E5B99AD-1F1D-B44C-ABDF-6F7E9177F3DE}" name="PreC" dataDxfId="15"/>
+    <tableColumn id="8" xr3:uid="{D4F97A81-E528-2841-B4DE-321362F90F65}" name="PreI" dataDxfId="14"/>
+    <tableColumn id="9" xr3:uid="{018427D6-D385-3447-B4A4-95003B3341F6}" name="PreA" dataDxfId="13"/>
+    <tableColumn id="10" xr3:uid="{8334AC57-4A09-5744-9484-073ECEE2E513}" name="Precondition" dataDxfId="12"/>
+    <tableColumn id="12" xr3:uid="{DDBE315D-E051-2C47-A765-EE1DB2E118EA}" name="PostC" dataDxfId="11">
       <calculatedColumnFormula>MID(N2,2,1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" xr3:uid="{243C1B9B-76C9-0345-B727-4F11FD75DF6B}" name="PostI" dataDxfId="9">
+    <tableColumn id="13" xr3:uid="{243C1B9B-76C9-0345-B727-4F11FD75DF6B}" name="PostI" dataDxfId="10">
       <calculatedColumnFormula>MID(N2,4,1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="14" xr3:uid="{DD688DAA-2C9A-C247-AEC4-CBDADE9B2B2E}" name="PostA" dataDxfId="8">
+    <tableColumn id="14" xr3:uid="{DD688DAA-2C9A-C247-AEC4-CBDADE9B2B2E}" name="PostA" dataDxfId="9">
       <calculatedColumnFormula>MID(N2,6,1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="15" xr3:uid="{CEE151EC-4E5B-0C41-8586-5A2D7E483661}" name="PostCondition" dataDxfId="7"/>
-    <tableColumn id="5" xr3:uid="{62EC5D77-1F78-1645-8697-BC5450583418}" name="CapecMeta" dataDxfId="6"/>
-    <tableColumn id="11" xr3:uid="{0DCD762C-4EE7-8141-BC05-9DB756A5BEF2}" name="CapecStandard" dataDxfId="5"/>
-    <tableColumn id="17" xr3:uid="{9EF317BA-855B-6E4A-9EC7-E1FB88A1FD56}" name="CapecDetailed" dataDxfId="4"/>
-    <tableColumn id="18" xr3:uid="{9BF6197D-4CF5-4941-A460-18823EEFB2E7}" name="Commento" dataDxfId="3"/>
+    <tableColumn id="15" xr3:uid="{CEE151EC-4E5B-0C41-8586-5A2D7E483661}" name="PostCondition" dataDxfId="8"/>
+    <tableColumn id="5" xr3:uid="{62EC5D77-1F78-1645-8697-BC5450583418}" name="CapecMeta" dataDxfId="7"/>
+    <tableColumn id="11" xr3:uid="{0DCD762C-4EE7-8141-BC05-9DB756A5BEF2}" name="CapecStandard" dataDxfId="6"/>
+    <tableColumn id="17" xr3:uid="{9EF317BA-855B-6E4A-9EC7-E1FB88A1FD56}" name="CapecDetailed" dataDxfId="5"/>
+    <tableColumn id="18" xr3:uid="{9BF6197D-4CF5-4941-A460-18823EEFB2E7}" name="Commento" dataDxfId="4"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -8330,14 +8339,15 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{5ECAFCE9-964F-A04C-B050-422AACCFD3F5}" name="Tabella4" displayName="Tabella4" ref="A1:E5" totalsRowShown="0">
-  <autoFilter ref="A1:E5" xr:uid="{5ECAFCE9-964F-A04C-B050-422AACCFD3F5}"/>
-  <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{6405AD35-9222-B34C-A112-EC4FDEAC5BE2}" name="ToolID" dataDxfId="2">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{5ECAFCE9-964F-A04C-B050-422AACCFD3F5}" name="Tabella4" displayName="Tabella4" ref="A1:F5" totalsRowShown="0">
+  <autoFilter ref="A1:F5" xr:uid="{5ECAFCE9-964F-A04C-B050-422AACCFD3F5}"/>
+  <tableColumns count="6">
+    <tableColumn id="1" xr3:uid="{6405AD35-9222-B34C-A112-EC4FDEAC5BE2}" name="ToolID" dataDxfId="3">
       <calculatedColumnFormula>ROW(Tabella4[[#This Row],[Name]])-1</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="4" xr3:uid="{94F8DBBB-A826-8B4A-8C87-395122CA233A}" name="Name"/>
-    <tableColumn id="2" xr3:uid="{FB636F07-AAD2-AE48-87BB-965F92F829C2}" name="CapecID" dataDxfId="0"/>
+    <tableColumn id="2" xr3:uid="{FB636F07-AAD2-AE48-87BB-965F92F829C2}" name="CapecID" dataDxfId="2"/>
+    <tableColumn id="7" xr3:uid="{80DB7B80-C531-B649-B58E-F29831E2ACA8}" name="QueryCypher" dataDxfId="0"/>
     <tableColumn id="3" xr3:uid="{52487567-ED26-B840-ABFD-DB1BF72A83C9}" name="Command"/>
     <tableColumn id="5" xr3:uid="{0296B95F-6562-0746-B0C6-FE3564F6272C}" name="Description"/>
   </tableColumns>
@@ -28786,10 +28796,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C51FC597-29FA-1D4E-A4C8-B79027768242}">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="181" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" zoomScale="200" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -28798,7 +28808,7 @@
     <col min="4" max="4" width="40.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:6">
       <c r="A1" t="s">
         <v>911</v>
       </c>
@@ -28809,13 +28819,16 @@
         <v>910</v>
       </c>
       <c r="D1" t="s">
+        <v>924</v>
+      </c>
+      <c r="E1" t="s">
         <v>912</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:6">
       <c r="A2">
         <f>ROW(Tabella4[[#This Row],[Name]])-1</f>
         <v>1</v>
@@ -28826,11 +28839,14 @@
       <c r="C2" s="23" t="s">
         <v>914</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="23" t="s">
+        <v>925</v>
+      </c>
+      <c r="E2" t="s">
         <v>918</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:6">
       <c r="A3">
         <f>ROW(Tabella4[[#This Row],[Name]])-1</f>
         <v>2</v>
@@ -28841,11 +28857,12 @@
       <c r="C3" s="23" t="s">
         <v>916</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="23"/>
+      <c r="E3" t="s">
         <v>919</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:6">
       <c r="A4">
         <f>ROW(Tabella4[[#This Row],[Name]])-1</f>
         <v>3</v>
@@ -28856,11 +28873,12 @@
       <c r="C4" s="23" t="s">
         <v>923</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="23"/>
+      <c r="E4" t="s">
         <v>921</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:6">
       <c r="A5">
         <f>ROW(Tabella4[[#This Row],[Name]])-1</f>
         <v>4</v>
@@ -28871,7 +28889,8 @@
       <c r="C5" s="23" t="s">
         <v>859</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" s="23"/>
+      <c r="E5" t="s">
         <v>922</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Modificata logica di ricaricamento dei database: ora viene droppata tutta la tabella
</commit_message>
<xml_diff>
--- a/apps/static/assets/dbs/ThreatCatalogComplete.xlsx
+++ b/apps/static/assets/dbs/ThreatCatalogComplete.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fefox/Desktop/Web/apps/static/assets/dbs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22227CA9-676B-E042-8250-82A4742424CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1201FE8-C94C-744E-903C-6D00169FFA36}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16380" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2860,10 +2860,10 @@
     <t>292, 300</t>
   </si>
   <si>
-    <t>QueryCypher</t>
-  </si>
-  <si>
     <t>match (target)-[:uses]-&gt;(b {type:'Service.DB'}) return target</t>
+  </si>
+  <si>
+    <t>CypherQuery</t>
   </si>
 </sst>
 </file>
@@ -8347,7 +8347,7 @@
     </tableColumn>
     <tableColumn id="4" xr3:uid="{94F8DBBB-A826-8B4A-8C87-395122CA233A}" name="Name"/>
     <tableColumn id="2" xr3:uid="{FB636F07-AAD2-AE48-87BB-965F92F829C2}" name="CapecID" dataDxfId="2"/>
-    <tableColumn id="7" xr3:uid="{80DB7B80-C531-B649-B58E-F29831E2ACA8}" name="QueryCypher" dataDxfId="0"/>
+    <tableColumn id="7" xr3:uid="{80DB7B80-C531-B649-B58E-F29831E2ACA8}" name="CypherQuery" dataDxfId="0"/>
     <tableColumn id="3" xr3:uid="{52487567-ED26-B840-ABFD-DB1BF72A83C9}" name="Command"/>
     <tableColumn id="5" xr3:uid="{0296B95F-6562-0746-B0C6-FE3564F6272C}" name="Description"/>
   </tableColumns>
@@ -28799,7 +28799,7 @@
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="200" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -28819,7 +28819,7 @@
         <v>910</v>
       </c>
       <c r="D1" t="s">
-        <v>924</v>
+        <v>925</v>
       </c>
       <c r="E1" t="s">
         <v>912</v>
@@ -28840,7 +28840,7 @@
         <v>914</v>
       </c>
       <c r="D2" s="23" t="s">
-        <v>925</v>
+        <v>924</v>
       </c>
       <c r="E2" t="s">
         <v>918</v>

</xml_diff>

<commit_message>
Aggiunto controllo sul macm per stabilire se un tool è applicabile
</commit_message>
<xml_diff>
--- a/apps/static/assets/dbs/ThreatCatalogComplete.xlsx
+++ b/apps/static/assets/dbs/ThreatCatalogComplete.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fefox/Desktop/Web/apps/static/assets/dbs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1201FE8-C94C-744E-903C-6D00169FFA36}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{703449EB-9946-664A-B7B2-E2AD55F2CA07}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16380" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -24,7 +24,7 @@
   </definedNames>
   <calcPr calcId="191028"/>
   <pivotCaches>
-    <pivotCache cacheId="1" r:id="rId6"/>
+    <pivotCache cacheId="7" r:id="rId6"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4045" uniqueCount="926">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4053" uniqueCount="935">
   <si>
     <t>TID</t>
   </si>
@@ -2665,9 +2665,6 @@
     <t>169</t>
   </si>
   <si>
-    <t>309</t>
-  </si>
-  <si>
     <t>Commento</t>
   </si>
   <si>
@@ -2854,16 +2851,46 @@
     <t>nmap -v -Pn {ip}</t>
   </si>
   <si>
-    <t>nmap -v -Pn {ip_range}</t>
-  </si>
-  <si>
-    <t>292, 300</t>
-  </si>
-  <si>
-    <t>match (target)-[:uses]-&gt;(b {type:'Service.DB'}) return target</t>
+    <t>match (target)-[:uses]-&gt;(b {type:'Service.DB'}) return target.component_id as component_id</t>
+  </si>
+  <si>
+    <t>match (n {type:'Service.Web'}) return n.component_id as component_id</t>
+  </si>
+  <si>
+    <t>match (target)-[:connects]-&gt;(net {type:'Network'}) return target.component_id as component_id</t>
+  </si>
+  <si>
+    <t>292, 309</t>
+  </si>
+  <si>
+    <t>match (n:Network) return n.component_id as component_id</t>
+  </si>
+  <si>
+    <t>nmap -v {ip_range}</t>
+  </si>
+  <si>
+    <t>JohnTheRipper</t>
+  </si>
+  <si>
+    <t>match (n {type:'Service.VM'}) return n.component_id as component_id</t>
+  </si>
+  <si>
+    <t>john --wordlist={wordlist_file} --rules {output_file}</t>
+  </si>
+  <si>
+    <t>This command should be executed on the machine.</t>
   </si>
   <si>
     <t>CypherQuery</t>
+  </si>
+  <si>
+    <t>309, 292</t>
+  </si>
+  <si>
+    <t>300</t>
+  </si>
+  <si>
+    <t>49</t>
   </si>
 </sst>
 </file>
@@ -2996,7 +3023,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -3063,11 +3090,17 @@
     <xf numFmtId="49" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -3075,14 +3108,14 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="23">
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-    </dxf>
+  <dxfs count="28">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -3094,10 +3127,30 @@
       </fill>
     </dxf>
     <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
@@ -8141,7 +8194,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{48CB07D6-9F6C-094F-A3D3-916741F281CD}" name="Tabella pivot1" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valori" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{48CB07D6-9F6C-094F-A3D3-916741F281CD}" name="Tabella pivot1" cacheId="7" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valori" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A1:B25" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="14">
     <pivotField showAll="0"/>
@@ -8282,11 +8335,11 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{DEFAB213-4389-184E-911C-CDCC8CABBD38}" name="Tabella1" displayName="Tabella1" ref="A1:R299" totalsRowShown="0" dataDxfId="22">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{DEFAB213-4389-184E-911C-CDCC8CABBD38}" name="Tabella1" displayName="Tabella1" ref="A1:R299" totalsRowShown="0" dataDxfId="27">
   <autoFilter ref="A1:R299" xr:uid="{DEFAB213-4389-184E-911C-CDCC8CABBD38}">
     <filterColumn colId="1">
       <filters>
-        <filter val="HW.IOTDevice"/>
+        <filter val="Network"/>
       </filters>
     </filterColumn>
   </autoFilter>
@@ -8294,32 +8347,32 @@
     <sortCondition ref="B1:B299"/>
   </sortState>
   <tableColumns count="18">
-    <tableColumn id="16" xr3:uid="{DE426BDB-E154-EE46-B7B3-5B538C8AEC32}" name="TID" dataDxfId="21">
+    <tableColumn id="16" xr3:uid="{DE426BDB-E154-EE46-B7B3-5B538C8AEC32}" name="TID" dataDxfId="26">
       <calculatedColumnFormula>CONCATENATE("T",ROW(A2)-1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="1" xr3:uid="{A0AE63DC-99F7-7D4F-B824-AB7765893284}" name="Asset" dataDxfId="20"/>
-    <tableColumn id="2" xr3:uid="{0FA38BFF-C67B-0C43-B1BA-F6338DBFB0C8}" name="Threat" dataDxfId="19"/>
-    <tableColumn id="3" xr3:uid="{BFC77F7C-F096-8345-97EA-317816ED869D}" name="Description" dataDxfId="18"/>
-    <tableColumn id="4" xr3:uid="{258F3B86-1461-D64A-AE3B-CEAC97B2B533}" name="STRIDE" dataDxfId="17"/>
-    <tableColumn id="6" xr3:uid="{0FD06C95-5962-AC4D-B9EF-4DBB5728E736}" name="Compromised" dataDxfId="16"/>
-    <tableColumn id="7" xr3:uid="{9E5B99AD-1F1D-B44C-ABDF-6F7E9177F3DE}" name="PreC" dataDxfId="15"/>
-    <tableColumn id="8" xr3:uid="{D4F97A81-E528-2841-B4DE-321362F90F65}" name="PreI" dataDxfId="14"/>
-    <tableColumn id="9" xr3:uid="{018427D6-D385-3447-B4A4-95003B3341F6}" name="PreA" dataDxfId="13"/>
-    <tableColumn id="10" xr3:uid="{8334AC57-4A09-5744-9484-073ECEE2E513}" name="Precondition" dataDxfId="12"/>
-    <tableColumn id="12" xr3:uid="{DDBE315D-E051-2C47-A765-EE1DB2E118EA}" name="PostC" dataDxfId="11">
+    <tableColumn id="1" xr3:uid="{A0AE63DC-99F7-7D4F-B824-AB7765893284}" name="Asset" dataDxfId="25"/>
+    <tableColumn id="2" xr3:uid="{0FA38BFF-C67B-0C43-B1BA-F6338DBFB0C8}" name="Threat" dataDxfId="24"/>
+    <tableColumn id="3" xr3:uid="{BFC77F7C-F096-8345-97EA-317816ED869D}" name="Description" dataDxfId="23"/>
+    <tableColumn id="4" xr3:uid="{258F3B86-1461-D64A-AE3B-CEAC97B2B533}" name="STRIDE" dataDxfId="22"/>
+    <tableColumn id="6" xr3:uid="{0FD06C95-5962-AC4D-B9EF-4DBB5728E736}" name="Compromised" dataDxfId="21"/>
+    <tableColumn id="7" xr3:uid="{9E5B99AD-1F1D-B44C-ABDF-6F7E9177F3DE}" name="PreC" dataDxfId="20"/>
+    <tableColumn id="8" xr3:uid="{D4F97A81-E528-2841-B4DE-321362F90F65}" name="PreI" dataDxfId="19"/>
+    <tableColumn id="9" xr3:uid="{018427D6-D385-3447-B4A4-95003B3341F6}" name="PreA" dataDxfId="18"/>
+    <tableColumn id="10" xr3:uid="{8334AC57-4A09-5744-9484-073ECEE2E513}" name="Precondition" dataDxfId="17"/>
+    <tableColumn id="12" xr3:uid="{DDBE315D-E051-2C47-A765-EE1DB2E118EA}" name="PostC" dataDxfId="16">
       <calculatedColumnFormula>MID(N2,2,1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" xr3:uid="{243C1B9B-76C9-0345-B727-4F11FD75DF6B}" name="PostI" dataDxfId="10">
+    <tableColumn id="13" xr3:uid="{243C1B9B-76C9-0345-B727-4F11FD75DF6B}" name="PostI" dataDxfId="15">
       <calculatedColumnFormula>MID(N2,4,1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="14" xr3:uid="{DD688DAA-2C9A-C247-AEC4-CBDADE9B2B2E}" name="PostA" dataDxfId="9">
+    <tableColumn id="14" xr3:uid="{DD688DAA-2C9A-C247-AEC4-CBDADE9B2B2E}" name="PostA" dataDxfId="14">
       <calculatedColumnFormula>MID(N2,6,1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="15" xr3:uid="{CEE151EC-4E5B-0C41-8586-5A2D7E483661}" name="PostCondition" dataDxfId="8"/>
-    <tableColumn id="5" xr3:uid="{62EC5D77-1F78-1645-8697-BC5450583418}" name="CapecMeta" dataDxfId="7"/>
-    <tableColumn id="11" xr3:uid="{0DCD762C-4EE7-8141-BC05-9DB756A5BEF2}" name="CapecStandard" dataDxfId="6"/>
-    <tableColumn id="17" xr3:uid="{9EF317BA-855B-6E4A-9EC7-E1FB88A1FD56}" name="CapecDetailed" dataDxfId="5"/>
-    <tableColumn id="18" xr3:uid="{9BF6197D-4CF5-4941-A460-18823EEFB2E7}" name="Commento" dataDxfId="4"/>
+    <tableColumn id="15" xr3:uid="{CEE151EC-4E5B-0C41-8586-5A2D7E483661}" name="PostCondition" dataDxfId="13"/>
+    <tableColumn id="5" xr3:uid="{62EC5D77-1F78-1645-8697-BC5450583418}" name="CapecMeta" dataDxfId="12"/>
+    <tableColumn id="11" xr3:uid="{0DCD762C-4EE7-8141-BC05-9DB756A5BEF2}" name="CapecStandard" dataDxfId="11"/>
+    <tableColumn id="17" xr3:uid="{9EF317BA-855B-6E4A-9EC7-E1FB88A1FD56}" name="CapecDetailed" dataDxfId="10"/>
+    <tableColumn id="18" xr3:uid="{9BF6197D-4CF5-4941-A460-18823EEFB2E7}" name="Commento" dataDxfId="9"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -8339,17 +8392,17 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{5ECAFCE9-964F-A04C-B050-422AACCFD3F5}" name="Tabella4" displayName="Tabella4" ref="A1:F5" totalsRowShown="0">
-  <autoFilter ref="A1:F5" xr:uid="{5ECAFCE9-964F-A04C-B050-422AACCFD3F5}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{5ECAFCE9-964F-A04C-B050-422AACCFD3F5}" name="Tabella4" displayName="Tabella4" ref="A1:F6" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7">
+  <autoFilter ref="A1:F6" xr:uid="{5ECAFCE9-964F-A04C-B050-422AACCFD3F5}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{6405AD35-9222-B34C-A112-EC4FDEAC5BE2}" name="ToolID" dataDxfId="3">
+    <tableColumn id="1" xr3:uid="{6405AD35-9222-B34C-A112-EC4FDEAC5BE2}" name="ToolID" dataDxfId="6">
       <calculatedColumnFormula>ROW(Tabella4[[#This Row],[Name]])-1</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{94F8DBBB-A826-8B4A-8C87-395122CA233A}" name="Name"/>
-    <tableColumn id="2" xr3:uid="{FB636F07-AAD2-AE48-87BB-965F92F829C2}" name="CapecID" dataDxfId="2"/>
-    <tableColumn id="7" xr3:uid="{80DB7B80-C531-B649-B58E-F29831E2ACA8}" name="CypherQuery" dataDxfId="0"/>
-    <tableColumn id="3" xr3:uid="{52487567-ED26-B840-ABFD-DB1BF72A83C9}" name="Command"/>
-    <tableColumn id="5" xr3:uid="{0296B95F-6562-0746-B0C6-FE3564F6272C}" name="Description"/>
+    <tableColumn id="4" xr3:uid="{94F8DBBB-A826-8B4A-8C87-395122CA233A}" name="Name" dataDxfId="5"/>
+    <tableColumn id="2" xr3:uid="{FB636F07-AAD2-AE48-87BB-965F92F829C2}" name="CapecID" dataDxfId="4"/>
+    <tableColumn id="6" xr3:uid="{1E4A4CA6-7FF1-6543-A718-93EC7B5F1624}" name="CypherQuery" dataDxfId="3"/>
+    <tableColumn id="3" xr3:uid="{52487567-ED26-B840-ABFD-DB1BF72A83C9}" name="Command" dataDxfId="2"/>
+    <tableColumn id="5" xr3:uid="{0296B95F-6562-0746-B0C6-FE3564F6272C}" name="Description" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -8620,9 +8673,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:R299"/>
   <sheetViews>
-    <sheetView zoomScale="125" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A63" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="O294" sqref="O294"/>
+    <sheetView topLeftCell="I1" zoomScale="125" zoomScaleNormal="115" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A103" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="S107" sqref="S107"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -8699,7 +8752,7 @@
         <v>16</v>
       </c>
       <c r="R1" s="23" t="s">
-        <v>860</v>
+        <v>859</v>
       </c>
     </row>
     <row r="2" spans="1:18" ht="48" hidden="1">
@@ -9717,10 +9770,10 @@
         <v>855</v>
       </c>
       <c r="P25" s="25" t="s">
+        <v>896</v>
+      </c>
+      <c r="Q25" s="25" t="s">
         <v>897</v>
-      </c>
-      <c r="Q25" s="25" t="s">
-        <v>898</v>
       </c>
       <c r="R25" s="24"/>
     </row>
@@ -11474,7 +11527,7 @@
       <c r="Q60" s="24"/>
       <c r="R60" s="24"/>
     </row>
-    <row r="61" spans="1:18" ht="64">
+    <row r="61" spans="1:18" ht="64" hidden="1">
       <c r="A61" s="20" t="str">
         <f t="shared" si="0"/>
         <v>T60</v>
@@ -11535,7 +11588,7 @@
       </c>
       <c r="R61" s="24"/>
     </row>
-    <row r="62" spans="1:18" ht="395">
+    <row r="62" spans="1:18" ht="395" hidden="1">
       <c r="A62" s="20" t="str">
         <f t="shared" si="0"/>
         <v>T61</v>
@@ -11592,11 +11645,11 @@
         <v>478</v>
       </c>
       <c r="Q62" s="24" t="s">
-        <v>908</v>
+        <v>907</v>
       </c>
       <c r="R62" s="24"/>
     </row>
-    <row r="63" spans="1:18" ht="80">
+    <row r="63" spans="1:18" ht="80" hidden="1">
       <c r="A63" s="20" t="str">
         <f t="shared" si="0"/>
         <v>T62</v>
@@ -11657,7 +11710,7 @@
       </c>
       <c r="R63" s="24"/>
     </row>
-    <row r="64" spans="1:18" ht="240">
+    <row r="64" spans="1:18" ht="240" hidden="1">
       <c r="A64" s="20" t="str">
         <f t="shared" si="0"/>
         <v>T63</v>
@@ -11718,7 +11771,7 @@
       </c>
       <c r="R64" s="24"/>
     </row>
-    <row r="65" spans="1:18" ht="48">
+    <row r="65" spans="1:18" ht="48" hidden="1">
       <c r="A65" s="20" t="str">
         <f t="shared" si="0"/>
         <v>T64</v>
@@ -11779,7 +11832,7 @@
       </c>
       <c r="R65" s="24"/>
     </row>
-    <row r="66" spans="1:18" ht="96">
+    <row r="66" spans="1:18" ht="96" hidden="1">
       <c r="A66" s="20" t="str">
         <f t="shared" ref="A66:A129" si="11">CONCATENATE("T",ROW(A66)-1)</f>
         <v>T65</v>
@@ -11830,19 +11883,19 @@
         <v>476</v>
       </c>
       <c r="O66" s="25" t="s">
+        <v>868</v>
+      </c>
+      <c r="P66" s="25" t="s">
         <v>869</v>
       </c>
-      <c r="P66" s="25" t="s">
+      <c r="Q66" s="25" t="s">
         <v>870</v>
       </c>
-      <c r="Q66" s="25" t="s">
+      <c r="R66" s="24" t="s">
         <v>871</v>
       </c>
-      <c r="R66" s="24" t="s">
-        <v>872</v>
-      </c>
-    </row>
-    <row r="67" spans="1:18" ht="256">
+    </row>
+    <row r="67" spans="1:18" ht="256" hidden="1">
       <c r="A67" s="20" t="str">
         <f t="shared" si="11"/>
         <v>T66</v>
@@ -11903,7 +11956,7 @@
       </c>
       <c r="R67" s="24"/>
     </row>
-    <row r="68" spans="1:18" ht="16">
+    <row r="68" spans="1:18" ht="16" hidden="1">
       <c r="A68" s="20" t="str">
         <f t="shared" si="11"/>
         <v>T67</v>
@@ -11960,7 +12013,7 @@
       <c r="Q68" s="24"/>
       <c r="R68" s="24"/>
     </row>
-    <row r="69" spans="1:18" ht="96">
+    <row r="69" spans="1:18" ht="96" hidden="1">
       <c r="A69" s="20" t="str">
         <f t="shared" si="11"/>
         <v>T68</v>
@@ -11969,10 +12022,10 @@
         <v>469</v>
       </c>
       <c r="C69" s="20" t="s">
+        <v>899</v>
+      </c>
+      <c r="D69" s="20" t="s">
         <v>900</v>
-      </c>
-      <c r="D69" s="20" t="s">
-        <v>901</v>
       </c>
       <c r="E69" s="20" t="s">
         <v>274</v>
@@ -12014,13 +12067,13 @@
         <v>855</v>
       </c>
       <c r="P69" s="24" t="s">
+        <v>901</v>
+      </c>
+      <c r="Q69" s="24" t="s">
         <v>902</v>
       </c>
-      <c r="Q69" s="24" t="s">
+      <c r="R69" s="24" t="s">
         <v>903</v>
-      </c>
-      <c r="R69" s="24" t="s">
-        <v>904</v>
       </c>
     </row>
     <row r="70" spans="1:18" ht="144" hidden="1">
@@ -12135,13 +12188,13 @@
         <v>282</v>
       </c>
       <c r="O71" s="24" t="s">
+        <v>887</v>
+      </c>
+      <c r="P71" s="24" t="s">
         <v>888</v>
       </c>
-      <c r="P71" s="24" t="s">
+      <c r="Q71" s="24" t="s">
         <v>889</v>
-      </c>
-      <c r="Q71" s="24" t="s">
-        <v>890</v>
       </c>
       <c r="R71" s="24"/>
     </row>
@@ -12199,7 +12252,7 @@
       <c r="P72" s="24"/>
       <c r="Q72" s="24"/>
       <c r="R72" s="24" t="s">
-        <v>864</v>
+        <v>863</v>
       </c>
     </row>
     <row r="73" spans="1:18" ht="48" hidden="1">
@@ -12617,13 +12670,13 @@
         <v>275</v>
       </c>
       <c r="O79" s="25" t="s">
+        <v>890</v>
+      </c>
+      <c r="P79" s="25" t="s">
         <v>891</v>
       </c>
-      <c r="P79" s="25" t="s">
+      <c r="Q79" s="25" t="s">
         <v>892</v>
-      </c>
-      <c r="Q79" s="25" t="s">
-        <v>893</v>
       </c>
       <c r="R79" s="24"/>
     </row>
@@ -12678,13 +12731,13 @@
         <v>288</v>
       </c>
       <c r="O80" s="25" t="s">
+        <v>894</v>
+      </c>
+      <c r="P80" s="25" t="s">
         <v>895</v>
       </c>
-      <c r="P80" s="25" t="s">
-        <v>896</v>
-      </c>
       <c r="Q80" s="25" t="s">
-        <v>894</v>
+        <v>893</v>
       </c>
       <c r="R80" s="24"/>
     </row>
@@ -13677,7 +13730,7 @@
       <c r="Q99" s="24"/>
       <c r="R99" s="24"/>
     </row>
-    <row r="100" spans="1:18" ht="32" hidden="1">
+    <row r="100" spans="1:18" ht="32">
       <c r="A100" s="20" t="str">
         <f t="shared" si="11"/>
         <v>T99</v>
@@ -13738,7 +13791,7 @@
       </c>
       <c r="R100" s="24"/>
     </row>
-    <row r="101" spans="1:18" ht="48" hidden="1">
+    <row r="101" spans="1:18" ht="48">
       <c r="A101" s="20" t="str">
         <f t="shared" si="11"/>
         <v>T100</v>
@@ -13795,7 +13848,7 @@
       <c r="Q101" s="24"/>
       <c r="R101" s="24"/>
     </row>
-    <row r="102" spans="1:18" ht="48" hidden="1">
+    <row r="102" spans="1:18" ht="48">
       <c r="A102" s="20" t="str">
         <f t="shared" si="11"/>
         <v>T101</v>
@@ -13846,13 +13899,13 @@
         <v>288</v>
       </c>
       <c r="O102" s="24" t="s">
-        <v>863</v>
+        <v>862</v>
       </c>
       <c r="P102" s="24"/>
       <c r="Q102" s="24"/>
       <c r="R102" s="24"/>
     </row>
-    <row r="103" spans="1:18" ht="112" hidden="1">
+    <row r="103" spans="1:18" ht="112">
       <c r="A103" s="20" t="str">
         <f t="shared" si="11"/>
         <v>T102</v>
@@ -13861,7 +13914,7 @@
         <v>575</v>
       </c>
       <c r="C103" s="20" t="s">
-        <v>899</v>
+        <v>898</v>
       </c>
       <c r="D103" s="20" t="s">
         <v>586</v>
@@ -13906,10 +13959,10 @@
       <c r="P103" s="24"/>
       <c r="Q103" s="24"/>
       <c r="R103" s="24" t="s">
-        <v>862</v>
-      </c>
-    </row>
-    <row r="104" spans="1:18" ht="64" hidden="1">
+        <v>861</v>
+      </c>
+    </row>
+    <row r="104" spans="1:18" ht="64">
       <c r="A104" s="20" t="str">
         <f t="shared" si="11"/>
         <v>T103</v>
@@ -13970,7 +14023,7 @@
       </c>
       <c r="R104" s="24"/>
     </row>
-    <row r="105" spans="1:18" ht="32" hidden="1">
+    <row r="105" spans="1:18" ht="32">
       <c r="A105" s="20" t="str">
         <f t="shared" si="11"/>
         <v>T104</v>
@@ -13988,7 +14041,7 @@
         <v>274</v>
       </c>
       <c r="F105" s="20" t="s">
-        <v>907</v>
+        <v>906</v>
       </c>
       <c r="G105" s="20" t="str">
         <f t="shared" si="14"/>
@@ -14024,14 +14077,14 @@
         <v>592</v>
       </c>
       <c r="P105" s="24" t="s">
+        <v>904</v>
+      </c>
+      <c r="Q105" s="24" t="s">
         <v>905</v>
       </c>
-      <c r="Q105" s="24" t="s">
-        <v>906</v>
-      </c>
       <c r="R105" s="24"/>
     </row>
-    <row r="106" spans="1:18" ht="32" hidden="1">
+    <row r="106" spans="1:18" ht="32">
       <c r="A106" s="20" t="str">
         <f t="shared" si="11"/>
         <v>T105</v>
@@ -14088,7 +14141,7 @@
       <c r="Q106" s="24"/>
       <c r="R106" s="24"/>
     </row>
-    <row r="107" spans="1:18" ht="144" hidden="1">
+    <row r="107" spans="1:18" ht="144">
       <c r="A107" s="20" t="str">
         <f t="shared" si="11"/>
         <v>T106</v>
@@ -14142,14 +14195,14 @@
         <v>858</v>
       </c>
       <c r="P107" s="25" t="s">
-        <v>859</v>
+        <v>932</v>
       </c>
       <c r="Q107" s="25"/>
       <c r="R107" s="25" t="s">
-        <v>861</v>
-      </c>
-    </row>
-    <row r="108" spans="1:18" ht="32" hidden="1">
+        <v>860</v>
+      </c>
+    </row>
+    <row r="108" spans="1:18" ht="32">
       <c r="A108" s="20" t="str">
         <f t="shared" si="11"/>
         <v>T107</v>
@@ -14206,7 +14259,7 @@
       <c r="Q108" s="25"/>
       <c r="R108" s="25"/>
     </row>
-    <row r="109" spans="1:18" ht="32" hidden="1">
+    <row r="109" spans="1:18" ht="32">
       <c r="A109" s="20" t="str">
         <f t="shared" si="11"/>
         <v>T108</v>
@@ -14262,7 +14315,7 @@
       <c r="Q109" s="25"/>
       <c r="R109" s="25"/>
     </row>
-    <row r="110" spans="1:18" ht="16" hidden="1">
+    <row r="110" spans="1:18" ht="16">
       <c r="A110" s="20" t="str">
         <f t="shared" si="11"/>
         <v>T109</v>
@@ -14319,7 +14372,7 @@
       <c r="Q110" s="24"/>
       <c r="R110" s="24"/>
     </row>
-    <row r="111" spans="1:18" ht="32" hidden="1">
+    <row r="111" spans="1:18" ht="32">
       <c r="A111" s="20" t="str">
         <f t="shared" si="11"/>
         <v>T110</v>
@@ -22187,7 +22240,7 @@
       <c r="P263" s="24"/>
       <c r="Q263" s="24"/>
       <c r="R263" s="24" t="s">
-        <v>864</v>
+        <v>863</v>
       </c>
     </row>
     <row r="264" spans="1:18" ht="32" hidden="1">
@@ -22488,7 +22541,7 @@
       <c r="P268" s="24"/>
       <c r="Q268" s="24"/>
       <c r="R268" s="24" t="s">
-        <v>864</v>
+        <v>863</v>
       </c>
     </row>
     <row r="269" spans="1:18" ht="32" hidden="1">
@@ -23022,13 +23075,13 @@
         <v>[p,p,p]</v>
       </c>
       <c r="O277" s="25" t="s">
+        <v>873</v>
+      </c>
+      <c r="P277" s="25" t="s">
+        <v>875</v>
+      </c>
+      <c r="Q277" s="25" t="s">
         <v>874</v>
-      </c>
-      <c r="P277" s="25" t="s">
-        <v>876</v>
-      </c>
-      <c r="Q277" s="25" t="s">
-        <v>875</v>
       </c>
       <c r="R277" s="24"/>
     </row>
@@ -23044,7 +23097,7 @@
         <v>527</v>
       </c>
       <c r="D278" s="20" t="s">
-        <v>873</v>
+        <v>872</v>
       </c>
       <c r="E278" s="20" t="s">
         <v>165</v>
@@ -23079,13 +23132,13 @@
         <v>[p,n,n]</v>
       </c>
       <c r="O278" s="25" t="s">
+        <v>876</v>
+      </c>
+      <c r="P278" s="25" t="s">
         <v>877</v>
       </c>
-      <c r="P278" s="25" t="s">
+      <c r="Q278" s="25" t="s">
         <v>878</v>
-      </c>
-      <c r="Q278" s="25" t="s">
-        <v>879</v>
       </c>
       <c r="R278" s="24"/>
     </row>
@@ -23140,13 +23193,13 @@
         <v>529</v>
       </c>
       <c r="O279" s="25" t="s">
+        <v>880</v>
+      </c>
+      <c r="P279" s="25" t="s">
         <v>881</v>
       </c>
-      <c r="P279" s="25" t="s">
-        <v>882</v>
-      </c>
       <c r="Q279" s="25" t="s">
-        <v>880</v>
+        <v>879</v>
       </c>
       <c r="R279" s="24"/>
     </row>
@@ -23204,7 +23257,7 @@
       <c r="P280" s="25"/>
       <c r="Q280" s="25"/>
       <c r="R280" s="24" t="s">
-        <v>864</v>
+        <v>863</v>
       </c>
     </row>
     <row r="281" spans="1:18" ht="48" hidden="1">
@@ -23561,13 +23614,13 @@
         <v>279</v>
       </c>
       <c r="O286" s="25" t="s">
+        <v>882</v>
+      </c>
+      <c r="P286" s="25" t="s">
+        <v>884</v>
+      </c>
+      <c r="Q286" s="25" t="s">
         <v>883</v>
-      </c>
-      <c r="P286" s="25" t="s">
-        <v>885</v>
-      </c>
-      <c r="Q286" s="25" t="s">
-        <v>884</v>
       </c>
       <c r="R286" s="24"/>
     </row>
@@ -23686,10 +23739,10 @@
         <v>612</v>
       </c>
       <c r="P288" s="25" t="s">
+        <v>885</v>
+      </c>
+      <c r="Q288" s="25" t="s">
         <v>886</v>
-      </c>
-      <c r="Q288" s="25" t="s">
-        <v>887</v>
       </c>
       <c r="R288" s="24"/>
     </row>
@@ -23866,16 +23919,16 @@
         <v>275</v>
       </c>
       <c r="O291" s="25" t="s">
+        <v>864</v>
+      </c>
+      <c r="P291" s="25" t="s">
         <v>865</v>
       </c>
-      <c r="P291" s="25" t="s">
+      <c r="Q291" s="25" t="s">
+        <v>867</v>
+      </c>
+      <c r="R291" s="24" t="s">
         <v>866</v>
-      </c>
-      <c r="Q291" s="25" t="s">
-        <v>868</v>
-      </c>
-      <c r="R291" s="24" t="s">
-        <v>867</v>
       </c>
     </row>
     <row r="292" spans="1:18" ht="176" hidden="1">
@@ -24057,7 +24110,7 @@
         <v>429</v>
       </c>
       <c r="Q294" s="24" t="s">
-        <v>909</v>
+        <v>908</v>
       </c>
       <c r="R294" s="24"/>
     </row>
@@ -24367,7 +24420,7 @@
   </sheetData>
   <phoneticPr fontId="11" type="noConversion"/>
   <conditionalFormatting sqref="O1:Q299">
-    <cfRule type="containsBlanks" dxfId="1" priority="1" stopIfTrue="1">
+    <cfRule type="containsBlanks" dxfId="0" priority="1" stopIfTrue="1">
       <formula>LEN(TRIM(O1))=0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -24448,7 +24501,7 @@
       </c>
     </row>
     <row r="2" spans="1:15" ht="90" customHeight="1">
-      <c r="A2" s="26" t="s">
+      <c r="A2" s="29" t="s">
         <v>667</v>
       </c>
       <c r="B2" s="5" t="s">
@@ -24494,7 +24547,7 @@
       </c>
     </row>
     <row r="3" spans="1:15" ht="65" customHeight="1">
-      <c r="A3" s="26"/>
+      <c r="A3" s="29"/>
       <c r="B3" s="5" t="s">
         <v>671</v>
       </c>
@@ -24538,7 +24591,7 @@
       </c>
     </row>
     <row r="4" spans="1:15" ht="64">
-      <c r="A4" s="26"/>
+      <c r="A4" s="29"/>
       <c r="B4" s="5" t="s">
         <v>674</v>
       </c>
@@ -24579,7 +24632,7 @@
       </c>
     </row>
     <row r="5" spans="1:15" ht="80">
-      <c r="A5" s="26"/>
+      <c r="A5" s="29"/>
       <c r="B5" s="5" t="s">
         <v>677</v>
       </c>
@@ -24620,7 +24673,7 @@
       </c>
     </row>
     <row r="6" spans="1:15" ht="48">
-      <c r="A6" s="26"/>
+      <c r="A6" s="29"/>
       <c r="B6" s="5" t="s">
         <v>679</v>
       </c>
@@ -24661,7 +24714,7 @@
       </c>
     </row>
     <row r="7" spans="1:15" ht="48">
-      <c r="A7" s="26"/>
+      <c r="A7" s="29"/>
       <c r="B7" s="5" t="s">
         <v>86</v>
       </c>
@@ -24702,7 +24755,7 @@
       </c>
     </row>
     <row r="8" spans="1:15" ht="32">
-      <c r="A8" s="26" t="s">
+      <c r="A8" s="29" t="s">
         <v>683</v>
       </c>
       <c r="B8" s="5" t="s">
@@ -24745,7 +24798,7 @@
       </c>
     </row>
     <row r="9" spans="1:15" ht="88" customHeight="1">
-      <c r="A9" s="26"/>
+      <c r="A9" s="29"/>
       <c r="B9" s="5" t="s">
         <v>414</v>
       </c>
@@ -24786,7 +24839,7 @@
       </c>
     </row>
     <row r="10" spans="1:15" ht="26" customHeight="1">
-      <c r="A10" s="26"/>
+      <c r="A10" s="29"/>
       <c r="B10" s="5" t="s">
         <v>81</v>
       </c>
@@ -24827,7 +24880,7 @@
       </c>
     </row>
     <row r="11" spans="1:15" ht="211" customHeight="1">
-      <c r="A11" s="26"/>
+      <c r="A11" s="29"/>
       <c r="B11" s="5" t="s">
         <v>688</v>
       </c>
@@ -24868,7 +24921,7 @@
       </c>
     </row>
     <row r="12" spans="1:15" ht="130" customHeight="1">
-      <c r="A12" s="26"/>
+      <c r="A12" s="29"/>
       <c r="B12" s="5" t="s">
         <v>690</v>
       </c>
@@ -24909,7 +24962,7 @@
       </c>
     </row>
     <row r="13" spans="1:15" ht="64">
-      <c r="A13" s="26"/>
+      <c r="A13" s="29"/>
       <c r="B13" s="5" t="s">
         <v>693</v>
       </c>
@@ -24950,7 +25003,7 @@
       </c>
     </row>
     <row r="14" spans="1:15" ht="32">
-      <c r="A14" s="26"/>
+      <c r="A14" s="29"/>
       <c r="B14" s="5" t="s">
         <v>695</v>
       </c>
@@ -24991,7 +25044,7 @@
       </c>
     </row>
     <row r="15" spans="1:15" ht="176">
-      <c r="A15" s="26" t="s">
+      <c r="A15" s="29" t="s">
         <v>698</v>
       </c>
       <c r="B15" s="5" t="s">
@@ -25034,7 +25087,7 @@
       </c>
     </row>
     <row r="16" spans="1:15" ht="32">
-      <c r="A16" s="26"/>
+      <c r="A16" s="29"/>
       <c r="B16" s="5" t="s">
         <v>701</v>
       </c>
@@ -25075,7 +25128,7 @@
       </c>
     </row>
     <row r="17" spans="1:13" ht="48">
-      <c r="A17" s="26"/>
+      <c r="A17" s="29"/>
       <c r="B17" s="5" t="s">
         <v>51</v>
       </c>
@@ -25116,7 +25169,7 @@
       </c>
     </row>
     <row r="18" spans="1:13" ht="64">
-      <c r="A18" s="26"/>
+      <c r="A18" s="29"/>
       <c r="B18" s="5" t="s">
         <v>704</v>
       </c>
@@ -25157,7 +25210,7 @@
       </c>
     </row>
     <row r="19" spans="1:13" ht="64">
-      <c r="A19" s="26"/>
+      <c r="A19" s="29"/>
       <c r="B19" s="5" t="s">
         <v>706</v>
       </c>
@@ -25198,7 +25251,7 @@
       </c>
     </row>
     <row r="20" spans="1:13" ht="48">
-      <c r="A20" s="26"/>
+      <c r="A20" s="29"/>
       <c r="B20" s="5" t="s">
         <v>708</v>
       </c>
@@ -25239,7 +25292,7 @@
       </c>
     </row>
     <row r="21" spans="1:13" ht="48">
-      <c r="A21" s="26"/>
+      <c r="A21" s="29"/>
       <c r="B21" s="5" t="s">
         <v>414</v>
       </c>
@@ -25280,7 +25333,7 @@
       </c>
     </row>
     <row r="22" spans="1:13">
-      <c r="A22" s="26"/>
+      <c r="A22" s="29"/>
       <c r="B22" s="5" t="s">
         <v>712</v>
       </c>
@@ -25321,7 +25374,7 @@
       </c>
     </row>
     <row r="23" spans="1:13" ht="48">
-      <c r="A23" s="26"/>
+      <c r="A23" s="29"/>
       <c r="B23" s="5" t="s">
         <v>714</v>
       </c>
@@ -25362,7 +25415,7 @@
       </c>
     </row>
     <row r="24" spans="1:13" ht="64">
-      <c r="A24" s="26"/>
+      <c r="A24" s="29"/>
       <c r="B24" s="3" t="s">
         <v>716</v>
       </c>
@@ -25403,7 +25456,7 @@
       </c>
     </row>
     <row r="25" spans="1:13" ht="48">
-      <c r="A25" s="26" t="s">
+      <c r="A25" s="29" t="s">
         <v>720</v>
       </c>
       <c r="B25" s="5" t="s">
@@ -25446,7 +25499,7 @@
       </c>
     </row>
     <row r="26" spans="1:13" ht="80">
-      <c r="A26" s="26"/>
+      <c r="A26" s="29"/>
       <c r="B26" s="5" t="s">
         <v>723</v>
       </c>
@@ -25487,7 +25540,7 @@
       </c>
     </row>
     <row r="27" spans="1:13" ht="32">
-      <c r="A27" s="26"/>
+      <c r="A27" s="29"/>
       <c r="B27" s="5" t="s">
         <v>725</v>
       </c>
@@ -25528,7 +25581,7 @@
       </c>
     </row>
     <row r="28" spans="1:13">
-      <c r="A28" s="26"/>
+      <c r="A28" s="29"/>
       <c r="B28" s="5" t="s">
         <v>727</v>
       </c>
@@ -25569,7 +25622,7 @@
       </c>
     </row>
     <row r="29" spans="1:13" ht="96">
-      <c r="A29" s="26"/>
+      <c r="A29" s="29"/>
       <c r="B29" s="5" t="s">
         <v>729</v>
       </c>
@@ -25610,7 +25663,7 @@
       </c>
     </row>
     <row r="30" spans="1:13" ht="48">
-      <c r="A30" s="27" t="s">
+      <c r="A30" s="32" t="s">
         <v>732</v>
       </c>
       <c r="B30" s="5" t="s">
@@ -25653,7 +25706,7 @@
       </c>
     </row>
     <row r="31" spans="1:13" ht="48">
-      <c r="A31" s="27"/>
+      <c r="A31" s="32"/>
       <c r="B31" s="5" t="s">
         <v>735</v>
       </c>
@@ -25694,7 +25747,7 @@
       </c>
     </row>
     <row r="32" spans="1:13" ht="32">
-      <c r="A32" s="27"/>
+      <c r="A32" s="32"/>
       <c r="B32" s="5" t="s">
         <v>737</v>
       </c>
@@ -25735,7 +25788,7 @@
       </c>
     </row>
     <row r="33" spans="1:13" ht="96">
-      <c r="A33" s="27"/>
+      <c r="A33" s="32"/>
       <c r="B33" s="5" t="s">
         <v>51</v>
       </c>
@@ -25776,7 +25829,7 @@
       </c>
     </row>
     <row r="34" spans="1:13" ht="32">
-      <c r="A34" s="27"/>
+      <c r="A34" s="32"/>
       <c r="B34" s="5" t="s">
         <v>740</v>
       </c>
@@ -25817,7 +25870,7 @@
       </c>
     </row>
     <row r="35" spans="1:13" ht="32">
-      <c r="A35" s="27"/>
+      <c r="A35" s="32"/>
       <c r="B35" s="5" t="s">
         <v>414</v>
       </c>
@@ -25858,7 +25911,7 @@
       </c>
     </row>
     <row r="36" spans="1:13" ht="80">
-      <c r="A36" s="27"/>
+      <c r="A36" s="32"/>
       <c r="B36" s="5" t="s">
         <v>743</v>
       </c>
@@ -25899,7 +25952,7 @@
       </c>
     </row>
     <row r="37" spans="1:13" ht="32">
-      <c r="A37" s="26" t="s">
+      <c r="A37" s="29" t="s">
         <v>745</v>
       </c>
       <c r="B37" s="5" t="s">
@@ -25942,7 +25995,7 @@
       </c>
     </row>
     <row r="38" spans="1:13" ht="96">
-      <c r="A38" s="26"/>
+      <c r="A38" s="29"/>
       <c r="B38" s="5" t="s">
         <v>729</v>
       </c>
@@ -25983,7 +26036,7 @@
       </c>
     </row>
     <row r="39" spans="1:13" ht="192">
-      <c r="A39" s="26"/>
+      <c r="A39" s="29"/>
       <c r="B39" s="5" t="s">
         <v>110</v>
       </c>
@@ -26024,7 +26077,7 @@
       </c>
     </row>
     <row r="40" spans="1:13" ht="32">
-      <c r="A40" s="26"/>
+      <c r="A40" s="29"/>
       <c r="B40" s="5" t="s">
         <v>695</v>
       </c>
@@ -26065,7 +26118,7 @@
       </c>
     </row>
     <row r="41" spans="1:13">
-      <c r="A41" s="26" t="s">
+      <c r="A41" s="29" t="s">
         <v>747</v>
       </c>
       <c r="B41" s="5" t="s">
@@ -26108,7 +26161,7 @@
       </c>
     </row>
     <row r="42" spans="1:13" ht="32">
-      <c r="A42" s="26"/>
+      <c r="A42" s="29"/>
       <c r="B42" s="5" t="s">
         <v>749</v>
       </c>
@@ -26149,7 +26202,7 @@
       </c>
     </row>
     <row r="43" spans="1:13">
-      <c r="A43" s="26"/>
+      <c r="A43" s="29"/>
       <c r="B43" s="5" t="s">
         <v>727</v>
       </c>
@@ -26190,7 +26243,7 @@
       </c>
     </row>
     <row r="44" spans="1:13" ht="32">
-      <c r="A44" s="26" t="s">
+      <c r="A44" s="29" t="s">
         <v>750</v>
       </c>
       <c r="B44" s="7" t="s">
@@ -26233,7 +26286,7 @@
       </c>
     </row>
     <row r="45" spans="1:13" ht="32">
-      <c r="A45" s="26"/>
+      <c r="A45" s="29"/>
       <c r="B45" s="7" t="s">
         <v>753</v>
       </c>
@@ -26274,7 +26327,7 @@
       </c>
     </row>
     <row r="46" spans="1:13" ht="16">
-      <c r="A46" s="26"/>
+      <c r="A46" s="29"/>
       <c r="B46" s="7" t="s">
         <v>755</v>
       </c>
@@ -26315,7 +26368,7 @@
       </c>
     </row>
     <row r="47" spans="1:13" ht="64">
-      <c r="A47" s="26"/>
+      <c r="A47" s="29"/>
       <c r="B47" s="7" t="s">
         <v>757</v>
       </c>
@@ -26356,7 +26409,7 @@
       </c>
     </row>
     <row r="48" spans="1:13" ht="48">
-      <c r="A48" s="26"/>
+      <c r="A48" s="29"/>
       <c r="B48" s="5" t="s">
         <v>759</v>
       </c>
@@ -26397,7 +26450,7 @@
       </c>
     </row>
     <row r="49" spans="1:13" ht="78" customHeight="1">
-      <c r="A49" s="27" t="s">
+      <c r="A49" s="32" t="s">
         <v>761</v>
       </c>
       <c r="B49" s="5" t="s">
@@ -26440,7 +26493,7 @@
       </c>
     </row>
     <row r="50" spans="1:13" ht="32">
-      <c r="A50" s="27"/>
+      <c r="A50" s="32"/>
       <c r="B50" s="5" t="s">
         <v>409</v>
       </c>
@@ -26481,7 +26534,7 @@
       </c>
     </row>
     <row r="51" spans="1:13" ht="16">
-      <c r="A51" s="27"/>
+      <c r="A51" s="32"/>
       <c r="B51" s="5" t="s">
         <v>414</v>
       </c>
@@ -26522,7 +26575,7 @@
       </c>
     </row>
     <row r="52" spans="1:13" ht="32">
-      <c r="A52" s="27"/>
+      <c r="A52" s="32"/>
       <c r="B52" s="5" t="s">
         <v>766</v>
       </c>
@@ -26563,7 +26616,7 @@
       </c>
     </row>
     <row r="53" spans="1:13" ht="96">
-      <c r="A53" s="27"/>
+      <c r="A53" s="32"/>
       <c r="B53" s="5" t="s">
         <v>768</v>
       </c>
@@ -26604,7 +26657,7 @@
       </c>
     </row>
     <row r="54" spans="1:13">
-      <c r="A54" s="27"/>
+      <c r="A54" s="32"/>
       <c r="B54" s="5" t="s">
         <v>770</v>
       </c>
@@ -26645,7 +26698,7 @@
       </c>
     </row>
     <row r="55" spans="1:13" ht="64">
-      <c r="A55" s="27"/>
+      <c r="A55" s="32"/>
       <c r="B55" s="5" t="s">
         <v>772</v>
       </c>
@@ -26686,7 +26739,7 @@
       </c>
     </row>
     <row r="56" spans="1:13" ht="64">
-      <c r="A56" s="27"/>
+      <c r="A56" s="32"/>
       <c r="B56" s="5" t="s">
         <v>774</v>
       </c>
@@ -26727,7 +26780,7 @@
       </c>
     </row>
     <row r="57" spans="1:13" ht="32">
-      <c r="A57" s="28" t="s">
+      <c r="A57" s="30" t="s">
         <v>776</v>
       </c>
       <c r="B57" s="6" t="s">
@@ -26769,7 +26822,7 @@
       </c>
     </row>
     <row r="58" spans="1:13" ht="80">
-      <c r="A58" s="28"/>
+      <c r="A58" s="30"/>
       <c r="B58" s="7" t="s">
         <v>779</v>
       </c>
@@ -26809,7 +26862,7 @@
       </c>
     </row>
     <row r="59" spans="1:13" ht="64" customHeight="1">
-      <c r="A59" s="28"/>
+      <c r="A59" s="30"/>
       <c r="B59" s="7" t="s">
         <v>781</v>
       </c>
@@ -26849,7 +26902,7 @@
       </c>
     </row>
     <row r="60" spans="1:13" ht="16">
-      <c r="A60" s="28"/>
+      <c r="A60" s="30"/>
       <c r="B60" s="7" t="s">
         <v>283</v>
       </c>
@@ -26889,7 +26942,7 @@
       </c>
     </row>
     <row r="61" spans="1:13" ht="32">
-      <c r="A61" s="28"/>
+      <c r="A61" s="30"/>
       <c r="B61" s="7" t="s">
         <v>785</v>
       </c>
@@ -26929,7 +26982,7 @@
       </c>
     </row>
     <row r="62" spans="1:13" ht="32">
-      <c r="A62" s="28"/>
+      <c r="A62" s="30"/>
       <c r="B62" s="7" t="s">
         <v>787</v>
       </c>
@@ -26969,7 +27022,7 @@
       </c>
     </row>
     <row r="63" spans="1:13" ht="16">
-      <c r="A63" s="28"/>
+      <c r="A63" s="30"/>
       <c r="B63" s="7" t="s">
         <v>790</v>
       </c>
@@ -27009,7 +27062,7 @@
       </c>
     </row>
     <row r="64" spans="1:13" ht="32">
-      <c r="A64" s="28"/>
+      <c r="A64" s="30"/>
       <c r="B64" s="6" t="s">
         <v>792</v>
       </c>
@@ -27049,7 +27102,7 @@
       </c>
     </row>
     <row r="65" spans="1:13" ht="16">
-      <c r="A65" s="28"/>
+      <c r="A65" s="30"/>
       <c r="B65" s="7" t="s">
         <v>81</v>
       </c>
@@ -27089,7 +27142,7 @@
       </c>
     </row>
     <row r="66" spans="1:13" ht="16">
-      <c r="A66" s="28"/>
+      <c r="A66" s="30"/>
       <c r="B66" s="7" t="s">
         <v>795</v>
       </c>
@@ -27129,7 +27182,7 @@
       </c>
     </row>
     <row r="67" spans="1:13" ht="48">
-      <c r="A67" s="28"/>
+      <c r="A67" s="30"/>
       <c r="B67" s="6" t="s">
         <v>280</v>
       </c>
@@ -27169,64 +27222,64 @@
       </c>
     </row>
     <row r="68" spans="1:13" ht="16">
-      <c r="A68" s="28"/>
-      <c r="B68" s="28" t="s">
+      <c r="A68" s="30"/>
+      <c r="B68" s="30" t="s">
         <v>357</v>
       </c>
       <c r="C68" s="6" t="s">
         <v>797</v>
       </c>
-      <c r="D68" s="28" t="s">
+      <c r="D68" s="30" t="s">
         <v>274</v>
       </c>
-      <c r="E68" s="28" t="s">
+      <c r="E68" s="30" t="s">
         <v>783</v>
       </c>
-      <c r="F68" s="28" t="s">
-        <v>22</v>
-      </c>
-      <c r="G68" s="28" t="s">
-        <v>22</v>
-      </c>
-      <c r="H68" s="26" t="s">
-        <v>22</v>
-      </c>
-      <c r="I68" s="28" t="s">
+      <c r="F68" s="30" t="s">
+        <v>22</v>
+      </c>
+      <c r="G68" s="30" t="s">
+        <v>22</v>
+      </c>
+      <c r="H68" s="29" t="s">
+        <v>22</v>
+      </c>
+      <c r="I68" s="30" t="s">
         <v>364</v>
       </c>
-      <c r="J68" s="28" t="s">
-        <v>22</v>
-      </c>
-      <c r="K68" s="28" t="s">
-        <v>22</v>
-      </c>
-      <c r="L68" s="28" t="s">
-        <v>23</v>
-      </c>
-      <c r="M68" s="26" t="str">
+      <c r="J68" s="30" t="s">
+        <v>22</v>
+      </c>
+      <c r="K68" s="30" t="s">
+        <v>22</v>
+      </c>
+      <c r="L68" s="30" t="s">
+        <v>23</v>
+      </c>
+      <c r="M68" s="29" t="str">
         <f t="shared" si="2"/>
         <v>[n,n,p]</v>
       </c>
     </row>
     <row r="69" spans="1:13" ht="16">
-      <c r="A69" s="28"/>
-      <c r="B69" s="28"/>
+      <c r="A69" s="30"/>
+      <c r="B69" s="30"/>
       <c r="C69" s="6" t="s">
         <v>798</v>
       </c>
-      <c r="D69" s="28"/>
-      <c r="E69" s="28"/>
-      <c r="F69" s="28"/>
-      <c r="G69" s="28"/>
-      <c r="H69" s="26"/>
-      <c r="I69" s="28"/>
-      <c r="J69" s="28"/>
-      <c r="K69" s="28"/>
-      <c r="L69" s="28"/>
-      <c r="M69" s="26"/>
+      <c r="D69" s="30"/>
+      <c r="E69" s="30"/>
+      <c r="F69" s="30"/>
+      <c r="G69" s="30"/>
+      <c r="H69" s="29"/>
+      <c r="I69" s="30"/>
+      <c r="J69" s="30"/>
+      <c r="K69" s="30"/>
+      <c r="L69" s="30"/>
+      <c r="M69" s="29"/>
     </row>
     <row r="70" spans="1:13" ht="28">
-      <c r="A70" s="29" t="s">
+      <c r="A70" s="31" t="s">
         <v>799</v>
       </c>
       <c r="B70" s="16" t="s">
@@ -27272,7 +27325,7 @@
       </c>
     </row>
     <row r="71" spans="1:13" ht="51">
-      <c r="A71" s="29"/>
+      <c r="A71" s="31"/>
       <c r="B71" s="16" t="s">
         <v>51</v>
       </c>
@@ -27316,7 +27369,7 @@
       </c>
     </row>
     <row r="72" spans="1:13" ht="28">
-      <c r="A72" s="29"/>
+      <c r="A72" s="31"/>
       <c r="B72" s="16" t="s">
         <v>684</v>
       </c>
@@ -27360,7 +27413,7 @@
       </c>
     </row>
     <row r="73" spans="1:13" ht="28">
-      <c r="A73" s="29"/>
+      <c r="A73" s="31"/>
       <c r="B73" s="16" t="s">
         <v>806</v>
       </c>
@@ -27404,7 +27457,7 @@
       </c>
     </row>
     <row r="74" spans="1:13" ht="16">
-      <c r="A74" s="26" t="s">
+      <c r="A74" s="29" t="s">
         <v>809</v>
       </c>
       <c r="B74" s="4" t="s">
@@ -27448,7 +27501,7 @@
       </c>
     </row>
     <row r="75" spans="1:13" ht="16">
-      <c r="A75" s="26"/>
+      <c r="A75" s="29"/>
       <c r="B75" s="4" t="s">
         <v>814</v>
       </c>
@@ -27490,7 +27543,7 @@
       </c>
     </row>
     <row r="76" spans="1:13" ht="16">
-      <c r="A76" s="26"/>
+      <c r="A76" s="29"/>
       <c r="B76" s="4" t="s">
         <v>816</v>
       </c>
@@ -27532,7 +27585,7 @@
       </c>
     </row>
     <row r="77" spans="1:13" ht="16">
-      <c r="A77" s="26"/>
+      <c r="A77" s="29"/>
       <c r="B77" s="4" t="s">
         <v>818</v>
       </c>
@@ -27574,7 +27627,7 @@
       </c>
     </row>
     <row r="78" spans="1:13" ht="16">
-      <c r="A78" s="26"/>
+      <c r="A78" s="29"/>
       <c r="B78" s="4" t="s">
         <v>821</v>
       </c>
@@ -27616,7 +27669,7 @@
       </c>
     </row>
     <row r="79" spans="1:13" ht="16">
-      <c r="A79" s="26"/>
+      <c r="A79" s="29"/>
       <c r="B79" s="4" t="s">
         <v>823</v>
       </c>
@@ -27658,7 +27711,7 @@
       </c>
     </row>
     <row r="80" spans="1:13" ht="16">
-      <c r="A80" s="26"/>
+      <c r="A80" s="29"/>
       <c r="B80" s="4" t="s">
         <v>826</v>
       </c>
@@ -27700,7 +27753,7 @@
       </c>
     </row>
     <row r="81" spans="1:13" ht="64">
-      <c r="A81" s="26"/>
+      <c r="A81" s="29"/>
       <c r="B81" s="4" t="s">
         <v>829</v>
       </c>
@@ -27742,7 +27795,7 @@
       </c>
     </row>
     <row r="82" spans="1:13" ht="16">
-      <c r="A82" s="26"/>
+      <c r="A82" s="29"/>
       <c r="B82" s="8" t="s">
         <v>832</v>
       </c>
@@ -27784,7 +27837,7 @@
       </c>
     </row>
     <row r="83" spans="1:13" ht="32">
-      <c r="A83" s="26"/>
+      <c r="A83" s="29"/>
       <c r="B83" s="8" t="s">
         <v>834</v>
       </c>
@@ -27826,7 +27879,7 @@
       </c>
     </row>
     <row r="84" spans="1:13" ht="16">
-      <c r="A84" s="26"/>
+      <c r="A84" s="29"/>
       <c r="B84" s="4" t="s">
         <v>836</v>
       </c>
@@ -27868,7 +27921,7 @@
       </c>
     </row>
     <row r="85" spans="1:13" ht="112">
-      <c r="A85" s="26"/>
+      <c r="A85" s="29"/>
       <c r="B85" s="4" t="s">
         <v>838</v>
       </c>
@@ -27922,6 +27975,15 @@
     </row>
   </sheetData>
   <mergeCells count="23">
+    <mergeCell ref="A2:A7"/>
+    <mergeCell ref="A8:A14"/>
+    <mergeCell ref="A25:A29"/>
+    <mergeCell ref="A15:A24"/>
+    <mergeCell ref="A49:A56"/>
+    <mergeCell ref="A44:A48"/>
+    <mergeCell ref="A41:A43"/>
+    <mergeCell ref="A30:A36"/>
+    <mergeCell ref="A37:A40"/>
     <mergeCell ref="M68:M69"/>
     <mergeCell ref="H68:H69"/>
     <mergeCell ref="A74:A85"/>
@@ -27936,15 +27998,6 @@
     <mergeCell ref="B68:B69"/>
     <mergeCell ref="D68:D69"/>
     <mergeCell ref="E68:E69"/>
-    <mergeCell ref="A2:A7"/>
-    <mergeCell ref="A8:A14"/>
-    <mergeCell ref="A25:A29"/>
-    <mergeCell ref="A15:A24"/>
-    <mergeCell ref="A49:A56"/>
-    <mergeCell ref="A44:A48"/>
-    <mergeCell ref="A41:A43"/>
-    <mergeCell ref="A30:A36"/>
-    <mergeCell ref="A37:A40"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -28796,102 +28849,134 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C51FC597-29FA-1D4E-A4C8-B79027768242}">
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="200" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+    <sheetView tabSelected="1" zoomScale="181" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
-    <col min="3" max="3" width="11.33203125" customWidth="1"/>
-    <col min="4" max="4" width="40.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.83203125" style="26"/>
+    <col min="2" max="2" width="12.5" style="26" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.33203125" style="28" customWidth="1"/>
+    <col min="4" max="4" width="40.33203125" style="27" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="40" style="26" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.6640625" style="27" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="10.83203125" style="26"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
-      <c r="A1" t="s">
+    <row r="1" spans="1:6" ht="16">
+      <c r="A1" s="26" t="s">
+        <v>910</v>
+      </c>
+      <c r="B1" s="26" t="s">
+        <v>916</v>
+      </c>
+      <c r="C1" s="28" t="s">
+        <v>909</v>
+      </c>
+      <c r="D1" s="27" t="s">
+        <v>931</v>
+      </c>
+      <c r="E1" s="26" t="s">
         <v>911</v>
       </c>
-      <c r="B1" t="s">
-        <v>917</v>
-      </c>
-      <c r="C1" t="s">
-        <v>910</v>
-      </c>
-      <c r="D1" t="s">
-        <v>925</v>
-      </c>
-      <c r="E1" t="s">
-        <v>912</v>
-      </c>
-      <c r="F1" t="s">
+      <c r="F1" s="27" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
-      <c r="A2">
+    <row r="2" spans="1:6" ht="48">
+      <c r="A2" s="26">
         <f>ROW(Tabella4[[#This Row],[Name]])-1</f>
         <v>1</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="26" t="s">
+        <v>912</v>
+      </c>
+      <c r="C2" s="28" t="s">
         <v>913</v>
       </c>
-      <c r="C2" s="23" t="s">
-        <v>914</v>
-      </c>
-      <c r="D2" s="23" t="s">
-        <v>924</v>
-      </c>
-      <c r="E2" t="s">
-        <v>918</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6">
-      <c r="A3">
+      <c r="D2" s="27" t="s">
+        <v>921</v>
+      </c>
+      <c r="E2" s="26" t="s">
+        <v>917</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="32">
+      <c r="A3" s="26">
         <f>ROW(Tabella4[[#This Row],[Name]])-1</f>
         <v>2</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="26" t="s">
+        <v>914</v>
+      </c>
+      <c r="C3" s="28" t="s">
         <v>915</v>
       </c>
-      <c r="C3" s="23" t="s">
-        <v>916</v>
-      </c>
-      <c r="D3" s="23"/>
-      <c r="E3" t="s">
-        <v>919</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6">
-      <c r="A4">
+      <c r="D3" s="27" t="s">
+        <v>922</v>
+      </c>
+      <c r="E3" s="26" t="s">
+        <v>918</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="32">
+      <c r="A4" s="26">
         <f>ROW(Tabella4[[#This Row],[Name]])-1</f>
         <v>3</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="26" t="s">
+        <v>919</v>
+      </c>
+      <c r="C4" s="28" t="s">
+        <v>933</v>
+      </c>
+      <c r="D4" s="27" t="s">
+        <v>923</v>
+      </c>
+      <c r="E4" s="26" t="s">
         <v>920</v>
       </c>
-      <c r="C4" s="23" t="s">
-        <v>923</v>
-      </c>
-      <c r="D4" s="23"/>
-      <c r="E4" t="s">
-        <v>921</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6">
-      <c r="A5">
+    </row>
+    <row r="5" spans="1:6" ht="32">
+      <c r="A5" s="26">
         <f>ROW(Tabella4[[#This Row],[Name]])-1</f>
         <v>4</v>
       </c>
-      <c r="B5" t="s">
-        <v>920</v>
-      </c>
-      <c r="C5" s="23" t="s">
-        <v>859</v>
-      </c>
-      <c r="D5" s="23"/>
-      <c r="E5" t="s">
-        <v>922</v>
+      <c r="B5" s="26" t="s">
+        <v>919</v>
+      </c>
+      <c r="C5" s="28" t="s">
+        <v>924</v>
+      </c>
+      <c r="D5" s="27" t="s">
+        <v>925</v>
+      </c>
+      <c r="E5" s="26" t="s">
+        <v>926</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="64">
+      <c r="A6" s="26">
+        <f>ROW(Tabella4[[#This Row],[Name]])-1</f>
+        <v>5</v>
+      </c>
+      <c r="B6" s="26" t="s">
+        <v>927</v>
+      </c>
+      <c r="C6" s="28" t="s">
+        <v>934</v>
+      </c>
+      <c r="D6" s="27" t="s">
+        <v>928</v>
+      </c>
+      <c r="E6" s="26" t="s">
+        <v>929</v>
+      </c>
+      <c r="F6" s="27" t="s">
+        <v>930</v>
       </c>
     </row>
   </sheetData>
@@ -28914,15 +28999,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x0101009A9CE0B21D9C3A45B31425227616CD6F" ma:contentTypeVersion="11" ma:contentTypeDescription="Creare un nuovo documento." ma:contentTypeScope="" ma:versionID="180d662eb9e2621fe5c8d1498a11e3bf">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="633f040f-4953-46e7-8610-82b0c5296ba0" xmlns:ns3="f62ef740-d444-4f18-80a2-7590fdcab1ce" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="64519aed5f694bce5dc2f4bcf073d27d" ns2:_="" ns3:_="">
     <xsd:import namespace="633f040f-4953-46e7-8610-82b0c5296ba0"/>
@@ -29133,32 +29209,33 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{83D5100D-0E56-4B30-B42D-2AEC6B837C39}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="633f040f-4953-46e7-8610-82b0c5296ba0"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="f62ef740-d444-4f18-80a2-7590fdcab1ce"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="f62ef740-d444-4f18-80a2-7590fdcab1ce"/>
-    <ds:schemaRef ds:uri="633f040f-4953-46e7-8610-82b0c5296ba0"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2C6CC7BA-2E2C-4B0D-8103-11A51D82E8EC}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CA355F46-8632-4C01-B7E7-8E7DCFF50FB7}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -29175,4 +29252,12 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2C6CC7BA-2E2C-4B0D-8103-11A51D82E8EC}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Introdotta funzione per ottenere il diagramma er del database
</commit_message>
<xml_diff>
--- a/apps/static/assets/dbs/ThreatCatalogComplete.xlsx
+++ b/apps/static/assets/dbs/ThreatCatalogComplete.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fefox/Desktop/Web/apps/static/assets/dbs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E037A329-F633-9443-A2B4-E1F83E1B22DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{0FFBDA05-331F-5048-8D0E-97ABEB39D016}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16380" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -24,7 +24,7 @@
   </definedNames>
   <calcPr calcId="191028"/>
   <pivotCaches>
-    <pivotCache cacheId="8" r:id="rId6"/>
+    <pivotCache cacheId="0" r:id="rId6"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -2857,9 +2857,6 @@
     <t>match (n {type:'Service.Web'}) return n.component_id as component_id</t>
   </si>
   <si>
-    <t>match (target)-[:connects]-&gt;(net {type:'Network'}) return target.component_id as component_id</t>
-  </si>
-  <si>
     <t>292, 309</t>
   </si>
   <si>
@@ -2903,6 +2900,9 @@
   </si>
   <si>
     <t>nmap -v -sV {ip}</t>
+  </si>
+  <si>
+    <t>match (net {type:'Network'})-[:connects]-&gt;(target) return target.component_id as component_id</t>
   </si>
 </sst>
 </file>
@@ -3035,7 +3035,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -3122,9 +3122,6 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -8209,7 +8206,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{48CB07D6-9F6C-094F-A3D3-916741F281CD}" name="Tabella pivot1" cacheId="8" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valori" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{48CB07D6-9F6C-094F-A3D3-916741F281CD}" name="Tabella pivot1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valori" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A1:B25" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="14">
     <pivotField showAll="0"/>
@@ -8351,13 +8348,7 @@
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{DEFAB213-4389-184E-911C-CDCC8CABBD38}" name="Tabella1" displayName="Tabella1" ref="A1:R299" totalsRowShown="0" dataDxfId="27">
-  <autoFilter ref="A1:R299" xr:uid="{DEFAB213-4389-184E-911C-CDCC8CABBD38}">
-    <filterColumn colId="1">
-      <filters>
-        <filter val="Network"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:R299" xr:uid="{DEFAB213-4389-184E-911C-CDCC8CABBD38}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:R299">
     <sortCondition ref="B1:B299"/>
   </sortState>
@@ -8688,8 +8679,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:R299"/>
   <sheetViews>
-    <sheetView topLeftCell="I1" zoomScale="125" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A103" activePane="bottomLeft" state="frozen"/>
+    <sheetView topLeftCell="D1" zoomScaleNormal="115" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A293" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="S107" sqref="S107"/>
     </sheetView>
   </sheetViews>
@@ -8770,7 +8761,7 @@
         <v>859</v>
       </c>
     </row>
-    <row r="2" spans="1:18" ht="48" hidden="1">
+    <row r="2" spans="1:18" ht="48">
       <c r="A2" s="20" t="str">
         <f t="shared" ref="A2:A65" si="0">CONCATENATE("T",ROW(A2)-1)</f>
         <v>T1</v>
@@ -8812,7 +8803,7 @@
       <c r="Q2" s="24"/>
       <c r="R2" s="24"/>
     </row>
-    <row r="3" spans="1:18" ht="32" hidden="1">
+    <row r="3" spans="1:18" ht="32">
       <c r="A3" s="20" t="str">
         <f t="shared" si="0"/>
         <v>T2</v>
@@ -8854,7 +8845,7 @@
       <c r="Q3" s="24"/>
       <c r="R3" s="24"/>
     </row>
-    <row r="4" spans="1:18" ht="80" hidden="1">
+    <row r="4" spans="1:18" ht="80">
       <c r="A4" s="20" t="str">
         <f t="shared" si="0"/>
         <v>T3</v>
@@ -8896,7 +8887,7 @@
       <c r="Q4" s="24"/>
       <c r="R4" s="24"/>
     </row>
-    <row r="5" spans="1:18" ht="32" hidden="1">
+    <row r="5" spans="1:18" ht="32">
       <c r="A5" s="20" t="str">
         <f t="shared" si="0"/>
         <v>T4</v>
@@ -8938,7 +8929,7 @@
       <c r="Q5" s="24"/>
       <c r="R5" s="24"/>
     </row>
-    <row r="6" spans="1:18" ht="48" hidden="1">
+    <row r="6" spans="1:18" ht="48">
       <c r="A6" s="20" t="str">
         <f t="shared" si="0"/>
         <v>T5</v>
@@ -8980,7 +8971,7 @@
       <c r="Q6" s="24"/>
       <c r="R6" s="24"/>
     </row>
-    <row r="7" spans="1:18" ht="48" hidden="1">
+    <row r="7" spans="1:18" ht="48">
       <c r="A7" s="20" t="str">
         <f t="shared" si="0"/>
         <v>T6</v>
@@ -9022,7 +9013,7 @@
       <c r="Q7" s="24"/>
       <c r="R7" s="24"/>
     </row>
-    <row r="8" spans="1:18" ht="48" hidden="1">
+    <row r="8" spans="1:18" ht="48">
       <c r="A8" s="20" t="str">
         <f t="shared" si="0"/>
         <v>T7</v>
@@ -9064,7 +9055,7 @@
       <c r="Q8" s="24"/>
       <c r="R8" s="24"/>
     </row>
-    <row r="9" spans="1:18" ht="16" hidden="1">
+    <row r="9" spans="1:18" ht="16">
       <c r="A9" s="20" t="str">
         <f t="shared" si="0"/>
         <v>T8</v>
@@ -9106,7 +9097,7 @@
       <c r="Q9" s="24"/>
       <c r="R9" s="24"/>
     </row>
-    <row r="10" spans="1:18" ht="32" hidden="1">
+    <row r="10" spans="1:18" ht="32">
       <c r="A10" s="20" t="str">
         <f t="shared" si="0"/>
         <v>T9</v>
@@ -9148,7 +9139,7 @@
       <c r="Q10" s="24"/>
       <c r="R10" s="24"/>
     </row>
-    <row r="11" spans="1:18" ht="32" hidden="1">
+    <row r="11" spans="1:18" ht="32">
       <c r="A11" s="20" t="str">
         <f t="shared" si="0"/>
         <v>T10</v>
@@ -9190,7 +9181,7 @@
       <c r="Q11" s="24"/>
       <c r="R11" s="24"/>
     </row>
-    <row r="12" spans="1:18" ht="48" hidden="1">
+    <row r="12" spans="1:18" ht="48">
       <c r="A12" s="20" t="str">
         <f t="shared" si="0"/>
         <v>T11</v>
@@ -9232,7 +9223,7 @@
       <c r="Q12" s="24"/>
       <c r="R12" s="24"/>
     </row>
-    <row r="13" spans="1:18" ht="48" hidden="1">
+    <row r="13" spans="1:18" ht="48">
       <c r="A13" s="20" t="str">
         <f t="shared" si="0"/>
         <v>T12</v>
@@ -9274,7 +9265,7 @@
       <c r="Q13" s="24"/>
       <c r="R13" s="24"/>
     </row>
-    <row r="14" spans="1:18" ht="64" hidden="1">
+    <row r="14" spans="1:18" ht="64">
       <c r="A14" s="20" t="str">
         <f t="shared" si="0"/>
         <v>T13</v>
@@ -9316,7 +9307,7 @@
       <c r="Q14" s="24"/>
       <c r="R14" s="24"/>
     </row>
-    <row r="15" spans="1:18" ht="48" hidden="1">
+    <row r="15" spans="1:18" ht="48">
       <c r="A15" s="20" t="str">
         <f t="shared" si="0"/>
         <v>T14</v>
@@ -9358,7 +9349,7 @@
       <c r="Q15" s="24"/>
       <c r="R15" s="24"/>
     </row>
-    <row r="16" spans="1:18" ht="80" hidden="1">
+    <row r="16" spans="1:18" ht="80">
       <c r="A16" s="20" t="str">
         <f t="shared" si="0"/>
         <v>T15</v>
@@ -9400,7 +9391,7 @@
       <c r="Q16" s="24"/>
       <c r="R16" s="24"/>
     </row>
-    <row r="17" spans="1:18" ht="32" hidden="1">
+    <row r="17" spans="1:18" ht="32">
       <c r="A17" s="20" t="str">
         <f t="shared" si="0"/>
         <v>T16</v>
@@ -9442,7 +9433,7 @@
       <c r="Q17" s="24"/>
       <c r="R17" s="24"/>
     </row>
-    <row r="18" spans="1:18" ht="32" hidden="1">
+    <row r="18" spans="1:18" ht="32">
       <c r="A18" s="20" t="str">
         <f t="shared" si="0"/>
         <v>T17</v>
@@ -9484,7 +9475,7 @@
       <c r="Q18" s="24"/>
       <c r="R18" s="24"/>
     </row>
-    <row r="19" spans="1:18" ht="48" hidden="1">
+    <row r="19" spans="1:18" ht="48">
       <c r="A19" s="20" t="str">
         <f t="shared" si="0"/>
         <v>T18</v>
@@ -9526,7 +9517,7 @@
       <c r="Q19" s="24"/>
       <c r="R19" s="24"/>
     </row>
-    <row r="20" spans="1:18" ht="32" hidden="1">
+    <row r="20" spans="1:18" ht="32">
       <c r="A20" s="20" t="str">
         <f t="shared" si="0"/>
         <v>T19</v>
@@ -9568,7 +9559,7 @@
       <c r="Q20" s="24"/>
       <c r="R20" s="24"/>
     </row>
-    <row r="21" spans="1:18" ht="48" hidden="1">
+    <row r="21" spans="1:18" ht="48">
       <c r="A21" s="20" t="str">
         <f t="shared" si="0"/>
         <v>T20</v>
@@ -9610,7 +9601,7 @@
       <c r="Q21" s="24"/>
       <c r="R21" s="24"/>
     </row>
-    <row r="22" spans="1:18" ht="48" hidden="1">
+    <row r="22" spans="1:18" ht="48">
       <c r="A22" s="20" t="str">
         <f t="shared" si="0"/>
         <v>T21</v>
@@ -9652,7 +9643,7 @@
       <c r="Q22" s="24"/>
       <c r="R22" s="24"/>
     </row>
-    <row r="23" spans="1:18" ht="48" hidden="1">
+    <row r="23" spans="1:18" ht="48">
       <c r="A23" s="20" t="str">
         <f t="shared" si="0"/>
         <v>T22</v>
@@ -9694,7 +9685,7 @@
       <c r="Q23" s="24"/>
       <c r="R23" s="24"/>
     </row>
-    <row r="24" spans="1:18" ht="48" hidden="1">
+    <row r="24" spans="1:18" ht="48">
       <c r="A24" s="20" t="str">
         <f t="shared" si="0"/>
         <v>T23</v>
@@ -9736,7 +9727,7 @@
       <c r="Q24" s="24"/>
       <c r="R24" s="24"/>
     </row>
-    <row r="25" spans="1:18" ht="48" hidden="1">
+    <row r="25" spans="1:18" ht="48">
       <c r="A25" s="20" t="str">
         <f t="shared" si="0"/>
         <v>T24</v>
@@ -9792,7 +9783,7 @@
       </c>
       <c r="R25" s="24"/>
     </row>
-    <row r="26" spans="1:18" ht="48" hidden="1">
+    <row r="26" spans="1:18" ht="48">
       <c r="A26" s="20" t="str">
         <f t="shared" si="0"/>
         <v>T25</v>
@@ -9842,7 +9833,7 @@
       <c r="Q26" s="24"/>
       <c r="R26" s="24"/>
     </row>
-    <row r="27" spans="1:18" ht="48" hidden="1">
+    <row r="27" spans="1:18" ht="48">
       <c r="A27" s="20" t="str">
         <f t="shared" si="0"/>
         <v>T26</v>
@@ -9892,7 +9883,7 @@
       <c r="Q27" s="24"/>
       <c r="R27" s="24"/>
     </row>
-    <row r="28" spans="1:18" ht="64" hidden="1">
+    <row r="28" spans="1:18" ht="64">
       <c r="A28" s="20" t="str">
         <f t="shared" si="0"/>
         <v>T27</v>
@@ -9942,7 +9933,7 @@
       <c r="Q28" s="24"/>
       <c r="R28" s="24"/>
     </row>
-    <row r="29" spans="1:18" ht="32" hidden="1">
+    <row r="29" spans="1:18" ht="32">
       <c r="A29" s="20" t="str">
         <f t="shared" si="0"/>
         <v>T28</v>
@@ -9992,7 +9983,7 @@
       <c r="Q29" s="24"/>
       <c r="R29" s="24"/>
     </row>
-    <row r="30" spans="1:18" ht="48" hidden="1">
+    <row r="30" spans="1:18" ht="48">
       <c r="A30" s="20" t="str">
         <f t="shared" si="0"/>
         <v>T29</v>
@@ -10042,7 +10033,7 @@
       <c r="Q30" s="24"/>
       <c r="R30" s="24"/>
     </row>
-    <row r="31" spans="1:18" ht="48" hidden="1">
+    <row r="31" spans="1:18" ht="48">
       <c r="A31" s="20" t="str">
         <f t="shared" si="0"/>
         <v>T30</v>
@@ -10092,7 +10083,7 @@
       <c r="Q31" s="24"/>
       <c r="R31" s="24"/>
     </row>
-    <row r="32" spans="1:18" ht="32" hidden="1">
+    <row r="32" spans="1:18" ht="32">
       <c r="A32" s="20" t="str">
         <f t="shared" si="0"/>
         <v>T31</v>
@@ -10142,7 +10133,7 @@
       <c r="Q32" s="24"/>
       <c r="R32" s="24"/>
     </row>
-    <row r="33" spans="1:18" ht="48" hidden="1">
+    <row r="33" spans="1:18" ht="48">
       <c r="A33" s="20" t="str">
         <f t="shared" si="0"/>
         <v>T32</v>
@@ -10192,7 +10183,7 @@
       <c r="Q33" s="24"/>
       <c r="R33" s="24"/>
     </row>
-    <row r="34" spans="1:18" ht="32" hidden="1">
+    <row r="34" spans="1:18" ht="32">
       <c r="A34" s="20" t="str">
         <f t="shared" si="0"/>
         <v>T33</v>
@@ -10242,7 +10233,7 @@
       <c r="Q34" s="24"/>
       <c r="R34" s="24"/>
     </row>
-    <row r="35" spans="1:18" ht="32" hidden="1">
+    <row r="35" spans="1:18" ht="32">
       <c r="A35" s="20" t="str">
         <f t="shared" si="0"/>
         <v>T34</v>
@@ -10292,7 +10283,7 @@
       <c r="Q35" s="24"/>
       <c r="R35" s="24"/>
     </row>
-    <row r="36" spans="1:18" ht="48" hidden="1">
+    <row r="36" spans="1:18" ht="48">
       <c r="A36" s="20" t="str">
         <f t="shared" si="0"/>
         <v>T35</v>
@@ -10342,7 +10333,7 @@
       <c r="Q36" s="24"/>
       <c r="R36" s="24"/>
     </row>
-    <row r="37" spans="1:18" ht="32" hidden="1">
+    <row r="37" spans="1:18" ht="32">
       <c r="A37" s="20" t="str">
         <f t="shared" si="0"/>
         <v>T36</v>
@@ -10392,7 +10383,7 @@
       <c r="Q37" s="24"/>
       <c r="R37" s="24"/>
     </row>
-    <row r="38" spans="1:18" ht="16" hidden="1">
+    <row r="38" spans="1:18" ht="16">
       <c r="A38" s="20" t="str">
         <f t="shared" si="0"/>
         <v>T37</v>
@@ -10442,7 +10433,7 @@
       <c r="Q38" s="24"/>
       <c r="R38" s="24"/>
     </row>
-    <row r="39" spans="1:18" ht="16" hidden="1">
+    <row r="39" spans="1:18" ht="16">
       <c r="A39" s="20" t="str">
         <f t="shared" si="0"/>
         <v>T38</v>
@@ -10492,7 +10483,7 @@
       <c r="Q39" s="24"/>
       <c r="R39" s="24"/>
     </row>
-    <row r="40" spans="1:18" ht="32" hidden="1">
+    <row r="40" spans="1:18" ht="32">
       <c r="A40" s="20" t="str">
         <f t="shared" si="0"/>
         <v>T39</v>
@@ -10542,7 +10533,7 @@
       <c r="Q40" s="24"/>
       <c r="R40" s="24"/>
     </row>
-    <row r="41" spans="1:18" ht="32" hidden="1">
+    <row r="41" spans="1:18" ht="32">
       <c r="A41" s="20" t="str">
         <f t="shared" si="0"/>
         <v>T40</v>
@@ -10592,7 +10583,7 @@
       <c r="Q41" s="24"/>
       <c r="R41" s="24"/>
     </row>
-    <row r="42" spans="1:18" ht="48" hidden="1">
+    <row r="42" spans="1:18" ht="48">
       <c r="A42" s="20" t="str">
         <f t="shared" si="0"/>
         <v>T41</v>
@@ -10642,7 +10633,7 @@
       <c r="Q42" s="24"/>
       <c r="R42" s="24"/>
     </row>
-    <row r="43" spans="1:18" ht="48" hidden="1">
+    <row r="43" spans="1:18" ht="48">
       <c r="A43" s="20" t="str">
         <f t="shared" si="0"/>
         <v>T42</v>
@@ -10692,7 +10683,7 @@
       <c r="Q43" s="24"/>
       <c r="R43" s="24"/>
     </row>
-    <row r="44" spans="1:18" ht="16" hidden="1">
+    <row r="44" spans="1:18" ht="16">
       <c r="A44" s="20" t="str">
         <f t="shared" si="0"/>
         <v>T43</v>
@@ -10742,7 +10733,7 @@
       <c r="Q44" s="24"/>
       <c r="R44" s="24"/>
     </row>
-    <row r="45" spans="1:18" ht="48" hidden="1">
+    <row r="45" spans="1:18" ht="48">
       <c r="A45" s="20" t="str">
         <f t="shared" si="0"/>
         <v>T44</v>
@@ -10792,7 +10783,7 @@
       <c r="Q45" s="24"/>
       <c r="R45" s="24"/>
     </row>
-    <row r="46" spans="1:18" ht="48" hidden="1">
+    <row r="46" spans="1:18" ht="48">
       <c r="A46" s="20" t="str">
         <f t="shared" si="0"/>
         <v>T45</v>
@@ -10842,7 +10833,7 @@
       <c r="Q46" s="24"/>
       <c r="R46" s="24"/>
     </row>
-    <row r="47" spans="1:18" ht="32" hidden="1">
+    <row r="47" spans="1:18" ht="32">
       <c r="A47" s="20" t="str">
         <f t="shared" si="0"/>
         <v>T46</v>
@@ -10892,7 +10883,7 @@
       <c r="Q47" s="24"/>
       <c r="R47" s="24"/>
     </row>
-    <row r="48" spans="1:18" ht="32" hidden="1">
+    <row r="48" spans="1:18" ht="32">
       <c r="A48" s="20" t="str">
         <f t="shared" si="0"/>
         <v>T47</v>
@@ -10942,7 +10933,7 @@
       <c r="Q48" s="24"/>
       <c r="R48" s="24"/>
     </row>
-    <row r="49" spans="1:18" ht="48" hidden="1">
+    <row r="49" spans="1:18" ht="48">
       <c r="A49" s="20" t="str">
         <f t="shared" si="0"/>
         <v>T48</v>
@@ -10992,7 +10983,7 @@
       <c r="Q49" s="24"/>
       <c r="R49" s="24"/>
     </row>
-    <row r="50" spans="1:18" ht="32" hidden="1">
+    <row r="50" spans="1:18" ht="32">
       <c r="A50" s="20" t="str">
         <f t="shared" si="0"/>
         <v>T49</v>
@@ -11042,7 +11033,7 @@
       <c r="Q50" s="24"/>
       <c r="R50" s="24"/>
     </row>
-    <row r="51" spans="1:18" ht="32" hidden="1">
+    <row r="51" spans="1:18" ht="32">
       <c r="A51" s="20" t="str">
         <f t="shared" si="0"/>
         <v>T50</v>
@@ -11092,7 +11083,7 @@
       <c r="Q51" s="24"/>
       <c r="R51" s="24"/>
     </row>
-    <row r="52" spans="1:18" ht="32" hidden="1">
+    <row r="52" spans="1:18" ht="32">
       <c r="A52" s="20" t="str">
         <f t="shared" si="0"/>
         <v>T51</v>
@@ -11142,7 +11133,7 @@
       <c r="Q52" s="24"/>
       <c r="R52" s="24"/>
     </row>
-    <row r="53" spans="1:18" ht="32" hidden="1">
+    <row r="53" spans="1:18" ht="32">
       <c r="A53" s="20" t="str">
         <f t="shared" si="0"/>
         <v>T52</v>
@@ -11192,7 +11183,7 @@
       <c r="Q53" s="24"/>
       <c r="R53" s="24"/>
     </row>
-    <row r="54" spans="1:18" ht="48" hidden="1">
+    <row r="54" spans="1:18" ht="48">
       <c r="A54" s="20" t="str">
         <f t="shared" si="0"/>
         <v>T53</v>
@@ -11242,7 +11233,7 @@
       <c r="Q54" s="24"/>
       <c r="R54" s="24"/>
     </row>
-    <row r="55" spans="1:18" ht="32" hidden="1">
+    <row r="55" spans="1:18" ht="32">
       <c r="A55" s="20" t="str">
         <f t="shared" si="0"/>
         <v>T54</v>
@@ -11292,7 +11283,7 @@
       <c r="Q55" s="24"/>
       <c r="R55" s="24"/>
     </row>
-    <row r="56" spans="1:18" ht="48" hidden="1">
+    <row r="56" spans="1:18" ht="48">
       <c r="A56" s="20" t="str">
         <f t="shared" si="0"/>
         <v>T55</v>
@@ -11342,7 +11333,7 @@
       <c r="Q56" s="24"/>
       <c r="R56" s="24"/>
     </row>
-    <row r="57" spans="1:18" ht="32" hidden="1">
+    <row r="57" spans="1:18" ht="32">
       <c r="A57" s="20" t="str">
         <f t="shared" si="0"/>
         <v>T56</v>
@@ -11392,7 +11383,7 @@
       <c r="Q57" s="24"/>
       <c r="R57" s="24"/>
     </row>
-    <row r="58" spans="1:18" ht="80" hidden="1">
+    <row r="58" spans="1:18" ht="80">
       <c r="A58" s="20" t="str">
         <f t="shared" si="0"/>
         <v>T57</v>
@@ -11442,7 +11433,7 @@
       <c r="Q58" s="24"/>
       <c r="R58" s="24"/>
     </row>
-    <row r="59" spans="1:18" ht="32" hidden="1">
+    <row r="59" spans="1:18" ht="32">
       <c r="A59" s="20" t="str">
         <f t="shared" si="0"/>
         <v>T58</v>
@@ -11492,7 +11483,7 @@
       <c r="Q59" s="24"/>
       <c r="R59" s="24"/>
     </row>
-    <row r="60" spans="1:18" ht="32" hidden="1">
+    <row r="60" spans="1:18" ht="32">
       <c r="A60" s="20" t="str">
         <f t="shared" si="0"/>
         <v>T59</v>
@@ -11542,7 +11533,7 @@
       <c r="Q60" s="24"/>
       <c r="R60" s="24"/>
     </row>
-    <row r="61" spans="1:18" ht="64" hidden="1">
+    <row r="61" spans="1:18" ht="64">
       <c r="A61" s="20" t="str">
         <f t="shared" si="0"/>
         <v>T60</v>
@@ -11603,7 +11594,7 @@
       </c>
       <c r="R61" s="24"/>
     </row>
-    <row r="62" spans="1:18" ht="395" hidden="1">
+    <row r="62" spans="1:18" ht="395">
       <c r="A62" s="20" t="str">
         <f t="shared" si="0"/>
         <v>T61</v>
@@ -11664,7 +11655,7 @@
       </c>
       <c r="R62" s="24"/>
     </row>
-    <row r="63" spans="1:18" ht="80" hidden="1">
+    <row r="63" spans="1:18" ht="80">
       <c r="A63" s="20" t="str">
         <f t="shared" si="0"/>
         <v>T62</v>
@@ -11725,7 +11716,7 @@
       </c>
       <c r="R63" s="24"/>
     </row>
-    <row r="64" spans="1:18" ht="240" hidden="1">
+    <row r="64" spans="1:18" ht="240">
       <c r="A64" s="20" t="str">
         <f t="shared" si="0"/>
         <v>T63</v>
@@ -11786,7 +11777,7 @@
       </c>
       <c r="R64" s="24"/>
     </row>
-    <row r="65" spans="1:18" ht="48" hidden="1">
+    <row r="65" spans="1:18" ht="48">
       <c r="A65" s="20" t="str">
         <f t="shared" si="0"/>
         <v>T64</v>
@@ -11847,7 +11838,7 @@
       </c>
       <c r="R65" s="24"/>
     </row>
-    <row r="66" spans="1:18" ht="96" hidden="1">
+    <row r="66" spans="1:18" ht="96">
       <c r="A66" s="20" t="str">
         <f t="shared" ref="A66:A129" si="11">CONCATENATE("T",ROW(A66)-1)</f>
         <v>T65</v>
@@ -11910,7 +11901,7 @@
         <v>871</v>
       </c>
     </row>
-    <row r="67" spans="1:18" ht="256" hidden="1">
+    <row r="67" spans="1:18" ht="256">
       <c r="A67" s="20" t="str">
         <f t="shared" si="11"/>
         <v>T66</v>
@@ -11971,7 +11962,7 @@
       </c>
       <c r="R67" s="24"/>
     </row>
-    <row r="68" spans="1:18" ht="16" hidden="1">
+    <row r="68" spans="1:18" ht="16">
       <c r="A68" s="20" t="str">
         <f t="shared" si="11"/>
         <v>T67</v>
@@ -12028,7 +12019,7 @@
       <c r="Q68" s="24"/>
       <c r="R68" s="24"/>
     </row>
-    <row r="69" spans="1:18" ht="96" hidden="1">
+    <row r="69" spans="1:18" ht="96">
       <c r="A69" s="20" t="str">
         <f t="shared" si="11"/>
         <v>T68</v>
@@ -12091,7 +12082,7 @@
         <v>903</v>
       </c>
     </row>
-    <row r="70" spans="1:18" ht="144" hidden="1">
+    <row r="70" spans="1:18" ht="144">
       <c r="A70" s="20" t="str">
         <f t="shared" si="11"/>
         <v>T69</v>
@@ -12152,7 +12143,7 @@
       </c>
       <c r="R70" s="24"/>
     </row>
-    <row r="71" spans="1:18" ht="96" hidden="1">
+    <row r="71" spans="1:18" ht="96">
       <c r="A71" s="20" t="str">
         <f t="shared" si="11"/>
         <v>T70</v>
@@ -12213,7 +12204,7 @@
       </c>
       <c r="R71" s="24"/>
     </row>
-    <row r="72" spans="1:18" ht="32" hidden="1">
+    <row r="72" spans="1:18" ht="32">
       <c r="A72" s="20" t="str">
         <f t="shared" si="11"/>
         <v>T71</v>
@@ -12270,7 +12261,7 @@
         <v>863</v>
       </c>
     </row>
-    <row r="73" spans="1:18" ht="48" hidden="1">
+    <row r="73" spans="1:18" ht="48">
       <c r="A73" s="20" t="str">
         <f t="shared" si="11"/>
         <v>T72</v>
@@ -12331,7 +12322,7 @@
       </c>
       <c r="R73" s="24"/>
     </row>
-    <row r="74" spans="1:18" ht="48" hidden="1">
+    <row r="74" spans="1:18" ht="48">
       <c r="A74" s="20" t="str">
         <f t="shared" si="11"/>
         <v>T73</v>
@@ -12392,7 +12383,7 @@
       </c>
       <c r="R74" s="24"/>
     </row>
-    <row r="75" spans="1:18" ht="32" hidden="1">
+    <row r="75" spans="1:18" ht="32">
       <c r="A75" s="20" t="str">
         <f t="shared" si="11"/>
         <v>T74</v>
@@ -12453,7 +12444,7 @@
       </c>
       <c r="R75" s="24"/>
     </row>
-    <row r="76" spans="1:18" ht="80" hidden="1">
+    <row r="76" spans="1:18" ht="80">
       <c r="A76" s="20" t="str">
         <f t="shared" si="11"/>
         <v>T75</v>
@@ -12514,7 +12505,7 @@
       </c>
       <c r="R76" s="24"/>
     </row>
-    <row r="77" spans="1:18" ht="160" hidden="1">
+    <row r="77" spans="1:18" ht="160">
       <c r="A77" s="20" t="str">
         <f t="shared" si="11"/>
         <v>T76</v>
@@ -12575,7 +12566,7 @@
       </c>
       <c r="R77" s="24"/>
     </row>
-    <row r="78" spans="1:18" ht="128" hidden="1">
+    <row r="78" spans="1:18" ht="128">
       <c r="A78" s="20" t="str">
         <f t="shared" si="11"/>
         <v>T77</v>
@@ -12634,7 +12625,7 @@
       <c r="Q78" s="24"/>
       <c r="R78" s="24"/>
     </row>
-    <row r="79" spans="1:18" ht="80" hidden="1">
+    <row r="79" spans="1:18" ht="80">
       <c r="A79" s="20" t="str">
         <f t="shared" si="11"/>
         <v>T78</v>
@@ -12695,7 +12686,7 @@
       </c>
       <c r="R79" s="24"/>
     </row>
-    <row r="80" spans="1:18" ht="96" hidden="1">
+    <row r="80" spans="1:18" ht="96">
       <c r="A80" s="20" t="str">
         <f t="shared" si="11"/>
         <v>T79</v>
@@ -12756,7 +12747,7 @@
       </c>
       <c r="R80" s="24"/>
     </row>
-    <row r="81" spans="1:18" ht="96" hidden="1">
+    <row r="81" spans="1:18" ht="96">
       <c r="A81" s="20" t="str">
         <f t="shared" si="11"/>
         <v>T80</v>
@@ -12817,7 +12808,7 @@
       </c>
       <c r="R81" s="24"/>
     </row>
-    <row r="82" spans="1:18" ht="240" hidden="1">
+    <row r="82" spans="1:18" ht="240">
       <c r="A82" s="20" t="str">
         <f t="shared" si="11"/>
         <v>T81</v>
@@ -12878,7 +12869,7 @@
       </c>
       <c r="R82" s="24"/>
     </row>
-    <row r="83" spans="1:18" ht="32" hidden="1">
+    <row r="83" spans="1:18" ht="32">
       <c r="A83" s="20" t="str">
         <f t="shared" si="11"/>
         <v>T82</v>
@@ -12929,7 +12920,7 @@
       <c r="Q83" s="24"/>
       <c r="R83" s="24"/>
     </row>
-    <row r="84" spans="1:18" ht="16" hidden="1">
+    <row r="84" spans="1:18" ht="16">
       <c r="A84" s="20" t="str">
         <f t="shared" si="11"/>
         <v>T83</v>
@@ -12980,7 +12971,7 @@
       <c r="Q84" s="24"/>
       <c r="R84" s="24"/>
     </row>
-    <row r="85" spans="1:18" ht="16" hidden="1">
+    <row r="85" spans="1:18" ht="16">
       <c r="A85" s="20" t="str">
         <f t="shared" si="11"/>
         <v>T84</v>
@@ -13031,7 +13022,7 @@
       <c r="Q85" s="24"/>
       <c r="R85" s="24"/>
     </row>
-    <row r="86" spans="1:18" ht="96" hidden="1">
+    <row r="86" spans="1:18" ht="96">
       <c r="A86" s="20" t="str">
         <f t="shared" si="11"/>
         <v>T85</v>
@@ -13082,7 +13073,7 @@
       <c r="Q86" s="24"/>
       <c r="R86" s="24"/>
     </row>
-    <row r="87" spans="1:18" ht="64" hidden="1">
+    <row r="87" spans="1:18" ht="64">
       <c r="A87" s="20" t="str">
         <f t="shared" si="11"/>
         <v>T86</v>
@@ -13133,7 +13124,7 @@
       <c r="Q87" s="24"/>
       <c r="R87" s="24"/>
     </row>
-    <row r="88" spans="1:18" ht="32" hidden="1">
+    <row r="88" spans="1:18" ht="32">
       <c r="A88" s="20" t="str">
         <f t="shared" si="11"/>
         <v>T87</v>
@@ -13184,7 +13175,7 @@
       <c r="Q88" s="24"/>
       <c r="R88" s="24"/>
     </row>
-    <row r="89" spans="1:18" ht="16" hidden="1">
+    <row r="89" spans="1:18" ht="16">
       <c r="A89" s="20" t="str">
         <f t="shared" si="11"/>
         <v>T88</v>
@@ -13235,7 +13226,7 @@
       <c r="Q89" s="24"/>
       <c r="R89" s="24"/>
     </row>
-    <row r="90" spans="1:18" ht="32" hidden="1">
+    <row r="90" spans="1:18" ht="32">
       <c r="A90" s="20" t="str">
         <f t="shared" si="11"/>
         <v>T89</v>
@@ -13286,7 +13277,7 @@
       <c r="Q90" s="24"/>
       <c r="R90" s="24"/>
     </row>
-    <row r="91" spans="1:18" ht="48" hidden="1">
+    <row r="91" spans="1:18" ht="48">
       <c r="A91" s="20" t="str">
         <f t="shared" si="11"/>
         <v>T90</v>
@@ -13337,7 +13328,7 @@
       <c r="Q91" s="24"/>
       <c r="R91" s="24"/>
     </row>
-    <row r="92" spans="1:18" ht="96" hidden="1">
+    <row r="92" spans="1:18" ht="96">
       <c r="A92" s="20" t="str">
         <f t="shared" si="11"/>
         <v>T91</v>
@@ -13388,7 +13379,7 @@
       <c r="Q92" s="24"/>
       <c r="R92" s="24"/>
     </row>
-    <row r="93" spans="1:18" ht="64" hidden="1">
+    <row r="93" spans="1:18" ht="64">
       <c r="A93" s="20" t="str">
         <f t="shared" si="11"/>
         <v>T92</v>
@@ -13439,7 +13430,7 @@
       <c r="Q93" s="24"/>
       <c r="R93" s="24"/>
     </row>
-    <row r="94" spans="1:18" ht="48" hidden="1">
+    <row r="94" spans="1:18" ht="48">
       <c r="A94" s="20" t="str">
         <f t="shared" si="11"/>
         <v>T93</v>
@@ -13490,7 +13481,7 @@
       <c r="Q94" s="24"/>
       <c r="R94" s="24"/>
     </row>
-    <row r="95" spans="1:18" ht="32" hidden="1">
+    <row r="95" spans="1:18" ht="32">
       <c r="A95" s="20" t="str">
         <f t="shared" si="11"/>
         <v>T94</v>
@@ -13541,7 +13532,7 @@
       <c r="Q95" s="24"/>
       <c r="R95" s="24"/>
     </row>
-    <row r="96" spans="1:18" ht="32" hidden="1">
+    <row r="96" spans="1:18" ht="32">
       <c r="A96" s="20" t="str">
         <f t="shared" si="11"/>
         <v>T95</v>
@@ -13592,7 +13583,7 @@
       <c r="Q96" s="24"/>
       <c r="R96" s="24"/>
     </row>
-    <row r="97" spans="1:18" ht="32" hidden="1">
+    <row r="97" spans="1:18" ht="32">
       <c r="A97" s="20" t="str">
         <f t="shared" si="11"/>
         <v>T96</v>
@@ -13643,7 +13634,7 @@
       <c r="Q97" s="24"/>
       <c r="R97" s="24"/>
     </row>
-    <row r="98" spans="1:18" ht="64" hidden="1">
+    <row r="98" spans="1:18" ht="64">
       <c r="A98" s="20" t="str">
         <f t="shared" si="11"/>
         <v>T97</v>
@@ -13694,7 +13685,7 @@
       <c r="Q98" s="24"/>
       <c r="R98" s="24"/>
     </row>
-    <row r="99" spans="1:18" ht="48" hidden="1">
+    <row r="99" spans="1:18" ht="48">
       <c r="A99" s="20" t="str">
         <f t="shared" si="11"/>
         <v>T98</v>
@@ -14210,7 +14201,7 @@
         <v>858</v>
       </c>
       <c r="P107" s="25" t="s">
-        <v>932</v>
+        <v>931</v>
       </c>
       <c r="Q107" s="25"/>
       <c r="R107" s="25" t="s">
@@ -14444,7 +14435,7 @@
       <c r="Q111" s="24"/>
       <c r="R111" s="24"/>
     </row>
-    <row r="112" spans="1:18" ht="48" hidden="1">
+    <row r="112" spans="1:18" ht="48">
       <c r="A112" s="20" t="str">
         <f t="shared" si="11"/>
         <v>T111</v>
@@ -14495,7 +14486,7 @@
       <c r="Q112" s="24"/>
       <c r="R112" s="24"/>
     </row>
-    <row r="113" spans="1:18" ht="80" hidden="1">
+    <row r="113" spans="1:18" ht="80">
       <c r="A113" s="20" t="str">
         <f t="shared" si="11"/>
         <v>T112</v>
@@ -14546,7 +14537,7 @@
       <c r="Q113" s="24"/>
       <c r="R113" s="24"/>
     </row>
-    <row r="114" spans="1:18" ht="64" hidden="1">
+    <row r="114" spans="1:18" ht="64">
       <c r="A114" s="20" t="str">
         <f t="shared" si="11"/>
         <v>T113</v>
@@ -14597,7 +14588,7 @@
       <c r="Q114" s="24"/>
       <c r="R114" s="24"/>
     </row>
-    <row r="115" spans="1:18" ht="48" hidden="1">
+    <row r="115" spans="1:18" ht="48">
       <c r="A115" s="20" t="str">
         <f t="shared" si="11"/>
         <v>T114</v>
@@ -14648,7 +14639,7 @@
       <c r="Q115" s="24"/>
       <c r="R115" s="24"/>
     </row>
-    <row r="116" spans="1:18" ht="48" hidden="1">
+    <row r="116" spans="1:18" ht="48">
       <c r="A116" s="20" t="str">
         <f t="shared" si="11"/>
         <v>T115</v>
@@ -14699,7 +14690,7 @@
       <c r="Q116" s="24"/>
       <c r="R116" s="24"/>
     </row>
-    <row r="117" spans="1:18" ht="16" hidden="1">
+    <row r="117" spans="1:18" ht="16">
       <c r="A117" s="20" t="str">
         <f t="shared" si="11"/>
         <v>T116</v>
@@ -14750,7 +14741,7 @@
       <c r="Q117" s="24"/>
       <c r="R117" s="24"/>
     </row>
-    <row r="118" spans="1:18" ht="16" hidden="1">
+    <row r="118" spans="1:18" ht="16">
       <c r="A118" s="20" t="str">
         <f t="shared" si="11"/>
         <v>T117</v>
@@ -14801,7 +14792,7 @@
       <c r="Q118" s="24"/>
       <c r="R118" s="24"/>
     </row>
-    <row r="119" spans="1:18" ht="48" hidden="1">
+    <row r="119" spans="1:18" ht="48">
       <c r="A119" s="20" t="str">
         <f t="shared" si="11"/>
         <v>T118</v>
@@ -14852,7 +14843,7 @@
       <c r="Q119" s="24"/>
       <c r="R119" s="24"/>
     </row>
-    <row r="120" spans="1:18" ht="96" hidden="1">
+    <row r="120" spans="1:18" ht="96">
       <c r="A120" s="20" t="str">
         <f t="shared" si="11"/>
         <v>T119</v>
@@ -14903,7 +14894,7 @@
       <c r="Q120" s="24"/>
       <c r="R120" s="24"/>
     </row>
-    <row r="121" spans="1:18" ht="64" hidden="1">
+    <row r="121" spans="1:18" ht="64">
       <c r="A121" s="20" t="str">
         <f t="shared" si="11"/>
         <v>T120</v>
@@ -14954,7 +14945,7 @@
       <c r="Q121" s="24"/>
       <c r="R121" s="24"/>
     </row>
-    <row r="122" spans="1:18" ht="48" hidden="1">
+    <row r="122" spans="1:18" ht="48">
       <c r="A122" s="20" t="str">
         <f t="shared" si="11"/>
         <v>T121</v>
@@ -15005,7 +14996,7 @@
       <c r="Q122" s="24"/>
       <c r="R122" s="24"/>
     </row>
-    <row r="123" spans="1:18" ht="48" hidden="1">
+    <row r="123" spans="1:18" ht="48">
       <c r="A123" s="20" t="str">
         <f t="shared" si="11"/>
         <v>T122</v>
@@ -15056,7 +15047,7 @@
       <c r="Q123" s="24"/>
       <c r="R123" s="24"/>
     </row>
-    <row r="124" spans="1:18" ht="16" hidden="1">
+    <row r="124" spans="1:18" ht="16">
       <c r="A124" s="20" t="str">
         <f t="shared" si="11"/>
         <v>T123</v>
@@ -15107,7 +15098,7 @@
       <c r="Q124" s="24"/>
       <c r="R124" s="24"/>
     </row>
-    <row r="125" spans="1:18" ht="32" hidden="1">
+    <row r="125" spans="1:18" ht="32">
       <c r="A125" s="20" t="str">
         <f t="shared" si="11"/>
         <v>T124</v>
@@ -15158,7 +15149,7 @@
       <c r="Q125" s="24"/>
       <c r="R125" s="24"/>
     </row>
-    <row r="126" spans="1:18" ht="16" hidden="1">
+    <row r="126" spans="1:18" ht="16">
       <c r="A126" s="20" t="str">
         <f t="shared" si="11"/>
         <v>T125</v>
@@ -15209,7 +15200,7 @@
       <c r="Q126" s="24"/>
       <c r="R126" s="24"/>
     </row>
-    <row r="127" spans="1:18" ht="64" hidden="1">
+    <row r="127" spans="1:18" ht="64">
       <c r="A127" s="20" t="str">
         <f t="shared" si="11"/>
         <v>T126</v>
@@ -15260,7 +15251,7 @@
       <c r="Q127" s="24"/>
       <c r="R127" s="24"/>
     </row>
-    <row r="128" spans="1:18" ht="48" hidden="1">
+    <row r="128" spans="1:18" ht="48">
       <c r="A128" s="20" t="str">
         <f t="shared" si="11"/>
         <v>T127</v>
@@ -15299,7 +15290,7 @@
       <c r="Q128" s="24"/>
       <c r="R128" s="24"/>
     </row>
-    <row r="129" spans="1:18" ht="96" hidden="1">
+    <row r="129" spans="1:18" ht="96">
       <c r="A129" s="20" t="str">
         <f t="shared" si="11"/>
         <v>T128</v>
@@ -15338,7 +15329,7 @@
       <c r="Q129" s="24"/>
       <c r="R129" s="24"/>
     </row>
-    <row r="130" spans="1:18" ht="32" hidden="1">
+    <row r="130" spans="1:18" ht="32">
       <c r="A130" s="20" t="str">
         <f t="shared" ref="A130:A193" si="22">CONCATENATE("T",ROW(A130)-1)</f>
         <v>T129</v>
@@ -15389,7 +15380,7 @@
       <c r="Q130" s="24"/>
       <c r="R130" s="24"/>
     </row>
-    <row r="131" spans="1:18" ht="64" hidden="1">
+    <row r="131" spans="1:18" ht="64">
       <c r="A131" s="20" t="str">
         <f t="shared" si="22"/>
         <v>T130</v>
@@ -15440,7 +15431,7 @@
       <c r="Q131" s="24"/>
       <c r="R131" s="24"/>
     </row>
-    <row r="132" spans="1:18" ht="48" hidden="1">
+    <row r="132" spans="1:18" ht="48">
       <c r="A132" s="20" t="str">
         <f t="shared" si="22"/>
         <v>T131</v>
@@ -15491,7 +15482,7 @@
       <c r="Q132" s="24"/>
       <c r="R132" s="24"/>
     </row>
-    <row r="133" spans="1:18" ht="32" hidden="1">
+    <row r="133" spans="1:18" ht="32">
       <c r="A133" s="20" t="str">
         <f t="shared" si="22"/>
         <v>T132</v>
@@ -15542,7 +15533,7 @@
       <c r="Q133" s="24"/>
       <c r="R133" s="24"/>
     </row>
-    <row r="134" spans="1:18" ht="48" hidden="1">
+    <row r="134" spans="1:18" ht="48">
       <c r="A134" s="20" t="str">
         <f t="shared" si="22"/>
         <v>T133</v>
@@ -15593,7 +15584,7 @@
       <c r="Q134" s="24"/>
       <c r="R134" s="24"/>
     </row>
-    <row r="135" spans="1:18" ht="48" hidden="1">
+    <row r="135" spans="1:18" ht="48">
       <c r="A135" s="20" t="str">
         <f t="shared" si="22"/>
         <v>T134</v>
@@ -15644,7 +15635,7 @@
       <c r="Q135" s="24"/>
       <c r="R135" s="24"/>
     </row>
-    <row r="136" spans="1:18" ht="64" hidden="1">
+    <row r="136" spans="1:18" ht="64">
       <c r="A136" s="20" t="str">
         <f t="shared" si="22"/>
         <v>T135</v>
@@ -15695,7 +15686,7 @@
       <c r="Q136" s="24"/>
       <c r="R136" s="24"/>
     </row>
-    <row r="137" spans="1:18" ht="48" hidden="1">
+    <row r="137" spans="1:18" ht="48">
       <c r="A137" s="20" t="str">
         <f t="shared" si="22"/>
         <v>T136</v>
@@ -15756,7 +15747,7 @@
       </c>
       <c r="R137" s="25"/>
     </row>
-    <row r="138" spans="1:18" ht="96" hidden="1">
+    <row r="138" spans="1:18" ht="96">
       <c r="A138" s="20" t="str">
         <f t="shared" si="22"/>
         <v>T137</v>
@@ -15807,7 +15798,7 @@
       <c r="Q138" s="24"/>
       <c r="R138" s="24"/>
     </row>
-    <row r="139" spans="1:18" ht="80" hidden="1">
+    <row r="139" spans="1:18" ht="80">
       <c r="A139" s="20" t="str">
         <f t="shared" si="22"/>
         <v>T138</v>
@@ -15858,7 +15849,7 @@
       <c r="Q139" s="24"/>
       <c r="R139" s="24"/>
     </row>
-    <row r="140" spans="1:18" ht="96" hidden="1">
+    <row r="140" spans="1:18" ht="96">
       <c r="A140" s="20" t="str">
         <f t="shared" si="22"/>
         <v>T139</v>
@@ -15909,7 +15900,7 @@
       <c r="Q140" s="24"/>
       <c r="R140" s="24"/>
     </row>
-    <row r="141" spans="1:18" ht="48" hidden="1">
+    <row r="141" spans="1:18" ht="48">
       <c r="A141" s="20" t="str">
         <f t="shared" si="22"/>
         <v>T140</v>
@@ -15960,7 +15951,7 @@
       <c r="Q141" s="24"/>
       <c r="R141" s="24"/>
     </row>
-    <row r="142" spans="1:18" ht="80" hidden="1">
+    <row r="142" spans="1:18" ht="80">
       <c r="A142" s="20" t="str">
         <f t="shared" si="22"/>
         <v>T141</v>
@@ -16011,7 +16002,7 @@
       <c r="Q142" s="24"/>
       <c r="R142" s="24"/>
     </row>
-    <row r="143" spans="1:18" ht="48" hidden="1">
+    <row r="143" spans="1:18" ht="48">
       <c r="A143" s="20" t="str">
         <f t="shared" si="22"/>
         <v>T142</v>
@@ -16062,7 +16053,7 @@
       <c r="Q143" s="24"/>
       <c r="R143" s="24"/>
     </row>
-    <row r="144" spans="1:18" ht="32" hidden="1">
+    <row r="144" spans="1:18" ht="32">
       <c r="A144" s="20" t="str">
         <f t="shared" si="22"/>
         <v>T143</v>
@@ -16113,7 +16104,7 @@
       <c r="Q144" s="24"/>
       <c r="R144" s="24"/>
     </row>
-    <row r="145" spans="1:18" ht="32" hidden="1">
+    <row r="145" spans="1:18" ht="32">
       <c r="A145" s="20" t="str">
         <f t="shared" si="22"/>
         <v>T144</v>
@@ -16164,7 +16155,7 @@
       <c r="Q145" s="24"/>
       <c r="R145" s="24"/>
     </row>
-    <row r="146" spans="1:18" ht="80" hidden="1">
+    <row r="146" spans="1:18" ht="80">
       <c r="A146" s="20" t="str">
         <f t="shared" si="22"/>
         <v>T145</v>
@@ -16215,7 +16206,7 @@
       <c r="Q146" s="24"/>
       <c r="R146" s="24"/>
     </row>
-    <row r="147" spans="1:18" ht="64" hidden="1">
+    <row r="147" spans="1:18" ht="64">
       <c r="A147" s="20" t="str">
         <f t="shared" si="22"/>
         <v>T146</v>
@@ -16266,7 +16257,7 @@
       <c r="Q147" s="24"/>
       <c r="R147" s="24"/>
     </row>
-    <row r="148" spans="1:18" ht="64" hidden="1">
+    <row r="148" spans="1:18" ht="64">
       <c r="A148" s="20" t="str">
         <f t="shared" si="22"/>
         <v>T147</v>
@@ -16317,7 +16308,7 @@
       <c r="Q148" s="24"/>
       <c r="R148" s="24"/>
     </row>
-    <row r="149" spans="1:18" ht="32" hidden="1">
+    <row r="149" spans="1:18" ht="32">
       <c r="A149" s="20" t="str">
         <f t="shared" si="22"/>
         <v>T148</v>
@@ -16368,7 +16359,7 @@
       <c r="Q149" s="24"/>
       <c r="R149" s="24"/>
     </row>
-    <row r="150" spans="1:18" ht="64" hidden="1">
+    <row r="150" spans="1:18" ht="64">
       <c r="A150" s="20" t="str">
         <f t="shared" si="22"/>
         <v>T149</v>
@@ -16419,7 +16410,7 @@
       <c r="Q150" s="24"/>
       <c r="R150" s="24"/>
     </row>
-    <row r="151" spans="1:18" ht="112" hidden="1">
+    <row r="151" spans="1:18" ht="112">
       <c r="A151" s="20" t="str">
         <f t="shared" si="22"/>
         <v>T150</v>
@@ -16470,7 +16461,7 @@
       <c r="Q151" s="24"/>
       <c r="R151" s="24"/>
     </row>
-    <row r="152" spans="1:18" ht="64" hidden="1">
+    <row r="152" spans="1:18" ht="64">
       <c r="A152" s="20" t="str">
         <f t="shared" si="22"/>
         <v>T151</v>
@@ -16521,7 +16512,7 @@
       <c r="Q152" s="24"/>
       <c r="R152" s="24"/>
     </row>
-    <row r="153" spans="1:18" ht="96" hidden="1">
+    <row r="153" spans="1:18" ht="96">
       <c r="A153" s="20" t="str">
         <f t="shared" si="22"/>
         <v>T152</v>
@@ -16572,7 +16563,7 @@
       <c r="Q153" s="24"/>
       <c r="R153" s="24"/>
     </row>
-    <row r="154" spans="1:18" ht="160" hidden="1">
+    <row r="154" spans="1:18" ht="160">
       <c r="A154" s="20" t="str">
         <f t="shared" si="22"/>
         <v>T153</v>
@@ -16623,7 +16614,7 @@
       <c r="Q154" s="24"/>
       <c r="R154" s="24"/>
     </row>
-    <row r="155" spans="1:18" ht="96" hidden="1">
+    <row r="155" spans="1:18" ht="96">
       <c r="A155" s="20" t="str">
         <f t="shared" si="22"/>
         <v>T154</v>
@@ -16674,7 +16665,7 @@
       <c r="Q155" s="24"/>
       <c r="R155" s="24"/>
     </row>
-    <row r="156" spans="1:18" ht="80" hidden="1">
+    <row r="156" spans="1:18" ht="80">
       <c r="A156" s="20" t="str">
         <f t="shared" si="22"/>
         <v>T155</v>
@@ -16725,7 +16716,7 @@
       <c r="Q156" s="24"/>
       <c r="R156" s="24"/>
     </row>
-    <row r="157" spans="1:18" ht="96" hidden="1">
+    <row r="157" spans="1:18" ht="96">
       <c r="A157" s="20" t="str">
         <f t="shared" si="22"/>
         <v>T156</v>
@@ -16776,7 +16767,7 @@
       <c r="Q157" s="24"/>
       <c r="R157" s="24"/>
     </row>
-    <row r="158" spans="1:18" ht="48" hidden="1">
+    <row r="158" spans="1:18" ht="48">
       <c r="A158" s="20" t="str">
         <f t="shared" si="22"/>
         <v>T157</v>
@@ -16827,7 +16818,7 @@
       <c r="Q158" s="24"/>
       <c r="R158" s="24"/>
     </row>
-    <row r="159" spans="1:18" ht="32" hidden="1">
+    <row r="159" spans="1:18" ht="32">
       <c r="A159" s="20" t="str">
         <f t="shared" si="22"/>
         <v>T158</v>
@@ -16878,7 +16869,7 @@
       <c r="Q159" s="24"/>
       <c r="R159" s="24"/>
     </row>
-    <row r="160" spans="1:18" ht="80" hidden="1">
+    <row r="160" spans="1:18" ht="80">
       <c r="A160" s="20" t="str">
         <f t="shared" si="22"/>
         <v>T159</v>
@@ -16929,7 +16920,7 @@
       <c r="Q160" s="24"/>
       <c r="R160" s="24"/>
     </row>
-    <row r="161" spans="1:18" ht="80" hidden="1">
+    <row r="161" spans="1:18" ht="80">
       <c r="A161" s="20" t="str">
         <f t="shared" si="22"/>
         <v>T160</v>
@@ -16980,7 +16971,7 @@
       <c r="Q161" s="24"/>
       <c r="R161" s="24"/>
     </row>
-    <row r="162" spans="1:18" ht="64" hidden="1">
+    <row r="162" spans="1:18" ht="64">
       <c r="A162" s="20" t="str">
         <f t="shared" si="22"/>
         <v>T161</v>
@@ -17031,7 +17022,7 @@
       <c r="Q162" s="24"/>
       <c r="R162" s="24"/>
     </row>
-    <row r="163" spans="1:18" ht="64" hidden="1">
+    <row r="163" spans="1:18" ht="64">
       <c r="A163" s="20" t="str">
         <f t="shared" si="22"/>
         <v>T162</v>
@@ -17082,7 +17073,7 @@
       <c r="Q163" s="24"/>
       <c r="R163" s="24"/>
     </row>
-    <row r="164" spans="1:18" ht="48" hidden="1">
+    <row r="164" spans="1:18" ht="48">
       <c r="A164" s="20" t="str">
         <f t="shared" si="22"/>
         <v>T163</v>
@@ -17133,7 +17124,7 @@
       <c r="Q164" s="24"/>
       <c r="R164" s="24"/>
     </row>
-    <row r="165" spans="1:18" ht="32" hidden="1">
+    <row r="165" spans="1:18" ht="32">
       <c r="A165" s="20" t="str">
         <f t="shared" si="22"/>
         <v>T164</v>
@@ -17184,7 +17175,7 @@
       <c r="Q165" s="24"/>
       <c r="R165" s="24"/>
     </row>
-    <row r="166" spans="1:18" ht="32" hidden="1">
+    <row r="166" spans="1:18" ht="32">
       <c r="A166" s="20" t="str">
         <f t="shared" si="22"/>
         <v>T165</v>
@@ -17235,7 +17226,7 @@
       <c r="Q166" s="24"/>
       <c r="R166" s="24"/>
     </row>
-    <row r="167" spans="1:18" ht="32" hidden="1">
+    <row r="167" spans="1:18" ht="32">
       <c r="A167" s="20" t="str">
         <f t="shared" si="22"/>
         <v>T166</v>
@@ -17286,7 +17277,7 @@
       <c r="Q167" s="24"/>
       <c r="R167" s="24"/>
     </row>
-    <row r="168" spans="1:18" ht="32" hidden="1">
+    <row r="168" spans="1:18" ht="32">
       <c r="A168" s="20" t="str">
         <f t="shared" si="22"/>
         <v>T167</v>
@@ -17337,7 +17328,7 @@
       <c r="Q168" s="24"/>
       <c r="R168" s="24"/>
     </row>
-    <row r="169" spans="1:18" ht="64" hidden="1">
+    <row r="169" spans="1:18" ht="64">
       <c r="A169" s="20" t="str">
         <f t="shared" si="22"/>
         <v>T168</v>
@@ -17388,7 +17379,7 @@
       <c r="Q169" s="24"/>
       <c r="R169" s="24"/>
     </row>
-    <row r="170" spans="1:18" ht="48" hidden="1">
+    <row r="170" spans="1:18" ht="48">
       <c r="A170" s="20" t="str">
         <f t="shared" si="22"/>
         <v>T169</v>
@@ -17439,7 +17430,7 @@
       <c r="Q170" s="24"/>
       <c r="R170" s="24"/>
     </row>
-    <row r="171" spans="1:18" ht="32" hidden="1">
+    <row r="171" spans="1:18" ht="32">
       <c r="A171" s="20" t="str">
         <f t="shared" si="22"/>
         <v>T170</v>
@@ -17490,7 +17481,7 @@
       <c r="Q171" s="24"/>
       <c r="R171" s="24"/>
     </row>
-    <row r="172" spans="1:18" ht="32" hidden="1">
+    <row r="172" spans="1:18" ht="32">
       <c r="A172" s="20" t="str">
         <f t="shared" si="22"/>
         <v>T171</v>
@@ -17541,7 +17532,7 @@
       <c r="Q172" s="24"/>
       <c r="R172" s="24"/>
     </row>
-    <row r="173" spans="1:18" ht="16" hidden="1">
+    <row r="173" spans="1:18" ht="16">
       <c r="A173" s="20" t="str">
         <f t="shared" si="22"/>
         <v>T172</v>
@@ -17592,7 +17583,7 @@
       <c r="Q173" s="24"/>
       <c r="R173" s="24"/>
     </row>
-    <row r="174" spans="1:18" ht="16" hidden="1">
+    <row r="174" spans="1:18" ht="16">
       <c r="A174" s="20" t="str">
         <f t="shared" si="22"/>
         <v>T173</v>
@@ -17643,7 +17634,7 @@
       <c r="Q174" s="24"/>
       <c r="R174" s="24"/>
     </row>
-    <row r="175" spans="1:18" ht="64" hidden="1">
+    <row r="175" spans="1:18" ht="64">
       <c r="A175" s="20" t="str">
         <f t="shared" si="22"/>
         <v>T174</v>
@@ -17694,7 +17685,7 @@
       <c r="Q175" s="24"/>
       <c r="R175" s="24"/>
     </row>
-    <row r="176" spans="1:18" ht="64" hidden="1">
+    <row r="176" spans="1:18" ht="64">
       <c r="A176" s="20" t="str">
         <f t="shared" si="22"/>
         <v>T175</v>
@@ -17745,7 +17736,7 @@
       <c r="Q176" s="24"/>
       <c r="R176" s="24"/>
     </row>
-    <row r="177" spans="1:18" ht="80" hidden="1">
+    <row r="177" spans="1:18" ht="80">
       <c r="A177" s="20" t="str">
         <f t="shared" si="22"/>
         <v>T176</v>
@@ -17796,7 +17787,7 @@
       <c r="Q177" s="24"/>
       <c r="R177" s="24"/>
     </row>
-    <row r="178" spans="1:18" ht="48" hidden="1">
+    <row r="178" spans="1:18" ht="48">
       <c r="A178" s="20" t="str">
         <f t="shared" si="22"/>
         <v>T177</v>
@@ -17847,7 +17838,7 @@
       <c r="Q178" s="24"/>
       <c r="R178" s="24"/>
     </row>
-    <row r="179" spans="1:18" ht="32" hidden="1">
+    <row r="179" spans="1:18" ht="32">
       <c r="A179" s="20" t="str">
         <f t="shared" si="22"/>
         <v>T178</v>
@@ -17898,7 +17889,7 @@
       <c r="Q179" s="24"/>
       <c r="R179" s="24"/>
     </row>
-    <row r="180" spans="1:18" ht="32" hidden="1">
+    <row r="180" spans="1:18" ht="32">
       <c r="A180" s="20" t="str">
         <f t="shared" si="22"/>
         <v>T179</v>
@@ -17949,7 +17940,7 @@
       <c r="Q180" s="24"/>
       <c r="R180" s="24"/>
     </row>
-    <row r="181" spans="1:18" ht="80" hidden="1">
+    <row r="181" spans="1:18" ht="80">
       <c r="A181" s="20" t="str">
         <f t="shared" si="22"/>
         <v>T180</v>
@@ -18000,7 +17991,7 @@
       <c r="Q181" s="24"/>
       <c r="R181" s="24"/>
     </row>
-    <row r="182" spans="1:18" ht="64" hidden="1">
+    <row r="182" spans="1:18" ht="64">
       <c r="A182" s="20" t="str">
         <f t="shared" si="22"/>
         <v>T181</v>
@@ -18051,7 +18042,7 @@
       <c r="Q182" s="24"/>
       <c r="R182" s="24"/>
     </row>
-    <row r="183" spans="1:18" ht="64" hidden="1">
+    <row r="183" spans="1:18" ht="64">
       <c r="A183" s="20" t="str">
         <f t="shared" si="22"/>
         <v>T182</v>
@@ -18102,7 +18093,7 @@
       <c r="Q183" s="24"/>
       <c r="R183" s="24"/>
     </row>
-    <row r="184" spans="1:18" ht="144" hidden="1">
+    <row r="184" spans="1:18" ht="144">
       <c r="A184" s="20" t="str">
         <f t="shared" si="22"/>
         <v>T183</v>
@@ -18153,7 +18144,7 @@
       <c r="Q184" s="24"/>
       <c r="R184" s="24"/>
     </row>
-    <row r="185" spans="1:18" ht="96" hidden="1">
+    <row r="185" spans="1:18" ht="96">
       <c r="A185" s="20" t="str">
         <f t="shared" si="22"/>
         <v>T184</v>
@@ -18204,7 +18195,7 @@
       <c r="Q185" s="24"/>
       <c r="R185" s="24"/>
     </row>
-    <row r="186" spans="1:18" ht="48" hidden="1">
+    <row r="186" spans="1:18" ht="48">
       <c r="A186" s="20" t="str">
         <f t="shared" si="22"/>
         <v>T185</v>
@@ -18255,7 +18246,7 @@
       <c r="Q186" s="24"/>
       <c r="R186" s="24"/>
     </row>
-    <row r="187" spans="1:18" ht="16" hidden="1">
+    <row r="187" spans="1:18" ht="16">
       <c r="A187" s="20" t="str">
         <f t="shared" si="22"/>
         <v>T186</v>
@@ -18306,7 +18297,7 @@
       <c r="Q187" s="24"/>
       <c r="R187" s="24"/>
     </row>
-    <row r="188" spans="1:18" ht="144" hidden="1">
+    <row r="188" spans="1:18" ht="144">
       <c r="A188" s="20" t="str">
         <f t="shared" si="22"/>
         <v>T187</v>
@@ -18357,7 +18348,7 @@
       <c r="Q188" s="24"/>
       <c r="R188" s="24"/>
     </row>
-    <row r="189" spans="1:18" ht="128" hidden="1">
+    <row r="189" spans="1:18" ht="128">
       <c r="A189" s="20" t="str">
         <f t="shared" si="22"/>
         <v>T188</v>
@@ -18408,7 +18399,7 @@
       <c r="Q189" s="24"/>
       <c r="R189" s="24"/>
     </row>
-    <row r="190" spans="1:18" ht="128" hidden="1">
+    <row r="190" spans="1:18" ht="128">
       <c r="A190" s="20" t="str">
         <f t="shared" si="22"/>
         <v>T189</v>
@@ -18459,7 +18450,7 @@
       <c r="Q190" s="24"/>
       <c r="R190" s="24"/>
     </row>
-    <row r="191" spans="1:18" ht="96" hidden="1">
+    <row r="191" spans="1:18" ht="96">
       <c r="A191" s="20" t="str">
         <f t="shared" si="22"/>
         <v>T190</v>
@@ -18510,7 +18501,7 @@
       <c r="Q191" s="24"/>
       <c r="R191" s="24"/>
     </row>
-    <row r="192" spans="1:18" ht="80" hidden="1">
+    <row r="192" spans="1:18" ht="80">
       <c r="A192" s="20" t="str">
         <f t="shared" si="22"/>
         <v>T191</v>
@@ -18561,7 +18552,7 @@
       <c r="Q192" s="24"/>
       <c r="R192" s="24"/>
     </row>
-    <row r="193" spans="1:18" ht="80" hidden="1">
+    <row r="193" spans="1:18" ht="80">
       <c r="A193" s="20" t="str">
         <f t="shared" si="22"/>
         <v>T192</v>
@@ -18612,7 +18603,7 @@
       <c r="Q193" s="24"/>
       <c r="R193" s="24"/>
     </row>
-    <row r="194" spans="1:18" ht="48" hidden="1">
+    <row r="194" spans="1:18" ht="48">
       <c r="A194" s="20" t="str">
         <f t="shared" ref="A194:A257" si="27">CONCATENATE("T",ROW(A194)-1)</f>
         <v>T193</v>
@@ -18663,7 +18654,7 @@
       <c r="Q194" s="24"/>
       <c r="R194" s="24"/>
     </row>
-    <row r="195" spans="1:18" ht="32" hidden="1">
+    <row r="195" spans="1:18" ht="32">
       <c r="A195" s="20" t="str">
         <f t="shared" si="27"/>
         <v>T194</v>
@@ -18714,7 +18705,7 @@
       <c r="Q195" s="24"/>
       <c r="R195" s="24"/>
     </row>
-    <row r="196" spans="1:18" ht="80" hidden="1">
+    <row r="196" spans="1:18" ht="80">
       <c r="A196" s="20" t="str">
         <f t="shared" si="27"/>
         <v>T195</v>
@@ -18765,7 +18756,7 @@
       <c r="Q196" s="24"/>
       <c r="R196" s="24"/>
     </row>
-    <row r="197" spans="1:18" ht="96" hidden="1">
+    <row r="197" spans="1:18" ht="96">
       <c r="A197" s="20" t="str">
         <f t="shared" si="27"/>
         <v>T196</v>
@@ -18816,7 +18807,7 @@
       <c r="Q197" s="24"/>
       <c r="R197" s="24"/>
     </row>
-    <row r="198" spans="1:18" ht="48" hidden="1">
+    <row r="198" spans="1:18" ht="48">
       <c r="A198" s="20" t="str">
         <f t="shared" si="27"/>
         <v>T197</v>
@@ -18867,7 +18858,7 @@
       <c r="Q198" s="24"/>
       <c r="R198" s="24"/>
     </row>
-    <row r="199" spans="1:18" ht="80" hidden="1">
+    <row r="199" spans="1:18" ht="80">
       <c r="A199" s="20" t="str">
         <f t="shared" si="27"/>
         <v>T198</v>
@@ -18918,7 +18909,7 @@
       <c r="Q199" s="24"/>
       <c r="R199" s="24"/>
     </row>
-    <row r="200" spans="1:18" ht="48" hidden="1">
+    <row r="200" spans="1:18" ht="48">
       <c r="A200" s="20" t="str">
         <f t="shared" si="27"/>
         <v>T199</v>
@@ -18969,7 +18960,7 @@
       <c r="Q200" s="24"/>
       <c r="R200" s="24"/>
     </row>
-    <row r="201" spans="1:18" ht="32" hidden="1">
+    <row r="201" spans="1:18" ht="32">
       <c r="A201" s="20" t="str">
         <f t="shared" si="27"/>
         <v>T200</v>
@@ -19020,7 +19011,7 @@
       <c r="Q201" s="24"/>
       <c r="R201" s="24"/>
     </row>
-    <row r="202" spans="1:18" ht="32" hidden="1">
+    <row r="202" spans="1:18" ht="32">
       <c r="A202" s="20" t="str">
         <f t="shared" si="27"/>
         <v>T201</v>
@@ -19071,7 +19062,7 @@
       <c r="Q202" s="24"/>
       <c r="R202" s="24"/>
     </row>
-    <row r="203" spans="1:18" ht="80" hidden="1">
+    <row r="203" spans="1:18" ht="80">
       <c r="A203" s="20" t="str">
         <f t="shared" si="27"/>
         <v>T202</v>
@@ -19122,7 +19113,7 @@
       <c r="Q203" s="24"/>
       <c r="R203" s="24"/>
     </row>
-    <row r="204" spans="1:18" ht="64" hidden="1">
+    <row r="204" spans="1:18" ht="64">
       <c r="A204" s="20" t="str">
         <f t="shared" si="27"/>
         <v>T203</v>
@@ -19173,7 +19164,7 @@
       <c r="Q204" s="24"/>
       <c r="R204" s="24"/>
     </row>
-    <row r="205" spans="1:18" ht="64" hidden="1">
+    <row r="205" spans="1:18" ht="64">
       <c r="A205" s="20" t="str">
         <f t="shared" si="27"/>
         <v>T204</v>
@@ -19224,7 +19215,7 @@
       <c r="Q205" s="24"/>
       <c r="R205" s="24"/>
     </row>
-    <row r="206" spans="1:18" ht="32" hidden="1">
+    <row r="206" spans="1:18" ht="32">
       <c r="A206" s="20" t="str">
         <f t="shared" si="27"/>
         <v>T205</v>
@@ -19275,7 +19266,7 @@
       <c r="Q206" s="24"/>
       <c r="R206" s="24"/>
     </row>
-    <row r="207" spans="1:18" ht="80" hidden="1">
+    <row r="207" spans="1:18" ht="80">
       <c r="A207" s="20" t="str">
         <f t="shared" si="27"/>
         <v>T206</v>
@@ -19326,7 +19317,7 @@
       <c r="Q207" s="24"/>
       <c r="R207" s="24"/>
     </row>
-    <row r="208" spans="1:18" ht="96" hidden="1">
+    <row r="208" spans="1:18" ht="96">
       <c r="A208" s="20" t="str">
         <f t="shared" si="27"/>
         <v>T207</v>
@@ -19377,7 +19368,7 @@
       <c r="Q208" s="24"/>
       <c r="R208" s="24"/>
     </row>
-    <row r="209" spans="1:18" ht="80" hidden="1">
+    <row r="209" spans="1:18" ht="80">
       <c r="A209" s="20" t="str">
         <f t="shared" si="27"/>
         <v>T208</v>
@@ -19428,7 +19419,7 @@
       <c r="Q209" s="24"/>
       <c r="R209" s="24"/>
     </row>
-    <row r="210" spans="1:18" ht="80" hidden="1">
+    <row r="210" spans="1:18" ht="80">
       <c r="A210" s="20" t="str">
         <f t="shared" si="27"/>
         <v>T209</v>
@@ -19479,7 +19470,7 @@
       <c r="Q210" s="24"/>
       <c r="R210" s="24"/>
     </row>
-    <row r="211" spans="1:18" ht="48" hidden="1">
+    <row r="211" spans="1:18" ht="48">
       <c r="A211" s="20" t="str">
         <f t="shared" si="27"/>
         <v>T210</v>
@@ -19530,7 +19521,7 @@
       <c r="Q211" s="24"/>
       <c r="R211" s="24"/>
     </row>
-    <row r="212" spans="1:18" ht="32" hidden="1">
+    <row r="212" spans="1:18" ht="32">
       <c r="A212" s="20" t="str">
         <f t="shared" si="27"/>
         <v>T211</v>
@@ -19581,7 +19572,7 @@
       <c r="Q212" s="24"/>
       <c r="R212" s="24"/>
     </row>
-    <row r="213" spans="1:18" ht="144" hidden="1">
+    <row r="213" spans="1:18" ht="144">
       <c r="A213" s="20" t="str">
         <f t="shared" si="27"/>
         <v>T212</v>
@@ -19632,7 +19623,7 @@
       <c r="Q213" s="24"/>
       <c r="R213" s="24"/>
     </row>
-    <row r="214" spans="1:18" ht="80" hidden="1">
+    <row r="214" spans="1:18" ht="80">
       <c r="A214" s="20" t="str">
         <f t="shared" si="27"/>
         <v>T213</v>
@@ -19683,7 +19674,7 @@
       <c r="Q214" s="24"/>
       <c r="R214" s="24"/>
     </row>
-    <row r="215" spans="1:18" ht="96" hidden="1">
+    <row r="215" spans="1:18" ht="96">
       <c r="A215" s="20" t="str">
         <f t="shared" si="27"/>
         <v>T214</v>
@@ -19734,7 +19725,7 @@
       <c r="Q215" s="24"/>
       <c r="R215" s="24"/>
     </row>
-    <row r="216" spans="1:18" ht="96" hidden="1">
+    <row r="216" spans="1:18" ht="96">
       <c r="A216" s="20" t="str">
         <f t="shared" si="27"/>
         <v>T215</v>
@@ -19785,7 +19776,7 @@
       <c r="Q216" s="24"/>
       <c r="R216" s="24"/>
     </row>
-    <row r="217" spans="1:18" ht="80" hidden="1">
+    <row r="217" spans="1:18" ht="80">
       <c r="A217" s="20" t="str">
         <f t="shared" si="27"/>
         <v>T216</v>
@@ -19836,7 +19827,7 @@
       <c r="Q217" s="24"/>
       <c r="R217" s="24"/>
     </row>
-    <row r="218" spans="1:18" ht="80" hidden="1">
+    <row r="218" spans="1:18" ht="80">
       <c r="A218" s="20" t="str">
         <f t="shared" si="27"/>
         <v>T217</v>
@@ -19887,7 +19878,7 @@
       <c r="Q218" s="24"/>
       <c r="R218" s="24"/>
     </row>
-    <row r="219" spans="1:18" ht="48" hidden="1">
+    <row r="219" spans="1:18" ht="48">
       <c r="A219" s="20" t="str">
         <f t="shared" si="27"/>
         <v>T218</v>
@@ -19938,7 +19929,7 @@
       <c r="Q219" s="24"/>
       <c r="R219" s="24"/>
     </row>
-    <row r="220" spans="1:18" ht="32" hidden="1">
+    <row r="220" spans="1:18" ht="32">
       <c r="A220" s="20" t="str">
         <f t="shared" si="27"/>
         <v>T219</v>
@@ -19989,7 +19980,7 @@
       <c r="Q220" s="24"/>
       <c r="R220" s="24"/>
     </row>
-    <row r="221" spans="1:18" ht="64" hidden="1">
+    <row r="221" spans="1:18" ht="64">
       <c r="A221" s="20" t="str">
         <f t="shared" si="27"/>
         <v>T220</v>
@@ -20040,7 +20031,7 @@
       <c r="Q221" s="24"/>
       <c r="R221" s="24"/>
     </row>
-    <row r="222" spans="1:18" ht="16" hidden="1">
+    <row r="222" spans="1:18" ht="16">
       <c r="A222" s="20" t="str">
         <f t="shared" si="27"/>
         <v>T221</v>
@@ -20091,7 +20082,7 @@
       <c r="Q222" s="24"/>
       <c r="R222" s="24"/>
     </row>
-    <row r="223" spans="1:18" ht="64" hidden="1">
+    <row r="223" spans="1:18" ht="64">
       <c r="A223" s="20" t="str">
         <f t="shared" si="27"/>
         <v>T222</v>
@@ -20142,7 +20133,7 @@
       <c r="Q223" s="24"/>
       <c r="R223" s="24"/>
     </row>
-    <row r="224" spans="1:18" ht="96" hidden="1">
+    <row r="224" spans="1:18" ht="96">
       <c r="A224" s="20" t="str">
         <f t="shared" si="27"/>
         <v>T223</v>
@@ -20193,7 +20184,7 @@
       <c r="Q224" s="24"/>
       <c r="R224" s="24"/>
     </row>
-    <row r="225" spans="1:18" ht="80" hidden="1">
+    <row r="225" spans="1:18" ht="80">
       <c r="A225" s="20" t="str">
         <f t="shared" si="27"/>
         <v>T224</v>
@@ -20244,7 +20235,7 @@
       <c r="Q225" s="24"/>
       <c r="R225" s="24"/>
     </row>
-    <row r="226" spans="1:18" ht="80" hidden="1">
+    <row r="226" spans="1:18" ht="80">
       <c r="A226" s="20" t="str">
         <f t="shared" si="27"/>
         <v>T225</v>
@@ -20295,7 +20286,7 @@
       <c r="Q226" s="24"/>
       <c r="R226" s="24"/>
     </row>
-    <row r="227" spans="1:18" ht="64" hidden="1">
+    <row r="227" spans="1:18" ht="64">
       <c r="A227" s="20" t="str">
         <f t="shared" si="27"/>
         <v>T226</v>
@@ -20346,7 +20337,7 @@
       <c r="Q227" s="24"/>
       <c r="R227" s="24"/>
     </row>
-    <row r="228" spans="1:18" ht="80" hidden="1">
+    <row r="228" spans="1:18" ht="80">
       <c r="A228" s="20" t="str">
         <f t="shared" si="27"/>
         <v>T227</v>
@@ -20397,7 +20388,7 @@
       <c r="Q228" s="24"/>
       <c r="R228" s="24"/>
     </row>
-    <row r="229" spans="1:18" ht="64" hidden="1">
+    <row r="229" spans="1:18" ht="64">
       <c r="A229" s="20" t="str">
         <f t="shared" si="27"/>
         <v>T228</v>
@@ -20448,7 +20439,7 @@
       <c r="Q229" s="24"/>
       <c r="R229" s="24"/>
     </row>
-    <row r="230" spans="1:18" ht="48" hidden="1">
+    <row r="230" spans="1:18" ht="48">
       <c r="A230" s="20" t="str">
         <f t="shared" si="27"/>
         <v>T229</v>
@@ -20499,7 +20490,7 @@
       <c r="Q230" s="24"/>
       <c r="R230" s="24"/>
     </row>
-    <row r="231" spans="1:18" ht="80" hidden="1">
+    <row r="231" spans="1:18" ht="80">
       <c r="A231" s="20" t="str">
         <f t="shared" si="27"/>
         <v>T230</v>
@@ -20550,7 +20541,7 @@
       <c r="Q231" s="24"/>
       <c r="R231" s="24"/>
     </row>
-    <row r="232" spans="1:18" ht="80" hidden="1">
+    <row r="232" spans="1:18" ht="80">
       <c r="A232" s="20" t="str">
         <f t="shared" si="27"/>
         <v>T231</v>
@@ -20601,7 +20592,7 @@
       <c r="Q232" s="24"/>
       <c r="R232" s="24"/>
     </row>
-    <row r="233" spans="1:18" ht="48" hidden="1">
+    <row r="233" spans="1:18" ht="48">
       <c r="A233" s="20" t="str">
         <f t="shared" si="27"/>
         <v>T232</v>
@@ -20652,7 +20643,7 @@
       <c r="Q233" s="24"/>
       <c r="R233" s="24"/>
     </row>
-    <row r="234" spans="1:18" ht="96" hidden="1">
+    <row r="234" spans="1:18" ht="96">
       <c r="A234" s="20" t="str">
         <f t="shared" si="27"/>
         <v>T233</v>
@@ -20703,7 +20694,7 @@
       <c r="Q234" s="24"/>
       <c r="R234" s="24"/>
     </row>
-    <row r="235" spans="1:18" ht="96" hidden="1">
+    <row r="235" spans="1:18" ht="96">
       <c r="A235" s="20" t="str">
         <f t="shared" si="27"/>
         <v>T234</v>
@@ -20754,7 +20745,7 @@
       <c r="Q235" s="24"/>
       <c r="R235" s="24"/>
     </row>
-    <row r="236" spans="1:18" ht="80" hidden="1">
+    <row r="236" spans="1:18" ht="80">
       <c r="A236" s="20" t="str">
         <f t="shared" si="27"/>
         <v>T235</v>
@@ -20805,7 +20796,7 @@
       <c r="Q236" s="24"/>
       <c r="R236" s="24"/>
     </row>
-    <row r="237" spans="1:18" ht="80" hidden="1">
+    <row r="237" spans="1:18" ht="80">
       <c r="A237" s="20" t="str">
         <f t="shared" si="27"/>
         <v>T236</v>
@@ -20856,7 +20847,7 @@
       <c r="Q237" s="24"/>
       <c r="R237" s="24"/>
     </row>
-    <row r="238" spans="1:18" ht="48" hidden="1">
+    <row r="238" spans="1:18" ht="48">
       <c r="A238" s="20" t="str">
         <f t="shared" si="27"/>
         <v>T237</v>
@@ -20907,7 +20898,7 @@
       <c r="Q238" s="24"/>
       <c r="R238" s="24"/>
     </row>
-    <row r="239" spans="1:18" ht="32" hidden="1">
+    <row r="239" spans="1:18" ht="32">
       <c r="A239" s="20" t="str">
         <f t="shared" si="27"/>
         <v>T238</v>
@@ -20958,7 +20949,7 @@
       <c r="Q239" s="24"/>
       <c r="R239" s="24"/>
     </row>
-    <row r="240" spans="1:18" ht="80" hidden="1">
+    <row r="240" spans="1:18" ht="80">
       <c r="A240" s="20" t="str">
         <f t="shared" si="27"/>
         <v>T239</v>
@@ -21009,7 +21000,7 @@
       <c r="Q240" s="24"/>
       <c r="R240" s="24"/>
     </row>
-    <row r="241" spans="1:18" ht="80" hidden="1">
+    <row r="241" spans="1:18" ht="80">
       <c r="A241" s="20" t="str">
         <f t="shared" si="27"/>
         <v>T240</v>
@@ -21060,7 +21051,7 @@
       <c r="Q241" s="24"/>
       <c r="R241" s="24"/>
     </row>
-    <row r="242" spans="1:18" ht="48" hidden="1">
+    <row r="242" spans="1:18" ht="48">
       <c r="A242" s="20" t="str">
         <f t="shared" si="27"/>
         <v>T241</v>
@@ -21111,7 +21102,7 @@
       <c r="Q242" s="24"/>
       <c r="R242" s="24"/>
     </row>
-    <row r="243" spans="1:18" ht="32" hidden="1">
+    <row r="243" spans="1:18" ht="32">
       <c r="A243" s="20" t="str">
         <f t="shared" si="27"/>
         <v>T242</v>
@@ -21162,7 +21153,7 @@
       <c r="Q243" s="24"/>
       <c r="R243" s="24"/>
     </row>
-    <row r="244" spans="1:18" ht="32" hidden="1">
+    <row r="244" spans="1:18" ht="32">
       <c r="A244" s="20" t="str">
         <f t="shared" si="27"/>
         <v>T243</v>
@@ -21213,7 +21204,7 @@
       <c r="Q244" s="24"/>
       <c r="R244" s="24"/>
     </row>
-    <row r="245" spans="1:18" ht="32" hidden="1">
+    <row r="245" spans="1:18" ht="32">
       <c r="A245" s="20" t="str">
         <f t="shared" si="27"/>
         <v>T244</v>
@@ -21264,7 +21255,7 @@
       <c r="Q245" s="24"/>
       <c r="R245" s="24"/>
     </row>
-    <row r="246" spans="1:18" ht="80" hidden="1">
+    <row r="246" spans="1:18" ht="80">
       <c r="A246" s="20" t="str">
         <f t="shared" si="27"/>
         <v>T245</v>
@@ -21315,7 +21306,7 @@
       <c r="Q246" s="24"/>
       <c r="R246" s="24"/>
     </row>
-    <row r="247" spans="1:18" ht="32" hidden="1">
+    <row r="247" spans="1:18" ht="32">
       <c r="A247" s="20" t="str">
         <f t="shared" si="27"/>
         <v>T246</v>
@@ -21366,7 +21357,7 @@
       <c r="Q247" s="24"/>
       <c r="R247" s="24"/>
     </row>
-    <row r="248" spans="1:18" ht="32" hidden="1">
+    <row r="248" spans="1:18" ht="32">
       <c r="A248" s="20" t="str">
         <f t="shared" si="27"/>
         <v>T247</v>
@@ -21417,7 +21408,7 @@
       <c r="Q248" s="24"/>
       <c r="R248" s="24"/>
     </row>
-    <row r="249" spans="1:18" ht="80" hidden="1">
+    <row r="249" spans="1:18" ht="80">
       <c r="A249" s="20" t="str">
         <f t="shared" si="27"/>
         <v>T248</v>
@@ -21468,7 +21459,7 @@
       <c r="Q249" s="24"/>
       <c r="R249" s="24"/>
     </row>
-    <row r="250" spans="1:18" ht="64" hidden="1">
+    <row r="250" spans="1:18" ht="64">
       <c r="A250" s="20" t="str">
         <f t="shared" si="27"/>
         <v>T249</v>
@@ -21519,7 +21510,7 @@
       <c r="Q250" s="24"/>
       <c r="R250" s="24"/>
     </row>
-    <row r="251" spans="1:18" ht="64" hidden="1">
+    <row r="251" spans="1:18" ht="64">
       <c r="A251" s="20" t="str">
         <f t="shared" si="27"/>
         <v>T250</v>
@@ -21570,7 +21561,7 @@
       <c r="Q251" s="24"/>
       <c r="R251" s="24"/>
     </row>
-    <row r="252" spans="1:18" ht="96" hidden="1">
+    <row r="252" spans="1:18" ht="96">
       <c r="A252" s="20" t="str">
         <f t="shared" si="27"/>
         <v>T251</v>
@@ -21621,7 +21612,7 @@
       <c r="Q252" s="24"/>
       <c r="R252" s="24"/>
     </row>
-    <row r="253" spans="1:18" ht="48" hidden="1">
+    <row r="253" spans="1:18" ht="48">
       <c r="A253" s="20" t="str">
         <f t="shared" si="27"/>
         <v>T252</v>
@@ -21672,7 +21663,7 @@
       <c r="Q253" s="24"/>
       <c r="R253" s="24"/>
     </row>
-    <row r="254" spans="1:18" ht="80" hidden="1">
+    <row r="254" spans="1:18" ht="80">
       <c r="A254" s="20" t="str">
         <f t="shared" si="27"/>
         <v>T253</v>
@@ -21723,7 +21714,7 @@
       <c r="Q254" s="24"/>
       <c r="R254" s="24"/>
     </row>
-    <row r="255" spans="1:18" ht="16" hidden="1">
+    <row r="255" spans="1:18" ht="16">
       <c r="A255" s="20" t="str">
         <f t="shared" si="27"/>
         <v>T254</v>
@@ -21774,7 +21765,7 @@
       <c r="Q255" s="24"/>
       <c r="R255" s="24"/>
     </row>
-    <row r="256" spans="1:18" ht="32" hidden="1">
+    <row r="256" spans="1:18" ht="32">
       <c r="A256" s="20" t="str">
         <f t="shared" si="27"/>
         <v>T255</v>
@@ -21835,7 +21826,7 @@
       </c>
       <c r="R256" s="24"/>
     </row>
-    <row r="257" spans="1:18" ht="32" hidden="1">
+    <row r="257" spans="1:18" ht="32">
       <c r="A257" s="20" t="str">
         <f t="shared" si="27"/>
         <v>T256</v>
@@ -21896,7 +21887,7 @@
       </c>
       <c r="R257" s="24"/>
     </row>
-    <row r="258" spans="1:18" ht="32" hidden="1">
+    <row r="258" spans="1:18" ht="32">
       <c r="A258" s="20" t="str">
         <f t="shared" ref="A258:A299" si="38">CONCATENATE("T",ROW(A258)-1)</f>
         <v>T257</v>
@@ -21957,7 +21948,7 @@
       </c>
       <c r="R258" s="24"/>
     </row>
-    <row r="259" spans="1:18" ht="16" hidden="1">
+    <row r="259" spans="1:18" ht="16">
       <c r="A259" s="20" t="str">
         <f t="shared" si="38"/>
         <v>T258</v>
@@ -22018,7 +22009,7 @@
       </c>
       <c r="R259" s="24"/>
     </row>
-    <row r="260" spans="1:18" ht="240" hidden="1">
+    <row r="260" spans="1:18" ht="240">
       <c r="A260" s="20" t="str">
         <f t="shared" si="38"/>
         <v>T259</v>
@@ -22079,7 +22070,7 @@
       </c>
       <c r="R260" s="24"/>
     </row>
-    <row r="261" spans="1:18" ht="32" hidden="1">
+    <row r="261" spans="1:18" ht="32">
       <c r="A261" s="20" t="str">
         <f t="shared" si="38"/>
         <v>T260</v>
@@ -22140,7 +22131,7 @@
       </c>
       <c r="R261" s="24"/>
     </row>
-    <row r="262" spans="1:18" ht="16" hidden="1">
+    <row r="262" spans="1:18" ht="16">
       <c r="A262" s="20" t="str">
         <f t="shared" si="38"/>
         <v>T261</v>
@@ -22201,7 +22192,7 @@
       </c>
       <c r="R262" s="24"/>
     </row>
-    <row r="263" spans="1:18" ht="32" hidden="1">
+    <row r="263" spans="1:18" ht="32">
       <c r="A263" s="20" t="str">
         <f t="shared" si="38"/>
         <v>T262</v>
@@ -22258,7 +22249,7 @@
         <v>863</v>
       </c>
     </row>
-    <row r="264" spans="1:18" ht="32" hidden="1">
+    <row r="264" spans="1:18" ht="32">
       <c r="A264" s="20" t="str">
         <f t="shared" si="38"/>
         <v>T263</v>
@@ -22319,7 +22310,7 @@
       </c>
       <c r="R264" s="24"/>
     </row>
-    <row r="265" spans="1:18" ht="128" hidden="1">
+    <row r="265" spans="1:18" ht="128">
       <c r="A265" s="20" t="str">
         <f t="shared" si="38"/>
         <v>T264</v>
@@ -22380,7 +22371,7 @@
       </c>
       <c r="R265" s="24"/>
     </row>
-    <row r="266" spans="1:18" ht="64" hidden="1">
+    <row r="266" spans="1:18" ht="64">
       <c r="A266" s="20" t="str">
         <f t="shared" si="38"/>
         <v>T265</v>
@@ -22441,7 +22432,7 @@
       </c>
       <c r="R266" s="24"/>
     </row>
-    <row r="267" spans="1:18" ht="48" hidden="1">
+    <row r="267" spans="1:18" ht="48">
       <c r="A267" s="20" t="str">
         <f t="shared" si="38"/>
         <v>T266</v>
@@ -22502,7 +22493,7 @@
       </c>
       <c r="R267" s="24"/>
     </row>
-    <row r="268" spans="1:18" ht="32" hidden="1">
+    <row r="268" spans="1:18" ht="32">
       <c r="A268" s="20" t="str">
         <f t="shared" si="38"/>
         <v>T267</v>
@@ -22559,7 +22550,7 @@
         <v>863</v>
       </c>
     </row>
-    <row r="269" spans="1:18" ht="32" hidden="1">
+    <row r="269" spans="1:18" ht="32">
       <c r="A269" s="20" t="str">
         <f t="shared" si="38"/>
         <v>T268</v>
@@ -22620,7 +22611,7 @@
       </c>
       <c r="R269" s="24"/>
     </row>
-    <row r="270" spans="1:18" ht="32" hidden="1">
+    <row r="270" spans="1:18" ht="32">
       <c r="A270" s="20" t="str">
         <f t="shared" si="38"/>
         <v>T269</v>
@@ -22681,7 +22672,7 @@
       </c>
       <c r="R270" s="24"/>
     </row>
-    <row r="271" spans="1:18" ht="128" hidden="1">
+    <row r="271" spans="1:18" ht="128">
       <c r="A271" s="20" t="str">
         <f t="shared" si="38"/>
         <v>T270</v>
@@ -22742,7 +22733,7 @@
       </c>
       <c r="R271" s="24"/>
     </row>
-    <row r="272" spans="1:18" ht="32" hidden="1">
+    <row r="272" spans="1:18" ht="32">
       <c r="A272" s="20" t="str">
         <f t="shared" si="38"/>
         <v>T271</v>
@@ -22803,7 +22794,7 @@
       </c>
       <c r="R272" s="24"/>
     </row>
-    <row r="273" spans="1:18" ht="96" hidden="1">
+    <row r="273" spans="1:18" ht="96">
       <c r="A273" s="20" t="str">
         <f t="shared" si="38"/>
         <v>T272</v>
@@ -22864,7 +22855,7 @@
       </c>
       <c r="R273" s="24"/>
     </row>
-    <row r="274" spans="1:18" ht="64" hidden="1">
+    <row r="274" spans="1:18" ht="64">
       <c r="A274" s="20" t="str">
         <f t="shared" si="38"/>
         <v>T273</v>
@@ -22925,7 +22916,7 @@
       </c>
       <c r="R274" s="24"/>
     </row>
-    <row r="275" spans="1:18" ht="128" hidden="1">
+    <row r="275" spans="1:18" ht="128">
       <c r="A275" s="20" t="str">
         <f t="shared" si="38"/>
         <v>T274</v>
@@ -22986,7 +22977,7 @@
       </c>
       <c r="R275" s="24"/>
     </row>
-    <row r="276" spans="1:18" ht="96" hidden="1">
+    <row r="276" spans="1:18" ht="96">
       <c r="A276" s="20" t="str">
         <f t="shared" si="38"/>
         <v>T275</v>
@@ -23043,7 +23034,7 @@
       </c>
       <c r="R276" s="24"/>
     </row>
-    <row r="277" spans="1:18" ht="80" hidden="1">
+    <row r="277" spans="1:18" ht="80">
       <c r="A277" s="20" t="str">
         <f t="shared" si="38"/>
         <v>T276</v>
@@ -23100,7 +23091,7 @@
       </c>
       <c r="R277" s="24"/>
     </row>
-    <row r="278" spans="1:18" ht="64" hidden="1">
+    <row r="278" spans="1:18" ht="64">
       <c r="A278" s="20" t="str">
         <f t="shared" si="38"/>
         <v>T277</v>
@@ -23157,7 +23148,7 @@
       </c>
       <c r="R278" s="24"/>
     </row>
-    <row r="279" spans="1:18" ht="96" hidden="1">
+    <row r="279" spans="1:18" ht="96">
       <c r="A279" s="20" t="str">
         <f t="shared" si="38"/>
         <v>T278</v>
@@ -23218,7 +23209,7 @@
       </c>
       <c r="R279" s="24"/>
     </row>
-    <row r="280" spans="1:18" ht="32" hidden="1">
+    <row r="280" spans="1:18" ht="32">
       <c r="A280" s="20" t="str">
         <f t="shared" si="38"/>
         <v>T279</v>
@@ -23275,7 +23266,7 @@
         <v>863</v>
       </c>
     </row>
-    <row r="281" spans="1:18" ht="48" hidden="1">
+    <row r="281" spans="1:18" ht="48">
       <c r="A281" s="20" t="str">
         <f t="shared" si="38"/>
         <v>T280</v>
@@ -23336,7 +23327,7 @@
       </c>
       <c r="R281" s="24"/>
     </row>
-    <row r="282" spans="1:18" ht="48" hidden="1">
+    <row r="282" spans="1:18" ht="48">
       <c r="A282" s="20" t="str">
         <f t="shared" si="38"/>
         <v>T281</v>
@@ -23397,7 +23388,7 @@
       </c>
       <c r="R282" s="24"/>
     </row>
-    <row r="283" spans="1:18" ht="32" hidden="1">
+    <row r="283" spans="1:18" ht="32">
       <c r="A283" s="20" t="str">
         <f t="shared" si="38"/>
         <v>T282</v>
@@ -23458,7 +23449,7 @@
       </c>
       <c r="R283" s="24"/>
     </row>
-    <row r="284" spans="1:18" ht="80" hidden="1">
+    <row r="284" spans="1:18" ht="80">
       <c r="A284" s="20" t="str">
         <f t="shared" si="38"/>
         <v>T283</v>
@@ -23517,7 +23508,7 @@
       <c r="Q284" s="24"/>
       <c r="R284" s="24"/>
     </row>
-    <row r="285" spans="1:18" ht="160" hidden="1">
+    <row r="285" spans="1:18" ht="160">
       <c r="A285" s="20" t="str">
         <f t="shared" si="38"/>
         <v>T284</v>
@@ -23578,7 +23569,7 @@
       </c>
       <c r="R285" s="24"/>
     </row>
-    <row r="286" spans="1:18" ht="128" hidden="1">
+    <row r="286" spans="1:18" ht="128">
       <c r="A286" s="20" t="str">
         <f t="shared" si="38"/>
         <v>T285</v>
@@ -23639,7 +23630,7 @@
       </c>
       <c r="R286" s="24"/>
     </row>
-    <row r="287" spans="1:18" ht="48" hidden="1">
+    <row r="287" spans="1:18" ht="48">
       <c r="A287" s="20" t="str">
         <f t="shared" si="38"/>
         <v>T286</v>
@@ -23700,7 +23691,7 @@
       </c>
       <c r="R287" s="24"/>
     </row>
-    <row r="288" spans="1:18" ht="96" hidden="1">
+    <row r="288" spans="1:18" ht="96">
       <c r="A288" s="20" t="str">
         <f t="shared" si="38"/>
         <v>T287</v>
@@ -23761,7 +23752,7 @@
       </c>
       <c r="R288" s="24"/>
     </row>
-    <row r="289" spans="1:18" ht="96" hidden="1">
+    <row r="289" spans="1:18" ht="96">
       <c r="A289" s="20" t="str">
         <f t="shared" si="38"/>
         <v>T288</v>
@@ -23822,7 +23813,7 @@
       </c>
       <c r="R289" s="24"/>
     </row>
-    <row r="290" spans="1:18" ht="240" hidden="1">
+    <row r="290" spans="1:18" ht="240">
       <c r="A290" s="20" t="str">
         <f t="shared" si="38"/>
         <v>T289</v>
@@ -23883,7 +23874,7 @@
       </c>
       <c r="R290" s="24"/>
     </row>
-    <row r="291" spans="1:18" ht="96" hidden="1">
+    <row r="291" spans="1:18" ht="96">
       <c r="A291" s="20" t="str">
         <f t="shared" si="38"/>
         <v>T290</v>
@@ -23946,7 +23937,7 @@
         <v>866</v>
       </c>
     </row>
-    <row r="292" spans="1:18" ht="176" hidden="1">
+    <row r="292" spans="1:18" ht="176">
       <c r="A292" s="20" t="str">
         <f t="shared" si="38"/>
         <v>T291</v>
@@ -24007,7 +23998,7 @@
       </c>
       <c r="R292" s="24"/>
     </row>
-    <row r="293" spans="1:18" ht="380" hidden="1">
+    <row r="293" spans="1:18" ht="380">
       <c r="A293" s="20" t="str">
         <f t="shared" si="38"/>
         <v>T292</v>
@@ -24068,7 +24059,7 @@
       </c>
       <c r="R293" s="24"/>
     </row>
-    <row r="294" spans="1:18" ht="144" hidden="1">
+    <row r="294" spans="1:18" ht="144">
       <c r="A294" s="20" t="str">
         <f t="shared" si="38"/>
         <v>T293</v>
@@ -24129,7 +24120,7 @@
       </c>
       <c r="R294" s="24"/>
     </row>
-    <row r="295" spans="1:18" ht="112" hidden="1">
+    <row r="295" spans="1:18" ht="112">
       <c r="A295" s="20" t="str">
         <f t="shared" si="38"/>
         <v>T294</v>
@@ -24190,7 +24181,7 @@
       </c>
       <c r="R295" s="24"/>
     </row>
-    <row r="296" spans="1:18" ht="96" hidden="1">
+    <row r="296" spans="1:18" ht="96">
       <c r="A296" s="20" t="str">
         <f t="shared" si="38"/>
         <v>T295</v>
@@ -24251,7 +24242,7 @@
       </c>
       <c r="R296" s="24"/>
     </row>
-    <row r="297" spans="1:18" ht="32" hidden="1">
+    <row r="297" spans="1:18" ht="32">
       <c r="A297" s="20" t="str">
         <f t="shared" si="38"/>
         <v>T296</v>
@@ -24310,7 +24301,7 @@
       <c r="Q297" s="24"/>
       <c r="R297" s="24"/>
     </row>
-    <row r="298" spans="1:18" ht="32" hidden="1">
+    <row r="298" spans="1:18" ht="32">
       <c r="A298" s="20" t="str">
         <f t="shared" si="38"/>
         <v>T297</v>
@@ -24371,7 +24362,7 @@
       </c>
       <c r="R298" s="24"/>
     </row>
-    <row r="299" spans="1:18" ht="48" hidden="1">
+    <row r="299" spans="1:18" ht="48">
       <c r="A299" s="20" t="str">
         <f t="shared" si="38"/>
         <v>T298</v>
@@ -28867,7 +28858,7 @@
   <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="181" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -28892,7 +28883,7 @@
         <v>909</v>
       </c>
       <c r="D1" s="27" t="s">
-        <v>931</v>
+        <v>930</v>
       </c>
       <c r="E1" s="26" t="s">
         <v>911</v>
@@ -28946,16 +28937,16 @@
         <v>919</v>
       </c>
       <c r="C4" s="28" t="s">
-        <v>933</v>
+        <v>932</v>
       </c>
       <c r="D4" s="27" t="s">
-        <v>923</v>
+        <v>938</v>
       </c>
       <c r="E4" s="26" t="s">
         <v>920</v>
       </c>
       <c r="F4" s="27" t="s">
-        <v>936</v>
+        <v>935</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="32">
@@ -28967,17 +28958,17 @@
         <v>919</v>
       </c>
       <c r="C5" s="28" t="s">
+        <v>923</v>
+      </c>
+      <c r="D5" s="27" t="s">
         <v>924</v>
       </c>
-      <c r="D5" s="27" t="s">
+      <c r="E5" s="26" t="s">
         <v>925</v>
       </c>
-      <c r="E5" s="26" t="s">
-        <v>926</v>
-      </c>
     </row>
     <row r="6" spans="1:6" ht="32">
-      <c r="A6" s="33">
+      <c r="A6" s="26">
         <f>ROW(Tabella4[[#This Row],[Name]])-1</f>
         <v>5</v>
       </c>
@@ -28985,16 +28976,16 @@
         <v>919</v>
       </c>
       <c r="C6" s="28" t="s">
+        <v>936</v>
+      </c>
+      <c r="D6" s="27" t="s">
+        <v>938</v>
+      </c>
+      <c r="E6" s="26" t="s">
         <v>937</v>
       </c>
-      <c r="D6" s="27" t="s">
-        <v>923</v>
-      </c>
-      <c r="E6" s="26" t="s">
-        <v>938</v>
-      </c>
       <c r="F6" s="27" t="s">
-        <v>935</v>
+        <v>934</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="64">
@@ -29003,19 +28994,19 @@
         <v>6</v>
       </c>
       <c r="B7" s="26" t="s">
+        <v>926</v>
+      </c>
+      <c r="C7" s="28" t="s">
+        <v>933</v>
+      </c>
+      <c r="D7" s="27" t="s">
         <v>927</v>
       </c>
-      <c r="C7" s="28" t="s">
-        <v>934</v>
-      </c>
-      <c r="D7" s="27" t="s">
+      <c r="E7" s="26" t="s">
         <v>928</v>
       </c>
-      <c r="E7" s="26" t="s">
+      <c r="F7" s="27" t="s">
         <v>929</v>
-      </c>
-      <c r="F7" s="27" t="s">
-        <v>930</v>
       </c>
     </row>
   </sheetData>
@@ -29280,16 +29271,16 @@
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{83D5100D-0E56-4B30-B42D-2AEC6B837C39}">
   <ds:schemaRefs>
+    <ds:schemaRef ds:uri="633f040f-4953-46e7-8610-82b0c5296ba0"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="f62ef740-d444-4f18-80a2-7590fdcab1ce"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="633f040f-4953-46e7-8610-82b0c5296ba0"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="f62ef740-d444-4f18-80a2-7590fdcab1ce"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Aggiunta descrizione nella pagina del capec
</commit_message>
<xml_diff>
--- a/apps/static/assets/dbs/ThreatCatalogComplete.xlsx
+++ b/apps/static/assets/dbs/ThreatCatalogComplete.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10917"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11008"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fefox/Desktop/Web/apps/static/assets/dbs/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fefox/Desktop/WebApp/apps/static/assets/dbs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0FFBDA05-331F-5048-8D0E-97ABEB39D016}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{CA6BF5BF-2BD4-5743-88F4-F55666DFF250}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16380" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-38400" yWindow="-3100" windowWidth="38400" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Threat Components" sheetId="1" r:id="rId1"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4059" uniqueCount="939">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4059" uniqueCount="941">
   <si>
     <t>TID</t>
   </si>
@@ -2903,6 +2903,12 @@
   </si>
   <si>
     <t>match (net {type:'Network'})-[:connects]-&gt;(target) return target.component_id as component_id</t>
+  </si>
+  <si>
+    <t>Some of the services and functionalities of the VM are no more available</t>
+  </si>
+  <si>
+    <t>604</t>
   </si>
 </sst>
 </file>
@@ -3114,14 +3120,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -8348,7 +8354,23 @@
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{DEFAB213-4389-184E-911C-CDCC8CABBD38}" name="Tabella1" displayName="Tabella1" ref="A1:R299" totalsRowShown="0" dataDxfId="27">
-  <autoFilter ref="A1:R299" xr:uid="{DEFAB213-4389-184E-911C-CDCC8CABBD38}"/>
+  <autoFilter ref="A1:R299" xr:uid="{DEFAB213-4389-184E-911C-CDCC8CABBD38}">
+    <filterColumn colId="1">
+      <filters>
+        <filter val="HW.Chassis"/>
+        <filter val="HW.IOTDevice"/>
+        <filter val="HW.Server"/>
+        <filter val="HW.UE"/>
+        <filter val="Network"/>
+        <filter val="Network.WiFI"/>
+        <filter val="Service.5G.AUSF"/>
+        <filter val="Service.DB"/>
+        <filter val="Service.MQTTBroker"/>
+        <filter val="Service.VM"/>
+        <filter val="Service.Web"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:R299">
     <sortCondition ref="B1:B299"/>
   </sortState>
@@ -8679,9 +8701,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:R299"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A293" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="S107" sqref="S107"/>
+    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="115" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A107" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D191" sqref="D191"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -8761,7 +8783,7 @@
         <v>859</v>
       </c>
     </row>
-    <row r="2" spans="1:18" ht="48">
+    <row r="2" spans="1:18" ht="48" hidden="1">
       <c r="A2" s="20" t="str">
         <f t="shared" ref="A2:A65" si="0">CONCATENATE("T",ROW(A2)-1)</f>
         <v>T1</v>
@@ -8803,7 +8825,7 @@
       <c r="Q2" s="24"/>
       <c r="R2" s="24"/>
     </row>
-    <row r="3" spans="1:18" ht="32">
+    <row r="3" spans="1:18" ht="32" hidden="1">
       <c r="A3" s="20" t="str">
         <f t="shared" si="0"/>
         <v>T2</v>
@@ -8845,7 +8867,7 @@
       <c r="Q3" s="24"/>
       <c r="R3" s="24"/>
     </row>
-    <row r="4" spans="1:18" ht="80">
+    <row r="4" spans="1:18" ht="80" hidden="1">
       <c r="A4" s="20" t="str">
         <f t="shared" si="0"/>
         <v>T3</v>
@@ -8887,7 +8909,7 @@
       <c r="Q4" s="24"/>
       <c r="R4" s="24"/>
     </row>
-    <row r="5" spans="1:18" ht="32">
+    <row r="5" spans="1:18" ht="32" hidden="1">
       <c r="A5" s="20" t="str">
         <f t="shared" si="0"/>
         <v>T4</v>
@@ -8929,7 +8951,7 @@
       <c r="Q5" s="24"/>
       <c r="R5" s="24"/>
     </row>
-    <row r="6" spans="1:18" ht="48">
+    <row r="6" spans="1:18" ht="48" hidden="1">
       <c r="A6" s="20" t="str">
         <f t="shared" si="0"/>
         <v>T5</v>
@@ -8971,7 +8993,7 @@
       <c r="Q6" s="24"/>
       <c r="R6" s="24"/>
     </row>
-    <row r="7" spans="1:18" ht="48">
+    <row r="7" spans="1:18" ht="48" hidden="1">
       <c r="A7" s="20" t="str">
         <f t="shared" si="0"/>
         <v>T6</v>
@@ -9013,7 +9035,7 @@
       <c r="Q7" s="24"/>
       <c r="R7" s="24"/>
     </row>
-    <row r="8" spans="1:18" ht="48">
+    <row r="8" spans="1:18" ht="48" hidden="1">
       <c r="A8" s="20" t="str">
         <f t="shared" si="0"/>
         <v>T7</v>
@@ -9055,7 +9077,7 @@
       <c r="Q8" s="24"/>
       <c r="R8" s="24"/>
     </row>
-    <row r="9" spans="1:18" ht="16">
+    <row r="9" spans="1:18" ht="16" hidden="1">
       <c r="A9" s="20" t="str">
         <f t="shared" si="0"/>
         <v>T8</v>
@@ -9097,7 +9119,7 @@
       <c r="Q9" s="24"/>
       <c r="R9" s="24"/>
     </row>
-    <row r="10" spans="1:18" ht="32">
+    <row r="10" spans="1:18" ht="32" hidden="1">
       <c r="A10" s="20" t="str">
         <f t="shared" si="0"/>
         <v>T9</v>
@@ -9139,7 +9161,7 @@
       <c r="Q10" s="24"/>
       <c r="R10" s="24"/>
     </row>
-    <row r="11" spans="1:18" ht="32">
+    <row r="11" spans="1:18" ht="32" hidden="1">
       <c r="A11" s="20" t="str">
         <f t="shared" si="0"/>
         <v>T10</v>
@@ -9181,7 +9203,7 @@
       <c r="Q11" s="24"/>
       <c r="R11" s="24"/>
     </row>
-    <row r="12" spans="1:18" ht="48">
+    <row r="12" spans="1:18" ht="48" hidden="1">
       <c r="A12" s="20" t="str">
         <f t="shared" si="0"/>
         <v>T11</v>
@@ -9223,7 +9245,7 @@
       <c r="Q12" s="24"/>
       <c r="R12" s="24"/>
     </row>
-    <row r="13" spans="1:18" ht="48">
+    <row r="13" spans="1:18" ht="48" hidden="1">
       <c r="A13" s="20" t="str">
         <f t="shared" si="0"/>
         <v>T12</v>
@@ -9265,7 +9287,7 @@
       <c r="Q13" s="24"/>
       <c r="R13" s="24"/>
     </row>
-    <row r="14" spans="1:18" ht="64">
+    <row r="14" spans="1:18" ht="64" hidden="1">
       <c r="A14" s="20" t="str">
         <f t="shared" si="0"/>
         <v>T13</v>
@@ -9307,7 +9329,7 @@
       <c r="Q14" s="24"/>
       <c r="R14" s="24"/>
     </row>
-    <row r="15" spans="1:18" ht="48">
+    <row r="15" spans="1:18" ht="48" hidden="1">
       <c r="A15" s="20" t="str">
         <f t="shared" si="0"/>
         <v>T14</v>
@@ -9349,7 +9371,7 @@
       <c r="Q15" s="24"/>
       <c r="R15" s="24"/>
     </row>
-    <row r="16" spans="1:18" ht="80">
+    <row r="16" spans="1:18" ht="80" hidden="1">
       <c r="A16" s="20" t="str">
         <f t="shared" si="0"/>
         <v>T15</v>
@@ -9391,7 +9413,7 @@
       <c r="Q16" s="24"/>
       <c r="R16" s="24"/>
     </row>
-    <row r="17" spans="1:18" ht="32">
+    <row r="17" spans="1:18" ht="32" hidden="1">
       <c r="A17" s="20" t="str">
         <f t="shared" si="0"/>
         <v>T16</v>
@@ -9433,7 +9455,7 @@
       <c r="Q17" s="24"/>
       <c r="R17" s="24"/>
     </row>
-    <row r="18" spans="1:18" ht="32">
+    <row r="18" spans="1:18" ht="32" hidden="1">
       <c r="A18" s="20" t="str">
         <f t="shared" si="0"/>
         <v>T17</v>
@@ -9475,7 +9497,7 @@
       <c r="Q18" s="24"/>
       <c r="R18" s="24"/>
     </row>
-    <row r="19" spans="1:18" ht="48">
+    <row r="19" spans="1:18" ht="48" hidden="1">
       <c r="A19" s="20" t="str">
         <f t="shared" si="0"/>
         <v>T18</v>
@@ -9517,7 +9539,7 @@
       <c r="Q19" s="24"/>
       <c r="R19" s="24"/>
     </row>
-    <row r="20" spans="1:18" ht="32">
+    <row r="20" spans="1:18" ht="32" hidden="1">
       <c r="A20" s="20" t="str">
         <f t="shared" si="0"/>
         <v>T19</v>
@@ -9559,7 +9581,7 @@
       <c r="Q20" s="24"/>
       <c r="R20" s="24"/>
     </row>
-    <row r="21" spans="1:18" ht="48">
+    <row r="21" spans="1:18" ht="48" hidden="1">
       <c r="A21" s="20" t="str">
         <f t="shared" si="0"/>
         <v>T20</v>
@@ -9601,7 +9623,7 @@
       <c r="Q21" s="24"/>
       <c r="R21" s="24"/>
     </row>
-    <row r="22" spans="1:18" ht="48">
+    <row r="22" spans="1:18" ht="48" hidden="1">
       <c r="A22" s="20" t="str">
         <f t="shared" si="0"/>
         <v>T21</v>
@@ -9643,7 +9665,7 @@
       <c r="Q22" s="24"/>
       <c r="R22" s="24"/>
     </row>
-    <row r="23" spans="1:18" ht="48">
+    <row r="23" spans="1:18" ht="48" hidden="1">
       <c r="A23" s="20" t="str">
         <f t="shared" si="0"/>
         <v>T22</v>
@@ -9685,7 +9707,7 @@
       <c r="Q23" s="24"/>
       <c r="R23" s="24"/>
     </row>
-    <row r="24" spans="1:18" ht="48">
+    <row r="24" spans="1:18" ht="48" hidden="1">
       <c r="A24" s="20" t="str">
         <f t="shared" si="0"/>
         <v>T23</v>
@@ -11133,7 +11155,7 @@
       <c r="Q52" s="24"/>
       <c r="R52" s="24"/>
     </row>
-    <row r="53" spans="1:18" ht="32">
+    <row r="53" spans="1:18" ht="32" hidden="1">
       <c r="A53" s="20" t="str">
         <f t="shared" si="0"/>
         <v>T52</v>
@@ -11183,7 +11205,7 @@
       <c r="Q53" s="24"/>
       <c r="R53" s="24"/>
     </row>
-    <row r="54" spans="1:18" ht="48">
+    <row r="54" spans="1:18" ht="48" hidden="1">
       <c r="A54" s="20" t="str">
         <f t="shared" si="0"/>
         <v>T53</v>
@@ -11233,7 +11255,7 @@
       <c r="Q54" s="24"/>
       <c r="R54" s="24"/>
     </row>
-    <row r="55" spans="1:18" ht="32">
+    <row r="55" spans="1:18" ht="32" hidden="1">
       <c r="A55" s="20" t="str">
         <f t="shared" si="0"/>
         <v>T54</v>
@@ -11283,7 +11305,7 @@
       <c r="Q55" s="24"/>
       <c r="R55" s="24"/>
     </row>
-    <row r="56" spans="1:18" ht="48">
+    <row r="56" spans="1:18" ht="48" hidden="1">
       <c r="A56" s="20" t="str">
         <f t="shared" si="0"/>
         <v>T55</v>
@@ -11333,7 +11355,7 @@
       <c r="Q56" s="24"/>
       <c r="R56" s="24"/>
     </row>
-    <row r="57" spans="1:18" ht="32">
+    <row r="57" spans="1:18" ht="32" hidden="1">
       <c r="A57" s="20" t="str">
         <f t="shared" si="0"/>
         <v>T56</v>
@@ -11383,7 +11405,7 @@
       <c r="Q57" s="24"/>
       <c r="R57" s="24"/>
     </row>
-    <row r="58" spans="1:18" ht="80">
+    <row r="58" spans="1:18" ht="80" hidden="1">
       <c r="A58" s="20" t="str">
         <f t="shared" si="0"/>
         <v>T57</v>
@@ -11433,7 +11455,7 @@
       <c r="Q58" s="24"/>
       <c r="R58" s="24"/>
     </row>
-    <row r="59" spans="1:18" ht="32">
+    <row r="59" spans="1:18" ht="32" hidden="1">
       <c r="A59" s="20" t="str">
         <f t="shared" si="0"/>
         <v>T58</v>
@@ -11483,7 +11505,7 @@
       <c r="Q59" s="24"/>
       <c r="R59" s="24"/>
     </row>
-    <row r="60" spans="1:18" ht="32">
+    <row r="60" spans="1:18" ht="32" hidden="1">
       <c r="A60" s="20" t="str">
         <f t="shared" si="0"/>
         <v>T59</v>
@@ -12637,7 +12659,7 @@
         <v>414</v>
       </c>
       <c r="D79" s="20" t="s">
-        <v>558</v>
+        <v>939</v>
       </c>
       <c r="E79" s="20" t="s">
         <v>274</v>
@@ -14435,7 +14457,7 @@
       <c r="Q111" s="24"/>
       <c r="R111" s="24"/>
     </row>
-    <row r="112" spans="1:18" ht="48">
+    <row r="112" spans="1:18" ht="48" hidden="1">
       <c r="A112" s="20" t="str">
         <f t="shared" si="11"/>
         <v>T111</v>
@@ -14486,7 +14508,7 @@
       <c r="Q112" s="24"/>
       <c r="R112" s="24"/>
     </row>
-    <row r="113" spans="1:18" ht="80">
+    <row r="113" spans="1:18" ht="80" hidden="1">
       <c r="A113" s="20" t="str">
         <f t="shared" si="11"/>
         <v>T112</v>
@@ -14537,7 +14559,7 @@
       <c r="Q113" s="24"/>
       <c r="R113" s="24"/>
     </row>
-    <row r="114" spans="1:18" ht="64">
+    <row r="114" spans="1:18" ht="64" hidden="1">
       <c r="A114" s="20" t="str">
         <f t="shared" si="11"/>
         <v>T113</v>
@@ -14588,7 +14610,7 @@
       <c r="Q114" s="24"/>
       <c r="R114" s="24"/>
     </row>
-    <row r="115" spans="1:18" ht="48">
+    <row r="115" spans="1:18" ht="48" hidden="1">
       <c r="A115" s="20" t="str">
         <f t="shared" si="11"/>
         <v>T114</v>
@@ -14639,7 +14661,7 @@
       <c r="Q115" s="24"/>
       <c r="R115" s="24"/>
     </row>
-    <row r="116" spans="1:18" ht="48">
+    <row r="116" spans="1:18" ht="48" hidden="1">
       <c r="A116" s="20" t="str">
         <f t="shared" si="11"/>
         <v>T115</v>
@@ -14690,7 +14712,7 @@
       <c r="Q116" s="24"/>
       <c r="R116" s="24"/>
     </row>
-    <row r="117" spans="1:18" ht="16">
+    <row r="117" spans="1:18" ht="16" hidden="1">
       <c r="A117" s="20" t="str">
         <f t="shared" si="11"/>
         <v>T116</v>
@@ -14741,7 +14763,7 @@
       <c r="Q117" s="24"/>
       <c r="R117" s="24"/>
     </row>
-    <row r="118" spans="1:18" ht="16">
+    <row r="118" spans="1:18" ht="16" hidden="1">
       <c r="A118" s="20" t="str">
         <f t="shared" si="11"/>
         <v>T117</v>
@@ -14792,7 +14814,7 @@
       <c r="Q118" s="24"/>
       <c r="R118" s="24"/>
     </row>
-    <row r="119" spans="1:18" ht="48">
+    <row r="119" spans="1:18" ht="48" hidden="1">
       <c r="A119" s="20" t="str">
         <f t="shared" si="11"/>
         <v>T118</v>
@@ -14843,7 +14865,7 @@
       <c r="Q119" s="24"/>
       <c r="R119" s="24"/>
     </row>
-    <row r="120" spans="1:18" ht="96">
+    <row r="120" spans="1:18" ht="96" hidden="1">
       <c r="A120" s="20" t="str">
         <f t="shared" si="11"/>
         <v>T119</v>
@@ -14894,7 +14916,7 @@
       <c r="Q120" s="24"/>
       <c r="R120" s="24"/>
     </row>
-    <row r="121" spans="1:18" ht="64">
+    <row r="121" spans="1:18" ht="64" hidden="1">
       <c r="A121" s="20" t="str">
         <f t="shared" si="11"/>
         <v>T120</v>
@@ -14945,7 +14967,7 @@
       <c r="Q121" s="24"/>
       <c r="R121" s="24"/>
     </row>
-    <row r="122" spans="1:18" ht="48">
+    <row r="122" spans="1:18" ht="48" hidden="1">
       <c r="A122" s="20" t="str">
         <f t="shared" si="11"/>
         <v>T121</v>
@@ -14996,7 +15018,7 @@
       <c r="Q122" s="24"/>
       <c r="R122" s="24"/>
     </row>
-    <row r="123" spans="1:18" ht="48">
+    <row r="123" spans="1:18" ht="48" hidden="1">
       <c r="A123" s="20" t="str">
         <f t="shared" si="11"/>
         <v>T122</v>
@@ -15047,7 +15069,7 @@
       <c r="Q123" s="24"/>
       <c r="R123" s="24"/>
     </row>
-    <row r="124" spans="1:18" ht="16">
+    <row r="124" spans="1:18" ht="16" hidden="1">
       <c r="A124" s="20" t="str">
         <f t="shared" si="11"/>
         <v>T123</v>
@@ -15098,7 +15120,7 @@
       <c r="Q124" s="24"/>
       <c r="R124" s="24"/>
     </row>
-    <row r="125" spans="1:18" ht="32">
+    <row r="125" spans="1:18" ht="32" hidden="1">
       <c r="A125" s="20" t="str">
         <f t="shared" si="11"/>
         <v>T124</v>
@@ -15149,7 +15171,7 @@
       <c r="Q125" s="24"/>
       <c r="R125" s="24"/>
     </row>
-    <row r="126" spans="1:18" ht="16">
+    <row r="126" spans="1:18" ht="16" hidden="1">
       <c r="A126" s="20" t="str">
         <f t="shared" si="11"/>
         <v>T125</v>
@@ -15200,7 +15222,7 @@
       <c r="Q126" s="24"/>
       <c r="R126" s="24"/>
     </row>
-    <row r="127" spans="1:18" ht="64">
+    <row r="127" spans="1:18" ht="64" hidden="1">
       <c r="A127" s="20" t="str">
         <f t="shared" si="11"/>
         <v>T126</v>
@@ -15251,7 +15273,7 @@
       <c r="Q127" s="24"/>
       <c r="R127" s="24"/>
     </row>
-    <row r="128" spans="1:18" ht="48">
+    <row r="128" spans="1:18" ht="48" hidden="1">
       <c r="A128" s="20" t="str">
         <f t="shared" si="11"/>
         <v>T127</v>
@@ -15290,7 +15312,7 @@
       <c r="Q128" s="24"/>
       <c r="R128" s="24"/>
     </row>
-    <row r="129" spans="1:18" ht="96">
+    <row r="129" spans="1:18" ht="96" hidden="1">
       <c r="A129" s="20" t="str">
         <f t="shared" si="11"/>
         <v>T128</v>
@@ -15329,7 +15351,7 @@
       <c r="Q129" s="24"/>
       <c r="R129" s="24"/>
     </row>
-    <row r="130" spans="1:18" ht="32">
+    <row r="130" spans="1:18" ht="32" hidden="1">
       <c r="A130" s="20" t="str">
         <f t="shared" ref="A130:A193" si="22">CONCATENATE("T",ROW(A130)-1)</f>
         <v>T129</v>
@@ -15380,7 +15402,7 @@
       <c r="Q130" s="24"/>
       <c r="R130" s="24"/>
     </row>
-    <row r="131" spans="1:18" ht="64">
+    <row r="131" spans="1:18" ht="64" hidden="1">
       <c r="A131" s="20" t="str">
         <f t="shared" si="22"/>
         <v>T130</v>
@@ -15431,7 +15453,7 @@
       <c r="Q131" s="24"/>
       <c r="R131" s="24"/>
     </row>
-    <row r="132" spans="1:18" ht="48">
+    <row r="132" spans="1:18" ht="48" hidden="1">
       <c r="A132" s="20" t="str">
         <f t="shared" si="22"/>
         <v>T131</v>
@@ -15482,7 +15504,7 @@
       <c r="Q132" s="24"/>
       <c r="R132" s="24"/>
     </row>
-    <row r="133" spans="1:18" ht="32">
+    <row r="133" spans="1:18" ht="32" hidden="1">
       <c r="A133" s="20" t="str">
         <f t="shared" si="22"/>
         <v>T132</v>
@@ -15533,7 +15555,7 @@
       <c r="Q133" s="24"/>
       <c r="R133" s="24"/>
     </row>
-    <row r="134" spans="1:18" ht="48">
+    <row r="134" spans="1:18" ht="48" hidden="1">
       <c r="A134" s="20" t="str">
         <f t="shared" si="22"/>
         <v>T133</v>
@@ -15584,7 +15606,7 @@
       <c r="Q134" s="24"/>
       <c r="R134" s="24"/>
     </row>
-    <row r="135" spans="1:18" ht="48">
+    <row r="135" spans="1:18" ht="48" hidden="1">
       <c r="A135" s="20" t="str">
         <f t="shared" si="22"/>
         <v>T134</v>
@@ -15635,7 +15657,7 @@
       <c r="Q135" s="24"/>
       <c r="R135" s="24"/>
     </row>
-    <row r="136" spans="1:18" ht="64">
+    <row r="136" spans="1:18" ht="64" hidden="1">
       <c r="A136" s="20" t="str">
         <f t="shared" si="22"/>
         <v>T135</v>
@@ -15743,11 +15765,11 @@
         <v>856</v>
       </c>
       <c r="Q137" s="25" t="s">
-        <v>855</v>
+        <v>940</v>
       </c>
       <c r="R137" s="25"/>
     </row>
-    <row r="138" spans="1:18" ht="96">
+    <row r="138" spans="1:18" ht="96" hidden="1">
       <c r="A138" s="20" t="str">
         <f t="shared" si="22"/>
         <v>T137</v>
@@ -15798,7 +15820,7 @@
       <c r="Q138" s="24"/>
       <c r="R138" s="24"/>
     </row>
-    <row r="139" spans="1:18" ht="80">
+    <row r="139" spans="1:18" ht="80" hidden="1">
       <c r="A139" s="20" t="str">
         <f t="shared" si="22"/>
         <v>T138</v>
@@ -15849,7 +15871,7 @@
       <c r="Q139" s="24"/>
       <c r="R139" s="24"/>
     </row>
-    <row r="140" spans="1:18" ht="96">
+    <row r="140" spans="1:18" ht="96" hidden="1">
       <c r="A140" s="20" t="str">
         <f t="shared" si="22"/>
         <v>T139</v>
@@ -15900,7 +15922,7 @@
       <c r="Q140" s="24"/>
       <c r="R140" s="24"/>
     </row>
-    <row r="141" spans="1:18" ht="48">
+    <row r="141" spans="1:18" ht="48" hidden="1">
       <c r="A141" s="20" t="str">
         <f t="shared" si="22"/>
         <v>T140</v>
@@ -15951,7 +15973,7 @@
       <c r="Q141" s="24"/>
       <c r="R141" s="24"/>
     </row>
-    <row r="142" spans="1:18" ht="80">
+    <row r="142" spans="1:18" ht="80" hidden="1">
       <c r="A142" s="20" t="str">
         <f t="shared" si="22"/>
         <v>T141</v>
@@ -16002,7 +16024,7 @@
       <c r="Q142" s="24"/>
       <c r="R142" s="24"/>
     </row>
-    <row r="143" spans="1:18" ht="48">
+    <row r="143" spans="1:18" ht="48" hidden="1">
       <c r="A143" s="20" t="str">
         <f t="shared" si="22"/>
         <v>T142</v>
@@ -16053,7 +16075,7 @@
       <c r="Q143" s="24"/>
       <c r="R143" s="24"/>
     </row>
-    <row r="144" spans="1:18" ht="32">
+    <row r="144" spans="1:18" ht="32" hidden="1">
       <c r="A144" s="20" t="str">
         <f t="shared" si="22"/>
         <v>T143</v>
@@ -16104,7 +16126,7 @@
       <c r="Q144" s="24"/>
       <c r="R144" s="24"/>
     </row>
-    <row r="145" spans="1:18" ht="32">
+    <row r="145" spans="1:18" ht="32" hidden="1">
       <c r="A145" s="20" t="str">
         <f t="shared" si="22"/>
         <v>T144</v>
@@ -16155,7 +16177,7 @@
       <c r="Q145" s="24"/>
       <c r="R145" s="24"/>
     </row>
-    <row r="146" spans="1:18" ht="80">
+    <row r="146" spans="1:18" ht="80" hidden="1">
       <c r="A146" s="20" t="str">
         <f t="shared" si="22"/>
         <v>T145</v>
@@ -16206,7 +16228,7 @@
       <c r="Q146" s="24"/>
       <c r="R146" s="24"/>
     </row>
-    <row r="147" spans="1:18" ht="64">
+    <row r="147" spans="1:18" ht="64" hidden="1">
       <c r="A147" s="20" t="str">
         <f t="shared" si="22"/>
         <v>T146</v>
@@ -16257,7 +16279,7 @@
       <c r="Q147" s="24"/>
       <c r="R147" s="24"/>
     </row>
-    <row r="148" spans="1:18" ht="64">
+    <row r="148" spans="1:18" ht="64" hidden="1">
       <c r="A148" s="20" t="str">
         <f t="shared" si="22"/>
         <v>T147</v>
@@ -16308,7 +16330,7 @@
       <c r="Q148" s="24"/>
       <c r="R148" s="24"/>
     </row>
-    <row r="149" spans="1:18" ht="32">
+    <row r="149" spans="1:18" ht="32" hidden="1">
       <c r="A149" s="20" t="str">
         <f t="shared" si="22"/>
         <v>T148</v>
@@ -16359,7 +16381,7 @@
       <c r="Q149" s="24"/>
       <c r="R149" s="24"/>
     </row>
-    <row r="150" spans="1:18" ht="64">
+    <row r="150" spans="1:18" ht="64" hidden="1">
       <c r="A150" s="20" t="str">
         <f t="shared" si="22"/>
         <v>T149</v>
@@ -16410,7 +16432,7 @@
       <c r="Q150" s="24"/>
       <c r="R150" s="24"/>
     </row>
-    <row r="151" spans="1:18" ht="112">
+    <row r="151" spans="1:18" ht="112" hidden="1">
       <c r="A151" s="20" t="str">
         <f t="shared" si="22"/>
         <v>T150</v>
@@ -16461,7 +16483,7 @@
       <c r="Q151" s="24"/>
       <c r="R151" s="24"/>
     </row>
-    <row r="152" spans="1:18" ht="64">
+    <row r="152" spans="1:18" ht="64" hidden="1">
       <c r="A152" s="20" t="str">
         <f t="shared" si="22"/>
         <v>T151</v>
@@ -16512,7 +16534,7 @@
       <c r="Q152" s="24"/>
       <c r="R152" s="24"/>
     </row>
-    <row r="153" spans="1:18" ht="96">
+    <row r="153" spans="1:18" ht="96" hidden="1">
       <c r="A153" s="20" t="str">
         <f t="shared" si="22"/>
         <v>T152</v>
@@ -16563,7 +16585,7 @@
       <c r="Q153" s="24"/>
       <c r="R153" s="24"/>
     </row>
-    <row r="154" spans="1:18" ht="160">
+    <row r="154" spans="1:18" ht="160" hidden="1">
       <c r="A154" s="20" t="str">
         <f t="shared" si="22"/>
         <v>T153</v>
@@ -16614,7 +16636,7 @@
       <c r="Q154" s="24"/>
       <c r="R154" s="24"/>
     </row>
-    <row r="155" spans="1:18" ht="96">
+    <row r="155" spans="1:18" ht="96" hidden="1">
       <c r="A155" s="20" t="str">
         <f t="shared" si="22"/>
         <v>T154</v>
@@ -16665,7 +16687,7 @@
       <c r="Q155" s="24"/>
       <c r="R155" s="24"/>
     </row>
-    <row r="156" spans="1:18" ht="80">
+    <row r="156" spans="1:18" ht="80" hidden="1">
       <c r="A156" s="20" t="str">
         <f t="shared" si="22"/>
         <v>T155</v>
@@ -16716,7 +16738,7 @@
       <c r="Q156" s="24"/>
       <c r="R156" s="24"/>
     </row>
-    <row r="157" spans="1:18" ht="96">
+    <row r="157" spans="1:18" ht="96" hidden="1">
       <c r="A157" s="20" t="str">
         <f t="shared" si="22"/>
         <v>T156</v>
@@ -16767,7 +16789,7 @@
       <c r="Q157" s="24"/>
       <c r="R157" s="24"/>
     </row>
-    <row r="158" spans="1:18" ht="48">
+    <row r="158" spans="1:18" ht="48" hidden="1">
       <c r="A158" s="20" t="str">
         <f t="shared" si="22"/>
         <v>T157</v>
@@ -16818,7 +16840,7 @@
       <c r="Q158" s="24"/>
       <c r="R158" s="24"/>
     </row>
-    <row r="159" spans="1:18" ht="32">
+    <row r="159" spans="1:18" ht="32" hidden="1">
       <c r="A159" s="20" t="str">
         <f t="shared" si="22"/>
         <v>T158</v>
@@ -16869,7 +16891,7 @@
       <c r="Q159" s="24"/>
       <c r="R159" s="24"/>
     </row>
-    <row r="160" spans="1:18" ht="80">
+    <row r="160" spans="1:18" ht="80" hidden="1">
       <c r="A160" s="20" t="str">
         <f t="shared" si="22"/>
         <v>T159</v>
@@ -16920,7 +16942,7 @@
       <c r="Q160" s="24"/>
       <c r="R160" s="24"/>
     </row>
-    <row r="161" spans="1:18" ht="80">
+    <row r="161" spans="1:18" ht="80" hidden="1">
       <c r="A161" s="20" t="str">
         <f t="shared" si="22"/>
         <v>T160</v>
@@ -16971,7 +16993,7 @@
       <c r="Q161" s="24"/>
       <c r="R161" s="24"/>
     </row>
-    <row r="162" spans="1:18" ht="64">
+    <row r="162" spans="1:18" ht="64" hidden="1">
       <c r="A162" s="20" t="str">
         <f t="shared" si="22"/>
         <v>T161</v>
@@ -17022,7 +17044,7 @@
       <c r="Q162" s="24"/>
       <c r="R162" s="24"/>
     </row>
-    <row r="163" spans="1:18" ht="64">
+    <row r="163" spans="1:18" ht="64" hidden="1">
       <c r="A163" s="20" t="str">
         <f t="shared" si="22"/>
         <v>T162</v>
@@ -17073,7 +17095,7 @@
       <c r="Q163" s="24"/>
       <c r="R163" s="24"/>
     </row>
-    <row r="164" spans="1:18" ht="48">
+    <row r="164" spans="1:18" ht="48" hidden="1">
       <c r="A164" s="20" t="str">
         <f t="shared" si="22"/>
         <v>T163</v>
@@ -17124,7 +17146,7 @@
       <c r="Q164" s="24"/>
       <c r="R164" s="24"/>
     </row>
-    <row r="165" spans="1:18" ht="32">
+    <row r="165" spans="1:18" ht="32" hidden="1">
       <c r="A165" s="20" t="str">
         <f t="shared" si="22"/>
         <v>T164</v>
@@ -17175,7 +17197,7 @@
       <c r="Q165" s="24"/>
       <c r="R165" s="24"/>
     </row>
-    <row r="166" spans="1:18" ht="32">
+    <row r="166" spans="1:18" ht="32" hidden="1">
       <c r="A166" s="20" t="str">
         <f t="shared" si="22"/>
         <v>T165</v>
@@ -17226,7 +17248,7 @@
       <c r="Q166" s="24"/>
       <c r="R166" s="24"/>
     </row>
-    <row r="167" spans="1:18" ht="32">
+    <row r="167" spans="1:18" ht="32" hidden="1">
       <c r="A167" s="20" t="str">
         <f t="shared" si="22"/>
         <v>T166</v>
@@ -17277,7 +17299,7 @@
       <c r="Q167" s="24"/>
       <c r="R167" s="24"/>
     </row>
-    <row r="168" spans="1:18" ht="32">
+    <row r="168" spans="1:18" ht="32" hidden="1">
       <c r="A168" s="20" t="str">
         <f t="shared" si="22"/>
         <v>T167</v>
@@ -17328,7 +17350,7 @@
       <c r="Q168" s="24"/>
       <c r="R168" s="24"/>
     </row>
-    <row r="169" spans="1:18" ht="64">
+    <row r="169" spans="1:18" ht="64" hidden="1">
       <c r="A169" s="20" t="str">
         <f t="shared" si="22"/>
         <v>T168</v>
@@ -17379,7 +17401,7 @@
       <c r="Q169" s="24"/>
       <c r="R169" s="24"/>
     </row>
-    <row r="170" spans="1:18" ht="48">
+    <row r="170" spans="1:18" ht="48" hidden="1">
       <c r="A170" s="20" t="str">
         <f t="shared" si="22"/>
         <v>T169</v>
@@ -17430,7 +17452,7 @@
       <c r="Q170" s="24"/>
       <c r="R170" s="24"/>
     </row>
-    <row r="171" spans="1:18" ht="32">
+    <row r="171" spans="1:18" ht="32" hidden="1">
       <c r="A171" s="20" t="str">
         <f t="shared" si="22"/>
         <v>T170</v>
@@ -17481,7 +17503,7 @@
       <c r="Q171" s="24"/>
       <c r="R171" s="24"/>
     </row>
-    <row r="172" spans="1:18" ht="32">
+    <row r="172" spans="1:18" ht="32" hidden="1">
       <c r="A172" s="20" t="str">
         <f t="shared" si="22"/>
         <v>T171</v>
@@ -17532,7 +17554,7 @@
       <c r="Q172" s="24"/>
       <c r="R172" s="24"/>
     </row>
-    <row r="173" spans="1:18" ht="16">
+    <row r="173" spans="1:18" ht="16" hidden="1">
       <c r="A173" s="20" t="str">
         <f t="shared" si="22"/>
         <v>T172</v>
@@ -17583,7 +17605,7 @@
       <c r="Q173" s="24"/>
       <c r="R173" s="24"/>
     </row>
-    <row r="174" spans="1:18" ht="16">
+    <row r="174" spans="1:18" ht="16" hidden="1">
       <c r="A174" s="20" t="str">
         <f t="shared" si="22"/>
         <v>T173</v>
@@ -17634,7 +17656,7 @@
       <c r="Q174" s="24"/>
       <c r="R174" s="24"/>
     </row>
-    <row r="175" spans="1:18" ht="64">
+    <row r="175" spans="1:18" ht="64" hidden="1">
       <c r="A175" s="20" t="str">
         <f t="shared" si="22"/>
         <v>T174</v>
@@ -17685,7 +17707,7 @@
       <c r="Q175" s="24"/>
       <c r="R175" s="24"/>
     </row>
-    <row r="176" spans="1:18" ht="64">
+    <row r="176" spans="1:18" ht="64" hidden="1">
       <c r="A176" s="20" t="str">
         <f t="shared" si="22"/>
         <v>T175</v>
@@ -17736,7 +17758,7 @@
       <c r="Q176" s="24"/>
       <c r="R176" s="24"/>
     </row>
-    <row r="177" spans="1:18" ht="80">
+    <row r="177" spans="1:18" ht="80" hidden="1">
       <c r="A177" s="20" t="str">
         <f t="shared" si="22"/>
         <v>T176</v>
@@ -17787,7 +17809,7 @@
       <c r="Q177" s="24"/>
       <c r="R177" s="24"/>
     </row>
-    <row r="178" spans="1:18" ht="48">
+    <row r="178" spans="1:18" ht="48" hidden="1">
       <c r="A178" s="20" t="str">
         <f t="shared" si="22"/>
         <v>T177</v>
@@ -17838,7 +17860,7 @@
       <c r="Q178" s="24"/>
       <c r="R178" s="24"/>
     </row>
-    <row r="179" spans="1:18" ht="32">
+    <row r="179" spans="1:18" ht="32" hidden="1">
       <c r="A179" s="20" t="str">
         <f t="shared" si="22"/>
         <v>T178</v>
@@ -17889,7 +17911,7 @@
       <c r="Q179" s="24"/>
       <c r="R179" s="24"/>
     </row>
-    <row r="180" spans="1:18" ht="32">
+    <row r="180" spans="1:18" ht="32" hidden="1">
       <c r="A180" s="20" t="str">
         <f t="shared" si="22"/>
         <v>T179</v>
@@ -17940,7 +17962,7 @@
       <c r="Q180" s="24"/>
       <c r="R180" s="24"/>
     </row>
-    <row r="181" spans="1:18" ht="80">
+    <row r="181" spans="1:18" ht="80" hidden="1">
       <c r="A181" s="20" t="str">
         <f t="shared" si="22"/>
         <v>T180</v>
@@ -17991,7 +18013,7 @@
       <c r="Q181" s="24"/>
       <c r="R181" s="24"/>
     </row>
-    <row r="182" spans="1:18" ht="64">
+    <row r="182" spans="1:18" ht="64" hidden="1">
       <c r="A182" s="20" t="str">
         <f t="shared" si="22"/>
         <v>T181</v>
@@ -18042,7 +18064,7 @@
       <c r="Q182" s="24"/>
       <c r="R182" s="24"/>
     </row>
-    <row r="183" spans="1:18" ht="64">
+    <row r="183" spans="1:18" ht="64" hidden="1">
       <c r="A183" s="20" t="str">
         <f t="shared" si="22"/>
         <v>T182</v>
@@ -18093,7 +18115,7 @@
       <c r="Q183" s="24"/>
       <c r="R183" s="24"/>
     </row>
-    <row r="184" spans="1:18" ht="144">
+    <row r="184" spans="1:18" ht="144" hidden="1">
       <c r="A184" s="20" t="str">
         <f t="shared" si="22"/>
         <v>T183</v>
@@ -18144,7 +18166,7 @@
       <c r="Q184" s="24"/>
       <c r="R184" s="24"/>
     </row>
-    <row r="185" spans="1:18" ht="96">
+    <row r="185" spans="1:18" ht="96" hidden="1">
       <c r="A185" s="20" t="str">
         <f t="shared" si="22"/>
         <v>T184</v>
@@ -18195,7 +18217,7 @@
       <c r="Q185" s="24"/>
       <c r="R185" s="24"/>
     </row>
-    <row r="186" spans="1:18" ht="48">
+    <row r="186" spans="1:18" ht="48" hidden="1">
       <c r="A186" s="20" t="str">
         <f t="shared" si="22"/>
         <v>T185</v>
@@ -18246,7 +18268,7 @@
       <c r="Q186" s="24"/>
       <c r="R186" s="24"/>
     </row>
-    <row r="187" spans="1:18" ht="16">
+    <row r="187" spans="1:18" ht="16" hidden="1">
       <c r="A187" s="20" t="str">
         <f t="shared" si="22"/>
         <v>T186</v>
@@ -18297,7 +18319,7 @@
       <c r="Q187" s="24"/>
       <c r="R187" s="24"/>
     </row>
-    <row r="188" spans="1:18" ht="144">
+    <row r="188" spans="1:18" ht="144" hidden="1">
       <c r="A188" s="20" t="str">
         <f t="shared" si="22"/>
         <v>T187</v>
@@ -18348,7 +18370,7 @@
       <c r="Q188" s="24"/>
       <c r="R188" s="24"/>
     </row>
-    <row r="189" spans="1:18" ht="128">
+    <row r="189" spans="1:18" ht="128" hidden="1">
       <c r="A189" s="20" t="str">
         <f t="shared" si="22"/>
         <v>T188</v>
@@ -18399,7 +18421,7 @@
       <c r="Q189" s="24"/>
       <c r="R189" s="24"/>
     </row>
-    <row r="190" spans="1:18" ht="128">
+    <row r="190" spans="1:18" ht="128" hidden="1">
       <c r="A190" s="20" t="str">
         <f t="shared" si="22"/>
         <v>T189</v>
@@ -18705,7 +18727,7 @@
       <c r="Q195" s="24"/>
       <c r="R195" s="24"/>
     </row>
-    <row r="196" spans="1:18" ht="80">
+    <row r="196" spans="1:18" ht="80" hidden="1">
       <c r="A196" s="20" t="str">
         <f t="shared" si="27"/>
         <v>T195</v>
@@ -18756,7 +18778,7 @@
       <c r="Q196" s="24"/>
       <c r="R196" s="24"/>
     </row>
-    <row r="197" spans="1:18" ht="96">
+    <row r="197" spans="1:18" ht="96" hidden="1">
       <c r="A197" s="20" t="str">
         <f t="shared" si="27"/>
         <v>T196</v>
@@ -18807,7 +18829,7 @@
       <c r="Q197" s="24"/>
       <c r="R197" s="24"/>
     </row>
-    <row r="198" spans="1:18" ht="48">
+    <row r="198" spans="1:18" ht="48" hidden="1">
       <c r="A198" s="20" t="str">
         <f t="shared" si="27"/>
         <v>T197</v>
@@ -18858,7 +18880,7 @@
       <c r="Q198" s="24"/>
       <c r="R198" s="24"/>
     </row>
-    <row r="199" spans="1:18" ht="80">
+    <row r="199" spans="1:18" ht="80" hidden="1">
       <c r="A199" s="20" t="str">
         <f t="shared" si="27"/>
         <v>T198</v>
@@ -18909,7 +18931,7 @@
       <c r="Q199" s="24"/>
       <c r="R199" s="24"/>
     </row>
-    <row r="200" spans="1:18" ht="48">
+    <row r="200" spans="1:18" ht="48" hidden="1">
       <c r="A200" s="20" t="str">
         <f t="shared" si="27"/>
         <v>T199</v>
@@ -18960,7 +18982,7 @@
       <c r="Q200" s="24"/>
       <c r="R200" s="24"/>
     </row>
-    <row r="201" spans="1:18" ht="32">
+    <row r="201" spans="1:18" ht="32" hidden="1">
       <c r="A201" s="20" t="str">
         <f t="shared" si="27"/>
         <v>T200</v>
@@ -19011,7 +19033,7 @@
       <c r="Q201" s="24"/>
       <c r="R201" s="24"/>
     </row>
-    <row r="202" spans="1:18" ht="32">
+    <row r="202" spans="1:18" ht="32" hidden="1">
       <c r="A202" s="20" t="str">
         <f t="shared" si="27"/>
         <v>T201</v>
@@ -19062,7 +19084,7 @@
       <c r="Q202" s="24"/>
       <c r="R202" s="24"/>
     </row>
-    <row r="203" spans="1:18" ht="80">
+    <row r="203" spans="1:18" ht="80" hidden="1">
       <c r="A203" s="20" t="str">
         <f t="shared" si="27"/>
         <v>T202</v>
@@ -19113,7 +19135,7 @@
       <c r="Q203" s="24"/>
       <c r="R203" s="24"/>
     </row>
-    <row r="204" spans="1:18" ht="64">
+    <row r="204" spans="1:18" ht="64" hidden="1">
       <c r="A204" s="20" t="str">
         <f t="shared" si="27"/>
         <v>T203</v>
@@ -19164,7 +19186,7 @@
       <c r="Q204" s="24"/>
       <c r="R204" s="24"/>
     </row>
-    <row r="205" spans="1:18" ht="64">
+    <row r="205" spans="1:18" ht="64" hidden="1">
       <c r="A205" s="20" t="str">
         <f t="shared" si="27"/>
         <v>T204</v>
@@ -19215,7 +19237,7 @@
       <c r="Q205" s="24"/>
       <c r="R205" s="24"/>
     </row>
-    <row r="206" spans="1:18" ht="32">
+    <row r="206" spans="1:18" ht="32" hidden="1">
       <c r="A206" s="20" t="str">
         <f t="shared" si="27"/>
         <v>T205</v>
@@ -19266,7 +19288,7 @@
       <c r="Q206" s="24"/>
       <c r="R206" s="24"/>
     </row>
-    <row r="207" spans="1:18" ht="80">
+    <row r="207" spans="1:18" ht="80" hidden="1">
       <c r="A207" s="20" t="str">
         <f t="shared" si="27"/>
         <v>T206</v>
@@ -19317,7 +19339,7 @@
       <c r="Q207" s="24"/>
       <c r="R207" s="24"/>
     </row>
-    <row r="208" spans="1:18" ht="96">
+    <row r="208" spans="1:18" ht="96" hidden="1">
       <c r="A208" s="20" t="str">
         <f t="shared" si="27"/>
         <v>T207</v>
@@ -19368,7 +19390,7 @@
       <c r="Q208" s="24"/>
       <c r="R208" s="24"/>
     </row>
-    <row r="209" spans="1:18" ht="80">
+    <row r="209" spans="1:18" ht="80" hidden="1">
       <c r="A209" s="20" t="str">
         <f t="shared" si="27"/>
         <v>T208</v>
@@ -19419,7 +19441,7 @@
       <c r="Q209" s="24"/>
       <c r="R209" s="24"/>
     </row>
-    <row r="210" spans="1:18" ht="80">
+    <row r="210" spans="1:18" ht="80" hidden="1">
       <c r="A210" s="20" t="str">
         <f t="shared" si="27"/>
         <v>T209</v>
@@ -19470,7 +19492,7 @@
       <c r="Q210" s="24"/>
       <c r="R210" s="24"/>
     </row>
-    <row r="211" spans="1:18" ht="48">
+    <row r="211" spans="1:18" ht="48" hidden="1">
       <c r="A211" s="20" t="str">
         <f t="shared" si="27"/>
         <v>T210</v>
@@ -19521,7 +19543,7 @@
       <c r="Q211" s="24"/>
       <c r="R211" s="24"/>
     </row>
-    <row r="212" spans="1:18" ht="32">
+    <row r="212" spans="1:18" ht="32" hidden="1">
       <c r="A212" s="20" t="str">
         <f t="shared" si="27"/>
         <v>T211</v>
@@ -19572,7 +19594,7 @@
       <c r="Q212" s="24"/>
       <c r="R212" s="24"/>
     </row>
-    <row r="213" spans="1:18" ht="144">
+    <row r="213" spans="1:18" ht="144" hidden="1">
       <c r="A213" s="20" t="str">
         <f t="shared" si="27"/>
         <v>T212</v>
@@ -19623,7 +19645,7 @@
       <c r="Q213" s="24"/>
       <c r="R213" s="24"/>
     </row>
-    <row r="214" spans="1:18" ht="80">
+    <row r="214" spans="1:18" ht="80" hidden="1">
       <c r="A214" s="20" t="str">
         <f t="shared" si="27"/>
         <v>T213</v>
@@ -19674,7 +19696,7 @@
       <c r="Q214" s="24"/>
       <c r="R214" s="24"/>
     </row>
-    <row r="215" spans="1:18" ht="96">
+    <row r="215" spans="1:18" ht="96" hidden="1">
       <c r="A215" s="20" t="str">
         <f t="shared" si="27"/>
         <v>T214</v>
@@ -19725,7 +19747,7 @@
       <c r="Q215" s="24"/>
       <c r="R215" s="24"/>
     </row>
-    <row r="216" spans="1:18" ht="96">
+    <row r="216" spans="1:18" ht="96" hidden="1">
       <c r="A216" s="20" t="str">
         <f t="shared" si="27"/>
         <v>T215</v>
@@ -19776,7 +19798,7 @@
       <c r="Q216" s="24"/>
       <c r="R216" s="24"/>
     </row>
-    <row r="217" spans="1:18" ht="80">
+    <row r="217" spans="1:18" ht="80" hidden="1">
       <c r="A217" s="20" t="str">
         <f t="shared" si="27"/>
         <v>T216</v>
@@ -19827,7 +19849,7 @@
       <c r="Q217" s="24"/>
       <c r="R217" s="24"/>
     </row>
-    <row r="218" spans="1:18" ht="80">
+    <row r="218" spans="1:18" ht="80" hidden="1">
       <c r="A218" s="20" t="str">
         <f t="shared" si="27"/>
         <v>T217</v>
@@ -19878,7 +19900,7 @@
       <c r="Q218" s="24"/>
       <c r="R218" s="24"/>
     </row>
-    <row r="219" spans="1:18" ht="48">
+    <row r="219" spans="1:18" ht="48" hidden="1">
       <c r="A219" s="20" t="str">
         <f t="shared" si="27"/>
         <v>T218</v>
@@ -19929,7 +19951,7 @@
       <c r="Q219" s="24"/>
       <c r="R219" s="24"/>
     </row>
-    <row r="220" spans="1:18" ht="32">
+    <row r="220" spans="1:18" ht="32" hidden="1">
       <c r="A220" s="20" t="str">
         <f t="shared" si="27"/>
         <v>T219</v>
@@ -19980,7 +20002,7 @@
       <c r="Q220" s="24"/>
       <c r="R220" s="24"/>
     </row>
-    <row r="221" spans="1:18" ht="64">
+    <row r="221" spans="1:18" ht="64" hidden="1">
       <c r="A221" s="20" t="str">
         <f t="shared" si="27"/>
         <v>T220</v>
@@ -20031,7 +20053,7 @@
       <c r="Q221" s="24"/>
       <c r="R221" s="24"/>
     </row>
-    <row r="222" spans="1:18" ht="16">
+    <row r="222" spans="1:18" ht="16" hidden="1">
       <c r="A222" s="20" t="str">
         <f t="shared" si="27"/>
         <v>T221</v>
@@ -20082,7 +20104,7 @@
       <c r="Q222" s="24"/>
       <c r="R222" s="24"/>
     </row>
-    <row r="223" spans="1:18" ht="64">
+    <row r="223" spans="1:18" ht="64" hidden="1">
       <c r="A223" s="20" t="str">
         <f t="shared" si="27"/>
         <v>T222</v>
@@ -20133,7 +20155,7 @@
       <c r="Q223" s="24"/>
       <c r="R223" s="24"/>
     </row>
-    <row r="224" spans="1:18" ht="96">
+    <row r="224" spans="1:18" ht="96" hidden="1">
       <c r="A224" s="20" t="str">
         <f t="shared" si="27"/>
         <v>T223</v>
@@ -20184,7 +20206,7 @@
       <c r="Q224" s="24"/>
       <c r="R224" s="24"/>
     </row>
-    <row r="225" spans="1:18" ht="80">
+    <row r="225" spans="1:18" ht="80" hidden="1">
       <c r="A225" s="20" t="str">
         <f t="shared" si="27"/>
         <v>T224</v>
@@ -20235,7 +20257,7 @@
       <c r="Q225" s="24"/>
       <c r="R225" s="24"/>
     </row>
-    <row r="226" spans="1:18" ht="80">
+    <row r="226" spans="1:18" ht="80" hidden="1">
       <c r="A226" s="20" t="str">
         <f t="shared" si="27"/>
         <v>T225</v>
@@ -20286,7 +20308,7 @@
       <c r="Q226" s="24"/>
       <c r="R226" s="24"/>
     </row>
-    <row r="227" spans="1:18" ht="64">
+    <row r="227" spans="1:18" ht="64" hidden="1">
       <c r="A227" s="20" t="str">
         <f t="shared" si="27"/>
         <v>T226</v>
@@ -20337,7 +20359,7 @@
       <c r="Q227" s="24"/>
       <c r="R227" s="24"/>
     </row>
-    <row r="228" spans="1:18" ht="80">
+    <row r="228" spans="1:18" ht="80" hidden="1">
       <c r="A228" s="20" t="str">
         <f t="shared" si="27"/>
         <v>T227</v>
@@ -20388,7 +20410,7 @@
       <c r="Q228" s="24"/>
       <c r="R228" s="24"/>
     </row>
-    <row r="229" spans="1:18" ht="64">
+    <row r="229" spans="1:18" ht="64" hidden="1">
       <c r="A229" s="20" t="str">
         <f t="shared" si="27"/>
         <v>T228</v>
@@ -20439,7 +20461,7 @@
       <c r="Q229" s="24"/>
       <c r="R229" s="24"/>
     </row>
-    <row r="230" spans="1:18" ht="48">
+    <row r="230" spans="1:18" ht="48" hidden="1">
       <c r="A230" s="20" t="str">
         <f t="shared" si="27"/>
         <v>T229</v>
@@ -20490,7 +20512,7 @@
       <c r="Q230" s="24"/>
       <c r="R230" s="24"/>
     </row>
-    <row r="231" spans="1:18" ht="80">
+    <row r="231" spans="1:18" ht="80" hidden="1">
       <c r="A231" s="20" t="str">
         <f t="shared" si="27"/>
         <v>T230</v>
@@ -20541,7 +20563,7 @@
       <c r="Q231" s="24"/>
       <c r="R231" s="24"/>
     </row>
-    <row r="232" spans="1:18" ht="80">
+    <row r="232" spans="1:18" ht="80" hidden="1">
       <c r="A232" s="20" t="str">
         <f t="shared" si="27"/>
         <v>T231</v>
@@ -20592,7 +20614,7 @@
       <c r="Q232" s="24"/>
       <c r="R232" s="24"/>
     </row>
-    <row r="233" spans="1:18" ht="48">
+    <row r="233" spans="1:18" ht="48" hidden="1">
       <c r="A233" s="20" t="str">
         <f t="shared" si="27"/>
         <v>T232</v>
@@ -20643,7 +20665,7 @@
       <c r="Q233" s="24"/>
       <c r="R233" s="24"/>
     </row>
-    <row r="234" spans="1:18" ht="96">
+    <row r="234" spans="1:18" ht="96" hidden="1">
       <c r="A234" s="20" t="str">
         <f t="shared" si="27"/>
         <v>T233</v>
@@ -20694,7 +20716,7 @@
       <c r="Q234" s="24"/>
       <c r="R234" s="24"/>
     </row>
-    <row r="235" spans="1:18" ht="96">
+    <row r="235" spans="1:18" ht="96" hidden="1">
       <c r="A235" s="20" t="str">
         <f t="shared" si="27"/>
         <v>T234</v>
@@ -20745,7 +20767,7 @@
       <c r="Q235" s="24"/>
       <c r="R235" s="24"/>
     </row>
-    <row r="236" spans="1:18" ht="80">
+    <row r="236" spans="1:18" ht="80" hidden="1">
       <c r="A236" s="20" t="str">
         <f t="shared" si="27"/>
         <v>T235</v>
@@ -20796,7 +20818,7 @@
       <c r="Q236" s="24"/>
       <c r="R236" s="24"/>
     </row>
-    <row r="237" spans="1:18" ht="80">
+    <row r="237" spans="1:18" ht="80" hidden="1">
       <c r="A237" s="20" t="str">
         <f t="shared" si="27"/>
         <v>T236</v>
@@ -20847,7 +20869,7 @@
       <c r="Q237" s="24"/>
       <c r="R237" s="24"/>
     </row>
-    <row r="238" spans="1:18" ht="48">
+    <row r="238" spans="1:18" ht="48" hidden="1">
       <c r="A238" s="20" t="str">
         <f t="shared" si="27"/>
         <v>T237</v>
@@ -20898,7 +20920,7 @@
       <c r="Q238" s="24"/>
       <c r="R238" s="24"/>
     </row>
-    <row r="239" spans="1:18" ht="32">
+    <row r="239" spans="1:18" ht="32" hidden="1">
       <c r="A239" s="20" t="str">
         <f t="shared" si="27"/>
         <v>T238</v>
@@ -20949,7 +20971,7 @@
       <c r="Q239" s="24"/>
       <c r="R239" s="24"/>
     </row>
-    <row r="240" spans="1:18" ht="80">
+    <row r="240" spans="1:18" ht="80" hidden="1">
       <c r="A240" s="20" t="str">
         <f t="shared" si="27"/>
         <v>T239</v>
@@ -21000,7 +21022,7 @@
       <c r="Q240" s="24"/>
       <c r="R240" s="24"/>
     </row>
-    <row r="241" spans="1:18" ht="80">
+    <row r="241" spans="1:18" ht="80" hidden="1">
       <c r="A241" s="20" t="str">
         <f t="shared" si="27"/>
         <v>T240</v>
@@ -21051,7 +21073,7 @@
       <c r="Q241" s="24"/>
       <c r="R241" s="24"/>
     </row>
-    <row r="242" spans="1:18" ht="48">
+    <row r="242" spans="1:18" ht="48" hidden="1">
       <c r="A242" s="20" t="str">
         <f t="shared" si="27"/>
         <v>T241</v>
@@ -21102,7 +21124,7 @@
       <c r="Q242" s="24"/>
       <c r="R242" s="24"/>
     </row>
-    <row r="243" spans="1:18" ht="32">
+    <row r="243" spans="1:18" ht="32" hidden="1">
       <c r="A243" s="20" t="str">
         <f t="shared" si="27"/>
         <v>T242</v>
@@ -21153,7 +21175,7 @@
       <c r="Q243" s="24"/>
       <c r="R243" s="24"/>
     </row>
-    <row r="244" spans="1:18" ht="32">
+    <row r="244" spans="1:18" ht="32" hidden="1">
       <c r="A244" s="20" t="str">
         <f t="shared" si="27"/>
         <v>T243</v>
@@ -21204,7 +21226,7 @@
       <c r="Q244" s="24"/>
       <c r="R244" s="24"/>
     </row>
-    <row r="245" spans="1:18" ht="32">
+    <row r="245" spans="1:18" ht="32" hidden="1">
       <c r="A245" s="20" t="str">
         <f t="shared" si="27"/>
         <v>T244</v>
@@ -21255,7 +21277,7 @@
       <c r="Q245" s="24"/>
       <c r="R245" s="24"/>
     </row>
-    <row r="246" spans="1:18" ht="80">
+    <row r="246" spans="1:18" ht="80" hidden="1">
       <c r="A246" s="20" t="str">
         <f t="shared" si="27"/>
         <v>T245</v>
@@ -21306,7 +21328,7 @@
       <c r="Q246" s="24"/>
       <c r="R246" s="24"/>
     </row>
-    <row r="247" spans="1:18" ht="32">
+    <row r="247" spans="1:18" ht="32" hidden="1">
       <c r="A247" s="20" t="str">
         <f t="shared" si="27"/>
         <v>T246</v>
@@ -21357,7 +21379,7 @@
       <c r="Q247" s="24"/>
       <c r="R247" s="24"/>
     </row>
-    <row r="248" spans="1:18" ht="32">
+    <row r="248" spans="1:18" ht="32" hidden="1">
       <c r="A248" s="20" t="str">
         <f t="shared" si="27"/>
         <v>T247</v>
@@ -21408,7 +21430,7 @@
       <c r="Q248" s="24"/>
       <c r="R248" s="24"/>
     </row>
-    <row r="249" spans="1:18" ht="80">
+    <row r="249" spans="1:18" ht="80" hidden="1">
       <c r="A249" s="20" t="str">
         <f t="shared" si="27"/>
         <v>T248</v>
@@ -21459,7 +21481,7 @@
       <c r="Q249" s="24"/>
       <c r="R249" s="24"/>
     </row>
-    <row r="250" spans="1:18" ht="64">
+    <row r="250" spans="1:18" ht="64" hidden="1">
       <c r="A250" s="20" t="str">
         <f t="shared" si="27"/>
         <v>T249</v>
@@ -21510,7 +21532,7 @@
       <c r="Q250" s="24"/>
       <c r="R250" s="24"/>
     </row>
-    <row r="251" spans="1:18" ht="64">
+    <row r="251" spans="1:18" ht="64" hidden="1">
       <c r="A251" s="20" t="str">
         <f t="shared" si="27"/>
         <v>T250</v>
@@ -21561,7 +21583,7 @@
       <c r="Q251" s="24"/>
       <c r="R251" s="24"/>
     </row>
-    <row r="252" spans="1:18" ht="96">
+    <row r="252" spans="1:18" ht="96" hidden="1">
       <c r="A252" s="20" t="str">
         <f t="shared" si="27"/>
         <v>T251</v>
@@ -21612,7 +21634,7 @@
       <c r="Q252" s="24"/>
       <c r="R252" s="24"/>
     </row>
-    <row r="253" spans="1:18" ht="48">
+    <row r="253" spans="1:18" ht="48" hidden="1">
       <c r="A253" s="20" t="str">
         <f t="shared" si="27"/>
         <v>T252</v>
@@ -21663,7 +21685,7 @@
       <c r="Q253" s="24"/>
       <c r="R253" s="24"/>
     </row>
-    <row r="254" spans="1:18" ht="80">
+    <row r="254" spans="1:18" ht="80" hidden="1">
       <c r="A254" s="20" t="str">
         <f t="shared" si="27"/>
         <v>T253</v>
@@ -21714,7 +21736,7 @@
       <c r="Q254" s="24"/>
       <c r="R254" s="24"/>
     </row>
-    <row r="255" spans="1:18" ht="16">
+    <row r="255" spans="1:18" ht="16" hidden="1">
       <c r="A255" s="20" t="str">
         <f t="shared" si="27"/>
         <v>T254</v>
@@ -25669,7 +25691,7 @@
       </c>
     </row>
     <row r="30" spans="1:13" ht="48">
-      <c r="A30" s="30" t="s">
+      <c r="A30" s="32" t="s">
         <v>732</v>
       </c>
       <c r="B30" s="5" t="s">
@@ -25712,7 +25734,7 @@
       </c>
     </row>
     <row r="31" spans="1:13" ht="48">
-      <c r="A31" s="30"/>
+      <c r="A31" s="32"/>
       <c r="B31" s="5" t="s">
         <v>735</v>
       </c>
@@ -25753,7 +25775,7 @@
       </c>
     </row>
     <row r="32" spans="1:13" ht="32">
-      <c r="A32" s="30"/>
+      <c r="A32" s="32"/>
       <c r="B32" s="5" t="s">
         <v>737</v>
       </c>
@@ -25794,7 +25816,7 @@
       </c>
     </row>
     <row r="33" spans="1:13" ht="96">
-      <c r="A33" s="30"/>
+      <c r="A33" s="32"/>
       <c r="B33" s="5" t="s">
         <v>51</v>
       </c>
@@ -25835,7 +25857,7 @@
       </c>
     </row>
     <row r="34" spans="1:13" ht="32">
-      <c r="A34" s="30"/>
+      <c r="A34" s="32"/>
       <c r="B34" s="5" t="s">
         <v>740</v>
       </c>
@@ -25876,7 +25898,7 @@
       </c>
     </row>
     <row r="35" spans="1:13" ht="32">
-      <c r="A35" s="30"/>
+      <c r="A35" s="32"/>
       <c r="B35" s="5" t="s">
         <v>414</v>
       </c>
@@ -25917,7 +25939,7 @@
       </c>
     </row>
     <row r="36" spans="1:13" ht="80">
-      <c r="A36" s="30"/>
+      <c r="A36" s="32"/>
       <c r="B36" s="5" t="s">
         <v>743</v>
       </c>
@@ -26456,7 +26478,7 @@
       </c>
     </row>
     <row r="49" spans="1:13" ht="78" customHeight="1">
-      <c r="A49" s="30" t="s">
+      <c r="A49" s="32" t="s">
         <v>761</v>
       </c>
       <c r="B49" s="5" t="s">
@@ -26499,7 +26521,7 @@
       </c>
     </row>
     <row r="50" spans="1:13" ht="32">
-      <c r="A50" s="30"/>
+      <c r="A50" s="32"/>
       <c r="B50" s="5" t="s">
         <v>409</v>
       </c>
@@ -26540,7 +26562,7 @@
       </c>
     </row>
     <row r="51" spans="1:13" ht="16">
-      <c r="A51" s="30"/>
+      <c r="A51" s="32"/>
       <c r="B51" s="5" t="s">
         <v>414</v>
       </c>
@@ -26581,7 +26603,7 @@
       </c>
     </row>
     <row r="52" spans="1:13" ht="32">
-      <c r="A52" s="30"/>
+      <c r="A52" s="32"/>
       <c r="B52" s="5" t="s">
         <v>766</v>
       </c>
@@ -26622,7 +26644,7 @@
       </c>
     </row>
     <row r="53" spans="1:13" ht="96">
-      <c r="A53" s="30"/>
+      <c r="A53" s="32"/>
       <c r="B53" s="5" t="s">
         <v>768</v>
       </c>
@@ -26663,7 +26685,7 @@
       </c>
     </row>
     <row r="54" spans="1:13">
-      <c r="A54" s="30"/>
+      <c r="A54" s="32"/>
       <c r="B54" s="5" t="s">
         <v>770</v>
       </c>
@@ -26704,7 +26726,7 @@
       </c>
     </row>
     <row r="55" spans="1:13" ht="64">
-      <c r="A55" s="30"/>
+      <c r="A55" s="32"/>
       <c r="B55" s="5" t="s">
         <v>772</v>
       </c>
@@ -26745,7 +26767,7 @@
       </c>
     </row>
     <row r="56" spans="1:13" ht="64">
-      <c r="A56" s="30"/>
+      <c r="A56" s="32"/>
       <c r="B56" s="5" t="s">
         <v>774</v>
       </c>
@@ -26786,7 +26808,7 @@
       </c>
     </row>
     <row r="57" spans="1:13" ht="32">
-      <c r="A57" s="31" t="s">
+      <c r="A57" s="30" t="s">
         <v>776</v>
       </c>
       <c r="B57" s="6" t="s">
@@ -26828,7 +26850,7 @@
       </c>
     </row>
     <row r="58" spans="1:13" ht="80">
-      <c r="A58" s="31"/>
+      <c r="A58" s="30"/>
       <c r="B58" s="7" t="s">
         <v>779</v>
       </c>
@@ -26868,7 +26890,7 @@
       </c>
     </row>
     <row r="59" spans="1:13" ht="64" customHeight="1">
-      <c r="A59" s="31"/>
+      <c r="A59" s="30"/>
       <c r="B59" s="7" t="s">
         <v>781</v>
       </c>
@@ -26908,7 +26930,7 @@
       </c>
     </row>
     <row r="60" spans="1:13" ht="16">
-      <c r="A60" s="31"/>
+      <c r="A60" s="30"/>
       <c r="B60" s="7" t="s">
         <v>283</v>
       </c>
@@ -26948,7 +26970,7 @@
       </c>
     </row>
     <row r="61" spans="1:13" ht="32">
-      <c r="A61" s="31"/>
+      <c r="A61" s="30"/>
       <c r="B61" s="7" t="s">
         <v>785</v>
       </c>
@@ -26988,7 +27010,7 @@
       </c>
     </row>
     <row r="62" spans="1:13" ht="32">
-      <c r="A62" s="31"/>
+      <c r="A62" s="30"/>
       <c r="B62" s="7" t="s">
         <v>787</v>
       </c>
@@ -27028,7 +27050,7 @@
       </c>
     </row>
     <row r="63" spans="1:13" ht="16">
-      <c r="A63" s="31"/>
+      <c r="A63" s="30"/>
       <c r="B63" s="7" t="s">
         <v>790</v>
       </c>
@@ -27068,7 +27090,7 @@
       </c>
     </row>
     <row r="64" spans="1:13" ht="32">
-      <c r="A64" s="31"/>
+      <c r="A64" s="30"/>
       <c r="B64" s="6" t="s">
         <v>792</v>
       </c>
@@ -27108,7 +27130,7 @@
       </c>
     </row>
     <row r="65" spans="1:13" ht="16">
-      <c r="A65" s="31"/>
+      <c r="A65" s="30"/>
       <c r="B65" s="7" t="s">
         <v>81</v>
       </c>
@@ -27148,7 +27170,7 @@
       </c>
     </row>
     <row r="66" spans="1:13" ht="16">
-      <c r="A66" s="31"/>
+      <c r="A66" s="30"/>
       <c r="B66" s="7" t="s">
         <v>795</v>
       </c>
@@ -27188,7 +27210,7 @@
       </c>
     </row>
     <row r="67" spans="1:13" ht="48">
-      <c r="A67" s="31"/>
+      <c r="A67" s="30"/>
       <c r="B67" s="6" t="s">
         <v>280</v>
       </c>
@@ -27228,38 +27250,38 @@
       </c>
     </row>
     <row r="68" spans="1:13" ht="16">
-      <c r="A68" s="31"/>
-      <c r="B68" s="31" t="s">
+      <c r="A68" s="30"/>
+      <c r="B68" s="30" t="s">
         <v>357</v>
       </c>
       <c r="C68" s="6" t="s">
         <v>797</v>
       </c>
-      <c r="D68" s="31" t="s">
+      <c r="D68" s="30" t="s">
         <v>274</v>
       </c>
-      <c r="E68" s="31" t="s">
+      <c r="E68" s="30" t="s">
         <v>783</v>
       </c>
-      <c r="F68" s="31" t="s">
-        <v>22</v>
-      </c>
-      <c r="G68" s="31" t="s">
+      <c r="F68" s="30" t="s">
+        <v>22</v>
+      </c>
+      <c r="G68" s="30" t="s">
         <v>22</v>
       </c>
       <c r="H68" s="29" t="s">
         <v>22</v>
       </c>
-      <c r="I68" s="31" t="s">
+      <c r="I68" s="30" t="s">
         <v>364</v>
       </c>
-      <c r="J68" s="31" t="s">
-        <v>22</v>
-      </c>
-      <c r="K68" s="31" t="s">
-        <v>22</v>
-      </c>
-      <c r="L68" s="31" t="s">
+      <c r="J68" s="30" t="s">
+        <v>22</v>
+      </c>
+      <c r="K68" s="30" t="s">
+        <v>22</v>
+      </c>
+      <c r="L68" s="30" t="s">
         <v>23</v>
       </c>
       <c r="M68" s="29" t="str">
@@ -27268,24 +27290,24 @@
       </c>
     </row>
     <row r="69" spans="1:13" ht="16">
-      <c r="A69" s="31"/>
-      <c r="B69" s="31"/>
+      <c r="A69" s="30"/>
+      <c r="B69" s="30"/>
       <c r="C69" s="6" t="s">
         <v>798</v>
       </c>
-      <c r="D69" s="31"/>
-      <c r="E69" s="31"/>
-      <c r="F69" s="31"/>
-      <c r="G69" s="31"/>
+      <c r="D69" s="30"/>
+      <c r="E69" s="30"/>
+      <c r="F69" s="30"/>
+      <c r="G69" s="30"/>
       <c r="H69" s="29"/>
-      <c r="I69" s="31"/>
-      <c r="J69" s="31"/>
-      <c r="K69" s="31"/>
-      <c r="L69" s="31"/>
+      <c r="I69" s="30"/>
+      <c r="J69" s="30"/>
+      <c r="K69" s="30"/>
+      <c r="L69" s="30"/>
       <c r="M69" s="29"/>
     </row>
     <row r="70" spans="1:13" ht="28">
-      <c r="A70" s="32" t="s">
+      <c r="A70" s="31" t="s">
         <v>799</v>
       </c>
       <c r="B70" s="16" t="s">
@@ -27331,7 +27353,7 @@
       </c>
     </row>
     <row r="71" spans="1:13" ht="51">
-      <c r="A71" s="32"/>
+      <c r="A71" s="31"/>
       <c r="B71" s="16" t="s">
         <v>51</v>
       </c>
@@ -27375,7 +27397,7 @@
       </c>
     </row>
     <row r="72" spans="1:13" ht="28">
-      <c r="A72" s="32"/>
+      <c r="A72" s="31"/>
       <c r="B72" s="16" t="s">
         <v>684</v>
       </c>
@@ -27419,7 +27441,7 @@
       </c>
     </row>
     <row r="73" spans="1:13" ht="28">
-      <c r="A73" s="32"/>
+      <c r="A73" s="31"/>
       <c r="B73" s="16" t="s">
         <v>806</v>
       </c>
@@ -27981,6 +28003,15 @@
     </row>
   </sheetData>
   <mergeCells count="23">
+    <mergeCell ref="A2:A7"/>
+    <mergeCell ref="A8:A14"/>
+    <mergeCell ref="A25:A29"/>
+    <mergeCell ref="A15:A24"/>
+    <mergeCell ref="A49:A56"/>
+    <mergeCell ref="A44:A48"/>
+    <mergeCell ref="A41:A43"/>
+    <mergeCell ref="A30:A36"/>
+    <mergeCell ref="A37:A40"/>
     <mergeCell ref="M68:M69"/>
     <mergeCell ref="H68:H69"/>
     <mergeCell ref="A74:A85"/>
@@ -27995,15 +28026,6 @@
     <mergeCell ref="B68:B69"/>
     <mergeCell ref="D68:D69"/>
     <mergeCell ref="E68:E69"/>
-    <mergeCell ref="A2:A7"/>
-    <mergeCell ref="A8:A14"/>
-    <mergeCell ref="A25:A29"/>
-    <mergeCell ref="A15:A24"/>
-    <mergeCell ref="A49:A56"/>
-    <mergeCell ref="A44:A48"/>
-    <mergeCell ref="A41:A43"/>
-    <mergeCell ref="A30:A36"/>
-    <mergeCell ref="A37:A40"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -28857,7 +28879,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C51FC597-29FA-1D4E-A4C8-B79027768242}">
   <dimension ref="A1:F7"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="181" workbookViewId="0">
+    <sheetView zoomScale="181" workbookViewId="0">
       <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
@@ -29019,6 +29041,17 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="633f040f-4953-46e7-8610-82b0c5296ba0">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="f62ef740-d444-4f18-80a2-7590fdcab1ce" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x0101009A9CE0B21D9C3A45B31425227616CD6F" ma:contentTypeVersion="11" ma:contentTypeDescription="Creare un nuovo documento." ma:contentTypeScope="" ma:versionID="180d662eb9e2621fe5c8d1498a11e3bf">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="633f040f-4953-46e7-8610-82b0c5296ba0" xmlns:ns3="f62ef740-d444-4f18-80a2-7590fdcab1ce" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="64519aed5f694bce5dc2f4bcf073d27d" ns2:_="" ns3:_="">
     <xsd:import namespace="633f040f-4953-46e7-8610-82b0c5296ba0"/>
@@ -29229,17 +29262,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="633f040f-4953-46e7-8610-82b0c5296ba0">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="f62ef740-d444-4f18-80a2-7590fdcab1ce" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -29250,6 +29272,23 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{83D5100D-0E56-4B30-B42D-2AEC6B837C39}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="f62ef740-d444-4f18-80a2-7590fdcab1ce"/>
+    <ds:schemaRef ds:uri="633f040f-4953-46e7-8610-82b0c5296ba0"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CA355F46-8632-4C01-B7E7-8E7DCFF50FB7}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -29268,23 +29307,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{83D5100D-0E56-4B30-B42D-2AEC6B837C39}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="633f040f-4953-46e7-8610-82b0c5296ba0"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="f62ef740-d444-4f18-80a2-7590fdcab1ce"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2C6CC7BA-2E2C-4B0D-8103-11A51D82E8EC}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
Modificato NOSQLDB in NoSQLDB
</commit_message>
<xml_diff>
--- a/apps/static/assets/dbs/ThreatCatalogComplete.xlsx
+++ b/apps/static/assets/dbs/ThreatCatalogComplete.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fefox/Desktop/WebApp/apps/static/assets/dbs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A61BCC03-42DB-A345-9199-FE223D956F2D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{FEF3B65C-6E70-F445-A433-D2AF0094FCA9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16380" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Threat Components" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
   </definedNames>
   <calcPr calcId="191028"/>
   <pivotCaches>
-    <pivotCache cacheId="1" r:id="rId6"/>
+    <pivotCache cacheId="3" r:id="rId6"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4196" uniqueCount="948">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4196" uniqueCount="949">
   <si>
     <t>TID</t>
   </si>
@@ -2920,9 +2920,6 @@
     <t>NoSQLMap</t>
   </si>
   <si>
-    <t>match (target)-[:uses]-&gt;(b {type:'Service.NOSQLDB'}) return target.component_id as component_id</t>
-  </si>
-  <si>
     <t>python NoSQLMap</t>
   </si>
   <si>
@@ -2930,6 +2927,12 @@
   </si>
   <si>
     <t>6, 15, 134, 182, 126, 128, 267, 251, 253, 185, 186, 66, 88, 136, 183, 250, 19, 23, 63, 468, 676</t>
+  </si>
+  <si>
+    <t>Service.NoSQLDB</t>
+  </si>
+  <si>
+    <t>match (target)-[:uses]-&gt;(b {type:'Service.NoSQLDB'}) return target.component_id as component_id</t>
   </si>
 </sst>
 </file>
@@ -8233,7 +8236,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{48CB07D6-9F6C-094F-A3D3-916741F281CD}" name="Tabella pivot1" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valori" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{48CB07D6-9F6C-094F-A3D3-916741F281CD}" name="Tabella pivot1" cacheId="3" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valori" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A1:B25" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="14">
     <pivotField showAll="0"/>
@@ -8378,7 +8381,7 @@
   <autoFilter ref="A1:R314" xr:uid="{DEFAB213-4389-184E-911C-CDCC8CABBD38}">
     <filterColumn colId="1">
       <filters>
-        <filter val="Service.Web"/>
+        <filter val="Service.NOSQLDB"/>
       </filters>
     </filterColumn>
   </autoFilter>
@@ -8712,9 +8715,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:R314"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="125" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView zoomScale="125" zoomScaleNormal="115" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A291" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="Q292" sqref="Q292"/>
+      <selection pane="bottomLeft" activeCell="C306" sqref="C306"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -23907,7 +23910,7 @@
       </c>
       <c r="R290" s="24"/>
     </row>
-    <row r="291" spans="1:18" ht="96">
+    <row r="291" spans="1:18" ht="96" hidden="1">
       <c r="A291" s="20" t="str">
         <f t="shared" si="38"/>
         <v>T290</v>
@@ -23970,7 +23973,7 @@
         <v>681</v>
       </c>
     </row>
-    <row r="292" spans="1:18" ht="176">
+    <row r="292" spans="1:18" ht="176" hidden="1">
       <c r="A292" s="20" t="str">
         <f t="shared" si="38"/>
         <v>T291</v>
@@ -24024,14 +24027,14 @@
         <v>683</v>
       </c>
       <c r="P292" s="24" t="s">
-        <v>947</v>
+        <v>946</v>
       </c>
       <c r="Q292" s="24" t="s">
         <v>684</v>
       </c>
       <c r="R292" s="24"/>
     </row>
-    <row r="293" spans="1:18" ht="380">
+    <row r="293" spans="1:18" ht="380" hidden="1">
       <c r="A293" s="20" t="str">
         <f t="shared" si="38"/>
         <v>T292</v>
@@ -24092,7 +24095,7 @@
       </c>
       <c r="R293" s="24"/>
     </row>
-    <row r="294" spans="1:18" ht="144">
+    <row r="294" spans="1:18" ht="144" hidden="1">
       <c r="A294" s="20" t="str">
         <f t="shared" si="38"/>
         <v>T293</v>
@@ -24153,7 +24156,7 @@
       </c>
       <c r="R294" s="24"/>
     </row>
-    <row r="295" spans="1:18" ht="112">
+    <row r="295" spans="1:18" ht="112" hidden="1">
       <c r="A295" s="20" t="str">
         <f t="shared" si="38"/>
         <v>T294</v>
@@ -24214,7 +24217,7 @@
       </c>
       <c r="R295" s="24"/>
     </row>
-    <row r="296" spans="1:18" ht="96">
+    <row r="296" spans="1:18" ht="96" hidden="1">
       <c r="A296" s="20" t="str">
         <f t="shared" si="38"/>
         <v>T295</v>
@@ -24275,7 +24278,7 @@
       </c>
       <c r="R296" s="24"/>
     </row>
-    <row r="297" spans="1:18" ht="32">
+    <row r="297" spans="1:18" ht="32" hidden="1">
       <c r="A297" s="20" t="str">
         <f t="shared" si="38"/>
         <v>T296</v>
@@ -24334,7 +24337,7 @@
       <c r="Q297" s="24"/>
       <c r="R297" s="24"/>
     </row>
-    <row r="298" spans="1:18" ht="32">
+    <row r="298" spans="1:18" ht="32" hidden="1">
       <c r="A298" s="20" t="str">
         <f t="shared" si="38"/>
         <v>T297</v>
@@ -24395,7 +24398,7 @@
       </c>
       <c r="R298" s="24"/>
     </row>
-    <row r="299" spans="1:18" ht="48">
+    <row r="299" spans="1:18" ht="48" hidden="1">
       <c r="A299" s="20" t="str">
         <f t="shared" si="38"/>
         <v>T298</v>
@@ -24456,13 +24459,13 @@
       </c>
       <c r="R299" s="24"/>
     </row>
-    <row r="300" spans="1:18" ht="16" hidden="1">
+    <row r="300" spans="1:18" ht="16">
       <c r="A300" s="20" t="str">
         <f t="shared" si="38"/>
         <v>T299</v>
       </c>
       <c r="B300" s="20" t="s">
-        <v>721</v>
+        <v>947</v>
       </c>
       <c r="C300" s="20" t="s">
         <v>568</v>
@@ -24515,13 +24518,13 @@
       <c r="Q300" s="24"/>
       <c r="R300" s="24"/>
     </row>
-    <row r="301" spans="1:18" ht="16" hidden="1">
+    <row r="301" spans="1:18" ht="16">
       <c r="A301" s="20" t="str">
         <f t="shared" si="38"/>
         <v>T300</v>
       </c>
       <c r="B301" s="20" t="s">
-        <v>721</v>
+        <v>947</v>
       </c>
       <c r="C301" s="20" t="s">
         <v>571</v>
@@ -24574,13 +24577,13 @@
       <c r="Q301" s="24"/>
       <c r="R301" s="24"/>
     </row>
-    <row r="302" spans="1:18" ht="16" hidden="1">
+    <row r="302" spans="1:18" ht="16">
       <c r="A302" s="20" t="str">
         <f t="shared" si="38"/>
         <v>T301</v>
       </c>
       <c r="B302" s="20" t="s">
-        <v>721</v>
+        <v>947</v>
       </c>
       <c r="C302" s="20" t="s">
         <v>573</v>
@@ -24633,13 +24636,13 @@
       <c r="Q302" s="24"/>
       <c r="R302" s="24"/>
     </row>
-    <row r="303" spans="1:18" ht="16" hidden="1">
+    <row r="303" spans="1:18" ht="16">
       <c r="A303" s="20" t="str">
         <f t="shared" si="38"/>
         <v>T302</v>
       </c>
       <c r="B303" s="20" t="s">
-        <v>721</v>
+        <v>947</v>
       </c>
       <c r="C303" s="20" t="s">
         <v>575</v>
@@ -24694,13 +24697,13 @@
       </c>
       <c r="R303" s="24"/>
     </row>
-    <row r="304" spans="1:18" ht="240" hidden="1">
+    <row r="304" spans="1:18" ht="240">
       <c r="A304" s="20" t="str">
         <f t="shared" si="38"/>
         <v>T303</v>
       </c>
       <c r="B304" s="20" t="s">
-        <v>721</v>
+        <v>947</v>
       </c>
       <c r="C304" s="20" t="s">
         <v>579</v>
@@ -24755,13 +24758,13 @@
       </c>
       <c r="R304" s="24"/>
     </row>
-    <row r="305" spans="1:18" ht="16" hidden="1">
+    <row r="305" spans="1:18" ht="16">
       <c r="A305" s="20" t="str">
         <f t="shared" si="38"/>
         <v>T304</v>
       </c>
       <c r="B305" s="20" t="s">
-        <v>721</v>
+        <v>947</v>
       </c>
       <c r="C305" s="20" t="s">
         <v>584</v>
@@ -24814,13 +24817,13 @@
       <c r="Q305" s="24"/>
       <c r="R305" s="24"/>
     </row>
-    <row r="306" spans="1:18" ht="16" hidden="1">
+    <row r="306" spans="1:18" ht="16">
       <c r="A306" s="20" t="str">
         <f t="shared" si="38"/>
         <v>T305</v>
       </c>
       <c r="B306" s="20" t="s">
-        <v>721</v>
+        <v>947</v>
       </c>
       <c r="C306" s="20" t="s">
         <v>585</v>
@@ -24875,13 +24878,13 @@
       </c>
       <c r="R306" s="24"/>
     </row>
-    <row r="307" spans="1:18" ht="32" hidden="1">
+    <row r="307" spans="1:18" ht="32">
       <c r="A307" s="20" t="str">
         <f t="shared" si="38"/>
         <v>T306</v>
       </c>
       <c r="B307" s="20" t="s">
-        <v>721</v>
+        <v>947</v>
       </c>
       <c r="C307" s="20" t="s">
         <v>587</v>
@@ -24932,13 +24935,13 @@
         <v>234</v>
       </c>
     </row>
-    <row r="308" spans="1:18" ht="32" hidden="1">
+    <row r="308" spans="1:18" ht="32">
       <c r="A308" s="20" t="str">
         <f t="shared" si="38"/>
         <v>T307</v>
       </c>
       <c r="B308" s="20" t="s">
-        <v>721</v>
+        <v>947</v>
       </c>
       <c r="C308" s="20" t="s">
         <v>590</v>
@@ -24993,7 +24996,7 @@
       </c>
       <c r="R308" s="24"/>
     </row>
-    <row r="309" spans="1:18" ht="128" hidden="1">
+    <row r="309" spans="1:18" ht="128">
       <c r="A309" s="20" t="str">
         <f t="shared" si="38"/>
         <v>T308</v>
@@ -25054,7 +25057,7 @@
       </c>
       <c r="R309" s="24"/>
     </row>
-    <row r="310" spans="1:18" ht="64" hidden="1">
+    <row r="310" spans="1:18" ht="64">
       <c r="A310" s="20" t="str">
         <f t="shared" si="38"/>
         <v>T309</v>
@@ -25115,7 +25118,7 @@
       </c>
       <c r="R310" s="24"/>
     </row>
-    <row r="311" spans="1:18" ht="48" hidden="1">
+    <row r="311" spans="1:18" ht="48">
       <c r="A311" s="20" t="str">
         <f t="shared" si="38"/>
         <v>T310</v>
@@ -25176,7 +25179,7 @@
       </c>
       <c r="R311" s="24"/>
     </row>
-    <row r="312" spans="1:18" ht="32" hidden="1">
+    <row r="312" spans="1:18" ht="32">
       <c r="A312" s="20" t="str">
         <f t="shared" si="38"/>
         <v>T311</v>
@@ -25233,7 +25236,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="313" spans="1:18" ht="32" hidden="1">
+    <row r="313" spans="1:18" ht="32">
       <c r="A313" s="20" t="str">
         <f t="shared" si="38"/>
         <v>T312</v>
@@ -25294,7 +25297,7 @@
       </c>
       <c r="R313" s="24"/>
     </row>
-    <row r="314" spans="1:18" ht="16" hidden="1">
+    <row r="314" spans="1:18" ht="16">
       <c r="A314" s="20" t="str">
         <f t="shared" si="38"/>
         <v>T313</v>
@@ -29787,8 +29790,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C51FC597-29FA-1D4E-A4C8-B79027768242}">
   <dimension ref="A1:F8"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" zoomScale="181" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="181" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15"/>
@@ -29951,13 +29954,13 @@
         <v>942</v>
       </c>
       <c r="D8" s="27" t="s">
+        <v>948</v>
+      </c>
+      <c r="E8" s="26" t="s">
         <v>944</v>
       </c>
-      <c r="E8" s="26" t="s">
+      <c r="F8" s="27" t="s">
         <v>945</v>
-      </c>
-      <c r="F8" s="27" t="s">
-        <v>946</v>
       </c>
     </row>
   </sheetData>
@@ -30230,16 +30233,16 @@
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{83D5100D-0E56-4B30-B42D-2AEC6B837C39}">
   <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="633f040f-4953-46e7-8610-82b0c5296ba0"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="f62ef740-d444-4f18-80a2-7590fdcab1ce"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="f62ef740-d444-4f18-80a2-7590fdcab1ce"/>
     <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="633f040f-4953-46e7-8610-82b0c5296ba0"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Introdotta tabella sulle fasi del pentest, manca retrieve del nome
</commit_message>
<xml_diff>
--- a/apps/static/assets/dbs/ThreatCatalogComplete.xlsx
+++ b/apps/static/assets/dbs/ThreatCatalogComplete.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fefox/Desktop/WebApp/apps/static/assets/dbs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{045C8804-F935-044B-84EC-CC801918E0AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{D64E7C08-6E7B-EB44-8A24-C67577B785E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16280" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16280" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Threat Components" sheetId="1" r:id="rId1"/>
@@ -18,13 +18,14 @@
     <sheet name="#ThreatPerAsset" sheetId="4" r:id="rId3"/>
     <sheet name="Threats" sheetId="5" r:id="rId4"/>
     <sheet name="Tools" sheetId="6" r:id="rId5"/>
+    <sheet name="Pentest Phases" sheetId="7" r:id="rId6"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">Threats!$A$1:$B$76</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
   <pivotCaches>
-    <pivotCache cacheId="0" r:id="rId6"/>
+    <pivotCache cacheId="0" r:id="rId7"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -46,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4202" uniqueCount="954">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4205" uniqueCount="957">
   <si>
     <t>TID</t>
   </si>
@@ -2948,6 +2949,15 @@
   </si>
   <si>
     <t>Phase</t>
+  </si>
+  <si>
+    <t>PhaseID</t>
+  </si>
+  <si>
+    <t>PhaseName</t>
+  </si>
+  <si>
+    <t>Information Gathering</t>
   </si>
 </sst>
 </file>
@@ -3159,23 +3169,20 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="29">
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -3185,6 +3192,9 @@
           <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -8461,7 +8471,18 @@
     <tableColumn id="6" xr3:uid="{1E4A4CA6-7FF1-6543-A718-93EC7B5F1624}" name="CypherQuery" dataDxfId="4"/>
     <tableColumn id="3" xr3:uid="{52487567-ED26-B840-ABFD-DB1BF72A83C9}" name="Command" dataDxfId="3"/>
     <tableColumn id="5" xr3:uid="{0296B95F-6562-0746-B0C6-FE3564F6272C}" name="Description" dataDxfId="2"/>
-    <tableColumn id="7" xr3:uid="{FF0722DB-3140-904D-9B8E-A0C7B3C1FFEF}" name="Phase" dataDxfId="0"/>
+    <tableColumn id="7" xr3:uid="{FF0722DB-3140-904D-9B8E-A0C7B3C1FFEF}" name="Phase" dataDxfId="1"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{A164EF60-F2D6-A14B-A77B-445D5CF4A93F}" name="Tabella5" displayName="Tabella5" ref="A1:B2" totalsRowShown="0">
+  <autoFilter ref="A1:B2" xr:uid="{A164EF60-F2D6-A14B-A77B-445D5CF4A93F}"/>
+  <tableColumns count="2">
+    <tableColumn id="1" xr3:uid="{4BA8FDDB-056D-5B41-80F1-2DA22BF7BA71}" name="PhaseID"/>
+    <tableColumn id="2" xr3:uid="{58ED2D85-DFF7-0840-8CC5-B82A4CA7A8B4}" name="PhaseName"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -25376,7 +25397,7 @@
   </sheetData>
   <phoneticPr fontId="11" type="noConversion"/>
   <conditionalFormatting sqref="O1:Q314">
-    <cfRule type="containsBlanks" dxfId="1" priority="1" stopIfTrue="1">
+    <cfRule type="containsBlanks" dxfId="0" priority="1" stopIfTrue="1">
       <formula>LEN(TRIM(O1))=0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -26619,7 +26640,7 @@
       </c>
     </row>
     <row r="30" spans="1:13" ht="48">
-      <c r="A30" s="32" t="s">
+      <c r="A30" s="30" t="s">
         <v>793</v>
       </c>
       <c r="B30" s="5" t="s">
@@ -26662,7 +26683,7 @@
       </c>
     </row>
     <row r="31" spans="1:13" ht="48">
-      <c r="A31" s="32"/>
+      <c r="A31" s="30"/>
       <c r="B31" s="5" t="s">
         <v>796</v>
       </c>
@@ -26703,7 +26724,7 @@
       </c>
     </row>
     <row r="32" spans="1:13" ht="32">
-      <c r="A32" s="32"/>
+      <c r="A32" s="30"/>
       <c r="B32" s="5" t="s">
         <v>798</v>
       </c>
@@ -26744,7 +26765,7 @@
       </c>
     </row>
     <row r="33" spans="1:13" ht="96">
-      <c r="A33" s="32"/>
+      <c r="A33" s="30"/>
       <c r="B33" s="5" t="s">
         <v>100</v>
       </c>
@@ -26785,7 +26806,7 @@
       </c>
     </row>
     <row r="34" spans="1:13" ht="32">
-      <c r="A34" s="32"/>
+      <c r="A34" s="30"/>
       <c r="B34" s="5" t="s">
         <v>801</v>
       </c>
@@ -26826,7 +26847,7 @@
       </c>
     </row>
     <row r="35" spans="1:13" ht="32">
-      <c r="A35" s="32"/>
+      <c r="A35" s="30"/>
       <c r="B35" s="5" t="s">
         <v>201</v>
       </c>
@@ -26867,7 +26888,7 @@
       </c>
     </row>
     <row r="36" spans="1:13" ht="80">
-      <c r="A36" s="32"/>
+      <c r="A36" s="30"/>
       <c r="B36" s="5" t="s">
         <v>804</v>
       </c>
@@ -27406,7 +27427,7 @@
       </c>
     </row>
     <row r="49" spans="1:13" ht="78" customHeight="1">
-      <c r="A49" s="32" t="s">
+      <c r="A49" s="30" t="s">
         <v>822</v>
       </c>
       <c r="B49" s="5" t="s">
@@ -27449,7 +27470,7 @@
       </c>
     </row>
     <row r="50" spans="1:13" ht="32">
-      <c r="A50" s="32"/>
+      <c r="A50" s="30"/>
       <c r="B50" s="5" t="s">
         <v>613</v>
       </c>
@@ -27490,7 +27511,7 @@
       </c>
     </row>
     <row r="51" spans="1:13" ht="16">
-      <c r="A51" s="32"/>
+      <c r="A51" s="30"/>
       <c r="B51" s="5" t="s">
         <v>201</v>
       </c>
@@ -27531,7 +27552,7 @@
       </c>
     </row>
     <row r="52" spans="1:13" ht="32">
-      <c r="A52" s="32"/>
+      <c r="A52" s="30"/>
       <c r="B52" s="5" t="s">
         <v>827</v>
       </c>
@@ -27572,7 +27593,7 @@
       </c>
     </row>
     <row r="53" spans="1:13" ht="96">
-      <c r="A53" s="32"/>
+      <c r="A53" s="30"/>
       <c r="B53" s="5" t="s">
         <v>829</v>
       </c>
@@ -27613,7 +27634,7 @@
       </c>
     </row>
     <row r="54" spans="1:13">
-      <c r="A54" s="32"/>
+      <c r="A54" s="30"/>
       <c r="B54" s="5" t="s">
         <v>831</v>
       </c>
@@ -27654,7 +27675,7 @@
       </c>
     </row>
     <row r="55" spans="1:13" ht="64">
-      <c r="A55" s="32"/>
+      <c r="A55" s="30"/>
       <c r="B55" s="5" t="s">
         <v>833</v>
       </c>
@@ -27695,7 +27716,7 @@
       </c>
     </row>
     <row r="56" spans="1:13" ht="64">
-      <c r="A56" s="32"/>
+      <c r="A56" s="30"/>
       <c r="B56" s="5" t="s">
         <v>835</v>
       </c>
@@ -27736,7 +27757,7 @@
       </c>
     </row>
     <row r="57" spans="1:13" ht="32">
-      <c r="A57" s="30" t="s">
+      <c r="A57" s="31" t="s">
         <v>837</v>
       </c>
       <c r="B57" s="6" t="s">
@@ -27778,7 +27799,7 @@
       </c>
     </row>
     <row r="58" spans="1:13" ht="80">
-      <c r="A58" s="30"/>
+      <c r="A58" s="31"/>
       <c r="B58" s="7" t="s">
         <v>840</v>
       </c>
@@ -27818,7 +27839,7 @@
       </c>
     </row>
     <row r="59" spans="1:13" ht="64" customHeight="1">
-      <c r="A59" s="30"/>
+      <c r="A59" s="31"/>
       <c r="B59" s="7" t="s">
         <v>842</v>
       </c>
@@ -27858,7 +27879,7 @@
       </c>
     </row>
     <row r="60" spans="1:13" ht="16">
-      <c r="A60" s="30"/>
+      <c r="A60" s="31"/>
       <c r="B60" s="7" t="s">
         <v>95</v>
       </c>
@@ -27898,7 +27919,7 @@
       </c>
     </row>
     <row r="61" spans="1:13" ht="32">
-      <c r="A61" s="30"/>
+      <c r="A61" s="31"/>
       <c r="B61" s="7" t="s">
         <v>846</v>
       </c>
@@ -27938,7 +27959,7 @@
       </c>
     </row>
     <row r="62" spans="1:13" ht="32">
-      <c r="A62" s="30"/>
+      <c r="A62" s="31"/>
       <c r="B62" s="7" t="s">
         <v>848</v>
       </c>
@@ -27978,7 +27999,7 @@
       </c>
     </row>
     <row r="63" spans="1:13" ht="16">
-      <c r="A63" s="30"/>
+      <c r="A63" s="31"/>
       <c r="B63" s="7" t="s">
         <v>851</v>
       </c>
@@ -28018,7 +28039,7 @@
       </c>
     </row>
     <row r="64" spans="1:13" ht="32">
-      <c r="A64" s="30"/>
+      <c r="A64" s="31"/>
       <c r="B64" s="6" t="s">
         <v>853</v>
       </c>
@@ -28058,7 +28079,7 @@
       </c>
     </row>
     <row r="65" spans="1:13" ht="16">
-      <c r="A65" s="30"/>
+      <c r="A65" s="31"/>
       <c r="B65" s="7" t="s">
         <v>79</v>
       </c>
@@ -28098,7 +28119,7 @@
       </c>
     </row>
     <row r="66" spans="1:13" ht="16">
-      <c r="A66" s="30"/>
+      <c r="A66" s="31"/>
       <c r="B66" s="7" t="s">
         <v>856</v>
       </c>
@@ -28138,7 +28159,7 @@
       </c>
     </row>
     <row r="67" spans="1:13" ht="48">
-      <c r="A67" s="30"/>
+      <c r="A67" s="31"/>
       <c r="B67" s="6" t="s">
         <v>92</v>
       </c>
@@ -28178,38 +28199,38 @@
       </c>
     </row>
     <row r="68" spans="1:13" ht="16">
-      <c r="A68" s="30"/>
-      <c r="B68" s="30" t="s">
+      <c r="A68" s="31"/>
+      <c r="B68" s="31" t="s">
         <v>169</v>
       </c>
       <c r="C68" s="6" t="s">
         <v>858</v>
       </c>
-      <c r="D68" s="30" t="s">
+      <c r="D68" s="31" t="s">
         <v>25</v>
       </c>
-      <c r="E68" s="30" t="s">
+      <c r="E68" s="31" t="s">
         <v>844</v>
       </c>
-      <c r="F68" s="30" t="s">
-        <v>82</v>
-      </c>
-      <c r="G68" s="30" t="s">
+      <c r="F68" s="31" t="s">
+        <v>82</v>
+      </c>
+      <c r="G68" s="31" t="s">
         <v>82</v>
       </c>
       <c r="H68" s="29" t="s">
         <v>82</v>
       </c>
-      <c r="I68" s="30" t="s">
+      <c r="I68" s="31" t="s">
         <v>181</v>
       </c>
-      <c r="J68" s="30" t="s">
-        <v>82</v>
-      </c>
-      <c r="K68" s="30" t="s">
-        <v>82</v>
-      </c>
-      <c r="L68" s="30" t="s">
+      <c r="J68" s="31" t="s">
+        <v>82</v>
+      </c>
+      <c r="K68" s="31" t="s">
+        <v>82</v>
+      </c>
+      <c r="L68" s="31" t="s">
         <v>83</v>
       </c>
       <c r="M68" s="29" t="str">
@@ -28218,24 +28239,24 @@
       </c>
     </row>
     <row r="69" spans="1:13" ht="16">
-      <c r="A69" s="30"/>
-      <c r="B69" s="30"/>
+      <c r="A69" s="31"/>
+      <c r="B69" s="31"/>
       <c r="C69" s="6" t="s">
         <v>859</v>
       </c>
-      <c r="D69" s="30"/>
-      <c r="E69" s="30"/>
-      <c r="F69" s="30"/>
-      <c r="G69" s="30"/>
+      <c r="D69" s="31"/>
+      <c r="E69" s="31"/>
+      <c r="F69" s="31"/>
+      <c r="G69" s="31"/>
       <c r="H69" s="29"/>
-      <c r="I69" s="30"/>
-      <c r="J69" s="30"/>
-      <c r="K69" s="30"/>
-      <c r="L69" s="30"/>
+      <c r="I69" s="31"/>
+      <c r="J69" s="31"/>
+      <c r="K69" s="31"/>
+      <c r="L69" s="31"/>
       <c r="M69" s="29"/>
     </row>
     <row r="70" spans="1:13" ht="28">
-      <c r="A70" s="31" t="s">
+      <c r="A70" s="32" t="s">
         <v>860</v>
       </c>
       <c r="B70" s="16" t="s">
@@ -28281,7 +28302,7 @@
       </c>
     </row>
     <row r="71" spans="1:13" ht="51">
-      <c r="A71" s="31"/>
+      <c r="A71" s="32"/>
       <c r="B71" s="16" t="s">
         <v>100</v>
       </c>
@@ -28325,7 +28346,7 @@
       </c>
     </row>
     <row r="72" spans="1:13" ht="28">
-      <c r="A72" s="31"/>
+      <c r="A72" s="32"/>
       <c r="B72" s="16" t="s">
         <v>745</v>
       </c>
@@ -28369,7 +28390,7 @@
       </c>
     </row>
     <row r="73" spans="1:13" ht="28">
-      <c r="A73" s="31"/>
+      <c r="A73" s="32"/>
       <c r="B73" s="16" t="s">
         <v>867</v>
       </c>
@@ -28931,15 +28952,6 @@
     </row>
   </sheetData>
   <mergeCells count="23">
-    <mergeCell ref="A2:A7"/>
-    <mergeCell ref="A8:A14"/>
-    <mergeCell ref="A25:A29"/>
-    <mergeCell ref="A15:A24"/>
-    <mergeCell ref="A49:A56"/>
-    <mergeCell ref="A44:A48"/>
-    <mergeCell ref="A41:A43"/>
-    <mergeCell ref="A30:A36"/>
-    <mergeCell ref="A37:A40"/>
     <mergeCell ref="M68:M69"/>
     <mergeCell ref="H68:H69"/>
     <mergeCell ref="A74:A85"/>
@@ -28954,6 +28966,15 @@
     <mergeCell ref="B68:B69"/>
     <mergeCell ref="D68:D69"/>
     <mergeCell ref="E68:E69"/>
+    <mergeCell ref="A2:A7"/>
+    <mergeCell ref="A8:A14"/>
+    <mergeCell ref="A25:A29"/>
+    <mergeCell ref="A15:A24"/>
+    <mergeCell ref="A49:A56"/>
+    <mergeCell ref="A44:A48"/>
+    <mergeCell ref="A41:A43"/>
+    <mergeCell ref="A30:A36"/>
+    <mergeCell ref="A37:A40"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -29807,7 +29828,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C51FC597-29FA-1D4E-A4C8-B79027768242}">
   <dimension ref="A1:G9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="163" workbookViewId="0">
+    <sheetView zoomScale="163" workbookViewId="0">
       <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
@@ -30022,7 +30043,64 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{48D12478-9988-534B-8D3B-482A1C74F489}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="222" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <cols>
+    <col min="2" max="2" width="18.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" t="s">
+        <v>954</v>
+      </c>
+      <c r="B1" t="s">
+        <v>955</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>956</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="633f040f-4953-46e7-8610-82b0c5296ba0">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="f62ef740-d444-4f18-80a2-7590fdcab1ce" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x0101009A9CE0B21D9C3A45B31425227616CD6F" ma:contentTypeVersion="12" ma:contentTypeDescription="Creare un nuovo documento." ma:contentTypeScope="" ma:versionID="577a0f91e6a70618273620f4b28b7476">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="633f040f-4953-46e7-8610-82b0c5296ba0" xmlns:ns3="f62ef740-d444-4f18-80a2-7590fdcab1ce" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="0eeb42859aa2ae2e58f994ed451e965e" ns2:_="" ns3:_="">
     <xsd:import namespace="633f040f-4953-46e7-8610-82b0c5296ba0"/>
@@ -30239,27 +30317,32 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{83D5100D-0E56-4B30-B42D-2AEC6B837C39}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="633f040f-4953-46e7-8610-82b0c5296ba0"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="f62ef740-d444-4f18-80a2-7590fdcab1ce"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="633f040f-4953-46e7-8610-82b0c5296ba0">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="f62ef740-d444-4f18-80a2-7590fdcab1ce" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2C6CC7BA-2E2C-4B0D-8103-11A51D82E8EC}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2F919C9F-DDA6-4ECE-8C26-43CAC964EF66}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -30276,29 +30359,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2C6CC7BA-2E2C-4B0D-8103-11A51D82E8EC}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{83D5100D-0E56-4B30-B42D-2AEC6B837C39}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="633f040f-4953-46e7-8610-82b0c5296ba0"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="f62ef740-d444-4f18-80a2-7590fdcab1ce"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Inizio introduizione fasi di pentest
</commit_message>
<xml_diff>
--- a/apps/static/assets/dbs/ThreatCatalogComplete.xlsx
+++ b/apps/static/assets/dbs/ThreatCatalogComplete.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fefox/Desktop/WebApp/apps/static/assets/dbs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D64E7C08-6E7B-EB44-8A24-C67577B785E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{09EA075B-9C8B-3E48-9639-9BBCA5719138}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16280" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16280" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Threat Components" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
   </definedNames>
   <calcPr calcId="191028"/>
   <pivotCaches>
-    <pivotCache cacheId="0" r:id="rId7"/>
+    <pivotCache cacheId="2" r:id="rId7"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4205" uniqueCount="957">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4205" uniqueCount="956">
   <si>
     <t>TID</t>
   </si>
@@ -2946,9 +2946,6 @@
   </si>
   <si>
     <t>This is a guided tool, so the parameters have to be specified during its use.</t>
-  </si>
-  <si>
-    <t>Phase</t>
   </si>
   <si>
     <t>PhaseID</t>
@@ -3169,14 +3166,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -8268,7 +8265,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{48CB07D6-9F6C-094F-A3D3-916741F281CD}" name="Tabella pivot1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valori" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{48CB07D6-9F6C-094F-A3D3-916741F281CD}" name="Tabella pivot1" cacheId="2" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valori" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A1:B25" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="14">
     <pivotField showAll="0"/>
@@ -8471,7 +8468,7 @@
     <tableColumn id="6" xr3:uid="{1E4A4CA6-7FF1-6543-A718-93EC7B5F1624}" name="CypherQuery" dataDxfId="4"/>
     <tableColumn id="3" xr3:uid="{52487567-ED26-B840-ABFD-DB1BF72A83C9}" name="Command" dataDxfId="3"/>
     <tableColumn id="5" xr3:uid="{0296B95F-6562-0746-B0C6-FE3564F6272C}" name="Description" dataDxfId="2"/>
-    <tableColumn id="7" xr3:uid="{FF0722DB-3140-904D-9B8E-A0C7B3C1FFEF}" name="Phase" dataDxfId="1"/>
+    <tableColumn id="7" xr3:uid="{FF0722DB-3140-904D-9B8E-A0C7B3C1FFEF}" name="PhaseID" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -26640,7 +26637,7 @@
       </c>
     </row>
     <row r="30" spans="1:13" ht="48">
-      <c r="A30" s="30" t="s">
+      <c r="A30" s="32" t="s">
         <v>793</v>
       </c>
       <c r="B30" s="5" t="s">
@@ -26683,7 +26680,7 @@
       </c>
     </row>
     <row r="31" spans="1:13" ht="48">
-      <c r="A31" s="30"/>
+      <c r="A31" s="32"/>
       <c r="B31" s="5" t="s">
         <v>796</v>
       </c>
@@ -26724,7 +26721,7 @@
       </c>
     </row>
     <row r="32" spans="1:13" ht="32">
-      <c r="A32" s="30"/>
+      <c r="A32" s="32"/>
       <c r="B32" s="5" t="s">
         <v>798</v>
       </c>
@@ -26765,7 +26762,7 @@
       </c>
     </row>
     <row r="33" spans="1:13" ht="96">
-      <c r="A33" s="30"/>
+      <c r="A33" s="32"/>
       <c r="B33" s="5" t="s">
         <v>100</v>
       </c>
@@ -26806,7 +26803,7 @@
       </c>
     </row>
     <row r="34" spans="1:13" ht="32">
-      <c r="A34" s="30"/>
+      <c r="A34" s="32"/>
       <c r="B34" s="5" t="s">
         <v>801</v>
       </c>
@@ -26847,7 +26844,7 @@
       </c>
     </row>
     <row r="35" spans="1:13" ht="32">
-      <c r="A35" s="30"/>
+      <c r="A35" s="32"/>
       <c r="B35" s="5" t="s">
         <v>201</v>
       </c>
@@ -26888,7 +26885,7 @@
       </c>
     </row>
     <row r="36" spans="1:13" ht="80">
-      <c r="A36" s="30"/>
+      <c r="A36" s="32"/>
       <c r="B36" s="5" t="s">
         <v>804</v>
       </c>
@@ -27427,7 +27424,7 @@
       </c>
     </row>
     <row r="49" spans="1:13" ht="78" customHeight="1">
-      <c r="A49" s="30" t="s">
+      <c r="A49" s="32" t="s">
         <v>822</v>
       </c>
       <c r="B49" s="5" t="s">
@@ -27470,7 +27467,7 @@
       </c>
     </row>
     <row r="50" spans="1:13" ht="32">
-      <c r="A50" s="30"/>
+      <c r="A50" s="32"/>
       <c r="B50" s="5" t="s">
         <v>613</v>
       </c>
@@ -27511,7 +27508,7 @@
       </c>
     </row>
     <row r="51" spans="1:13" ht="16">
-      <c r="A51" s="30"/>
+      <c r="A51" s="32"/>
       <c r="B51" s="5" t="s">
         <v>201</v>
       </c>
@@ -27552,7 +27549,7 @@
       </c>
     </row>
     <row r="52" spans="1:13" ht="32">
-      <c r="A52" s="30"/>
+      <c r="A52" s="32"/>
       <c r="B52" s="5" t="s">
         <v>827</v>
       </c>
@@ -27593,7 +27590,7 @@
       </c>
     </row>
     <row r="53" spans="1:13" ht="96">
-      <c r="A53" s="30"/>
+      <c r="A53" s="32"/>
       <c r="B53" s="5" t="s">
         <v>829</v>
       </c>
@@ -27634,7 +27631,7 @@
       </c>
     </row>
     <row r="54" spans="1:13">
-      <c r="A54" s="30"/>
+      <c r="A54" s="32"/>
       <c r="B54" s="5" t="s">
         <v>831</v>
       </c>
@@ -27675,7 +27672,7 @@
       </c>
     </row>
     <row r="55" spans="1:13" ht="64">
-      <c r="A55" s="30"/>
+      <c r="A55" s="32"/>
       <c r="B55" s="5" t="s">
         <v>833</v>
       </c>
@@ -27716,7 +27713,7 @@
       </c>
     </row>
     <row r="56" spans="1:13" ht="64">
-      <c r="A56" s="30"/>
+      <c r="A56" s="32"/>
       <c r="B56" s="5" t="s">
         <v>835</v>
       </c>
@@ -27757,7 +27754,7 @@
       </c>
     </row>
     <row r="57" spans="1:13" ht="32">
-      <c r="A57" s="31" t="s">
+      <c r="A57" s="30" t="s">
         <v>837</v>
       </c>
       <c r="B57" s="6" t="s">
@@ -27799,7 +27796,7 @@
       </c>
     </row>
     <row r="58" spans="1:13" ht="80">
-      <c r="A58" s="31"/>
+      <c r="A58" s="30"/>
       <c r="B58" s="7" t="s">
         <v>840</v>
       </c>
@@ -27839,7 +27836,7 @@
       </c>
     </row>
     <row r="59" spans="1:13" ht="64" customHeight="1">
-      <c r="A59" s="31"/>
+      <c r="A59" s="30"/>
       <c r="B59" s="7" t="s">
         <v>842</v>
       </c>
@@ -27879,7 +27876,7 @@
       </c>
     </row>
     <row r="60" spans="1:13" ht="16">
-      <c r="A60" s="31"/>
+      <c r="A60" s="30"/>
       <c r="B60" s="7" t="s">
         <v>95</v>
       </c>
@@ -27919,7 +27916,7 @@
       </c>
     </row>
     <row r="61" spans="1:13" ht="32">
-      <c r="A61" s="31"/>
+      <c r="A61" s="30"/>
       <c r="B61" s="7" t="s">
         <v>846</v>
       </c>
@@ -27959,7 +27956,7 @@
       </c>
     </row>
     <row r="62" spans="1:13" ht="32">
-      <c r="A62" s="31"/>
+      <c r="A62" s="30"/>
       <c r="B62" s="7" t="s">
         <v>848</v>
       </c>
@@ -27999,7 +27996,7 @@
       </c>
     </row>
     <row r="63" spans="1:13" ht="16">
-      <c r="A63" s="31"/>
+      <c r="A63" s="30"/>
       <c r="B63" s="7" t="s">
         <v>851</v>
       </c>
@@ -28039,7 +28036,7 @@
       </c>
     </row>
     <row r="64" spans="1:13" ht="32">
-      <c r="A64" s="31"/>
+      <c r="A64" s="30"/>
       <c r="B64" s="6" t="s">
         <v>853</v>
       </c>
@@ -28079,7 +28076,7 @@
       </c>
     </row>
     <row r="65" spans="1:13" ht="16">
-      <c r="A65" s="31"/>
+      <c r="A65" s="30"/>
       <c r="B65" s="7" t="s">
         <v>79</v>
       </c>
@@ -28119,7 +28116,7 @@
       </c>
     </row>
     <row r="66" spans="1:13" ht="16">
-      <c r="A66" s="31"/>
+      <c r="A66" s="30"/>
       <c r="B66" s="7" t="s">
         <v>856</v>
       </c>
@@ -28159,7 +28156,7 @@
       </c>
     </row>
     <row r="67" spans="1:13" ht="48">
-      <c r="A67" s="31"/>
+      <c r="A67" s="30"/>
       <c r="B67" s="6" t="s">
         <v>92</v>
       </c>
@@ -28199,38 +28196,38 @@
       </c>
     </row>
     <row r="68" spans="1:13" ht="16">
-      <c r="A68" s="31"/>
-      <c r="B68" s="31" t="s">
+      <c r="A68" s="30"/>
+      <c r="B68" s="30" t="s">
         <v>169</v>
       </c>
       <c r="C68" s="6" t="s">
         <v>858</v>
       </c>
-      <c r="D68" s="31" t="s">
+      <c r="D68" s="30" t="s">
         <v>25</v>
       </c>
-      <c r="E68" s="31" t="s">
+      <c r="E68" s="30" t="s">
         <v>844</v>
       </c>
-      <c r="F68" s="31" t="s">
-        <v>82</v>
-      </c>
-      <c r="G68" s="31" t="s">
+      <c r="F68" s="30" t="s">
+        <v>82</v>
+      </c>
+      <c r="G68" s="30" t="s">
         <v>82</v>
       </c>
       <c r="H68" s="29" t="s">
         <v>82</v>
       </c>
-      <c r="I68" s="31" t="s">
+      <c r="I68" s="30" t="s">
         <v>181</v>
       </c>
-      <c r="J68" s="31" t="s">
-        <v>82</v>
-      </c>
-      <c r="K68" s="31" t="s">
-        <v>82</v>
-      </c>
-      <c r="L68" s="31" t="s">
+      <c r="J68" s="30" t="s">
+        <v>82</v>
+      </c>
+      <c r="K68" s="30" t="s">
+        <v>82</v>
+      </c>
+      <c r="L68" s="30" t="s">
         <v>83</v>
       </c>
       <c r="M68" s="29" t="str">
@@ -28239,24 +28236,24 @@
       </c>
     </row>
     <row r="69" spans="1:13" ht="16">
-      <c r="A69" s="31"/>
-      <c r="B69" s="31"/>
+      <c r="A69" s="30"/>
+      <c r="B69" s="30"/>
       <c r="C69" s="6" t="s">
         <v>859</v>
       </c>
-      <c r="D69" s="31"/>
-      <c r="E69" s="31"/>
-      <c r="F69" s="31"/>
-      <c r="G69" s="31"/>
+      <c r="D69" s="30"/>
+      <c r="E69" s="30"/>
+      <c r="F69" s="30"/>
+      <c r="G69" s="30"/>
       <c r="H69" s="29"/>
-      <c r="I69" s="31"/>
-      <c r="J69" s="31"/>
-      <c r="K69" s="31"/>
-      <c r="L69" s="31"/>
+      <c r="I69" s="30"/>
+      <c r="J69" s="30"/>
+      <c r="K69" s="30"/>
+      <c r="L69" s="30"/>
       <c r="M69" s="29"/>
     </row>
     <row r="70" spans="1:13" ht="28">
-      <c r="A70" s="32" t="s">
+      <c r="A70" s="31" t="s">
         <v>860</v>
       </c>
       <c r="B70" s="16" t="s">
@@ -28302,7 +28299,7 @@
       </c>
     </row>
     <row r="71" spans="1:13" ht="51">
-      <c r="A71" s="32"/>
+      <c r="A71" s="31"/>
       <c r="B71" s="16" t="s">
         <v>100</v>
       </c>
@@ -28346,7 +28343,7 @@
       </c>
     </row>
     <row r="72" spans="1:13" ht="28">
-      <c r="A72" s="32"/>
+      <c r="A72" s="31"/>
       <c r="B72" s="16" t="s">
         <v>745</v>
       </c>
@@ -28390,7 +28387,7 @@
       </c>
     </row>
     <row r="73" spans="1:13" ht="28">
-      <c r="A73" s="32"/>
+      <c r="A73" s="31"/>
       <c r="B73" s="16" t="s">
         <v>867</v>
       </c>
@@ -28952,6 +28949,15 @@
     </row>
   </sheetData>
   <mergeCells count="23">
+    <mergeCell ref="A2:A7"/>
+    <mergeCell ref="A8:A14"/>
+    <mergeCell ref="A25:A29"/>
+    <mergeCell ref="A15:A24"/>
+    <mergeCell ref="A49:A56"/>
+    <mergeCell ref="A44:A48"/>
+    <mergeCell ref="A41:A43"/>
+    <mergeCell ref="A30:A36"/>
+    <mergeCell ref="A37:A40"/>
     <mergeCell ref="M68:M69"/>
     <mergeCell ref="H68:H69"/>
     <mergeCell ref="A74:A85"/>
@@ -28966,15 +28972,6 @@
     <mergeCell ref="B68:B69"/>
     <mergeCell ref="D68:D69"/>
     <mergeCell ref="E68:E69"/>
-    <mergeCell ref="A2:A7"/>
-    <mergeCell ref="A8:A14"/>
-    <mergeCell ref="A25:A29"/>
-    <mergeCell ref="A15:A24"/>
-    <mergeCell ref="A49:A56"/>
-    <mergeCell ref="A44:A48"/>
-    <mergeCell ref="A41:A43"/>
-    <mergeCell ref="A30:A36"/>
-    <mergeCell ref="A37:A40"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -29828,8 +29825,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C51FC597-29FA-1D4E-A4C8-B79027768242}">
   <dimension ref="A1:G9"/>
   <sheetViews>
-    <sheetView zoomScale="163" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+    <sheetView tabSelected="1" zoomScale="163" workbookViewId="0">
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15"/>
@@ -30047,8 +30044,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{48D12478-9988-534B-8D3B-482A1C74F489}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="222" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView zoomScale="222" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -30058,10 +30055,10 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
+        <v>953</v>
+      </c>
+      <c r="B1" t="s">
         <v>954</v>
-      </c>
-      <c r="B1" t="s">
-        <v>955</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -30069,7 +30066,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>956</v>
+        <v>955</v>
       </c>
     </row>
   </sheetData>
@@ -30081,6 +30078,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <lcf76f155ced4ddcb4097134ff3c332f xmlns="633f040f-4953-46e7-8610-82b0c5296ba0">
@@ -30089,15 +30095,6 @@
     <TaxCatchAll xmlns="f62ef740-d444-4f18-80a2-7590fdcab1ce" xsi:nil="true"/>
   </documentManagement>
 </p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -30318,26 +30315,26 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{83D5100D-0E56-4B30-B42D-2AEC6B837C39}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2C6CC7BA-2E2C-4B0D-8103-11A51D82E8EC}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="633f040f-4953-46e7-8610-82b0c5296ba0"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="f62ef740-d444-4f18-80a2-7590fdcab1ce"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2C6CC7BA-2E2C-4B0D-8103-11A51D82E8EC}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{83D5100D-0E56-4B30-B42D-2AEC6B837C39}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="f62ef740-d444-4f18-80a2-7590fdcab1ce"/>
+    <ds:schemaRef ds:uri="633f040f-4953-46e7-8610-82b0c5296ba0"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Aggiunto supporto a più fasi per i tool
</commit_message>
<xml_diff>
--- a/apps/static/assets/dbs/ThreatCatalogComplete.xlsx
+++ b/apps/static/assets/dbs/ThreatCatalogComplete.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fefox/Desktop/WebApp/apps/static/assets/dbs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D7348373-BEC2-2B49-93A5-2E6AFA591C0D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{2F91EC13-0121-F548-AA44-383F9ACC0960}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="800" yWindow="500" windowWidth="14400" windowHeight="16280" firstSheet="1" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-38400" yWindow="-3100" windowWidth="38400" windowHeight="21100" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Threat Components" sheetId="1" r:id="rId1"/>
@@ -3656,9 +3656,6 @@
     <t>Illicit improvement of a specific product or production capability, The primary target is to acquire production processes or assets rather than a business process</t>
   </si>
   <si>
-    <t>8, 19</t>
-  </si>
-  <si>
     <t>Discovery of active hosts.</t>
   </si>
   <si>
@@ -3684,6 +3681,9 @@
   </si>
   <si>
     <t>Enumeration (Collection)</t>
+  </si>
+  <si>
+    <t>8, 17</t>
   </si>
 </sst>
 </file>
@@ -4068,14 +4068,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -9314,7 +9314,7 @@
   <autoFilter ref="A1:R322" xr:uid="{DEFAB213-4389-184E-911C-CDCC8CABBD38}">
     <filterColumn colId="1">
       <filters>
-        <filter val="Device.MEC"/>
+        <filter val="Service.VM"/>
       </filters>
     </filterColumn>
   </autoFilter>
@@ -9667,8 +9667,8 @@
   <dimension ref="A1:R322"/>
   <sheetViews>
     <sheetView topLeftCell="D1" zoomScale="125" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F19" sqref="F19"/>
+      <pane ySplit="1" topLeftCell="A287" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C106" sqref="C106"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -9748,7 +9748,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:18" ht="48">
+    <row r="2" spans="1:18" ht="48" hidden="1">
       <c r="A2" s="20" t="str">
         <f t="shared" ref="A2:A64" si="0">CONCATENATE("T",ROW(A2)-1)</f>
         <v>T1</v>
@@ -9801,7 +9801,7 @@
       <c r="Q2" s="24"/>
       <c r="R2" s="24"/>
     </row>
-    <row r="3" spans="1:18" ht="32">
+    <row r="3" spans="1:18" ht="32" hidden="1">
       <c r="A3" s="20" t="str">
         <f t="shared" si="0"/>
         <v>T2</v>
@@ -9854,7 +9854,7 @@
       <c r="Q3" s="24"/>
       <c r="R3" s="24"/>
     </row>
-    <row r="4" spans="1:18" ht="80">
+    <row r="4" spans="1:18" ht="80" hidden="1">
       <c r="A4" s="20" t="str">
         <f t="shared" si="0"/>
         <v>T3</v>
@@ -9907,7 +9907,7 @@
       <c r="Q4" s="24"/>
       <c r="R4" s="24"/>
     </row>
-    <row r="5" spans="1:18" ht="32">
+    <row r="5" spans="1:18" ht="32" hidden="1">
       <c r="A5" s="20" t="str">
         <f t="shared" si="0"/>
         <v>T4</v>
@@ -9960,7 +9960,7 @@
       <c r="Q5" s="24"/>
       <c r="R5" s="24"/>
     </row>
-    <row r="6" spans="1:18" ht="48">
+    <row r="6" spans="1:18" ht="48" hidden="1">
       <c r="A6" s="20" t="str">
         <f t="shared" si="0"/>
         <v>T5</v>
@@ -10013,7 +10013,7 @@
       <c r="Q6" s="24"/>
       <c r="R6" s="24"/>
     </row>
-    <row r="7" spans="1:18" ht="48">
+    <row r="7" spans="1:18" ht="48" hidden="1">
       <c r="A7" s="20" t="str">
         <f t="shared" si="0"/>
         <v>T6</v>
@@ -10066,7 +10066,7 @@
       <c r="Q7" s="24"/>
       <c r="R7" s="24"/>
     </row>
-    <row r="8" spans="1:18" ht="48">
+    <row r="8" spans="1:18" ht="48" hidden="1">
       <c r="A8" s="20" t="str">
         <f t="shared" si="0"/>
         <v>T7</v>
@@ -10119,7 +10119,7 @@
       <c r="Q8" s="24"/>
       <c r="R8" s="24"/>
     </row>
-    <row r="9" spans="1:18" ht="16">
+    <row r="9" spans="1:18" ht="16" hidden="1">
       <c r="A9" s="20" t="str">
         <f t="shared" si="0"/>
         <v>T8</v>
@@ -10172,7 +10172,7 @@
       <c r="Q9" s="24"/>
       <c r="R9" s="24"/>
     </row>
-    <row r="10" spans="1:18" ht="32">
+    <row r="10" spans="1:18" ht="32" hidden="1">
       <c r="A10" s="20" t="str">
         <f t="shared" si="0"/>
         <v>T9</v>
@@ -10225,7 +10225,7 @@
       <c r="Q10" s="24"/>
       <c r="R10" s="24"/>
     </row>
-    <row r="11" spans="1:18" ht="32">
+    <row r="11" spans="1:18" ht="32" hidden="1">
       <c r="A11" s="20" t="str">
         <f t="shared" si="0"/>
         <v>T10</v>
@@ -10278,7 +10278,7 @@
       <c r="Q11" s="24"/>
       <c r="R11" s="24"/>
     </row>
-    <row r="12" spans="1:18" ht="48">
+    <row r="12" spans="1:18" ht="48" hidden="1">
       <c r="A12" s="20" t="str">
         <f t="shared" si="0"/>
         <v>T11</v>
@@ -10331,7 +10331,7 @@
       <c r="Q12" s="24"/>
       <c r="R12" s="24"/>
     </row>
-    <row r="13" spans="1:18" ht="64">
+    <row r="13" spans="1:18" ht="64" hidden="1">
       <c r="A13" s="20" t="str">
         <f t="shared" si="0"/>
         <v>T12</v>
@@ -10384,7 +10384,7 @@
       <c r="Q13" s="24"/>
       <c r="R13" s="24"/>
     </row>
-    <row r="14" spans="1:18" ht="48">
+    <row r="14" spans="1:18" ht="48" hidden="1">
       <c r="A14" s="20" t="str">
         <f t="shared" si="0"/>
         <v>T13</v>
@@ -10437,7 +10437,7 @@
       <c r="Q14" s="24"/>
       <c r="R14" s="24"/>
     </row>
-    <row r="15" spans="1:18" ht="80">
+    <row r="15" spans="1:18" ht="80" hidden="1">
       <c r="A15" s="20" t="str">
         <f t="shared" si="0"/>
         <v>T14</v>
@@ -10490,7 +10490,7 @@
       <c r="Q15" s="24"/>
       <c r="R15" s="24"/>
     </row>
-    <row r="16" spans="1:18" ht="32">
+    <row r="16" spans="1:18" ht="32" hidden="1">
       <c r="A16" s="20" t="str">
         <f t="shared" si="0"/>
         <v>T15</v>
@@ -10543,7 +10543,7 @@
       <c r="Q16" s="24"/>
       <c r="R16" s="24"/>
     </row>
-    <row r="17" spans="1:18" ht="32">
+    <row r="17" spans="1:18" ht="32" hidden="1">
       <c r="A17" s="20" t="str">
         <f t="shared" si="0"/>
         <v>T16</v>
@@ -10596,7 +10596,7 @@
       <c r="Q17" s="24"/>
       <c r="R17" s="24"/>
     </row>
-    <row r="18" spans="1:18" ht="48">
+    <row r="18" spans="1:18" ht="48" hidden="1">
       <c r="A18" s="20" t="str">
         <f t="shared" si="0"/>
         <v>T17</v>
@@ -10649,7 +10649,7 @@
       <c r="Q18" s="24"/>
       <c r="R18" s="24"/>
     </row>
-    <row r="19" spans="1:18" ht="32">
+    <row r="19" spans="1:18" ht="32" hidden="1">
       <c r="A19" s="20" t="str">
         <f t="shared" si="0"/>
         <v>T18</v>
@@ -10702,7 +10702,7 @@
       <c r="Q19" s="24"/>
       <c r="R19" s="24"/>
     </row>
-    <row r="20" spans="1:18" ht="48">
+    <row r="20" spans="1:18" ht="48" hidden="1">
       <c r="A20" s="20" t="str">
         <f t="shared" si="0"/>
         <v>T19</v>
@@ -10755,7 +10755,7 @@
       <c r="Q20" s="24"/>
       <c r="R20" s="24"/>
     </row>
-    <row r="21" spans="1:18" ht="48">
+    <row r="21" spans="1:18" ht="48" hidden="1">
       <c r="A21" s="20" t="str">
         <f t="shared" si="0"/>
         <v>T20</v>
@@ -10808,7 +10808,7 @@
       <c r="Q21" s="24"/>
       <c r="R21" s="24"/>
     </row>
-    <row r="22" spans="1:18" ht="48">
+    <row r="22" spans="1:18" ht="48" hidden="1">
       <c r="A22" s="20" t="str">
         <f t="shared" si="0"/>
         <v>T21</v>
@@ -10861,7 +10861,7 @@
       <c r="Q22" s="24"/>
       <c r="R22" s="24"/>
     </row>
-    <row r="23" spans="1:18" ht="48">
+    <row r="23" spans="1:18" ht="48" hidden="1">
       <c r="A23" s="20" t="str">
         <f t="shared" si="0"/>
         <v>T22</v>
@@ -24164,7 +24164,7 @@
       </c>
       <c r="R274" s="24"/>
     </row>
-    <row r="275" spans="1:18" ht="96" hidden="1">
+    <row r="275" spans="1:18" ht="96">
       <c r="A275" s="20" t="str">
         <f t="shared" si="40"/>
         <v>T274</v>
@@ -24221,7 +24221,7 @@
       </c>
       <c r="R275" s="24"/>
     </row>
-    <row r="276" spans="1:18" ht="80" hidden="1">
+    <row r="276" spans="1:18" ht="80">
       <c r="A276" s="20" t="str">
         <f t="shared" si="40"/>
         <v>T275</v>
@@ -24278,7 +24278,7 @@
       </c>
       <c r="R276" s="24"/>
     </row>
-    <row r="277" spans="1:18" ht="64" hidden="1">
+    <row r="277" spans="1:18" ht="64">
       <c r="A277" s="20" t="str">
         <f t="shared" si="40"/>
         <v>T276</v>
@@ -24335,7 +24335,7 @@
       </c>
       <c r="R277" s="24"/>
     </row>
-    <row r="278" spans="1:18" ht="96" hidden="1">
+    <row r="278" spans="1:18" ht="96">
       <c r="A278" s="20" t="str">
         <f t="shared" si="40"/>
         <v>T277</v>
@@ -24396,7 +24396,7 @@
       </c>
       <c r="R278" s="24"/>
     </row>
-    <row r="279" spans="1:18" ht="32" hidden="1">
+    <row r="279" spans="1:18" ht="32">
       <c r="A279" s="20" t="str">
         <f t="shared" si="40"/>
         <v>T278</v>
@@ -24453,7 +24453,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="280" spans="1:18" ht="48" hidden="1">
+    <row r="280" spans="1:18" ht="48">
       <c r="A280" s="20" t="str">
         <f t="shared" si="40"/>
         <v>T279</v>
@@ -24514,7 +24514,7 @@
       </c>
       <c r="R280" s="24"/>
     </row>
-    <row r="281" spans="1:18" ht="48" hidden="1">
+    <row r="281" spans="1:18" ht="48">
       <c r="A281" s="20" t="str">
         <f t="shared" si="40"/>
         <v>T280</v>
@@ -24575,7 +24575,7 @@
       </c>
       <c r="R281" s="24"/>
     </row>
-    <row r="282" spans="1:18" ht="32" hidden="1">
+    <row r="282" spans="1:18" ht="32">
       <c r="A282" s="20" t="str">
         <f t="shared" si="40"/>
         <v>T281</v>
@@ -24636,7 +24636,7 @@
       </c>
       <c r="R282" s="24"/>
     </row>
-    <row r="283" spans="1:18" ht="80" hidden="1">
+    <row r="283" spans="1:18" ht="80">
       <c r="A283" s="20" t="str">
         <f t="shared" si="40"/>
         <v>T282</v>
@@ -24695,7 +24695,7 @@
       <c r="Q283" s="24"/>
       <c r="R283" s="24"/>
     </row>
-    <row r="284" spans="1:18" ht="160" hidden="1">
+    <row r="284" spans="1:18" ht="160">
       <c r="A284" s="20" t="str">
         <f t="shared" si="40"/>
         <v>T283</v>
@@ -24756,7 +24756,7 @@
       </c>
       <c r="R284" s="24"/>
     </row>
-    <row r="285" spans="1:18" ht="128" hidden="1">
+    <row r="285" spans="1:18" ht="128">
       <c r="A285" s="20" t="str">
         <f t="shared" si="40"/>
         <v>T284</v>
@@ -24817,7 +24817,7 @@
       </c>
       <c r="R285" s="24"/>
     </row>
-    <row r="286" spans="1:18" ht="48" hidden="1">
+    <row r="286" spans="1:18" ht="48">
       <c r="A286" s="20" t="str">
         <f t="shared" si="40"/>
         <v>T285</v>
@@ -24878,7 +24878,7 @@
       </c>
       <c r="R286" s="24"/>
     </row>
-    <row r="287" spans="1:18" ht="96" hidden="1">
+    <row r="287" spans="1:18" ht="96">
       <c r="A287" s="20" t="str">
         <f t="shared" si="40"/>
         <v>T286</v>
@@ -24939,7 +24939,7 @@
       </c>
       <c r="R287" s="24"/>
     </row>
-    <row r="288" spans="1:18" ht="96" hidden="1">
+    <row r="288" spans="1:18" ht="96">
       <c r="A288" s="20" t="str">
         <f t="shared" si="40"/>
         <v>T287</v>
@@ -25000,7 +25000,7 @@
       </c>
       <c r="R288" s="24"/>
     </row>
-    <row r="289" spans="1:18" ht="240" hidden="1">
+    <row r="289" spans="1:18" ht="240">
       <c r="A289" s="20" t="str">
         <f t="shared" si="40"/>
         <v>T288</v>
@@ -26507,7 +26507,7 @@
       <c r="Q313" s="24"/>
       <c r="R313" s="24"/>
     </row>
-    <row r="314" spans="1:18" ht="96">
+    <row r="314" spans="1:18" ht="96" hidden="1">
       <c r="A314" s="20" t="str">
         <f t="shared" ref="A314:A320" si="53">CONCATENATE("T",ROW(A314)-1)</f>
         <v>T313</v>
@@ -26558,7 +26558,7 @@
       <c r="Q314" s="24"/>
       <c r="R314" s="24"/>
     </row>
-    <row r="315" spans="1:18" ht="32">
+    <row r="315" spans="1:18" ht="32" hidden="1">
       <c r="A315" s="20" t="str">
         <f t="shared" si="53"/>
         <v>T314</v>
@@ -26609,7 +26609,7 @@
       <c r="Q315" s="24"/>
       <c r="R315" s="24"/>
     </row>
-    <row r="316" spans="1:18" ht="80">
+    <row r="316" spans="1:18" ht="80" hidden="1">
       <c r="A316" s="20" t="str">
         <f t="shared" si="53"/>
         <v>T315</v>
@@ -26660,7 +26660,7 @@
       <c r="Q316" s="24"/>
       <c r="R316" s="24"/>
     </row>
-    <row r="317" spans="1:18" ht="96">
+    <row r="317" spans="1:18" ht="96" hidden="1">
       <c r="A317" s="20" t="str">
         <f t="shared" si="53"/>
         <v>T316</v>
@@ -26711,7 +26711,7 @@
       <c r="Q317" s="24"/>
       <c r="R317" s="24"/>
     </row>
-    <row r="318" spans="1:18" ht="64">
+    <row r="318" spans="1:18" ht="64" hidden="1">
       <c r="A318" s="20" t="str">
         <f t="shared" si="53"/>
         <v>T317</v>
@@ -26762,7 +26762,7 @@
       <c r="Q318" s="24"/>
       <c r="R318" s="24"/>
     </row>
-    <row r="319" spans="1:18" ht="112">
+    <row r="319" spans="1:18" ht="112" hidden="1">
       <c r="A319" s="20" t="str">
         <f t="shared" si="53"/>
         <v>T318</v>
@@ -26813,7 +26813,7 @@
       <c r="Q319" s="24"/>
       <c r="R319" s="24"/>
     </row>
-    <row r="320" spans="1:18" ht="64">
+    <row r="320" spans="1:18" ht="64" hidden="1">
       <c r="A320" s="20" t="str">
         <f t="shared" si="53"/>
         <v>T319</v>
@@ -26864,7 +26864,7 @@
       <c r="Q320" s="24"/>
       <c r="R320" s="24"/>
     </row>
-    <row r="321" spans="1:18" ht="16">
+    <row r="321" spans="1:18" ht="16" hidden="1">
       <c r="A321" s="20" t="str">
         <f t="shared" ref="A321:A322" si="56">CONCATENATE("T",ROW(A321)-1)</f>
         <v>T320</v>
@@ -26915,7 +26915,7 @@
       <c r="Q321" s="24"/>
       <c r="R321" s="24"/>
     </row>
-    <row r="322" spans="1:18" ht="80">
+    <row r="322" spans="1:18" ht="80" hidden="1">
       <c r="A322" s="20" t="str">
         <f t="shared" si="56"/>
         <v>T321</v>
@@ -28813,7 +28813,7 @@
       </c>
     </row>
     <row r="30" spans="1:13" ht="48">
-      <c r="A30" s="54" t="s">
+      <c r="A30" s="56" t="s">
         <v>811</v>
       </c>
       <c r="B30" s="5" t="s">
@@ -28856,7 +28856,7 @@
       </c>
     </row>
     <row r="31" spans="1:13" ht="48">
-      <c r="A31" s="54"/>
+      <c r="A31" s="56"/>
       <c r="B31" s="5" t="s">
         <v>814</v>
       </c>
@@ -28897,7 +28897,7 @@
       </c>
     </row>
     <row r="32" spans="1:13" ht="32">
-      <c r="A32" s="54"/>
+      <c r="A32" s="56"/>
       <c r="B32" s="5" t="s">
         <v>816</v>
       </c>
@@ -28938,7 +28938,7 @@
       </c>
     </row>
     <row r="33" spans="1:13" ht="96">
-      <c r="A33" s="54"/>
+      <c r="A33" s="56"/>
       <c r="B33" s="5" t="s">
         <v>100</v>
       </c>
@@ -28979,7 +28979,7 @@
       </c>
     </row>
     <row r="34" spans="1:13" ht="32">
-      <c r="A34" s="54"/>
+      <c r="A34" s="56"/>
       <c r="B34" s="5" t="s">
         <v>819</v>
       </c>
@@ -29020,7 +29020,7 @@
       </c>
     </row>
     <row r="35" spans="1:13" ht="32">
-      <c r="A35" s="54"/>
+      <c r="A35" s="56"/>
       <c r="B35" s="5" t="s">
         <v>201</v>
       </c>
@@ -29061,7 +29061,7 @@
       </c>
     </row>
     <row r="36" spans="1:13" ht="80">
-      <c r="A36" s="54"/>
+      <c r="A36" s="56"/>
       <c r="B36" s="5" t="s">
         <v>822</v>
       </c>
@@ -29600,7 +29600,7 @@
       </c>
     </row>
     <row r="49" spans="1:13" ht="78" customHeight="1">
-      <c r="A49" s="54" t="s">
+      <c r="A49" s="56" t="s">
         <v>840</v>
       </c>
       <c r="B49" s="5" t="s">
@@ -29643,7 +29643,7 @@
       </c>
     </row>
     <row r="50" spans="1:13" ht="32">
-      <c r="A50" s="54"/>
+      <c r="A50" s="56"/>
       <c r="B50" s="5" t="s">
         <v>613</v>
       </c>
@@ -29684,7 +29684,7 @@
       </c>
     </row>
     <row r="51" spans="1:13" ht="16">
-      <c r="A51" s="54"/>
+      <c r="A51" s="56"/>
       <c r="B51" s="5" t="s">
         <v>201</v>
       </c>
@@ -29725,7 +29725,7 @@
       </c>
     </row>
     <row r="52" spans="1:13" ht="32">
-      <c r="A52" s="54"/>
+      <c r="A52" s="56"/>
       <c r="B52" s="5" t="s">
         <v>845</v>
       </c>
@@ -29766,7 +29766,7 @@
       </c>
     </row>
     <row r="53" spans="1:13" ht="96">
-      <c r="A53" s="54"/>
+      <c r="A53" s="56"/>
       <c r="B53" s="5" t="s">
         <v>847</v>
       </c>
@@ -29807,7 +29807,7 @@
       </c>
     </row>
     <row r="54" spans="1:13">
-      <c r="A54" s="54"/>
+      <c r="A54" s="56"/>
       <c r="B54" s="5" t="s">
         <v>849</v>
       </c>
@@ -29848,7 +29848,7 @@
       </c>
     </row>
     <row r="55" spans="1:13" ht="64">
-      <c r="A55" s="54"/>
+      <c r="A55" s="56"/>
       <c r="B55" s="5" t="s">
         <v>851</v>
       </c>
@@ -29889,7 +29889,7 @@
       </c>
     </row>
     <row r="56" spans="1:13" ht="64">
-      <c r="A56" s="54"/>
+      <c r="A56" s="56"/>
       <c r="B56" s="5" t="s">
         <v>853</v>
       </c>
@@ -29930,7 +29930,7 @@
       </c>
     </row>
     <row r="57" spans="1:13" ht="32">
-      <c r="A57" s="55" t="s">
+      <c r="A57" s="54" t="s">
         <v>855</v>
       </c>
       <c r="B57" s="6" t="s">
@@ -29972,7 +29972,7 @@
       </c>
     </row>
     <row r="58" spans="1:13" ht="80">
-      <c r="A58" s="55"/>
+      <c r="A58" s="54"/>
       <c r="B58" s="7" t="s">
         <v>858</v>
       </c>
@@ -30012,7 +30012,7 @@
       </c>
     </row>
     <row r="59" spans="1:13" ht="64" customHeight="1">
-      <c r="A59" s="55"/>
+      <c r="A59" s="54"/>
       <c r="B59" s="7" t="s">
         <v>860</v>
       </c>
@@ -30052,7 +30052,7 @@
       </c>
     </row>
     <row r="60" spans="1:13" ht="16">
-      <c r="A60" s="55"/>
+      <c r="A60" s="54"/>
       <c r="B60" s="7" t="s">
         <v>95</v>
       </c>
@@ -30092,7 +30092,7 @@
       </c>
     </row>
     <row r="61" spans="1:13" ht="32">
-      <c r="A61" s="55"/>
+      <c r="A61" s="54"/>
       <c r="B61" s="7" t="s">
         <v>864</v>
       </c>
@@ -30132,7 +30132,7 @@
       </c>
     </row>
     <row r="62" spans="1:13" ht="32">
-      <c r="A62" s="55"/>
+      <c r="A62" s="54"/>
       <c r="B62" s="7" t="s">
         <v>866</v>
       </c>
@@ -30172,7 +30172,7 @@
       </c>
     </row>
     <row r="63" spans="1:13" ht="16">
-      <c r="A63" s="55"/>
+      <c r="A63" s="54"/>
       <c r="B63" s="7" t="s">
         <v>869</v>
       </c>
@@ -30212,7 +30212,7 @@
       </c>
     </row>
     <row r="64" spans="1:13" ht="32">
-      <c r="A64" s="55"/>
+      <c r="A64" s="54"/>
       <c r="B64" s="6" t="s">
         <v>871</v>
       </c>
@@ -30252,7 +30252,7 @@
       </c>
     </row>
     <row r="65" spans="1:13" ht="16">
-      <c r="A65" s="55"/>
+      <c r="A65" s="54"/>
       <c r="B65" s="7" t="s">
         <v>82</v>
       </c>
@@ -30292,7 +30292,7 @@
       </c>
     </row>
     <row r="66" spans="1:13" ht="16">
-      <c r="A66" s="55"/>
+      <c r="A66" s="54"/>
       <c r="B66" s="7" t="s">
         <v>874</v>
       </c>
@@ -30332,7 +30332,7 @@
       </c>
     </row>
     <row r="67" spans="1:13" ht="48">
-      <c r="A67" s="55"/>
+      <c r="A67" s="54"/>
       <c r="B67" s="6" t="s">
         <v>92</v>
       </c>
@@ -30372,38 +30372,38 @@
       </c>
     </row>
     <row r="68" spans="1:13" ht="16">
-      <c r="A68" s="55"/>
-      <c r="B68" s="55" t="s">
+      <c r="A68" s="54"/>
+      <c r="B68" s="54" t="s">
         <v>169</v>
       </c>
       <c r="C68" s="6" t="s">
         <v>876</v>
       </c>
-      <c r="D68" s="55" t="s">
+      <c r="D68" s="54" t="s">
         <v>27</v>
       </c>
-      <c r="E68" s="55" t="s">
+      <c r="E68" s="54" t="s">
         <v>862</v>
       </c>
-      <c r="F68" s="55" t="s">
-        <v>23</v>
-      </c>
-      <c r="G68" s="55" t="s">
+      <c r="F68" s="54" t="s">
+        <v>23</v>
+      </c>
+      <c r="G68" s="54" t="s">
         <v>23</v>
       </c>
       <c r="H68" s="53" t="s">
         <v>23</v>
       </c>
-      <c r="I68" s="55" t="s">
+      <c r="I68" s="54" t="s">
         <v>181</v>
       </c>
-      <c r="J68" s="55" t="s">
-        <v>23</v>
-      </c>
-      <c r="K68" s="55" t="s">
-        <v>23</v>
-      </c>
-      <c r="L68" s="55" t="s">
+      <c r="J68" s="54" t="s">
+        <v>23</v>
+      </c>
+      <c r="K68" s="54" t="s">
+        <v>23</v>
+      </c>
+      <c r="L68" s="54" t="s">
         <v>84</v>
       </c>
       <c r="M68" s="53" t="str">
@@ -30412,24 +30412,24 @@
       </c>
     </row>
     <row r="69" spans="1:13" ht="16">
-      <c r="A69" s="55"/>
-      <c r="B69" s="55"/>
+      <c r="A69" s="54"/>
+      <c r="B69" s="54"/>
       <c r="C69" s="6" t="s">
         <v>877</v>
       </c>
-      <c r="D69" s="55"/>
-      <c r="E69" s="55"/>
-      <c r="F69" s="55"/>
-      <c r="G69" s="55"/>
+      <c r="D69" s="54"/>
+      <c r="E69" s="54"/>
+      <c r="F69" s="54"/>
+      <c r="G69" s="54"/>
       <c r="H69" s="53"/>
-      <c r="I69" s="55"/>
-      <c r="J69" s="55"/>
-      <c r="K69" s="55"/>
-      <c r="L69" s="55"/>
+      <c r="I69" s="54"/>
+      <c r="J69" s="54"/>
+      <c r="K69" s="54"/>
+      <c r="L69" s="54"/>
       <c r="M69" s="53"/>
     </row>
     <row r="70" spans="1:13" ht="28">
-      <c r="A70" s="56" t="s">
+      <c r="A70" s="55" t="s">
         <v>878</v>
       </c>
       <c r="B70" s="16" t="s">
@@ -30475,7 +30475,7 @@
       </c>
     </row>
     <row r="71" spans="1:13" ht="51">
-      <c r="A71" s="56"/>
+      <c r="A71" s="55"/>
       <c r="B71" s="16" t="s">
         <v>100</v>
       </c>
@@ -30519,7 +30519,7 @@
       </c>
     </row>
     <row r="72" spans="1:13" ht="28">
-      <c r="A72" s="56"/>
+      <c r="A72" s="55"/>
       <c r="B72" s="16" t="s">
         <v>763</v>
       </c>
@@ -30563,7 +30563,7 @@
       </c>
     </row>
     <row r="73" spans="1:13" ht="28">
-      <c r="A73" s="56"/>
+      <c r="A73" s="55"/>
       <c r="B73" s="16" t="s">
         <v>885</v>
       </c>
@@ -31125,6 +31125,15 @@
     </row>
   </sheetData>
   <mergeCells count="23">
+    <mergeCell ref="A2:A7"/>
+    <mergeCell ref="A8:A14"/>
+    <mergeCell ref="A25:A29"/>
+    <mergeCell ref="A15:A24"/>
+    <mergeCell ref="A49:A56"/>
+    <mergeCell ref="A44:A48"/>
+    <mergeCell ref="A41:A43"/>
+    <mergeCell ref="A30:A36"/>
+    <mergeCell ref="A37:A40"/>
     <mergeCell ref="M68:M69"/>
     <mergeCell ref="H68:H69"/>
     <mergeCell ref="A74:A85"/>
@@ -31139,15 +31148,6 @@
     <mergeCell ref="B68:B69"/>
     <mergeCell ref="D68:D69"/>
     <mergeCell ref="E68:E69"/>
-    <mergeCell ref="A2:A7"/>
-    <mergeCell ref="A8:A14"/>
-    <mergeCell ref="A25:A29"/>
-    <mergeCell ref="A15:A24"/>
-    <mergeCell ref="A49:A56"/>
-    <mergeCell ref="A44:A48"/>
-    <mergeCell ref="A41:A43"/>
-    <mergeCell ref="A30:A36"/>
-    <mergeCell ref="A37:A40"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -32001,8 +32001,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C51FC597-29FA-1D4E-A4C8-B79027768242}">
   <dimension ref="A1:G9"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" zoomScale="163" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+    <sheetView zoomScale="163" workbookViewId="0">
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15"/>
@@ -32058,10 +32058,10 @@
         <v>944</v>
       </c>
       <c r="F2" s="27" t="s">
-        <v>1189</v>
+        <v>1188</v>
       </c>
       <c r="G2" s="28" t="s">
-        <v>1187</v>
+        <v>1196</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="64">
@@ -32106,7 +32106,7 @@
         <v>951</v>
       </c>
       <c r="F4" s="27" t="s">
-        <v>1190</v>
+        <v>1189</v>
       </c>
       <c r="G4" s="28">
         <v>6</v>
@@ -32130,7 +32130,7 @@
         <v>955</v>
       </c>
       <c r="F5" s="27" t="s">
-        <v>1191</v>
+        <v>1190</v>
       </c>
       <c r="G5" s="28">
         <v>5</v>
@@ -32154,7 +32154,7 @@
         <v>958</v>
       </c>
       <c r="F6" s="27" t="s">
-        <v>1188</v>
+        <v>1187</v>
       </c>
       <c r="G6" s="28">
         <v>5</v>
@@ -32178,7 +32178,7 @@
         <v>960</v>
       </c>
       <c r="F7" s="27" t="s">
-        <v>1192</v>
+        <v>1191</v>
       </c>
       <c r="G7" s="28">
         <v>5</v>
@@ -32229,15 +32229,12 @@
         <v>969</v>
       </c>
       <c r="G9" s="28" t="s">
-        <v>1187</v>
+        <v>1196</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
-  <ignoredErrors>
-    <ignoredError sqref="G2 G9" twoDigitTextYear="1"/>
-  </ignoredErrors>
   <tableParts count="1">
     <tablePart r:id="rId1"/>
   </tableParts>
@@ -32251,7 +32248,7 @@
   </sheetPr>
   <dimension ref="A1:C24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="164" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="164" workbookViewId="0">
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
@@ -32337,7 +32334,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>1196</v>
+        <v>1195</v>
       </c>
       <c r="C7">
         <f>INDEX(Tabella5[[PhaseID]:[PhaseName]],MATCH("Scanning",Tabella5[PhaseName],0),1)</f>
@@ -32373,7 +32370,7 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>1193</v>
+        <v>1192</v>
       </c>
       <c r="C10">
         <f>INDEX(Tabella5[[PhaseID]:[PhaseName]],MATCH("System Access",Tabella5[PhaseName],0),1)</f>
@@ -32386,7 +32383,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="47" t="s">
-        <v>1195</v>
+        <v>1194</v>
       </c>
       <c r="C11" s="47">
         <f>INDEX(Tabella5[[PhaseID]:[PhaseName]],MATCH("System Access",Tabella5[PhaseName],0),1)</f>
@@ -32412,7 +32409,7 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>1194</v>
+        <v>1193</v>
       </c>
       <c r="C13">
         <f>INDEX(Tabella5[[PhaseID]:[PhaseName]],MATCH("System Access",Tabella5[PhaseName],0),1)</f>
@@ -33318,6 +33315,26 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="633f040f-4953-46e7-8610-82b0c5296ba0">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="f62ef740-d444-4f18-80a2-7590fdcab1ce" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x0101009A9CE0B21D9C3A45B31425227616CD6F" ma:contentTypeVersion="12" ma:contentTypeDescription="Creare un nuovo documento." ma:contentTypeScope="" ma:versionID="577a0f91e6a70618273620f4b28b7476">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="633f040f-4953-46e7-8610-82b0c5296ba0" xmlns:ns3="f62ef740-d444-4f18-80a2-7590fdcab1ce" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="0eeb42859aa2ae2e58f994ed451e965e" ns2:_="" ns3:_="">
     <xsd:import namespace="633f040f-4953-46e7-8610-82b0c5296ba0"/>
@@ -33534,27 +33551,32 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="633f040f-4953-46e7-8610-82b0c5296ba0">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="f62ef740-d444-4f18-80a2-7590fdcab1ce" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2C6CC7BA-2E2C-4B0D-8103-11A51D82E8EC}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{83D5100D-0E56-4B30-B42D-2AEC6B837C39}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="633f040f-4953-46e7-8610-82b0c5296ba0"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="f62ef740-d444-4f18-80a2-7590fdcab1ce"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2F919C9F-DDA6-4ECE-8C26-43CAC964EF66}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -33571,29 +33593,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{83D5100D-0E56-4B30-B42D-2AEC6B837C39}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="f62ef740-d444-4f18-80a2-7590fdcab1ce"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="633f040f-4953-46e7-8610-82b0c5296ba0"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2C6CC7BA-2E2C-4B0D-8103-11A51D82E8EC}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
aggiunta possibilità di caricare il file di output di un comando.
</commit_message>
<xml_diff>
--- a/apps/static/assets/dbs/ThreatCatalogComplete.xlsx
+++ b/apps/static/assets/dbs/ThreatCatalogComplete.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11013"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fefox/Desktop/WebApp/apps/static/assets/dbs/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fefox/Desktop/AutomaticAttackPlanGenerator/apps/static/assets/dbs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2F91EC13-0121-F548-AA44-383F9ACC0960}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{8DB641AA-0336-A840-B72A-42884C5543B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38400" yWindow="-3100" windowWidth="38400" windowHeight="21100" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16260" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Threat Components" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
   </definedNames>
   <calcPr calcId="191028"/>
   <pivotCaches>
-    <pivotCache cacheId="2" r:id="rId11"/>
+    <pivotCache cacheId="3" r:id="rId11"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -51,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4663" uniqueCount="1197">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4674" uniqueCount="1202">
   <si>
     <t>TID</t>
   </si>
@@ -3684,6 +3684,21 @@
   </si>
   <si>
     <t>8, 17</t>
+  </si>
+  <si>
+    <t>IsExecutable</t>
+  </si>
+  <si>
+    <t>False</t>
+  </si>
+  <si>
+    <t>True</t>
+  </si>
+  <si>
+    <t>OutputParser</t>
+  </si>
+  <si>
+    <t>nmap_classic</t>
   </si>
 </sst>
 </file>
@@ -4081,7 +4096,7 @@
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="29">
+  <dxfs count="31">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -4091,6 +4106,12 @@
           <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
@@ -4202,6 +4223,10 @@
 </styleSheet>
 </file>
 
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Microsoft Office User" refreshedDate="45147.557552430553" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="305" xr:uid="{3720CB22-BF16-1D46-AA6B-0CE8D2023C71}">
   <cacheSource type="worksheet">
@@ -9169,7 +9194,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{48CB07D6-9F6C-094F-A3D3-916741F281CD}" name="Tabella pivot1" cacheId="2" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valori" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{48CB07D6-9F6C-094F-A3D3-916741F281CD}" name="Tabella pivot1" cacheId="3" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valori" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A1:B25" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="14">
     <pivotField showAll="0"/>
@@ -9310,44 +9335,38 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{DEFAB213-4389-184E-911C-CDCC8CABBD38}" name="Tabella1" displayName="Tabella1" ref="A1:R322" totalsRowShown="0" dataDxfId="28">
-  <autoFilter ref="A1:R322" xr:uid="{DEFAB213-4389-184E-911C-CDCC8CABBD38}">
-    <filterColumn colId="1">
-      <filters>
-        <filter val="Service.VM"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{DEFAB213-4389-184E-911C-CDCC8CABBD38}" name="Tabella1" displayName="Tabella1" ref="A1:R322" totalsRowShown="0" dataDxfId="30">
+  <autoFilter ref="A1:R322" xr:uid="{DEFAB213-4389-184E-911C-CDCC8CABBD38}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A255:R269">
     <sortCondition ref="B1:B313"/>
   </sortState>
   <tableColumns count="18">
-    <tableColumn id="16" xr3:uid="{DE426BDB-E154-EE46-B7B3-5B538C8AEC32}" name="TID" dataDxfId="27">
+    <tableColumn id="16" xr3:uid="{DE426BDB-E154-EE46-B7B3-5B538C8AEC32}" name="TID" dataDxfId="29">
       <calculatedColumnFormula>CONCATENATE("T",ROW(A2)-1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="1" xr3:uid="{A0AE63DC-99F7-7D4F-B824-AB7765893284}" name="Asset" dataDxfId="26"/>
-    <tableColumn id="2" xr3:uid="{0FA38BFF-C67B-0C43-B1BA-F6338DBFB0C8}" name="Threat" dataDxfId="25"/>
-    <tableColumn id="3" xr3:uid="{BFC77F7C-F096-8345-97EA-317816ED869D}" name="Description" dataDxfId="24"/>
-    <tableColumn id="4" xr3:uid="{258F3B86-1461-D64A-AE3B-CEAC97B2B533}" name="STRIDE" dataDxfId="23"/>
-    <tableColumn id="6" xr3:uid="{0FD06C95-5962-AC4D-B9EF-4DBB5728E736}" name="Compromised" dataDxfId="22"/>
-    <tableColumn id="7" xr3:uid="{9E5B99AD-1F1D-B44C-ABDF-6F7E9177F3DE}" name="PreC" dataDxfId="21"/>
-    <tableColumn id="8" xr3:uid="{D4F97A81-E528-2841-B4DE-321362F90F65}" name="PreI" dataDxfId="20"/>
-    <tableColumn id="9" xr3:uid="{018427D6-D385-3447-B4A4-95003B3341F6}" name="PreA" dataDxfId="19"/>
-    <tableColumn id="10" xr3:uid="{8334AC57-4A09-5744-9484-073ECEE2E513}" name="Precondition" dataDxfId="18"/>
-    <tableColumn id="12" xr3:uid="{DDBE315D-E051-2C47-A765-EE1DB2E118EA}" name="PostC" dataDxfId="17">
+    <tableColumn id="1" xr3:uid="{A0AE63DC-99F7-7D4F-B824-AB7765893284}" name="Asset" dataDxfId="28"/>
+    <tableColumn id="2" xr3:uid="{0FA38BFF-C67B-0C43-B1BA-F6338DBFB0C8}" name="Threat" dataDxfId="27"/>
+    <tableColumn id="3" xr3:uid="{BFC77F7C-F096-8345-97EA-317816ED869D}" name="Description" dataDxfId="26"/>
+    <tableColumn id="4" xr3:uid="{258F3B86-1461-D64A-AE3B-CEAC97B2B533}" name="STRIDE" dataDxfId="25"/>
+    <tableColumn id="6" xr3:uid="{0FD06C95-5962-AC4D-B9EF-4DBB5728E736}" name="Compromised" dataDxfId="24"/>
+    <tableColumn id="7" xr3:uid="{9E5B99AD-1F1D-B44C-ABDF-6F7E9177F3DE}" name="PreC" dataDxfId="23"/>
+    <tableColumn id="8" xr3:uid="{D4F97A81-E528-2841-B4DE-321362F90F65}" name="PreI" dataDxfId="22"/>
+    <tableColumn id="9" xr3:uid="{018427D6-D385-3447-B4A4-95003B3341F6}" name="PreA" dataDxfId="21"/>
+    <tableColumn id="10" xr3:uid="{8334AC57-4A09-5744-9484-073ECEE2E513}" name="Precondition" dataDxfId="20"/>
+    <tableColumn id="12" xr3:uid="{DDBE315D-E051-2C47-A765-EE1DB2E118EA}" name="PostC" dataDxfId="19">
       <calculatedColumnFormula>MID(N2,2,1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" xr3:uid="{243C1B9B-76C9-0345-B727-4F11FD75DF6B}" name="PostI" dataDxfId="16">
+    <tableColumn id="13" xr3:uid="{243C1B9B-76C9-0345-B727-4F11FD75DF6B}" name="PostI" dataDxfId="18">
       <calculatedColumnFormula>MID(N2,4,1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="14" xr3:uid="{DD688DAA-2C9A-C247-AEC4-CBDADE9B2B2E}" name="PostA" dataDxfId="15">
+    <tableColumn id="14" xr3:uid="{DD688DAA-2C9A-C247-AEC4-CBDADE9B2B2E}" name="PostA" dataDxfId="17">
       <calculatedColumnFormula>MID(N2,6,1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="15" xr3:uid="{CEE151EC-4E5B-0C41-8586-5A2D7E483661}" name="PostCondition" dataDxfId="14"/>
-    <tableColumn id="5" xr3:uid="{62EC5D77-1F78-1645-8697-BC5450583418}" name="CapecMeta" dataDxfId="13"/>
-    <tableColumn id="11" xr3:uid="{0DCD762C-4EE7-8141-BC05-9DB756A5BEF2}" name="CapecStandard" dataDxfId="12"/>
-    <tableColumn id="17" xr3:uid="{9EF317BA-855B-6E4A-9EC7-E1FB88A1FD56}" name="CapecDetailed" dataDxfId="11"/>
-    <tableColumn id="18" xr3:uid="{9BF6197D-4CF5-4941-A460-18823EEFB2E7}" name="Commento" dataDxfId="10"/>
+    <tableColumn id="15" xr3:uid="{CEE151EC-4E5B-0C41-8586-5A2D7E483661}" name="PostCondition" dataDxfId="16"/>
+    <tableColumn id="5" xr3:uid="{62EC5D77-1F78-1645-8697-BC5450583418}" name="CapecMeta" dataDxfId="15"/>
+    <tableColumn id="11" xr3:uid="{0DCD762C-4EE7-8141-BC05-9DB756A5BEF2}" name="CapecStandard" dataDxfId="14"/>
+    <tableColumn id="17" xr3:uid="{9EF317BA-855B-6E4A-9EC7-E1FB88A1FD56}" name="CapecDetailed" dataDxfId="13"/>
+    <tableColumn id="18" xr3:uid="{9BF6197D-4CF5-4941-A460-18823EEFB2E7}" name="Commento" dataDxfId="12"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -9367,18 +9386,20 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{5ECAFCE9-964F-A04C-B050-422AACCFD3F5}" name="Tabella4" displayName="Tabella4" ref="A1:G9" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8">
-  <autoFilter ref="A1:G9" xr:uid="{5ECAFCE9-964F-A04C-B050-422AACCFD3F5}"/>
-  <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{6405AD35-9222-B34C-A112-EC4FDEAC5BE2}" name="ToolID" dataDxfId="7">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{5ECAFCE9-964F-A04C-B050-422AACCFD3F5}" name="Tabella4" displayName="Tabella4" ref="A1:I9" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
+  <autoFilter ref="A1:I9" xr:uid="{5ECAFCE9-964F-A04C-B050-422AACCFD3F5}"/>
+  <tableColumns count="9">
+    <tableColumn id="1" xr3:uid="{6405AD35-9222-B34C-A112-EC4FDEAC5BE2}" name="ToolID" dataDxfId="9">
       <calculatedColumnFormula>ROW(Tabella4[[#This Row],[Name]])-1</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{94F8DBBB-A826-8B4A-8C87-395122CA233A}" name="Name" dataDxfId="6"/>
-    <tableColumn id="2" xr3:uid="{FB636F07-AAD2-AE48-87BB-965F92F829C2}" name="CapecID" dataDxfId="5"/>
-    <tableColumn id="6" xr3:uid="{1E4A4CA6-7FF1-6543-A718-93EC7B5F1624}" name="CypherQuery" dataDxfId="4"/>
-    <tableColumn id="3" xr3:uid="{52487567-ED26-B840-ABFD-DB1BF72A83C9}" name="Command" dataDxfId="3"/>
-    <tableColumn id="5" xr3:uid="{0296B95F-6562-0746-B0C6-FE3564F6272C}" name="Description" dataDxfId="2"/>
-    <tableColumn id="7" xr3:uid="{FF0722DB-3140-904D-9B8E-A0C7B3C1FFEF}" name="PhaseID" dataDxfId="1"/>
+    <tableColumn id="4" xr3:uid="{94F8DBBB-A826-8B4A-8C87-395122CA233A}" name="Name" dataDxfId="8"/>
+    <tableColumn id="2" xr3:uid="{FB636F07-AAD2-AE48-87BB-965F92F829C2}" name="CapecID" dataDxfId="7"/>
+    <tableColumn id="6" xr3:uid="{1E4A4CA6-7FF1-6543-A718-93EC7B5F1624}" name="CypherQuery" dataDxfId="6"/>
+    <tableColumn id="3" xr3:uid="{52487567-ED26-B840-ABFD-DB1BF72A83C9}" name="Command" dataDxfId="5"/>
+    <tableColumn id="5" xr3:uid="{0296B95F-6562-0746-B0C6-FE3564F6272C}" name="Description" dataDxfId="4"/>
+    <tableColumn id="7" xr3:uid="{FF0722DB-3140-904D-9B8E-A0C7B3C1FFEF}" name="PhaseID" dataDxfId="3"/>
+    <tableColumn id="8" xr3:uid="{2C7E754F-9F49-044B-9F1A-B62738B70258}" name="IsExecutable" dataDxfId="2"/>
+    <tableColumn id="9" xr3:uid="{6A4595CA-3FDC-EC4F-B8F1-4344144E8149}" name="OutputParser" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -9666,9 +9687,9 @@
   </sheetPr>
   <dimension ref="A1:R322"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" zoomScale="125" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A287" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C106" sqref="C106"/>
+    <sheetView zoomScale="125" zoomScaleNormal="115" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -9748,7 +9769,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:18" ht="48" hidden="1">
+    <row r="2" spans="1:18" ht="48">
       <c r="A2" s="20" t="str">
         <f t="shared" ref="A2:A64" si="0">CONCATENATE("T",ROW(A2)-1)</f>
         <v>T1</v>
@@ -9801,7 +9822,7 @@
       <c r="Q2" s="24"/>
       <c r="R2" s="24"/>
     </row>
-    <row r="3" spans="1:18" ht="32" hidden="1">
+    <row r="3" spans="1:18" ht="32">
       <c r="A3" s="20" t="str">
         <f t="shared" si="0"/>
         <v>T2</v>
@@ -9854,7 +9875,7 @@
       <c r="Q3" s="24"/>
       <c r="R3" s="24"/>
     </row>
-    <row r="4" spans="1:18" ht="80" hidden="1">
+    <row r="4" spans="1:18" ht="80">
       <c r="A4" s="20" t="str">
         <f t="shared" si="0"/>
         <v>T3</v>
@@ -9907,7 +9928,7 @@
       <c r="Q4" s="24"/>
       <c r="R4" s="24"/>
     </row>
-    <row r="5" spans="1:18" ht="32" hidden="1">
+    <row r="5" spans="1:18" ht="32">
       <c r="A5" s="20" t="str">
         <f t="shared" si="0"/>
         <v>T4</v>
@@ -9960,7 +9981,7 @@
       <c r="Q5" s="24"/>
       <c r="R5" s="24"/>
     </row>
-    <row r="6" spans="1:18" ht="48" hidden="1">
+    <row r="6" spans="1:18" ht="48">
       <c r="A6" s="20" t="str">
         <f t="shared" si="0"/>
         <v>T5</v>
@@ -10013,7 +10034,7 @@
       <c r="Q6" s="24"/>
       <c r="R6" s="24"/>
     </row>
-    <row r="7" spans="1:18" ht="48" hidden="1">
+    <row r="7" spans="1:18" ht="48">
       <c r="A7" s="20" t="str">
         <f t="shared" si="0"/>
         <v>T6</v>
@@ -10066,7 +10087,7 @@
       <c r="Q7" s="24"/>
       <c r="R7" s="24"/>
     </row>
-    <row r="8" spans="1:18" ht="48" hidden="1">
+    <row r="8" spans="1:18" ht="48">
       <c r="A8" s="20" t="str">
         <f t="shared" si="0"/>
         <v>T7</v>
@@ -10119,7 +10140,7 @@
       <c r="Q8" s="24"/>
       <c r="R8" s="24"/>
     </row>
-    <row r="9" spans="1:18" ht="16" hidden="1">
+    <row r="9" spans="1:18" ht="16">
       <c r="A9" s="20" t="str">
         <f t="shared" si="0"/>
         <v>T8</v>
@@ -10172,7 +10193,7 @@
       <c r="Q9" s="24"/>
       <c r="R9" s="24"/>
     </row>
-    <row r="10" spans="1:18" ht="32" hidden="1">
+    <row r="10" spans="1:18" ht="32">
       <c r="A10" s="20" t="str">
         <f t="shared" si="0"/>
         <v>T9</v>
@@ -10225,7 +10246,7 @@
       <c r="Q10" s="24"/>
       <c r="R10" s="24"/>
     </row>
-    <row r="11" spans="1:18" ht="32" hidden="1">
+    <row r="11" spans="1:18" ht="32">
       <c r="A11" s="20" t="str">
         <f t="shared" si="0"/>
         <v>T10</v>
@@ -10278,7 +10299,7 @@
       <c r="Q11" s="24"/>
       <c r="R11" s="24"/>
     </row>
-    <row r="12" spans="1:18" ht="48" hidden="1">
+    <row r="12" spans="1:18" ht="48">
       <c r="A12" s="20" t="str">
         <f t="shared" si="0"/>
         <v>T11</v>
@@ -10331,7 +10352,7 @@
       <c r="Q12" s="24"/>
       <c r="R12" s="24"/>
     </row>
-    <row r="13" spans="1:18" ht="64" hidden="1">
+    <row r="13" spans="1:18" ht="64">
       <c r="A13" s="20" t="str">
         <f t="shared" si="0"/>
         <v>T12</v>
@@ -10384,7 +10405,7 @@
       <c r="Q13" s="24"/>
       <c r="R13" s="24"/>
     </row>
-    <row r="14" spans="1:18" ht="48" hidden="1">
+    <row r="14" spans="1:18" ht="48">
       <c r="A14" s="20" t="str">
         <f t="shared" si="0"/>
         <v>T13</v>
@@ -10437,7 +10458,7 @@
       <c r="Q14" s="24"/>
       <c r="R14" s="24"/>
     </row>
-    <row r="15" spans="1:18" ht="80" hidden="1">
+    <row r="15" spans="1:18" ht="80">
       <c r="A15" s="20" t="str">
         <f t="shared" si="0"/>
         <v>T14</v>
@@ -10490,7 +10511,7 @@
       <c r="Q15" s="24"/>
       <c r="R15" s="24"/>
     </row>
-    <row r="16" spans="1:18" ht="32" hidden="1">
+    <row r="16" spans="1:18" ht="32">
       <c r="A16" s="20" t="str">
         <f t="shared" si="0"/>
         <v>T15</v>
@@ -10543,7 +10564,7 @@
       <c r="Q16" s="24"/>
       <c r="R16" s="24"/>
     </row>
-    <row r="17" spans="1:18" ht="32" hidden="1">
+    <row r="17" spans="1:18" ht="32">
       <c r="A17" s="20" t="str">
         <f t="shared" si="0"/>
         <v>T16</v>
@@ -10596,7 +10617,7 @@
       <c r="Q17" s="24"/>
       <c r="R17" s="24"/>
     </row>
-    <row r="18" spans="1:18" ht="48" hidden="1">
+    <row r="18" spans="1:18" ht="48">
       <c r="A18" s="20" t="str">
         <f t="shared" si="0"/>
         <v>T17</v>
@@ -10649,7 +10670,7 @@
       <c r="Q18" s="24"/>
       <c r="R18" s="24"/>
     </row>
-    <row r="19" spans="1:18" ht="32" hidden="1">
+    <row r="19" spans="1:18" ht="32">
       <c r="A19" s="20" t="str">
         <f t="shared" si="0"/>
         <v>T18</v>
@@ -10702,7 +10723,7 @@
       <c r="Q19" s="24"/>
       <c r="R19" s="24"/>
     </row>
-    <row r="20" spans="1:18" ht="48" hidden="1">
+    <row r="20" spans="1:18" ht="48">
       <c r="A20" s="20" t="str">
         <f t="shared" si="0"/>
         <v>T19</v>
@@ -10755,7 +10776,7 @@
       <c r="Q20" s="24"/>
       <c r="R20" s="24"/>
     </row>
-    <row r="21" spans="1:18" ht="48" hidden="1">
+    <row r="21" spans="1:18" ht="48">
       <c r="A21" s="20" t="str">
         <f t="shared" si="0"/>
         <v>T20</v>
@@ -10808,7 +10829,7 @@
       <c r="Q21" s="24"/>
       <c r="R21" s="24"/>
     </row>
-    <row r="22" spans="1:18" ht="48" hidden="1">
+    <row r="22" spans="1:18" ht="48">
       <c r="A22" s="20" t="str">
         <f t="shared" si="0"/>
         <v>T21</v>
@@ -10861,7 +10882,7 @@
       <c r="Q22" s="24"/>
       <c r="R22" s="24"/>
     </row>
-    <row r="23" spans="1:18" ht="48" hidden="1">
+    <row r="23" spans="1:18" ht="48">
       <c r="A23" s="20" t="str">
         <f t="shared" si="0"/>
         <v>T22</v>
@@ -10914,7 +10935,7 @@
       <c r="Q23" s="24"/>
       <c r="R23" s="24"/>
     </row>
-    <row r="24" spans="1:18" ht="48" hidden="1">
+    <row r="24" spans="1:18" ht="48">
       <c r="A24" s="20" t="str">
         <f t="shared" si="0"/>
         <v>T23</v>
@@ -10970,7 +10991,7 @@
       </c>
       <c r="R24" s="24"/>
     </row>
-    <row r="25" spans="1:18" ht="48" hidden="1">
+    <row r="25" spans="1:18" ht="48">
       <c r="A25" s="20" t="str">
         <f t="shared" si="0"/>
         <v>T24</v>
@@ -11020,7 +11041,7 @@
       <c r="Q25" s="24"/>
       <c r="R25" s="24"/>
     </row>
-    <row r="26" spans="1:18" ht="48" hidden="1">
+    <row r="26" spans="1:18" ht="48">
       <c r="A26" s="20" t="str">
         <f t="shared" si="0"/>
         <v>T25</v>
@@ -11070,7 +11091,7 @@
       <c r="Q26" s="24"/>
       <c r="R26" s="24"/>
     </row>
-    <row r="27" spans="1:18" ht="64" hidden="1">
+    <row r="27" spans="1:18" ht="64">
       <c r="A27" s="20" t="str">
         <f t="shared" si="0"/>
         <v>T26</v>
@@ -11120,7 +11141,7 @@
       <c r="Q27" s="24"/>
       <c r="R27" s="24"/>
     </row>
-    <row r="28" spans="1:18" ht="32" hidden="1">
+    <row r="28" spans="1:18" ht="32">
       <c r="A28" s="20" t="str">
         <f t="shared" si="0"/>
         <v>T27</v>
@@ -11170,7 +11191,7 @@
       <c r="Q28" s="24"/>
       <c r="R28" s="24"/>
     </row>
-    <row r="29" spans="1:18" ht="48" hidden="1">
+    <row r="29" spans="1:18" ht="48">
       <c r="A29" s="20" t="str">
         <f t="shared" si="0"/>
         <v>T28</v>
@@ -11220,7 +11241,7 @@
       <c r="Q29" s="24"/>
       <c r="R29" s="24"/>
     </row>
-    <row r="30" spans="1:18" ht="48" hidden="1">
+    <row r="30" spans="1:18" ht="48">
       <c r="A30" s="20" t="str">
         <f t="shared" si="0"/>
         <v>T29</v>
@@ -11270,7 +11291,7 @@
       <c r="Q30" s="24"/>
       <c r="R30" s="24"/>
     </row>
-    <row r="31" spans="1:18" ht="32" hidden="1">
+    <row r="31" spans="1:18" ht="32">
       <c r="A31" s="20" t="str">
         <f t="shared" si="0"/>
         <v>T30</v>
@@ -11320,7 +11341,7 @@
       <c r="Q31" s="24"/>
       <c r="R31" s="24"/>
     </row>
-    <row r="32" spans="1:18" ht="48" hidden="1">
+    <row r="32" spans="1:18" ht="48">
       <c r="A32" s="20" t="str">
         <f t="shared" si="0"/>
         <v>T31</v>
@@ -11370,7 +11391,7 @@
       <c r="Q32" s="24"/>
       <c r="R32" s="24"/>
     </row>
-    <row r="33" spans="1:18" ht="32" hidden="1">
+    <row r="33" spans="1:18" ht="32">
       <c r="A33" s="20" t="str">
         <f t="shared" si="0"/>
         <v>T32</v>
@@ -11420,7 +11441,7 @@
       <c r="Q33" s="24"/>
       <c r="R33" s="24"/>
     </row>
-    <row r="34" spans="1:18" ht="32" hidden="1">
+    <row r="34" spans="1:18" ht="32">
       <c r="A34" s="20" t="str">
         <f t="shared" si="0"/>
         <v>T33</v>
@@ -11470,7 +11491,7 @@
       <c r="Q34" s="24"/>
       <c r="R34" s="24"/>
     </row>
-    <row r="35" spans="1:18" ht="48" hidden="1">
+    <row r="35" spans="1:18" ht="48">
       <c r="A35" s="20" t="str">
         <f t="shared" si="0"/>
         <v>T34</v>
@@ -11520,7 +11541,7 @@
       <c r="Q35" s="24"/>
       <c r="R35" s="24"/>
     </row>
-    <row r="36" spans="1:18" ht="32" hidden="1">
+    <row r="36" spans="1:18" ht="32">
       <c r="A36" s="20" t="str">
         <f t="shared" si="0"/>
         <v>T35</v>
@@ -11570,7 +11591,7 @@
       <c r="Q36" s="24"/>
       <c r="R36" s="24"/>
     </row>
-    <row r="37" spans="1:18" ht="16" hidden="1">
+    <row r="37" spans="1:18" ht="16">
       <c r="A37" s="20" t="str">
         <f t="shared" si="0"/>
         <v>T36</v>
@@ -11620,7 +11641,7 @@
       <c r="Q37" s="24"/>
       <c r="R37" s="24"/>
     </row>
-    <row r="38" spans="1:18" ht="16" hidden="1">
+    <row r="38" spans="1:18" ht="16">
       <c r="A38" s="20" t="str">
         <f t="shared" si="0"/>
         <v>T37</v>
@@ -11670,7 +11691,7 @@
       <c r="Q38" s="24"/>
       <c r="R38" s="24"/>
     </row>
-    <row r="39" spans="1:18" ht="32" hidden="1">
+    <row r="39" spans="1:18" ht="32">
       <c r="A39" s="20" t="str">
         <f t="shared" si="0"/>
         <v>T38</v>
@@ -11720,7 +11741,7 @@
       <c r="Q39" s="24"/>
       <c r="R39" s="24"/>
     </row>
-    <row r="40" spans="1:18" ht="32" hidden="1">
+    <row r="40" spans="1:18" ht="32">
       <c r="A40" s="20" t="str">
         <f t="shared" si="0"/>
         <v>T39</v>
@@ -11770,7 +11791,7 @@
       <c r="Q40" s="24"/>
       <c r="R40" s="24"/>
     </row>
-    <row r="41" spans="1:18" ht="48" hidden="1">
+    <row r="41" spans="1:18" ht="48">
       <c r="A41" s="20" t="str">
         <f t="shared" si="0"/>
         <v>T40</v>
@@ -11820,7 +11841,7 @@
       <c r="Q41" s="24"/>
       <c r="R41" s="24"/>
     </row>
-    <row r="42" spans="1:18" ht="48" hidden="1">
+    <row r="42" spans="1:18" ht="48">
       <c r="A42" s="20" t="str">
         <f t="shared" si="0"/>
         <v>T41</v>
@@ -11870,7 +11891,7 @@
       <c r="Q42" s="24"/>
       <c r="R42" s="24"/>
     </row>
-    <row r="43" spans="1:18" ht="16" hidden="1">
+    <row r="43" spans="1:18" ht="16">
       <c r="A43" s="20" t="str">
         <f t="shared" si="0"/>
         <v>T42</v>
@@ -11920,7 +11941,7 @@
       <c r="Q43" s="24"/>
       <c r="R43" s="24"/>
     </row>
-    <row r="44" spans="1:18" ht="48" hidden="1">
+    <row r="44" spans="1:18" ht="48">
       <c r="A44" s="20" t="str">
         <f t="shared" si="0"/>
         <v>T43</v>
@@ -11970,7 +11991,7 @@
       <c r="Q44" s="24"/>
       <c r="R44" s="24"/>
     </row>
-    <row r="45" spans="1:18" ht="48" hidden="1">
+    <row r="45" spans="1:18" ht="48">
       <c r="A45" s="20" t="str">
         <f t="shared" si="0"/>
         <v>T44</v>
@@ -12020,7 +12041,7 @@
       <c r="Q45" s="24"/>
       <c r="R45" s="24"/>
     </row>
-    <row r="46" spans="1:18" ht="32" hidden="1">
+    <row r="46" spans="1:18" ht="32">
       <c r="A46" s="20" t="str">
         <f t="shared" si="0"/>
         <v>T45</v>
@@ -12070,7 +12091,7 @@
       <c r="Q46" s="24"/>
       <c r="R46" s="24"/>
     </row>
-    <row r="47" spans="1:18" ht="32" hidden="1">
+    <row r="47" spans="1:18" ht="32">
       <c r="A47" s="20" t="str">
         <f t="shared" si="0"/>
         <v>T46</v>
@@ -12120,7 +12141,7 @@
       <c r="Q47" s="24"/>
       <c r="R47" s="24"/>
     </row>
-    <row r="48" spans="1:18" ht="48" hidden="1">
+    <row r="48" spans="1:18" ht="48">
       <c r="A48" s="20" t="str">
         <f t="shared" si="0"/>
         <v>T47</v>
@@ -12170,7 +12191,7 @@
       <c r="Q48" s="24"/>
       <c r="R48" s="24"/>
     </row>
-    <row r="49" spans="1:18" ht="32" hidden="1">
+    <row r="49" spans="1:18" ht="32">
       <c r="A49" s="20" t="str">
         <f t="shared" si="0"/>
         <v>T48</v>
@@ -12220,7 +12241,7 @@
       <c r="Q49" s="24"/>
       <c r="R49" s="24"/>
     </row>
-    <row r="50" spans="1:18" ht="32" hidden="1">
+    <row r="50" spans="1:18" ht="32">
       <c r="A50" s="20" t="str">
         <f t="shared" si="0"/>
         <v>T49</v>
@@ -12270,7 +12291,7 @@
       <c r="Q50" s="24"/>
       <c r="R50" s="24"/>
     </row>
-    <row r="51" spans="1:18" ht="32" hidden="1">
+    <row r="51" spans="1:18" ht="32">
       <c r="A51" s="20" t="str">
         <f t="shared" si="0"/>
         <v>T50</v>
@@ -12320,7 +12341,7 @@
       <c r="Q51" s="24"/>
       <c r="R51" s="24"/>
     </row>
-    <row r="52" spans="1:18" ht="32" hidden="1">
+    <row r="52" spans="1:18" ht="32">
       <c r="A52" s="20" t="str">
         <f t="shared" si="0"/>
         <v>T51</v>
@@ -12370,7 +12391,7 @@
       <c r="Q52" s="24"/>
       <c r="R52" s="24"/>
     </row>
-    <row r="53" spans="1:18" ht="48" hidden="1">
+    <row r="53" spans="1:18" ht="48">
       <c r="A53" s="20" t="str">
         <f t="shared" si="0"/>
         <v>T52</v>
@@ -12420,7 +12441,7 @@
       <c r="Q53" s="24"/>
       <c r="R53" s="24"/>
     </row>
-    <row r="54" spans="1:18" ht="32" hidden="1">
+    <row r="54" spans="1:18" ht="32">
       <c r="A54" s="20" t="str">
         <f t="shared" si="0"/>
         <v>T53</v>
@@ -12470,7 +12491,7 @@
       <c r="Q54" s="24"/>
       <c r="R54" s="24"/>
     </row>
-    <row r="55" spans="1:18" ht="48" hidden="1">
+    <row r="55" spans="1:18" ht="48">
       <c r="A55" s="20" t="str">
         <f t="shared" si="0"/>
         <v>T54</v>
@@ -12520,7 +12541,7 @@
       <c r="Q55" s="24"/>
       <c r="R55" s="24"/>
     </row>
-    <row r="56" spans="1:18" ht="32" hidden="1">
+    <row r="56" spans="1:18" ht="32">
       <c r="A56" s="20" t="str">
         <f t="shared" si="0"/>
         <v>T55</v>
@@ -12570,7 +12591,7 @@
       <c r="Q56" s="24"/>
       <c r="R56" s="24"/>
     </row>
-    <row r="57" spans="1:18" ht="80" hidden="1">
+    <row r="57" spans="1:18" ht="80">
       <c r="A57" s="20" t="str">
         <f t="shared" si="0"/>
         <v>T56</v>
@@ -12620,7 +12641,7 @@
       <c r="Q57" s="24"/>
       <c r="R57" s="24"/>
     </row>
-    <row r="58" spans="1:18" ht="32" hidden="1">
+    <row r="58" spans="1:18" ht="32">
       <c r="A58" s="20" t="str">
         <f t="shared" si="0"/>
         <v>T57</v>
@@ -12670,7 +12691,7 @@
       <c r="Q58" s="24"/>
       <c r="R58" s="24"/>
     </row>
-    <row r="59" spans="1:18" ht="32" hidden="1">
+    <row r="59" spans="1:18" ht="32">
       <c r="A59" s="20" t="str">
         <f t="shared" si="0"/>
         <v>T58</v>
@@ -12720,7 +12741,7 @@
       <c r="Q59" s="24"/>
       <c r="R59" s="24"/>
     </row>
-    <row r="60" spans="1:18" ht="64" hidden="1">
+    <row r="60" spans="1:18" ht="64">
       <c r="A60" s="20" t="str">
         <f t="shared" si="0"/>
         <v>T59</v>
@@ -12781,7 +12802,7 @@
       </c>
       <c r="R60" s="24"/>
     </row>
-    <row r="61" spans="1:18" ht="395" hidden="1">
+    <row r="61" spans="1:18" ht="395">
       <c r="A61" s="20" t="str">
         <f t="shared" si="0"/>
         <v>T60</v>
@@ -12842,7 +12863,7 @@
       </c>
       <c r="R61" s="24"/>
     </row>
-    <row r="62" spans="1:18" ht="80" hidden="1">
+    <row r="62" spans="1:18" ht="80">
       <c r="A62" s="20" t="str">
         <f t="shared" si="0"/>
         <v>T61</v>
@@ -12903,7 +12924,7 @@
       </c>
       <c r="R62" s="24"/>
     </row>
-    <row r="63" spans="1:18" ht="240" hidden="1">
+    <row r="63" spans="1:18" ht="240">
       <c r="A63" s="20" t="str">
         <f t="shared" si="0"/>
         <v>T62</v>
@@ -12964,7 +12985,7 @@
       </c>
       <c r="R63" s="24"/>
     </row>
-    <row r="64" spans="1:18" ht="48" hidden="1">
+    <row r="64" spans="1:18" ht="48">
       <c r="A64" s="20" t="str">
         <f t="shared" si="0"/>
         <v>T63</v>
@@ -13025,7 +13046,7 @@
       </c>
       <c r="R64" s="24"/>
     </row>
-    <row r="65" spans="1:18" ht="96" hidden="1">
+    <row r="65" spans="1:18" ht="96">
       <c r="A65" s="20" t="str">
         <f t="shared" ref="A65:A128" si="12">CONCATENATE("T",ROW(A65)-1)</f>
         <v>T64</v>
@@ -13088,7 +13109,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="66" spans="1:18" ht="256" hidden="1">
+    <row r="66" spans="1:18" ht="256">
       <c r="A66" s="20" t="str">
         <f t="shared" si="12"/>
         <v>T65</v>
@@ -13149,7 +13170,7 @@
       </c>
       <c r="R66" s="24"/>
     </row>
-    <row r="67" spans="1:18" ht="16" hidden="1">
+    <row r="67" spans="1:18" ht="16">
       <c r="A67" s="20" t="str">
         <f t="shared" si="12"/>
         <v>T66</v>
@@ -13206,7 +13227,7 @@
       <c r="Q67" s="24"/>
       <c r="R67" s="24"/>
     </row>
-    <row r="68" spans="1:18" ht="96" hidden="1">
+    <row r="68" spans="1:18" ht="96">
       <c r="A68" s="20" t="str">
         <f t="shared" si="12"/>
         <v>T67</v>
@@ -13269,7 +13290,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="69" spans="1:18" ht="144" hidden="1">
+    <row r="69" spans="1:18" ht="144">
       <c r="A69" s="20" t="str">
         <f t="shared" si="12"/>
         <v>T68</v>
@@ -13330,7 +13351,7 @@
       </c>
       <c r="R69" s="24"/>
     </row>
-    <row r="70" spans="1:18" ht="96" hidden="1">
+    <row r="70" spans="1:18" ht="96">
       <c r="A70" s="20" t="str">
         <f t="shared" si="12"/>
         <v>T69</v>
@@ -13391,7 +13412,7 @@
       </c>
       <c r="R70" s="24"/>
     </row>
-    <row r="71" spans="1:18" ht="32" hidden="1">
+    <row r="71" spans="1:18" ht="32">
       <c r="A71" s="20" t="str">
         <f t="shared" si="12"/>
         <v>T70</v>
@@ -13448,7 +13469,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="72" spans="1:18" ht="48" hidden="1">
+    <row r="72" spans="1:18" ht="48">
       <c r="A72" s="20" t="str">
         <f t="shared" si="12"/>
         <v>T71</v>
@@ -13509,7 +13530,7 @@
       </c>
       <c r="R72" s="24"/>
     </row>
-    <row r="73" spans="1:18" ht="48" hidden="1">
+    <row r="73" spans="1:18" ht="48">
       <c r="A73" s="20" t="str">
         <f t="shared" si="12"/>
         <v>T72</v>
@@ -13570,7 +13591,7 @@
       </c>
       <c r="R73" s="24"/>
     </row>
-    <row r="74" spans="1:18" ht="32" hidden="1">
+    <row r="74" spans="1:18" ht="32">
       <c r="A74" s="20" t="str">
         <f t="shared" si="12"/>
         <v>T73</v>
@@ -13631,7 +13652,7 @@
       </c>
       <c r="R74" s="24"/>
     </row>
-    <row r="75" spans="1:18" ht="80" hidden="1">
+    <row r="75" spans="1:18" ht="80">
       <c r="A75" s="20" t="str">
         <f t="shared" si="12"/>
         <v>T74</v>
@@ -13692,7 +13713,7 @@
       </c>
       <c r="R75" s="24"/>
     </row>
-    <row r="76" spans="1:18" ht="160" hidden="1">
+    <row r="76" spans="1:18" ht="160">
       <c r="A76" s="20" t="str">
         <f t="shared" si="12"/>
         <v>T75</v>
@@ -13753,7 +13774,7 @@
       </c>
       <c r="R76" s="24"/>
     </row>
-    <row r="77" spans="1:18" ht="128" hidden="1">
+    <row r="77" spans="1:18" ht="128">
       <c r="A77" s="20" t="str">
         <f t="shared" si="12"/>
         <v>T76</v>
@@ -13812,7 +13833,7 @@
       <c r="Q77" s="24"/>
       <c r="R77" s="24"/>
     </row>
-    <row r="78" spans="1:18" ht="80" hidden="1">
+    <row r="78" spans="1:18" ht="80">
       <c r="A78" s="20" t="str">
         <f t="shared" si="12"/>
         <v>T77</v>
@@ -13873,7 +13894,7 @@
       </c>
       <c r="R78" s="24"/>
     </row>
-    <row r="79" spans="1:18" ht="96" hidden="1">
+    <row r="79" spans="1:18" ht="96">
       <c r="A79" s="20" t="str">
         <f t="shared" si="12"/>
         <v>T78</v>
@@ -13934,7 +13955,7 @@
       </c>
       <c r="R79" s="24"/>
     </row>
-    <row r="80" spans="1:18" ht="96" hidden="1">
+    <row r="80" spans="1:18" ht="96">
       <c r="A80" s="20" t="str">
         <f t="shared" si="12"/>
         <v>T79</v>
@@ -13995,7 +14016,7 @@
       </c>
       <c r="R80" s="24"/>
     </row>
-    <row r="81" spans="1:18" ht="240" hidden="1">
+    <row r="81" spans="1:18" ht="240">
       <c r="A81" s="20" t="str">
         <f t="shared" si="12"/>
         <v>T80</v>
@@ -14056,7 +14077,7 @@
       </c>
       <c r="R81" s="24"/>
     </row>
-    <row r="82" spans="1:18" ht="32" hidden="1">
+    <row r="82" spans="1:18" ht="32">
       <c r="A82" s="20" t="str">
         <f t="shared" si="12"/>
         <v>T81</v>
@@ -14107,7 +14128,7 @@
       <c r="Q82" s="24"/>
       <c r="R82" s="24"/>
     </row>
-    <row r="83" spans="1:18" ht="16" hidden="1">
+    <row r="83" spans="1:18" ht="16">
       <c r="A83" s="20" t="str">
         <f t="shared" si="12"/>
         <v>T82</v>
@@ -14158,7 +14179,7 @@
       <c r="Q83" s="24"/>
       <c r="R83" s="24"/>
     </row>
-    <row r="84" spans="1:18" ht="16" hidden="1">
+    <row r="84" spans="1:18" ht="16">
       <c r="A84" s="20" t="str">
         <f t="shared" si="12"/>
         <v>T83</v>
@@ -14209,7 +14230,7 @@
       <c r="Q84" s="24"/>
       <c r="R84" s="24"/>
     </row>
-    <row r="85" spans="1:18" ht="96" hidden="1">
+    <row r="85" spans="1:18" ht="96">
       <c r="A85" s="20" t="str">
         <f t="shared" si="12"/>
         <v>T84</v>
@@ -14260,7 +14281,7 @@
       <c r="Q85" s="24"/>
       <c r="R85" s="24"/>
     </row>
-    <row r="86" spans="1:18" ht="64" hidden="1">
+    <row r="86" spans="1:18" ht="64">
       <c r="A86" s="20" t="str">
         <f t="shared" si="12"/>
         <v>T85</v>
@@ -14311,7 +14332,7 @@
       <c r="Q86" s="24"/>
       <c r="R86" s="24"/>
     </row>
-    <row r="87" spans="1:18" ht="32" hidden="1">
+    <row r="87" spans="1:18" ht="32">
       <c r="A87" s="20" t="str">
         <f t="shared" si="12"/>
         <v>T86</v>
@@ -14362,7 +14383,7 @@
       <c r="Q87" s="24"/>
       <c r="R87" s="24"/>
     </row>
-    <row r="88" spans="1:18" ht="16" hidden="1">
+    <row r="88" spans="1:18" ht="16">
       <c r="A88" s="20" t="str">
         <f t="shared" si="12"/>
         <v>T87</v>
@@ -14413,7 +14434,7 @@
       <c r="Q88" s="24"/>
       <c r="R88" s="24"/>
     </row>
-    <row r="89" spans="1:18" ht="32" hidden="1">
+    <row r="89" spans="1:18" ht="32">
       <c r="A89" s="20" t="str">
         <f t="shared" si="12"/>
         <v>T88</v>
@@ -14464,7 +14485,7 @@
       <c r="Q89" s="24"/>
       <c r="R89" s="24"/>
     </row>
-    <row r="90" spans="1:18" ht="48" hidden="1">
+    <row r="90" spans="1:18" ht="48">
       <c r="A90" s="20" t="str">
         <f t="shared" si="12"/>
         <v>T89</v>
@@ -14515,7 +14536,7 @@
       <c r="Q90" s="24"/>
       <c r="R90" s="24"/>
     </row>
-    <row r="91" spans="1:18" ht="96" hidden="1">
+    <row r="91" spans="1:18" ht="96">
       <c r="A91" s="20" t="str">
         <f t="shared" si="12"/>
         <v>T90</v>
@@ -14566,7 +14587,7 @@
       <c r="Q91" s="24"/>
       <c r="R91" s="24"/>
     </row>
-    <row r="92" spans="1:18" ht="64" hidden="1">
+    <row r="92" spans="1:18" ht="64">
       <c r="A92" s="20" t="str">
         <f t="shared" si="12"/>
         <v>T91</v>
@@ -14617,7 +14638,7 @@
       <c r="Q92" s="24"/>
       <c r="R92" s="24"/>
     </row>
-    <row r="93" spans="1:18" ht="48" hidden="1">
+    <row r="93" spans="1:18" ht="48">
       <c r="A93" s="20" t="str">
         <f t="shared" si="12"/>
         <v>T92</v>
@@ -14668,7 +14689,7 @@
       <c r="Q93" s="24"/>
       <c r="R93" s="24"/>
     </row>
-    <row r="94" spans="1:18" ht="32" hidden="1">
+    <row r="94" spans="1:18" ht="32">
       <c r="A94" s="20" t="str">
         <f t="shared" si="12"/>
         <v>T93</v>
@@ -14719,7 +14740,7 @@
       <c r="Q94" s="24"/>
       <c r="R94" s="24"/>
     </row>
-    <row r="95" spans="1:18" ht="32" hidden="1">
+    <row r="95" spans="1:18" ht="32">
       <c r="A95" s="20" t="str">
         <f t="shared" si="12"/>
         <v>T94</v>
@@ -14770,7 +14791,7 @@
       <c r="Q95" s="24"/>
       <c r="R95" s="24"/>
     </row>
-    <row r="96" spans="1:18" ht="32" hidden="1">
+    <row r="96" spans="1:18" ht="32">
       <c r="A96" s="20" t="str">
         <f t="shared" si="12"/>
         <v>T95</v>
@@ -14821,7 +14842,7 @@
       <c r="Q96" s="24"/>
       <c r="R96" s="24"/>
     </row>
-    <row r="97" spans="1:18" ht="64" hidden="1">
+    <row r="97" spans="1:18" ht="64">
       <c r="A97" s="20" t="str">
         <f t="shared" si="12"/>
         <v>T96</v>
@@ -14872,7 +14893,7 @@
       <c r="Q97" s="24"/>
       <c r="R97" s="24"/>
     </row>
-    <row r="98" spans="1:18" ht="48" hidden="1">
+    <row r="98" spans="1:18" ht="48">
       <c r="A98" s="20" t="str">
         <f t="shared" si="12"/>
         <v>T97</v>
@@ -14923,7 +14944,7 @@
       <c r="Q98" s="24"/>
       <c r="R98" s="24"/>
     </row>
-    <row r="99" spans="1:18" ht="32" hidden="1">
+    <row r="99" spans="1:18" ht="32">
       <c r="A99" s="20" t="str">
         <f t="shared" si="12"/>
         <v>T98</v>
@@ -14984,7 +15005,7 @@
       </c>
       <c r="R99" s="24"/>
     </row>
-    <row r="100" spans="1:18" ht="48" hidden="1">
+    <row r="100" spans="1:18" ht="48">
       <c r="A100" s="20" t="str">
         <f t="shared" si="12"/>
         <v>T99</v>
@@ -15041,7 +15062,7 @@
       <c r="Q100" s="24"/>
       <c r="R100" s="24"/>
     </row>
-    <row r="101" spans="1:18" ht="48" hidden="1">
+    <row r="101" spans="1:18" ht="48">
       <c r="A101" s="20" t="str">
         <f t="shared" si="12"/>
         <v>T100</v>
@@ -15098,7 +15119,7 @@
       <c r="Q101" s="24"/>
       <c r="R101" s="24"/>
     </row>
-    <row r="102" spans="1:18" ht="112" hidden="1">
+    <row r="102" spans="1:18" ht="112">
       <c r="A102" s="20" t="str">
         <f t="shared" si="12"/>
         <v>T101</v>
@@ -15155,7 +15176,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="103" spans="1:18" ht="64" hidden="1">
+    <row r="103" spans="1:18" ht="64">
       <c r="A103" s="20" t="str">
         <f t="shared" si="12"/>
         <v>T102</v>
@@ -15216,7 +15237,7 @@
       </c>
       <c r="R103" s="24"/>
     </row>
-    <row r="104" spans="1:18" ht="32" hidden="1">
+    <row r="104" spans="1:18" ht="32">
       <c r="A104" s="20" t="str">
         <f t="shared" si="12"/>
         <v>T103</v>
@@ -15277,7 +15298,7 @@
       </c>
       <c r="R104" s="24"/>
     </row>
-    <row r="105" spans="1:18" ht="32" hidden="1">
+    <row r="105" spans="1:18" ht="32">
       <c r="A105" s="20" t="str">
         <f t="shared" si="12"/>
         <v>T104</v>
@@ -15334,7 +15355,7 @@
       <c r="Q105" s="24"/>
       <c r="R105" s="24"/>
     </row>
-    <row r="106" spans="1:18" ht="144" hidden="1">
+    <row r="106" spans="1:18" ht="144">
       <c r="A106" s="20" t="str">
         <f t="shared" si="12"/>
         <v>T105</v>
@@ -15395,7 +15416,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="107" spans="1:18" ht="32" hidden="1">
+    <row r="107" spans="1:18" ht="32">
       <c r="A107" s="20" t="str">
         <f t="shared" si="12"/>
         <v>T106</v>
@@ -15452,7 +15473,7 @@
       <c r="Q107" s="25"/>
       <c r="R107" s="25"/>
     </row>
-    <row r="108" spans="1:18" ht="32" hidden="1">
+    <row r="108" spans="1:18" ht="32">
       <c r="A108" s="20" t="str">
         <f t="shared" si="12"/>
         <v>T107</v>
@@ -15508,7 +15529,7 @@
       <c r="Q108" s="25"/>
       <c r="R108" s="25"/>
     </row>
-    <row r="109" spans="1:18" ht="16" hidden="1">
+    <row r="109" spans="1:18" ht="16">
       <c r="A109" s="20" t="str">
         <f t="shared" si="12"/>
         <v>T108</v>
@@ -15565,7 +15586,7 @@
       <c r="Q109" s="24"/>
       <c r="R109" s="24"/>
     </row>
-    <row r="110" spans="1:18" ht="32" hidden="1">
+    <row r="110" spans="1:18" ht="32">
       <c r="A110" s="20" t="str">
         <f t="shared" si="12"/>
         <v>T109</v>
@@ -15622,7 +15643,7 @@
       <c r="Q110" s="24"/>
       <c r="R110" s="24"/>
     </row>
-    <row r="111" spans="1:18" ht="48" hidden="1">
+    <row r="111" spans="1:18" ht="48">
       <c r="A111" s="20" t="str">
         <f t="shared" si="12"/>
         <v>T110</v>
@@ -15673,7 +15694,7 @@
       <c r="Q111" s="24"/>
       <c r="R111" s="24"/>
     </row>
-    <row r="112" spans="1:18" ht="80" hidden="1">
+    <row r="112" spans="1:18" ht="80">
       <c r="A112" s="20" t="str">
         <f t="shared" si="12"/>
         <v>T111</v>
@@ -15724,7 +15745,7 @@
       <c r="Q112" s="24"/>
       <c r="R112" s="24"/>
     </row>
-    <row r="113" spans="1:18" ht="64" hidden="1">
+    <row r="113" spans="1:18" ht="64">
       <c r="A113" s="20" t="str">
         <f t="shared" si="12"/>
         <v>T112</v>
@@ -15775,7 +15796,7 @@
       <c r="Q113" s="24"/>
       <c r="R113" s="24"/>
     </row>
-    <row r="114" spans="1:18" ht="48" hidden="1">
+    <row r="114" spans="1:18" ht="48">
       <c r="A114" s="20" t="str">
         <f t="shared" si="12"/>
         <v>T113</v>
@@ -15826,7 +15847,7 @@
       <c r="Q114" s="24"/>
       <c r="R114" s="24"/>
     </row>
-    <row r="115" spans="1:18" ht="48" hidden="1">
+    <row r="115" spans="1:18" ht="48">
       <c r="A115" s="20" t="str">
         <f t="shared" si="12"/>
         <v>T114</v>
@@ -15877,7 +15898,7 @@
       <c r="Q115" s="24"/>
       <c r="R115" s="24"/>
     </row>
-    <row r="116" spans="1:18" ht="16" hidden="1">
+    <row r="116" spans="1:18" ht="16">
       <c r="A116" s="20" t="str">
         <f t="shared" si="12"/>
         <v>T115</v>
@@ -15928,7 +15949,7 @@
       <c r="Q116" s="24"/>
       <c r="R116" s="24"/>
     </row>
-    <row r="117" spans="1:18" ht="16" hidden="1">
+    <row r="117" spans="1:18" ht="16">
       <c r="A117" s="20" t="str">
         <f t="shared" si="12"/>
         <v>T116</v>
@@ -15979,7 +16000,7 @@
       <c r="Q117" s="24"/>
       <c r="R117" s="24"/>
     </row>
-    <row r="118" spans="1:18" ht="48" hidden="1">
+    <row r="118" spans="1:18" ht="48">
       <c r="A118" s="20" t="str">
         <f t="shared" si="12"/>
         <v>T117</v>
@@ -16030,7 +16051,7 @@
       <c r="Q118" s="24"/>
       <c r="R118" s="24"/>
     </row>
-    <row r="119" spans="1:18" ht="96" hidden="1">
+    <row r="119" spans="1:18" ht="96">
       <c r="A119" s="20" t="str">
         <f t="shared" si="12"/>
         <v>T118</v>
@@ -16081,7 +16102,7 @@
       <c r="Q119" s="24"/>
       <c r="R119" s="24"/>
     </row>
-    <row r="120" spans="1:18" ht="64" hidden="1">
+    <row r="120" spans="1:18" ht="64">
       <c r="A120" s="20" t="str">
         <f t="shared" si="12"/>
         <v>T119</v>
@@ -16132,7 +16153,7 @@
       <c r="Q120" s="24"/>
       <c r="R120" s="24"/>
     </row>
-    <row r="121" spans="1:18" ht="48" hidden="1">
+    <row r="121" spans="1:18" ht="48">
       <c r="A121" s="20" t="str">
         <f t="shared" si="12"/>
         <v>T120</v>
@@ -16183,7 +16204,7 @@
       <c r="Q121" s="24"/>
       <c r="R121" s="24"/>
     </row>
-    <row r="122" spans="1:18" ht="48" hidden="1">
+    <row r="122" spans="1:18" ht="48">
       <c r="A122" s="20" t="str">
         <f t="shared" si="12"/>
         <v>T121</v>
@@ -16234,7 +16255,7 @@
       <c r="Q122" s="24"/>
       <c r="R122" s="24"/>
     </row>
-    <row r="123" spans="1:18" ht="16" hidden="1">
+    <row r="123" spans="1:18" ht="16">
       <c r="A123" s="20" t="str">
         <f t="shared" si="12"/>
         <v>T122</v>
@@ -16285,7 +16306,7 @@
       <c r="Q123" s="24"/>
       <c r="R123" s="24"/>
     </row>
-    <row r="124" spans="1:18" ht="32" hidden="1">
+    <row r="124" spans="1:18" ht="32">
       <c r="A124" s="20" t="str">
         <f t="shared" si="12"/>
         <v>T123</v>
@@ -16336,7 +16357,7 @@
       <c r="Q124" s="24"/>
       <c r="R124" s="24"/>
     </row>
-    <row r="125" spans="1:18" ht="16" hidden="1">
+    <row r="125" spans="1:18" ht="16">
       <c r="A125" s="20" t="str">
         <f t="shared" si="12"/>
         <v>T124</v>
@@ -16387,7 +16408,7 @@
       <c r="Q125" s="24"/>
       <c r="R125" s="24"/>
     </row>
-    <row r="126" spans="1:18" ht="64" hidden="1">
+    <row r="126" spans="1:18" ht="64">
       <c r="A126" s="20" t="str">
         <f t="shared" si="12"/>
         <v>T125</v>
@@ -16438,7 +16459,7 @@
       <c r="Q126" s="24"/>
       <c r="R126" s="24"/>
     </row>
-    <row r="127" spans="1:18" ht="48" hidden="1">
+    <row r="127" spans="1:18" ht="48">
       <c r="A127" s="20" t="str">
         <f t="shared" si="12"/>
         <v>T126</v>
@@ -16477,7 +16498,7 @@
       <c r="Q127" s="24"/>
       <c r="R127" s="24"/>
     </row>
-    <row r="128" spans="1:18" ht="96" hidden="1">
+    <row r="128" spans="1:18" ht="96">
       <c r="A128" s="20" t="str">
         <f t="shared" si="12"/>
         <v>T127</v>
@@ -16516,7 +16537,7 @@
       <c r="Q128" s="24"/>
       <c r="R128" s="24"/>
     </row>
-    <row r="129" spans="1:18" ht="32" hidden="1">
+    <row r="129" spans="1:18" ht="32">
       <c r="A129" s="20" t="str">
         <f t="shared" ref="A129:A192" si="23">CONCATENATE("T",ROW(A129)-1)</f>
         <v>T128</v>
@@ -16567,7 +16588,7 @@
       <c r="Q129" s="24"/>
       <c r="R129" s="24"/>
     </row>
-    <row r="130" spans="1:18" ht="64" hidden="1">
+    <row r="130" spans="1:18" ht="64">
       <c r="A130" s="20" t="str">
         <f t="shared" si="23"/>
         <v>T129</v>
@@ -16618,7 +16639,7 @@
       <c r="Q130" s="24"/>
       <c r="R130" s="24"/>
     </row>
-    <row r="131" spans="1:18" ht="48" hidden="1">
+    <row r="131" spans="1:18" ht="48">
       <c r="A131" s="20" t="str">
         <f t="shared" si="23"/>
         <v>T130</v>
@@ -16669,7 +16690,7 @@
       <c r="Q131" s="24"/>
       <c r="R131" s="24"/>
     </row>
-    <row r="132" spans="1:18" ht="32" hidden="1">
+    <row r="132" spans="1:18" ht="32">
       <c r="A132" s="20" t="str">
         <f t="shared" si="23"/>
         <v>T131</v>
@@ -16720,7 +16741,7 @@
       <c r="Q132" s="24"/>
       <c r="R132" s="24"/>
     </row>
-    <row r="133" spans="1:18" ht="48" hidden="1">
+    <row r="133" spans="1:18" ht="48">
       <c r="A133" s="20" t="str">
         <f t="shared" si="23"/>
         <v>T132</v>
@@ -16771,7 +16792,7 @@
       <c r="Q133" s="24"/>
       <c r="R133" s="24"/>
     </row>
-    <row r="134" spans="1:18" ht="48" hidden="1">
+    <row r="134" spans="1:18" ht="48">
       <c r="A134" s="20" t="str">
         <f t="shared" si="23"/>
         <v>T133</v>
@@ -16822,7 +16843,7 @@
       <c r="Q134" s="24"/>
       <c r="R134" s="24"/>
     </row>
-    <row r="135" spans="1:18" ht="64" hidden="1">
+    <row r="135" spans="1:18" ht="64">
       <c r="A135" s="20" t="str">
         <f t="shared" si="23"/>
         <v>T134</v>
@@ -16873,7 +16894,7 @@
       <c r="Q135" s="24"/>
       <c r="R135" s="24"/>
     </row>
-    <row r="136" spans="1:18" ht="48" hidden="1">
+    <row r="136" spans="1:18" ht="48">
       <c r="A136" s="20" t="str">
         <f t="shared" si="23"/>
         <v>T135</v>
@@ -16934,7 +16955,7 @@
       </c>
       <c r="R136" s="25"/>
     </row>
-    <row r="137" spans="1:18" ht="96" hidden="1">
+    <row r="137" spans="1:18" ht="96">
       <c r="A137" s="20" t="str">
         <f t="shared" si="23"/>
         <v>T136</v>
@@ -16985,7 +17006,7 @@
       <c r="Q137" s="24"/>
       <c r="R137" s="24"/>
     </row>
-    <row r="138" spans="1:18" ht="80" hidden="1">
+    <row r="138" spans="1:18" ht="80">
       <c r="A138" s="20" t="str">
         <f t="shared" si="23"/>
         <v>T137</v>
@@ -17036,7 +17057,7 @@
       <c r="Q138" s="24"/>
       <c r="R138" s="24"/>
     </row>
-    <row r="139" spans="1:18" ht="96" hidden="1">
+    <row r="139" spans="1:18" ht="96">
       <c r="A139" s="20" t="str">
         <f t="shared" si="23"/>
         <v>T138</v>
@@ -17087,7 +17108,7 @@
       <c r="Q139" s="24"/>
       <c r="R139" s="24"/>
     </row>
-    <row r="140" spans="1:18" ht="48" hidden="1">
+    <row r="140" spans="1:18" ht="48">
       <c r="A140" s="20" t="str">
         <f t="shared" si="23"/>
         <v>T139</v>
@@ -17138,7 +17159,7 @@
       <c r="Q140" s="24"/>
       <c r="R140" s="24"/>
     </row>
-    <row r="141" spans="1:18" ht="80" hidden="1">
+    <row r="141" spans="1:18" ht="80">
       <c r="A141" s="20" t="str">
         <f t="shared" si="23"/>
         <v>T140</v>
@@ -17189,7 +17210,7 @@
       <c r="Q141" s="24"/>
       <c r="R141" s="24"/>
     </row>
-    <row r="142" spans="1:18" ht="48" hidden="1">
+    <row r="142" spans="1:18" ht="48">
       <c r="A142" s="20" t="str">
         <f t="shared" si="23"/>
         <v>T141</v>
@@ -17240,7 +17261,7 @@
       <c r="Q142" s="24"/>
       <c r="R142" s="24"/>
     </row>
-    <row r="143" spans="1:18" ht="32" hidden="1">
+    <row r="143" spans="1:18" ht="32">
       <c r="A143" s="20" t="str">
         <f t="shared" si="23"/>
         <v>T142</v>
@@ -17291,7 +17312,7 @@
       <c r="Q143" s="24"/>
       <c r="R143" s="24"/>
     </row>
-    <row r="144" spans="1:18" ht="32" hidden="1">
+    <row r="144" spans="1:18" ht="32">
       <c r="A144" s="20" t="str">
         <f t="shared" si="23"/>
         <v>T143</v>
@@ -17342,7 +17363,7 @@
       <c r="Q144" s="24"/>
       <c r="R144" s="24"/>
     </row>
-    <row r="145" spans="1:18" ht="80" hidden="1">
+    <row r="145" spans="1:18" ht="80">
       <c r="A145" s="20" t="str">
         <f t="shared" si="23"/>
         <v>T144</v>
@@ -17393,7 +17414,7 @@
       <c r="Q145" s="24"/>
       <c r="R145" s="24"/>
     </row>
-    <row r="146" spans="1:18" ht="64" hidden="1">
+    <row r="146" spans="1:18" ht="64">
       <c r="A146" s="20" t="str">
         <f t="shared" si="23"/>
         <v>T145</v>
@@ -17444,7 +17465,7 @@
       <c r="Q146" s="24"/>
       <c r="R146" s="24"/>
     </row>
-    <row r="147" spans="1:18" ht="64" hidden="1">
+    <row r="147" spans="1:18" ht="64">
       <c r="A147" s="20" t="str">
         <f t="shared" si="23"/>
         <v>T146</v>
@@ -17495,7 +17516,7 @@
       <c r="Q147" s="24"/>
       <c r="R147" s="24"/>
     </row>
-    <row r="148" spans="1:18" ht="32" hidden="1">
+    <row r="148" spans="1:18" ht="32">
       <c r="A148" s="20" t="str">
         <f t="shared" si="23"/>
         <v>T147</v>
@@ -17546,7 +17567,7 @@
       <c r="Q148" s="24"/>
       <c r="R148" s="24"/>
     </row>
-    <row r="149" spans="1:18" ht="64" hidden="1">
+    <row r="149" spans="1:18" ht="64">
       <c r="A149" s="20" t="str">
         <f t="shared" si="23"/>
         <v>T148</v>
@@ -17597,7 +17618,7 @@
       <c r="Q149" s="24"/>
       <c r="R149" s="24"/>
     </row>
-    <row r="150" spans="1:18" ht="112" hidden="1">
+    <row r="150" spans="1:18" ht="112">
       <c r="A150" s="20" t="str">
         <f t="shared" si="23"/>
         <v>T149</v>
@@ -17648,7 +17669,7 @@
       <c r="Q150" s="24"/>
       <c r="R150" s="24"/>
     </row>
-    <row r="151" spans="1:18" ht="64" hidden="1">
+    <row r="151" spans="1:18" ht="64">
       <c r="A151" s="20" t="str">
         <f t="shared" si="23"/>
         <v>T150</v>
@@ -17699,7 +17720,7 @@
       <c r="Q151" s="24"/>
       <c r="R151" s="24"/>
     </row>
-    <row r="152" spans="1:18" ht="96" hidden="1">
+    <row r="152" spans="1:18" ht="96">
       <c r="A152" s="20" t="str">
         <f t="shared" si="23"/>
         <v>T151</v>
@@ -17750,7 +17771,7 @@
       <c r="Q152" s="24"/>
       <c r="R152" s="24"/>
     </row>
-    <row r="153" spans="1:18" ht="160" hidden="1">
+    <row r="153" spans="1:18" ht="160">
       <c r="A153" s="20" t="str">
         <f t="shared" si="23"/>
         <v>T152</v>
@@ -17801,7 +17822,7 @@
       <c r="Q153" s="24"/>
       <c r="R153" s="24"/>
     </row>
-    <row r="154" spans="1:18" ht="96" hidden="1">
+    <row r="154" spans="1:18" ht="96">
       <c r="A154" s="20" t="str">
         <f t="shared" si="23"/>
         <v>T153</v>
@@ -17852,7 +17873,7 @@
       <c r="Q154" s="24"/>
       <c r="R154" s="24"/>
     </row>
-    <row r="155" spans="1:18" ht="80" hidden="1">
+    <row r="155" spans="1:18" ht="80">
       <c r="A155" s="20" t="str">
         <f t="shared" si="23"/>
         <v>T154</v>
@@ -17903,7 +17924,7 @@
       <c r="Q155" s="24"/>
       <c r="R155" s="24"/>
     </row>
-    <row r="156" spans="1:18" ht="96" hidden="1">
+    <row r="156" spans="1:18" ht="96">
       <c r="A156" s="20" t="str">
         <f t="shared" si="23"/>
         <v>T155</v>
@@ -17954,7 +17975,7 @@
       <c r="Q156" s="24"/>
       <c r="R156" s="24"/>
     </row>
-    <row r="157" spans="1:18" ht="48" hidden="1">
+    <row r="157" spans="1:18" ht="48">
       <c r="A157" s="20" t="str">
         <f t="shared" si="23"/>
         <v>T156</v>
@@ -18005,7 +18026,7 @@
       <c r="Q157" s="24"/>
       <c r="R157" s="24"/>
     </row>
-    <row r="158" spans="1:18" ht="32" hidden="1">
+    <row r="158" spans="1:18" ht="32">
       <c r="A158" s="20" t="str">
         <f t="shared" si="23"/>
         <v>T157</v>
@@ -18056,7 +18077,7 @@
       <c r="Q158" s="24"/>
       <c r="R158" s="24"/>
     </row>
-    <row r="159" spans="1:18" ht="80" hidden="1">
+    <row r="159" spans="1:18" ht="80">
       <c r="A159" s="20" t="str">
         <f t="shared" si="23"/>
         <v>T158</v>
@@ -18107,7 +18128,7 @@
       <c r="Q159" s="24"/>
       <c r="R159" s="24"/>
     </row>
-    <row r="160" spans="1:18" ht="80" hidden="1">
+    <row r="160" spans="1:18" ht="80">
       <c r="A160" s="20" t="str">
         <f t="shared" si="23"/>
         <v>T159</v>
@@ -18158,7 +18179,7 @@
       <c r="Q160" s="24"/>
       <c r="R160" s="24"/>
     </row>
-    <row r="161" spans="1:18" ht="64" hidden="1">
+    <row r="161" spans="1:18" ht="64">
       <c r="A161" s="20" t="str">
         <f t="shared" si="23"/>
         <v>T160</v>
@@ -18209,7 +18230,7 @@
       <c r="Q161" s="24"/>
       <c r="R161" s="24"/>
     </row>
-    <row r="162" spans="1:18" ht="64" hidden="1">
+    <row r="162" spans="1:18" ht="64">
       <c r="A162" s="20" t="str">
         <f t="shared" si="23"/>
         <v>T161</v>
@@ -18260,7 +18281,7 @@
       <c r="Q162" s="24"/>
       <c r="R162" s="24"/>
     </row>
-    <row r="163" spans="1:18" ht="48" hidden="1">
+    <row r="163" spans="1:18" ht="48">
       <c r="A163" s="20" t="str">
         <f t="shared" si="23"/>
         <v>T162</v>
@@ -18311,7 +18332,7 @@
       <c r="Q163" s="24"/>
       <c r="R163" s="24"/>
     </row>
-    <row r="164" spans="1:18" ht="32" hidden="1">
+    <row r="164" spans="1:18" ht="32">
       <c r="A164" s="20" t="str">
         <f t="shared" si="23"/>
         <v>T163</v>
@@ -18362,7 +18383,7 @@
       <c r="Q164" s="24"/>
       <c r="R164" s="24"/>
     </row>
-    <row r="165" spans="1:18" ht="32" hidden="1">
+    <row r="165" spans="1:18" ht="32">
       <c r="A165" s="20" t="str">
         <f t="shared" si="23"/>
         <v>T164</v>
@@ -18413,7 +18434,7 @@
       <c r="Q165" s="24"/>
       <c r="R165" s="24"/>
     </row>
-    <row r="166" spans="1:18" ht="32" hidden="1">
+    <row r="166" spans="1:18" ht="32">
       <c r="A166" s="20" t="str">
         <f t="shared" si="23"/>
         <v>T165</v>
@@ -18464,7 +18485,7 @@
       <c r="Q166" s="24"/>
       <c r="R166" s="24"/>
     </row>
-    <row r="167" spans="1:18" ht="32" hidden="1">
+    <row r="167" spans="1:18" ht="32">
       <c r="A167" s="20" t="str">
         <f t="shared" si="23"/>
         <v>T166</v>
@@ -18515,7 +18536,7 @@
       <c r="Q167" s="24"/>
       <c r="R167" s="24"/>
     </row>
-    <row r="168" spans="1:18" ht="64" hidden="1">
+    <row r="168" spans="1:18" ht="64">
       <c r="A168" s="20" t="str">
         <f t="shared" si="23"/>
         <v>T167</v>
@@ -18566,7 +18587,7 @@
       <c r="Q168" s="24"/>
       <c r="R168" s="24"/>
     </row>
-    <row r="169" spans="1:18" ht="48" hidden="1">
+    <row r="169" spans="1:18" ht="48">
       <c r="A169" s="20" t="str">
         <f t="shared" si="23"/>
         <v>T168</v>
@@ -18617,7 +18638,7 @@
       <c r="Q169" s="24"/>
       <c r="R169" s="24"/>
     </row>
-    <row r="170" spans="1:18" ht="32" hidden="1">
+    <row r="170" spans="1:18" ht="32">
       <c r="A170" s="20" t="str">
         <f t="shared" si="23"/>
         <v>T169</v>
@@ -18668,7 +18689,7 @@
       <c r="Q170" s="24"/>
       <c r="R170" s="24"/>
     </row>
-    <row r="171" spans="1:18" ht="32" hidden="1">
+    <row r="171" spans="1:18" ht="32">
       <c r="A171" s="20" t="str">
         <f t="shared" si="23"/>
         <v>T170</v>
@@ -18719,7 +18740,7 @@
       <c r="Q171" s="24"/>
       <c r="R171" s="24"/>
     </row>
-    <row r="172" spans="1:18" ht="16" hidden="1">
+    <row r="172" spans="1:18" ht="16">
       <c r="A172" s="20" t="str">
         <f t="shared" si="23"/>
         <v>T171</v>
@@ -18770,7 +18791,7 @@
       <c r="Q172" s="24"/>
       <c r="R172" s="24"/>
     </row>
-    <row r="173" spans="1:18" ht="16" hidden="1">
+    <row r="173" spans="1:18" ht="16">
       <c r="A173" s="20" t="str">
         <f t="shared" si="23"/>
         <v>T172</v>
@@ -18821,7 +18842,7 @@
       <c r="Q173" s="24"/>
       <c r="R173" s="24"/>
     </row>
-    <row r="174" spans="1:18" ht="64" hidden="1">
+    <row r="174" spans="1:18" ht="64">
       <c r="A174" s="20" t="str">
         <f t="shared" si="23"/>
         <v>T173</v>
@@ -18872,7 +18893,7 @@
       <c r="Q174" s="24"/>
       <c r="R174" s="24"/>
     </row>
-    <row r="175" spans="1:18" ht="64" hidden="1">
+    <row r="175" spans="1:18" ht="64">
       <c r="A175" s="20" t="str">
         <f t="shared" si="23"/>
         <v>T174</v>
@@ -18923,7 +18944,7 @@
       <c r="Q175" s="24"/>
       <c r="R175" s="24"/>
     </row>
-    <row r="176" spans="1:18" ht="80" hidden="1">
+    <row r="176" spans="1:18" ht="80">
       <c r="A176" s="20" t="str">
         <f t="shared" si="23"/>
         <v>T175</v>
@@ -18974,7 +18995,7 @@
       <c r="Q176" s="24"/>
       <c r="R176" s="24"/>
     </row>
-    <row r="177" spans="1:18" ht="48" hidden="1">
+    <row r="177" spans="1:18" ht="48">
       <c r="A177" s="20" t="str">
         <f t="shared" si="23"/>
         <v>T176</v>
@@ -19025,7 +19046,7 @@
       <c r="Q177" s="24"/>
       <c r="R177" s="24"/>
     </row>
-    <row r="178" spans="1:18" ht="32" hidden="1">
+    <row r="178" spans="1:18" ht="32">
       <c r="A178" s="20" t="str">
         <f t="shared" si="23"/>
         <v>T177</v>
@@ -19076,7 +19097,7 @@
       <c r="Q178" s="24"/>
       <c r="R178" s="24"/>
     </row>
-    <row r="179" spans="1:18" ht="32" hidden="1">
+    <row r="179" spans="1:18" ht="32">
       <c r="A179" s="20" t="str">
         <f t="shared" si="23"/>
         <v>T178</v>
@@ -19127,7 +19148,7 @@
       <c r="Q179" s="24"/>
       <c r="R179" s="24"/>
     </row>
-    <row r="180" spans="1:18" ht="80" hidden="1">
+    <row r="180" spans="1:18" ht="80">
       <c r="A180" s="20" t="str">
         <f t="shared" si="23"/>
         <v>T179</v>
@@ -19178,7 +19199,7 @@
       <c r="Q180" s="24"/>
       <c r="R180" s="24"/>
     </row>
-    <row r="181" spans="1:18" ht="64" hidden="1">
+    <row r="181" spans="1:18" ht="64">
       <c r="A181" s="20" t="str">
         <f t="shared" si="23"/>
         <v>T180</v>
@@ -19229,7 +19250,7 @@
       <c r="Q181" s="24"/>
       <c r="R181" s="24"/>
     </row>
-    <row r="182" spans="1:18" ht="64" hidden="1">
+    <row r="182" spans="1:18" ht="64">
       <c r="A182" s="20" t="str">
         <f t="shared" si="23"/>
         <v>T181</v>
@@ -19280,7 +19301,7 @@
       <c r="Q182" s="24"/>
       <c r="R182" s="24"/>
     </row>
-    <row r="183" spans="1:18" ht="144" hidden="1">
+    <row r="183" spans="1:18" ht="144">
       <c r="A183" s="20" t="str">
         <f t="shared" si="23"/>
         <v>T182</v>
@@ -19331,7 +19352,7 @@
       <c r="Q183" s="24"/>
       <c r="R183" s="24"/>
     </row>
-    <row r="184" spans="1:18" ht="96" hidden="1">
+    <row r="184" spans="1:18" ht="96">
       <c r="A184" s="20" t="str">
         <f t="shared" si="23"/>
         <v>T183</v>
@@ -19382,7 +19403,7 @@
       <c r="Q184" s="24"/>
       <c r="R184" s="24"/>
     </row>
-    <row r="185" spans="1:18" ht="48" hidden="1">
+    <row r="185" spans="1:18" ht="48">
       <c r="A185" s="20" t="str">
         <f t="shared" si="23"/>
         <v>T184</v>
@@ -19433,7 +19454,7 @@
       <c r="Q185" s="24"/>
       <c r="R185" s="24"/>
     </row>
-    <row r="186" spans="1:18" ht="16" hidden="1">
+    <row r="186" spans="1:18" ht="16">
       <c r="A186" s="20" t="str">
         <f t="shared" si="23"/>
         <v>T185</v>
@@ -19484,7 +19505,7 @@
       <c r="Q186" s="24"/>
       <c r="R186" s="24"/>
     </row>
-    <row r="187" spans="1:18" ht="144" hidden="1">
+    <row r="187" spans="1:18" ht="144">
       <c r="A187" s="20" t="str">
         <f t="shared" si="23"/>
         <v>T186</v>
@@ -19535,7 +19556,7 @@
       <c r="Q187" s="24"/>
       <c r="R187" s="24"/>
     </row>
-    <row r="188" spans="1:18" ht="128" hidden="1">
+    <row r="188" spans="1:18" ht="128">
       <c r="A188" s="20" t="str">
         <f t="shared" si="23"/>
         <v>T187</v>
@@ -19586,7 +19607,7 @@
       <c r="Q188" s="24"/>
       <c r="R188" s="24"/>
     </row>
-    <row r="189" spans="1:18" ht="128" hidden="1">
+    <row r="189" spans="1:18" ht="128">
       <c r="A189" s="20" t="str">
         <f t="shared" si="23"/>
         <v>T188</v>
@@ -19637,7 +19658,7 @@
       <c r="Q189" s="24"/>
       <c r="R189" s="24"/>
     </row>
-    <row r="190" spans="1:18" ht="96" hidden="1">
+    <row r="190" spans="1:18" ht="96">
       <c r="A190" s="20" t="str">
         <f t="shared" si="23"/>
         <v>T189</v>
@@ -19688,7 +19709,7 @@
       <c r="Q190" s="24"/>
       <c r="R190" s="24"/>
     </row>
-    <row r="191" spans="1:18" ht="80" hidden="1">
+    <row r="191" spans="1:18" ht="80">
       <c r="A191" s="20" t="str">
         <f t="shared" si="23"/>
         <v>T190</v>
@@ -19739,7 +19760,7 @@
       <c r="Q191" s="24"/>
       <c r="R191" s="24"/>
     </row>
-    <row r="192" spans="1:18" ht="80" hidden="1">
+    <row r="192" spans="1:18" ht="80">
       <c r="A192" s="20" t="str">
         <f t="shared" si="23"/>
         <v>T191</v>
@@ -19790,7 +19811,7 @@
       <c r="Q192" s="24"/>
       <c r="R192" s="24"/>
     </row>
-    <row r="193" spans="1:18" ht="48" hidden="1">
+    <row r="193" spans="1:18" ht="48">
       <c r="A193" s="20" t="str">
         <f t="shared" ref="A193:A254" si="28">CONCATENATE("T",ROW(A193)-1)</f>
         <v>T192</v>
@@ -19841,7 +19862,7 @@
       <c r="Q193" s="24"/>
       <c r="R193" s="24"/>
     </row>
-    <row r="194" spans="1:18" ht="32" hidden="1">
+    <row r="194" spans="1:18" ht="32">
       <c r="A194" s="20" t="str">
         <f t="shared" si="28"/>
         <v>T193</v>
@@ -19892,7 +19913,7 @@
       <c r="Q194" s="24"/>
       <c r="R194" s="24"/>
     </row>
-    <row r="195" spans="1:18" ht="80" hidden="1">
+    <row r="195" spans="1:18" ht="80">
       <c r="A195" s="20" t="str">
         <f t="shared" si="28"/>
         <v>T194</v>
@@ -19943,7 +19964,7 @@
       <c r="Q195" s="24"/>
       <c r="R195" s="24"/>
     </row>
-    <row r="196" spans="1:18" ht="96" hidden="1">
+    <row r="196" spans="1:18" ht="96">
       <c r="A196" s="20" t="str">
         <f t="shared" si="28"/>
         <v>T195</v>
@@ -19994,7 +20015,7 @@
       <c r="Q196" s="24"/>
       <c r="R196" s="24"/>
     </row>
-    <row r="197" spans="1:18" ht="48" hidden="1">
+    <row r="197" spans="1:18" ht="48">
       <c r="A197" s="20" t="str">
         <f t="shared" si="28"/>
         <v>T196</v>
@@ -20045,7 +20066,7 @@
       <c r="Q197" s="24"/>
       <c r="R197" s="24"/>
     </row>
-    <row r="198" spans="1:18" ht="80" hidden="1">
+    <row r="198" spans="1:18" ht="80">
       <c r="A198" s="20" t="str">
         <f t="shared" si="28"/>
         <v>T197</v>
@@ -20096,7 +20117,7 @@
       <c r="Q198" s="24"/>
       <c r="R198" s="24"/>
     </row>
-    <row r="199" spans="1:18" ht="48" hidden="1">
+    <row r="199" spans="1:18" ht="48">
       <c r="A199" s="20" t="str">
         <f t="shared" si="28"/>
         <v>T198</v>
@@ -20147,7 +20168,7 @@
       <c r="Q199" s="24"/>
       <c r="R199" s="24"/>
     </row>
-    <row r="200" spans="1:18" ht="32" hidden="1">
+    <row r="200" spans="1:18" ht="32">
       <c r="A200" s="20" t="str">
         <f t="shared" si="28"/>
         <v>T199</v>
@@ -20198,7 +20219,7 @@
       <c r="Q200" s="24"/>
       <c r="R200" s="24"/>
     </row>
-    <row r="201" spans="1:18" ht="32" hidden="1">
+    <row r="201" spans="1:18" ht="32">
       <c r="A201" s="20" t="str">
         <f t="shared" si="28"/>
         <v>T200</v>
@@ -20249,7 +20270,7 @@
       <c r="Q201" s="24"/>
       <c r="R201" s="24"/>
     </row>
-    <row r="202" spans="1:18" ht="80" hidden="1">
+    <row r="202" spans="1:18" ht="80">
       <c r="A202" s="20" t="str">
         <f t="shared" si="28"/>
         <v>T201</v>
@@ -20300,7 +20321,7 @@
       <c r="Q202" s="24"/>
       <c r="R202" s="24"/>
     </row>
-    <row r="203" spans="1:18" ht="64" hidden="1">
+    <row r="203" spans="1:18" ht="64">
       <c r="A203" s="20" t="str">
         <f t="shared" si="28"/>
         <v>T202</v>
@@ -20351,7 +20372,7 @@
       <c r="Q203" s="24"/>
       <c r="R203" s="24"/>
     </row>
-    <row r="204" spans="1:18" ht="64" hidden="1">
+    <row r="204" spans="1:18" ht="64">
       <c r="A204" s="20" t="str">
         <f t="shared" si="28"/>
         <v>T203</v>
@@ -20402,7 +20423,7 @@
       <c r="Q204" s="24"/>
       <c r="R204" s="24"/>
     </row>
-    <row r="205" spans="1:18" ht="32" hidden="1">
+    <row r="205" spans="1:18" ht="32">
       <c r="A205" s="20" t="str">
         <f t="shared" si="28"/>
         <v>T204</v>
@@ -20453,7 +20474,7 @@
       <c r="Q205" s="24"/>
       <c r="R205" s="24"/>
     </row>
-    <row r="206" spans="1:18" ht="80" hidden="1">
+    <row r="206" spans="1:18" ht="80">
       <c r="A206" s="20" t="str">
         <f t="shared" si="28"/>
         <v>T205</v>
@@ -20504,7 +20525,7 @@
       <c r="Q206" s="24"/>
       <c r="R206" s="24"/>
     </row>
-    <row r="207" spans="1:18" ht="96" hidden="1">
+    <row r="207" spans="1:18" ht="96">
       <c r="A207" s="20" t="str">
         <f t="shared" si="28"/>
         <v>T206</v>
@@ -20555,7 +20576,7 @@
       <c r="Q207" s="24"/>
       <c r="R207" s="24"/>
     </row>
-    <row r="208" spans="1:18" ht="80" hidden="1">
+    <row r="208" spans="1:18" ht="80">
       <c r="A208" s="20" t="str">
         <f t="shared" si="28"/>
         <v>T207</v>
@@ -20606,7 +20627,7 @@
       <c r="Q208" s="24"/>
       <c r="R208" s="24"/>
     </row>
-    <row r="209" spans="1:18" ht="80" hidden="1">
+    <row r="209" spans="1:18" ht="80">
       <c r="A209" s="20" t="str">
         <f t="shared" si="28"/>
         <v>T208</v>
@@ -20657,7 +20678,7 @@
       <c r="Q209" s="24"/>
       <c r="R209" s="24"/>
     </row>
-    <row r="210" spans="1:18" ht="48" hidden="1">
+    <row r="210" spans="1:18" ht="48">
       <c r="A210" s="20" t="str">
         <f t="shared" si="28"/>
         <v>T209</v>
@@ -20708,7 +20729,7 @@
       <c r="Q210" s="24"/>
       <c r="R210" s="24"/>
     </row>
-    <row r="211" spans="1:18" ht="32" hidden="1">
+    <row r="211" spans="1:18" ht="32">
       <c r="A211" s="20" t="str">
         <f t="shared" si="28"/>
         <v>T210</v>
@@ -20759,7 +20780,7 @@
       <c r="Q211" s="24"/>
       <c r="R211" s="24"/>
     </row>
-    <row r="212" spans="1:18" ht="144" hidden="1">
+    <row r="212" spans="1:18" ht="144">
       <c r="A212" s="20" t="str">
         <f t="shared" si="28"/>
         <v>T211</v>
@@ -20810,7 +20831,7 @@
       <c r="Q212" s="24"/>
       <c r="R212" s="24"/>
     </row>
-    <row r="213" spans="1:18" ht="80" hidden="1">
+    <row r="213" spans="1:18" ht="80">
       <c r="A213" s="20" t="str">
         <f t="shared" si="28"/>
         <v>T212</v>
@@ -20861,7 +20882,7 @@
       <c r="Q213" s="24"/>
       <c r="R213" s="24"/>
     </row>
-    <row r="214" spans="1:18" ht="96" hidden="1">
+    <row r="214" spans="1:18" ht="96">
       <c r="A214" s="20" t="str">
         <f t="shared" si="28"/>
         <v>T213</v>
@@ -20912,7 +20933,7 @@
       <c r="Q214" s="24"/>
       <c r="R214" s="24"/>
     </row>
-    <row r="215" spans="1:18" ht="96" hidden="1">
+    <row r="215" spans="1:18" ht="96">
       <c r="A215" s="20" t="str">
         <f t="shared" si="28"/>
         <v>T214</v>
@@ -20963,7 +20984,7 @@
       <c r="Q215" s="24"/>
       <c r="R215" s="24"/>
     </row>
-    <row r="216" spans="1:18" ht="80" hidden="1">
+    <row r="216" spans="1:18" ht="80">
       <c r="A216" s="20" t="str">
         <f t="shared" si="28"/>
         <v>T215</v>
@@ -21014,7 +21035,7 @@
       <c r="Q216" s="24"/>
       <c r="R216" s="24"/>
     </row>
-    <row r="217" spans="1:18" ht="80" hidden="1">
+    <row r="217" spans="1:18" ht="80">
       <c r="A217" s="20" t="str">
         <f t="shared" si="28"/>
         <v>T216</v>
@@ -21065,7 +21086,7 @@
       <c r="Q217" s="24"/>
       <c r="R217" s="24"/>
     </row>
-    <row r="218" spans="1:18" ht="48" hidden="1">
+    <row r="218" spans="1:18" ht="48">
       <c r="A218" s="20" t="str">
         <f t="shared" si="28"/>
         <v>T217</v>
@@ -21116,7 +21137,7 @@
       <c r="Q218" s="24"/>
       <c r="R218" s="24"/>
     </row>
-    <row r="219" spans="1:18" ht="32" hidden="1">
+    <row r="219" spans="1:18" ht="32">
       <c r="A219" s="20" t="str">
         <f t="shared" si="28"/>
         <v>T218</v>
@@ -21167,7 +21188,7 @@
       <c r="Q219" s="24"/>
       <c r="R219" s="24"/>
     </row>
-    <row r="220" spans="1:18" ht="64" hidden="1">
+    <row r="220" spans="1:18" ht="64">
       <c r="A220" s="20" t="str">
         <f t="shared" si="28"/>
         <v>T219</v>
@@ -21218,7 +21239,7 @@
       <c r="Q220" s="24"/>
       <c r="R220" s="24"/>
     </row>
-    <row r="221" spans="1:18" ht="16" hidden="1">
+    <row r="221" spans="1:18" ht="16">
       <c r="A221" s="20" t="str">
         <f t="shared" si="28"/>
         <v>T220</v>
@@ -21269,7 +21290,7 @@
       <c r="Q221" s="24"/>
       <c r="R221" s="24"/>
     </row>
-    <row r="222" spans="1:18" ht="64" hidden="1">
+    <row r="222" spans="1:18" ht="64">
       <c r="A222" s="20" t="str">
         <f t="shared" si="28"/>
         <v>T221</v>
@@ -21320,7 +21341,7 @@
       <c r="Q222" s="24"/>
       <c r="R222" s="24"/>
     </row>
-    <row r="223" spans="1:18" ht="96" hidden="1">
+    <row r="223" spans="1:18" ht="96">
       <c r="A223" s="20" t="str">
         <f t="shared" si="28"/>
         <v>T222</v>
@@ -21371,7 +21392,7 @@
       <c r="Q223" s="24"/>
       <c r="R223" s="24"/>
     </row>
-    <row r="224" spans="1:18" ht="80" hidden="1">
+    <row r="224" spans="1:18" ht="80">
       <c r="A224" s="20" t="str">
         <f t="shared" si="28"/>
         <v>T223</v>
@@ -21422,7 +21443,7 @@
       <c r="Q224" s="24"/>
       <c r="R224" s="24"/>
     </row>
-    <row r="225" spans="1:18" ht="80" hidden="1">
+    <row r="225" spans="1:18" ht="80">
       <c r="A225" s="20" t="str">
         <f t="shared" si="28"/>
         <v>T224</v>
@@ -21473,7 +21494,7 @@
       <c r="Q225" s="24"/>
       <c r="R225" s="24"/>
     </row>
-    <row r="226" spans="1:18" ht="64" hidden="1">
+    <row r="226" spans="1:18" ht="64">
       <c r="A226" s="20" t="str">
         <f t="shared" si="28"/>
         <v>T225</v>
@@ -21524,7 +21545,7 @@
       <c r="Q226" s="24"/>
       <c r="R226" s="24"/>
     </row>
-    <row r="227" spans="1:18" ht="80" hidden="1">
+    <row r="227" spans="1:18" ht="80">
       <c r="A227" s="20" t="str">
         <f t="shared" si="28"/>
         <v>T226</v>
@@ -21575,7 +21596,7 @@
       <c r="Q227" s="24"/>
       <c r="R227" s="24"/>
     </row>
-    <row r="228" spans="1:18" ht="64" hidden="1">
+    <row r="228" spans="1:18" ht="64">
       <c r="A228" s="20" t="str">
         <f t="shared" si="28"/>
         <v>T227</v>
@@ -21626,7 +21647,7 @@
       <c r="Q228" s="24"/>
       <c r="R228" s="24"/>
     </row>
-    <row r="229" spans="1:18" ht="48" hidden="1">
+    <row r="229" spans="1:18" ht="48">
       <c r="A229" s="20" t="str">
         <f t="shared" si="28"/>
         <v>T228</v>
@@ -21677,7 +21698,7 @@
       <c r="Q229" s="24"/>
       <c r="R229" s="24"/>
     </row>
-    <row r="230" spans="1:18" ht="80" hidden="1">
+    <row r="230" spans="1:18" ht="80">
       <c r="A230" s="20" t="str">
         <f t="shared" si="28"/>
         <v>T229</v>
@@ -21728,7 +21749,7 @@
       <c r="Q230" s="24"/>
       <c r="R230" s="24"/>
     </row>
-    <row r="231" spans="1:18" ht="80" hidden="1">
+    <row r="231" spans="1:18" ht="80">
       <c r="A231" s="20" t="str">
         <f t="shared" si="28"/>
         <v>T230</v>
@@ -21779,7 +21800,7 @@
       <c r="Q231" s="24"/>
       <c r="R231" s="24"/>
     </row>
-    <row r="232" spans="1:18" ht="48" hidden="1">
+    <row r="232" spans="1:18" ht="48">
       <c r="A232" s="20" t="str">
         <f t="shared" si="28"/>
         <v>T231</v>
@@ -21830,7 +21851,7 @@
       <c r="Q232" s="24"/>
       <c r="R232" s="24"/>
     </row>
-    <row r="233" spans="1:18" ht="96" hidden="1">
+    <row r="233" spans="1:18" ht="96">
       <c r="A233" s="20" t="str">
         <f t="shared" si="28"/>
         <v>T232</v>
@@ -21881,7 +21902,7 @@
       <c r="Q233" s="24"/>
       <c r="R233" s="24"/>
     </row>
-    <row r="234" spans="1:18" ht="96" hidden="1">
+    <row r="234" spans="1:18" ht="96">
       <c r="A234" s="20" t="str">
         <f t="shared" si="28"/>
         <v>T233</v>
@@ -21932,7 +21953,7 @@
       <c r="Q234" s="24"/>
       <c r="R234" s="24"/>
     </row>
-    <row r="235" spans="1:18" ht="80" hidden="1">
+    <row r="235" spans="1:18" ht="80">
       <c r="A235" s="20" t="str">
         <f t="shared" si="28"/>
         <v>T234</v>
@@ -21983,7 +22004,7 @@
       <c r="Q235" s="24"/>
       <c r="R235" s="24"/>
     </row>
-    <row r="236" spans="1:18" ht="80" hidden="1">
+    <row r="236" spans="1:18" ht="80">
       <c r="A236" s="20" t="str">
         <f t="shared" si="28"/>
         <v>T235</v>
@@ -22034,7 +22055,7 @@
       <c r="Q236" s="24"/>
       <c r="R236" s="24"/>
     </row>
-    <row r="237" spans="1:18" ht="48" hidden="1">
+    <row r="237" spans="1:18" ht="48">
       <c r="A237" s="20" t="str">
         <f t="shared" si="28"/>
         <v>T236</v>
@@ -22085,7 +22106,7 @@
       <c r="Q237" s="24"/>
       <c r="R237" s="24"/>
     </row>
-    <row r="238" spans="1:18" ht="32" hidden="1">
+    <row r="238" spans="1:18" ht="32">
       <c r="A238" s="20" t="str">
         <f t="shared" si="28"/>
         <v>T237</v>
@@ -22136,7 +22157,7 @@
       <c r="Q238" s="24"/>
       <c r="R238" s="24"/>
     </row>
-    <row r="239" spans="1:18" ht="80" hidden="1">
+    <row r="239" spans="1:18" ht="80">
       <c r="A239" s="20" t="str">
         <f t="shared" si="28"/>
         <v>T238</v>
@@ -22187,7 +22208,7 @@
       <c r="Q239" s="24"/>
       <c r="R239" s="24"/>
     </row>
-    <row r="240" spans="1:18" ht="80" hidden="1">
+    <row r="240" spans="1:18" ht="80">
       <c r="A240" s="20" t="str">
         <f t="shared" si="28"/>
         <v>T239</v>
@@ -22238,7 +22259,7 @@
       <c r="Q240" s="24"/>
       <c r="R240" s="24"/>
     </row>
-    <row r="241" spans="1:18" ht="48" hidden="1">
+    <row r="241" spans="1:18" ht="48">
       <c r="A241" s="20" t="str">
         <f t="shared" si="28"/>
         <v>T240</v>
@@ -22289,7 +22310,7 @@
       <c r="Q241" s="24"/>
       <c r="R241" s="24"/>
     </row>
-    <row r="242" spans="1:18" ht="32" hidden="1">
+    <row r="242" spans="1:18" ht="32">
       <c r="A242" s="20" t="str">
         <f t="shared" si="28"/>
         <v>T241</v>
@@ -22340,7 +22361,7 @@
       <c r="Q242" s="24"/>
       <c r="R242" s="24"/>
     </row>
-    <row r="243" spans="1:18" ht="32" hidden="1">
+    <row r="243" spans="1:18" ht="32">
       <c r="A243" s="20" t="str">
         <f t="shared" si="28"/>
         <v>T242</v>
@@ -22391,7 +22412,7 @@
       <c r="Q243" s="24"/>
       <c r="R243" s="24"/>
     </row>
-    <row r="244" spans="1:18" ht="32" hidden="1">
+    <row r="244" spans="1:18" ht="32">
       <c r="A244" s="20" t="str">
         <f t="shared" si="28"/>
         <v>T243</v>
@@ -22442,7 +22463,7 @@
       <c r="Q244" s="24"/>
       <c r="R244" s="24"/>
     </row>
-    <row r="245" spans="1:18" ht="80" hidden="1">
+    <row r="245" spans="1:18" ht="80">
       <c r="A245" s="20" t="str">
         <f t="shared" si="28"/>
         <v>T244</v>
@@ -22493,7 +22514,7 @@
       <c r="Q245" s="24"/>
       <c r="R245" s="24"/>
     </row>
-    <row r="246" spans="1:18" ht="32" hidden="1">
+    <row r="246" spans="1:18" ht="32">
       <c r="A246" s="20" t="str">
         <f t="shared" si="28"/>
         <v>T245</v>
@@ -22544,7 +22565,7 @@
       <c r="Q246" s="24"/>
       <c r="R246" s="24"/>
     </row>
-    <row r="247" spans="1:18" ht="32" hidden="1">
+    <row r="247" spans="1:18" ht="32">
       <c r="A247" s="20" t="str">
         <f t="shared" si="28"/>
         <v>T246</v>
@@ -22595,7 +22616,7 @@
       <c r="Q247" s="24"/>
       <c r="R247" s="24"/>
     </row>
-    <row r="248" spans="1:18" ht="80" hidden="1">
+    <row r="248" spans="1:18" ht="80">
       <c r="A248" s="20" t="str">
         <f t="shared" si="28"/>
         <v>T247</v>
@@ -22646,7 +22667,7 @@
       <c r="Q248" s="24"/>
       <c r="R248" s="24"/>
     </row>
-    <row r="249" spans="1:18" ht="64" hidden="1">
+    <row r="249" spans="1:18" ht="64">
       <c r="A249" s="20" t="str">
         <f t="shared" si="28"/>
         <v>T248</v>
@@ -22697,7 +22718,7 @@
       <c r="Q249" s="24"/>
       <c r="R249" s="24"/>
     </row>
-    <row r="250" spans="1:18" ht="64" hidden="1">
+    <row r="250" spans="1:18" ht="64">
       <c r="A250" s="20" t="str">
         <f t="shared" si="28"/>
         <v>T249</v>
@@ -22748,7 +22769,7 @@
       <c r="Q250" s="24"/>
       <c r="R250" s="24"/>
     </row>
-    <row r="251" spans="1:18" ht="96" hidden="1">
+    <row r="251" spans="1:18" ht="96">
       <c r="A251" s="20" t="str">
         <f t="shared" si="28"/>
         <v>T250</v>
@@ -22799,7 +22820,7 @@
       <c r="Q251" s="24"/>
       <c r="R251" s="24"/>
     </row>
-    <row r="252" spans="1:18" ht="48" hidden="1">
+    <row r="252" spans="1:18" ht="48">
       <c r="A252" s="20" t="str">
         <f t="shared" si="28"/>
         <v>T251</v>
@@ -22850,7 +22871,7 @@
       <c r="Q252" s="24"/>
       <c r="R252" s="24"/>
     </row>
-    <row r="253" spans="1:18" ht="80" hidden="1">
+    <row r="253" spans="1:18" ht="80">
       <c r="A253" s="20" t="str">
         <f t="shared" si="28"/>
         <v>T252</v>
@@ -22901,7 +22922,7 @@
       <c r="Q253" s="24"/>
       <c r="R253" s="24"/>
     </row>
-    <row r="254" spans="1:18" ht="16" hidden="1">
+    <row r="254" spans="1:18" ht="16">
       <c r="A254" s="20" t="str">
         <f t="shared" si="28"/>
         <v>T253</v>
@@ -22952,7 +22973,7 @@
       <c r="Q254" s="24"/>
       <c r="R254" s="24"/>
     </row>
-    <row r="255" spans="1:18" ht="16" hidden="1">
+    <row r="255" spans="1:18" ht="16">
       <c r="A255" s="20" t="str">
         <f t="shared" ref="A255:A269" si="33">CONCATENATE("T",ROW(A255)-1)</f>
         <v>T254</v>
@@ -23013,7 +23034,7 @@
       </c>
       <c r="R255" s="24"/>
     </row>
-    <row r="256" spans="1:18" ht="16" hidden="1">
+    <row r="256" spans="1:18" ht="16">
       <c r="A256" s="20" t="str">
         <f t="shared" si="33"/>
         <v>T255</v>
@@ -23074,7 +23095,7 @@
       </c>
       <c r="R256" s="24"/>
     </row>
-    <row r="257" spans="1:18" ht="16" hidden="1">
+    <row r="257" spans="1:18" ht="16">
       <c r="A257" s="20" t="str">
         <f t="shared" si="33"/>
         <v>T256</v>
@@ -23135,7 +23156,7 @@
       </c>
       <c r="R257" s="24"/>
     </row>
-    <row r="258" spans="1:18" ht="16" hidden="1">
+    <row r="258" spans="1:18" ht="16">
       <c r="A258" s="20" t="str">
         <f t="shared" si="33"/>
         <v>T257</v>
@@ -23196,7 +23217,7 @@
       </c>
       <c r="R258" s="24"/>
     </row>
-    <row r="259" spans="1:18" ht="240" hidden="1">
+    <row r="259" spans="1:18" ht="240">
       <c r="A259" s="20" t="str">
         <f t="shared" si="33"/>
         <v>T258</v>
@@ -23257,7 +23278,7 @@
       </c>
       <c r="R259" s="24"/>
     </row>
-    <row r="260" spans="1:18" ht="16" hidden="1">
+    <row r="260" spans="1:18" ht="16">
       <c r="A260" s="20" t="str">
         <f t="shared" si="33"/>
         <v>T259</v>
@@ -23318,7 +23339,7 @@
       </c>
       <c r="R260" s="24"/>
     </row>
-    <row r="261" spans="1:18" ht="16" hidden="1">
+    <row r="261" spans="1:18" ht="16">
       <c r="A261" s="20" t="str">
         <f t="shared" si="33"/>
         <v>T260</v>
@@ -23379,7 +23400,7 @@
       </c>
       <c r="R261" s="24"/>
     </row>
-    <row r="262" spans="1:18" ht="32" hidden="1">
+    <row r="262" spans="1:18" ht="32">
       <c r="A262" s="20" t="str">
         <f t="shared" si="33"/>
         <v>T261</v>
@@ -23436,7 +23457,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="263" spans="1:18" ht="32" hidden="1">
+    <row r="263" spans="1:18" ht="32">
       <c r="A263" s="20" t="str">
         <f t="shared" si="33"/>
         <v>T262</v>
@@ -23497,7 +23518,7 @@
       </c>
       <c r="R263" s="24"/>
     </row>
-    <row r="264" spans="1:18" ht="128" hidden="1">
+    <row r="264" spans="1:18" ht="128">
       <c r="A264" s="20" t="str">
         <f t="shared" si="33"/>
         <v>T263</v>
@@ -23558,7 +23579,7 @@
       </c>
       <c r="R264" s="24"/>
     </row>
-    <row r="265" spans="1:18" ht="64" hidden="1">
+    <row r="265" spans="1:18" ht="64">
       <c r="A265" s="20" t="str">
         <f t="shared" si="33"/>
         <v>T264</v>
@@ -23619,7 +23640,7 @@
       </c>
       <c r="R265" s="24"/>
     </row>
-    <row r="266" spans="1:18" ht="48" hidden="1">
+    <row r="266" spans="1:18" ht="48">
       <c r="A266" s="20" t="str">
         <f t="shared" si="33"/>
         <v>T265</v>
@@ -23680,7 +23701,7 @@
       </c>
       <c r="R266" s="24"/>
     </row>
-    <row r="267" spans="1:18" ht="32" hidden="1">
+    <row r="267" spans="1:18" ht="32">
       <c r="A267" s="20" t="str">
         <f t="shared" si="33"/>
         <v>T266</v>
@@ -23737,7 +23758,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="268" spans="1:18" ht="32" hidden="1">
+    <row r="268" spans="1:18" ht="32">
       <c r="A268" s="20" t="str">
         <f t="shared" si="33"/>
         <v>T267</v>
@@ -23798,7 +23819,7 @@
       </c>
       <c r="R268" s="24"/>
     </row>
-    <row r="269" spans="1:18" ht="32" hidden="1">
+    <row r="269" spans="1:18" ht="32">
       <c r="A269" s="20" t="str">
         <f t="shared" si="33"/>
         <v>T268</v>
@@ -23859,7 +23880,7 @@
       </c>
       <c r="R269" s="24"/>
     </row>
-    <row r="270" spans="1:18" ht="128" hidden="1">
+    <row r="270" spans="1:18" ht="128">
       <c r="A270" s="20" t="str">
         <f t="shared" ref="A270:A313" si="40">CONCATENATE("T",ROW(A270)-1)</f>
         <v>T269</v>
@@ -23920,7 +23941,7 @@
       </c>
       <c r="R270" s="24"/>
     </row>
-    <row r="271" spans="1:18" ht="32" hidden="1">
+    <row r="271" spans="1:18" ht="32">
       <c r="A271" s="20" t="str">
         <f t="shared" si="40"/>
         <v>T270</v>
@@ -23981,7 +24002,7 @@
       </c>
       <c r="R271" s="24"/>
     </row>
-    <row r="272" spans="1:18" ht="96" hidden="1">
+    <row r="272" spans="1:18" ht="96">
       <c r="A272" s="20" t="str">
         <f t="shared" si="40"/>
         <v>T271</v>
@@ -24042,7 +24063,7 @@
       </c>
       <c r="R272" s="24"/>
     </row>
-    <row r="273" spans="1:18" ht="64" hidden="1">
+    <row r="273" spans="1:18" ht="64">
       <c r="A273" s="20" t="str">
         <f t="shared" si="40"/>
         <v>T272</v>
@@ -24103,7 +24124,7 @@
       </c>
       <c r="R273" s="24"/>
     </row>
-    <row r="274" spans="1:18" ht="128" hidden="1">
+    <row r="274" spans="1:18" ht="128">
       <c r="A274" s="20" t="str">
         <f t="shared" si="40"/>
         <v>T273</v>
@@ -25061,7 +25082,7 @@
       </c>
       <c r="R289" s="24"/>
     </row>
-    <row r="290" spans="1:18" ht="96" hidden="1">
+    <row r="290" spans="1:18" ht="96">
       <c r="A290" s="20" t="str">
         <f t="shared" si="40"/>
         <v>T289</v>
@@ -25124,7 +25145,7 @@
         <v>681</v>
       </c>
     </row>
-    <row r="291" spans="1:18" ht="176" hidden="1">
+    <row r="291" spans="1:18" ht="176">
       <c r="A291" s="20" t="str">
         <f t="shared" si="40"/>
         <v>T290</v>
@@ -25185,7 +25206,7 @@
       </c>
       <c r="R291" s="24"/>
     </row>
-    <row r="292" spans="1:18" ht="380" hidden="1">
+    <row r="292" spans="1:18" ht="380">
       <c r="A292" s="20" t="str">
         <f t="shared" si="40"/>
         <v>T291</v>
@@ -25246,7 +25267,7 @@
       </c>
       <c r="R292" s="24"/>
     </row>
-    <row r="293" spans="1:18" ht="144" hidden="1">
+    <row r="293" spans="1:18" ht="144">
       <c r="A293" s="20" t="str">
         <f t="shared" si="40"/>
         <v>T292</v>
@@ -25307,7 +25328,7 @@
       </c>
       <c r="R293" s="24"/>
     </row>
-    <row r="294" spans="1:18" ht="112" hidden="1">
+    <row r="294" spans="1:18" ht="112">
       <c r="A294" s="20" t="str">
         <f t="shared" si="40"/>
         <v>T293</v>
@@ -25368,7 +25389,7 @@
       </c>
       <c r="R294" s="24"/>
     </row>
-    <row r="295" spans="1:18" ht="96" hidden="1">
+    <row r="295" spans="1:18" ht="96">
       <c r="A295" s="20" t="str">
         <f t="shared" si="40"/>
         <v>T294</v>
@@ -25429,7 +25450,7 @@
       </c>
       <c r="R295" s="24"/>
     </row>
-    <row r="296" spans="1:18" ht="32" hidden="1">
+    <row r="296" spans="1:18" ht="32">
       <c r="A296" s="20" t="str">
         <f t="shared" si="40"/>
         <v>T295</v>
@@ -25488,7 +25509,7 @@
       <c r="Q296" s="24"/>
       <c r="R296" s="24"/>
     </row>
-    <row r="297" spans="1:18" ht="32" hidden="1">
+    <row r="297" spans="1:18" ht="32">
       <c r="A297" s="20" t="str">
         <f t="shared" si="40"/>
         <v>T296</v>
@@ -25549,7 +25570,7 @@
       </c>
       <c r="R297" s="24"/>
     </row>
-    <row r="298" spans="1:18" ht="48" hidden="1">
+    <row r="298" spans="1:18" ht="48">
       <c r="A298" s="20" t="str">
         <f t="shared" si="40"/>
         <v>T297</v>
@@ -25610,7 +25631,7 @@
       </c>
       <c r="R298" s="24"/>
     </row>
-    <row r="299" spans="1:18" ht="16" hidden="1">
+    <row r="299" spans="1:18" ht="16">
       <c r="A299" s="20" t="str">
         <f t="shared" si="40"/>
         <v>T298</v>
@@ -25669,7 +25690,7 @@
       <c r="Q299" s="24"/>
       <c r="R299" s="24"/>
     </row>
-    <row r="300" spans="1:18" ht="16" hidden="1">
+    <row r="300" spans="1:18" ht="16">
       <c r="A300" s="20" t="str">
         <f t="shared" si="40"/>
         <v>T299</v>
@@ -25728,7 +25749,7 @@
       <c r="Q300" s="24"/>
       <c r="R300" s="24"/>
     </row>
-    <row r="301" spans="1:18" ht="16" hidden="1">
+    <row r="301" spans="1:18" ht="16">
       <c r="A301" s="20" t="str">
         <f t="shared" si="40"/>
         <v>T300</v>
@@ -25787,7 +25808,7 @@
       <c r="Q301" s="24"/>
       <c r="R301" s="24"/>
     </row>
-    <row r="302" spans="1:18" ht="16" hidden="1">
+    <row r="302" spans="1:18" ht="16">
       <c r="A302" s="20" t="str">
         <f t="shared" si="40"/>
         <v>T301</v>
@@ -25848,7 +25869,7 @@
       </c>
       <c r="R302" s="24"/>
     </row>
-    <row r="303" spans="1:18" ht="240" hidden="1">
+    <row r="303" spans="1:18" ht="240">
       <c r="A303" s="20" t="str">
         <f t="shared" si="40"/>
         <v>T302</v>
@@ -25909,7 +25930,7 @@
       </c>
       <c r="R303" s="24"/>
     </row>
-    <row r="304" spans="1:18" ht="16" hidden="1">
+    <row r="304" spans="1:18" ht="16">
       <c r="A304" s="20" t="str">
         <f t="shared" si="40"/>
         <v>T303</v>
@@ -25968,7 +25989,7 @@
       <c r="Q304" s="24"/>
       <c r="R304" s="24"/>
     </row>
-    <row r="305" spans="1:18" ht="16" hidden="1">
+    <row r="305" spans="1:18" ht="16">
       <c r="A305" s="20" t="str">
         <f t="shared" si="40"/>
         <v>T304</v>
@@ -26029,7 +26050,7 @@
       </c>
       <c r="R305" s="24"/>
     </row>
-    <row r="306" spans="1:18" ht="32" hidden="1">
+    <row r="306" spans="1:18" ht="32">
       <c r="A306" s="20" t="str">
         <f t="shared" si="40"/>
         <v>T305</v>
@@ -26086,7 +26107,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="307" spans="1:18" ht="32" hidden="1">
+    <row r="307" spans="1:18" ht="32">
       <c r="A307" s="20" t="str">
         <f t="shared" si="40"/>
         <v>T306</v>
@@ -26147,7 +26168,7 @@
       </c>
       <c r="R307" s="24"/>
     </row>
-    <row r="308" spans="1:18" ht="128" hidden="1">
+    <row r="308" spans="1:18" ht="128">
       <c r="A308" s="20" t="str">
         <f t="shared" si="40"/>
         <v>T307</v>
@@ -26208,7 +26229,7 @@
       </c>
       <c r="R308" s="24"/>
     </row>
-    <row r="309" spans="1:18" ht="64" hidden="1">
+    <row r="309" spans="1:18" ht="64">
       <c r="A309" s="20" t="str">
         <f t="shared" si="40"/>
         <v>T308</v>
@@ -26269,7 +26290,7 @@
       </c>
       <c r="R309" s="24"/>
     </row>
-    <row r="310" spans="1:18" ht="48" hidden="1">
+    <row r="310" spans="1:18" ht="48">
       <c r="A310" s="20" t="str">
         <f t="shared" si="40"/>
         <v>T309</v>
@@ -26330,7 +26351,7 @@
       </c>
       <c r="R310" s="24"/>
     </row>
-    <row r="311" spans="1:18" ht="32" hidden="1">
+    <row r="311" spans="1:18" ht="32">
       <c r="A311" s="20" t="str">
         <f t="shared" si="40"/>
         <v>T310</v>
@@ -26387,7 +26408,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="312" spans="1:18" ht="32" hidden="1">
+    <row r="312" spans="1:18" ht="32">
       <c r="A312" s="20" t="str">
         <f t="shared" si="40"/>
         <v>T311</v>
@@ -26448,7 +26469,7 @@
       </c>
       <c r="R312" s="24"/>
     </row>
-    <row r="313" spans="1:18" ht="16" hidden="1">
+    <row r="313" spans="1:18" ht="16">
       <c r="A313" s="20" t="str">
         <f t="shared" si="40"/>
         <v>T312</v>
@@ -26507,7 +26528,7 @@
       <c r="Q313" s="24"/>
       <c r="R313" s="24"/>
     </row>
-    <row r="314" spans="1:18" ht="96" hidden="1">
+    <row r="314" spans="1:18" ht="96">
       <c r="A314" s="20" t="str">
         <f t="shared" ref="A314:A320" si="53">CONCATENATE("T",ROW(A314)-1)</f>
         <v>T313</v>
@@ -26558,7 +26579,7 @@
       <c r="Q314" s="24"/>
       <c r="R314" s="24"/>
     </row>
-    <row r="315" spans="1:18" ht="32" hidden="1">
+    <row r="315" spans="1:18" ht="32">
       <c r="A315" s="20" t="str">
         <f t="shared" si="53"/>
         <v>T314</v>
@@ -26609,7 +26630,7 @@
       <c r="Q315" s="24"/>
       <c r="R315" s="24"/>
     </row>
-    <row r="316" spans="1:18" ht="80" hidden="1">
+    <row r="316" spans="1:18" ht="80">
       <c r="A316" s="20" t="str">
         <f t="shared" si="53"/>
         <v>T315</v>
@@ -26660,7 +26681,7 @@
       <c r="Q316" s="24"/>
       <c r="R316" s="24"/>
     </row>
-    <row r="317" spans="1:18" ht="96" hidden="1">
+    <row r="317" spans="1:18" ht="96">
       <c r="A317" s="20" t="str">
         <f t="shared" si="53"/>
         <v>T316</v>
@@ -26711,7 +26732,7 @@
       <c r="Q317" s="24"/>
       <c r="R317" s="24"/>
     </row>
-    <row r="318" spans="1:18" ht="64" hidden="1">
+    <row r="318" spans="1:18" ht="64">
       <c r="A318" s="20" t="str">
         <f t="shared" si="53"/>
         <v>T317</v>
@@ -26762,7 +26783,7 @@
       <c r="Q318" s="24"/>
       <c r="R318" s="24"/>
     </row>
-    <row r="319" spans="1:18" ht="112" hidden="1">
+    <row r="319" spans="1:18" ht="112">
       <c r="A319" s="20" t="str">
         <f t="shared" si="53"/>
         <v>T318</v>
@@ -26813,7 +26834,7 @@
       <c r="Q319" s="24"/>
       <c r="R319" s="24"/>
     </row>
-    <row r="320" spans="1:18" ht="64" hidden="1">
+    <row r="320" spans="1:18" ht="64">
       <c r="A320" s="20" t="str">
         <f t="shared" si="53"/>
         <v>T319</v>
@@ -26864,7 +26885,7 @@
       <c r="Q320" s="24"/>
       <c r="R320" s="24"/>
     </row>
-    <row r="321" spans="1:18" ht="16" hidden="1">
+    <row r="321" spans="1:18" ht="16">
       <c r="A321" s="20" t="str">
         <f t="shared" ref="A321:A322" si="56">CONCATENATE("T",ROW(A321)-1)</f>
         <v>T320</v>
@@ -26915,7 +26936,7 @@
       <c r="Q321" s="24"/>
       <c r="R321" s="24"/>
     </row>
-    <row r="322" spans="1:18" ht="80" hidden="1">
+    <row r="322" spans="1:18" ht="80">
       <c r="A322" s="20" t="str">
         <f t="shared" si="56"/>
         <v>T321</v>
@@ -31999,10 +32020,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C51FC597-29FA-1D4E-A4C8-B79027768242}">
-  <dimension ref="A1:G9"/>
+  <dimension ref="A1:I9"/>
   <sheetViews>
-    <sheetView zoomScale="163" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+    <sheetView tabSelected="1" topLeftCell="D4" zoomScale="163" workbookViewId="0">
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15"/>
@@ -32017,7 +32038,7 @@
     <col min="8" max="16384" width="10.83203125" style="26"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="16">
+    <row r="1" spans="1:9" ht="16">
       <c r="A1" s="26" t="s">
         <v>935</v>
       </c>
@@ -32039,8 +32060,14 @@
       <c r="G1" s="28" t="s">
         <v>940</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" ht="64">
+      <c r="H1" s="26" t="s">
+        <v>1197</v>
+      </c>
+      <c r="I1" s="26" t="s">
+        <v>1200</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="64">
       <c r="A2" s="26">
         <f>ROW(Tabella4[[#This Row],[Name]])-1</f>
         <v>1</v>
@@ -32063,8 +32090,11 @@
       <c r="G2" s="28" t="s">
         <v>1196</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" ht="64">
+      <c r="H2" s="26" t="s">
+        <v>1198</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="64">
       <c r="A3" s="26">
         <f>ROW(Tabella4[[#This Row],[Name]])-1</f>
         <v>2</v>
@@ -32087,8 +32117,11 @@
       <c r="G3" s="28">
         <v>8</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" ht="80">
+      <c r="H3" s="26" t="s">
+        <v>1198</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="80">
       <c r="A4" s="26">
         <f>ROW(Tabella4[[#This Row],[Name]])-1</f>
         <v>3</v>
@@ -32111,8 +32144,11 @@
       <c r="G4" s="28">
         <v>6</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" ht="32">
+      <c r="H4" s="26" t="s">
+        <v>1198</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="32">
       <c r="A5" s="26">
         <f>ROW(Tabella4[[#This Row],[Name]])-1</f>
         <v>4</v>
@@ -32135,8 +32171,11 @@
       <c r="G5" s="28">
         <v>5</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" ht="32">
+      <c r="H5" s="26" t="s">
+        <v>1199</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="32">
       <c r="A6" s="26">
         <f>ROW(Tabella4[[#This Row],[Name]])-1</f>
         <v>5</v>
@@ -32159,8 +32198,14 @@
       <c r="G6" s="28">
         <v>5</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" ht="32">
+      <c r="H6" s="26" t="s">
+        <v>1199</v>
+      </c>
+      <c r="I6" s="26" t="s">
+        <v>1201</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="32">
       <c r="A7" s="26">
         <f>ROW(Tabella4[[#This Row],[Name]])-1</f>
         <v>6</v>
@@ -32183,8 +32228,11 @@
       <c r="G7" s="28">
         <v>5</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" ht="80">
+      <c r="H7" s="26" t="s">
+        <v>1199</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="80">
       <c r="A8" s="26">
         <f>ROW(Tabella4[[#This Row],[Name]])-1</f>
         <v>7</v>
@@ -32207,8 +32255,11 @@
       <c r="G8" s="28">
         <v>11</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" ht="96">
+      <c r="H8" s="26" t="s">
+        <v>1198</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="96">
       <c r="A9" s="26">
         <f>ROW(Tabella4[[#This Row],[Name]])-1</f>
         <v>8</v>
@@ -32230,6 +32281,9 @@
       </c>
       <c r="G9" s="28" t="s">
         <v>1196</v>
+      </c>
+      <c r="H9" s="26" t="s">
+        <v>1198</v>
       </c>
     </row>
   </sheetData>
@@ -32248,7 +32302,7 @@
   </sheetPr>
   <dimension ref="A1:C24"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="164" workbookViewId="0">
+    <sheetView zoomScale="164" workbookViewId="0">
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
@@ -33315,28 +33369,8 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="633f040f-4953-46e7-8610-82b0c5296ba0">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="f62ef740-d444-4f18-80a2-7590fdcab1ce" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x0101009A9CE0B21D9C3A45B31425227616CD6F" ma:contentTypeVersion="12" ma:contentTypeDescription="Creare un nuovo documento." ma:contentTypeScope="" ma:versionID="577a0f91e6a70618273620f4b28b7476">
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="633f040f-4953-46e7-8610-82b0c5296ba0" xmlns:ns3="f62ef740-d444-4f18-80a2-7590fdcab1ce" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="0eeb42859aa2ae2e58f994ed451e965e" ns2:_="" ns3:_="">
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x0101009A9CE0B21D9C3A45B31425227616CD6F" ma:contentTypeVersion="34" ma:contentTypeDescription="Creare un nuovo documento." ma:contentTypeScope="" ma:versionID="8a882b22c4c6ceab40c069a6a2420ef3">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="633f040f-4953-46e7-8610-82b0c5296ba0" xmlns:ns3="f62ef740-d444-4f18-80a2-7590fdcab1ce" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="77035a69dc4d6b80a35ec1b02b2030a4" ns2:_="" ns3:_="">
     <xsd:import namespace="633f040f-4953-46e7-8610-82b0c5296ba0"/>
     <xsd:import namespace="f62ef740-d444-4f18-80a2-7590fdcab1ce"/>
     <xsd:element name="properties">
@@ -33356,6 +33390,28 @@
                 <xsd:element ref="ns2:MediaServiceEventHashCode" minOccurs="0"/>
                 <xsd:element ref="ns2:MediaServiceObjectDetectorVersions" minOccurs="0"/>
                 <xsd:element ref="ns2:MediaServiceSearchProperties" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceDateTaken" minOccurs="0"/>
+                <xsd:element ref="ns2:NotebookType" minOccurs="0"/>
+                <xsd:element ref="ns2:FolderType" minOccurs="0"/>
+                <xsd:element ref="ns2:CultureName" minOccurs="0"/>
+                <xsd:element ref="ns2:AppVersion" minOccurs="0"/>
+                <xsd:element ref="ns2:TeamsChannelId" minOccurs="0"/>
+                <xsd:element ref="ns2:Owner" minOccurs="0"/>
+                <xsd:element ref="ns2:Math_Settings" minOccurs="0"/>
+                <xsd:element ref="ns2:DefaultSectionNames" minOccurs="0"/>
+                <xsd:element ref="ns2:Templates" minOccurs="0"/>
+                <xsd:element ref="ns2:Teachers" minOccurs="0"/>
+                <xsd:element ref="ns2:Students" minOccurs="0"/>
+                <xsd:element ref="ns2:Student_Groups" minOccurs="0"/>
+                <xsd:element ref="ns2:Distribution_Groups" minOccurs="0"/>
+                <xsd:element ref="ns2:LMS_Mappings" minOccurs="0"/>
+                <xsd:element ref="ns2:Invited_Teachers" minOccurs="0"/>
+                <xsd:element ref="ns2:Invited_Students" minOccurs="0"/>
+                <xsd:element ref="ns2:Self_Registration_Enabled" minOccurs="0"/>
+                <xsd:element ref="ns2:Has_Teacher_Only_SectionGroup" minOccurs="0"/>
+                <xsd:element ref="ns2:Is_Collaboration_Space_Locked" minOccurs="0"/>
+                <xsd:element ref="ns2:IsNotebookLocked" minOccurs="0"/>
+                <xsd:element ref="ns2:Teams_Channel_Section_Location" minOccurs="0"/>
               </xsd:all>
             </xsd:complexType>
           </xsd:element>
@@ -33408,6 +33464,184 @@
     <xsd:element name="MediaServiceSearchProperties" ma:index="19" nillable="true" ma:displayName="MediaServiceSearchProperties" ma:hidden="true" ma:internalName="MediaServiceSearchProperties" ma:readOnly="true">
       <xsd:simpleType>
         <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceDateTaken" ma:index="20" nillable="true" ma:displayName="MediaServiceDateTaken" ma:hidden="true" ma:indexed="true" ma:internalName="MediaServiceDateTaken" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="NotebookType" ma:index="21" nillable="true" ma:displayName="Notebook Type" ma:internalName="NotebookType">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="FolderType" ma:index="22" nillable="true" ma:displayName="Folder Type" ma:internalName="FolderType">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="CultureName" ma:index="23" nillable="true" ma:displayName="Culture Name" ma:internalName="CultureName">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="AppVersion" ma:index="24" nillable="true" ma:displayName="App Version" ma:internalName="AppVersion">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="TeamsChannelId" ma:index="25" nillable="true" ma:displayName="Teams Channel Id" ma:internalName="TeamsChannelId">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="Owner" ma:index="26" nillable="true" ma:displayName="Owner" ma:internalName="Owner">
+      <xsd:complexType>
+        <xsd:complexContent>
+          <xsd:extension base="dms:User">
+            <xsd:sequence>
+              <xsd:element name="UserInfo" minOccurs="0" maxOccurs="unbounded">
+                <xsd:complexType>
+                  <xsd:sequence>
+                    <xsd:element name="DisplayName" type="xsd:string" minOccurs="0"/>
+                    <xsd:element name="AccountId" type="dms:UserId" minOccurs="0" nillable="true"/>
+                    <xsd:element name="AccountType" type="xsd:string" minOccurs="0"/>
+                  </xsd:sequence>
+                </xsd:complexType>
+              </xsd:element>
+            </xsd:sequence>
+          </xsd:extension>
+        </xsd:complexContent>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="Math_Settings" ma:index="27" nillable="true" ma:displayName="Math Settings" ma:internalName="Math_Settings">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="DefaultSectionNames" ma:index="28" nillable="true" ma:displayName="Default Section Names" ma:internalName="DefaultSectionNames">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="Templates" ma:index="29" nillable="true" ma:displayName="Templates" ma:internalName="Templates">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="Teachers" ma:index="30" nillable="true" ma:displayName="Teachers" ma:internalName="Teachers">
+      <xsd:complexType>
+        <xsd:complexContent>
+          <xsd:extension base="dms:UserMulti">
+            <xsd:sequence>
+              <xsd:element name="UserInfo" minOccurs="0" maxOccurs="unbounded">
+                <xsd:complexType>
+                  <xsd:sequence>
+                    <xsd:element name="DisplayName" type="xsd:string" minOccurs="0"/>
+                    <xsd:element name="AccountId" type="dms:UserId" minOccurs="0" nillable="true"/>
+                    <xsd:element name="AccountType" type="xsd:string" minOccurs="0"/>
+                  </xsd:sequence>
+                </xsd:complexType>
+              </xsd:element>
+            </xsd:sequence>
+          </xsd:extension>
+        </xsd:complexContent>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="Students" ma:index="31" nillable="true" ma:displayName="Students" ma:internalName="Students">
+      <xsd:complexType>
+        <xsd:complexContent>
+          <xsd:extension base="dms:UserMulti">
+            <xsd:sequence>
+              <xsd:element name="UserInfo" minOccurs="0" maxOccurs="unbounded">
+                <xsd:complexType>
+                  <xsd:sequence>
+                    <xsd:element name="DisplayName" type="xsd:string" minOccurs="0"/>
+                    <xsd:element name="AccountId" type="dms:UserId" minOccurs="0" nillable="true"/>
+                    <xsd:element name="AccountType" type="xsd:string" minOccurs="0"/>
+                  </xsd:sequence>
+                </xsd:complexType>
+              </xsd:element>
+            </xsd:sequence>
+          </xsd:extension>
+        </xsd:complexContent>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="Student_Groups" ma:index="32" nillable="true" ma:displayName="Student Groups" ma:internalName="Student_Groups">
+      <xsd:complexType>
+        <xsd:complexContent>
+          <xsd:extension base="dms:UserMulti">
+            <xsd:sequence>
+              <xsd:element name="UserInfo" minOccurs="0" maxOccurs="unbounded">
+                <xsd:complexType>
+                  <xsd:sequence>
+                    <xsd:element name="DisplayName" type="xsd:string" minOccurs="0"/>
+                    <xsd:element name="AccountId" type="dms:UserId" minOccurs="0" nillable="true"/>
+                    <xsd:element name="AccountType" type="xsd:string" minOccurs="0"/>
+                  </xsd:sequence>
+                </xsd:complexType>
+              </xsd:element>
+            </xsd:sequence>
+          </xsd:extension>
+        </xsd:complexContent>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="Distribution_Groups" ma:index="33" nillable="true" ma:displayName="Distribution Groups" ma:internalName="Distribution_Groups">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="LMS_Mappings" ma:index="34" nillable="true" ma:displayName="LMS Mappings" ma:internalName="LMS_Mappings">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="Invited_Teachers" ma:index="35" nillable="true" ma:displayName="Invited Teachers" ma:internalName="Invited_Teachers">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="Invited_Students" ma:index="36" nillable="true" ma:displayName="Invited Students" ma:internalName="Invited_Students">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="Self_Registration_Enabled" ma:index="37" nillable="true" ma:displayName="Self Registration Enabled" ma:internalName="Self_Registration_Enabled">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Boolean"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="Has_Teacher_Only_SectionGroup" ma:index="38" nillable="true" ma:displayName="Has Teacher Only SectionGroup" ma:internalName="Has_Teacher_Only_SectionGroup">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Boolean"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="Is_Collaboration_Space_Locked" ma:index="39" nillable="true" ma:displayName="Is Collaboration Space Locked" ma:internalName="Is_Collaboration_Space_Locked">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Boolean"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="IsNotebookLocked" ma:index="40" nillable="true" ma:displayName="Is Notebook Locked" ma:internalName="IsNotebookLocked">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Boolean"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="Teams_Channel_Section_Location" ma:index="41" nillable="true" ma:displayName="Teams Channel Section Location" ma:internalName="Teams_Channel_Section_Location">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
       </xsd:simpleType>
     </xsd:element>
   </xsd:schema>
@@ -33551,33 +33785,73 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2C6CC7BA-2E2C-4B0D-8103-11A51D82E8EC}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{83D5100D-0E56-4B30-B42D-2AEC6B837C39}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="633f040f-4953-46e7-8610-82b0c5296ba0"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="f62ef740-d444-4f18-80a2-7590fdcab1ce"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="633f040f-4953-46e7-8610-82b0c5296ba0">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="f62ef740-d444-4f18-80a2-7590fdcab1ce" xsi:nil="true"/>
+    <Has_Teacher_Only_SectionGroup xmlns="633f040f-4953-46e7-8610-82b0c5296ba0" xsi:nil="true"/>
+    <Teachers xmlns="633f040f-4953-46e7-8610-82b0c5296ba0">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </Teachers>
+    <IsNotebookLocked xmlns="633f040f-4953-46e7-8610-82b0c5296ba0" xsi:nil="true"/>
+    <CultureName xmlns="633f040f-4953-46e7-8610-82b0c5296ba0" xsi:nil="true"/>
+    <Owner xmlns="633f040f-4953-46e7-8610-82b0c5296ba0">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </Owner>
+    <Distribution_Groups xmlns="633f040f-4953-46e7-8610-82b0c5296ba0" xsi:nil="true"/>
+    <TeamsChannelId xmlns="633f040f-4953-46e7-8610-82b0c5296ba0" xsi:nil="true"/>
+    <Invited_Teachers xmlns="633f040f-4953-46e7-8610-82b0c5296ba0" xsi:nil="true"/>
+    <NotebookType xmlns="633f040f-4953-46e7-8610-82b0c5296ba0" xsi:nil="true"/>
+    <AppVersion xmlns="633f040f-4953-46e7-8610-82b0c5296ba0" xsi:nil="true"/>
+    <DefaultSectionNames xmlns="633f040f-4953-46e7-8610-82b0c5296ba0" xsi:nil="true"/>
+    <Is_Collaboration_Space_Locked xmlns="633f040f-4953-46e7-8610-82b0c5296ba0" xsi:nil="true"/>
+    <Templates xmlns="633f040f-4953-46e7-8610-82b0c5296ba0" xsi:nil="true"/>
+    <FolderType xmlns="633f040f-4953-46e7-8610-82b0c5296ba0" xsi:nil="true"/>
+    <Student_Groups xmlns="633f040f-4953-46e7-8610-82b0c5296ba0">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </Student_Groups>
+    <Teams_Channel_Section_Location xmlns="633f040f-4953-46e7-8610-82b0c5296ba0" xsi:nil="true"/>
+    <Math_Settings xmlns="633f040f-4953-46e7-8610-82b0c5296ba0" xsi:nil="true"/>
+    <Self_Registration_Enabled xmlns="633f040f-4953-46e7-8610-82b0c5296ba0" xsi:nil="true"/>
+    <Students xmlns="633f040f-4953-46e7-8610-82b0c5296ba0">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </Students>
+    <LMS_Mappings xmlns="633f040f-4953-46e7-8610-82b0c5296ba0" xsi:nil="true"/>
+    <Invited_Students xmlns="633f040f-4953-46e7-8610-82b0c5296ba0" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2F919C9F-DDA6-4ECE-8C26-43CAC964EF66}">
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{36C20BFB-BCC5-4457-BE44-22D2F12F84BE}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
@@ -33593,4 +33867,29 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2C6CC7BA-2E2C-4B0D-8103-11A51D82E8EC}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{83D5100D-0E56-4B30-B42D-2AEC6B837C39}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="f62ef740-d444-4f18-80a2-7590fdcab1ce"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="633f040f-4953-46e7-8610-82b0c5296ba0"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
aggiunte funzioni di aggiornamento macm e di rimozione di asset
</commit_message>
<xml_diff>
--- a/apps/static/assets/dbs/ThreatCatalogComplete.xlsx
+++ b/apps/static/assets/dbs/ThreatCatalogComplete.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11013"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11027"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fefox/Desktop/AutomaticAttackPlanGenerator/apps/static/assets/dbs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8DB641AA-0336-A840-B72A-42884C5543B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{6941AD7D-1109-9345-93F2-E361D1A3B189}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16260" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,7 +29,7 @@
   </definedNames>
   <calcPr calcId="191028"/>
   <pivotCaches>
-    <pivotCache cacheId="3" r:id="rId11"/>
+    <pivotCache cacheId="6" r:id="rId11"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -51,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4674" uniqueCount="1202">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4676" uniqueCount="1204">
   <si>
     <t>TID</t>
   </si>
@@ -2967,9 +2967,6 @@
     <t>match (n:Network) return n.component_id as component_id</t>
   </si>
   <si>
-    <t>nmap -v {ip_range}</t>
-  </si>
-  <si>
     <t>573, 574</t>
   </si>
   <si>
@@ -3699,6 +3696,15 @@
   </si>
   <si>
     <t>nmap_classic</t>
+  </si>
+  <si>
+    <t>AllowedOutputExtensions</t>
+  </si>
+  <si>
+    <t>.xml</t>
+  </si>
+  <si>
+    <t>nmap -sV -O -oX {output_file} -T4 --min-parallelism 100 {ip_range}</t>
   </si>
 </sst>
 </file>
@@ -4083,20 +4089,20 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="31">
+  <dxfs count="32">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -4106,6 +4112,9 @@
           <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -9194,7 +9203,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{48CB07D6-9F6C-094F-A3D3-916741F281CD}" name="Tabella pivot1" cacheId="3" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valori" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{48CB07D6-9F6C-094F-A3D3-916741F281CD}" name="Tabella pivot1" cacheId="6" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valori" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A1:B25" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="14">
     <pivotField showAll="0"/>
@@ -9335,38 +9344,38 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{DEFAB213-4389-184E-911C-CDCC8CABBD38}" name="Tabella1" displayName="Tabella1" ref="A1:R322" totalsRowShown="0" dataDxfId="30">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{DEFAB213-4389-184E-911C-CDCC8CABBD38}" name="Tabella1" displayName="Tabella1" ref="A1:R322" totalsRowShown="0" dataDxfId="31">
   <autoFilter ref="A1:R322" xr:uid="{DEFAB213-4389-184E-911C-CDCC8CABBD38}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A255:R269">
     <sortCondition ref="B1:B313"/>
   </sortState>
   <tableColumns count="18">
-    <tableColumn id="16" xr3:uid="{DE426BDB-E154-EE46-B7B3-5B538C8AEC32}" name="TID" dataDxfId="29">
+    <tableColumn id="16" xr3:uid="{DE426BDB-E154-EE46-B7B3-5B538C8AEC32}" name="TID" dataDxfId="30">
       <calculatedColumnFormula>CONCATENATE("T",ROW(A2)-1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="1" xr3:uid="{A0AE63DC-99F7-7D4F-B824-AB7765893284}" name="Asset" dataDxfId="28"/>
-    <tableColumn id="2" xr3:uid="{0FA38BFF-C67B-0C43-B1BA-F6338DBFB0C8}" name="Threat" dataDxfId="27"/>
-    <tableColumn id="3" xr3:uid="{BFC77F7C-F096-8345-97EA-317816ED869D}" name="Description" dataDxfId="26"/>
-    <tableColumn id="4" xr3:uid="{258F3B86-1461-D64A-AE3B-CEAC97B2B533}" name="STRIDE" dataDxfId="25"/>
-    <tableColumn id="6" xr3:uid="{0FD06C95-5962-AC4D-B9EF-4DBB5728E736}" name="Compromised" dataDxfId="24"/>
-    <tableColumn id="7" xr3:uid="{9E5B99AD-1F1D-B44C-ABDF-6F7E9177F3DE}" name="PreC" dataDxfId="23"/>
-    <tableColumn id="8" xr3:uid="{D4F97A81-E528-2841-B4DE-321362F90F65}" name="PreI" dataDxfId="22"/>
-    <tableColumn id="9" xr3:uid="{018427D6-D385-3447-B4A4-95003B3341F6}" name="PreA" dataDxfId="21"/>
-    <tableColumn id="10" xr3:uid="{8334AC57-4A09-5744-9484-073ECEE2E513}" name="Precondition" dataDxfId="20"/>
-    <tableColumn id="12" xr3:uid="{DDBE315D-E051-2C47-A765-EE1DB2E118EA}" name="PostC" dataDxfId="19">
+    <tableColumn id="1" xr3:uid="{A0AE63DC-99F7-7D4F-B824-AB7765893284}" name="Asset" dataDxfId="29"/>
+    <tableColumn id="2" xr3:uid="{0FA38BFF-C67B-0C43-B1BA-F6338DBFB0C8}" name="Threat" dataDxfId="28"/>
+    <tableColumn id="3" xr3:uid="{BFC77F7C-F096-8345-97EA-317816ED869D}" name="Description" dataDxfId="27"/>
+    <tableColumn id="4" xr3:uid="{258F3B86-1461-D64A-AE3B-CEAC97B2B533}" name="STRIDE" dataDxfId="26"/>
+    <tableColumn id="6" xr3:uid="{0FD06C95-5962-AC4D-B9EF-4DBB5728E736}" name="Compromised" dataDxfId="25"/>
+    <tableColumn id="7" xr3:uid="{9E5B99AD-1F1D-B44C-ABDF-6F7E9177F3DE}" name="PreC" dataDxfId="24"/>
+    <tableColumn id="8" xr3:uid="{D4F97A81-E528-2841-B4DE-321362F90F65}" name="PreI" dataDxfId="23"/>
+    <tableColumn id="9" xr3:uid="{018427D6-D385-3447-B4A4-95003B3341F6}" name="PreA" dataDxfId="22"/>
+    <tableColumn id="10" xr3:uid="{8334AC57-4A09-5744-9484-073ECEE2E513}" name="Precondition" dataDxfId="21"/>
+    <tableColumn id="12" xr3:uid="{DDBE315D-E051-2C47-A765-EE1DB2E118EA}" name="PostC" dataDxfId="20">
       <calculatedColumnFormula>MID(N2,2,1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" xr3:uid="{243C1B9B-76C9-0345-B727-4F11FD75DF6B}" name="PostI" dataDxfId="18">
+    <tableColumn id="13" xr3:uid="{243C1B9B-76C9-0345-B727-4F11FD75DF6B}" name="PostI" dataDxfId="19">
       <calculatedColumnFormula>MID(N2,4,1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="14" xr3:uid="{DD688DAA-2C9A-C247-AEC4-CBDADE9B2B2E}" name="PostA" dataDxfId="17">
+    <tableColumn id="14" xr3:uid="{DD688DAA-2C9A-C247-AEC4-CBDADE9B2B2E}" name="PostA" dataDxfId="18">
       <calculatedColumnFormula>MID(N2,6,1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="15" xr3:uid="{CEE151EC-4E5B-0C41-8586-5A2D7E483661}" name="PostCondition" dataDxfId="16"/>
-    <tableColumn id="5" xr3:uid="{62EC5D77-1F78-1645-8697-BC5450583418}" name="CapecMeta" dataDxfId="15"/>
-    <tableColumn id="11" xr3:uid="{0DCD762C-4EE7-8141-BC05-9DB756A5BEF2}" name="CapecStandard" dataDxfId="14"/>
-    <tableColumn id="17" xr3:uid="{9EF317BA-855B-6E4A-9EC7-E1FB88A1FD56}" name="CapecDetailed" dataDxfId="13"/>
-    <tableColumn id="18" xr3:uid="{9BF6197D-4CF5-4941-A460-18823EEFB2E7}" name="Commento" dataDxfId="12"/>
+    <tableColumn id="15" xr3:uid="{CEE151EC-4E5B-0C41-8586-5A2D7E483661}" name="PostCondition" dataDxfId="17"/>
+    <tableColumn id="5" xr3:uid="{62EC5D77-1F78-1645-8697-BC5450583418}" name="CapecMeta" dataDxfId="16"/>
+    <tableColumn id="11" xr3:uid="{0DCD762C-4EE7-8141-BC05-9DB756A5BEF2}" name="CapecStandard" dataDxfId="15"/>
+    <tableColumn id="17" xr3:uid="{9EF317BA-855B-6E4A-9EC7-E1FB88A1FD56}" name="CapecDetailed" dataDxfId="14"/>
+    <tableColumn id="18" xr3:uid="{9BF6197D-4CF5-4941-A460-18823EEFB2E7}" name="Commento" dataDxfId="13"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -9386,20 +9395,21 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{5ECAFCE9-964F-A04C-B050-422AACCFD3F5}" name="Tabella4" displayName="Tabella4" ref="A1:I9" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
-  <autoFilter ref="A1:I9" xr:uid="{5ECAFCE9-964F-A04C-B050-422AACCFD3F5}"/>
-  <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{6405AD35-9222-B34C-A112-EC4FDEAC5BE2}" name="ToolID" dataDxfId="9">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{5ECAFCE9-964F-A04C-B050-422AACCFD3F5}" name="Tabella4" displayName="Tabella4" ref="A1:J9" totalsRowShown="0" headerRowDxfId="12" dataDxfId="11">
+  <autoFilter ref="A1:J9" xr:uid="{5ECAFCE9-964F-A04C-B050-422AACCFD3F5}"/>
+  <tableColumns count="10">
+    <tableColumn id="1" xr3:uid="{6405AD35-9222-B34C-A112-EC4FDEAC5BE2}" name="ToolID" dataDxfId="10">
       <calculatedColumnFormula>ROW(Tabella4[[#This Row],[Name]])-1</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{94F8DBBB-A826-8B4A-8C87-395122CA233A}" name="Name" dataDxfId="8"/>
-    <tableColumn id="2" xr3:uid="{FB636F07-AAD2-AE48-87BB-965F92F829C2}" name="CapecID" dataDxfId="7"/>
-    <tableColumn id="6" xr3:uid="{1E4A4CA6-7FF1-6543-A718-93EC7B5F1624}" name="CypherQuery" dataDxfId="6"/>
-    <tableColumn id="3" xr3:uid="{52487567-ED26-B840-ABFD-DB1BF72A83C9}" name="Command" dataDxfId="5"/>
-    <tableColumn id="5" xr3:uid="{0296B95F-6562-0746-B0C6-FE3564F6272C}" name="Description" dataDxfId="4"/>
-    <tableColumn id="7" xr3:uid="{FF0722DB-3140-904D-9B8E-A0C7B3C1FFEF}" name="PhaseID" dataDxfId="3"/>
-    <tableColumn id="8" xr3:uid="{2C7E754F-9F49-044B-9F1A-B62738B70258}" name="IsExecutable" dataDxfId="2"/>
-    <tableColumn id="9" xr3:uid="{6A4595CA-3FDC-EC4F-B8F1-4344144E8149}" name="OutputParser" dataDxfId="1"/>
+    <tableColumn id="4" xr3:uid="{94F8DBBB-A826-8B4A-8C87-395122CA233A}" name="Name" dataDxfId="9"/>
+    <tableColumn id="2" xr3:uid="{FB636F07-AAD2-AE48-87BB-965F92F829C2}" name="CapecID" dataDxfId="8"/>
+    <tableColumn id="6" xr3:uid="{1E4A4CA6-7FF1-6543-A718-93EC7B5F1624}" name="CypherQuery" dataDxfId="7"/>
+    <tableColumn id="3" xr3:uid="{52487567-ED26-B840-ABFD-DB1BF72A83C9}" name="Command" dataDxfId="6"/>
+    <tableColumn id="5" xr3:uid="{0296B95F-6562-0746-B0C6-FE3564F6272C}" name="Description" dataDxfId="5"/>
+    <tableColumn id="7" xr3:uid="{FF0722DB-3140-904D-9B8E-A0C7B3C1FFEF}" name="PhaseID" dataDxfId="4"/>
+    <tableColumn id="8" xr3:uid="{2C7E754F-9F49-044B-9F1A-B62738B70258}" name="IsExecutable" dataDxfId="3"/>
+    <tableColumn id="9" xr3:uid="{6A4595CA-3FDC-EC4F-B8F1-4344144E8149}" name="OutputParser" dataDxfId="2"/>
+    <tableColumn id="10" xr3:uid="{1CDFEE20-E2A1-E348-BB9C-16F2A7D9AEC0}" name="AllowedOutputExtensions" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -27022,19 +27032,19 @@
   <sheetData>
     <row r="1" spans="1:5" ht="16">
       <c r="A1" s="29" t="s">
-        <v>1003</v>
+        <v>1002</v>
       </c>
       <c r="B1" s="29" t="s">
-        <v>1022</v>
+        <v>1021</v>
       </c>
       <c r="C1" s="29" t="s">
-        <v>1121</v>
+        <v>1120</v>
       </c>
       <c r="D1" s="33" t="s">
         <v>3</v>
       </c>
       <c r="E1" s="29" t="s">
-        <v>1122</v>
+        <v>1121</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="29">
@@ -27042,13 +27052,13 @@
         <v>1</v>
       </c>
       <c r="B2" s="30" t="s">
+        <v>1122</v>
+      </c>
+      <c r="C2" s="30" t="s">
         <v>1123</v>
       </c>
-      <c r="C2" s="30" t="s">
+      <c r="D2" s="34" t="s">
         <v>1124</v>
-      </c>
-      <c r="D2" s="34" t="s">
-        <v>1125</v>
       </c>
       <c r="E2" s="30">
         <v>1</v>
@@ -27059,13 +27069,13 @@
         <v>2</v>
       </c>
       <c r="B3" s="30" t="s">
-        <v>1123</v>
+        <v>1122</v>
       </c>
       <c r="C3" s="30" t="s">
+        <v>1125</v>
+      </c>
+      <c r="D3" s="34" t="s">
         <v>1126</v>
-      </c>
-      <c r="D3" s="34" t="s">
-        <v>1127</v>
       </c>
       <c r="E3" s="30">
         <v>2</v>
@@ -27076,13 +27086,13 @@
         <v>3</v>
       </c>
       <c r="B4" s="30" t="s">
+        <v>1127</v>
+      </c>
+      <c r="C4" s="30" t="s">
         <v>1128</v>
       </c>
-      <c r="C4" s="30" t="s">
+      <c r="D4" s="34" t="s">
         <v>1129</v>
-      </c>
-      <c r="D4" s="34" t="s">
-        <v>1130</v>
       </c>
       <c r="E4" s="30">
         <v>1</v>
@@ -27093,13 +27103,13 @@
         <v>4</v>
       </c>
       <c r="B5" s="30" t="s">
-        <v>1128</v>
+        <v>1127</v>
       </c>
       <c r="C5" s="30" t="s">
+        <v>1130</v>
+      </c>
+      <c r="D5" s="34" t="s">
         <v>1131</v>
-      </c>
-      <c r="D5" s="34" t="s">
-        <v>1132</v>
       </c>
       <c r="E5" s="30">
         <v>2</v>
@@ -27110,13 +27120,13 @@
         <v>5</v>
       </c>
       <c r="B6" s="30" t="s">
+        <v>1132</v>
+      </c>
+      <c r="C6" s="30" t="s">
         <v>1133</v>
       </c>
-      <c r="C6" s="30" t="s">
+      <c r="D6" s="34" t="s">
         <v>1134</v>
-      </c>
-      <c r="D6" s="34" t="s">
-        <v>1135</v>
       </c>
       <c r="E6" s="30">
         <v>1</v>
@@ -27127,13 +27137,13 @@
         <v>6</v>
       </c>
       <c r="B7" s="30" t="s">
-        <v>1133</v>
+        <v>1132</v>
       </c>
       <c r="C7" s="30" t="s">
+        <v>1135</v>
+      </c>
+      <c r="D7" s="34" t="s">
         <v>1136</v>
-      </c>
-      <c r="D7" s="34" t="s">
-        <v>1137</v>
       </c>
       <c r="E7" s="30">
         <v>2</v>
@@ -27144,13 +27154,13 @@
         <v>7</v>
       </c>
       <c r="B8" s="30" t="s">
-        <v>1133</v>
+        <v>1132</v>
       </c>
       <c r="C8" s="30" t="s">
+        <v>1137</v>
+      </c>
+      <c r="D8" s="34" t="s">
         <v>1138</v>
-      </c>
-      <c r="D8" s="34" t="s">
-        <v>1139</v>
       </c>
       <c r="E8" s="30">
         <v>3</v>
@@ -27161,13 +27171,13 @@
         <v>8</v>
       </c>
       <c r="B9" s="30" t="s">
-        <v>1133</v>
+        <v>1132</v>
       </c>
       <c r="C9" s="30" t="s">
-        <v>1005</v>
+        <v>1004</v>
       </c>
       <c r="D9" s="34" t="s">
-        <v>1140</v>
+        <v>1139</v>
       </c>
       <c r="E9" s="30">
         <v>4</v>
@@ -27178,13 +27188,13 @@
         <v>9</v>
       </c>
       <c r="B10" s="30" t="s">
+        <v>1140</v>
+      </c>
+      <c r="C10" s="30" t="s">
         <v>1141</v>
       </c>
-      <c r="C10" s="30" t="s">
+      <c r="D10" s="34" t="s">
         <v>1142</v>
-      </c>
-      <c r="D10" s="34" t="s">
-        <v>1143</v>
       </c>
       <c r="E10" s="30">
         <v>1</v>
@@ -27195,13 +27205,13 @@
         <v>10</v>
       </c>
       <c r="B11" s="30" t="s">
-        <v>1141</v>
+        <v>1140</v>
       </c>
       <c r="C11" s="30" t="s">
+        <v>1143</v>
+      </c>
+      <c r="D11" s="34" t="s">
         <v>1144</v>
-      </c>
-      <c r="D11" s="34" t="s">
-        <v>1145</v>
       </c>
       <c r="E11" s="30">
         <v>2</v>
@@ -27212,13 +27222,13 @@
         <v>11</v>
       </c>
       <c r="B12" s="30" t="s">
-        <v>1141</v>
+        <v>1140</v>
       </c>
       <c r="C12" s="30" t="s">
+        <v>1145</v>
+      </c>
+      <c r="D12" s="34" t="s">
         <v>1146</v>
-      </c>
-      <c r="D12" s="34" t="s">
-        <v>1147</v>
       </c>
       <c r="E12" s="30">
         <v>3</v>
@@ -27229,13 +27239,13 @@
         <v>12</v>
       </c>
       <c r="B13" s="30" t="s">
-        <v>1141</v>
+        <v>1140</v>
       </c>
       <c r="C13" s="30" t="s">
+        <v>1147</v>
+      </c>
+      <c r="D13" s="34" t="s">
         <v>1148</v>
-      </c>
-      <c r="D13" s="34" t="s">
-        <v>1149</v>
       </c>
       <c r="E13" s="30">
         <v>4</v>
@@ -27246,13 +27256,13 @@
         <v>13</v>
       </c>
       <c r="B14" s="30" t="s">
-        <v>1141</v>
+        <v>1140</v>
       </c>
       <c r="C14" s="30" t="s">
+        <v>1149</v>
+      </c>
+      <c r="D14" s="34" t="s">
         <v>1150</v>
-      </c>
-      <c r="D14" s="34" t="s">
-        <v>1151</v>
       </c>
       <c r="E14" s="30">
         <v>5</v>
@@ -27263,13 +27273,13 @@
         <v>14</v>
       </c>
       <c r="B15" s="30" t="s">
-        <v>1141</v>
+        <v>1140</v>
       </c>
       <c r="C15" s="30" t="s">
+        <v>1151</v>
+      </c>
+      <c r="D15" s="34" t="s">
         <v>1152</v>
-      </c>
-      <c r="D15" s="34" t="s">
-        <v>1153</v>
       </c>
       <c r="E15" s="30">
         <v>6</v>
@@ -27280,13 +27290,13 @@
         <v>15</v>
       </c>
       <c r="B16" s="30" t="s">
+        <v>1153</v>
+      </c>
+      <c r="C16" s="30" t="s">
         <v>1154</v>
       </c>
-      <c r="C16" s="30" t="s">
+      <c r="D16" s="34" t="s">
         <v>1155</v>
-      </c>
-      <c r="D16" s="34" t="s">
-        <v>1156</v>
       </c>
       <c r="E16" s="30">
         <v>1</v>
@@ -27297,13 +27307,13 @@
         <v>16</v>
       </c>
       <c r="B17" s="30" t="s">
-        <v>1154</v>
+        <v>1153</v>
       </c>
       <c r="C17" s="30" t="s">
+        <v>1156</v>
+      </c>
+      <c r="D17" s="34" t="s">
         <v>1157</v>
-      </c>
-      <c r="D17" s="34" t="s">
-        <v>1158</v>
       </c>
       <c r="E17" s="30">
         <v>2</v>
@@ -27314,13 +27324,13 @@
         <v>17</v>
       </c>
       <c r="B18" s="30" t="s">
-        <v>1154</v>
+        <v>1153</v>
       </c>
       <c r="C18" s="30" t="s">
+        <v>1158</v>
+      </c>
+      <c r="D18" s="34" t="s">
         <v>1159</v>
-      </c>
-      <c r="D18" s="34" t="s">
-        <v>1160</v>
       </c>
       <c r="E18" s="30">
         <v>3</v>
@@ -27331,13 +27341,13 @@
         <v>18</v>
       </c>
       <c r="B19" s="30" t="s">
-        <v>1154</v>
+        <v>1153</v>
       </c>
       <c r="C19" s="30" t="s">
+        <v>1160</v>
+      </c>
+      <c r="D19" s="34" t="s">
         <v>1161</v>
-      </c>
-      <c r="D19" s="34" t="s">
-        <v>1162</v>
       </c>
       <c r="E19" s="30">
         <v>4</v>
@@ -27348,13 +27358,13 @@
         <v>19</v>
       </c>
       <c r="B20" s="30" t="s">
+        <v>1162</v>
+      </c>
+      <c r="C20" s="30" t="s">
         <v>1163</v>
       </c>
-      <c r="C20" s="30" t="s">
+      <c r="D20" s="34" t="s">
         <v>1164</v>
-      </c>
-      <c r="D20" s="34" t="s">
-        <v>1165</v>
       </c>
       <c r="E20" s="30">
         <v>1</v>
@@ -27365,13 +27375,13 @@
         <v>20</v>
       </c>
       <c r="B21" s="30" t="s">
-        <v>1163</v>
+        <v>1162</v>
       </c>
       <c r="C21" s="30" t="s">
+        <v>1165</v>
+      </c>
+      <c r="D21" s="34" t="s">
         <v>1166</v>
-      </c>
-      <c r="D21" s="34" t="s">
-        <v>1167</v>
       </c>
       <c r="E21" s="30">
         <v>2</v>
@@ -27382,13 +27392,13 @@
         <v>21</v>
       </c>
       <c r="B22" s="30" t="s">
-        <v>1163</v>
+        <v>1162</v>
       </c>
       <c r="C22" s="30" t="s">
+        <v>1167</v>
+      </c>
+      <c r="D22" s="34" t="s">
         <v>1168</v>
-      </c>
-      <c r="D22" s="34" t="s">
-        <v>1169</v>
       </c>
       <c r="E22" s="30">
         <v>3</v>
@@ -27399,13 +27409,13 @@
         <v>22</v>
       </c>
       <c r="B23" s="30" t="s">
-        <v>1163</v>
+        <v>1162</v>
       </c>
       <c r="C23" s="30" t="s">
+        <v>1169</v>
+      </c>
+      <c r="D23" s="34" t="s">
         <v>1170</v>
-      </c>
-      <c r="D23" s="34" t="s">
-        <v>1171</v>
       </c>
       <c r="E23" s="30">
         <v>4</v>
@@ -27416,13 +27426,13 @@
         <v>23</v>
       </c>
       <c r="B24" s="30" t="s">
+        <v>1171</v>
+      </c>
+      <c r="C24" s="30" t="s">
+        <v>1009</v>
+      </c>
+      <c r="D24" s="34" t="s">
         <v>1172</v>
-      </c>
-      <c r="C24" s="30" t="s">
-        <v>1010</v>
-      </c>
-      <c r="D24" s="34" t="s">
-        <v>1173</v>
       </c>
       <c r="E24" s="30">
         <v>1</v>
@@ -27433,13 +27443,13 @@
         <v>24</v>
       </c>
       <c r="B25" s="30" t="s">
-        <v>1172</v>
+        <v>1171</v>
       </c>
       <c r="C25" s="30" t="s">
-        <v>1011</v>
+        <v>1010</v>
       </c>
       <c r="D25" s="34" t="s">
-        <v>1174</v>
+        <v>1173</v>
       </c>
       <c r="E25" s="30">
         <v>2</v>
@@ -27450,13 +27460,13 @@
         <v>25</v>
       </c>
       <c r="B26" s="30" t="s">
-        <v>1172</v>
+        <v>1171</v>
       </c>
       <c r="C26" s="30" t="s">
-        <v>1013</v>
+        <v>1012</v>
       </c>
       <c r="D26" s="34" t="s">
-        <v>1175</v>
+        <v>1174</v>
       </c>
       <c r="E26" s="30">
         <v>3</v>
@@ -27467,13 +27477,13 @@
         <v>26</v>
       </c>
       <c r="B27" s="30" t="s">
-        <v>1172</v>
+        <v>1171</v>
       </c>
       <c r="C27" s="30" t="s">
         <v>140</v>
       </c>
       <c r="D27" s="34" t="s">
-        <v>1176</v>
+        <v>1175</v>
       </c>
       <c r="E27" s="30">
         <v>4</v>
@@ -27484,13 +27494,13 @@
         <v>27</v>
       </c>
       <c r="B28" s="30" t="s">
-        <v>1172</v>
+        <v>1171</v>
       </c>
       <c r="C28" s="30" t="s">
-        <v>1014</v>
+        <v>1013</v>
       </c>
       <c r="D28" s="34" t="s">
-        <v>1177</v>
+        <v>1176</v>
       </c>
       <c r="E28" s="30">
         <v>5</v>
@@ -27501,13 +27511,13 @@
         <v>28</v>
       </c>
       <c r="B29" s="30" t="s">
-        <v>1172</v>
+        <v>1171</v>
       </c>
       <c r="C29" s="30" t="s">
-        <v>1012</v>
+        <v>1011</v>
       </c>
       <c r="D29" s="34" t="s">
-        <v>1178</v>
+        <v>1177</v>
       </c>
       <c r="E29" s="30">
         <v>6</v>
@@ -27518,13 +27528,13 @@
         <v>29</v>
       </c>
       <c r="B30" s="30" t="s">
+        <v>1178</v>
+      </c>
+      <c r="C30" s="30" t="s">
         <v>1179</v>
       </c>
-      <c r="C30" s="30" t="s">
+      <c r="D30" s="34" t="s">
         <v>1180</v>
-      </c>
-      <c r="D30" s="34" t="s">
-        <v>1181</v>
       </c>
       <c r="E30" s="30">
         <v>1</v>
@@ -27535,13 +27545,13 @@
         <v>30</v>
       </c>
       <c r="B31" s="30" t="s">
-        <v>1179</v>
+        <v>1178</v>
       </c>
       <c r="C31" s="30" t="s">
-        <v>1019</v>
+        <v>1018</v>
       </c>
       <c r="D31" s="34" t="s">
-        <v>1182</v>
+        <v>1181</v>
       </c>
       <c r="E31" s="30">
         <v>2</v>
@@ -27552,13 +27562,13 @@
         <v>31</v>
       </c>
       <c r="B32" s="30" t="s">
-        <v>1179</v>
+        <v>1178</v>
       </c>
       <c r="C32" s="30" t="s">
+        <v>1182</v>
+      </c>
+      <c r="D32" s="34" t="s">
         <v>1183</v>
-      </c>
-      <c r="D32" s="34" t="s">
-        <v>1184</v>
       </c>
       <c r="E32" s="30">
         <v>3</v>
@@ -27569,13 +27579,13 @@
         <v>32</v>
       </c>
       <c r="B33" s="30" t="s">
-        <v>1179</v>
+        <v>1178</v>
       </c>
       <c r="C33" s="30" t="s">
-        <v>1017</v>
+        <v>1016</v>
       </c>
       <c r="D33" s="34" t="s">
-        <v>1185</v>
+        <v>1184</v>
       </c>
       <c r="E33" s="30">
         <v>4</v>
@@ -27586,13 +27596,13 @@
         <v>33</v>
       </c>
       <c r="B34" s="30" t="s">
-        <v>1179</v>
+        <v>1178</v>
       </c>
       <c r="C34" s="30" t="s">
-        <v>1018</v>
+        <v>1017</v>
       </c>
       <c r="D34" s="34" t="s">
-        <v>1186</v>
+        <v>1185</v>
       </c>
       <c r="E34" s="30">
         <v>5</v>
@@ -28834,7 +28844,7 @@
       </c>
     </row>
     <row r="30" spans="1:13" ht="48">
-      <c r="A30" s="56" t="s">
+      <c r="A30" s="54" t="s">
         <v>811</v>
       </c>
       <c r="B30" s="5" t="s">
@@ -28877,7 +28887,7 @@
       </c>
     </row>
     <row r="31" spans="1:13" ht="48">
-      <c r="A31" s="56"/>
+      <c r="A31" s="54"/>
       <c r="B31" s="5" t="s">
         <v>814</v>
       </c>
@@ -28918,7 +28928,7 @@
       </c>
     </row>
     <row r="32" spans="1:13" ht="32">
-      <c r="A32" s="56"/>
+      <c r="A32" s="54"/>
       <c r="B32" s="5" t="s">
         <v>816</v>
       </c>
@@ -28959,7 +28969,7 @@
       </c>
     </row>
     <row r="33" spans="1:13" ht="96">
-      <c r="A33" s="56"/>
+      <c r="A33" s="54"/>
       <c r="B33" s="5" t="s">
         <v>100</v>
       </c>
@@ -29000,7 +29010,7 @@
       </c>
     </row>
     <row r="34" spans="1:13" ht="32">
-      <c r="A34" s="56"/>
+      <c r="A34" s="54"/>
       <c r="B34" s="5" t="s">
         <v>819</v>
       </c>
@@ -29041,7 +29051,7 @@
       </c>
     </row>
     <row r="35" spans="1:13" ht="32">
-      <c r="A35" s="56"/>
+      <c r="A35" s="54"/>
       <c r="B35" s="5" t="s">
         <v>201</v>
       </c>
@@ -29082,7 +29092,7 @@
       </c>
     </row>
     <row r="36" spans="1:13" ht="80">
-      <c r="A36" s="56"/>
+      <c r="A36" s="54"/>
       <c r="B36" s="5" t="s">
         <v>822</v>
       </c>
@@ -29621,7 +29631,7 @@
       </c>
     </row>
     <row r="49" spans="1:13" ht="78" customHeight="1">
-      <c r="A49" s="56" t="s">
+      <c r="A49" s="54" t="s">
         <v>840</v>
       </c>
       <c r="B49" s="5" t="s">
@@ -29664,7 +29674,7 @@
       </c>
     </row>
     <row r="50" spans="1:13" ht="32">
-      <c r="A50" s="56"/>
+      <c r="A50" s="54"/>
       <c r="B50" s="5" t="s">
         <v>613</v>
       </c>
@@ -29705,7 +29715,7 @@
       </c>
     </row>
     <row r="51" spans="1:13" ht="16">
-      <c r="A51" s="56"/>
+      <c r="A51" s="54"/>
       <c r="B51" s="5" t="s">
         <v>201</v>
       </c>
@@ -29746,7 +29756,7 @@
       </c>
     </row>
     <row r="52" spans="1:13" ht="32">
-      <c r="A52" s="56"/>
+      <c r="A52" s="54"/>
       <c r="B52" s="5" t="s">
         <v>845</v>
       </c>
@@ -29787,7 +29797,7 @@
       </c>
     </row>
     <row r="53" spans="1:13" ht="96">
-      <c r="A53" s="56"/>
+      <c r="A53" s="54"/>
       <c r="B53" s="5" t="s">
         <v>847</v>
       </c>
@@ -29828,7 +29838,7 @@
       </c>
     </row>
     <row r="54" spans="1:13">
-      <c r="A54" s="56"/>
+      <c r="A54" s="54"/>
       <c r="B54" s="5" t="s">
         <v>849</v>
       </c>
@@ -29869,7 +29879,7 @@
       </c>
     </row>
     <row r="55" spans="1:13" ht="64">
-      <c r="A55" s="56"/>
+      <c r="A55" s="54"/>
       <c r="B55" s="5" t="s">
         <v>851</v>
       </c>
@@ -29910,7 +29920,7 @@
       </c>
     </row>
     <row r="56" spans="1:13" ht="64">
-      <c r="A56" s="56"/>
+      <c r="A56" s="54"/>
       <c r="B56" s="5" t="s">
         <v>853</v>
       </c>
@@ -29951,7 +29961,7 @@
       </c>
     </row>
     <row r="57" spans="1:13" ht="32">
-      <c r="A57" s="54" t="s">
+      <c r="A57" s="55" t="s">
         <v>855</v>
       </c>
       <c r="B57" s="6" t="s">
@@ -29993,7 +30003,7 @@
       </c>
     </row>
     <row r="58" spans="1:13" ht="80">
-      <c r="A58" s="54"/>
+      <c r="A58" s="55"/>
       <c r="B58" s="7" t="s">
         <v>858</v>
       </c>
@@ -30033,7 +30043,7 @@
       </c>
     </row>
     <row r="59" spans="1:13" ht="64" customHeight="1">
-      <c r="A59" s="54"/>
+      <c r="A59" s="55"/>
       <c r="B59" s="7" t="s">
         <v>860</v>
       </c>
@@ -30073,7 +30083,7 @@
       </c>
     </row>
     <row r="60" spans="1:13" ht="16">
-      <c r="A60" s="54"/>
+      <c r="A60" s="55"/>
       <c r="B60" s="7" t="s">
         <v>95</v>
       </c>
@@ -30113,7 +30123,7 @@
       </c>
     </row>
     <row r="61" spans="1:13" ht="32">
-      <c r="A61" s="54"/>
+      <c r="A61" s="55"/>
       <c r="B61" s="7" t="s">
         <v>864</v>
       </c>
@@ -30153,7 +30163,7 @@
       </c>
     </row>
     <row r="62" spans="1:13" ht="32">
-      <c r="A62" s="54"/>
+      <c r="A62" s="55"/>
       <c r="B62" s="7" t="s">
         <v>866</v>
       </c>
@@ -30193,7 +30203,7 @@
       </c>
     </row>
     <row r="63" spans="1:13" ht="16">
-      <c r="A63" s="54"/>
+      <c r="A63" s="55"/>
       <c r="B63" s="7" t="s">
         <v>869</v>
       </c>
@@ -30233,7 +30243,7 @@
       </c>
     </row>
     <row r="64" spans="1:13" ht="32">
-      <c r="A64" s="54"/>
+      <c r="A64" s="55"/>
       <c r="B64" s="6" t="s">
         <v>871</v>
       </c>
@@ -30273,7 +30283,7 @@
       </c>
     </row>
     <row r="65" spans="1:13" ht="16">
-      <c r="A65" s="54"/>
+      <c r="A65" s="55"/>
       <c r="B65" s="7" t="s">
         <v>82</v>
       </c>
@@ -30313,7 +30323,7 @@
       </c>
     </row>
     <row r="66" spans="1:13" ht="16">
-      <c r="A66" s="54"/>
+      <c r="A66" s="55"/>
       <c r="B66" s="7" t="s">
         <v>874</v>
       </c>
@@ -30353,7 +30363,7 @@
       </c>
     </row>
     <row r="67" spans="1:13" ht="48">
-      <c r="A67" s="54"/>
+      <c r="A67" s="55"/>
       <c r="B67" s="6" t="s">
         <v>92</v>
       </c>
@@ -30393,38 +30403,38 @@
       </c>
     </row>
     <row r="68" spans="1:13" ht="16">
-      <c r="A68" s="54"/>
-      <c r="B68" s="54" t="s">
+      <c r="A68" s="55"/>
+      <c r="B68" s="55" t="s">
         <v>169</v>
       </c>
       <c r="C68" s="6" t="s">
         <v>876</v>
       </c>
-      <c r="D68" s="54" t="s">
+      <c r="D68" s="55" t="s">
         <v>27</v>
       </c>
-      <c r="E68" s="54" t="s">
+      <c r="E68" s="55" t="s">
         <v>862</v>
       </c>
-      <c r="F68" s="54" t="s">
-        <v>23</v>
-      </c>
-      <c r="G68" s="54" t="s">
+      <c r="F68" s="55" t="s">
+        <v>23</v>
+      </c>
+      <c r="G68" s="55" t="s">
         <v>23</v>
       </c>
       <c r="H68" s="53" t="s">
         <v>23</v>
       </c>
-      <c r="I68" s="54" t="s">
+      <c r="I68" s="55" t="s">
         <v>181</v>
       </c>
-      <c r="J68" s="54" t="s">
-        <v>23</v>
-      </c>
-      <c r="K68" s="54" t="s">
-        <v>23</v>
-      </c>
-      <c r="L68" s="54" t="s">
+      <c r="J68" s="55" t="s">
+        <v>23</v>
+      </c>
+      <c r="K68" s="55" t="s">
+        <v>23</v>
+      </c>
+      <c r="L68" s="55" t="s">
         <v>84</v>
       </c>
       <c r="M68" s="53" t="str">
@@ -30433,24 +30443,24 @@
       </c>
     </row>
     <row r="69" spans="1:13" ht="16">
-      <c r="A69" s="54"/>
-      <c r="B69" s="54"/>
+      <c r="A69" s="55"/>
+      <c r="B69" s="55"/>
       <c r="C69" s="6" t="s">
         <v>877</v>
       </c>
-      <c r="D69" s="54"/>
-      <c r="E69" s="54"/>
-      <c r="F69" s="54"/>
-      <c r="G69" s="54"/>
+      <c r="D69" s="55"/>
+      <c r="E69" s="55"/>
+      <c r="F69" s="55"/>
+      <c r="G69" s="55"/>
       <c r="H69" s="53"/>
-      <c r="I69" s="54"/>
-      <c r="J69" s="54"/>
-      <c r="K69" s="54"/>
-      <c r="L69" s="54"/>
+      <c r="I69" s="55"/>
+      <c r="J69" s="55"/>
+      <c r="K69" s="55"/>
+      <c r="L69" s="55"/>
       <c r="M69" s="53"/>
     </row>
     <row r="70" spans="1:13" ht="28">
-      <c r="A70" s="55" t="s">
+      <c r="A70" s="56" t="s">
         <v>878</v>
       </c>
       <c r="B70" s="16" t="s">
@@ -30496,7 +30506,7 @@
       </c>
     </row>
     <row r="71" spans="1:13" ht="51">
-      <c r="A71" s="55"/>
+      <c r="A71" s="56"/>
       <c r="B71" s="16" t="s">
         <v>100</v>
       </c>
@@ -30540,7 +30550,7 @@
       </c>
     </row>
     <row r="72" spans="1:13" ht="28">
-      <c r="A72" s="55"/>
+      <c r="A72" s="56"/>
       <c r="B72" s="16" t="s">
         <v>763</v>
       </c>
@@ -30584,7 +30594,7 @@
       </c>
     </row>
     <row r="73" spans="1:13" ht="28">
-      <c r="A73" s="55"/>
+      <c r="A73" s="56"/>
       <c r="B73" s="16" t="s">
         <v>885</v>
       </c>
@@ -31146,15 +31156,6 @@
     </row>
   </sheetData>
   <mergeCells count="23">
-    <mergeCell ref="A2:A7"/>
-    <mergeCell ref="A8:A14"/>
-    <mergeCell ref="A25:A29"/>
-    <mergeCell ref="A15:A24"/>
-    <mergeCell ref="A49:A56"/>
-    <mergeCell ref="A44:A48"/>
-    <mergeCell ref="A41:A43"/>
-    <mergeCell ref="A30:A36"/>
-    <mergeCell ref="A37:A40"/>
     <mergeCell ref="M68:M69"/>
     <mergeCell ref="H68:H69"/>
     <mergeCell ref="A74:A85"/>
@@ -31169,6 +31170,15 @@
     <mergeCell ref="B68:B69"/>
     <mergeCell ref="D68:D69"/>
     <mergeCell ref="E68:E69"/>
+    <mergeCell ref="A2:A7"/>
+    <mergeCell ref="A8:A14"/>
+    <mergeCell ref="A25:A29"/>
+    <mergeCell ref="A15:A24"/>
+    <mergeCell ref="A49:A56"/>
+    <mergeCell ref="A44:A48"/>
+    <mergeCell ref="A41:A43"/>
+    <mergeCell ref="A30:A36"/>
+    <mergeCell ref="A37:A40"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -31394,7 +31404,7 @@
   <dimension ref="A1:B76"/>
   <sheetViews>
     <sheetView topLeftCell="A2" zoomScale="150" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15"/>
@@ -32020,10 +32030,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C51FC597-29FA-1D4E-A4C8-B79027768242}">
-  <dimension ref="A1:I9"/>
+  <dimension ref="A1:J9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D4" zoomScale="163" workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+    <sheetView tabSelected="1" topLeftCell="B2" zoomScale="163" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15"/>
@@ -32038,7 +32048,7 @@
     <col min="8" max="16384" width="10.83203125" style="26"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="16">
+    <row r="1" spans="1:10" ht="16">
       <c r="A1" s="26" t="s">
         <v>935</v>
       </c>
@@ -32061,13 +32071,16 @@
         <v>940</v>
       </c>
       <c r="H1" s="26" t="s">
-        <v>1197</v>
+        <v>1196</v>
       </c>
       <c r="I1" s="26" t="s">
-        <v>1200</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" ht="64">
+        <v>1199</v>
+      </c>
+      <c r="J1" s="26" t="s">
+        <v>1201</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" ht="64">
       <c r="A2" s="26">
         <f>ROW(Tabella4[[#This Row],[Name]])-1</f>
         <v>1</v>
@@ -32085,16 +32098,16 @@
         <v>944</v>
       </c>
       <c r="F2" s="27" t="s">
-        <v>1188</v>
+        <v>1187</v>
       </c>
       <c r="G2" s="28" t="s">
-        <v>1196</v>
+        <v>1195</v>
       </c>
       <c r="H2" s="26" t="s">
-        <v>1198</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" ht="64">
+        <v>1197</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" ht="64">
       <c r="A3" s="26">
         <f>ROW(Tabella4[[#This Row],[Name]])-1</f>
         <v>2</v>
@@ -32118,10 +32131,10 @@
         <v>8</v>
       </c>
       <c r="H3" s="26" t="s">
-        <v>1198</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" ht="80">
+        <v>1197</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" ht="80">
       <c r="A4" s="26">
         <f>ROW(Tabella4[[#This Row],[Name]])-1</f>
         <v>3</v>
@@ -32139,16 +32152,16 @@
         <v>951</v>
       </c>
       <c r="F4" s="27" t="s">
-        <v>1189</v>
+        <v>1188</v>
       </c>
       <c r="G4" s="28">
         <v>6</v>
       </c>
       <c r="H4" s="26" t="s">
-        <v>1198</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" ht="32">
+        <v>1197</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="32">
       <c r="A5" s="26">
         <f>ROW(Tabella4[[#This Row],[Name]])-1</f>
         <v>4</v>
@@ -32166,16 +32179,16 @@
         <v>955</v>
       </c>
       <c r="F5" s="27" t="s">
-        <v>1190</v>
+        <v>1189</v>
       </c>
       <c r="G5" s="28">
         <v>5</v>
       </c>
       <c r="H5" s="26" t="s">
-        <v>1199</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" ht="32">
+        <v>1198</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" ht="32">
       <c r="A6" s="26">
         <f>ROW(Tabella4[[#This Row],[Name]])-1</f>
         <v>5</v>
@@ -32190,22 +32203,25 @@
         <v>957</v>
       </c>
       <c r="E6" s="26" t="s">
-        <v>958</v>
+        <v>1203</v>
       </c>
       <c r="F6" s="27" t="s">
-        <v>1187</v>
+        <v>1186</v>
       </c>
       <c r="G6" s="28">
         <v>5</v>
       </c>
       <c r="H6" s="26" t="s">
-        <v>1199</v>
+        <v>1198</v>
       </c>
       <c r="I6" s="26" t="s">
-        <v>1201</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" ht="32">
+        <v>1200</v>
+      </c>
+      <c r="J6" s="26" t="s">
+        <v>1202</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" ht="32">
       <c r="A7" s="26">
         <f>ROW(Tabella4[[#This Row],[Name]])-1</f>
         <v>6</v>
@@ -32214,76 +32230,76 @@
         <v>952</v>
       </c>
       <c r="C7" s="28" t="s">
-        <v>959</v>
+        <v>958</v>
       </c>
       <c r="D7" s="27" t="s">
         <v>954</v>
       </c>
       <c r="E7" s="26" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
       <c r="F7" s="27" t="s">
-        <v>1191</v>
+        <v>1190</v>
       </c>
       <c r="G7" s="28">
         <v>5</v>
       </c>
       <c r="H7" s="26" t="s">
-        <v>1199</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" ht="80">
+        <v>1198</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" ht="80">
       <c r="A8" s="26">
         <f>ROW(Tabella4[[#This Row],[Name]])-1</f>
         <v>7</v>
       </c>
       <c r="B8" s="26" t="s">
+        <v>960</v>
+      </c>
+      <c r="C8" s="28" t="s">
         <v>961</v>
       </c>
-      <c r="C8" s="28" t="s">
+      <c r="D8" s="27" t="s">
         <v>962</v>
       </c>
-      <c r="D8" s="27" t="s">
+      <c r="E8" s="26" t="s">
         <v>963</v>
       </c>
-      <c r="E8" s="26" t="s">
+      <c r="F8" s="27" t="s">
         <v>964</v>
-      </c>
-      <c r="F8" s="27" t="s">
-        <v>965</v>
       </c>
       <c r="G8" s="28">
         <v>11</v>
       </c>
       <c r="H8" s="26" t="s">
-        <v>1198</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" ht="96">
+        <v>1197</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" ht="96">
       <c r="A9" s="26">
         <f>ROW(Tabella4[[#This Row],[Name]])-1</f>
         <v>8</v>
       </c>
       <c r="B9" s="26" t="s">
-        <v>966</v>
+        <v>965</v>
       </c>
       <c r="C9" s="28" t="s">
         <v>723</v>
       </c>
       <c r="D9" s="27" t="s">
+        <v>966</v>
+      </c>
+      <c r="E9" s="26" t="s">
         <v>967</v>
       </c>
-      <c r="E9" s="26" t="s">
+      <c r="F9" s="27" t="s">
         <v>968</v>
       </c>
-      <c r="F9" s="27" t="s">
-        <v>969</v>
-      </c>
       <c r="G9" s="28" t="s">
-        <v>1196</v>
+        <v>1195</v>
       </c>
       <c r="H9" s="26" t="s">
-        <v>1198</v>
+        <v>1197</v>
       </c>
     </row>
   </sheetData>
@@ -32317,10 +32333,10 @@
         <v>940</v>
       </c>
       <c r="B1" t="s">
+        <v>969</v>
+      </c>
+      <c r="C1" t="s">
         <v>970</v>
-      </c>
-      <c r="C1" t="s">
-        <v>971</v>
       </c>
     </row>
     <row r="2" spans="1:3">
@@ -32329,7 +32345,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="45" t="s">
-        <v>972</v>
+        <v>971</v>
       </c>
       <c r="C2" s="45"/>
     </row>
@@ -32339,7 +32355,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>973</v>
+        <v>972</v>
       </c>
       <c r="C3">
         <f>INDEX(Tabella5[[PhaseID]:[PhaseName]],MATCH("Reconnaissance",Tabella5[PhaseName],0),1)</f>
@@ -32352,7 +32368,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>974</v>
+        <v>973</v>
       </c>
       <c r="C4">
         <f>INDEX(Tabella5[[PhaseID]:[PhaseName]],MATCH("Reconnaissance",Tabella5[PhaseName],0),1)</f>
@@ -32375,7 +32391,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>975</v>
+        <v>974</v>
       </c>
       <c r="C6">
         <f>INDEX(Tabella5[[PhaseID]:[PhaseName]],MATCH("Scanning",Tabella5[PhaseName],0),1)</f>
@@ -32388,7 +32404,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>1195</v>
+        <v>1194</v>
       </c>
       <c r="C7">
         <f>INDEX(Tabella5[[PhaseID]:[PhaseName]],MATCH("Scanning",Tabella5[PhaseName],0),1)</f>
@@ -32401,7 +32417,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>976</v>
+        <v>975</v>
       </c>
       <c r="C8">
         <f>INDEX(Tabella5[[PhaseID]:[PhaseName]],MATCH("Scanning",Tabella5[PhaseName],0),1)</f>
@@ -32414,7 +32430,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="45" t="s">
-        <v>977</v>
+        <v>976</v>
       </c>
       <c r="C9" s="46"/>
     </row>
@@ -32424,7 +32440,7 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>1192</v>
+        <v>1191</v>
       </c>
       <c r="C10">
         <f>INDEX(Tabella5[[PhaseID]:[PhaseName]],MATCH("System Access",Tabella5[PhaseName],0),1)</f>
@@ -32437,7 +32453,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="47" t="s">
-        <v>1194</v>
+        <v>1193</v>
       </c>
       <c r="C11" s="47">
         <f>INDEX(Tabella5[[PhaseID]:[PhaseName]],MATCH("System Access",Tabella5[PhaseName],0),1)</f>
@@ -32450,7 +32466,7 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>978</v>
+        <v>977</v>
       </c>
       <c r="C12">
         <f>INDEX(Tabella5[[PhaseID]:[PhaseName]],MATCH("Escalating Privileges (Privilege Escalation)",Tabella5[PhaseName],0),1)</f>
@@ -32463,7 +32479,7 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>1193</v>
+        <v>1192</v>
       </c>
       <c r="C13">
         <f>INDEX(Tabella5[[PhaseID]:[PhaseName]],MATCH("System Access",Tabella5[PhaseName],0),1)</f>
@@ -32476,7 +32492,7 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>979</v>
+        <v>978</v>
       </c>
       <c r="C14">
         <f>INDEX(Tabella5[[PhaseID]:[PhaseName]],MATCH("System Access",Tabella5[PhaseName],0),1)</f>
@@ -32499,7 +32515,7 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>980</v>
+        <v>979</v>
       </c>
       <c r="C16">
         <f>INDEX(Tabella5[[PhaseID]:[PhaseName]],MATCH("Damage",Tabella5[PhaseName],0),1)</f>
@@ -32512,7 +32528,7 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>981</v>
+        <v>980</v>
       </c>
       <c r="C17">
         <f>INDEX(Tabella5[[PhaseID]:[PhaseName]],MATCH("Damage",Tabella5[PhaseName],0),1)</f>
@@ -32525,7 +32541,7 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>982</v>
+        <v>981</v>
       </c>
       <c r="C18">
         <f>INDEX(Tabella5[[PhaseID]:[PhaseName]],MATCH("Damage",Tabella5[PhaseName],0),1)</f>
@@ -32551,7 +32567,7 @@
         <v>19</v>
       </c>
       <c r="B20" s="47" t="s">
-        <v>983</v>
+        <v>982</v>
       </c>
       <c r="C20" s="47">
         <f>INDEX(Tabella5[[PhaseID]:[PhaseName]],MATCH("Damage",Tabella5[PhaseName],0),1)</f>
@@ -32564,7 +32580,7 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>984</v>
+        <v>983</v>
       </c>
       <c r="C21">
         <f>INDEX(Tabella5[[PhaseID]:[PhaseName]],MATCH("Backdoors",Tabella5[PhaseName],0),1)</f>
@@ -32577,7 +32593,7 @@
         <v>21</v>
       </c>
       <c r="B22" s="45" t="s">
-        <v>985</v>
+        <v>984</v>
       </c>
       <c r="C22" s="45"/>
     </row>
@@ -32587,7 +32603,7 @@
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>986</v>
+        <v>985</v>
       </c>
       <c r="C23">
         <f>INDEX(Tabella5[[PhaseID]:[PhaseName]],MATCH("Covering Tracks",Tabella5[PhaseName],0),1)</f>
@@ -32600,7 +32616,7 @@
         <v>23</v>
       </c>
       <c r="B24" s="45" t="s">
-        <v>987</v>
+        <v>986</v>
       </c>
       <c r="C24" s="45"/>
     </row>
@@ -32632,16 +32648,16 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="31" t="s">
+        <v>987</v>
+      </c>
+      <c r="B1" s="31" t="s">
         <v>988</v>
       </c>
-      <c r="B1" s="31" t="s">
+      <c r="C1" s="31" t="s">
         <v>989</v>
       </c>
-      <c r="C1" s="31" t="s">
+      <c r="D1" s="42" t="s">
         <v>990</v>
-      </c>
-      <c r="D1" s="42" t="s">
-        <v>991</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="30">
@@ -32649,10 +32665,10 @@
         <v>1</v>
       </c>
       <c r="B2" s="48" t="s">
+        <v>991</v>
+      </c>
+      <c r="C2" s="30" t="s">
         <v>992</v>
-      </c>
-      <c r="C2" s="30" t="s">
-        <v>993</v>
       </c>
       <c r="D2" s="30">
         <v>1.2</v>
@@ -32663,13 +32679,13 @@
         <v>2</v>
       </c>
       <c r="B3" s="30" t="s">
+        <v>993</v>
+      </c>
+      <c r="C3" s="30" t="s">
         <v>994</v>
       </c>
-      <c r="C3" s="30" t="s">
+      <c r="D3" s="43" t="s">
         <v>995</v>
-      </c>
-      <c r="D3" s="43" t="s">
-        <v>996</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -32677,13 +32693,13 @@
         <v>3</v>
       </c>
       <c r="B4" s="30" t="s">
+        <v>996</v>
+      </c>
+      <c r="C4" s="30" t="s">
         <v>997</v>
       </c>
-      <c r="C4" s="30" t="s">
+      <c r="D4" s="42" t="s">
         <v>998</v>
-      </c>
-      <c r="D4" s="42" t="s">
-        <v>999</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="30">
@@ -32691,13 +32707,13 @@
         <v>4</v>
       </c>
       <c r="B5" s="48" t="s">
+        <v>999</v>
+      </c>
+      <c r="C5" s="30" t="s">
         <v>1000</v>
       </c>
-      <c r="C5" s="30" t="s">
+      <c r="D5" s="42" t="s">
         <v>1001</v>
-      </c>
-      <c r="D5" s="42" t="s">
-        <v>1002</v>
       </c>
     </row>
   </sheetData>
@@ -32724,13 +32740,13 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="44" t="s">
+        <v>1002</v>
+      </c>
+      <c r="B1" s="44" t="s">
         <v>1003</v>
       </c>
-      <c r="B1" s="44" t="s">
+      <c r="C1" s="44" t="s">
         <v>1004</v>
-      </c>
-      <c r="C1" s="44" t="s">
-        <v>1005</v>
       </c>
     </row>
     <row r="2" spans="1:3">
@@ -32738,7 +32754,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>1006</v>
+        <v>1005</v>
       </c>
       <c r="C2">
         <v>0</v>
@@ -32749,7 +32765,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>1007</v>
+        <v>1006</v>
       </c>
       <c r="C3">
         <v>0</v>
@@ -32760,7 +32776,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>1008</v>
+        <v>1007</v>
       </c>
       <c r="C4">
         <v>0</v>
@@ -32771,7 +32787,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>1009</v>
+        <v>1008</v>
       </c>
       <c r="C5">
         <v>0</v>
@@ -32782,7 +32798,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>1010</v>
+        <v>1009</v>
       </c>
       <c r="C6">
         <v>1</v>
@@ -32793,7 +32809,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>1011</v>
+        <v>1010</v>
       </c>
       <c r="C7">
         <v>1</v>
@@ -32804,7 +32820,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>1012</v>
+        <v>1011</v>
       </c>
       <c r="C8">
         <v>1</v>
@@ -32815,7 +32831,7 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>1013</v>
+        <v>1012</v>
       </c>
       <c r="C9">
         <v>1</v>
@@ -32837,7 +32853,7 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>1014</v>
+        <v>1013</v>
       </c>
       <c r="C11">
         <v>1</v>
@@ -32848,7 +32864,7 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>1015</v>
+        <v>1014</v>
       </c>
       <c r="C12">
         <v>1</v>
@@ -32859,7 +32875,7 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>1016</v>
+        <v>1015</v>
       </c>
       <c r="C13">
         <v>1</v>
@@ -32870,7 +32886,7 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>1017</v>
+        <v>1016</v>
       </c>
       <c r="C14">
         <v>1</v>
@@ -32881,7 +32897,7 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>1018</v>
+        <v>1017</v>
       </c>
       <c r="C15">
         <v>1</v>
@@ -32892,7 +32908,7 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>1019</v>
+        <v>1018</v>
       </c>
       <c r="C16">
         <v>1</v>
@@ -32925,22 +32941,22 @@
   <sheetData>
     <row r="1" spans="1:6" ht="16">
       <c r="A1" s="29" t="s">
-        <v>1003</v>
+        <v>1002</v>
       </c>
       <c r="B1" s="29" t="s">
-        <v>1020</v>
+        <v>1019</v>
       </c>
       <c r="C1" s="29" t="s">
         <v>3</v>
       </c>
       <c r="D1" s="37" t="s">
+        <v>1020</v>
+      </c>
+      <c r="E1" s="40" t="s">
+        <v>1003</v>
+      </c>
+      <c r="F1" s="29" t="s">
         <v>1021</v>
-      </c>
-      <c r="E1" s="40" t="s">
-        <v>1004</v>
-      </c>
-      <c r="F1" s="29" t="s">
-        <v>1022</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="29">
@@ -32948,19 +32964,19 @@
         <v>1</v>
       </c>
       <c r="B2" s="30" t="s">
+        <v>1022</v>
+      </c>
+      <c r="C2" s="30" t="s">
         <v>1023</v>
       </c>
-      <c r="C2" s="30" t="s">
+      <c r="D2" s="38" t="s">
         <v>1024</v>
       </c>
-      <c r="D2" s="38" t="s">
+      <c r="E2" s="41" t="s">
         <v>1025</v>
       </c>
-      <c r="E2" s="41" t="s">
+      <c r="F2" s="36" t="s">
         <v>1026</v>
-      </c>
-      <c r="F2" s="36" t="s">
-        <v>1027</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="29">
@@ -32968,19 +32984,19 @@
         <v>2</v>
       </c>
       <c r="B3" s="30" t="s">
+        <v>1027</v>
+      </c>
+      <c r="C3" s="30" t="s">
         <v>1028</v>
       </c>
-      <c r="C3" s="30" t="s">
+      <c r="D3" s="38" t="s">
         <v>1029</v>
       </c>
-      <c r="D3" s="38" t="s">
+      <c r="E3" s="41" t="s">
+        <v>1025</v>
+      </c>
+      <c r="F3" s="36" t="s">
         <v>1030</v>
-      </c>
-      <c r="E3" s="41" t="s">
-        <v>1026</v>
-      </c>
-      <c r="F3" s="36" t="s">
-        <v>1031</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="29">
@@ -32988,19 +33004,19 @@
         <v>3</v>
       </c>
       <c r="B4" s="30" t="s">
+        <v>1031</v>
+      </c>
+      <c r="C4" s="30" t="s">
         <v>1032</v>
       </c>
-      <c r="C4" s="30" t="s">
+      <c r="D4" s="38" t="s">
         <v>1033</v>
       </c>
-      <c r="D4" s="38" t="s">
+      <c r="E4" s="41" t="s">
+        <v>1025</v>
+      </c>
+      <c r="F4" s="36" t="s">
         <v>1034</v>
-      </c>
-      <c r="E4" s="41" t="s">
-        <v>1026</v>
-      </c>
-      <c r="F4" s="36" t="s">
-        <v>1035</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="29">
@@ -33008,19 +33024,19 @@
         <v>4</v>
       </c>
       <c r="B5" s="30" t="s">
+        <v>1035</v>
+      </c>
+      <c r="C5" s="30" t="s">
         <v>1036</v>
       </c>
-      <c r="C5" s="30" t="s">
+      <c r="D5" s="38" t="s">
         <v>1037</v>
       </c>
-      <c r="D5" s="38" t="s">
+      <c r="E5" s="41" t="s">
         <v>1038</v>
       </c>
-      <c r="E5" s="41" t="s">
+      <c r="F5" s="36" t="s">
         <v>1039</v>
-      </c>
-      <c r="F5" s="36" t="s">
-        <v>1040</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="29">
@@ -33028,19 +33044,19 @@
         <v>5</v>
       </c>
       <c r="B6" s="30" t="s">
+        <v>1040</v>
+      </c>
+      <c r="C6" s="30" t="s">
         <v>1041</v>
       </c>
-      <c r="C6" s="30" t="s">
+      <c r="D6" s="38" t="s">
         <v>1042</v>
       </c>
-      <c r="D6" s="38" t="s">
+      <c r="E6" s="41" t="s">
         <v>1043</v>
       </c>
-      <c r="E6" s="41" t="s">
+      <c r="F6" s="36" t="s">
         <v>1044</v>
-      </c>
-      <c r="F6" s="36" t="s">
-        <v>1045</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -33048,19 +33064,19 @@
         <v>6</v>
       </c>
       <c r="B7" s="30" t="s">
+        <v>1045</v>
+      </c>
+      <c r="C7" s="30" t="s">
         <v>1046</v>
       </c>
-      <c r="C7" s="30" t="s">
+      <c r="D7" s="38" t="s">
         <v>1047</v>
       </c>
-      <c r="D7" s="38" t="s">
+      <c r="E7" s="41" t="s">
         <v>1048</v>
       </c>
-      <c r="E7" s="41" t="s">
+      <c r="F7" s="36" t="s">
         <v>1049</v>
-      </c>
-      <c r="F7" s="36" t="s">
-        <v>1050</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="29">
@@ -33068,19 +33084,19 @@
         <v>7</v>
       </c>
       <c r="B8" s="30" t="s">
+        <v>1050</v>
+      </c>
+      <c r="C8" s="30" t="s">
         <v>1051</v>
       </c>
-      <c r="C8" s="30" t="s">
+      <c r="D8" s="38" t="s">
         <v>1052</v>
       </c>
-      <c r="D8" s="38" t="s">
+      <c r="E8" s="41" t="s">
         <v>1053</v>
       </c>
-      <c r="E8" s="41" t="s">
+      <c r="F8" s="36" t="s">
         <v>1054</v>
-      </c>
-      <c r="F8" s="36" t="s">
-        <v>1055</v>
       </c>
     </row>
     <row r="9" spans="1:6">
@@ -33088,19 +33104,19 @@
         <v>8</v>
       </c>
       <c r="B9" s="30" t="s">
+        <v>1055</v>
+      </c>
+      <c r="C9" s="30" t="s">
         <v>1056</v>
       </c>
-      <c r="C9" s="30" t="s">
+      <c r="D9" s="38" t="s">
         <v>1057</v>
       </c>
-      <c r="D9" s="38" t="s">
+      <c r="E9" s="41" t="s">
         <v>1058</v>
       </c>
-      <c r="E9" s="41" t="s">
+      <c r="F9" s="36" t="s">
         <v>1059</v>
-      </c>
-      <c r="F9" s="36" t="s">
-        <v>1060</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="29">
@@ -33108,19 +33124,19 @@
         <v>9</v>
       </c>
       <c r="B10" s="30" t="s">
+        <v>1060</v>
+      </c>
+      <c r="C10" s="30" t="s">
         <v>1061</v>
       </c>
-      <c r="C10" s="30" t="s">
+      <c r="D10" s="38" t="s">
         <v>1062</v>
       </c>
-      <c r="D10" s="38" t="s">
+      <c r="E10" s="41" t="s">
         <v>1063</v>
       </c>
-      <c r="E10" s="41" t="s">
+      <c r="F10" s="36" t="s">
         <v>1064</v>
-      </c>
-      <c r="F10" s="36" t="s">
-        <v>1065</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="57">
@@ -33128,19 +33144,19 @@
         <v>10</v>
       </c>
       <c r="B11" s="30" t="s">
+        <v>1065</v>
+      </c>
+      <c r="C11" s="30" t="s">
         <v>1066</v>
       </c>
-      <c r="C11" s="30" t="s">
+      <c r="D11" s="38" t="s">
         <v>1067</v>
       </c>
-      <c r="D11" s="38" t="s">
+      <c r="E11" s="41" t="s">
         <v>1068</v>
       </c>
-      <c r="E11" s="41" t="s">
+      <c r="F11" s="36" t="s">
         <v>1069</v>
-      </c>
-      <c r="F11" s="36" t="s">
-        <v>1070</v>
       </c>
     </row>
     <row r="12" spans="1:6">
@@ -33148,19 +33164,19 @@
         <v>11</v>
       </c>
       <c r="B12" s="30" t="s">
+        <v>1070</v>
+      </c>
+      <c r="C12" s="30" t="s">
         <v>1071</v>
       </c>
-      <c r="C12" s="30" t="s">
+      <c r="D12" s="38" t="s">
+        <v>1047</v>
+      </c>
+      <c r="E12" s="41" t="s">
         <v>1072</v>
       </c>
-      <c r="D12" s="38" t="s">
-        <v>1048</v>
-      </c>
-      <c r="E12" s="41" t="s">
+      <c r="F12" s="36" t="s">
         <v>1073</v>
-      </c>
-      <c r="F12" s="36" t="s">
-        <v>1074</v>
       </c>
     </row>
     <row r="13" spans="1:6">
@@ -33168,19 +33184,19 @@
         <v>12</v>
       </c>
       <c r="B13" s="30" t="s">
+        <v>1074</v>
+      </c>
+      <c r="C13" s="30" t="s">
         <v>1075</v>
       </c>
-      <c r="C13" s="30" t="s">
+      <c r="D13" s="38" t="s">
+        <v>1057</v>
+      </c>
+      <c r="E13" s="41" t="s">
         <v>1076</v>
       </c>
-      <c r="D13" s="38" t="s">
-        <v>1058</v>
-      </c>
-      <c r="E13" s="41" t="s">
+      <c r="F13" s="36" t="s">
         <v>1077</v>
-      </c>
-      <c r="F13" s="36" t="s">
-        <v>1078</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="29">
@@ -33188,19 +33204,19 @@
         <v>13</v>
       </c>
       <c r="B14" s="30" t="s">
+        <v>1078</v>
+      </c>
+      <c r="C14" s="30" t="s">
         <v>1079</v>
       </c>
-      <c r="C14" s="30" t="s">
+      <c r="D14" s="38" t="s">
         <v>1080</v>
       </c>
-      <c r="D14" s="38" t="s">
+      <c r="E14" s="41" t="s">
         <v>1081</v>
       </c>
-      <c r="E14" s="41" t="s">
+      <c r="F14" s="36" t="s">
         <v>1082</v>
-      </c>
-      <c r="F14" s="36" t="s">
-        <v>1083</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="29">
@@ -33208,19 +33224,19 @@
         <v>14</v>
       </c>
       <c r="B15" s="30" t="s">
+        <v>1083</v>
+      </c>
+      <c r="C15" s="30" t="s">
         <v>1084</v>
       </c>
-      <c r="C15" s="30" t="s">
+      <c r="D15" s="38" t="s">
         <v>1085</v>
       </c>
-      <c r="D15" s="38" t="s">
+      <c r="E15" s="41" t="s">
         <v>1086</v>
       </c>
-      <c r="E15" s="41" t="s">
+      <c r="F15" s="36" t="s">
         <v>1087</v>
-      </c>
-      <c r="F15" s="36" t="s">
-        <v>1088</v>
       </c>
     </row>
     <row r="16" spans="1:6">
@@ -33228,19 +33244,19 @@
         <v>15</v>
       </c>
       <c r="B16" s="30" t="s">
+        <v>1088</v>
+      </c>
+      <c r="C16" s="30" t="s">
         <v>1089</v>
       </c>
-      <c r="C16" s="30" t="s">
+      <c r="D16" s="38" t="s">
         <v>1090</v>
       </c>
-      <c r="D16" s="38" t="s">
+      <c r="E16" s="41" t="s">
         <v>1091</v>
       </c>
-      <c r="E16" s="41" t="s">
+      <c r="F16" s="36" t="s">
         <v>1092</v>
-      </c>
-      <c r="F16" s="36" t="s">
-        <v>1093</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="29">
@@ -33248,19 +33264,19 @@
         <v>16</v>
       </c>
       <c r="B17" s="30" t="s">
+        <v>1093</v>
+      </c>
+      <c r="C17" s="30" t="s">
         <v>1094</v>
       </c>
-      <c r="C17" s="30" t="s">
+      <c r="D17" s="38" t="s">
         <v>1095</v>
       </c>
-      <c r="D17" s="38" t="s">
+      <c r="E17" s="41" t="s">
         <v>1096</v>
       </c>
-      <c r="E17" s="41" t="s">
+      <c r="F17" s="36" t="s">
         <v>1097</v>
-      </c>
-      <c r="F17" s="36" t="s">
-        <v>1098</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="29">
@@ -33268,19 +33284,19 @@
         <v>17</v>
       </c>
       <c r="B18" s="30" t="s">
+        <v>1098</v>
+      </c>
+      <c r="C18" s="30" t="s">
         <v>1099</v>
       </c>
-      <c r="C18" s="30" t="s">
+      <c r="D18" s="38" t="s">
         <v>1100</v>
       </c>
-      <c r="D18" s="38" t="s">
+      <c r="E18" s="41" t="s">
+        <v>1081</v>
+      </c>
+      <c r="F18" s="36" t="s">
         <v>1101</v>
-      </c>
-      <c r="E18" s="41" t="s">
-        <v>1082</v>
-      </c>
-      <c r="F18" s="36" t="s">
-        <v>1102</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="29">
@@ -33288,19 +33304,19 @@
         <v>18</v>
       </c>
       <c r="B19" s="30" t="s">
+        <v>1102</v>
+      </c>
+      <c r="C19" s="30" t="s">
         <v>1103</v>
       </c>
-      <c r="C19" s="30" t="s">
+      <c r="D19" s="38" t="s">
         <v>1104</v>
       </c>
-      <c r="D19" s="38" t="s">
+      <c r="E19" s="41" t="s">
         <v>1105</v>
       </c>
-      <c r="E19" s="41" t="s">
+      <c r="F19" s="36" t="s">
         <v>1106</v>
-      </c>
-      <c r="F19" s="36" t="s">
-        <v>1107</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="29">
@@ -33308,19 +33324,19 @@
         <v>19</v>
       </c>
       <c r="B20" s="30" t="s">
+        <v>1107</v>
+      </c>
+      <c r="C20" s="30" t="s">
         <v>1108</v>
       </c>
-      <c r="C20" s="30" t="s">
+      <c r="D20" s="38" t="s">
         <v>1109</v>
       </c>
-      <c r="D20" s="38" t="s">
+      <c r="E20" s="41" t="s">
         <v>1110</v>
       </c>
-      <c r="E20" s="41" t="s">
+      <c r="F20" s="36" t="s">
         <v>1111</v>
-      </c>
-      <c r="F20" s="36" t="s">
-        <v>1112</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="29">
@@ -33328,19 +33344,19 @@
         <v>20</v>
       </c>
       <c r="B21" s="30" t="s">
+        <v>1112</v>
+      </c>
+      <c r="C21" s="30" t="s">
         <v>1113</v>
       </c>
-      <c r="C21" s="30" t="s">
+      <c r="D21" s="38" t="s">
         <v>1114</v>
       </c>
-      <c r="D21" s="38" t="s">
+      <c r="E21" s="41" t="s">
+        <v>1081</v>
+      </c>
+      <c r="F21" s="36" t="s">
         <v>1115</v>
-      </c>
-      <c r="E21" s="41" t="s">
-        <v>1082</v>
-      </c>
-      <c r="F21" s="36" t="s">
-        <v>1116</v>
       </c>
     </row>
     <row r="22" spans="1:6">
@@ -33348,19 +33364,19 @@
         <v>21</v>
       </c>
       <c r="B22" s="30" t="s">
+        <v>1116</v>
+      </c>
+      <c r="C22" s="30" t="s">
         <v>1117</v>
       </c>
-      <c r="C22" s="30" t="s">
+      <c r="D22" s="38" t="s">
+        <v>1047</v>
+      </c>
+      <c r="E22" s="41" t="s">
         <v>1118</v>
       </c>
-      <c r="D22" s="38" t="s">
-        <v>1048</v>
-      </c>
-      <c r="E22" s="41" t="s">
+      <c r="F22" s="36" t="s">
         <v>1119</v>
-      </c>
-      <c r="F22" s="36" t="s">
-        <v>1120</v>
       </c>
     </row>
   </sheetData>
@@ -33786,15 +33802,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <lcf76f155ced4ddcb4097134ff3c332f xmlns="633f040f-4953-46e7-8610-82b0c5296ba0">
@@ -33850,6 +33857,15 @@
 </p:properties>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{36C20BFB-BCC5-4457-BE44-22D2F12F84BE}">
   <ds:schemaRefs>
@@ -33870,26 +33886,26 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{83D5100D-0E56-4B30-B42D-2AEC6B837C39}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="633f040f-4953-46e7-8610-82b0c5296ba0"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="f62ef740-d444-4f18-80a2-7590fdcab1ce"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2C6CC7BA-2E2C-4B0D-8103-11A51D82E8EC}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{83D5100D-0E56-4B30-B42D-2AEC6B837C39}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="f62ef740-d444-4f18-80a2-7590fdcab1ce"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="633f040f-4953-46e7-8610-82b0c5296ba0"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
caricamento dei servizi funzionante
</commit_message>
<xml_diff>
--- a/apps/static/assets/dbs/ThreatCatalogComplete.xlsx
+++ b/apps/static/assets/dbs/ThreatCatalogComplete.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fefox/Desktop/AutomaticAttackPlanGenerator/apps/static/assets/dbs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{29CF1719-3165-304C-AE2B-C3EC834E1427}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{B3FD85A3-5A49-1643-AA03-47E27CF20998}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16260" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,7 +29,7 @@
   </definedNames>
   <calcPr calcId="191028"/>
   <pivotCaches>
-    <pivotCache cacheId="0" r:id="rId11"/>
+    <pivotCache cacheId="3" r:id="rId11"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -51,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4676" uniqueCount="1204">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4679" uniqueCount="1205">
   <si>
     <t>TID</t>
   </si>
@@ -3689,9 +3689,6 @@
     <t>OutputParser</t>
   </si>
   <si>
-    <t>nmap_classic</t>
-  </si>
-  <si>
     <t>AllowedOutputExtensions</t>
   </si>
   <si>
@@ -3705,6 +3702,12 @@
   </si>
   <si>
     <t>nmap -sV -p- -oX {output_file} -T4 --min-parallelism 100 {ip}</t>
+  </si>
+  <si>
+    <t>nmap/classic</t>
+  </si>
+  <si>
+    <t>nmap/services</t>
   </si>
 </sst>
 </file>
@@ -9203,7 +9206,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{48CB07D6-9F6C-094F-A3D3-916741F281CD}" name="Tabella pivot1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valori" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{48CB07D6-9F6C-094F-A3D3-916741F281CD}" name="Tabella pivot1" cacheId="3" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valori" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A1:B25" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="14">
     <pivotField showAll="0"/>
@@ -32032,8 +32035,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C51FC597-29FA-1D4E-A4C8-B79027768242}">
   <dimension ref="A1:J9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B4" zoomScale="163" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView tabSelected="1" topLeftCell="E3" zoomScale="163" workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15"/>
@@ -32077,7 +32080,7 @@
         <v>1197</v>
       </c>
       <c r="J1" s="26" t="s">
-        <v>1199</v>
+        <v>1198</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="64">
@@ -32176,7 +32179,7 @@
         <v>954</v>
       </c>
       <c r="E5" s="26" t="s">
-        <v>1202</v>
+        <v>1201</v>
       </c>
       <c r="F5" s="27" t="s">
         <v>1187</v>
@@ -32186,6 +32189,9 @@
       </c>
       <c r="H5" s="26" t="s">
         <v>1196</v>
+      </c>
+      <c r="J5" s="26" t="s">
+        <v>1199</v>
       </c>
     </row>
     <row r="6" spans="1:10" ht="32">
@@ -32203,7 +32209,7 @@
         <v>956</v>
       </c>
       <c r="E6" s="26" t="s">
-        <v>1201</v>
+        <v>1200</v>
       </c>
       <c r="F6" s="27" t="s">
         <v>1184</v>
@@ -32215,10 +32221,10 @@
         <v>1196</v>
       </c>
       <c r="I6" s="26" t="s">
-        <v>1198</v>
+        <v>1203</v>
       </c>
       <c r="J6" s="26" t="s">
-        <v>1200</v>
+        <v>1199</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="32">
@@ -32236,7 +32242,7 @@
         <v>954</v>
       </c>
       <c r="E7" s="26" t="s">
-        <v>1203</v>
+        <v>1202</v>
       </c>
       <c r="F7" s="27" t="s">
         <v>1188</v>
@@ -32246,6 +32252,12 @@
       </c>
       <c r="H7" s="26" t="s">
         <v>1196</v>
+      </c>
+      <c r="I7" s="26" t="s">
+        <v>1204</v>
+      </c>
+      <c r="J7" s="26" t="s">
+        <v>1199</v>
       </c>
     </row>
     <row r="8" spans="1:10" ht="80">
@@ -33397,6 +33409,71 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="633f040f-4953-46e7-8610-82b0c5296ba0">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="f62ef740-d444-4f18-80a2-7590fdcab1ce" xsi:nil="true"/>
+    <Has_Teacher_Only_SectionGroup xmlns="633f040f-4953-46e7-8610-82b0c5296ba0" xsi:nil="true"/>
+    <Teachers xmlns="633f040f-4953-46e7-8610-82b0c5296ba0">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </Teachers>
+    <IsNotebookLocked xmlns="633f040f-4953-46e7-8610-82b0c5296ba0" xsi:nil="true"/>
+    <CultureName xmlns="633f040f-4953-46e7-8610-82b0c5296ba0" xsi:nil="true"/>
+    <Owner xmlns="633f040f-4953-46e7-8610-82b0c5296ba0">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </Owner>
+    <Distribution_Groups xmlns="633f040f-4953-46e7-8610-82b0c5296ba0" xsi:nil="true"/>
+    <TeamsChannelId xmlns="633f040f-4953-46e7-8610-82b0c5296ba0" xsi:nil="true"/>
+    <Invited_Teachers xmlns="633f040f-4953-46e7-8610-82b0c5296ba0" xsi:nil="true"/>
+    <NotebookType xmlns="633f040f-4953-46e7-8610-82b0c5296ba0" xsi:nil="true"/>
+    <AppVersion xmlns="633f040f-4953-46e7-8610-82b0c5296ba0" xsi:nil="true"/>
+    <DefaultSectionNames xmlns="633f040f-4953-46e7-8610-82b0c5296ba0" xsi:nil="true"/>
+    <Is_Collaboration_Space_Locked xmlns="633f040f-4953-46e7-8610-82b0c5296ba0" xsi:nil="true"/>
+    <Templates xmlns="633f040f-4953-46e7-8610-82b0c5296ba0" xsi:nil="true"/>
+    <FolderType xmlns="633f040f-4953-46e7-8610-82b0c5296ba0" xsi:nil="true"/>
+    <Student_Groups xmlns="633f040f-4953-46e7-8610-82b0c5296ba0">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </Student_Groups>
+    <Teams_Channel_Section_Location xmlns="633f040f-4953-46e7-8610-82b0c5296ba0" xsi:nil="true"/>
+    <Math_Settings xmlns="633f040f-4953-46e7-8610-82b0c5296ba0" xsi:nil="true"/>
+    <Self_Registration_Enabled xmlns="633f040f-4953-46e7-8610-82b0c5296ba0" xsi:nil="true"/>
+    <Students xmlns="633f040f-4953-46e7-8610-82b0c5296ba0">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </Students>
+    <LMS_Mappings xmlns="633f040f-4953-46e7-8610-82b0c5296ba0" xsi:nil="true"/>
+    <Invited_Students xmlns="633f040f-4953-46e7-8610-82b0c5296ba0" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x0101009A9CE0B21D9C3A45B31425227616CD6F" ma:contentTypeVersion="34" ma:contentTypeDescription="Creare un nuovo documento." ma:contentTypeScope="" ma:versionID="8a882b22c4c6ceab40c069a6a2420ef3">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="633f040f-4953-46e7-8610-82b0c5296ba0" xmlns:ns3="f62ef740-d444-4f18-80a2-7590fdcab1ce" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="77035a69dc4d6b80a35ec1b02b2030a4" ns2:_="" ns3:_="">
     <xsd:import namespace="633f040f-4953-46e7-8610-82b0c5296ba0"/>
@@ -33813,72 +33890,32 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="633f040f-4953-46e7-8610-82b0c5296ba0">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="f62ef740-d444-4f18-80a2-7590fdcab1ce" xsi:nil="true"/>
-    <Has_Teacher_Only_SectionGroup xmlns="633f040f-4953-46e7-8610-82b0c5296ba0" xsi:nil="true"/>
-    <Teachers xmlns="633f040f-4953-46e7-8610-82b0c5296ba0">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </Teachers>
-    <IsNotebookLocked xmlns="633f040f-4953-46e7-8610-82b0c5296ba0" xsi:nil="true"/>
-    <CultureName xmlns="633f040f-4953-46e7-8610-82b0c5296ba0" xsi:nil="true"/>
-    <Owner xmlns="633f040f-4953-46e7-8610-82b0c5296ba0">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </Owner>
-    <Distribution_Groups xmlns="633f040f-4953-46e7-8610-82b0c5296ba0" xsi:nil="true"/>
-    <TeamsChannelId xmlns="633f040f-4953-46e7-8610-82b0c5296ba0" xsi:nil="true"/>
-    <Invited_Teachers xmlns="633f040f-4953-46e7-8610-82b0c5296ba0" xsi:nil="true"/>
-    <NotebookType xmlns="633f040f-4953-46e7-8610-82b0c5296ba0" xsi:nil="true"/>
-    <AppVersion xmlns="633f040f-4953-46e7-8610-82b0c5296ba0" xsi:nil="true"/>
-    <DefaultSectionNames xmlns="633f040f-4953-46e7-8610-82b0c5296ba0" xsi:nil="true"/>
-    <Is_Collaboration_Space_Locked xmlns="633f040f-4953-46e7-8610-82b0c5296ba0" xsi:nil="true"/>
-    <Templates xmlns="633f040f-4953-46e7-8610-82b0c5296ba0" xsi:nil="true"/>
-    <FolderType xmlns="633f040f-4953-46e7-8610-82b0c5296ba0" xsi:nil="true"/>
-    <Student_Groups xmlns="633f040f-4953-46e7-8610-82b0c5296ba0">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </Student_Groups>
-    <Teams_Channel_Section_Location xmlns="633f040f-4953-46e7-8610-82b0c5296ba0" xsi:nil="true"/>
-    <Math_Settings xmlns="633f040f-4953-46e7-8610-82b0c5296ba0" xsi:nil="true"/>
-    <Self_Registration_Enabled xmlns="633f040f-4953-46e7-8610-82b0c5296ba0" xsi:nil="true"/>
-    <Students xmlns="633f040f-4953-46e7-8610-82b0c5296ba0">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </Students>
-    <LMS_Mappings xmlns="633f040f-4953-46e7-8610-82b0c5296ba0" xsi:nil="true"/>
-    <Invited_Students xmlns="633f040f-4953-46e7-8610-82b0c5296ba0" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{83D5100D-0E56-4B30-B42D-2AEC6B837C39}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="f62ef740-d444-4f18-80a2-7590fdcab1ce"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="633f040f-4953-46e7-8610-82b0c5296ba0"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2C6CC7BA-2E2C-4B0D-8103-11A51D82E8EC}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{36C20BFB-BCC5-4457-BE44-22D2F12F84BE}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -33895,29 +33932,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{83D5100D-0E56-4B30-B42D-2AEC6B837C39}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="633f040f-4953-46e7-8610-82b0c5296ba0"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="f62ef740-d444-4f18-80a2-7590fdcab1ce"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2C6CC7BA-2E2C-4B0D-8103-11A51D82E8EC}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Migliorato scss macm-detail Introdotta possibiltà di caricare, scaricare, fare il parsing e cancellare i report per tutti i comandi.
</commit_message>
<xml_diff>
--- a/apps/static/assets/dbs/ThreatCatalogComplete.xlsx
+++ b/apps/static/assets/dbs/ThreatCatalogComplete.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11027"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fefox/Desktop/AutomaticAttackPlanGenerator/apps/static/assets/dbs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB2DDE12-9042-4C4B-8134-991D4F1855B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{C9B71BAB-1A4B-C34B-83E3-43CEF385E322}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-4840" yWindow="-21100" windowWidth="38400" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-4840" yWindow="-21100" windowWidth="38400" windowHeight="21100" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Threat Components" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
   </definedNames>
   <calcPr calcId="191028"/>
   <pivotCaches>
-    <pivotCache cacheId="3" r:id="rId12"/>
+    <pivotCache cacheId="0" r:id="rId12"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -52,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4697" uniqueCount="1218">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4702" uniqueCount="1219">
   <si>
     <t>TID</t>
   </si>
@@ -3687,12 +3687,6 @@
     <t>True</t>
   </si>
   <si>
-    <t>OutputParser</t>
-  </si>
-  <si>
-    <t>AllowedOutputExtensions</t>
-  </si>
-  <si>
     <t>.xml</t>
   </si>
   <si>
@@ -3748,6 +3742,15 @@
   </si>
   <si>
     <t>1</t>
+  </si>
+  <si>
+    <t>ReportParser</t>
+  </si>
+  <si>
+    <t>AllowedReportExtensions</t>
+  </si>
+  <si>
+    <t>*</t>
   </si>
 </sst>
 </file>
@@ -4147,18 +4150,6 @@
   </cellStyles>
   <dxfs count="33">
     <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <font>
         <color rgb="FF9C0006"/>
       </font>
@@ -4206,6 +4197,18 @@
     </dxf>
     <dxf>
       <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
@@ -9250,7 +9253,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{48CB07D6-9F6C-094F-A3D3-916741F281CD}" name="Tabella pivot1" cacheId="3" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valori" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{48CB07D6-9F6C-094F-A3D3-916741F281CD}" name="Tabella pivot1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valori" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A1:B25" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="14">
     <pivotField showAll="0"/>
@@ -9421,9 +9424,9 @@
     <tableColumn id="15" xr3:uid="{CEE151EC-4E5B-0C41-8586-5A2D7E483661}" name="PostCondition" dataDxfId="18"/>
     <tableColumn id="5" xr3:uid="{62EC5D77-1F78-1645-8697-BC5450583418}" name="CapecMeta" dataDxfId="17"/>
     <tableColumn id="11" xr3:uid="{0DCD762C-4EE7-8141-BC05-9DB756A5BEF2}" name="CapecStandard" dataDxfId="16"/>
-    <tableColumn id="17" xr3:uid="{9EF317BA-855B-6E4A-9EC7-E1FB88A1FD56}" name="CapecDetailed" dataDxfId="2"/>
-    <tableColumn id="20" xr3:uid="{EFADD164-FE35-0949-9988-883343158BA4}" name="Methodology" dataDxfId="0"/>
-    <tableColumn id="18" xr3:uid="{9BF6197D-4CF5-4941-A460-18823EEFB2E7}" name="Commento" dataDxfId="1"/>
+    <tableColumn id="17" xr3:uid="{9EF317BA-855B-6E4A-9EC7-E1FB88A1FD56}" name="CapecDetailed" dataDxfId="15"/>
+    <tableColumn id="20" xr3:uid="{EFADD164-FE35-0949-9988-883343158BA4}" name="Methodology" dataDxfId="14"/>
+    <tableColumn id="18" xr3:uid="{9BF6197D-4CF5-4941-A460-18823EEFB2E7}" name="Commento" dataDxfId="13"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -9456,21 +9459,21 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{5ECAFCE9-964F-A04C-B050-422AACCFD3F5}" name="Tabella4" displayName="Tabella4" ref="A1:J9" totalsRowShown="0" headerRowDxfId="15" dataDxfId="14">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{5ECAFCE9-964F-A04C-B050-422AACCFD3F5}" name="Tabella4" displayName="Tabella4" ref="A1:J9" totalsRowShown="0" headerRowDxfId="12" dataDxfId="11">
   <autoFilter ref="A1:J9" xr:uid="{5ECAFCE9-964F-A04C-B050-422AACCFD3F5}"/>
   <tableColumns count="10">
-    <tableColumn id="1" xr3:uid="{6405AD35-9222-B34C-A112-EC4FDEAC5BE2}" name="ToolID" dataDxfId="13">
+    <tableColumn id="1" xr3:uid="{6405AD35-9222-B34C-A112-EC4FDEAC5BE2}" name="ToolID" dataDxfId="10">
       <calculatedColumnFormula>ROW(Tabella4[[#This Row],[Name]])-1</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{94F8DBBB-A826-8B4A-8C87-395122CA233A}" name="Name" dataDxfId="12"/>
-    <tableColumn id="2" xr3:uid="{FB636F07-AAD2-AE48-87BB-965F92F829C2}" name="CapecID" dataDxfId="11"/>
-    <tableColumn id="6" xr3:uid="{1E4A4CA6-7FF1-6543-A718-93EC7B5F1624}" name="CypherQuery" dataDxfId="10"/>
-    <tableColumn id="3" xr3:uid="{52487567-ED26-B840-ABFD-DB1BF72A83C9}" name="Command" dataDxfId="9"/>
-    <tableColumn id="5" xr3:uid="{0296B95F-6562-0746-B0C6-FE3564F6272C}" name="Description" dataDxfId="8"/>
-    <tableColumn id="7" xr3:uid="{FF0722DB-3140-904D-9B8E-A0C7B3C1FFEF}" name="PhaseID" dataDxfId="7"/>
-    <tableColumn id="8" xr3:uid="{2C7E754F-9F49-044B-9F1A-B62738B70258}" name="IsExecutable" dataDxfId="6"/>
-    <tableColumn id="9" xr3:uid="{6A4595CA-3FDC-EC4F-B8F1-4344144E8149}" name="OutputParser" dataDxfId="5"/>
-    <tableColumn id="10" xr3:uid="{1CDFEE20-E2A1-E348-BB9C-16F2A7D9AEC0}" name="AllowedOutputExtensions" dataDxfId="4"/>
+    <tableColumn id="4" xr3:uid="{94F8DBBB-A826-8B4A-8C87-395122CA233A}" name="Name" dataDxfId="9"/>
+    <tableColumn id="2" xr3:uid="{FB636F07-AAD2-AE48-87BB-965F92F829C2}" name="CapecID" dataDxfId="8"/>
+    <tableColumn id="6" xr3:uid="{1E4A4CA6-7FF1-6543-A718-93EC7B5F1624}" name="CypherQuery" dataDxfId="7"/>
+    <tableColumn id="3" xr3:uid="{52487567-ED26-B840-ABFD-DB1BF72A83C9}" name="Command" dataDxfId="6"/>
+    <tableColumn id="5" xr3:uid="{0296B95F-6562-0746-B0C6-FE3564F6272C}" name="Description" dataDxfId="5"/>
+    <tableColumn id="7" xr3:uid="{FF0722DB-3140-904D-9B8E-A0C7B3C1FFEF}" name="PhaseID" dataDxfId="4"/>
+    <tableColumn id="8" xr3:uid="{2C7E754F-9F49-044B-9F1A-B62738B70258}" name="IsExecutable" dataDxfId="3"/>
+    <tableColumn id="9" xr3:uid="{6A4595CA-3FDC-EC4F-B8F1-4344144E8149}" name="ReportParser" dataDxfId="2"/>
+    <tableColumn id="10" xr3:uid="{1CDFEE20-E2A1-E348-BB9C-16F2A7D9AEC0}" name="AllowedReportExtensions" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -9758,9 +9761,9 @@
   </sheetPr>
   <dimension ref="A1:S326"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="125" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView topLeftCell="F1" zoomScale="125" zoomScaleNormal="115" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A317" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="Q324" sqref="Q324"/>
+      <selection pane="bottomLeft" activeCell="R319" sqref="R319"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -9837,7 +9840,7 @@
         <v>16</v>
       </c>
       <c r="R1" s="23" t="s">
-        <v>1216</v>
+        <v>1214</v>
       </c>
       <c r="S1" s="23" t="s">
         <v>17</v>
@@ -27388,13 +27391,13 @@
         <v>T322</v>
       </c>
       <c r="B323" s="20" t="s">
+        <v>1203</v>
+      </c>
+      <c r="C323" s="20" t="s">
+        <v>1204</v>
+      </c>
+      <c r="D323" s="20" t="s">
         <v>1205</v>
-      </c>
-      <c r="C323" s="20" t="s">
-        <v>1206</v>
-      </c>
-      <c r="D323" s="20" t="s">
-        <v>1207</v>
       </c>
       <c r="E323" s="20"/>
       <c r="F323" s="20"/>
@@ -27427,13 +27430,13 @@
         <v>T323</v>
       </c>
       <c r="B324" s="20" t="s">
+        <v>1203</v>
+      </c>
+      <c r="C324" s="20" t="s">
+        <v>1209</v>
+      </c>
+      <c r="D324" s="20" t="s">
         <v>1205</v>
-      </c>
-      <c r="C324" s="20" t="s">
-        <v>1211</v>
-      </c>
-      <c r="D324" s="20" t="s">
-        <v>1207</v>
       </c>
       <c r="E324" s="20"/>
       <c r="F324" s="20"/>
@@ -27458,7 +27461,7 @@
       <c r="P324" s="24"/>
       <c r="Q324" s="24"/>
       <c r="R324" s="24" t="s">
-        <v>1217</v>
+        <v>1215</v>
       </c>
       <c r="S324" s="24"/>
     </row>
@@ -27468,10 +27471,10 @@
         <v>T324</v>
       </c>
       <c r="B325" s="20" t="s">
-        <v>1208</v>
+        <v>1206</v>
       </c>
       <c r="C325" s="20" t="s">
-        <v>1209</v>
+        <v>1207</v>
       </c>
       <c r="D325" s="20"/>
       <c r="E325" s="20"/>
@@ -27505,10 +27508,10 @@
         <v>T325</v>
       </c>
       <c r="B326" s="20" t="s">
+        <v>1206</v>
+      </c>
+      <c r="C326" s="20" t="s">
         <v>1208</v>
-      </c>
-      <c r="C326" s="20" t="s">
-        <v>1210</v>
       </c>
       <c r="D326" s="20"/>
       <c r="E326" s="20"/>
@@ -27539,7 +27542,7 @@
   </sheetData>
   <phoneticPr fontId="11" type="noConversion"/>
   <conditionalFormatting sqref="O1:R326">
-    <cfRule type="containsBlanks" dxfId="3" priority="1" stopIfTrue="1">
+    <cfRule type="containsBlanks" dxfId="0" priority="1" stopIfTrue="1">
       <formula>LEN(TRIM(O1))=0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -28633,7 +28636,7 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
-        <v>1212</v>
+        <v>1210</v>
       </c>
       <c r="B1" t="s">
         <v>936</v>
@@ -28642,7 +28645,7 @@
         <v>3</v>
       </c>
       <c r="D1" t="s">
-        <v>1213</v>
+        <v>1211</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -28650,10 +28653,10 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>1215</v>
+        <v>1213</v>
       </c>
       <c r="D2" t="s">
-        <v>1214</v>
+        <v>1212</v>
       </c>
     </row>
   </sheetData>
@@ -33083,8 +33086,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C51FC597-29FA-1D4E-A4C8-B79027768242}">
   <dimension ref="A1:J9"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" zoomScale="137" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+    <sheetView tabSelected="1" zoomScale="137" workbookViewId="0">
+      <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15"/>
@@ -33096,7 +33099,10 @@
     <col min="5" max="5" width="55.5" style="26" customWidth="1"/>
     <col min="6" max="6" width="12.6640625" style="27" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="10.83203125" style="28"/>
-    <col min="8" max="16384" width="10.83203125" style="26"/>
+    <col min="8" max="8" width="10.83203125" style="26"/>
+    <col min="9" max="9" width="11.6640625" style="26" customWidth="1"/>
+    <col min="10" max="10" width="21.83203125" style="26" customWidth="1"/>
+    <col min="11" max="16384" width="10.83203125" style="26"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="16">
@@ -33125,10 +33131,10 @@
         <v>1194</v>
       </c>
       <c r="I1" s="26" t="s">
-        <v>1197</v>
+        <v>1216</v>
       </c>
       <c r="J1" s="26" t="s">
-        <v>1198</v>
+        <v>1217</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="64">
@@ -33157,6 +33163,9 @@
       <c r="H2" s="26" t="s">
         <v>1195</v>
       </c>
+      <c r="J2" s="26" t="s">
+        <v>1218</v>
+      </c>
     </row>
     <row r="3" spans="1:10" ht="64">
       <c r="A3" s="26">
@@ -33184,6 +33193,9 @@
       <c r="H3" s="26" t="s">
         <v>1195</v>
       </c>
+      <c r="J3" s="26" t="s">
+        <v>1218</v>
+      </c>
     </row>
     <row r="4" spans="1:10" ht="80">
       <c r="A4" s="26">
@@ -33211,6 +33223,9 @@
       <c r="H4" s="26" t="s">
         <v>1195</v>
       </c>
+      <c r="J4" s="26" t="s">
+        <v>1218</v>
+      </c>
     </row>
     <row r="5" spans="1:10" ht="32">
       <c r="A5" s="26">
@@ -33227,7 +33242,7 @@
         <v>954</v>
       </c>
       <c r="E5" s="26" t="s">
-        <v>1201</v>
+        <v>1199</v>
       </c>
       <c r="F5" s="27" t="s">
         <v>1187</v>
@@ -33239,7 +33254,7 @@
         <v>1196</v>
       </c>
       <c r="J5" s="26" t="s">
-        <v>1199</v>
+        <v>1197</v>
       </c>
     </row>
     <row r="6" spans="1:10" ht="32">
@@ -33257,7 +33272,7 @@
         <v>956</v>
       </c>
       <c r="E6" s="26" t="s">
-        <v>1200</v>
+        <v>1198</v>
       </c>
       <c r="F6" s="27" t="s">
         <v>1184</v>
@@ -33269,10 +33284,10 @@
         <v>1196</v>
       </c>
       <c r="I6" s="26" t="s">
-        <v>1203</v>
+        <v>1201</v>
       </c>
       <c r="J6" s="26" t="s">
-        <v>1199</v>
+        <v>1197</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="32">
@@ -33290,7 +33305,7 @@
         <v>954</v>
       </c>
       <c r="E7" s="26" t="s">
-        <v>1202</v>
+        <v>1200</v>
       </c>
       <c r="F7" s="27" t="s">
         <v>1188</v>
@@ -33302,10 +33317,10 @@
         <v>1196</v>
       </c>
       <c r="I7" s="26" t="s">
-        <v>1204</v>
+        <v>1202</v>
       </c>
       <c r="J7" s="26" t="s">
-        <v>1199</v>
+        <v>1197</v>
       </c>
     </row>
     <row r="8" spans="1:10" ht="80">
@@ -33334,6 +33349,9 @@
       <c r="H8" s="26" t="s">
         <v>1195</v>
       </c>
+      <c r="J8" s="26" t="s">
+        <v>1218</v>
+      </c>
     </row>
     <row r="9" spans="1:10" ht="96">
       <c r="A9" s="26">
@@ -33360,6 +33378,9 @@
       </c>
       <c r="H9" s="26" t="s">
         <v>1195</v>
+      </c>
+      <c r="J9" s="26" t="s">
+        <v>1218</v>
       </c>
     </row>
   </sheetData>
@@ -34503,16 +34524,16 @@
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{83D5100D-0E56-4B30-B42D-2AEC6B837C39}">
   <ds:schemaRefs>
+    <ds:schemaRef ds:uri="633f040f-4953-46e7-8610-82b0c5296ba0"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="f62ef740-d444-4f18-80a2-7590fdcab1ce"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
     <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="f62ef740-d444-4f18-80a2-7590fdcab1ce"/>
-    <ds:schemaRef ds:uri="633f040f-4953-46e7-8610-82b0c5296ba0"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
aggiunta possibilità di caricare il file excel
</commit_message>
<xml_diff>
--- a/apps/static/assets/dbs/ThreatCatalogComplete.xlsx
+++ b/apps/static/assets/dbs/ThreatCatalogComplete.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fefox/Desktop/AutomaticAttackPlanGenerator/apps/static/assets/dbs/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fefox/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27A4C853-70C6-354C-9AC1-15F98DA7914F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{920A5635-0276-F14A-AD85-2157E180E7DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16280" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -52,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4712" uniqueCount="1219">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4703" uniqueCount="1220">
   <si>
     <t>TID</t>
   </si>
@@ -3751,6 +3751,9 @@
   </si>
   <si>
     <t>HW.SOC</t>
+  </si>
+  <si>
+    <t>blabla</t>
   </si>
 </sst>
 </file>
@@ -4010,7 +4013,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="58">
+  <cellXfs count="57">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -4135,23 +4138,20 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="35">
+  <dxfs count="33">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -4163,24 +4163,43 @@
       </fill>
     </dxf>
     <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
@@ -4247,45 +4266,6 @@
     </dxf>
     <dxf>
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -9417,39 +9397,39 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{DEFAB213-4389-184E-911C-CDCC8CABBD38}" name="Tabella1" displayName="Tabella1" ref="A1:S327" totalsRowShown="0" dataDxfId="22">
-  <autoFilter ref="A1:S327" xr:uid="{DEFAB213-4389-184E-911C-CDCC8CABBD38}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{DEFAB213-4389-184E-911C-CDCC8CABBD38}" name="Tabella1" displayName="Tabella1" ref="A1:S326" totalsRowShown="0" dataDxfId="32">
+  <autoFilter ref="A1:S326" xr:uid="{DEFAB213-4389-184E-911C-CDCC8CABBD38}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A255:S269">
     <sortCondition ref="B1:B313"/>
   </sortState>
   <tableColumns count="19">
-    <tableColumn id="16" xr3:uid="{DE426BDB-E154-EE46-B7B3-5B538C8AEC32}" name="TID" dataDxfId="21">
+    <tableColumn id="16" xr3:uid="{DE426BDB-E154-EE46-B7B3-5B538C8AEC32}" name="TID" dataDxfId="31">
       <calculatedColumnFormula>CONCATENATE("T",ROW(A2)-1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="1" xr3:uid="{A0AE63DC-99F7-7D4F-B824-AB7765893284}" name="Asset" dataDxfId="20"/>
-    <tableColumn id="2" xr3:uid="{0FA38BFF-C67B-0C43-B1BA-F6338DBFB0C8}" name="Threat" dataDxfId="19"/>
-    <tableColumn id="3" xr3:uid="{BFC77F7C-F096-8345-97EA-317816ED869D}" name="Description" dataDxfId="18"/>
-    <tableColumn id="4" xr3:uid="{258F3B86-1461-D64A-AE3B-CEAC97B2B533}" name="STRIDE" dataDxfId="17"/>
-    <tableColumn id="6" xr3:uid="{0FD06C95-5962-AC4D-B9EF-4DBB5728E736}" name="Compromised" dataDxfId="16"/>
-    <tableColumn id="7" xr3:uid="{9E5B99AD-1F1D-B44C-ABDF-6F7E9177F3DE}" name="PreC" dataDxfId="15"/>
-    <tableColumn id="8" xr3:uid="{D4F97A81-E528-2841-B4DE-321362F90F65}" name="PreI" dataDxfId="14"/>
-    <tableColumn id="9" xr3:uid="{018427D6-D385-3447-B4A4-95003B3341F6}" name="PreA" dataDxfId="13"/>
-    <tableColumn id="10" xr3:uid="{8334AC57-4A09-5744-9484-073ECEE2E513}" name="Precondition" dataDxfId="12"/>
-    <tableColumn id="12" xr3:uid="{DDBE315D-E051-2C47-A765-EE1DB2E118EA}" name="PostC" dataDxfId="11">
+    <tableColumn id="1" xr3:uid="{A0AE63DC-99F7-7D4F-B824-AB7765893284}" name="Asset" dataDxfId="30"/>
+    <tableColumn id="2" xr3:uid="{0FA38BFF-C67B-0C43-B1BA-F6338DBFB0C8}" name="Threat" dataDxfId="29"/>
+    <tableColumn id="3" xr3:uid="{BFC77F7C-F096-8345-97EA-317816ED869D}" name="Description" dataDxfId="28"/>
+    <tableColumn id="4" xr3:uid="{258F3B86-1461-D64A-AE3B-CEAC97B2B533}" name="STRIDE" dataDxfId="27"/>
+    <tableColumn id="6" xr3:uid="{0FD06C95-5962-AC4D-B9EF-4DBB5728E736}" name="Compromised" dataDxfId="26"/>
+    <tableColumn id="7" xr3:uid="{9E5B99AD-1F1D-B44C-ABDF-6F7E9177F3DE}" name="PreC" dataDxfId="25"/>
+    <tableColumn id="8" xr3:uid="{D4F97A81-E528-2841-B4DE-321362F90F65}" name="PreI" dataDxfId="24"/>
+    <tableColumn id="9" xr3:uid="{018427D6-D385-3447-B4A4-95003B3341F6}" name="PreA" dataDxfId="23"/>
+    <tableColumn id="10" xr3:uid="{8334AC57-4A09-5744-9484-073ECEE2E513}" name="Precondition" dataDxfId="22"/>
+    <tableColumn id="12" xr3:uid="{DDBE315D-E051-2C47-A765-EE1DB2E118EA}" name="PostC" dataDxfId="21">
       <calculatedColumnFormula>MID(N2,2,1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" xr3:uid="{243C1B9B-76C9-0345-B727-4F11FD75DF6B}" name="PostI" dataDxfId="10">
+    <tableColumn id="13" xr3:uid="{243C1B9B-76C9-0345-B727-4F11FD75DF6B}" name="PostI" dataDxfId="20">
       <calculatedColumnFormula>MID(N2,4,1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="14" xr3:uid="{DD688DAA-2C9A-C247-AEC4-CBDADE9B2B2E}" name="PostA" dataDxfId="9">
+    <tableColumn id="14" xr3:uid="{DD688DAA-2C9A-C247-AEC4-CBDADE9B2B2E}" name="PostA" dataDxfId="19">
       <calculatedColumnFormula>MID(N2,6,1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="15" xr3:uid="{CEE151EC-4E5B-0C41-8586-5A2D7E483661}" name="PostCondition" dataDxfId="8"/>
-    <tableColumn id="5" xr3:uid="{62EC5D77-1F78-1645-8697-BC5450583418}" name="CapecMeta" dataDxfId="7"/>
-    <tableColumn id="11" xr3:uid="{0DCD762C-4EE7-8141-BC05-9DB756A5BEF2}" name="CapecStandard" dataDxfId="6"/>
-    <tableColumn id="17" xr3:uid="{9EF317BA-855B-6E4A-9EC7-E1FB88A1FD56}" name="CapecDetailed" dataDxfId="5"/>
-    <tableColumn id="20" xr3:uid="{EFADD164-FE35-0949-9988-883343158BA4}" name="Methodology" dataDxfId="4"/>
-    <tableColumn id="18" xr3:uid="{9BF6197D-4CF5-4941-A460-18823EEFB2E7}" name="Commento" dataDxfId="3"/>
+    <tableColumn id="15" xr3:uid="{CEE151EC-4E5B-0C41-8586-5A2D7E483661}" name="PostCondition" dataDxfId="18"/>
+    <tableColumn id="5" xr3:uid="{62EC5D77-1F78-1645-8697-BC5450583418}" name="CapecMeta" dataDxfId="17"/>
+    <tableColumn id="11" xr3:uid="{0DCD762C-4EE7-8141-BC05-9DB756A5BEF2}" name="CapecStandard" dataDxfId="16"/>
+    <tableColumn id="17" xr3:uid="{9EF317BA-855B-6E4A-9EC7-E1FB88A1FD56}" name="CapecDetailed" dataDxfId="15"/>
+    <tableColumn id="20" xr3:uid="{EFADD164-FE35-0949-9988-883343158BA4}" name="Methodology" dataDxfId="14"/>
+    <tableColumn id="18" xr3:uid="{9BF6197D-4CF5-4941-A460-18823EEFB2E7}" name="Commento" dataDxfId="13"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -9482,21 +9462,21 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{5ECAFCE9-964F-A04C-B050-422AACCFD3F5}" name="Tabella4" displayName="Tabella4" ref="A1:J9" totalsRowShown="0" headerRowDxfId="34" dataDxfId="33">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{5ECAFCE9-964F-A04C-B050-422AACCFD3F5}" name="Tabella4" displayName="Tabella4" ref="A1:J9" totalsRowShown="0" headerRowDxfId="12" dataDxfId="11">
   <autoFilter ref="A1:J9" xr:uid="{5ECAFCE9-964F-A04C-B050-422AACCFD3F5}"/>
   <tableColumns count="10">
-    <tableColumn id="1" xr3:uid="{6405AD35-9222-B34C-A112-EC4FDEAC5BE2}" name="ToolID" dataDxfId="32">
+    <tableColumn id="1" xr3:uid="{6405AD35-9222-B34C-A112-EC4FDEAC5BE2}" name="ToolID" dataDxfId="10">
       <calculatedColumnFormula>ROW(Tabella4[[#This Row],[Name]])-1</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{94F8DBBB-A826-8B4A-8C87-395122CA233A}" name="Name" dataDxfId="31"/>
-    <tableColumn id="2" xr3:uid="{FB636F07-AAD2-AE48-87BB-965F92F829C2}" name="CapecID" dataDxfId="30"/>
-    <tableColumn id="6" xr3:uid="{1E4A4CA6-7FF1-6543-A718-93EC7B5F1624}" name="CypherQuery" dataDxfId="29"/>
-    <tableColumn id="3" xr3:uid="{52487567-ED26-B840-ABFD-DB1BF72A83C9}" name="Command" dataDxfId="28"/>
-    <tableColumn id="5" xr3:uid="{0296B95F-6562-0746-B0C6-FE3564F6272C}" name="Description" dataDxfId="27"/>
-    <tableColumn id="7" xr3:uid="{FF0722DB-3140-904D-9B8E-A0C7B3C1FFEF}" name="PhaseID" dataDxfId="26"/>
-    <tableColumn id="8" xr3:uid="{2C7E754F-9F49-044B-9F1A-B62738B70258}" name="IsExecutable" dataDxfId="25"/>
-    <tableColumn id="9" xr3:uid="{6A4595CA-3FDC-EC4F-B8F1-4344144E8149}" name="ReportParser" dataDxfId="24"/>
-    <tableColumn id="10" xr3:uid="{1CDFEE20-E2A1-E348-BB9C-16F2A7D9AEC0}" name="AllowedReportExtensions" dataDxfId="23"/>
+    <tableColumn id="4" xr3:uid="{94F8DBBB-A826-8B4A-8C87-395122CA233A}" name="Name" dataDxfId="9"/>
+    <tableColumn id="2" xr3:uid="{FB636F07-AAD2-AE48-87BB-965F92F829C2}" name="CapecID" dataDxfId="8"/>
+    <tableColumn id="6" xr3:uid="{1E4A4CA6-7FF1-6543-A718-93EC7B5F1624}" name="CypherQuery" dataDxfId="7"/>
+    <tableColumn id="3" xr3:uid="{52487567-ED26-B840-ABFD-DB1BF72A83C9}" name="Command" dataDxfId="6"/>
+    <tableColumn id="5" xr3:uid="{0296B95F-6562-0746-B0C6-FE3564F6272C}" name="Description" dataDxfId="5"/>
+    <tableColumn id="7" xr3:uid="{FF0722DB-3140-904D-9B8E-A0C7B3C1FFEF}" name="PhaseID" dataDxfId="4"/>
+    <tableColumn id="8" xr3:uid="{2C7E754F-9F49-044B-9F1A-B62738B70258}" name="IsExecutable" dataDxfId="3"/>
+    <tableColumn id="9" xr3:uid="{6A4595CA-3FDC-EC4F-B8F1-4344144E8149}" name="ReportParser" dataDxfId="2"/>
+    <tableColumn id="10" xr3:uid="{1CDFEE20-E2A1-E348-BB9C-16F2A7D9AEC0}" name="AllowedReportExtensions" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -9782,11 +9762,11 @@
   <sheetPr>
     <tabColor rgb="FF00B050"/>
   </sheetPr>
-  <dimension ref="A1:S327"/>
+  <dimension ref="A1:S326"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="185" zoomScaleNormal="185" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A323" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C327" sqref="C327"/>
+    <sheetView tabSelected="1" zoomScale="185" zoomScaleNormal="115" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A320" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D326" sqref="D326"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -27499,7 +27479,9 @@
       <c r="C325" s="20" t="s">
         <v>1206</v>
       </c>
-      <c r="D325" s="20"/>
+      <c r="D325" s="20" t="s">
+        <v>1219</v>
+      </c>
       <c r="E325" s="20"/>
       <c r="F325" s="20"/>
       <c r="G325" s="20"/>
@@ -27562,78 +27544,11 @@
       <c r="R326" s="24"/>
       <c r="S326" s="24"/>
     </row>
-    <row r="327" spans="1:19" ht="240">
-      <c r="A327" s="57" t="str">
-        <f>CONCATENATE("T",ROW(A327)-1)</f>
-        <v>T326</v>
-      </c>
-      <c r="B327" s="20" t="s">
-        <v>1218</v>
-      </c>
-      <c r="C327" s="20" t="s">
-        <v>279</v>
-      </c>
-      <c r="D327" s="20" t="s">
-        <v>280</v>
-      </c>
-      <c r="E327" s="20" t="s">
-        <v>43</v>
-      </c>
-      <c r="F327" s="20" t="s">
-        <v>160</v>
-      </c>
-      <c r="G327" s="20" t="str">
-        <f t="shared" ref="G327" si="57">MID(J327,2,1)</f>
-        <v>p</v>
-      </c>
-      <c r="H327" s="20" t="str">
-        <f t="shared" ref="H327" si="58">MID(J327,4,1)</f>
-        <v>p</v>
-      </c>
-      <c r="I327" s="20" t="str">
-        <f t="shared" ref="I327" si="59">MID(J327,6,1)</f>
-        <v>n</v>
-      </c>
-      <c r="J327" s="20" t="s">
-        <v>91</v>
-      </c>
-      <c r="K327" s="20" t="str">
-        <f t="shared" ref="K327" si="60">MID(N327,2,1)</f>
-        <v>n</v>
-      </c>
-      <c r="L327" s="20" t="str">
-        <f t="shared" ref="L327" si="61">MID(N327,4,1)</f>
-        <v>n</v>
-      </c>
-      <c r="M327" s="20" t="str">
-        <f t="shared" ref="M327" si="62">MID(N327,6,1)</f>
-        <v>n</v>
-      </c>
-      <c r="N327" s="20" t="s">
-        <v>181</v>
-      </c>
-      <c r="O327" s="24" t="s">
-        <v>281</v>
-      </c>
-      <c r="P327" s="24" t="s">
-        <v>282</v>
-      </c>
-      <c r="Q327" s="24" t="s">
-        <v>283</v>
-      </c>
-      <c r="R327" s="24"/>
-      <c r="S327" s="24"/>
-    </row>
   </sheetData>
   <phoneticPr fontId="11" type="noConversion"/>
-  <conditionalFormatting sqref="O1:R327">
-    <cfRule type="containsBlanks" dxfId="2" priority="2" stopIfTrue="1">
+  <conditionalFormatting sqref="O1:R326">
+    <cfRule type="containsBlanks" dxfId="0" priority="1" stopIfTrue="1">
       <formula>LEN(TRIM(O1))=0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="O327:R327">
-    <cfRule type="containsBlanks" dxfId="1" priority="1" stopIfTrue="1">
-      <formula>LEN(TRIM(O327))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -29988,7 +29903,7 @@
       </c>
     </row>
     <row r="30" spans="1:13" ht="48">
-      <c r="A30" s="56" t="s">
+      <c r="A30" s="54" t="s">
         <v>811</v>
       </c>
       <c r="B30" s="5" t="s">
@@ -30031,7 +29946,7 @@
       </c>
     </row>
     <row r="31" spans="1:13" ht="48">
-      <c r="A31" s="56"/>
+      <c r="A31" s="54"/>
       <c r="B31" s="5" t="s">
         <v>814</v>
       </c>
@@ -30072,7 +29987,7 @@
       </c>
     </row>
     <row r="32" spans="1:13" ht="32">
-      <c r="A32" s="56"/>
+      <c r="A32" s="54"/>
       <c r="B32" s="5" t="s">
         <v>816</v>
       </c>
@@ -30113,7 +30028,7 @@
       </c>
     </row>
     <row r="33" spans="1:13" ht="96">
-      <c r="A33" s="56"/>
+      <c r="A33" s="54"/>
       <c r="B33" s="5" t="s">
         <v>100</v>
       </c>
@@ -30154,7 +30069,7 @@
       </c>
     </row>
     <row r="34" spans="1:13" ht="32">
-      <c r="A34" s="56"/>
+      <c r="A34" s="54"/>
       <c r="B34" s="5" t="s">
         <v>819</v>
       </c>
@@ -30195,7 +30110,7 @@
       </c>
     </row>
     <row r="35" spans="1:13" ht="32">
-      <c r="A35" s="56"/>
+      <c r="A35" s="54"/>
       <c r="B35" s="5" t="s">
         <v>201</v>
       </c>
@@ -30236,7 +30151,7 @@
       </c>
     </row>
     <row r="36" spans="1:13" ht="80">
-      <c r="A36" s="56"/>
+      <c r="A36" s="54"/>
       <c r="B36" s="5" t="s">
         <v>822</v>
       </c>
@@ -30775,7 +30690,7 @@
       </c>
     </row>
     <row r="49" spans="1:13" ht="78" customHeight="1">
-      <c r="A49" s="56" t="s">
+      <c r="A49" s="54" t="s">
         <v>840</v>
       </c>
       <c r="B49" s="5" t="s">
@@ -30818,7 +30733,7 @@
       </c>
     </row>
     <row r="50" spans="1:13" ht="32">
-      <c r="A50" s="56"/>
+      <c r="A50" s="54"/>
       <c r="B50" s="5" t="s">
         <v>613</v>
       </c>
@@ -30859,7 +30774,7 @@
       </c>
     </row>
     <row r="51" spans="1:13" ht="16">
-      <c r="A51" s="56"/>
+      <c r="A51" s="54"/>
       <c r="B51" s="5" t="s">
         <v>201</v>
       </c>
@@ -30900,7 +30815,7 @@
       </c>
     </row>
     <row r="52" spans="1:13" ht="32">
-      <c r="A52" s="56"/>
+      <c r="A52" s="54"/>
       <c r="B52" s="5" t="s">
         <v>845</v>
       </c>
@@ -30941,7 +30856,7 @@
       </c>
     </row>
     <row r="53" spans="1:13" ht="96">
-      <c r="A53" s="56"/>
+      <c r="A53" s="54"/>
       <c r="B53" s="5" t="s">
         <v>847</v>
       </c>
@@ -30982,7 +30897,7 @@
       </c>
     </row>
     <row r="54" spans="1:13">
-      <c r="A54" s="56"/>
+      <c r="A54" s="54"/>
       <c r="B54" s="5" t="s">
         <v>849</v>
       </c>
@@ -31023,7 +30938,7 @@
       </c>
     </row>
     <row r="55" spans="1:13" ht="64">
-      <c r="A55" s="56"/>
+      <c r="A55" s="54"/>
       <c r="B55" s="5" t="s">
         <v>851</v>
       </c>
@@ -31064,7 +30979,7 @@
       </c>
     </row>
     <row r="56" spans="1:13" ht="64">
-      <c r="A56" s="56"/>
+      <c r="A56" s="54"/>
       <c r="B56" s="5" t="s">
         <v>853</v>
       </c>
@@ -31105,7 +31020,7 @@
       </c>
     </row>
     <row r="57" spans="1:13" ht="32">
-      <c r="A57" s="54" t="s">
+      <c r="A57" s="55" t="s">
         <v>855</v>
       </c>
       <c r="B57" s="6" t="s">
@@ -31147,7 +31062,7 @@
       </c>
     </row>
     <row r="58" spans="1:13" ht="80">
-      <c r="A58" s="54"/>
+      <c r="A58" s="55"/>
       <c r="B58" s="7" t="s">
         <v>858</v>
       </c>
@@ -31187,7 +31102,7 @@
       </c>
     </row>
     <row r="59" spans="1:13" ht="64" customHeight="1">
-      <c r="A59" s="54"/>
+      <c r="A59" s="55"/>
       <c r="B59" s="7" t="s">
         <v>860</v>
       </c>
@@ -31227,7 +31142,7 @@
       </c>
     </row>
     <row r="60" spans="1:13" ht="16">
-      <c r="A60" s="54"/>
+      <c r="A60" s="55"/>
       <c r="B60" s="7" t="s">
         <v>95</v>
       </c>
@@ -31267,7 +31182,7 @@
       </c>
     </row>
     <row r="61" spans="1:13" ht="32">
-      <c r="A61" s="54"/>
+      <c r="A61" s="55"/>
       <c r="B61" s="7" t="s">
         <v>864</v>
       </c>
@@ -31307,7 +31222,7 @@
       </c>
     </row>
     <row r="62" spans="1:13" ht="32">
-      <c r="A62" s="54"/>
+      <c r="A62" s="55"/>
       <c r="B62" s="7" t="s">
         <v>866</v>
       </c>
@@ -31347,7 +31262,7 @@
       </c>
     </row>
     <row r="63" spans="1:13" ht="16">
-      <c r="A63" s="54"/>
+      <c r="A63" s="55"/>
       <c r="B63" s="7" t="s">
         <v>869</v>
       </c>
@@ -31387,7 +31302,7 @@
       </c>
     </row>
     <row r="64" spans="1:13" ht="32">
-      <c r="A64" s="54"/>
+      <c r="A64" s="55"/>
       <c r="B64" s="6" t="s">
         <v>871</v>
       </c>
@@ -31427,7 +31342,7 @@
       </c>
     </row>
     <row r="65" spans="1:13" ht="16">
-      <c r="A65" s="54"/>
+      <c r="A65" s="55"/>
       <c r="B65" s="7" t="s">
         <v>82</v>
       </c>
@@ -31467,7 +31382,7 @@
       </c>
     </row>
     <row r="66" spans="1:13" ht="16">
-      <c r="A66" s="54"/>
+      <c r="A66" s="55"/>
       <c r="B66" s="7" t="s">
         <v>874</v>
       </c>
@@ -31507,7 +31422,7 @@
       </c>
     </row>
     <row r="67" spans="1:13" ht="48">
-      <c r="A67" s="54"/>
+      <c r="A67" s="55"/>
       <c r="B67" s="6" t="s">
         <v>92</v>
       </c>
@@ -31547,38 +31462,38 @@
       </c>
     </row>
     <row r="68" spans="1:13" ht="16">
-      <c r="A68" s="54"/>
-      <c r="B68" s="54" t="s">
+      <c r="A68" s="55"/>
+      <c r="B68" s="55" t="s">
         <v>169</v>
       </c>
       <c r="C68" s="6" t="s">
         <v>876</v>
       </c>
-      <c r="D68" s="54" t="s">
+      <c r="D68" s="55" t="s">
         <v>27</v>
       </c>
-      <c r="E68" s="54" t="s">
+      <c r="E68" s="55" t="s">
         <v>862</v>
       </c>
-      <c r="F68" s="54" t="s">
-        <v>23</v>
-      </c>
-      <c r="G68" s="54" t="s">
+      <c r="F68" s="55" t="s">
+        <v>23</v>
+      </c>
+      <c r="G68" s="55" t="s">
         <v>23</v>
       </c>
       <c r="H68" s="53" t="s">
         <v>23</v>
       </c>
-      <c r="I68" s="54" t="s">
+      <c r="I68" s="55" t="s">
         <v>181</v>
       </c>
-      <c r="J68" s="54" t="s">
-        <v>23</v>
-      </c>
-      <c r="K68" s="54" t="s">
-        <v>23</v>
-      </c>
-      <c r="L68" s="54" t="s">
+      <c r="J68" s="55" t="s">
+        <v>23</v>
+      </c>
+      <c r="K68" s="55" t="s">
+        <v>23</v>
+      </c>
+      <c r="L68" s="55" t="s">
         <v>84</v>
       </c>
       <c r="M68" s="53" t="str">
@@ -31587,24 +31502,24 @@
       </c>
     </row>
     <row r="69" spans="1:13" ht="16">
-      <c r="A69" s="54"/>
-      <c r="B69" s="54"/>
+      <c r="A69" s="55"/>
+      <c r="B69" s="55"/>
       <c r="C69" s="6" t="s">
         <v>877</v>
       </c>
-      <c r="D69" s="54"/>
-      <c r="E69" s="54"/>
-      <c r="F69" s="54"/>
-      <c r="G69" s="54"/>
+      <c r="D69" s="55"/>
+      <c r="E69" s="55"/>
+      <c r="F69" s="55"/>
+      <c r="G69" s="55"/>
       <c r="H69" s="53"/>
-      <c r="I69" s="54"/>
-      <c r="J69" s="54"/>
-      <c r="K69" s="54"/>
-      <c r="L69" s="54"/>
+      <c r="I69" s="55"/>
+      <c r="J69" s="55"/>
+      <c r="K69" s="55"/>
+      <c r="L69" s="55"/>
       <c r="M69" s="53"/>
     </row>
     <row r="70" spans="1:13" ht="28">
-      <c r="A70" s="55" t="s">
+      <c r="A70" s="56" t="s">
         <v>878</v>
       </c>
       <c r="B70" s="16" t="s">
@@ -31650,7 +31565,7 @@
       </c>
     </row>
     <row r="71" spans="1:13" ht="51">
-      <c r="A71" s="55"/>
+      <c r="A71" s="56"/>
       <c r="B71" s="16" t="s">
         <v>100</v>
       </c>
@@ -31694,7 +31609,7 @@
       </c>
     </row>
     <row r="72" spans="1:13" ht="28">
-      <c r="A72" s="55"/>
+      <c r="A72" s="56"/>
       <c r="B72" s="16" t="s">
         <v>763</v>
       </c>
@@ -31738,7 +31653,7 @@
       </c>
     </row>
     <row r="73" spans="1:13" ht="28">
-      <c r="A73" s="55"/>
+      <c r="A73" s="56"/>
       <c r="B73" s="16" t="s">
         <v>885</v>
       </c>
@@ -32300,15 +32215,6 @@
     </row>
   </sheetData>
   <mergeCells count="23">
-    <mergeCell ref="A2:A7"/>
-    <mergeCell ref="A8:A14"/>
-    <mergeCell ref="A25:A29"/>
-    <mergeCell ref="A15:A24"/>
-    <mergeCell ref="A49:A56"/>
-    <mergeCell ref="A44:A48"/>
-    <mergeCell ref="A41:A43"/>
-    <mergeCell ref="A30:A36"/>
-    <mergeCell ref="A37:A40"/>
     <mergeCell ref="M68:M69"/>
     <mergeCell ref="H68:H69"/>
     <mergeCell ref="A74:A85"/>
@@ -32323,6 +32229,15 @@
     <mergeCell ref="B68:B69"/>
     <mergeCell ref="D68:D69"/>
     <mergeCell ref="E68:E69"/>
+    <mergeCell ref="A2:A7"/>
+    <mergeCell ref="A8:A14"/>
+    <mergeCell ref="A25:A29"/>
+    <mergeCell ref="A15:A24"/>
+    <mergeCell ref="A49:A56"/>
+    <mergeCell ref="A44:A48"/>
+    <mergeCell ref="A41:A43"/>
+    <mergeCell ref="A30:A36"/>
+    <mergeCell ref="A37:A40"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -34520,15 +34435,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <lcf76f155ced4ddcb4097134ff3c332f xmlns="633f040f-4953-46e7-8610-82b0c5296ba0">
@@ -34584,6 +34490,15 @@
 </p:properties>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{36C20BFB-BCC5-4457-BE44-22D2F12F84BE}">
   <ds:schemaRefs>
@@ -34604,26 +34519,26 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{83D5100D-0E56-4B30-B42D-2AEC6B837C39}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="633f040f-4953-46e7-8610-82b0c5296ba0"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="f62ef740-d444-4f18-80a2-7590fdcab1ce"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2C6CC7BA-2E2C-4B0D-8103-11A51D82E8EC}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{83D5100D-0E56-4B30-B42D-2AEC6B837C39}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="f62ef740-d444-4f18-80a2-7590fdcab1ce"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="633f040f-4953-46e7-8610-82b0c5296ba0"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Aggiunta admin views, manca una da correggere. Modifiche al modello per risk analysis.
</commit_message>
<xml_diff>
--- a/apps/static/assets/dbs/ThreatCatalogComplete.xlsx
+++ b/apps/static/assets/dbs/ThreatCatalogComplete.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fefox/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{280C890A-FA6C-914E-9D32-77F3A9800CD2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE7E0C08-BAEB-4049-BA08-75AC14A77107}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16280" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16300" firstSheet="2" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Threat Components" sheetId="1" r:id="rId1"/>
@@ -23,14 +23,16 @@
     <sheet name="ThreatAgentQuestions" sheetId="8" r:id="rId8"/>
     <sheet name="ThreatAgentReply" sheetId="13" r:id="rId9"/>
     <sheet name="ThreatAgentCategory" sheetId="9" r:id="rId10"/>
-    <sheet name="ThreatAgentAttribute" sheetId="12" r:id="rId11"/>
+    <sheet name="ThreatAgentReplyCategory" sheetId="15" r:id="rId11"/>
+    <sheet name="ThreatAgentAttribute" sheetId="12" r:id="rId12"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">Threats!$A$1:$B$76</definedName>
+    <definedName name="ThreatAgentReplyCategory" localSheetId="10">ThreatAgentReplyCategory!$A$2:$C$152</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
   <pivotCaches>
-    <pivotCache cacheId="1" r:id="rId12"/>
+    <pivotCache cacheId="1" r:id="rId13"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -51,8 +53,22 @@
 </workbook>
 </file>
 
+<file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
+<connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16">
+  <connection id="1" xr16:uid="{C9BB50AB-6299-6B4E-B0AD-5E8DA7DF5CBF}" name="ThreatAgentReplyCategory" type="6" refreshedVersion="8" background="1" saveData="1">
+    <textPr sourceFile="/Users/danielegranata/Desktop/ThreatAgentReplyCategory.csv" decimal="," thousands="." tab="0" comma="1">
+      <textFields count="3">
+        <textField/>
+        <textField/>
+        <textField/>
+      </textFields>
+    </textPr>
+  </connection>
+</connections>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5232" uniqueCount="1355">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5235" uniqueCount="1359">
   <si>
     <t>TID</t>
   </si>
@@ -4209,6 +4225,18 @@
   </si>
   <si>
     <t>AssetType</t>
+  </si>
+  <si>
+    <t>PreCondition</t>
+  </si>
+  <si>
+    <t>Id</t>
+  </si>
+  <si>
+    <t>Reply_id</t>
+  </si>
+  <si>
+    <t>Category_id</t>
   </si>
 </sst>
 </file>
@@ -4663,14 +4691,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -9923,6 +9951,10 @@
 </pivotTableDefinition>
 </file>
 
+<file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="ThreatAgentReplyCategory" connectionId="1" xr16:uid="{EAE361E3-2BFC-CA43-BBB6-0E422B13C5A1}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{DEFAB213-4389-184E-911C-CDCC8CABBD38}" name="Tabella1" displayName="Tabella1" ref="A1:R393" totalsRowShown="0" dataDxfId="32">
   <autoFilter ref="A1:R393" xr:uid="{DEFAB213-4389-184E-911C-CDCC8CABBD38}"/>
@@ -9941,7 +9973,7 @@
     <tableColumn id="7" xr3:uid="{9E5B99AD-1F1D-B44C-ABDF-6F7E9177F3DE}" name="PreC" dataDxfId="25"/>
     <tableColumn id="8" xr3:uid="{D4F97A81-E528-2841-B4DE-321362F90F65}" name="PreI" dataDxfId="24"/>
     <tableColumn id="9" xr3:uid="{018427D6-D385-3447-B4A4-95003B3341F6}" name="PreA" dataDxfId="23"/>
-    <tableColumn id="10" xr3:uid="{8334AC57-4A09-5744-9484-073ECEE2E513}" name="Precondition" dataDxfId="22"/>
+    <tableColumn id="10" xr3:uid="{8334AC57-4A09-5744-9484-073ECEE2E513}" name="PreCondition" dataDxfId="22"/>
     <tableColumn id="12" xr3:uid="{DDBE315D-E051-2C47-A765-EE1DB2E118EA}" name="PostC" dataDxfId="21">
       <calculatedColumnFormula>MID(N2,2,1)</calculatedColumnFormula>
     </tableColumn>
@@ -10291,9 +10323,9 @@
   </sheetPr>
   <dimension ref="A1:R393"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A322" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="R1" sqref="R1:R1048576"/>
+    <sheetView zoomScaleNormal="115" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -10345,7 +10377,7 @@
         <v>8</v>
       </c>
       <c r="J1" t="s">
-        <v>9</v>
+        <v>1355</v>
       </c>
       <c r="K1" t="s">
         <v>10</v>
@@ -31409,6 +31441,1701 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D9628EC2-10D1-124D-9116-6DD9EB1BE094}">
+  <sheetPr>
+    <tabColor rgb="FFFF0000"/>
+  </sheetPr>
+  <dimension ref="A1:C152"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="200" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="4.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.6640625" customWidth="1"/>
+    <col min="3" max="3" width="19.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" t="s">
+        <v>1356</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1357</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1358</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="C6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7">
+        <v>1</v>
+      </c>
+      <c r="C7">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8">
+        <v>1</v>
+      </c>
+      <c r="C8">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9">
+        <v>1</v>
+      </c>
+      <c r="C9">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10">
+        <v>1</v>
+      </c>
+      <c r="C10">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11">
+        <v>1</v>
+      </c>
+      <c r="C11">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12">
+        <v>1</v>
+      </c>
+      <c r="C12">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13">
+        <v>1</v>
+      </c>
+      <c r="C13">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14">
+        <v>1</v>
+      </c>
+      <c r="C14">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15">
+        <v>1</v>
+      </c>
+      <c r="C15">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16">
+        <v>1</v>
+      </c>
+      <c r="C16">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17">
+        <v>1</v>
+      </c>
+      <c r="C17">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
+      <c r="A18">
+        <v>18</v>
+      </c>
+      <c r="B18">
+        <v>1</v>
+      </c>
+      <c r="C18">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="A19">
+        <v>19</v>
+      </c>
+      <c r="B19">
+        <v>1</v>
+      </c>
+      <c r="C19">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
+      <c r="A20">
+        <v>20</v>
+      </c>
+      <c r="B20">
+        <v>1</v>
+      </c>
+      <c r="C20">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3">
+      <c r="A21">
+        <v>21</v>
+      </c>
+      <c r="B21">
+        <v>1</v>
+      </c>
+      <c r="C21">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3">
+      <c r="A22">
+        <v>22</v>
+      </c>
+      <c r="B22">
+        <v>2</v>
+      </c>
+      <c r="C22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3">
+      <c r="A23">
+        <v>23</v>
+      </c>
+      <c r="B23">
+        <v>2</v>
+      </c>
+      <c r="C23">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3">
+      <c r="A24">
+        <v>24</v>
+      </c>
+      <c r="B24">
+        <v>2</v>
+      </c>
+      <c r="C24">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3">
+      <c r="A25">
+        <v>25</v>
+      </c>
+      <c r="B25">
+        <v>2</v>
+      </c>
+      <c r="C25">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3">
+      <c r="A26">
+        <v>26</v>
+      </c>
+      <c r="B26">
+        <v>2</v>
+      </c>
+      <c r="C26">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3">
+      <c r="A27">
+        <v>27</v>
+      </c>
+      <c r="B27">
+        <v>2</v>
+      </c>
+      <c r="C27">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3">
+      <c r="A28">
+        <v>28</v>
+      </c>
+      <c r="B28">
+        <v>3</v>
+      </c>
+      <c r="C28">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3">
+      <c r="A29">
+        <v>30</v>
+      </c>
+      <c r="B29">
+        <v>3</v>
+      </c>
+      <c r="C29">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3">
+      <c r="A30">
+        <v>31</v>
+      </c>
+      <c r="B30">
+        <v>3</v>
+      </c>
+      <c r="C30">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3">
+      <c r="A31">
+        <v>32</v>
+      </c>
+      <c r="B31">
+        <v>3</v>
+      </c>
+      <c r="C31">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3">
+      <c r="A32">
+        <v>33</v>
+      </c>
+      <c r="B32">
+        <v>3</v>
+      </c>
+      <c r="C32">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3">
+      <c r="A33">
+        <v>34</v>
+      </c>
+      <c r="B33">
+        <v>3</v>
+      </c>
+      <c r="C33">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3">
+      <c r="A34">
+        <v>35</v>
+      </c>
+      <c r="B34">
+        <v>3</v>
+      </c>
+      <c r="C34">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3">
+      <c r="A35">
+        <v>36</v>
+      </c>
+      <c r="B35">
+        <v>3</v>
+      </c>
+      <c r="C35">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3">
+      <c r="A36">
+        <v>37</v>
+      </c>
+      <c r="B36">
+        <v>3</v>
+      </c>
+      <c r="C36">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3">
+      <c r="A37">
+        <v>38</v>
+      </c>
+      <c r="B37">
+        <v>3</v>
+      </c>
+      <c r="C37">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3">
+      <c r="A38">
+        <v>39</v>
+      </c>
+      <c r="B38">
+        <v>3</v>
+      </c>
+      <c r="C38">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3">
+      <c r="A39">
+        <v>40</v>
+      </c>
+      <c r="B39">
+        <v>3</v>
+      </c>
+      <c r="C39">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3">
+      <c r="A40">
+        <v>41</v>
+      </c>
+      <c r="B40">
+        <v>4</v>
+      </c>
+      <c r="C40">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3">
+      <c r="A41">
+        <v>42</v>
+      </c>
+      <c r="B41">
+        <v>4</v>
+      </c>
+      <c r="C41">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3">
+      <c r="A42">
+        <v>44</v>
+      </c>
+      <c r="B42">
+        <v>4</v>
+      </c>
+      <c r="C42">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3">
+      <c r="A43">
+        <v>45</v>
+      </c>
+      <c r="B43">
+        <v>4</v>
+      </c>
+      <c r="C43">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3">
+      <c r="A44">
+        <v>46</v>
+      </c>
+      <c r="B44">
+        <v>4</v>
+      </c>
+      <c r="C44">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3">
+      <c r="A45">
+        <v>47</v>
+      </c>
+      <c r="B45">
+        <v>4</v>
+      </c>
+      <c r="C45">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3">
+      <c r="A46">
+        <v>48</v>
+      </c>
+      <c r="B46">
+        <v>4</v>
+      </c>
+      <c r="C46">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3">
+      <c r="A47">
+        <v>50</v>
+      </c>
+      <c r="B47">
+        <v>4</v>
+      </c>
+      <c r="C47">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3">
+      <c r="A48">
+        <v>54</v>
+      </c>
+      <c r="B48">
+        <v>4</v>
+      </c>
+      <c r="C48">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3">
+      <c r="A49">
+        <v>55</v>
+      </c>
+      <c r="B49">
+        <v>4</v>
+      </c>
+      <c r="C49">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3">
+      <c r="A50">
+        <v>57</v>
+      </c>
+      <c r="B50">
+        <v>4</v>
+      </c>
+      <c r="C50">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3">
+      <c r="A51">
+        <v>58</v>
+      </c>
+      <c r="B51">
+        <v>4</v>
+      </c>
+      <c r="C51">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3">
+      <c r="A52">
+        <v>60</v>
+      </c>
+      <c r="B52">
+        <v>4</v>
+      </c>
+      <c r="C52">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3">
+      <c r="A53">
+        <v>61</v>
+      </c>
+      <c r="B53">
+        <v>5</v>
+      </c>
+      <c r="C53">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3">
+      <c r="A54">
+        <v>62</v>
+      </c>
+      <c r="B54">
+        <v>4</v>
+      </c>
+      <c r="C54">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3">
+      <c r="A55">
+        <v>63</v>
+      </c>
+      <c r="B55">
+        <v>5</v>
+      </c>
+      <c r="C55">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3">
+      <c r="A56">
+        <v>64</v>
+      </c>
+      <c r="B56">
+        <v>5</v>
+      </c>
+      <c r="C56">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3">
+      <c r="A57">
+        <v>65</v>
+      </c>
+      <c r="B57">
+        <v>5</v>
+      </c>
+      <c r="C57">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3">
+      <c r="A58">
+        <v>66</v>
+      </c>
+      <c r="B58">
+        <v>5</v>
+      </c>
+      <c r="C58">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3">
+      <c r="A59">
+        <v>67</v>
+      </c>
+      <c r="B59">
+        <v>5</v>
+      </c>
+      <c r="C59">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3">
+      <c r="A60">
+        <v>68</v>
+      </c>
+      <c r="B60">
+        <v>5</v>
+      </c>
+      <c r="C60">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3">
+      <c r="A61">
+        <v>69</v>
+      </c>
+      <c r="B61">
+        <v>5</v>
+      </c>
+      <c r="C61">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3">
+      <c r="A62">
+        <v>70</v>
+      </c>
+      <c r="B62">
+        <v>5</v>
+      </c>
+      <c r="C62">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3">
+      <c r="A63">
+        <v>71</v>
+      </c>
+      <c r="B63">
+        <v>6</v>
+      </c>
+      <c r="C63">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3">
+      <c r="A64">
+        <v>72</v>
+      </c>
+      <c r="B64">
+        <v>7</v>
+      </c>
+      <c r="C64">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3">
+      <c r="A65">
+        <v>73</v>
+      </c>
+      <c r="B65">
+        <v>6</v>
+      </c>
+      <c r="C65">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3">
+      <c r="A66">
+        <v>74</v>
+      </c>
+      <c r="B66">
+        <v>6</v>
+      </c>
+      <c r="C66">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3">
+      <c r="A67">
+        <v>75</v>
+      </c>
+      <c r="B67">
+        <v>6</v>
+      </c>
+      <c r="C67">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3">
+      <c r="A68">
+        <v>76</v>
+      </c>
+      <c r="B68">
+        <v>7</v>
+      </c>
+      <c r="C68">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3">
+      <c r="A69">
+        <v>77</v>
+      </c>
+      <c r="B69">
+        <v>12</v>
+      </c>
+      <c r="C69">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3">
+      <c r="A70">
+        <v>78</v>
+      </c>
+      <c r="B70">
+        <v>7</v>
+      </c>
+      <c r="C70">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3">
+      <c r="A71">
+        <v>79</v>
+      </c>
+      <c r="B71">
+        <v>7</v>
+      </c>
+      <c r="C71">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3">
+      <c r="A72">
+        <v>80</v>
+      </c>
+      <c r="B72">
+        <v>7</v>
+      </c>
+      <c r="C72">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3">
+      <c r="A73">
+        <v>81</v>
+      </c>
+      <c r="B73">
+        <v>7</v>
+      </c>
+      <c r="C73">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3">
+      <c r="A74">
+        <v>82</v>
+      </c>
+      <c r="B74">
+        <v>13</v>
+      </c>
+      <c r="C74">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3">
+      <c r="A75">
+        <v>83</v>
+      </c>
+      <c r="B75">
+        <v>7</v>
+      </c>
+      <c r="C75">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3">
+      <c r="A76">
+        <v>84</v>
+      </c>
+      <c r="B76">
+        <v>8</v>
+      </c>
+      <c r="C76">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3">
+      <c r="A77">
+        <v>86</v>
+      </c>
+      <c r="B77">
+        <v>8</v>
+      </c>
+      <c r="C77">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3">
+      <c r="A78">
+        <v>87</v>
+      </c>
+      <c r="B78">
+        <v>8</v>
+      </c>
+      <c r="C78">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3">
+      <c r="A79">
+        <v>88</v>
+      </c>
+      <c r="B79">
+        <v>8</v>
+      </c>
+      <c r="C79">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3">
+      <c r="A80">
+        <v>89</v>
+      </c>
+      <c r="B80">
+        <v>8</v>
+      </c>
+      <c r="C80">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3">
+      <c r="A81">
+        <v>90</v>
+      </c>
+      <c r="B81">
+        <v>8</v>
+      </c>
+      <c r="C81">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3">
+      <c r="A82">
+        <v>91</v>
+      </c>
+      <c r="B82">
+        <v>9</v>
+      </c>
+      <c r="C82">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3">
+      <c r="A83">
+        <v>93</v>
+      </c>
+      <c r="B83">
+        <v>9</v>
+      </c>
+      <c r="C83">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3">
+      <c r="A84">
+        <v>94</v>
+      </c>
+      <c r="B84">
+        <v>9</v>
+      </c>
+      <c r="C84">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3">
+      <c r="A85">
+        <v>95</v>
+      </c>
+      <c r="B85">
+        <v>9</v>
+      </c>
+      <c r="C85">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3">
+      <c r="A86">
+        <v>96</v>
+      </c>
+      <c r="B86">
+        <v>9</v>
+      </c>
+      <c r="C86">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3">
+      <c r="A87">
+        <v>97</v>
+      </c>
+      <c r="B87">
+        <v>9</v>
+      </c>
+      <c r="C87">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3">
+      <c r="A88">
+        <v>98</v>
+      </c>
+      <c r="B88">
+        <v>10</v>
+      </c>
+      <c r="C88">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3">
+      <c r="A89">
+        <v>100</v>
+      </c>
+      <c r="B89">
+        <v>10</v>
+      </c>
+      <c r="C89">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3">
+      <c r="A90">
+        <v>101</v>
+      </c>
+      <c r="B90">
+        <v>10</v>
+      </c>
+      <c r="C90">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3">
+      <c r="A91">
+        <v>102</v>
+      </c>
+      <c r="B91">
+        <v>10</v>
+      </c>
+      <c r="C91">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3">
+      <c r="A92">
+        <v>103</v>
+      </c>
+      <c r="B92">
+        <v>10</v>
+      </c>
+      <c r="C92">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3">
+      <c r="A93">
+        <v>104</v>
+      </c>
+      <c r="B93">
+        <v>10</v>
+      </c>
+      <c r="C93">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3">
+      <c r="A94">
+        <v>105</v>
+      </c>
+      <c r="B94">
+        <v>11</v>
+      </c>
+      <c r="C94">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3">
+      <c r="A95">
+        <v>107</v>
+      </c>
+      <c r="B95">
+        <v>11</v>
+      </c>
+      <c r="C95">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3">
+      <c r="A96">
+        <v>108</v>
+      </c>
+      <c r="B96">
+        <v>11</v>
+      </c>
+      <c r="C96">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3">
+      <c r="A97">
+        <v>109</v>
+      </c>
+      <c r="B97">
+        <v>11</v>
+      </c>
+      <c r="C97">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3">
+      <c r="A98">
+        <v>110</v>
+      </c>
+      <c r="B98">
+        <v>11</v>
+      </c>
+      <c r="C98">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3">
+      <c r="A99">
+        <v>111</v>
+      </c>
+      <c r="B99">
+        <v>12</v>
+      </c>
+      <c r="C99">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3">
+      <c r="A100">
+        <v>113</v>
+      </c>
+      <c r="B100">
+        <v>12</v>
+      </c>
+      <c r="C100">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3">
+      <c r="A101">
+        <v>114</v>
+      </c>
+      <c r="B101">
+        <v>12</v>
+      </c>
+      <c r="C101">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="102" spans="1:3">
+      <c r="A102">
+        <v>115</v>
+      </c>
+      <c r="B102">
+        <v>12</v>
+      </c>
+      <c r="C102">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="103" spans="1:3">
+      <c r="A103">
+        <v>116</v>
+      </c>
+      <c r="B103">
+        <v>12</v>
+      </c>
+      <c r="C103">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="104" spans="1:3">
+      <c r="A104">
+        <v>117</v>
+      </c>
+      <c r="B104">
+        <v>12</v>
+      </c>
+      <c r="C104">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="105" spans="1:3">
+      <c r="A105">
+        <v>118</v>
+      </c>
+      <c r="B105">
+        <v>12</v>
+      </c>
+      <c r="C105">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="106" spans="1:3">
+      <c r="A106">
+        <v>119</v>
+      </c>
+      <c r="B106">
+        <v>12</v>
+      </c>
+      <c r="C106">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="107" spans="1:3">
+      <c r="A107">
+        <v>121</v>
+      </c>
+      <c r="B107">
+        <v>12</v>
+      </c>
+      <c r="C107">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="108" spans="1:3">
+      <c r="A108">
+        <v>122</v>
+      </c>
+      <c r="B108">
+        <v>13</v>
+      </c>
+      <c r="C108">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="109" spans="1:3">
+      <c r="A109">
+        <v>124</v>
+      </c>
+      <c r="B109">
+        <v>13</v>
+      </c>
+      <c r="C109">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="110" spans="1:3">
+      <c r="A110">
+        <v>125</v>
+      </c>
+      <c r="B110">
+        <v>13</v>
+      </c>
+      <c r="C110">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="111" spans="1:3">
+      <c r="A111">
+        <v>126</v>
+      </c>
+      <c r="B111">
+        <v>13</v>
+      </c>
+      <c r="C111">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="112" spans="1:3">
+      <c r="A112">
+        <v>127</v>
+      </c>
+      <c r="B112">
+        <v>13</v>
+      </c>
+      <c r="C112">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="113" spans="1:3">
+      <c r="A113">
+        <v>128</v>
+      </c>
+      <c r="B113">
+        <v>13</v>
+      </c>
+      <c r="C113">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="114" spans="1:3">
+      <c r="A114">
+        <v>129</v>
+      </c>
+      <c r="B114">
+        <v>13</v>
+      </c>
+      <c r="C114">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="115" spans="1:3">
+      <c r="A115">
+        <v>130</v>
+      </c>
+      <c r="B115">
+        <v>13</v>
+      </c>
+      <c r="C115">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="116" spans="1:3">
+      <c r="A116">
+        <v>131</v>
+      </c>
+      <c r="B116">
+        <v>13</v>
+      </c>
+      <c r="C116">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="117" spans="1:3">
+      <c r="A117">
+        <v>133</v>
+      </c>
+      <c r="B117">
+        <v>14</v>
+      </c>
+      <c r="C117">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="118" spans="1:3">
+      <c r="A118">
+        <v>135</v>
+      </c>
+      <c r="B118">
+        <v>14</v>
+      </c>
+      <c r="C118">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="119" spans="1:3">
+      <c r="A119">
+        <v>136</v>
+      </c>
+      <c r="B119">
+        <v>14</v>
+      </c>
+      <c r="C119">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="120" spans="1:3">
+      <c r="A120">
+        <v>137</v>
+      </c>
+      <c r="B120">
+        <v>14</v>
+      </c>
+      <c r="C120">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="121" spans="1:3">
+      <c r="A121">
+        <v>138</v>
+      </c>
+      <c r="B121">
+        <v>14</v>
+      </c>
+      <c r="C121">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="122" spans="1:3">
+      <c r="A122">
+        <v>139</v>
+      </c>
+      <c r="B122">
+        <v>14</v>
+      </c>
+      <c r="C122">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="123" spans="1:3">
+      <c r="A123">
+        <v>140</v>
+      </c>
+      <c r="B123">
+        <v>14</v>
+      </c>
+      <c r="C123">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="124" spans="1:3">
+      <c r="A124">
+        <v>141</v>
+      </c>
+      <c r="B124">
+        <v>14</v>
+      </c>
+      <c r="C124">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="125" spans="1:3">
+      <c r="A125">
+        <v>142</v>
+      </c>
+      <c r="B125">
+        <v>15</v>
+      </c>
+      <c r="C125">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="126" spans="1:3">
+      <c r="A126">
+        <v>144</v>
+      </c>
+      <c r="B126">
+        <v>15</v>
+      </c>
+      <c r="C126">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="127" spans="1:3">
+      <c r="A127">
+        <v>145</v>
+      </c>
+      <c r="B127">
+        <v>15</v>
+      </c>
+      <c r="C127">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="128" spans="1:3">
+      <c r="A128">
+        <v>146</v>
+      </c>
+      <c r="B128">
+        <v>15</v>
+      </c>
+      <c r="C128">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="129" spans="1:3">
+      <c r="A129">
+        <v>147</v>
+      </c>
+      <c r="B129">
+        <v>15</v>
+      </c>
+      <c r="C129">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="130" spans="1:3">
+      <c r="A130">
+        <v>148</v>
+      </c>
+      <c r="B130">
+        <v>15</v>
+      </c>
+      <c r="C130">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="131" spans="1:3">
+      <c r="A131">
+        <v>149</v>
+      </c>
+      <c r="B131">
+        <v>15</v>
+      </c>
+      <c r="C131">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="132" spans="1:3">
+      <c r="A132">
+        <v>150</v>
+      </c>
+      <c r="B132">
+        <v>4</v>
+      </c>
+      <c r="C132">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="133" spans="1:3">
+      <c r="A133">
+        <v>151</v>
+      </c>
+      <c r="B133">
+        <v>4</v>
+      </c>
+      <c r="C133">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="134" spans="1:3">
+      <c r="A134">
+        <v>154</v>
+      </c>
+      <c r="B134">
+        <v>4</v>
+      </c>
+      <c r="C134">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="135" spans="1:3">
+      <c r="A135">
+        <v>155</v>
+      </c>
+      <c r="B135">
+        <v>4</v>
+      </c>
+      <c r="C135">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="136" spans="1:3">
+      <c r="A136">
+        <v>156</v>
+      </c>
+      <c r="B136">
+        <v>4</v>
+      </c>
+      <c r="C136">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="137" spans="1:3">
+      <c r="A137">
+        <v>157</v>
+      </c>
+      <c r="B137">
+        <v>4</v>
+      </c>
+      <c r="C137">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="138" spans="1:3">
+      <c r="A138">
+        <v>159</v>
+      </c>
+      <c r="B138">
+        <v>1</v>
+      </c>
+      <c r="C138">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="139" spans="1:3">
+      <c r="A139">
+        <v>160</v>
+      </c>
+      <c r="B139">
+        <v>2</v>
+      </c>
+      <c r="C139">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="140" spans="1:3">
+      <c r="A140">
+        <v>161</v>
+      </c>
+      <c r="B140">
+        <v>3</v>
+      </c>
+      <c r="C140">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="141" spans="1:3">
+      <c r="A141">
+        <v>162</v>
+      </c>
+      <c r="B141">
+        <v>4</v>
+      </c>
+      <c r="C141">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="142" spans="1:3">
+      <c r="A142">
+        <v>163</v>
+      </c>
+      <c r="B142">
+        <v>5</v>
+      </c>
+      <c r="C142">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="143" spans="1:3">
+      <c r="A143">
+        <v>164</v>
+      </c>
+      <c r="B143">
+        <v>6</v>
+      </c>
+      <c r="C143">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="144" spans="1:3">
+      <c r="A144">
+        <v>165</v>
+      </c>
+      <c r="B144">
+        <v>7</v>
+      </c>
+      <c r="C144">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="145" spans="1:3">
+      <c r="A145">
+        <v>166</v>
+      </c>
+      <c r="B145">
+        <v>8</v>
+      </c>
+      <c r="C145">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="146" spans="1:3">
+      <c r="A146">
+        <v>167</v>
+      </c>
+      <c r="B146">
+        <v>9</v>
+      </c>
+      <c r="C146">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="147" spans="1:3">
+      <c r="A147">
+        <v>168</v>
+      </c>
+      <c r="B147">
+        <v>10</v>
+      </c>
+      <c r="C147">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="148" spans="1:3">
+      <c r="A148">
+        <v>169</v>
+      </c>
+      <c r="B148">
+        <v>11</v>
+      </c>
+      <c r="C148">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="149" spans="1:3">
+      <c r="A149">
+        <v>170</v>
+      </c>
+      <c r="B149">
+        <v>12</v>
+      </c>
+      <c r="C149">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="150" spans="1:3">
+      <c r="A150">
+        <v>171</v>
+      </c>
+      <c r="B150">
+        <v>13</v>
+      </c>
+      <c r="C150">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="151" spans="1:3">
+      <c r="A151">
+        <v>172</v>
+      </c>
+      <c r="B151">
+        <v>14</v>
+      </c>
+      <c r="C151">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="152" spans="1:3">
+      <c r="A152">
+        <v>173</v>
+      </c>
+      <c r="B152">
+        <v>15</v>
+      </c>
+      <c r="C152">
+        <v>17</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57805981-D162-4E30-B88F-BB8439796E51}">
   <sheetPr>
     <tabColor rgb="FFFF0000"/>
@@ -32013,7 +33740,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B7B1B9EE-67F1-4840-BF11-417278E68DBE}">
   <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
@@ -33294,7 +35021,7 @@
       </c>
     </row>
     <row r="30" spans="1:13" ht="48">
-      <c r="A30" s="61" t="s">
+      <c r="A30" s="63" t="s">
         <v>811</v>
       </c>
       <c r="B30" s="5" t="s">
@@ -33337,7 +35064,7 @@
       </c>
     </row>
     <row r="31" spans="1:13" ht="48">
-      <c r="A31" s="61"/>
+      <c r="A31" s="63"/>
       <c r="B31" s="5" t="s">
         <v>814</v>
       </c>
@@ -33378,7 +35105,7 @@
       </c>
     </row>
     <row r="32" spans="1:13" ht="32">
-      <c r="A32" s="61"/>
+      <c r="A32" s="63"/>
       <c r="B32" s="5" t="s">
         <v>816</v>
       </c>
@@ -33419,7 +35146,7 @@
       </c>
     </row>
     <row r="33" spans="1:13" ht="96">
-      <c r="A33" s="61"/>
+      <c r="A33" s="63"/>
       <c r="B33" s="5" t="s">
         <v>100</v>
       </c>
@@ -33460,7 +35187,7 @@
       </c>
     </row>
     <row r="34" spans="1:13" ht="32">
-      <c r="A34" s="61"/>
+      <c r="A34" s="63"/>
       <c r="B34" s="5" t="s">
         <v>819</v>
       </c>
@@ -33501,7 +35228,7 @@
       </c>
     </row>
     <row r="35" spans="1:13" ht="32">
-      <c r="A35" s="61"/>
+      <c r="A35" s="63"/>
       <c r="B35" s="5" t="s">
         <v>201</v>
       </c>
@@ -33542,7 +35269,7 @@
       </c>
     </row>
     <row r="36" spans="1:13" ht="80">
-      <c r="A36" s="61"/>
+      <c r="A36" s="63"/>
       <c r="B36" s="5" t="s">
         <v>822</v>
       </c>
@@ -34081,7 +35808,7 @@
       </c>
     </row>
     <row r="49" spans="1:13" ht="78" customHeight="1">
-      <c r="A49" s="61" t="s">
+      <c r="A49" s="63" t="s">
         <v>840</v>
       </c>
       <c r="B49" s="5" t="s">
@@ -34124,7 +35851,7 @@
       </c>
     </row>
     <row r="50" spans="1:13" ht="32">
-      <c r="A50" s="61"/>
+      <c r="A50" s="63"/>
       <c r="B50" s="5" t="s">
         <v>613</v>
       </c>
@@ -34165,7 +35892,7 @@
       </c>
     </row>
     <row r="51" spans="1:13" ht="16">
-      <c r="A51" s="61"/>
+      <c r="A51" s="63"/>
       <c r="B51" s="5" t="s">
         <v>201</v>
       </c>
@@ -34206,7 +35933,7 @@
       </c>
     </row>
     <row r="52" spans="1:13" ht="32">
-      <c r="A52" s="61"/>
+      <c r="A52" s="63"/>
       <c r="B52" s="5" t="s">
         <v>845</v>
       </c>
@@ -34247,7 +35974,7 @@
       </c>
     </row>
     <row r="53" spans="1:13" ht="96">
-      <c r="A53" s="61"/>
+      <c r="A53" s="63"/>
       <c r="B53" s="5" t="s">
         <v>847</v>
       </c>
@@ -34288,7 +36015,7 @@
       </c>
     </row>
     <row r="54" spans="1:13">
-      <c r="A54" s="61"/>
+      <c r="A54" s="63"/>
       <c r="B54" s="5" t="s">
         <v>849</v>
       </c>
@@ -34329,7 +36056,7 @@
       </c>
     </row>
     <row r="55" spans="1:13" ht="64">
-      <c r="A55" s="61"/>
+      <c r="A55" s="63"/>
       <c r="B55" s="5" t="s">
         <v>851</v>
       </c>
@@ -34370,7 +36097,7 @@
       </c>
     </row>
     <row r="56" spans="1:13" ht="64">
-      <c r="A56" s="61"/>
+      <c r="A56" s="63"/>
       <c r="B56" s="5" t="s">
         <v>853</v>
       </c>
@@ -34411,7 +36138,7 @@
       </c>
     </row>
     <row r="57" spans="1:13" ht="32">
-      <c r="A57" s="62" t="s">
+      <c r="A57" s="61" t="s">
         <v>855</v>
       </c>
       <c r="B57" s="6" t="s">
@@ -34453,7 +36180,7 @@
       </c>
     </row>
     <row r="58" spans="1:13" ht="80">
-      <c r="A58" s="62"/>
+      <c r="A58" s="61"/>
       <c r="B58" s="7" t="s">
         <v>858</v>
       </c>
@@ -34493,7 +36220,7 @@
       </c>
     </row>
     <row r="59" spans="1:13" ht="64" customHeight="1">
-      <c r="A59" s="62"/>
+      <c r="A59" s="61"/>
       <c r="B59" s="7" t="s">
         <v>860</v>
       </c>
@@ -34533,7 +36260,7 @@
       </c>
     </row>
     <row r="60" spans="1:13" ht="16">
-      <c r="A60" s="62"/>
+      <c r="A60" s="61"/>
       <c r="B60" s="7" t="s">
         <v>95</v>
       </c>
@@ -34573,7 +36300,7 @@
       </c>
     </row>
     <row r="61" spans="1:13" ht="32">
-      <c r="A61" s="62"/>
+      <c r="A61" s="61"/>
       <c r="B61" s="7" t="s">
         <v>864</v>
       </c>
@@ -34613,7 +36340,7 @@
       </c>
     </row>
     <row r="62" spans="1:13" ht="32">
-      <c r="A62" s="62"/>
+      <c r="A62" s="61"/>
       <c r="B62" s="7" t="s">
         <v>866</v>
       </c>
@@ -34653,7 +36380,7 @@
       </c>
     </row>
     <row r="63" spans="1:13" ht="16">
-      <c r="A63" s="62"/>
+      <c r="A63" s="61"/>
       <c r="B63" s="7" t="s">
         <v>869</v>
       </c>
@@ -34693,7 +36420,7 @@
       </c>
     </row>
     <row r="64" spans="1:13" ht="32">
-      <c r="A64" s="62"/>
+      <c r="A64" s="61"/>
       <c r="B64" s="6" t="s">
         <v>871</v>
       </c>
@@ -34733,7 +36460,7 @@
       </c>
     </row>
     <row r="65" spans="1:13" ht="16">
-      <c r="A65" s="62"/>
+      <c r="A65" s="61"/>
       <c r="B65" s="7" t="s">
         <v>82</v>
       </c>
@@ -34773,7 +36500,7 @@
       </c>
     </row>
     <row r="66" spans="1:13" ht="16">
-      <c r="A66" s="62"/>
+      <c r="A66" s="61"/>
       <c r="B66" s="7" t="s">
         <v>874</v>
       </c>
@@ -34813,7 +36540,7 @@
       </c>
     </row>
     <row r="67" spans="1:13" ht="48">
-      <c r="A67" s="62"/>
+      <c r="A67" s="61"/>
       <c r="B67" s="6" t="s">
         <v>92</v>
       </c>
@@ -34853,38 +36580,38 @@
       </c>
     </row>
     <row r="68" spans="1:13" ht="16">
-      <c r="A68" s="62"/>
-      <c r="B68" s="62" t="s">
+      <c r="A68" s="61"/>
+      <c r="B68" s="61" t="s">
         <v>169</v>
       </c>
       <c r="C68" s="6" t="s">
         <v>876</v>
       </c>
-      <c r="D68" s="62" t="s">
+      <c r="D68" s="61" t="s">
         <v>27</v>
       </c>
-      <c r="E68" s="62" t="s">
+      <c r="E68" s="61" t="s">
         <v>862</v>
       </c>
-      <c r="F68" s="62" t="s">
-        <v>23</v>
-      </c>
-      <c r="G68" s="62" t="s">
+      <c r="F68" s="61" t="s">
+        <v>23</v>
+      </c>
+      <c r="G68" s="61" t="s">
         <v>23</v>
       </c>
       <c r="H68" s="60" t="s">
         <v>23</v>
       </c>
-      <c r="I68" s="62" t="s">
+      <c r="I68" s="61" t="s">
         <v>181</v>
       </c>
-      <c r="J68" s="62" t="s">
-        <v>23</v>
-      </c>
-      <c r="K68" s="62" t="s">
-        <v>23</v>
-      </c>
-      <c r="L68" s="62" t="s">
+      <c r="J68" s="61" t="s">
+        <v>23</v>
+      </c>
+      <c r="K68" s="61" t="s">
+        <v>23</v>
+      </c>
+      <c r="L68" s="61" t="s">
         <v>84</v>
       </c>
       <c r="M68" s="60" t="str">
@@ -34893,24 +36620,24 @@
       </c>
     </row>
     <row r="69" spans="1:13" ht="16">
-      <c r="A69" s="62"/>
-      <c r="B69" s="62"/>
+      <c r="A69" s="61"/>
+      <c r="B69" s="61"/>
       <c r="C69" s="6" t="s">
         <v>877</v>
       </c>
-      <c r="D69" s="62"/>
-      <c r="E69" s="62"/>
-      <c r="F69" s="62"/>
-      <c r="G69" s="62"/>
+      <c r="D69" s="61"/>
+      <c r="E69" s="61"/>
+      <c r="F69" s="61"/>
+      <c r="G69" s="61"/>
       <c r="H69" s="60"/>
-      <c r="I69" s="62"/>
-      <c r="J69" s="62"/>
-      <c r="K69" s="62"/>
-      <c r="L69" s="62"/>
+      <c r="I69" s="61"/>
+      <c r="J69" s="61"/>
+      <c r="K69" s="61"/>
+      <c r="L69" s="61"/>
       <c r="M69" s="60"/>
     </row>
     <row r="70" spans="1:13" ht="28">
-      <c r="A70" s="63" t="s">
+      <c r="A70" s="62" t="s">
         <v>878</v>
       </c>
       <c r="B70" s="16" t="s">
@@ -34956,7 +36683,7 @@
       </c>
     </row>
     <row r="71" spans="1:13" ht="51">
-      <c r="A71" s="63"/>
+      <c r="A71" s="62"/>
       <c r="B71" s="16" t="s">
         <v>100</v>
       </c>
@@ -35000,7 +36727,7 @@
       </c>
     </row>
     <row r="72" spans="1:13" ht="28">
-      <c r="A72" s="63"/>
+      <c r="A72" s="62"/>
       <c r="B72" s="16" t="s">
         <v>763</v>
       </c>
@@ -35044,7 +36771,7 @@
       </c>
     </row>
     <row r="73" spans="1:13" ht="28">
-      <c r="A73" s="63"/>
+      <c r="A73" s="62"/>
       <c r="B73" s="16" t="s">
         <v>885</v>
       </c>
@@ -35606,6 +37333,15 @@
     </row>
   </sheetData>
   <mergeCells count="23">
+    <mergeCell ref="A2:A7"/>
+    <mergeCell ref="A8:A14"/>
+    <mergeCell ref="A25:A29"/>
+    <mergeCell ref="A15:A24"/>
+    <mergeCell ref="A49:A56"/>
+    <mergeCell ref="A44:A48"/>
+    <mergeCell ref="A41:A43"/>
+    <mergeCell ref="A30:A36"/>
+    <mergeCell ref="A37:A40"/>
     <mergeCell ref="M68:M69"/>
     <mergeCell ref="H68:H69"/>
     <mergeCell ref="A74:A85"/>
@@ -35620,15 +37356,6 @@
     <mergeCell ref="B68:B69"/>
     <mergeCell ref="D68:D69"/>
     <mergeCell ref="E68:E69"/>
-    <mergeCell ref="A2:A7"/>
-    <mergeCell ref="A8:A14"/>
-    <mergeCell ref="A25:A29"/>
-    <mergeCell ref="A15:A24"/>
-    <mergeCell ref="A49:A56"/>
-    <mergeCell ref="A44:A48"/>
-    <mergeCell ref="A41:A43"/>
-    <mergeCell ref="A30:A36"/>
-    <mergeCell ref="A37:A40"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -37607,6 +39334,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <lcf76f155ced4ddcb4097134ff3c332f xmlns="633f040f-4953-46e7-8610-82b0c5296ba0">
@@ -37660,15 +39396,6 @@
     <Invited_Students xmlns="633f040f-4953-46e7-8610-82b0c5296ba0" xsi:nil="true"/>
   </documentManagement>
 </p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -38089,6 +39816,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2C6CC7BA-2E2C-4B0D-8103-11A51D82E8EC}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{83D5100D-0E56-4B30-B42D-2AEC6B837C39}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
@@ -38101,14 +39836,6 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <ds:schemaRef ds:uri="633f040f-4953-46e7-8610-82b0c5296ba0"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2C6CC7BA-2E2C-4B0D-8103-11A51D82E8EC}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
aggiunto js per macm_riskRating
</commit_message>
<xml_diff>
--- a/apps/static/assets/dbs/ThreatCatalogComplete.xlsx
+++ b/apps/static/assets/dbs/ThreatCatalogComplete.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fefox/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE7E0C08-BAEB-4049-BA08-75AC14A77107}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F683730-BBD2-1D44-9CA6-D0BA905A95A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16300" firstSheet="2" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16280" firstSheet="3" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Threat Components" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
     <sheet name="Tools" sheetId="6" r:id="rId6"/>
     <sheet name="Pentest Phases" sheetId="7" r:id="rId7"/>
     <sheet name="ThreatAgentQuestions" sheetId="8" r:id="rId8"/>
-    <sheet name="ThreatAgentReply" sheetId="13" r:id="rId9"/>
+    <sheet name="ThreatAgentQuestionReplies" sheetId="13" r:id="rId9"/>
     <sheet name="ThreatAgentCategory" sheetId="9" r:id="rId10"/>
     <sheet name="ThreatAgentReplyCategory" sheetId="15" r:id="rId11"/>
     <sheet name="ThreatAgentAttribute" sheetId="12" r:id="rId12"/>
@@ -32,7 +32,7 @@
   </definedNames>
   <calcPr calcId="191028"/>
   <pivotCaches>
-    <pivotCache cacheId="1" r:id="rId13"/>
+    <pivotCache cacheId="3" r:id="rId13"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -4691,14 +4691,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -9811,7 +9811,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{48CB07D6-9F6C-094F-A3D3-916741F281CD}" name="Tabella pivot1" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valori" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{48CB07D6-9F6C-094F-A3D3-916741F281CD}" name="Tabella pivot1" cacheId="3" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valori" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A1:B25" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="14">
     <pivotField showAll="0"/>
@@ -31447,7 +31447,7 @@
   </sheetPr>
   <dimension ref="A1:C152"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="200" workbookViewId="0">
+    <sheetView zoomScale="200" workbookViewId="0">
       <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
@@ -35021,7 +35021,7 @@
       </c>
     </row>
     <row r="30" spans="1:13" ht="48">
-      <c r="A30" s="63" t="s">
+      <c r="A30" s="61" t="s">
         <v>811</v>
       </c>
       <c r="B30" s="5" t="s">
@@ -35064,7 +35064,7 @@
       </c>
     </row>
     <row r="31" spans="1:13" ht="48">
-      <c r="A31" s="63"/>
+      <c r="A31" s="61"/>
       <c r="B31" s="5" t="s">
         <v>814</v>
       </c>
@@ -35105,7 +35105,7 @@
       </c>
     </row>
     <row r="32" spans="1:13" ht="32">
-      <c r="A32" s="63"/>
+      <c r="A32" s="61"/>
       <c r="B32" s="5" t="s">
         <v>816</v>
       </c>
@@ -35146,7 +35146,7 @@
       </c>
     </row>
     <row r="33" spans="1:13" ht="96">
-      <c r="A33" s="63"/>
+      <c r="A33" s="61"/>
       <c r="B33" s="5" t="s">
         <v>100</v>
       </c>
@@ -35187,7 +35187,7 @@
       </c>
     </row>
     <row r="34" spans="1:13" ht="32">
-      <c r="A34" s="63"/>
+      <c r="A34" s="61"/>
       <c r="B34" s="5" t="s">
         <v>819</v>
       </c>
@@ -35228,7 +35228,7 @@
       </c>
     </row>
     <row r="35" spans="1:13" ht="32">
-      <c r="A35" s="63"/>
+      <c r="A35" s="61"/>
       <c r="B35" s="5" t="s">
         <v>201</v>
       </c>
@@ -35269,7 +35269,7 @@
       </c>
     </row>
     <row r="36" spans="1:13" ht="80">
-      <c r="A36" s="63"/>
+      <c r="A36" s="61"/>
       <c r="B36" s="5" t="s">
         <v>822</v>
       </c>
@@ -35808,7 +35808,7 @@
       </c>
     </row>
     <row r="49" spans="1:13" ht="78" customHeight="1">
-      <c r="A49" s="63" t="s">
+      <c r="A49" s="61" t="s">
         <v>840</v>
       </c>
       <c r="B49" s="5" t="s">
@@ -35851,7 +35851,7 @@
       </c>
     </row>
     <row r="50" spans="1:13" ht="32">
-      <c r="A50" s="63"/>
+      <c r="A50" s="61"/>
       <c r="B50" s="5" t="s">
         <v>613</v>
       </c>
@@ -35892,7 +35892,7 @@
       </c>
     </row>
     <row r="51" spans="1:13" ht="16">
-      <c r="A51" s="63"/>
+      <c r="A51" s="61"/>
       <c r="B51" s="5" t="s">
         <v>201</v>
       </c>
@@ -35933,7 +35933,7 @@
       </c>
     </row>
     <row r="52" spans="1:13" ht="32">
-      <c r="A52" s="63"/>
+      <c r="A52" s="61"/>
       <c r="B52" s="5" t="s">
         <v>845</v>
       </c>
@@ -35974,7 +35974,7 @@
       </c>
     </row>
     <row r="53" spans="1:13" ht="96">
-      <c r="A53" s="63"/>
+      <c r="A53" s="61"/>
       <c r="B53" s="5" t="s">
         <v>847</v>
       </c>
@@ -36015,7 +36015,7 @@
       </c>
     </row>
     <row r="54" spans="1:13">
-      <c r="A54" s="63"/>
+      <c r="A54" s="61"/>
       <c r="B54" s="5" t="s">
         <v>849</v>
       </c>
@@ -36056,7 +36056,7 @@
       </c>
     </row>
     <row r="55" spans="1:13" ht="64">
-      <c r="A55" s="63"/>
+      <c r="A55" s="61"/>
       <c r="B55" s="5" t="s">
         <v>851</v>
       </c>
@@ -36097,7 +36097,7 @@
       </c>
     </row>
     <row r="56" spans="1:13" ht="64">
-      <c r="A56" s="63"/>
+      <c r="A56" s="61"/>
       <c r="B56" s="5" t="s">
         <v>853</v>
       </c>
@@ -36138,7 +36138,7 @@
       </c>
     </row>
     <row r="57" spans="1:13" ht="32">
-      <c r="A57" s="61" t="s">
+      <c r="A57" s="62" t="s">
         <v>855</v>
       </c>
       <c r="B57" s="6" t="s">
@@ -36180,7 +36180,7 @@
       </c>
     </row>
     <row r="58" spans="1:13" ht="80">
-      <c r="A58" s="61"/>
+      <c r="A58" s="62"/>
       <c r="B58" s="7" t="s">
         <v>858</v>
       </c>
@@ -36220,7 +36220,7 @@
       </c>
     </row>
     <row r="59" spans="1:13" ht="64" customHeight="1">
-      <c r="A59" s="61"/>
+      <c r="A59" s="62"/>
       <c r="B59" s="7" t="s">
         <v>860</v>
       </c>
@@ -36260,7 +36260,7 @@
       </c>
     </row>
     <row r="60" spans="1:13" ht="16">
-      <c r="A60" s="61"/>
+      <c r="A60" s="62"/>
       <c r="B60" s="7" t="s">
         <v>95</v>
       </c>
@@ -36300,7 +36300,7 @@
       </c>
     </row>
     <row r="61" spans="1:13" ht="32">
-      <c r="A61" s="61"/>
+      <c r="A61" s="62"/>
       <c r="B61" s="7" t="s">
         <v>864</v>
       </c>
@@ -36340,7 +36340,7 @@
       </c>
     </row>
     <row r="62" spans="1:13" ht="32">
-      <c r="A62" s="61"/>
+      <c r="A62" s="62"/>
       <c r="B62" s="7" t="s">
         <v>866</v>
       </c>
@@ -36380,7 +36380,7 @@
       </c>
     </row>
     <row r="63" spans="1:13" ht="16">
-      <c r="A63" s="61"/>
+      <c r="A63" s="62"/>
       <c r="B63" s="7" t="s">
         <v>869</v>
       </c>
@@ -36420,7 +36420,7 @@
       </c>
     </row>
     <row r="64" spans="1:13" ht="32">
-      <c r="A64" s="61"/>
+      <c r="A64" s="62"/>
       <c r="B64" s="6" t="s">
         <v>871</v>
       </c>
@@ -36460,7 +36460,7 @@
       </c>
     </row>
     <row r="65" spans="1:13" ht="16">
-      <c r="A65" s="61"/>
+      <c r="A65" s="62"/>
       <c r="B65" s="7" t="s">
         <v>82</v>
       </c>
@@ -36500,7 +36500,7 @@
       </c>
     </row>
     <row r="66" spans="1:13" ht="16">
-      <c r="A66" s="61"/>
+      <c r="A66" s="62"/>
       <c r="B66" s="7" t="s">
         <v>874</v>
       </c>
@@ -36540,7 +36540,7 @@
       </c>
     </row>
     <row r="67" spans="1:13" ht="48">
-      <c r="A67" s="61"/>
+      <c r="A67" s="62"/>
       <c r="B67" s="6" t="s">
         <v>92</v>
       </c>
@@ -36580,38 +36580,38 @@
       </c>
     </row>
     <row r="68" spans="1:13" ht="16">
-      <c r="A68" s="61"/>
-      <c r="B68" s="61" t="s">
+      <c r="A68" s="62"/>
+      <c r="B68" s="62" t="s">
         <v>169</v>
       </c>
       <c r="C68" s="6" t="s">
         <v>876</v>
       </c>
-      <c r="D68" s="61" t="s">
+      <c r="D68" s="62" t="s">
         <v>27</v>
       </c>
-      <c r="E68" s="61" t="s">
+      <c r="E68" s="62" t="s">
         <v>862</v>
       </c>
-      <c r="F68" s="61" t="s">
-        <v>23</v>
-      </c>
-      <c r="G68" s="61" t="s">
+      <c r="F68" s="62" t="s">
+        <v>23</v>
+      </c>
+      <c r="G68" s="62" t="s">
         <v>23</v>
       </c>
       <c r="H68" s="60" t="s">
         <v>23</v>
       </c>
-      <c r="I68" s="61" t="s">
+      <c r="I68" s="62" t="s">
         <v>181</v>
       </c>
-      <c r="J68" s="61" t="s">
-        <v>23</v>
-      </c>
-      <c r="K68" s="61" t="s">
-        <v>23</v>
-      </c>
-      <c r="L68" s="61" t="s">
+      <c r="J68" s="62" t="s">
+        <v>23</v>
+      </c>
+      <c r="K68" s="62" t="s">
+        <v>23</v>
+      </c>
+      <c r="L68" s="62" t="s">
         <v>84</v>
       </c>
       <c r="M68" s="60" t="str">
@@ -36620,24 +36620,24 @@
       </c>
     </row>
     <row r="69" spans="1:13" ht="16">
-      <c r="A69" s="61"/>
-      <c r="B69" s="61"/>
+      <c r="A69" s="62"/>
+      <c r="B69" s="62"/>
       <c r="C69" s="6" t="s">
         <v>877</v>
       </c>
-      <c r="D69" s="61"/>
-      <c r="E69" s="61"/>
-      <c r="F69" s="61"/>
-      <c r="G69" s="61"/>
+      <c r="D69" s="62"/>
+      <c r="E69" s="62"/>
+      <c r="F69" s="62"/>
+      <c r="G69" s="62"/>
       <c r="H69" s="60"/>
-      <c r="I69" s="61"/>
-      <c r="J69" s="61"/>
-      <c r="K69" s="61"/>
-      <c r="L69" s="61"/>
+      <c r="I69" s="62"/>
+      <c r="J69" s="62"/>
+      <c r="K69" s="62"/>
+      <c r="L69" s="62"/>
       <c r="M69" s="60"/>
     </row>
     <row r="70" spans="1:13" ht="28">
-      <c r="A70" s="62" t="s">
+      <c r="A70" s="63" t="s">
         <v>878</v>
       </c>
       <c r="B70" s="16" t="s">
@@ -36683,7 +36683,7 @@
       </c>
     </row>
     <row r="71" spans="1:13" ht="51">
-      <c r="A71" s="62"/>
+      <c r="A71" s="63"/>
       <c r="B71" s="16" t="s">
         <v>100</v>
       </c>
@@ -36727,7 +36727,7 @@
       </c>
     </row>
     <row r="72" spans="1:13" ht="28">
-      <c r="A72" s="62"/>
+      <c r="A72" s="63"/>
       <c r="B72" s="16" t="s">
         <v>763</v>
       </c>
@@ -36771,7 +36771,7 @@
       </c>
     </row>
     <row r="73" spans="1:13" ht="28">
-      <c r="A73" s="62"/>
+      <c r="A73" s="63"/>
       <c r="B73" s="16" t="s">
         <v>885</v>
       </c>
@@ -37333,15 +37333,6 @@
     </row>
   </sheetData>
   <mergeCells count="23">
-    <mergeCell ref="A2:A7"/>
-    <mergeCell ref="A8:A14"/>
-    <mergeCell ref="A25:A29"/>
-    <mergeCell ref="A15:A24"/>
-    <mergeCell ref="A49:A56"/>
-    <mergeCell ref="A44:A48"/>
-    <mergeCell ref="A41:A43"/>
-    <mergeCell ref="A30:A36"/>
-    <mergeCell ref="A37:A40"/>
     <mergeCell ref="M68:M69"/>
     <mergeCell ref="H68:H69"/>
     <mergeCell ref="A74:A85"/>
@@ -37356,6 +37347,15 @@
     <mergeCell ref="B68:B69"/>
     <mergeCell ref="D68:D69"/>
     <mergeCell ref="E68:E69"/>
+    <mergeCell ref="A2:A7"/>
+    <mergeCell ref="A8:A14"/>
+    <mergeCell ref="A25:A29"/>
+    <mergeCell ref="A15:A24"/>
+    <mergeCell ref="A49:A56"/>
+    <mergeCell ref="A44:A48"/>
+    <mergeCell ref="A41:A43"/>
+    <mergeCell ref="A30:A36"/>
+    <mergeCell ref="A37:A40"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -39142,7 +39142,7 @@
   </sheetPr>
   <dimension ref="A1:C16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
@@ -39334,71 +39334,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="633f040f-4953-46e7-8610-82b0c5296ba0">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="f62ef740-d444-4f18-80a2-7590fdcab1ce" xsi:nil="true"/>
-    <Has_Teacher_Only_SectionGroup xmlns="633f040f-4953-46e7-8610-82b0c5296ba0" xsi:nil="true"/>
-    <Teachers xmlns="633f040f-4953-46e7-8610-82b0c5296ba0">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </Teachers>
-    <IsNotebookLocked xmlns="633f040f-4953-46e7-8610-82b0c5296ba0" xsi:nil="true"/>
-    <CultureName xmlns="633f040f-4953-46e7-8610-82b0c5296ba0" xsi:nil="true"/>
-    <Owner xmlns="633f040f-4953-46e7-8610-82b0c5296ba0">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </Owner>
-    <Distribution_Groups xmlns="633f040f-4953-46e7-8610-82b0c5296ba0" xsi:nil="true"/>
-    <TeamsChannelId xmlns="633f040f-4953-46e7-8610-82b0c5296ba0" xsi:nil="true"/>
-    <Invited_Teachers xmlns="633f040f-4953-46e7-8610-82b0c5296ba0" xsi:nil="true"/>
-    <NotebookType xmlns="633f040f-4953-46e7-8610-82b0c5296ba0" xsi:nil="true"/>
-    <AppVersion xmlns="633f040f-4953-46e7-8610-82b0c5296ba0" xsi:nil="true"/>
-    <DefaultSectionNames xmlns="633f040f-4953-46e7-8610-82b0c5296ba0" xsi:nil="true"/>
-    <Is_Collaboration_Space_Locked xmlns="633f040f-4953-46e7-8610-82b0c5296ba0" xsi:nil="true"/>
-    <Templates xmlns="633f040f-4953-46e7-8610-82b0c5296ba0" xsi:nil="true"/>
-    <FolderType xmlns="633f040f-4953-46e7-8610-82b0c5296ba0" xsi:nil="true"/>
-    <Student_Groups xmlns="633f040f-4953-46e7-8610-82b0c5296ba0">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </Student_Groups>
-    <Teams_Channel_Section_Location xmlns="633f040f-4953-46e7-8610-82b0c5296ba0" xsi:nil="true"/>
-    <Math_Settings xmlns="633f040f-4953-46e7-8610-82b0c5296ba0" xsi:nil="true"/>
-    <Self_Registration_Enabled xmlns="633f040f-4953-46e7-8610-82b0c5296ba0" xsi:nil="true"/>
-    <Students xmlns="633f040f-4953-46e7-8610-82b0c5296ba0">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </Students>
-    <LMS_Mappings xmlns="633f040f-4953-46e7-8610-82b0c5296ba0" xsi:nil="true"/>
-    <Invited_Students xmlns="633f040f-4953-46e7-8610-82b0c5296ba0" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x0101009A9CE0B21D9C3A45B31425227616CD6F" ma:contentTypeVersion="34" ma:contentTypeDescription="Creare un nuovo documento." ma:contentTypeScope="" ma:versionID="8a882b22c4c6ceab40c069a6a2420ef3">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="633f040f-4953-46e7-8610-82b0c5296ba0" xmlns:ns3="f62ef740-d444-4f18-80a2-7590fdcab1ce" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="77035a69dc4d6b80a35ec1b02b2030a4" ns2:_="" ns3:_="">
     <xsd:import namespace="633f040f-4953-46e7-8610-82b0c5296ba0"/>
@@ -39815,10 +39750,86 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="633f040f-4953-46e7-8610-82b0c5296ba0">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="f62ef740-d444-4f18-80a2-7590fdcab1ce" xsi:nil="true"/>
+    <Has_Teacher_Only_SectionGroup xmlns="633f040f-4953-46e7-8610-82b0c5296ba0" xsi:nil="true"/>
+    <Teachers xmlns="633f040f-4953-46e7-8610-82b0c5296ba0">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </Teachers>
+    <IsNotebookLocked xmlns="633f040f-4953-46e7-8610-82b0c5296ba0" xsi:nil="true"/>
+    <CultureName xmlns="633f040f-4953-46e7-8610-82b0c5296ba0" xsi:nil="true"/>
+    <Owner xmlns="633f040f-4953-46e7-8610-82b0c5296ba0">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </Owner>
+    <Distribution_Groups xmlns="633f040f-4953-46e7-8610-82b0c5296ba0" xsi:nil="true"/>
+    <TeamsChannelId xmlns="633f040f-4953-46e7-8610-82b0c5296ba0" xsi:nil="true"/>
+    <Invited_Teachers xmlns="633f040f-4953-46e7-8610-82b0c5296ba0" xsi:nil="true"/>
+    <NotebookType xmlns="633f040f-4953-46e7-8610-82b0c5296ba0" xsi:nil="true"/>
+    <AppVersion xmlns="633f040f-4953-46e7-8610-82b0c5296ba0" xsi:nil="true"/>
+    <DefaultSectionNames xmlns="633f040f-4953-46e7-8610-82b0c5296ba0" xsi:nil="true"/>
+    <Is_Collaboration_Space_Locked xmlns="633f040f-4953-46e7-8610-82b0c5296ba0" xsi:nil="true"/>
+    <Templates xmlns="633f040f-4953-46e7-8610-82b0c5296ba0" xsi:nil="true"/>
+    <FolderType xmlns="633f040f-4953-46e7-8610-82b0c5296ba0" xsi:nil="true"/>
+    <Student_Groups xmlns="633f040f-4953-46e7-8610-82b0c5296ba0">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </Student_Groups>
+    <Teams_Channel_Section_Location xmlns="633f040f-4953-46e7-8610-82b0c5296ba0" xsi:nil="true"/>
+    <Math_Settings xmlns="633f040f-4953-46e7-8610-82b0c5296ba0" xsi:nil="true"/>
+    <Self_Registration_Enabled xmlns="633f040f-4953-46e7-8610-82b0c5296ba0" xsi:nil="true"/>
+    <Students xmlns="633f040f-4953-46e7-8610-82b0c5296ba0">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </Students>
+    <LMS_Mappings xmlns="633f040f-4953-46e7-8610-82b0c5296ba0" xsi:nil="true"/>
+    <Invited_Students xmlns="633f040f-4953-46e7-8610-82b0c5296ba0" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2C6CC7BA-2E2C-4B0D-8103-11A51D82E8EC}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{36C20BFB-BCC5-4457-BE44-22D2F12F84BE}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="633f040f-4953-46e7-8610-82b0c5296ba0"/>
+    <ds:schemaRef ds:uri="f62ef740-d444-4f18-80a2-7590fdcab1ce"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -39841,20 +39852,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{36C20BFB-BCC5-4457-BE44-22D2F12F84BE}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2C6CC7BA-2E2C-4B0D-8103-11A51D82E8EC}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="633f040f-4953-46e7-8610-82b0c5296ba0"/>
-    <ds:schemaRef ds:uri="f62ef740-d444-4f18-80a2-7590fdcab1ce"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
risolto bug del calcolo del rischio complessivo
</commit_message>
<xml_diff>
--- a/apps/static/assets/dbs/ThreatCatalogComplete.xlsx
+++ b/apps/static/assets/dbs/ThreatCatalogComplete.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/danielegranata/PycharmProjects/AutomaticAttackPlanGenerator/apps/static/assets/dbs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D388EA8A-96E6-4841-9140-7F3A5759AC1C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4E930D1-469C-4441-BFB8-499CE6D1B9B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="880" windowWidth="36000" windowHeight="21020" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
   </definedNames>
   <calcPr calcId="191028"/>
   <pivotCaches>
-    <pivotCache cacheId="2" r:id="rId12"/>
+    <pivotCache cacheId="3" r:id="rId12"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -4156,14 +4156,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -9302,7 +9302,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{48CB07D6-9F6C-094F-A3D3-916741F281CD}" name="Tabella pivot1" cacheId="2" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valori" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{48CB07D6-9F6C-094F-A3D3-916741F281CD}" name="Tabella pivot1" cacheId="3" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valori" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A1:B25" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="14">
     <pivotField showAll="0"/>
@@ -33824,7 +33824,7 @@
       </c>
     </row>
     <row r="30" spans="1:13" ht="48">
-      <c r="A30" s="54" t="s">
+      <c r="A30" s="56" t="s">
         <v>811</v>
       </c>
       <c r="B30" s="5" t="s">
@@ -33867,7 +33867,7 @@
       </c>
     </row>
     <row r="31" spans="1:13" ht="48">
-      <c r="A31" s="54"/>
+      <c r="A31" s="56"/>
       <c r="B31" s="5" t="s">
         <v>814</v>
       </c>
@@ -33908,7 +33908,7 @@
       </c>
     </row>
     <row r="32" spans="1:13" ht="32">
-      <c r="A32" s="54"/>
+      <c r="A32" s="56"/>
       <c r="B32" s="5" t="s">
         <v>816</v>
       </c>
@@ -33949,7 +33949,7 @@
       </c>
     </row>
     <row r="33" spans="1:13" ht="96">
-      <c r="A33" s="54"/>
+      <c r="A33" s="56"/>
       <c r="B33" s="5" t="s">
         <v>100</v>
       </c>
@@ -33990,7 +33990,7 @@
       </c>
     </row>
     <row r="34" spans="1:13" ht="32">
-      <c r="A34" s="54"/>
+      <c r="A34" s="56"/>
       <c r="B34" s="5" t="s">
         <v>819</v>
       </c>
@@ -34031,7 +34031,7 @@
       </c>
     </row>
     <row r="35" spans="1:13" ht="32">
-      <c r="A35" s="54"/>
+      <c r="A35" s="56"/>
       <c r="B35" s="5" t="s">
         <v>201</v>
       </c>
@@ -34072,7 +34072,7 @@
       </c>
     </row>
     <row r="36" spans="1:13" ht="80">
-      <c r="A36" s="54"/>
+      <c r="A36" s="56"/>
       <c r="B36" s="5" t="s">
         <v>822</v>
       </c>
@@ -34611,7 +34611,7 @@
       </c>
     </row>
     <row r="49" spans="1:13" ht="78" customHeight="1">
-      <c r="A49" s="54" t="s">
+      <c r="A49" s="56" t="s">
         <v>840</v>
       </c>
       <c r="B49" s="5" t="s">
@@ -34654,7 +34654,7 @@
       </c>
     </row>
     <row r="50" spans="1:13" ht="32">
-      <c r="A50" s="54"/>
+      <c r="A50" s="56"/>
       <c r="B50" s="5" t="s">
         <v>613</v>
       </c>
@@ -34695,7 +34695,7 @@
       </c>
     </row>
     <row r="51" spans="1:13" ht="16">
-      <c r="A51" s="54"/>
+      <c r="A51" s="56"/>
       <c r="B51" s="5" t="s">
         <v>201</v>
       </c>
@@ -34736,7 +34736,7 @@
       </c>
     </row>
     <row r="52" spans="1:13" ht="32">
-      <c r="A52" s="54"/>
+      <c r="A52" s="56"/>
       <c r="B52" s="5" t="s">
         <v>845</v>
       </c>
@@ -34777,7 +34777,7 @@
       </c>
     </row>
     <row r="53" spans="1:13" ht="96">
-      <c r="A53" s="54"/>
+      <c r="A53" s="56"/>
       <c r="B53" s="5" t="s">
         <v>847</v>
       </c>
@@ -34818,7 +34818,7 @@
       </c>
     </row>
     <row r="54" spans="1:13">
-      <c r="A54" s="54"/>
+      <c r="A54" s="56"/>
       <c r="B54" s="5" t="s">
         <v>849</v>
       </c>
@@ -34859,7 +34859,7 @@
       </c>
     </row>
     <row r="55" spans="1:13" ht="64">
-      <c r="A55" s="54"/>
+      <c r="A55" s="56"/>
       <c r="B55" s="5" t="s">
         <v>851</v>
       </c>
@@ -34900,7 +34900,7 @@
       </c>
     </row>
     <row r="56" spans="1:13" ht="64">
-      <c r="A56" s="54"/>
+      <c r="A56" s="56"/>
       <c r="B56" s="5" t="s">
         <v>853</v>
       </c>
@@ -34941,7 +34941,7 @@
       </c>
     </row>
     <row r="57" spans="1:13" ht="32">
-      <c r="A57" s="55" t="s">
+      <c r="A57" s="54" t="s">
         <v>855</v>
       </c>
       <c r="B57" s="6" t="s">
@@ -34983,7 +34983,7 @@
       </c>
     </row>
     <row r="58" spans="1:13" ht="80">
-      <c r="A58" s="55"/>
+      <c r="A58" s="54"/>
       <c r="B58" s="7" t="s">
         <v>858</v>
       </c>
@@ -35023,7 +35023,7 @@
       </c>
     </row>
     <row r="59" spans="1:13" ht="64" customHeight="1">
-      <c r="A59" s="55"/>
+      <c r="A59" s="54"/>
       <c r="B59" s="7" t="s">
         <v>860</v>
       </c>
@@ -35063,7 +35063,7 @@
       </c>
     </row>
     <row r="60" spans="1:13" ht="16">
-      <c r="A60" s="55"/>
+      <c r="A60" s="54"/>
       <c r="B60" s="7" t="s">
         <v>95</v>
       </c>
@@ -35103,7 +35103,7 @@
       </c>
     </row>
     <row r="61" spans="1:13" ht="32">
-      <c r="A61" s="55"/>
+      <c r="A61" s="54"/>
       <c r="B61" s="7" t="s">
         <v>864</v>
       </c>
@@ -35143,7 +35143,7 @@
       </c>
     </row>
     <row r="62" spans="1:13" ht="32">
-      <c r="A62" s="55"/>
+      <c r="A62" s="54"/>
       <c r="B62" s="7" t="s">
         <v>866</v>
       </c>
@@ -35183,7 +35183,7 @@
       </c>
     </row>
     <row r="63" spans="1:13" ht="16">
-      <c r="A63" s="55"/>
+      <c r="A63" s="54"/>
       <c r="B63" s="7" t="s">
         <v>869</v>
       </c>
@@ -35223,7 +35223,7 @@
       </c>
     </row>
     <row r="64" spans="1:13" ht="32">
-      <c r="A64" s="55"/>
+      <c r="A64" s="54"/>
       <c r="B64" s="6" t="s">
         <v>871</v>
       </c>
@@ -35263,7 +35263,7 @@
       </c>
     </row>
     <row r="65" spans="1:13" ht="16">
-      <c r="A65" s="55"/>
+      <c r="A65" s="54"/>
       <c r="B65" s="7" t="s">
         <v>82</v>
       </c>
@@ -35303,7 +35303,7 @@
       </c>
     </row>
     <row r="66" spans="1:13" ht="16">
-      <c r="A66" s="55"/>
+      <c r="A66" s="54"/>
       <c r="B66" s="7" t="s">
         <v>874</v>
       </c>
@@ -35343,7 +35343,7 @@
       </c>
     </row>
     <row r="67" spans="1:13" ht="48">
-      <c r="A67" s="55"/>
+      <c r="A67" s="54"/>
       <c r="B67" s="6" t="s">
         <v>92</v>
       </c>
@@ -35383,38 +35383,38 @@
       </c>
     </row>
     <row r="68" spans="1:13" ht="16">
-      <c r="A68" s="55"/>
-      <c r="B68" s="55" t="s">
+      <c r="A68" s="54"/>
+      <c r="B68" s="54" t="s">
         <v>169</v>
       </c>
       <c r="C68" s="6" t="s">
         <v>876</v>
       </c>
-      <c r="D68" s="55" t="s">
+      <c r="D68" s="54" t="s">
         <v>27</v>
       </c>
-      <c r="E68" s="55" t="s">
+      <c r="E68" s="54" t="s">
         <v>862</v>
       </c>
-      <c r="F68" s="55" t="s">
-        <v>23</v>
-      </c>
-      <c r="G68" s="55" t="s">
+      <c r="F68" s="54" t="s">
+        <v>23</v>
+      </c>
+      <c r="G68" s="54" t="s">
         <v>23</v>
       </c>
       <c r="H68" s="53" t="s">
         <v>23</v>
       </c>
-      <c r="I68" s="55" t="s">
+      <c r="I68" s="54" t="s">
         <v>181</v>
       </c>
-      <c r="J68" s="55" t="s">
-        <v>23</v>
-      </c>
-      <c r="K68" s="55" t="s">
-        <v>23</v>
-      </c>
-      <c r="L68" s="55" t="s">
+      <c r="J68" s="54" t="s">
+        <v>23</v>
+      </c>
+      <c r="K68" s="54" t="s">
+        <v>23</v>
+      </c>
+      <c r="L68" s="54" t="s">
         <v>84</v>
       </c>
       <c r="M68" s="53" t="str">
@@ -35423,24 +35423,24 @@
       </c>
     </row>
     <row r="69" spans="1:13" ht="16">
-      <c r="A69" s="55"/>
-      <c r="B69" s="55"/>
+      <c r="A69" s="54"/>
+      <c r="B69" s="54"/>
       <c r="C69" s="6" t="s">
         <v>877</v>
       </c>
-      <c r="D69" s="55"/>
-      <c r="E69" s="55"/>
-      <c r="F69" s="55"/>
-      <c r="G69" s="55"/>
+      <c r="D69" s="54"/>
+      <c r="E69" s="54"/>
+      <c r="F69" s="54"/>
+      <c r="G69" s="54"/>
       <c r="H69" s="53"/>
-      <c r="I69" s="55"/>
-      <c r="J69" s="55"/>
-      <c r="K69" s="55"/>
-      <c r="L69" s="55"/>
+      <c r="I69" s="54"/>
+      <c r="J69" s="54"/>
+      <c r="K69" s="54"/>
+      <c r="L69" s="54"/>
       <c r="M69" s="53"/>
     </row>
     <row r="70" spans="1:13" ht="28">
-      <c r="A70" s="56" t="s">
+      <c r="A70" s="55" t="s">
         <v>878</v>
       </c>
       <c r="B70" s="16" t="s">
@@ -35486,7 +35486,7 @@
       </c>
     </row>
     <row r="71" spans="1:13" ht="51">
-      <c r="A71" s="56"/>
+      <c r="A71" s="55"/>
       <c r="B71" s="16" t="s">
         <v>100</v>
       </c>
@@ -35530,7 +35530,7 @@
       </c>
     </row>
     <row r="72" spans="1:13" ht="28">
-      <c r="A72" s="56"/>
+      <c r="A72" s="55"/>
       <c r="B72" s="16" t="s">
         <v>763</v>
       </c>
@@ -35574,7 +35574,7 @@
       </c>
     </row>
     <row r="73" spans="1:13" ht="28">
-      <c r="A73" s="56"/>
+      <c r="A73" s="55"/>
       <c r="B73" s="16" t="s">
         <v>885</v>
       </c>
@@ -36136,6 +36136,15 @@
     </row>
   </sheetData>
   <mergeCells count="23">
+    <mergeCell ref="A2:A7"/>
+    <mergeCell ref="A8:A14"/>
+    <mergeCell ref="A25:A29"/>
+    <mergeCell ref="A15:A24"/>
+    <mergeCell ref="A49:A56"/>
+    <mergeCell ref="A44:A48"/>
+    <mergeCell ref="A41:A43"/>
+    <mergeCell ref="A30:A36"/>
+    <mergeCell ref="A37:A40"/>
     <mergeCell ref="M68:M69"/>
     <mergeCell ref="H68:H69"/>
     <mergeCell ref="A74:A85"/>
@@ -36150,15 +36159,6 @@
     <mergeCell ref="B68:B69"/>
     <mergeCell ref="D68:D69"/>
     <mergeCell ref="E68:E69"/>
-    <mergeCell ref="A2:A7"/>
-    <mergeCell ref="A8:A14"/>
-    <mergeCell ref="A25:A29"/>
-    <mergeCell ref="A15:A24"/>
-    <mergeCell ref="A49:A56"/>
-    <mergeCell ref="A44:A48"/>
-    <mergeCell ref="A41:A43"/>
-    <mergeCell ref="A30:A36"/>
-    <mergeCell ref="A37:A40"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -37921,71 +37921,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="633f040f-4953-46e7-8610-82b0c5296ba0">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="f62ef740-d444-4f18-80a2-7590fdcab1ce" xsi:nil="true"/>
-    <Has_Teacher_Only_SectionGroup xmlns="633f040f-4953-46e7-8610-82b0c5296ba0" xsi:nil="true"/>
-    <Teachers xmlns="633f040f-4953-46e7-8610-82b0c5296ba0">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </Teachers>
-    <IsNotebookLocked xmlns="633f040f-4953-46e7-8610-82b0c5296ba0" xsi:nil="true"/>
-    <CultureName xmlns="633f040f-4953-46e7-8610-82b0c5296ba0" xsi:nil="true"/>
-    <Owner xmlns="633f040f-4953-46e7-8610-82b0c5296ba0">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </Owner>
-    <Distribution_Groups xmlns="633f040f-4953-46e7-8610-82b0c5296ba0" xsi:nil="true"/>
-    <TeamsChannelId xmlns="633f040f-4953-46e7-8610-82b0c5296ba0" xsi:nil="true"/>
-    <Invited_Teachers xmlns="633f040f-4953-46e7-8610-82b0c5296ba0" xsi:nil="true"/>
-    <NotebookType xmlns="633f040f-4953-46e7-8610-82b0c5296ba0" xsi:nil="true"/>
-    <AppVersion xmlns="633f040f-4953-46e7-8610-82b0c5296ba0" xsi:nil="true"/>
-    <DefaultSectionNames xmlns="633f040f-4953-46e7-8610-82b0c5296ba0" xsi:nil="true"/>
-    <Is_Collaboration_Space_Locked xmlns="633f040f-4953-46e7-8610-82b0c5296ba0" xsi:nil="true"/>
-    <Templates xmlns="633f040f-4953-46e7-8610-82b0c5296ba0" xsi:nil="true"/>
-    <FolderType xmlns="633f040f-4953-46e7-8610-82b0c5296ba0" xsi:nil="true"/>
-    <Student_Groups xmlns="633f040f-4953-46e7-8610-82b0c5296ba0">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </Student_Groups>
-    <Teams_Channel_Section_Location xmlns="633f040f-4953-46e7-8610-82b0c5296ba0" xsi:nil="true"/>
-    <Math_Settings xmlns="633f040f-4953-46e7-8610-82b0c5296ba0" xsi:nil="true"/>
-    <Self_Registration_Enabled xmlns="633f040f-4953-46e7-8610-82b0c5296ba0" xsi:nil="true"/>
-    <Students xmlns="633f040f-4953-46e7-8610-82b0c5296ba0">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </Students>
-    <LMS_Mappings xmlns="633f040f-4953-46e7-8610-82b0c5296ba0" xsi:nil="true"/>
-    <Invited_Students xmlns="633f040f-4953-46e7-8610-82b0c5296ba0" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x0101009A9CE0B21D9C3A45B31425227616CD6F" ma:contentTypeVersion="34" ma:contentTypeDescription="Creare un nuovo documento." ma:contentTypeScope="" ma:versionID="8a882b22c4c6ceab40c069a6a2420ef3">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="633f040f-4953-46e7-8610-82b0c5296ba0" xmlns:ns3="f62ef740-d444-4f18-80a2-7590fdcab1ce" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="77035a69dc4d6b80a35ec1b02b2030a4" ns2:_="" ns3:_="">
     <xsd:import namespace="633f040f-4953-46e7-8610-82b0c5296ba0"/>
@@ -38402,32 +38337,72 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{83D5100D-0E56-4B30-B42D-2AEC6B837C39}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="f62ef740-d444-4f18-80a2-7590fdcab1ce"/>
-    <ds:schemaRef ds:uri="633f040f-4953-46e7-8610-82b0c5296ba0"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2C6CC7BA-2E2C-4B0D-8103-11A51D82E8EC}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="633f040f-4953-46e7-8610-82b0c5296ba0">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="f62ef740-d444-4f18-80a2-7590fdcab1ce" xsi:nil="true"/>
+    <Has_Teacher_Only_SectionGroup xmlns="633f040f-4953-46e7-8610-82b0c5296ba0" xsi:nil="true"/>
+    <Teachers xmlns="633f040f-4953-46e7-8610-82b0c5296ba0">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </Teachers>
+    <IsNotebookLocked xmlns="633f040f-4953-46e7-8610-82b0c5296ba0" xsi:nil="true"/>
+    <CultureName xmlns="633f040f-4953-46e7-8610-82b0c5296ba0" xsi:nil="true"/>
+    <Owner xmlns="633f040f-4953-46e7-8610-82b0c5296ba0">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </Owner>
+    <Distribution_Groups xmlns="633f040f-4953-46e7-8610-82b0c5296ba0" xsi:nil="true"/>
+    <TeamsChannelId xmlns="633f040f-4953-46e7-8610-82b0c5296ba0" xsi:nil="true"/>
+    <Invited_Teachers xmlns="633f040f-4953-46e7-8610-82b0c5296ba0" xsi:nil="true"/>
+    <NotebookType xmlns="633f040f-4953-46e7-8610-82b0c5296ba0" xsi:nil="true"/>
+    <AppVersion xmlns="633f040f-4953-46e7-8610-82b0c5296ba0" xsi:nil="true"/>
+    <DefaultSectionNames xmlns="633f040f-4953-46e7-8610-82b0c5296ba0" xsi:nil="true"/>
+    <Is_Collaboration_Space_Locked xmlns="633f040f-4953-46e7-8610-82b0c5296ba0" xsi:nil="true"/>
+    <Templates xmlns="633f040f-4953-46e7-8610-82b0c5296ba0" xsi:nil="true"/>
+    <FolderType xmlns="633f040f-4953-46e7-8610-82b0c5296ba0" xsi:nil="true"/>
+    <Student_Groups xmlns="633f040f-4953-46e7-8610-82b0c5296ba0">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </Student_Groups>
+    <Teams_Channel_Section_Location xmlns="633f040f-4953-46e7-8610-82b0c5296ba0" xsi:nil="true"/>
+    <Math_Settings xmlns="633f040f-4953-46e7-8610-82b0c5296ba0" xsi:nil="true"/>
+    <Self_Registration_Enabled xmlns="633f040f-4953-46e7-8610-82b0c5296ba0" xsi:nil="true"/>
+    <Students xmlns="633f040f-4953-46e7-8610-82b0c5296ba0">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </Students>
+    <LMS_Mappings xmlns="633f040f-4953-46e7-8610-82b0c5296ba0" xsi:nil="true"/>
+    <Invited_Students xmlns="633f040f-4953-46e7-8610-82b0c5296ba0" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{36C20BFB-BCC5-4457-BE44-22D2F12F84BE}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -38444,4 +38419,29 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2C6CC7BA-2E2C-4B0D-8103-11A51D82E8EC}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{83D5100D-0E56-4B30-B42D-2AEC6B837C39}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="f62ef740-d444-4f18-80a2-7590fdcab1ce"/>
+    <ds:schemaRef ds:uri="633f040f-4953-46e7-8610-82b0c5296ba0"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
cambiata libreria per il rendering di neo4j
</commit_message>
<xml_diff>
--- a/apps/static/assets/dbs/ThreatCatalogComplete.xlsx
+++ b/apps/static/assets/dbs/ThreatCatalogComplete.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fefox/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CC31BA2-C05E-A544-8EDA-FF4438826770}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85312539-9C47-034C-821A-0C7A11CAD11F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17460" firstSheet="5" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
   </definedNames>
   <calcPr calcId="191028"/>
   <pivotCaches>
-    <pivotCache cacheId="8" r:id="rId13"/>
+    <pivotCache cacheId="14" r:id="rId13"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -53,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5296" uniqueCount="1369">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5335" uniqueCount="1408">
   <si>
     <t>TID</t>
   </si>
@@ -4252,6 +4252,123 @@
   </si>
   <si>
     <t>Secondary Label</t>
+  </si>
+  <si>
+    <t>Color</t>
+  </si>
+  <si>
+    <t>HW.PC</t>
+  </si>
+  <si>
+    <t>Network.PAN</t>
+  </si>
+  <si>
+    <t>HW.Device</t>
+  </si>
+  <si>
+    <t>CSC</t>
+  </si>
+  <si>
+    <t>#054A91</t>
+  </si>
+  <si>
+    <t>#3E7CB1</t>
+  </si>
+  <si>
+    <t>#F17300</t>
+  </si>
+  <si>
+    <t>#1CCAD8</t>
+  </si>
+  <si>
+    <t>#15E6CD</t>
+  </si>
+  <si>
+    <t>#0CF574</t>
+  </si>
+  <si>
+    <t>#587291</t>
+  </si>
+  <si>
+    <t>#E54B4B</t>
+  </si>
+  <si>
+    <t>#444140</t>
+  </si>
+  <si>
+    <t>#C589E8</t>
+  </si>
+  <si>
+    <t>#4C191B</t>
+  </si>
+  <si>
+    <t>#963D5A</t>
+  </si>
+  <si>
+    <t>#6A0F49</t>
+  </si>
+  <si>
+    <t>#A7C4C2</t>
+  </si>
+  <si>
+    <t>#97EFE9</t>
+  </si>
+  <si>
+    <t>#2E0219</t>
+  </si>
+  <si>
+    <t>#3D405B</t>
+  </si>
+  <si>
+    <t>#81B29A</t>
+  </si>
+  <si>
+    <t>#F2CC8F</t>
+  </si>
+  <si>
+    <t>#5171A5</t>
+  </si>
+  <si>
+    <t>#326273</t>
+  </si>
+  <si>
+    <t>#71ACC1</t>
+  </si>
+  <si>
+    <t>#AACDDA</t>
+  </si>
+  <si>
+    <t>#5A5E87</t>
+  </si>
+  <si>
+    <t>#8588AD</t>
+  </si>
+  <si>
+    <t>#F7CE5B</t>
+  </si>
+  <si>
+    <t>#F7B05B</t>
+  </si>
+  <si>
+    <t>#FCA311</t>
+  </si>
+  <si>
+    <t>#DF2935</t>
+  </si>
+  <si>
+    <t>#23C9FF</t>
+  </si>
+  <si>
+    <t>#1F0812</t>
+  </si>
+  <si>
+    <t>#F3B3A6</t>
+  </si>
+  <si>
+    <t>CSP</t>
+  </si>
+  <si>
+    <t>#BEB7A4</t>
   </si>
 </sst>
 </file>
@@ -4560,7 +4677,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="68">
+  <cellXfs count="66">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -4719,33 +4836,11 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="44">
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -4765,6 +4860,26 @@
           <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
     </dxf>
     <dxf>
       <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -11298,7 +11413,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{48CB07D6-9F6C-094F-A3D3-916741F281CD}" name="Tabella pivot1" cacheId="8" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valori" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{48CB07D6-9F6C-094F-A3D3-916741F281CD}" name="Tabella pivot1" cacheId="14" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valori" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A1:B31" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="14">
     <pivotField showAll="0"/>
@@ -11571,16 +11686,17 @@
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{B024E82E-800B-1F45-9E1D-69CB0CB1D53F}" name="Tabella6" displayName="Tabella6" ref="A1:E29" totalsRowShown="0" headerRowDxfId="1">
-  <autoFilter ref="A1:E29" xr:uid="{B024E82E-800B-1F45-9E1D-69CB0CB1D53F}"/>
-  <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{9883E0EC-0AE3-A34B-B1D0-333E1D538D0C}" name="ID" dataDxfId="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{B024E82E-800B-1F45-9E1D-69CB0CB1D53F}" name="Tabella6" displayName="Tabella6" ref="A1:F34" totalsRowShown="0" headerRowDxfId="4">
+  <autoFilter ref="A1:F34" xr:uid="{B024E82E-800B-1F45-9E1D-69CB0CB1D53F}"/>
+  <tableColumns count="6">
+    <tableColumn id="1" xr3:uid="{9883E0EC-0AE3-A34B-B1D0-333E1D538D0C}" name="ID" dataDxfId="3">
       <calculatedColumnFormula>ROW()-1</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="2" xr3:uid="{56C065B9-CABE-8E4D-B2C4-2C20E6DDE461}" name="Primary Label"/>
     <tableColumn id="3" xr3:uid="{843CC80E-4364-2F4B-98AB-684079953AC7}" name="Secondary Label"/>
     <tableColumn id="4" xr3:uid="{78C10894-AB17-7748-BFA0-46CCB17E3A38}" name="Name" dataDxfId="2"/>
     <tableColumn id="5" xr3:uid="{BF79DB0A-B64B-444B-B78F-F733C7E5F194}" name="Description"/>
+    <tableColumn id="6" xr3:uid="{96734FC5-BA6B-694D-9EC2-E984F3AE92E3}" name="Color"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -36879,12 +36995,12 @@
   </sheetData>
   <phoneticPr fontId="11" type="noConversion"/>
   <conditionalFormatting sqref="O1:Q46 O48:Q339 O341:Q382">
-    <cfRule type="containsBlanks" dxfId="4" priority="11" stopIfTrue="1">
+    <cfRule type="containsBlanks" dxfId="1" priority="11" stopIfTrue="1">
       <formula>LEN(TRIM(O1))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O384:Q393">
-    <cfRule type="containsBlanks" dxfId="3" priority="1" stopIfTrue="1">
+    <cfRule type="containsBlanks" dxfId="0" priority="1" stopIfTrue="1">
       <formula>LEN(TRIM(O384))=0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -37972,10 +38088,10 @@
   <sheetPr>
     <tabColor theme="5" tint="-0.249977111117893"/>
   </sheetPr>
-  <dimension ref="A1:E29"/>
+  <dimension ref="A1:F34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -37986,276 +38102,424 @@
     <col min="5" max="5" width="17.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
-      <c r="A1" s="67" t="s">
+    <row r="1" spans="1:6">
+      <c r="A1" t="s">
         <v>986</v>
       </c>
-      <c r="B1" s="67" t="s">
+      <c r="B1" t="s">
         <v>1367</v>
       </c>
-      <c r="C1" s="67" t="s">
+      <c r="C1" t="s">
         <v>1368</v>
       </c>
-      <c r="D1" s="67" t="s">
+      <c r="D1" t="s">
         <v>932</v>
       </c>
-      <c r="E1" s="67" t="s">
+      <c r="E1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:5">
+      <c r="F1" t="s">
+        <v>1369</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
       <c r="A2">
-        <f t="shared" ref="A2:A29" si="0">ROW()-1</f>
+        <f>ROW()-1</f>
         <v>1</v>
       </c>
-      <c r="D2" s="22" t="s">
+      <c r="D2" t="s">
+        <v>1373</v>
+      </c>
+      <c r="F2" t="s">
+        <v>1374</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3">
+        <f>ROW()-1</f>
+        <v>2</v>
+      </c>
+      <c r="D3" t="s">
+        <v>1406</v>
+      </c>
+      <c r="F3" t="s">
+        <v>1407</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4">
+        <f t="shared" ref="A4:A34" si="0">ROW()-1</f>
+        <v>3</v>
+      </c>
+      <c r="D4" s="22" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="3" spans="1:5">
-      <c r="A3">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="D3" s="22" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5">
-      <c r="A4">
-        <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="D4" s="22" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5">
+      <c r="F4" t="s">
+        <v>1375</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
       <c r="A5">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="D5" s="22" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5">
+        <v>81</v>
+      </c>
+      <c r="F5" t="s">
+        <v>1376</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
       <c r="A6">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
       <c r="D6" s="22" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5">
+        <v>158</v>
+      </c>
+      <c r="F6" t="s">
+        <v>1377</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
       <c r="A7">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="D7" s="22" t="s">
-        <v>284</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5">
+        <v>173</v>
+      </c>
+      <c r="F7" t="s">
+        <v>1378</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
       <c r="A8">
-        <f t="shared" si="0"/>
+        <f>ROW()-1</f>
         <v>7</v>
       </c>
       <c r="D8" s="22" t="s">
-        <v>330</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5">
+        <v>1372</v>
+      </c>
+      <c r="F8" t="s">
+        <v>1379</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
       <c r="A9">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
       <c r="D9" s="22" t="s">
-        <v>369</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5">
+        <v>220</v>
+      </c>
+      <c r="F9" t="s">
+        <v>1380</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
       <c r="A10">
-        <f t="shared" si="0"/>
+        <f>ROW()-1</f>
         <v>9</v>
       </c>
       <c r="D10" s="22" t="s">
-        <v>426</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5">
+        <v>1370</v>
+      </c>
+      <c r="F10" t="s">
+        <v>1381</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
       <c r="A11">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
       <c r="D11" s="22" t="s">
-        <v>430</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5">
+        <v>284</v>
+      </c>
+      <c r="F11" t="s">
+        <v>1382</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
       <c r="A12">
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
       <c r="D12" s="22" t="s">
-        <v>509</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5">
+        <v>330</v>
+      </c>
+      <c r="F12" t="s">
+        <v>1393</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
       <c r="A13">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
       <c r="D13" s="22" t="s">
-        <v>510</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5">
+        <v>369</v>
+      </c>
+      <c r="F13" t="s">
+        <v>1394</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
       <c r="A14">
-        <f t="shared" si="0"/>
+        <f>ROW()-1</f>
         <v>13</v>
       </c>
       <c r="D14" s="22" t="s">
-        <v>517</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5">
+        <v>1371</v>
+      </c>
+      <c r="F14" t="s">
+        <v>1396</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
       <c r="A15">
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
       <c r="D15" s="22" t="s">
-        <v>524</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5">
+        <v>426</v>
+      </c>
+      <c r="F15" t="s">
+        <v>1395</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
       <c r="A16">
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
       <c r="D16" s="22" t="s">
-        <v>529</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4">
+        <v>430</v>
+      </c>
+      <c r="F16" t="s">
+        <v>1383</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6">
       <c r="A17">
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
       <c r="D17" s="22" t="s">
-        <v>553</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4">
+        <v>509</v>
+      </c>
+      <c r="F17" t="s">
+        <v>1385</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6">
       <c r="A18">
         <f t="shared" si="0"/>
         <v>17</v>
       </c>
       <c r="D18" s="22" t="s">
-        <v>554</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4">
+        <v>510</v>
+      </c>
+      <c r="F18" t="s">
+        <v>1386</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6">
       <c r="A19">
         <f t="shared" si="0"/>
         <v>18</v>
       </c>
       <c r="D19" s="22" t="s">
-        <v>561</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4">
+        <v>517</v>
+      </c>
+      <c r="F19" t="s">
+        <v>1387</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6">
       <c r="A20">
         <f t="shared" si="0"/>
         <v>19</v>
       </c>
       <c r="D20" s="22" t="s">
-        <v>567</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4">
+        <v>524</v>
+      </c>
+      <c r="F20" t="s">
+        <v>1388</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6">
       <c r="A21">
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
       <c r="D21" s="22" t="s">
-        <v>618</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4">
+        <v>529</v>
+      </c>
+      <c r="F21" t="s">
+        <v>1389</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6">
       <c r="A22">
         <f t="shared" si="0"/>
         <v>21</v>
       </c>
       <c r="D22" s="22" t="s">
-        <v>644</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4">
+        <v>553</v>
+      </c>
+      <c r="F22" t="s">
+        <v>1390</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6">
       <c r="A23">
         <f t="shared" si="0"/>
         <v>22</v>
       </c>
       <c r="D23" s="22" t="s">
-        <v>676</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4">
+        <v>554</v>
+      </c>
+      <c r="F23" t="s">
+        <v>1397</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6">
       <c r="A24">
         <f t="shared" si="0"/>
         <v>23</v>
       </c>
       <c r="D24" s="22" t="s">
-        <v>722</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4">
+        <v>561</v>
+      </c>
+      <c r="F24" t="s">
+        <v>1398</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6">
       <c r="A25">
         <f t="shared" si="0"/>
         <v>24</v>
       </c>
       <c r="D25" s="22" t="s">
-        <v>1151</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4">
+        <v>567</v>
+      </c>
+      <c r="F25" t="s">
+        <v>1384</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6">
       <c r="A26">
         <f t="shared" si="0"/>
         <v>25</v>
       </c>
       <c r="D26" s="22" t="s">
-        <v>1197</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4">
+        <v>618</v>
+      </c>
+      <c r="F26" t="s">
+        <v>1391</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6">
       <c r="A27">
         <f t="shared" si="0"/>
         <v>26</v>
       </c>
       <c r="D27" s="22" t="s">
-        <v>1163</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4">
+        <v>644</v>
+      </c>
+      <c r="F27" t="s">
+        <v>1400</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6">
       <c r="A28">
         <f t="shared" si="0"/>
         <v>27</v>
       </c>
       <c r="D28" s="22" t="s">
-        <v>1275</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4">
+        <v>676</v>
+      </c>
+      <c r="F28" t="s">
+        <v>1399</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6">
       <c r="A29">
         <f t="shared" si="0"/>
         <v>28</v>
       </c>
       <c r="D29" s="22" t="s">
+        <v>722</v>
+      </c>
+      <c r="F29" t="s">
+        <v>1402</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6">
+      <c r="A30">
+        <f t="shared" si="0"/>
+        <v>29</v>
+      </c>
+      <c r="D30" s="22" t="s">
+        <v>1151</v>
+      </c>
+      <c r="F30" t="s">
+        <v>1403</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6">
+      <c r="A31">
+        <f t="shared" si="0"/>
+        <v>30</v>
+      </c>
+      <c r="D31" s="22" t="s">
+        <v>1197</v>
+      </c>
+      <c r="F31" t="s">
+        <v>1392</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6">
+      <c r="A32">
+        <f t="shared" si="0"/>
+        <v>31</v>
+      </c>
+      <c r="D32" s="22" t="s">
+        <v>1163</v>
+      </c>
+      <c r="F32" t="s">
+        <v>1404</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6">
+      <c r="A33">
+        <f t="shared" si="0"/>
+        <v>32</v>
+      </c>
+      <c r="D33" s="22" t="s">
+        <v>1275</v>
+      </c>
+      <c r="F33" t="s">
+        <v>1405</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6">
+      <c r="A34">
+        <f t="shared" si="0"/>
+        <v>33</v>
+      </c>
+      <c r="D34" s="22" t="s">
         <v>1298</v>
       </c>
+      <c r="F34" t="s">
+        <v>1401</v>
+      </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="11" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
     <tablePart r:id="rId1"/>
@@ -41922,7 +42186,7 @@
       <c r="A2" s="22" t="s">
         <v>18</v>
       </c>
-      <c r="B2" s="66">
+      <c r="B2">
         <v>31</v>
       </c>
     </row>
@@ -41930,7 +42194,7 @@
       <c r="A3" s="22" t="s">
         <v>81</v>
       </c>
-      <c r="B3" s="66">
+      <c r="B3">
         <v>27</v>
       </c>
     </row>
@@ -41938,7 +42202,7 @@
       <c r="A4" s="22" t="s">
         <v>158</v>
       </c>
-      <c r="B4" s="66">
+      <c r="B4">
         <v>8</v>
       </c>
     </row>
@@ -41946,7 +42210,7 @@
       <c r="A5" s="22" t="s">
         <v>173</v>
       </c>
-      <c r="B5" s="66">
+      <c r="B5">
         <v>9</v>
       </c>
     </row>
@@ -41954,7 +42218,7 @@
       <c r="A6" s="22" t="s">
         <v>220</v>
       </c>
-      <c r="B6" s="66">
+      <c r="B6">
         <v>13</v>
       </c>
     </row>
@@ -41962,7 +42226,7 @@
       <c r="A7" s="22" t="s">
         <v>284</v>
       </c>
-      <c r="B7" s="66">
+      <c r="B7">
         <v>17</v>
       </c>
     </row>
@@ -41970,7 +42234,7 @@
       <c r="A8" s="22" t="s">
         <v>330</v>
       </c>
-      <c r="B8" s="66">
+      <c r="B8">
         <v>12</v>
       </c>
     </row>
@@ -41978,7 +42242,7 @@
       <c r="A9" s="22" t="s">
         <v>369</v>
       </c>
-      <c r="B9" s="66">
+      <c r="B9">
         <v>25</v>
       </c>
     </row>
@@ -41986,7 +42250,7 @@
       <c r="A10" s="22" t="s">
         <v>426</v>
       </c>
-      <c r="B10" s="66">
+      <c r="B10">
         <v>1</v>
       </c>
     </row>
@@ -41994,7 +42258,7 @@
       <c r="A11" s="22" t="s">
         <v>430</v>
       </c>
-      <c r="B11" s="66">
+      <c r="B11">
         <v>53</v>
       </c>
     </row>
@@ -42002,7 +42266,7 @@
       <c r="A12" s="22" t="s">
         <v>509</v>
       </c>
-      <c r="B12" s="66">
+      <c r="B12">
         <v>5</v>
       </c>
     </row>
@@ -42010,7 +42274,7 @@
       <c r="A13" s="22" t="s">
         <v>510</v>
       </c>
-      <c r="B13" s="66">
+      <c r="B13">
         <v>12</v>
       </c>
     </row>
@@ -42018,7 +42282,7 @@
       <c r="A14" s="22" t="s">
         <v>517</v>
       </c>
-      <c r="B14" s="66">
+      <c r="B14">
         <v>8</v>
       </c>
     </row>
@@ -42026,7 +42290,7 @@
       <c r="A15" s="22" t="s">
         <v>524</v>
       </c>
-      <c r="B15" s="66">
+      <c r="B15">
         <v>8</v>
       </c>
     </row>
@@ -42034,7 +42298,7 @@
       <c r="A16" s="22" t="s">
         <v>529</v>
       </c>
-      <c r="B16" s="66">
+      <c r="B16">
         <v>11</v>
       </c>
     </row>
@@ -42042,7 +42306,7 @@
       <c r="A17" s="22" t="s">
         <v>553</v>
       </c>
-      <c r="B17" s="66">
+      <c r="B17">
         <v>5</v>
       </c>
     </row>
@@ -42050,7 +42314,7 @@
       <c r="A18" s="22" t="s">
         <v>554</v>
       </c>
-      <c r="B18" s="66">
+      <c r="B18">
         <v>7</v>
       </c>
     </row>
@@ -42058,7 +42322,7 @@
       <c r="A19" s="22" t="s">
         <v>561</v>
       </c>
-      <c r="B19" s="66">
+      <c r="B19">
         <v>9</v>
       </c>
     </row>
@@ -42066,7 +42330,7 @@
       <c r="A20" s="22" t="s">
         <v>567</v>
       </c>
-      <c r="B20" s="66">
+      <c r="B20">
         <v>15</v>
       </c>
     </row>
@@ -42074,7 +42338,7 @@
       <c r="A21" s="22" t="s">
         <v>618</v>
       </c>
-      <c r="B21" s="66">
+      <c r="B21">
         <v>5</v>
       </c>
     </row>
@@ -42082,7 +42346,7 @@
       <c r="A22" s="22" t="s">
         <v>644</v>
       </c>
-      <c r="B22" s="66">
+      <c r="B22">
         <v>16</v>
       </c>
     </row>
@@ -42090,7 +42354,7 @@
       <c r="A23" s="22" t="s">
         <v>676</v>
       </c>
-      <c r="B23" s="66">
+      <c r="B23">
         <v>9</v>
       </c>
     </row>
@@ -42098,13 +42362,12 @@
       <c r="A24" s="22" t="s">
         <v>924</v>
       </c>
-      <c r="B24" s="66"/>
     </row>
     <row r="25" spans="1:2">
       <c r="A25" s="22" t="s">
         <v>722</v>
       </c>
-      <c r="B25" s="66">
+      <c r="B25">
         <v>15</v>
       </c>
     </row>
@@ -42112,7 +42375,7 @@
       <c r="A26" s="22" t="s">
         <v>1151</v>
       </c>
-      <c r="B26" s="66">
+      <c r="B26">
         <v>19</v>
       </c>
     </row>
@@ -42120,7 +42383,7 @@
       <c r="A27" s="22" t="s">
         <v>1197</v>
       </c>
-      <c r="B27" s="66">
+      <c r="B27">
         <v>14</v>
       </c>
     </row>
@@ -42128,7 +42391,7 @@
       <c r="A28" s="22" t="s">
         <v>1163</v>
       </c>
-      <c r="B28" s="66">
+      <c r="B28">
         <v>20</v>
       </c>
     </row>
@@ -42136,7 +42399,7 @@
       <c r="A29" s="22" t="s">
         <v>1275</v>
       </c>
-      <c r="B29" s="66">
+      <c r="B29">
         <v>7</v>
       </c>
     </row>
@@ -42144,7 +42407,7 @@
       <c r="A30" s="22" t="s">
         <v>1298</v>
       </c>
-      <c r="B30" s="66">
+      <c r="B30">
         <v>11</v>
       </c>
     </row>
@@ -42152,7 +42415,7 @@
       <c r="A31" s="22" t="s">
         <v>925</v>
       </c>
-      <c r="B31" s="66">
+      <c r="B31">
         <v>392</v>
       </c>
     </row>
@@ -43968,6 +44231,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x0101009A9CE0B21D9C3A45B31425227616CD6F" ma:contentTypeVersion="34" ma:contentTypeDescription="Creare un nuovo documento." ma:contentTypeScope="" ma:versionID="8a882b22c4c6ceab40c069a6a2420ef3">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="633f040f-4953-46e7-8610-82b0c5296ba0" xmlns:ns3="f62ef740-d444-4f18-80a2-7590fdcab1ce" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="77035a69dc4d6b80a35ec1b02b2030a4" ns2:_="" ns3:_="">
     <xsd:import namespace="633f040f-4953-46e7-8610-82b0c5296ba0"/>
@@ -44384,7 +44656,7 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <lcf76f155ced4ddcb4097134ff3c332f xmlns="633f040f-4953-46e7-8610-82b0c5296ba0">
@@ -44440,16 +44712,15 @@
 </p:properties>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2C6CC7BA-2E2C-4B0D-8103-11A51D82E8EC}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{36C20BFB-BCC5-4457-BE44-22D2F12F84BE}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -44468,7 +44739,7 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{83D5100D-0E56-4B30-B42D-2AEC6B837C39}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
@@ -44483,12 +44754,4 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2C6CC7BA-2E2C-4B0D-8103-11A51D82E8EC}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
aggiunti colori ai badge del catalogo degli asset type
</commit_message>
<xml_diff>
--- a/apps/static/assets/dbs/ThreatCatalogComplete.xlsx
+++ b/apps/static/assets/dbs/ThreatCatalogComplete.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fefox/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85312539-9C47-034C-821A-0C7A11CAD11F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A99CE4DC-191E-7F47-8A7C-1BE8F6425186}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17460" firstSheet="5" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
   </definedNames>
   <calcPr calcId="191028"/>
   <pivotCaches>
-    <pivotCache cacheId="14" r:id="rId13"/>
+    <pivotCache cacheId="15" r:id="rId13"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -4359,9 +4359,6 @@
     <t>#23C9FF</t>
   </si>
   <si>
-    <t>#1F0812</t>
-  </si>
-  <si>
     <t>#F3B3A6</t>
   </si>
   <si>
@@ -4369,6 +4366,9 @@
   </si>
   <si>
     <t>#BEB7A4</t>
+  </si>
+  <si>
+    <t>#82214B</t>
   </si>
 </sst>
 </file>
@@ -4827,14 +4827,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -11413,7 +11413,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{48CB07D6-9F6C-094F-A3D3-916741F281CD}" name="Tabella pivot1" cacheId="14" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valori" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{48CB07D6-9F6C-094F-A3D3-916741F281CD}" name="Tabella pivot1" cacheId="15" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valori" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A1:B31" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="14">
     <pivotField showAll="0"/>
@@ -38091,7 +38091,7 @@
   <dimension ref="A1:F34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+      <selection activeCell="F32" sqref="F32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -38140,10 +38140,10 @@
         <v>2</v>
       </c>
       <c r="D3" t="s">
+        <v>1405</v>
+      </c>
+      <c r="F3" t="s">
         <v>1406</v>
-      </c>
-      <c r="F3" t="s">
-        <v>1407</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -38491,7 +38491,7 @@
         <v>1163</v>
       </c>
       <c r="F32" t="s">
-        <v>1404</v>
+        <v>1407</v>
       </c>
     </row>
     <row r="33" spans="1:6">
@@ -38503,7 +38503,7 @@
         <v>1275</v>
       </c>
       <c r="F33" t="s">
-        <v>1405</v>
+        <v>1404</v>
       </c>
     </row>
     <row r="34" spans="1:6">
@@ -39812,7 +39812,7 @@
       </c>
     </row>
     <row r="30" spans="1:13" ht="48">
-      <c r="A30" s="63" t="s">
+      <c r="A30" s="65" t="s">
         <v>811</v>
       </c>
       <c r="B30" s="5" t="s">
@@ -39855,7 +39855,7 @@
       </c>
     </row>
     <row r="31" spans="1:13" ht="48">
-      <c r="A31" s="63"/>
+      <c r="A31" s="65"/>
       <c r="B31" s="5" t="s">
         <v>814</v>
       </c>
@@ -39896,7 +39896,7 @@
       </c>
     </row>
     <row r="32" spans="1:13" ht="32">
-      <c r="A32" s="63"/>
+      <c r="A32" s="65"/>
       <c r="B32" s="5" t="s">
         <v>816</v>
       </c>
@@ -39937,7 +39937,7 @@
       </c>
     </row>
     <row r="33" spans="1:13" ht="96">
-      <c r="A33" s="63"/>
+      <c r="A33" s="65"/>
       <c r="B33" s="5" t="s">
         <v>100</v>
       </c>
@@ -39978,7 +39978,7 @@
       </c>
     </row>
     <row r="34" spans="1:13" ht="32">
-      <c r="A34" s="63"/>
+      <c r="A34" s="65"/>
       <c r="B34" s="5" t="s">
         <v>819</v>
       </c>
@@ -40019,7 +40019,7 @@
       </c>
     </row>
     <row r="35" spans="1:13" ht="32">
-      <c r="A35" s="63"/>
+      <c r="A35" s="65"/>
       <c r="B35" s="5" t="s">
         <v>201</v>
       </c>
@@ -40060,7 +40060,7 @@
       </c>
     </row>
     <row r="36" spans="1:13" ht="80">
-      <c r="A36" s="63"/>
+      <c r="A36" s="65"/>
       <c r="B36" s="5" t="s">
         <v>822</v>
       </c>
@@ -40599,7 +40599,7 @@
       </c>
     </row>
     <row r="49" spans="1:13" ht="78" customHeight="1">
-      <c r="A49" s="63" t="s">
+      <c r="A49" s="65" t="s">
         <v>840</v>
       </c>
       <c r="B49" s="5" t="s">
@@ -40642,7 +40642,7 @@
       </c>
     </row>
     <row r="50" spans="1:13" ht="32">
-      <c r="A50" s="63"/>
+      <c r="A50" s="65"/>
       <c r="B50" s="5" t="s">
         <v>613</v>
       </c>
@@ -40683,7 +40683,7 @@
       </c>
     </row>
     <row r="51" spans="1:13" ht="16">
-      <c r="A51" s="63"/>
+      <c r="A51" s="65"/>
       <c r="B51" s="5" t="s">
         <v>201</v>
       </c>
@@ -40724,7 +40724,7 @@
       </c>
     </row>
     <row r="52" spans="1:13" ht="32">
-      <c r="A52" s="63"/>
+      <c r="A52" s="65"/>
       <c r="B52" s="5" t="s">
         <v>845</v>
       </c>
@@ -40765,7 +40765,7 @@
       </c>
     </row>
     <row r="53" spans="1:13" ht="96">
-      <c r="A53" s="63"/>
+      <c r="A53" s="65"/>
       <c r="B53" s="5" t="s">
         <v>847</v>
       </c>
@@ -40806,7 +40806,7 @@
       </c>
     </row>
     <row r="54" spans="1:13">
-      <c r="A54" s="63"/>
+      <c r="A54" s="65"/>
       <c r="B54" s="5" t="s">
         <v>849</v>
       </c>
@@ -40847,7 +40847,7 @@
       </c>
     </row>
     <row r="55" spans="1:13" ht="64">
-      <c r="A55" s="63"/>
+      <c r="A55" s="65"/>
       <c r="B55" s="5" t="s">
         <v>851</v>
       </c>
@@ -40888,7 +40888,7 @@
       </c>
     </row>
     <row r="56" spans="1:13" ht="64">
-      <c r="A56" s="63"/>
+      <c r="A56" s="65"/>
       <c r="B56" s="5" t="s">
         <v>853</v>
       </c>
@@ -40929,7 +40929,7 @@
       </c>
     </row>
     <row r="57" spans="1:13" ht="32">
-      <c r="A57" s="64" t="s">
+      <c r="A57" s="63" t="s">
         <v>855</v>
       </c>
       <c r="B57" s="6" t="s">
@@ -40971,7 +40971,7 @@
       </c>
     </row>
     <row r="58" spans="1:13" ht="80">
-      <c r="A58" s="64"/>
+      <c r="A58" s="63"/>
       <c r="B58" s="7" t="s">
         <v>858</v>
       </c>
@@ -41011,7 +41011,7 @@
       </c>
     </row>
     <row r="59" spans="1:13" ht="64" customHeight="1">
-      <c r="A59" s="64"/>
+      <c r="A59" s="63"/>
       <c r="B59" s="7" t="s">
         <v>860</v>
       </c>
@@ -41051,7 +41051,7 @@
       </c>
     </row>
     <row r="60" spans="1:13" ht="16">
-      <c r="A60" s="64"/>
+      <c r="A60" s="63"/>
       <c r="B60" s="7" t="s">
         <v>95</v>
       </c>
@@ -41091,7 +41091,7 @@
       </c>
     </row>
     <row r="61" spans="1:13" ht="32">
-      <c r="A61" s="64"/>
+      <c r="A61" s="63"/>
       <c r="B61" s="7" t="s">
         <v>864</v>
       </c>
@@ -41131,7 +41131,7 @@
       </c>
     </row>
     <row r="62" spans="1:13" ht="32">
-      <c r="A62" s="64"/>
+      <c r="A62" s="63"/>
       <c r="B62" s="7" t="s">
         <v>866</v>
       </c>
@@ -41171,7 +41171,7 @@
       </c>
     </row>
     <row r="63" spans="1:13" ht="16">
-      <c r="A63" s="64"/>
+      <c r="A63" s="63"/>
       <c r="B63" s="7" t="s">
         <v>869</v>
       </c>
@@ -41211,7 +41211,7 @@
       </c>
     </row>
     <row r="64" spans="1:13" ht="32">
-      <c r="A64" s="64"/>
+      <c r="A64" s="63"/>
       <c r="B64" s="6" t="s">
         <v>871</v>
       </c>
@@ -41251,7 +41251,7 @@
       </c>
     </row>
     <row r="65" spans="1:13" ht="16">
-      <c r="A65" s="64"/>
+      <c r="A65" s="63"/>
       <c r="B65" s="7" t="s">
         <v>82</v>
       </c>
@@ -41291,7 +41291,7 @@
       </c>
     </row>
     <row r="66" spans="1:13" ht="16">
-      <c r="A66" s="64"/>
+      <c r="A66" s="63"/>
       <c r="B66" s="7" t="s">
         <v>874</v>
       </c>
@@ -41331,7 +41331,7 @@
       </c>
     </row>
     <row r="67" spans="1:13" ht="48">
-      <c r="A67" s="64"/>
+      <c r="A67" s="63"/>
       <c r="B67" s="6" t="s">
         <v>92</v>
       </c>
@@ -41371,38 +41371,38 @@
       </c>
     </row>
     <row r="68" spans="1:13" ht="16">
-      <c r="A68" s="64"/>
-      <c r="B68" s="64" t="s">
+      <c r="A68" s="63"/>
+      <c r="B68" s="63" t="s">
         <v>169</v>
       </c>
       <c r="C68" s="6" t="s">
         <v>876</v>
       </c>
-      <c r="D68" s="64" t="s">
+      <c r="D68" s="63" t="s">
         <v>27</v>
       </c>
-      <c r="E68" s="64" t="s">
+      <c r="E68" s="63" t="s">
         <v>862</v>
       </c>
-      <c r="F68" s="64" t="s">
-        <v>23</v>
-      </c>
-      <c r="G68" s="64" t="s">
+      <c r="F68" s="63" t="s">
+        <v>23</v>
+      </c>
+      <c r="G68" s="63" t="s">
         <v>23</v>
       </c>
       <c r="H68" s="62" t="s">
         <v>23</v>
       </c>
-      <c r="I68" s="64" t="s">
+      <c r="I68" s="63" t="s">
         <v>181</v>
       </c>
-      <c r="J68" s="64" t="s">
-        <v>23</v>
-      </c>
-      <c r="K68" s="64" t="s">
-        <v>23</v>
-      </c>
-      <c r="L68" s="64" t="s">
+      <c r="J68" s="63" t="s">
+        <v>23</v>
+      </c>
+      <c r="K68" s="63" t="s">
+        <v>23</v>
+      </c>
+      <c r="L68" s="63" t="s">
         <v>84</v>
       </c>
       <c r="M68" s="62" t="str">
@@ -41411,24 +41411,24 @@
       </c>
     </row>
     <row r="69" spans="1:13" ht="16">
-      <c r="A69" s="64"/>
-      <c r="B69" s="64"/>
+      <c r="A69" s="63"/>
+      <c r="B69" s="63"/>
       <c r="C69" s="6" t="s">
         <v>877</v>
       </c>
-      <c r="D69" s="64"/>
-      <c r="E69" s="64"/>
-      <c r="F69" s="64"/>
-      <c r="G69" s="64"/>
+      <c r="D69" s="63"/>
+      <c r="E69" s="63"/>
+      <c r="F69" s="63"/>
+      <c r="G69" s="63"/>
       <c r="H69" s="62"/>
-      <c r="I69" s="64"/>
-      <c r="J69" s="64"/>
-      <c r="K69" s="64"/>
-      <c r="L69" s="64"/>
+      <c r="I69" s="63"/>
+      <c r="J69" s="63"/>
+      <c r="K69" s="63"/>
+      <c r="L69" s="63"/>
       <c r="M69" s="62"/>
     </row>
     <row r="70" spans="1:13" ht="28">
-      <c r="A70" s="65" t="s">
+      <c r="A70" s="64" t="s">
         <v>878</v>
       </c>
       <c r="B70" s="16" t="s">
@@ -41474,7 +41474,7 @@
       </c>
     </row>
     <row r="71" spans="1:13" ht="51">
-      <c r="A71" s="65"/>
+      <c r="A71" s="64"/>
       <c r="B71" s="16" t="s">
         <v>100</v>
       </c>
@@ -41518,7 +41518,7 @@
       </c>
     </row>
     <row r="72" spans="1:13" ht="28">
-      <c r="A72" s="65"/>
+      <c r="A72" s="64"/>
       <c r="B72" s="16" t="s">
         <v>763</v>
       </c>
@@ -41562,7 +41562,7 @@
       </c>
     </row>
     <row r="73" spans="1:13" ht="28">
-      <c r="A73" s="65"/>
+      <c r="A73" s="64"/>
       <c r="B73" s="16" t="s">
         <v>885</v>
       </c>
@@ -42124,6 +42124,15 @@
     </row>
   </sheetData>
   <mergeCells count="23">
+    <mergeCell ref="A2:A7"/>
+    <mergeCell ref="A8:A14"/>
+    <mergeCell ref="A25:A29"/>
+    <mergeCell ref="A15:A24"/>
+    <mergeCell ref="A49:A56"/>
+    <mergeCell ref="A44:A48"/>
+    <mergeCell ref="A41:A43"/>
+    <mergeCell ref="A30:A36"/>
+    <mergeCell ref="A37:A40"/>
     <mergeCell ref="M68:M69"/>
     <mergeCell ref="H68:H69"/>
     <mergeCell ref="A74:A85"/>
@@ -42138,15 +42147,6 @@
     <mergeCell ref="B68:B69"/>
     <mergeCell ref="D68:D69"/>
     <mergeCell ref="E68:E69"/>
-    <mergeCell ref="A2:A7"/>
-    <mergeCell ref="A8:A14"/>
-    <mergeCell ref="A25:A29"/>
-    <mergeCell ref="A15:A24"/>
-    <mergeCell ref="A49:A56"/>
-    <mergeCell ref="A44:A48"/>
-    <mergeCell ref="A41:A43"/>
-    <mergeCell ref="A30:A36"/>
-    <mergeCell ref="A37:A40"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -44231,12 +44231,59 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="633f040f-4953-46e7-8610-82b0c5296ba0">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="f62ef740-d444-4f18-80a2-7590fdcab1ce" xsi:nil="true"/>
+    <Has_Teacher_Only_SectionGroup xmlns="633f040f-4953-46e7-8610-82b0c5296ba0" xsi:nil="true"/>
+    <Teachers xmlns="633f040f-4953-46e7-8610-82b0c5296ba0">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </Teachers>
+    <IsNotebookLocked xmlns="633f040f-4953-46e7-8610-82b0c5296ba0" xsi:nil="true"/>
+    <CultureName xmlns="633f040f-4953-46e7-8610-82b0c5296ba0" xsi:nil="true"/>
+    <Owner xmlns="633f040f-4953-46e7-8610-82b0c5296ba0">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </Owner>
+    <Distribution_Groups xmlns="633f040f-4953-46e7-8610-82b0c5296ba0" xsi:nil="true"/>
+    <TeamsChannelId xmlns="633f040f-4953-46e7-8610-82b0c5296ba0" xsi:nil="true"/>
+    <Invited_Teachers xmlns="633f040f-4953-46e7-8610-82b0c5296ba0" xsi:nil="true"/>
+    <NotebookType xmlns="633f040f-4953-46e7-8610-82b0c5296ba0" xsi:nil="true"/>
+    <AppVersion xmlns="633f040f-4953-46e7-8610-82b0c5296ba0" xsi:nil="true"/>
+    <DefaultSectionNames xmlns="633f040f-4953-46e7-8610-82b0c5296ba0" xsi:nil="true"/>
+    <Is_Collaboration_Space_Locked xmlns="633f040f-4953-46e7-8610-82b0c5296ba0" xsi:nil="true"/>
+    <Templates xmlns="633f040f-4953-46e7-8610-82b0c5296ba0" xsi:nil="true"/>
+    <FolderType xmlns="633f040f-4953-46e7-8610-82b0c5296ba0" xsi:nil="true"/>
+    <Student_Groups xmlns="633f040f-4953-46e7-8610-82b0c5296ba0">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </Student_Groups>
+    <Teams_Channel_Section_Location xmlns="633f040f-4953-46e7-8610-82b0c5296ba0" xsi:nil="true"/>
+    <Math_Settings xmlns="633f040f-4953-46e7-8610-82b0c5296ba0" xsi:nil="true"/>
+    <Self_Registration_Enabled xmlns="633f040f-4953-46e7-8610-82b0c5296ba0" xsi:nil="true"/>
+    <Students xmlns="633f040f-4953-46e7-8610-82b0c5296ba0">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </Students>
+    <LMS_Mappings xmlns="633f040f-4953-46e7-8610-82b0c5296ba0" xsi:nil="true"/>
+    <Invited_Students xmlns="633f040f-4953-46e7-8610-82b0c5296ba0" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -44657,65 +44704,27 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="633f040f-4953-46e7-8610-82b0c5296ba0">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="f62ef740-d444-4f18-80a2-7590fdcab1ce" xsi:nil="true"/>
-    <Has_Teacher_Only_SectionGroup xmlns="633f040f-4953-46e7-8610-82b0c5296ba0" xsi:nil="true"/>
-    <Teachers xmlns="633f040f-4953-46e7-8610-82b0c5296ba0">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </Teachers>
-    <IsNotebookLocked xmlns="633f040f-4953-46e7-8610-82b0c5296ba0" xsi:nil="true"/>
-    <CultureName xmlns="633f040f-4953-46e7-8610-82b0c5296ba0" xsi:nil="true"/>
-    <Owner xmlns="633f040f-4953-46e7-8610-82b0c5296ba0">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </Owner>
-    <Distribution_Groups xmlns="633f040f-4953-46e7-8610-82b0c5296ba0" xsi:nil="true"/>
-    <TeamsChannelId xmlns="633f040f-4953-46e7-8610-82b0c5296ba0" xsi:nil="true"/>
-    <Invited_Teachers xmlns="633f040f-4953-46e7-8610-82b0c5296ba0" xsi:nil="true"/>
-    <NotebookType xmlns="633f040f-4953-46e7-8610-82b0c5296ba0" xsi:nil="true"/>
-    <AppVersion xmlns="633f040f-4953-46e7-8610-82b0c5296ba0" xsi:nil="true"/>
-    <DefaultSectionNames xmlns="633f040f-4953-46e7-8610-82b0c5296ba0" xsi:nil="true"/>
-    <Is_Collaboration_Space_Locked xmlns="633f040f-4953-46e7-8610-82b0c5296ba0" xsi:nil="true"/>
-    <Templates xmlns="633f040f-4953-46e7-8610-82b0c5296ba0" xsi:nil="true"/>
-    <FolderType xmlns="633f040f-4953-46e7-8610-82b0c5296ba0" xsi:nil="true"/>
-    <Student_Groups xmlns="633f040f-4953-46e7-8610-82b0c5296ba0">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </Student_Groups>
-    <Teams_Channel_Section_Location xmlns="633f040f-4953-46e7-8610-82b0c5296ba0" xsi:nil="true"/>
-    <Math_Settings xmlns="633f040f-4953-46e7-8610-82b0c5296ba0" xsi:nil="true"/>
-    <Self_Registration_Enabled xmlns="633f040f-4953-46e7-8610-82b0c5296ba0" xsi:nil="true"/>
-    <Students xmlns="633f040f-4953-46e7-8610-82b0c5296ba0">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </Students>
-    <LMS_Mappings xmlns="633f040f-4953-46e7-8610-82b0c5296ba0" xsi:nil="true"/>
-    <Invited_Students xmlns="633f040f-4953-46e7-8610-82b0c5296ba0" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2C6CC7BA-2E2C-4B0D-8103-11A51D82E8EC}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{83D5100D-0E56-4B30-B42D-2AEC6B837C39}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="f62ef740-d444-4f18-80a2-7590fdcab1ce"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="633f040f-4953-46e7-8610-82b0c5296ba0"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -44740,18 +44749,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{83D5100D-0E56-4B30-B42D-2AEC6B837C39}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2C6CC7BA-2E2C-4B0D-8103-11A51D82E8EC}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="f62ef740-d444-4f18-80a2-7590fdcab1ce"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="633f040f-4953-46e7-8610-82b0c5296ba0"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>